<commit_message>
Final build ready for deployment
</commit_message>
<xml_diff>
--- a/examples/Australia OGD/SA Open Data/SA development application register_profile.xlsx
+++ b/examples/Australia OGD/SA Open Data/SA development application register_profile.xlsx
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -615,7 +615,7 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>2922355/2020</t>
+          <t>WIA/81/2020</t>
         </is>
       </c>
       <c r="T2" t="n">
@@ -623,24 +623,24 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>29219/2012/A</t>
+          <t>2922439/2020</t>
         </is>
       </c>
       <c r="V2" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="W2" t="n">
         <v>0</v>
       </c>
       <c r="X2" t="n">
-        <v>30096</v>
+        <v>33840</v>
       </c>
       <c r="Y2" t="n">
-        <v>2500</v>
+        <v>2796</v>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t xml:space="preserve">['2921/2016/8', '2921/2020', '29210/2020', '292100/2020', '2921000/2020', '2921001/2020', '2921002/2020', '2921003/2020', '2921004/2020', '2921005/2020', '2921006/2020', '2921007/2020', '2921008/2020', '2921009/2020', '292101/2020', '2921010/2020', '2921011/2020', '2921012/2020', '2921013/2020', '2921014/2020', '2921015/2020', '2921016/2020', '2921017/2020', '2921018/2020', '2921019/2020', '292102/2020', '2921020/2020', '2921021/2020', '2921022/2020', '2921023/2020', '2921024/2020', '2921025/2020', '2921026/2020', '2921027/2020', '2921028/2020', '2921029/2020', '292103/2020', '2921030/2020', '2921031/2020', '2921032/2020', '2921033/2020', '2921034/2020', '2921035/2020', '2921036/2020', '2921037/2020', '2921038/2020', '2921039/2020', '292104/2020', '2921040/2020', '2921041/2020', '2921042/2020', '2921043/2020', '2921044/2020', '2921045/2020', '2921046/2020', '2921047/2020', '2921048/2020', '2921049/2020', '292105/2020', '2921050/2020', '2921051/2020', '2921052/2020', '2921053/2020', '2921054/2020', '2921055/2020', '2921056/2020', '2921057/2020', '2921058/2020', '2921059/2020', '292106/2020', '2921060/2020', '2921061/2020', '2921062/2020', '2921063/2020', '2921064/2020', '2921065/2020', '2921066/2020', '2921067/2020', '2921068/2020', '2921069/2020', '292107/2020', '2921070/2020', '2921071/2020', '2921072/2020', '2921073/2020', '2921074/2020', '2921075/2020', '2921076/2020', '2921077/2020', '2921078/2020', '2921079/2020', '292108/2020', '2921080/2020', '2921081/2020', '2921082/2020', '2921083/2020', '2921083/2020/1', '2921084/2020', '2921085/2020', '2921086/2020', '2921087/2020', '2921088/2020', '2921089/2020', '292109/2020', '2921090/2020', '2921091/2019/1', '2921091/2019/2', '2921091/2019/3', '2921091/2020', '2921092/2020', '2921093/2020', '2921094/2020', '2921095/2020', '2921096/2020', '2921097/2019/1', '2921097/2019/2', '2921097/2020', '2921098/2020', '2921099/2020', '29211/2020', '292110/2020', '2921100/2020', '2921101/2020', '2921102/2020', '2921103/2020', '2921104/2020', '2921105/2020', '2921106/2020', '2921107/2020', '2921108/2020', '2921109/2020', '292111/2020', '2921110/2020', '2921111/2020', '2921112/2020', '2921113/2020', '2921114/2020', '2921115/2020', '2921116/2020', '2921117/2020', '2921118/2020', '2921119/2020', '292112/2020', '2921120/2020', '2921121/2020', '2921122/2020', '2921123/2020', '2921124/2020', '2921125/2020', '2921126/2020', '2921127/2020', '2921128/2020', '2921129/2020', '292113/2020', '2921130/2020', '2921131/2020', '2921132/2020', '2921133/2020', '2921134/2020', '2921135/2020', '2921136/2020', '2921137/2020', '2921138/2020', '2921139/2020', '292114/2020', '2921140/2020', '2921141/2020', '2921142/2020', '2921143/2020', '2921144/2020', '2921145/2020', '2921146/2020', '2921147/2020', '2921148/2020', '2921149/2020', '292115/2018/2', '292115/2018/B', '292115/2018/C', '292115/2020', '2921150/2020', '2921151/2020', '2921152/2020', '2921153/2020', '2921154/2017/A', '2921154/2018/A', '2921154/2020', '2921155/2020', '2921156/2020', '2921157/2020', '2921158/2020', '2921159/2020', '292116/2020', '2921160/2020', '2921161/2020', '2921162/2020', '2921163/2020', '2921164/2020', '2921165/2020', '2921166/2020', '2921167/2020', '2921168/2020', '2921169/2020', '292117/2020', '2921170/2020', '2921171/2020', '2921172/2020', '2921173/2020', '2921174/2020', '2921175/2020', '2921176/2020', '2921177/2020', '2921178/2020', '2921179/2020', '292118/2020', '2921180/2020', '2921181/2020', '2921182/2020', '2921183/2020', '2921184/2020', '2921185/2020', '2921186/2020', '2921187/2020', '2921188/2020', '2921189/2019/A', '2921189/2020', '292119/2020', '2921190/2020', '2921191/2020', '2921192/2020', '2921193/2020', '2921194/2020', '2921195/2020', '2921196/2020', '2921197/2020', '2921198/2020', '2921199/2020', '29212/2020', '292120/2020', '2921200/2020', '2921201/2020', '2921202/2020', '2921203/2020', '2921204/2020', '2921205/2020', '2921206/2020', '2921207/2020', '2921208/2020', '2921208/2020/1', '2921209/2020', '292121/2020', '2921210/2020', '2921211/2020', '2921212/2020', '2921213/2020', '2921214/2020', '2921215/2020', '2921216/2020', '2921217/2020', '2921218/2020', '2921219/2020', '292122/2020', '2921220/2020', '2921221/2020', '2921222/2020', '2921223/2020', '2921224/2020', '2921225/2020', '2921226/2020', '2921227/2020', '2921228/2020', '2921229/2020', '292123/2020', '2921230/2020', '2921231/2020', '2921232/2020', '2921233/2020', '2921234/2020', '2921235/2020', '2921236/2020', '2921237/2020', '2921238/2020', '2921239/2020', '292124/2020', '2921240/2020', '2921241/2020', '2921242/2020', '2921243/2020', '2921244/2020', '2921245/2020', '2921246/2020', '2921247/2020', '2921248/2020', '2921249/2020', '292125/2020', '2921250/2020', '2921251/2020', '2921252/2020', '2921253/2020', '2921254/2020', '2921255/2020', '2921256/2020', '2921257/2020', '2921258/2020', '2921259/2020', '292126/2020', '2921260/2020', '2921261/2020', '2921262/2020', '2921263/2020', '2921264/2020', '2921265/2020', '2921266/2020', '2921267/2020', '2921268/2020', '2921269/2020', '292127/2020', '2921270/2020', '2921270/2020/1', '2921271/2020', '2921272/2020', '2921273/2020', '2921274/2020', '2921275/2020', '2921276/2020', '2921277/2020', '2921278/2020', '2921279/2020', '292128/2020', '2921280/2020', '2921281/2020', '2921282/2020', '2921283/2020', '2921284/2020', '2921285/2020', '2921286/2020', '2921287/2020', '2921288/2020', '2921289/2020', '292129/2020', '2921290/2020', '2921291/2020', '2921292/2020', '2921293/2020', '2921294/2020', '2921295/2020', '2921296/2020', '2921297/2020', '2921298/2020', '2921299/2020', '29213/2020', '292130/2020', '2921300/2020', '2921301/2020', '2921302/2017/2', '2921302/2020', '2921303/2020', '2921304/2020', '2921305/2020', '2921306/2020', '2921307/2020', '2921308/2020', '2921309/2020', '292131/2020', '2921310/2020', '2921311/2020', '2921312/2020', '2921313/2020', '2921314/2020', '2921315/2020', '2921316/2020', '2921317/2020', '2921318/2020', '2921319/2020', '292132/2020', '2921320/2020', '2921321/2020', '2921322/2020', '2921323/2020', '2921324/2020', '2921325/2020', '2921326/2020', '2921327/2020', '2921328/2020', '2921329/2020', '292133/2020', '2921330/2020', '2921331/2020', '2921332/2020', '2921333/2020', '2921334/2020', '2921335/2020', '2921336/2020', '2921337/2020', '2921338/2020', '2921339/2020', '292134/2020', '2921340/2020', '2921341/2020', '2921342/2020', '2921343/2020', '2921344/2020', '2921345/2020', '2921346/2020', '2921347/2020', '2921348/2020', '2921349/2020', '292135/2020', '2921350/2020', '2921351/2020', '2921352/2020', '2921353/2020', '2921354/2020', '2921355/2020', '2921357/2020', '2921358/2020', '2921359/2020', '292136/2020', '2921360/2020', '2921361/2020', '2921362/2020', '2921363/2020', '2921364/2020', '2921365/2020', '2921366/2020', '2921367/2020', '2921368/2020', '2921369/2020', '292137/2020', '2921370/2020', '2921371/2020', '2921372/2020', '2921373/2020', '2921374/2020', '2921375/2020', '2921376/2020', '2921377/2020', '2921378/2020', '2921379/2020', '292138/2020', '2921380/2020', '2921381/2020', '2921382/2020', '2921383/2020', '2921384/2020', '2921385/2020', '2921386/2020', '2921387/2020', '2921388/2020', '2921389/2020', '292139/2020', '2921390/2020', '2921391/2020', '2921392/2020', '2921393/2020', '2921394/2020', '2921395/2020', '2921396/2020', '2921397/2020', '2921398/2020', '2921399/2020', '29214/2020', '292140/2020', '2921400/2020', '2921401/2020', '2921402/2020', '2921403/2020', '2921404/2020', '2921405/2020', '2921406/2020', '2921407/2020', '2921408/2020', '2921409/2020', '292141/2020', '2921410/2020', '2921411/2020', '2921412/2020', '2921413/2020', '2921414/2020', '2921415/2020', '2921416/2020', '2921417/2020', '2921418/2020', '2921419/2020', '292142/2020', '2921420/2020', '2921421/2019/1', '2921421/2019/2', '2921421/2020', '2921422/2020', '2921423/2020', '2921424/2020', '2921425/2020', '2921426/2020', '2921427/2020', '2921428/2020', '2921429/2020', '292143/2020', '2921430/2020', '2921431/2020', '2921432/2020', '2921433/2020', '2921434/2020', '2921435/2020', '2921436/2020', '2921437/2020', '2921438/2020', '2921439/2020', '292144/2020', '2921440/2020', '2921441/2020', '2921442/2020', '2921443/2020', '2921444/2020', '2921445/2020', '2921446/2020', '2921447/2020', '2921448/2020', '2921449/2018/A', '2921449/2020', '292145/2020', '2921450/2020', '2921451/2020', '2921452/2020', '2921453/2020', '2921454/2020', '2921455/2020', '2921456/2020', '2921457/2020', '2921458/2020', '2921459/2020', '292146/2020', '2921460/2020', '2921461/2020', '2921462/2020', '2921463/2020', '2921464/2020', '2921465/2020', '2921466/2020', '2921467/2020', '2921468/2020', '2921469/2020', '292147/2020', '2921470/2020', '2921471/2020', '2921472/2020', '2921473/2020', '2921474/2020', '2921475/2020', '2921476/2020', '2921477/2020', '2921478/2020', '2921479/2020', '292148/2020', '2921480/2020', '2921481/2020', '2921482/2020', '2921483/2020', '2921484/2020', '2921485/2020', '2921486/2020', '2921487/2020', '2921488/2020', '2921489/2020', '292149/2020', '2921490/2020', '2921491/2017/A', '2921491/2020', '2921492/2020', '2921493/2020', '2921494/2020', '2921495/2020', '2921496/2020', '2921497/2020', '2921498/2020', '2921499/2020', '29215/2020', '292150/2020', '2921500/2020', '2921501/2020', '2921502/2020', '2921503/2020', '2921504/2020', '2921505/2020', '2921506/2020', '2921507/2020', '2921508/2020', '2921509/2020', '292151/2020', '2921510/2020', '2921511/2020', '2921512/2020', '2921513/2020', '2921514/2020', '2921515/2020', '2921516/2020', '2921518/2020', '2921519/2020', '292152/2020', '2921520/2020', '2921522/2018/1', '2921522/2018/A', '2921522/2020', '2921523/2020', '2921524/2020', '2921525/2020', '2921526/2020', '2921527/2020', '2921528/2020', '2921529/2020', '292153/2020', '2921530/2020', '2921531/2020', '2921532/2020', '2921533/2020', '2921534/2020', '2921535/2020', '2921536/2020', '2921537/2020', '2921538/2020', '2921539/2020', '292154/2020', '2921540/2020', '2921541/2020', '2921542/2020', '2921543/2020', '2921544/2020', '2921545/2020', '2921546/2020', '2921547/2020', '2921548/2020', '2921549/2020', '292155/2020', '2921550/2020', '2921551/2020', '2921552/2020', '2921553/2020', '2921554/2017/2', '2921554/2017/3', '2921554/2020', '2921555/2020', '2921556/2020', '2921557/2020', '2921558/2020', '2921559/2020', '292156/2020', '2921560/2020', '2921561/2020', '2921562/2020', '2921563/2020', '2921564/2020', '2921565/2020', '2921566/2020', '2921567/2020', '2921568/2020', '2921569/2020', '2921570/2020', '2921571/2020', '2921572/2020', '2921573/2020', '2921574/2020', '2921575/2020', '2921576/2020', '2921577/2020', '2921578/2020', '2921579/2020', '292158/2020', '2921580/2020', '2921581/2020', '2921582/2020', '2921583/2020', '2921584/2020', '2921585/2020', '2921586/2020', '2921587/2020', '2921588/2020', '2921589/2020', '292159/2020', '2921590/2020', '2921591/2020', '2921592/2020', '2921593/2020', '2921594/2020', '2921595/2020', '2921596/2020', '2921597/2020', '2921598/2020', '2921599/2020', '29216/2020', '292160/2020', '2921600/2020', '2921601/2020', '2921602/2020', '2921603/2020', '2921604/2020', '2921605/2020', '2921606/2020', '2921607/2020', '2921608/2020', '2921609/2020', '292161/2020', '2921610/2020', '2921611/2020', '2921612/2020', '2921613/2020', '2921614/2020', '2921615/2020', '2921616/2020', '2921617/2020', '2921618/2020', '2921619/2020', '292162/2020', '2921620/2020', '2921621/2020', '2921622/2020', '2921623/2020', '2921624/2020', '2921625/2020', '2921626/2020', '2921627/2020', '2921628/2020', '2921629/2020', '292163/2020', '2921630/2020', '2921631/2020', '2921632/2020', '2921633/2020', '2921634/2020', '2921635/2020', '2921636/2020', '2921637/2020', '2921638/2020', '2921639/2020', '292164/2020', '2921640/2020', '2921641/2020', '2921642/2020', '2921643/2020', '2921644/2020', '2921645/2020', '2921646/2020', '2921647/2020', '2921648/2020', '2921649/2020', '292165/2020', '2921650/2020', '2921651/2020', '2921652/2020', '2921653/2020', '2921654/2020', '2921655/2020', '2921656/2020', '2921657/2020', '2921658/2020', '2921659/2020', '292166/2020', '2921660/2020', '2921661/2020', '2921662/2020', '2921663/2020', '2921664/2020', '2921665/2020', '2921666/2020', '2921667/2020', '2921668/2020', '2921669/2020', '292167/2020', '2921670/2020', '2921671/2020', '2921672/2020', '2921673/2020', '2921674/2020', '2921675/2020', '2921676/2020', '2921677/2020', '2921678/2020', '2921679/2020', '292168/2020', '2921680/2020', '2921681/2020', '2921682/2020', '2921683/2020', '2921684/2020', '2921685/2019/A', '2921685/2020', '2921686/2020', '2921687/2020', '2921688/2020', '2921689/2020', '292169/2020', '2921690/2020', '2921691/2020', '2921692/2020', '2921693/2020', '2921694/2020', '2921695/2020', '2921696/2020', '2921697/2020', '2921698/2020', '2921699/2020', '29217/2020', '292170/2020', '2921700/2016/2', '2921700/2020', '2921701/2020', '2921702/2018/A', '2921702/2020', '2921703/2017/4', '2921703/2017/5', '2921703/2020', '2921704/2020', '2921705/2019/A', '2921705/2020', '2921706/2020', '2921707/2020', '2921708/2020', '2921709/2018/B', '2921709/2020', '292171/2019/1/A', '292171/2019/2/A', '292171/2019/B', '292171/2020', '2921710/2020', '2921711/2020', '2921712/2020', '2921713/2020', '2921714/2020', '2921715/2020', '2921716/2020', '2921717/2020', '2921718/2020', '2921719/2020', '292172/2020', '2921720/2020', '2921721/2020', '2921722/2020', '2921723/2020', '2921724/2020', '2921725/2020', '2921726/2020', '2921727/2020', '2921728/2020', '2921729/2020', '292173/2020', '2921730/2020', '2921731/2020', '2921732/2020', '2921733/2020', '2921734/2020', '2921735/2020', '2921736/2020', '2921737/2020', '2921738/2020', '2921739/2020', '292174/2020', '2921740/2020', '2921741/2020', '2921742/2020', '2921743/2019/1', '2921743/2019/2', '2921743/2020', '2921744/2020', '2921745/2020', '2921746/2016/1/A', '2921746/2016/2/A', '2921746/2020', '2921747/2020', '2921748/2020', '2921749/2020', '292175/2020', '292175/2020/1', '292175/2020/2', '2921750/2020', '2921751/2020', '2921752/2020', '2921753/2020', '2921754/2020', '2921755/2020', '2921756/2018/2/A', '2921756/2020', '2921757/2020', '2921758/2020', '2921759/2020', '292176/2020', '2921760/2020', '2921761/2020', '2921762/2020', '2921763/2020', '2921764/2020', '2921765/2020', '2921766/2020', '2921767/2020', '2921768/2020', '2921769/2020', '292177/2020', '2921770/2020', '2921771/2020', '2921772/2020', '2921773/2020', '2921774/2020', '2921775/2020', '2921776/2020', '2921777/2020', '2921778/2020', '2921779/2020', '2921780/2020', '2921781/2020', '2921782/2020', '2921783/2020', '2921784/2020', '2921785/2020', '2921786/2020', '2921787/2020', '2921788/2020', '2921789/2020', '292179/2020', '2921790/2020', '2921791/2020', '2921792/2020', '2921793/2020', '2921794/2020', '2921795/2020', '2921796/2020', '2921797/2020', '2921798/2020', '2921799/2020', '29218/2020', '292180/2020', '2921800/2020', '2921801/2020', '2921802/2020', '2921803/2020', '2921804/2020', '2921805/2020', '2921806/2020', '2921807/2020', '2921808/2020', '2921809/2020', '292181/2020', '2921810/2020', '2921811/2017/A', '2921811/2020', '2921812/2020', '2921813/2020', '2921814/2020', '2921815/2020', '2921816/2020', '2921817/2020', '2921818/2020', '2921819/2020', '292182/2020', '2921820/2020', '2921821/2020', '2921822/2020', '2921823/2020', '2921824/2020', '2921825/2020', '2921826/2020', '2921827/2020', '2921828/2020', '2921829/2020', '292183/2020', '2921830/2020', '2921831/2020', '2921832/2020', '2921833/2020', '2921834/2020', '2921835/2019/A', '2921835/2020', '2921836/2020', '2921837/2020', '2921838/2020', '2921839/2020', '292184/2020', '2921840/2020', '2921841/2020', '2921842/2020', '2921843/2020', '2921844/2020', '2921845/2020', '2921846/2020', '2921847/2020', '2921848/2020', '2921849/2020', '292185/2020', '2921850/2020', '2921851/2020', '2921852/2020', '2921853/2020', '2921854/2020', '2921855/2020', '2921856/2020', '2921857/2020', '2921858/2020', '2921859/2020', '292186/2020', '2921860/2020', '2921861/2020', '2921862/2020', '2921863/2020', '2921864/2020', '2921865/2019/1', '2921865/2019/2', '2921865/2020', '2921866/2020', '2921867/2020', '2921868/2020', '2921869/2020', '292187/2020', '2921870/2020', '2921871/2020', '2921872/2020', '2921873/2020', '2921874/2020', '2921875/2020', '2921876/2020', '2921877/2020', '2921878/2020', '2921879/2020', '292188/2020', '2921880/2020', '2921881/2020', '2921882/2020', '2921883/2020', '2921884/2019/1', '2921884/2019/2', '2921884/2020', '2921885/2020', '2921886/2020', '2921887/2020', '2921888/2020', '2921889/2020', '292189/2020', '2921890/2020', '2921891/2020', '2921892/2020', '2921893/2020', '2921894/2020', '2921895/2020', '2921896/2020', '2921897/2020', '2921898/2020', '2921899/2020', '29219/2012/A', '29219/2020', '292190/2020', '2921900/2020', '2921901/2020', '2921902/2020', '2921903/2020', '2921904/2020', '2921905/2020', '2921906/2020', '2921907/2020', '2921908/2020', '2921909/2020', '292191/2020', '2921910/2020', '2921911/2020', '2921912/2020', '2921913/2020', '2921914/2020', '2921915/2020', '2921916/2019/1', '2921916/2020', '2921917/2019/1', '2921917/2020', '2921918/2020', '2921919/2020', '292192/2020', '2921920/2020', '2921921/2020', '2921922/2020', '2921923/2020', '2921924/2020', '2921925/2020', '2921926/2020', '2921927/2020', '2921928/2020', '2921929/2020', '292193/2020', '2921930/2020', '2921931/2020', '2921932/2020', '2921933/2020', '2921934/2020', '2921935/2020', '2921936/2020', '2921937/2020', '2921938/2020', '2921939/2020', '292194/2020', '2921940/2020', '2921941/2020', '2921942/2020', '2921943/2020', '2921944/2020', '2921945/2020', '2921946/2020', '2921947/2020', '2921948/2020', '2921949/2020', '292195/2020', '2921950/2020', '2921951/2020', '2921952/2020', '2921953/2020', '2921954/2020', '2921955/2020', '2921956/2020', '2921957/2020', '2921958/2020', '2921959/2020', '292196/2020', '2921960/2020', '2921961/2020', '2921962/2020', '2921963/2020', '2921964/2020', '2921965/2020', '2921966/2020', '2921967/2020', '2921968/2020', '2921969/2020', '292197/2020', '2921970/2020', '2921971/2020', '2921972/2020', '2921973/2020', '2921974/2020', '2921975/2020', '2921976/2020', '2921977/2020', '2921978/2020', '2921979/2020', '292198/2020', '2921980/2020', '2921981/2020', '2921982/2020', '2921983/2020', '2921984/2020', '2921985/2020', '2921986/2020', '2921987/2020', '2921988/2020', '2921989/2020', '292199/2020', '2921990/2020', '2921991/2020', '2921992/2020', '2921993/2019/A', '2921993/2020', '2921994/2020', '2921995/2020', '2921996/2020', '2921997/2020', '2921998/2020', '2921999/2020', '2922/2020', '29220/2020', '292200/2020', '2922000/2020', '2922001/2020', '2922002/2020', '2922003/2020', '2922004/2020', '2922005/2020', '2922006/2020', '2922007/2020', '2922008/2020', '2922009/2020', '292201/2020', '2922010/2020', '2922011/2020', '2922012/2020', '2922013/2020', '2922014/2020', '2922015/2020', '2922016/2020', '2922017/2020', '2922018/2020', '2922019/2020', '292202/2020', '2922020/2020', '2922021/2020', '2922022/2020', '2922023/2020', '2922024/2020', '2922026/2020', '2922027/2020', '2922028/2020', '2922029/2020', '292203/2020', '2922030/2020', '2922031/2020', '2922032/2020', '2922033/2020', '2922034/2020', '2922035/2020', '2922036/2020', '2922037/2020', '2922038/2020', '2922039/2020', '292204/2020', '2922040/2020', '2922041/2020', '2922042/2020', '2922043/2020', '2922044/2020', '2922045/2020', '2922046/2020', '2922047/2020', '2922048/2020', '2922049/2020', '292205/2020', '2922050/2020', '2922051/2020', '2922052/2020', '2922053/2020', '2922054/2020', '2922055/2020', '2922056/2020', '2922057/2020', '2922058/2020', '2922059/2020', '292206/2020', '2922060/2020', '2922061/2020', '2922062/2020', '2922063/2020', '2922064/2020', '2922065/2020', '2922066/2020', '2922067/2020', '2922068/2020', '2922069/2020', '292207/2020', '2922070/2020', '2922071/2020', '2922072/2020', '2922073/2020', '2922074/2020', '2922075/2020', '2922076/2020', '2922077/2020', '2922078/2020', '2922079/2020', '292208/2020', '2922080/2020', '2922081/2020', '2922082/2020', '2922083/2020', '2922084/2020', '2922085/2020', '2922086/2020', '2922087/2020', '2922088/2020', '2922089/2020', '292209/2020', '2922090/2020', '2922091/2020', '2922092/2020', '2922093/2020', '2922094/2020', '2922095/2020', '2922096/2020', '2922097/2020', '2922098/2020', '2922099/2020', '29221/2020', '292210/2020', '2922100/2020', '2922101/2020', '2922102/2020', '2922103/2020', '2922104/2020', '2922105/2020', '2922106/2020', '2922107/2020', '2922108/2020', '2922109/2020', '292211/2020', '2922110/2020', '2922111/2020', '2922112/2020', '2922113/2020', '2922114/2020', '2922115/2020', '2922116/2020', '2922117/2020', '2922118/2020', '2922119/2020', '292212/2020', '2922120/2020', '2922121/2020', '2922122/2020', '2922123/2020', '2922124/2020', '2922125/2020', '2922126/2020', '2922127/2020', '2922128/2020', '2922129/2020', '292213/2020', '2922130/2020', '2922131/2020', '2922132/2020', '2922133/2020', '2922134/2020', '2922135/2020', '2922136/2020', '2922137/2020', '2922138/2020', '2922139/2020', '292214/2020', '2922140/2020', '2922141/2020', '2922142/2020', '2922143/2020', '2922144/2020', '2922145/2020', '2922146/2020', '2922147/2020', '2922148/2020', '2922149/2020', '292215/2020', '2922150/2020', '2922151/2020', '2922152/2020', '2922153/2020', '2922154/2020', '2922155/2020', '2922156/2020', '2922157/2020', '2922158/2020', '2922159/2020', '292216/2020', '2922160/2020', '2922161/2020', '2922162/2020', '2922163/2020', '2922164/2020', '2922165/2020', '2922166/2020', '2922167/2020', '2922168/2020', '2922169/2020', '2922170/2020', '2922171/2020', '2922172/2020', '2922173/2020', '2922174/2020', '2922175/2020', '2922176/2020', '2922177/2020', '2922178/2020', '2922179/2020', '292218/2020', '2922180/2020', '2922181/2020', '2922182/2020', '2922183/2020', '2922184/2020', '2922185/2020', '2922186/2020', '2922187/2020', '2922188/2020', '2922189/2020', '292219/2020', '2922190/2020', '2922191/2020', '2922192/2020', '2922193/2020', '2922194/2020', '2922195/2020', '2922196/2020', '2922197/2020', '2922198/2020', '2922199/2020', '29222/2020', '292220/2020', '2922200/2020', '2922201/2020', '2922202/2020', '2922203/2020', '2922204/2020', '2922205/2020', '2922206/2020', '2922207/2020', '2922208/2020', '2922209/2020', '292221/2020', '2922210/2020', '2922211/2020', '2922212/2020', '2922213/2020', '2922214/2020', '2922215/2020', '2922216/2020', '2922217/2020', '2922218/2020', '2922219/2020', '292222/2020', '2922220/2020', '2922221/2020', '2922222/2020', '2922223/2020', '2922224/2020', '2922225/2020', '2922226/2020', '2922227/2020', '2922229/2020', '292223/2020', '2922230/2020', '2922231/2020', '2922232/2020', '2922233/2020', '2922234/2020', '2922235/2020', '2922236/2020', '2922237/2020', '2922238/2020', '2922239/2020', '292224/2020', '2922240/2020', '2922241/2020', '2922242/2020', '2922243/2020', '2922244/2020', '2922245/2020', '2922246/2020', '2922247/2020', '2922248/2020', '2922249/2020', '292225/2020', '2922250/2020', '2922251/2020', '2922252/2020', '2922253/2020', '2922254/2020', '2922255/2020', '2922256/2020', '2922257/2020', '2922258/2020', '2922259/2020', '292226/2020', '2922260/2020', '2922261/2020', '2922262/2020', '2922263/2020', '2922264/2020', '2922265/2020', '2922266/2020', '2922267/2020', '2922268/2020', '2922269/2020', '292227/2020', '2922270/2020', '2922271/2020', '2922272/2020', '2922273/2020', '2922274/2020', '2922275/2020', '2922276/2020', '2922277/2020', '2922278/2020', '2922279/2020', '292228/2020', '2922280/2020', '2922281/2020', '2922282/2020', '2922283/2020', '2922284/2020', '2922285/2020', '2922286/2020', '2922287/2020', '2922288/2020', '2922289/2020', '292229/2020', '2922290/2020', '2922291/2020', '2922292/2020', '2922293/2020', '2922294/2020', '2922295/2020', '2922296/2020', '2922297/2020', '2922298/2020', '2922299/2020', '29223/2020', '292230/2020', '2922300/2020', '2922301/2020', '2922302/2020', '2922303/2020', '2922304/2020', '2922305/2020', '2922306/2020', '2922307/2020', '2922308/2020', '2922309/2020', '292231/2020', '2922310/2020', '2922311/2020', '2922312/2020', '2922313/2020', '2922314/2020', '2922315/2020', '2922316/2020', '2922317/2020', '2922318/2020', '2922319/2020', '292232/2020', '2922320/2020', '2922321/2020', '2922322/2020', '2922323/2020', '2922324/2020', '2922325/2020', '2922326/2020', '2922327/2020', '2922328/2020', '2922329/2020', '292233/2020', '2922330/2020', '2922331/2020', '2922332/2020', '2922333/2020', '2922334/2020', '2922335/2020', '2922336/2020', '2922337/2020', '2922338/2020', '2922339/2020', '292234/2020', '2922340/2020', '2922341/2020', '2922342/2020', '2922343/2020', '2922344/2020', '2922345/2020', '2922346/2020', '2922347/2020', '2922348/2020', '2922349/2020', '292235/2020', '2922350/2020', '2922351/2020', '2922352/2020', '2922353/2020', '2922354/2020', '2922355/2020', '2922356/2020', '292236/2020', '292237/2020', '292238/2020', '292239/2017/A', '292239/2020', '29224/2020', '292240/2020', '292240/2020/A', '292241/2020', '292242/2020', '292243/2020', '292244/2020', '292245/2020', '292246/2020', '292247/2020', '292248/2020', '292249/2020', '29225/2020', '292250/2020', '292251/2020', '292252/2020', '292253/2020', '292254/2020', '292255/2020', '292256/2020', '292257/2020', '292258/2020', '292259/2020', '29226/2020', '292260/2020', '292261/2020', '292262/2020', '292263/2020', '292264/2020', '292265/2020', '292266/2020', '292267/2020', '292268/2020', '292269/2020', '29227/2020', '292270/2020', '292271/2020', '292272/2020', '292273/2020', '292274/2020', '292275/2020', '292276/2020', '292277/2020', '292278/2020', '292279/2020', '29228/2020', '292280/2020', '292281/2020', '292282/2020', '292283/2020', '292284/2020', '292286/2020', '292287/2020', '292288/2016/2', '292289/2020', '29229/2020', '292290/2016/1/C', '292290/2020', '292291/2020', '292292/2020', '292293/2020', '292294/2020', '292295/2020', '292296/2020', '292297/2020', '292298/2020', '292299/2019/A', '292299/2020', '2923/2020', '292300/2020', '292301/2020', '292302/2020', '292303/2020', '292304/2020', '292305/2020', '292306/2020', '292307/2020', '292308/2020', '292309/2020', '292310/2020', '292311/2020', '292312/2018/2', '292312/2020', '292313/2020', '292314/2020', '292315/2020', '292316/2020', '292317/2020', '292318/2020', '292319/2020', '29232/2020', '292320/2020', '292321/2020', '292322/2020', '292323/2020', '292324/2020', '292325/2020', '292326/2020', '292327/2020', '292328/2020', '292329/2020', '29233/2020', '292330/2020', '292331/2020', '292332/2020', '292333/2020', '292334/2020', '292335/2020', '292336/2020', '292337/2020', '292338/2020', '292338/2020/1', '292338/2020/2', '292339/2020', '29234/2020', '292340/2020', '292341/2020', '292341/2020/A', '292342/2020', '292343/2020', '292344/2020', '292345/2020', '292346/2020', '292347/2020', '292348/2019/1', '292348/2019/2', '292348/2020', '292349/2020', '29235/2020', '292350/2020', '292351/2020', '292352/2020', '292353/2020', '292354/2020', '292355/2020', '292356/2020', '292357/2020', '292358/2019/1/A', '292358/2020', '292359/2020', '29236/2018/A', '29236/2020', '292360/2020', '292361/2020', '292362/2020', '292363/2020', '292364/2020', '292365/2020', '292366/2020', '292367/2020', '292368/2020', '292369/2020', '29237/2020', '292370/2020', '292371/2020', '292372/2020', '292373/2020', '292374/2020', '292375/2020', '292376/2020', '292378/2020', '292379/2020', '29238/2020', '292380/2020', '292381/2020', '292382/2020', '292383/2020', '292384/2020', '292385/2020', '292386/2020', '292387/2020', '292388/2020', '292389/2020', '29239/2020', '292390/2020', '292391/2020', '292392/2020', '292393/2020', '292394/2020', '292395/2020', '292396/2020', '292397/2020', '292398/2020', '292399/2020', '2924/2020', '29240/2020', '292400/2007/A', '292400/2020', '292401/2020', '292402/2020', '292403/2020', '292404/2020', '292405/2020', '292406/2020', '292407/2020', '292408/2020', '292409/2020', '29241/2020', '292410/2020', '292411/2020', '292412/2020', '292413/2020', '292414/2020', '292415/2020', '292416/2020', '292417/2020', '292418/2020', '292419/2020', '29242/2020', '292420/2020', '292421/2020', '292422/2020', '292423/2020', '292424/2020', '292426/2020', '292427/2020', '292428/2020', '292429/2020', '29243/2020', '292430/2020', '292431/2020', '292434/2020', '292435/2020', '292436/2020', '292437/2020', '292438/2020', '292439/2020', '29244/2020', '292440/2020', '292441/2020', '292442/2020', '292443/2020', '292444/2020', '292445/2020', '292446/2020', '292447/2020', '292448/2020', '292449/2020', '29245/2020', '292450/2020', '292451/2020', '292452/2020', '292453/2020', '292454/2020', '292455/2020', '292456/2020', '292457/2020', '292458/2020', '292459/2020', '29246/2020', '292460/2020', '292461/2020', '292462/2020', '292463/2020', '292464/2020', '292465/2020', '292466/2020', '292467/2020', '292468/2020', '292469/2020', '29247/2020', '292470/2020', '292471/2020', '292472/2020', '292473/2020', '292474/2020', '292475/2020', '292476/2020', '292477/2020', '292478/2020', '292479/2020', '29248/2020', '292480/2020', '292481/2020', '292482/2020', '292483/2020', '292484/2020', '292485/2020', '292486/2020', '292487/2020', '292488/2020', '292489/2020', '29249/2020', '292490/2020', '292491/2020', '292492/2020', '292493/2020', '292494/2020', '292495/2020', '292496/2020', '292497/2020', '292498/2020', '292499/2020', '2925/2020', '29250/2020', '292500/2020', '292501/2020', '292502/2020', '292503/2020', '292504/2020', '292505/2020', '292506/2020', '292507/2020', '292508/2020', '292509/2020', '29251/2020', '292510/2020', '292511/2020', '292512/2020', '292513/2020', '292514/2020', '292515/2020', '292516/2020', '292517/2020', '292518/2020', '292519/2020', '29252/2020', '292520/2020', '292521/2020', '292522/2020', '292523/2020', '292524/2020', '292525/2020', '292526/2020', '292527/2020', '292528/2020', '292529/2020', '29253/2020', '292530/2020', '292531/2020', '292532/2020', '292533/2020', '292534/2020', '292535/2020', '292536/2020', '292537/2020', '292538/2020', '292539/2020', '292540/2020', '292541/2020', '292542/2020', '292543/2020', '292544/2017/3', '292544/2020', '292545/2020', '292546/2020', '292547/2020', '292548/2020', '292549/2020', '29255/2020', '292550/2020', '292551/2020', '292552/2020', '292553/2020', '292554/2020', '292555/2020', '292556/2020', '292557/2020', '292558/2020', '292559/2020', '29256/2020', '292560/2020', '292561/2020', '292562/2020', '292563/2020', '292564/2020', '292565/2020', '292566/2020', '292567/2020', '292568/2020', '292569/2020', '29257/2020', '292570/2020', '292571/2020', '292572/2020', '292573/2020', '292574/2020', '292575/2020', '292576/2020', '292577/2020', '292578/2020', '292579/2020', '29258/2020', '292580/2020', '292581/2020', '292582/2020', '292583/2020', '292584/2020', '292585/2020', '292586/2020', '292587/2020', '292588/2020', '292589/2020', '29259/2020', '292590/2020', '292591/2020', '292592/2020', '292593/2020', '292594/2020', '292595/2020', '292596/2020', '292597/2020', '292598/2020', '292599/2020', '2926/2020', '29260/2020', '292600/2020', '292601/2020', '292602/2020', '292603/2020', '292604/2020', '292605/2020', '292606/2020', '292607/2020', '292608/2020', '292609/2020', '29261/2020', '292610/2020', '292611/2020', '292612/2020', '292613/2020', '292614/2020', '292615/2020', '292616/2020', '292617/2020', '292618/2020', '292619/2020', '29262/2020', '292620/2020', '292621/2020', '292622/2020', '292623/2020', '292624/2020', '292625/2020', '292626/2020', '292627/2020', '292628/2020', '292629/2020', '29263/2020', '292630/2020', '292631/2020', '292632/2020', '292633/2020', '292634/2020', '292635/2020', '292636/2020', '292637/2020', '292638/2020', '292639/2020', '29264/2020', '292640/2020', '292641/2020', '292642/2020', '292643/2020', '292644/2020', '292645/2020', '292646/2020', '292647/2020', '292648/2020', '292649/2020', '29265/2020', '292650/2020', '292651/2020', '292652/2020', '292653/2020', '292654/2020', '292655/2020', '292656/2020', '292657/2020', '292658/2020', '292659/2020', '29266/2012/6', '29266/2020', '292660/2020', '292661/2020', '292662/2020', '292662/2020/1', '292662/2020/2', '292663/2020', '292664/2020', '292665/2020', '292666/2020', '292667/2020', '292668/2020', '292669/2020', '29267/2020', '292670/2020', '292671/2020', '292672/2020', '292672/2020/1', '292673/2020', '292674/2020', '292675/2020', '292676/2020', '292677/2020', '292678/2020', '292679/2020', '29268/2020', '292680/2020', '292681/2019/1/A', '292681/2020', '292682/2020', '292683/2020', '292684/2020', '292685/2020', '292686/2020', '292687/2020', '292688/2020', '292689/2020', '29269/2020', '292690/2020', '292691/2020', '292692/2020', '292693/2020', '292694/2020', '292695/2020', '292696/2020', '292697/2020', '292698/2020', '292699/2020', '2927/2020', '29270/2020', '292700/2020', '292701/2017/B', '292701/2020', '292702/2020', '292703/2020', '292704/2020', '292705/2020', </t>
+          <t xml:space="preserve">['2921/2016/8', '2921/2020', '29210/2020', '292100/2020', '2921000/2020', '2921001/2020', '2921002/2020', '2921003/2020', '2921004/2020', '2921005/2020', '2921006/2020', '2921007/2020', '2921008/2020', '2921009/2020', '292101/2020', '2921010/2020', '2921011/2020', '2921012/2020', '2921013/2020', '2921014/2020', '2921015/2020', '2921016/2020', '2921017/2020', '2921018/2020', '2921019/2020', '292102/2020', '2921020/2020', '2921021/2020', '2921022/2020', '2921023/2020', '2921024/2020', '2921025/2020', '2921026/2020', '2921027/2020', '2921028/2020', '2921029/2020', '292103/2020', '2921030/2020', '2921031/2020', '2921032/2020', '2921033/2020', '2921034/2020', '2921035/2020', '2921036/2020', '2921037/2020', '2921038/2020', '2921039/2020', '292104/2020', '2921040/2020', '2921041/2020', '2921042/2020', '2921043/2020', '2921044/2020', '2921045/2020', '2921046/2020', '2921047/2020', '2921048/2020', '2921049/2020', '292105/2020', '2921050/2020', '2921051/2020', '2921052/2020', '2921053/2020', '2921054/2020', '2921055/2020', '2921056/2020', '2921057/2020', '2921058/2020', '2921059/2020', '292106/2020', '2921060/2020', '2921061/2020', '2921062/2020', '2921063/2020', '2921064/2020', '2921065/2020', '2921066/2020', '2921067/2020', '2921068/2020', '2921069/2020', '292107/2020', '2921070/2020', '2921071/2020', '2921072/2020', '2921073/2020', '2921074/2020', '2921075/2020', '2921076/2020', '2921077/2020', '2921078/2020', '2921079/2020', '292108/2020', '2921080/2020', '2921081/2020', '2921082/2020', '2921083/2020', '2921083/2020/1', '2921084/2020', '2921085/2020', '2921086/2020', '2921087/2020', '2921088/2020', '2921089/2020', '292109/2020', '2921090/2020', '2921091/2019/1', '2921091/2019/2', '2921091/2019/3', '2921091/2020', '2921092/2020', '2921093/2020', '2921094/2020', '2921095/2020', '2921096/2020', '2921097/2019/1', '2921097/2019/2', '2921097/2020', '2921098/2020', '2921099/2020', '29211/2020', '292110/2020', '2921100/2020', '2921101/2020', '2921102/2020', '2921103/2020', '2921104/2020', '2921105/2020', '2921106/2020', '2921107/2020', '2921108/2020', '2921109/2020', '292111/2020', '2921110/2020', '2921111/2020', '2921112/2020', '2921113/2020', '2921114/2020', '2921115/2020', '2921116/2020', '2921117/2020', '2921118/2020', '2921119/2020', '292112/2020', '2921120/2020', '2921121/2020', '2921122/2020', '2921123/2020', '2921124/2020', '2921125/2020', '2921126/2020', '2921127/2020', '2921128/2020', '2921129/2020', '292113/2020', '2921130/2020', '2921131/2020', '2921132/2020', '2921133/2020', '2921134/2020', '2921135/2020', '2921136/2020', '2921137/2020', '2921138/2020', '2921139/2020', '292114/2020', '2921140/2020', '2921141/2020', '2921142/2020', '2921143/2020', '2921144/2020', '2921145/2020', '2921146/2020', '2921147/2020', '2921148/2020', '2921149/2020', '292115/2018/2', '292115/2018/B', '292115/2018/C', '292115/2020', '2921150/2020', '2921151/2020', '2921152/2020', '2921153/2020', '2921154/2017/A', '2921154/2018/A', '2921154/2020', '2921155/2020', '2921156/2020', '2921157/2020', '2921158/2020', '2921159/2020', '292116/2020', '2921160/2020', '2921161/2020', '2921162/2020', '2921163/2020', '2921164/2020', '2921165/2020', '2921166/2020', '2921167/2020', '2921168/2020', '2921169/2020', '292117/2020', '2921170/2020', '2921171/2020', '2921172/2020', '2921173/2020', '2921174/2020', '2921175/2020', '2921176/2020', '2921177/2020', '2921178/2020', '2921179/2020', '292118/2020', '2921180/2020', '2921181/2020', '2921182/2020', '2921183/2020', '2921184/2020', '2921185/2020', '2921186/2020', '2921187/2020', '2921188/2020', '2921189/2019/A', '2921189/2020', '292119/2020', '2921190/2020', '2921191/2020', '2921192/2020', '2921193/2020', '2921194/2020', '2921195/2020', '2921196/2020', '2921197/2020', '2921198/2020', '2921199/2020', '29212/2020', '292120/2020', '2921200/2020', '2921201/2020', '2921202/2020', '2921203/2020', '2921204/2020', '2921205/2020', '2921206/2020', '2921207/2020', '2921208/2020', '2921208/2020/1', '2921209/2020', '292121/2020', '2921210/2020', '2921211/2020', '2921212/2020', '2921213/2020', '2921214/2020', '2921215/2020', '2921216/2020', '2921217/2020', '2921218/2020', '2921219/2020', '292122/2020', '2921220/2020', '2921221/2020', '2921222/2020', '2921223/2020', '2921224/2020', '2921225/2020', '2921226/2020', '2921227/2020', '2921228/2020', '2921229/2020', '292123/2020', '2921230/2020', '2921231/2020', '2921232/2020', '2921233/2020', '2921234/2020', '2921235/2020', '2921236/2020', '2921237/2020', '2921238/2020', '2921239/2020', '292124/2020', '2921240/2020', '2921241/2020', '2921242/2020', '2921243/2020', '2921244/2020', '2921245/2020', '2921246/2020', '2921247/2020', '2921248/2020', '2921249/2020', '292125/2020', '2921250/2020', '2921251/2020', '2921252/2020', '2921253/2020', '2921254/2020', '2921255/2020', '2921256/2020', '2921257/2020', '2921258/2020', '2921259/2020', '292126/2020', '2921260/2020', '2921261/2020', '2921262/2020', '2921263/2020', '2921264/2020', '2921265/2020', '2921266/2020', '2921267/2020', '2921268/2020', '2921269/2020', '292127/2020', '2921270/2020', '2921270/2020/1', '2921271/2020', '2921272/2020', '2921273/2020', '2921274/2020', '2921275/2020', '2921276/2020', '2921277/2020', '2921278/2020', '2921279/2020', '292128/2020', '2921280/2020', '2921281/2020', '2921282/2020', '2921283/2020', '2921284/2020', '2921285/2020', '2921286/2020', '2921287/2020', '2921288/2020', '2921289/2020', '292129/2020', '2921290/2020', '2921291/2020', '2921292/2020', '2921293/2020', '2921294/2020', '2921295/2020', '2921296/2020', '2921297/2020', '2921298/2020', '2921299/2020', '29213/2020', '292130/2020', '2921300/2020', '2921301/2020', '2921302/2017/2', '2921302/2020', '2921303/2020', '2921304/2020', '2921305/2020', '2921306/2020', '2921307/2020', '2921308/2020', '2921309/2020', '292131/2020', '2921310/2020', '2921311/2020', '2921312/2020', '2921313/2020', '2921314/2020', '2921315/2020', '2921316/2020', '2921317/2020', '2921318/2020', '2921319/2020', '292132/2020', '2921320/2020', '2921321/2020', '2921322/2020', '2921323/2020', '2921324/2020', '2921325/2020', '2921326/2020', '2921327/2020', '2921328/2020', '2921329/2020', '292133/2020', '2921330/2020', '2921331/2020', '2921332/2020', '2921333/2020', '2921334/2020', '2921335/2020', '2921336/2020', '2921337/2020', '2921338/2020', '2921339/2020', '292134/2020', '2921340/2020', '2921341/2020', '2921342/2020', '2921343/2020', '2921344/2020', '2921345/2020', '2921346/2020', '2921347/2020', '2921348/2020', '2921349/2020', '292135/2020', '2921350/2020', '2921351/2020', '2921352/2020', '2921353/2020', '2921354/2020', '2921355/2020', '2921357/2020', '2921358/2020', '2921359/2020', '292136/2020', '2921360/2020', '2921361/2020', '2921362/2020', '2921363/2020', '2921364/2020', '2921365/2020', '2921366/2020', '2921367/2020', '2921368/2020', '2921369/2020', '292137/2020', '2921370/2020', '2921371/2020', '2921372/2020', '2921373/2020', '2921374/2020', '2921375/2020', '2921376/2020', '2921377/2020', '2921378/2020', '2921379/2020', '292138/2020', '2921380/2020', '2921381/2020', '2921382/2020', '2921383/2020', '2921384/2020', '2921385/2020', '2921386/2020', '2921387/2020', '2921388/2020', '2921389/2020', '292139/2020', '2921390/2020', '2921391/2020', '2921392/2020', '2921393/2020', '2921394/2020', '2921395/2020', '2921396/2020', '2921397/2020', '2921398/2020', '2921399/2020', '29214/2020', '292140/2020', '2921400/2020', '2921401/2020', '2921402/2020', '2921403/2020', '2921404/2020', '2921405/2020', '2921406/2020', '2921407/2020', '2921408/2020', '2921409/2020', '292141/2020', '2921410/2020', '2921411/2020', '2921412/2020', '2921413/2020', '2921414/2020', '2921415/2020', '2921416/2020', '2921417/2020', '2921418/2020', '2921419/2020', '292142/2020', '2921420/2020', '2921421/2019/1', '2921421/2019/2', '2921421/2020', '2921422/2020', '2921423/2020', '2921424/2020', '2921425/2020', '2921426/2020', '2921427/2020', '2921428/2020', '2921429/2020', '292143/2020', '2921430/2020', '2921431/2020', '2921432/2020', '2921433/2020', '2921434/2020', '2921435/2020', '2921436/2020', '2921437/2020', '2921438/2020', '2921439/2020', '292144/2020', '2921440/2020', '2921441/2020', '2921442/2020', '2921443/2020', '2921444/2020', '2921445/2020', '2921446/2020', '2921447/2020', '2921448/2020', '2921449/2018/2', '2921449/2018/A', '2921449/2020', '292145/2020', '2921450/2020', '2921451/2020', '2921452/2020', '2921453/2020', '2921454/2020', '2921455/2020', '2921456/2020', '2921457/2020', '2921458/2020', '2921459/2020', '292146/2020', '2921460/2020', '2921461/2020', '2921462/2020', '2921463/2020', '2921464/2020', '2921465/2020', '2921466/2020', '2921467/2020', '2921468/2020', '2921469/2020', '292147/2020', '2921470/2020', '2921471/2020', '2921472/2020', '2921473/2020', '2921474/2020', '2921475/2020', '2921476/2020', '2921477/2020', '2921478/2020', '2921479/2020', '292148/2020', '2921480/2020', '2921481/2020', '2921482/2020', '2921483/2020', '2921484/2020', '2921485/2020', '2921486/2020', '2921487/2020', '2921488/2020', '2921489/2020', '292149/2020', '2921490/2020', '2921491/2017/A', '2921491/2020', '2921492/2020', '2921493/2020', '2921494/2020', '2921495/2020', '2921496/2020', '2921497/2020', '2921498/2020', '2921499/2020', '29215/2020', '292150/2020', '2921500/2020', '2921501/2020', '2921502/2020', '2921503/2020', '2921504/2020', '2921505/2020', '2921506/2020', '2921507/2020', '2921508/2020', '2921509/2020', '292151/2020', '2921510/2020', '2921511/2020', '2921512/2020', '2921513/2020', '2921514/2020', '2921515/2020', '2921516/2020', '2921518/2020', '2921519/2020', '292152/2020', '2921520/2020', '2921522/2018/1', '2921522/2018/A', '2921522/2020', '2921523/2020', '2921524/2020', '2921525/2020', '2921526/2020', '2921527/2020', '2921528/2020', '2921529/2020', '292153/2020', '2921530/2020', '2921531/2020', '2921532/2020', '2921533/2020', '2921534/2020', '2921535/2020', '2921536/2020', '2921537/2020', '2921538/2020', '2921539/2020', '292154/2020', '2921540/2020', '2921541/2020', '2921542/2020', '2921543/2020', '2921544/2020', '2921545/2020', '2921546/2020', '2921547/2020', '2921548/2020', '2921549/2020', '292155/2020', '2921550/2020', '2921551/2020', '2921552/2020', '2921553/2020', '2921554/2017/2', '2921554/2017/3', '2921554/2020', '2921555/2020', '2921556/2020', '2921557/2020', '2921558/2020', '2921559/2020', '292156/2020', '2921560/2020', '2921561/2020', '2921562/2020', '2921563/2020', '2921564/2020', '2921565/2020', '2921566/2020', '2921567/2020', '2921568/2020', '2921569/2020', '2921570/2020', '2921571/2020', '2921572/2020', '2921573/2020', '2921574/2020', '2921575/2020', '2921576/2020', '2921577/2020', '2921578/2020', '2921579/2020', '292158/2020', '2921580/2020', '2921581/2020', '2921582/2020', '2921583/2020', '2921584/2020', '2921585/2020', '2921586/2020', '2921587/2020', '2921588/2020', '2921589/2020', '292159/2020', '2921590/2020', '2921591/2020', '2921592/2020', '2921593/2020', '2921594/2020', '2921595/2020', '2921596/2020', '2921597/2020', '2921598/2020', '2921599/2020', '29216/2020', '292160/2020', '2921600/2020', '2921601/2020', '2921602/2020', '2921603/2020', '2921604/2020', '2921605/2020', '2921606/2020', '2921607/2020', '2921608/2020', '2921609/2020', '292161/2020', '2921610/2020', '2921611/2020', '2921612/2020', '2921613/2020', '2921614/2020', '2921615/2020', '2921616/2020', '2921617/2020', '2921618/2020', '2921619/2020', '292162/2020', '2921620/2020', '2921621/2020', '2921622/2020', '2921623/2020', '2921624/2020', '2921625/2020', '2921626/2020', '2921627/2020', '2921628/2020', '2921629/2020', '292163/2020', '2921630/2020', '2921631/2020', '2921632/2020', '2921633/2020', '2921634/2020', '2921635/2020', '2921636/2020', '2921637/2020', '2921638/2020', '2921639/2020', '292164/2020', '2921640/2020', '2921641/2020', '2921642/2020', '2921643/2020', '2921644/2020', '2921645/2020', '2921646/2020', '2921647/2020', '2921648/2020', '2921649/2020', '292165/2020', '2921650/2020', '2921651/2020', '2921652/2020', '2921653/2020', '2921654/2020', '2921655/2020', '2921656/2020', '2921657/2020', '2921658/2020', '2921659/2020', '292166/2020', '2921660/2020', '2921661/2020', '2921662/2020', '2921663/2020', '2921664/2020', '2921665/2020', '2921666/2020', '2921667/2020', '2921668/2020', '2921669/2020', '292167/2020', '2921670/2020', '2921671/2020', '2921672/2020', '2921673/2020', '2921674/2020', '2921675/2020', '2921676/2020', '2921677/2020', '2921678/2020', '2921679/2020', '292168/2020', '2921680/2020', '2921681/2020', '2921682/2020', '2921683/2020', '2921684/2020', '2921685/2019/A', '2921685/2020', '2921686/2020', '2921687/2020', '2921688/2020', '2921689/2020', '292169/2020', '2921690/2020', '2921691/2020', '2921692/2020', '2921693/2020', '2921694/2020', '2921695/2020', '2921696/2020', '2921697/2020', '2921698/2020', '2921699/2020', '29217/2020', '292170/2020', '2921700/2016/2', '2921700/2016/3', '2921700/2020', '2921701/2020', '2921702/2018/A', '2921702/2020', '2921703/2017/4', '2921703/2017/5', '2921703/2020', '2921704/2020', '2921705/2019/A', '2921705/2020', '2921706/2020', '2921707/2020', '2921708/2020', '2921709/2018/B', '2921709/2020', '292171/2019/1/A', '292171/2019/2/A', '292171/2019/B', '292171/2020', '2921710/2020', '2921711/2020', '2921712/2020', '2921713/2020', '2921714/2020', '2921715/2020', '2921716/2020', '2921717/2020', '2921718/2020', '2921719/2020', '292172/2020', '2921720/2020', '2921721/2020', '2921722/2020', '2921723/2020', '2921724/2020', '2921725/2020', '2921726/2020', '2921727/2020', '2921728/2020', '2921729/2020', '292173/2020', '2921730/2020', '2921731/2020', '2921732/2020', '2921733/2020', '2921734/2020', '2921735/2020', '2921736/2020', '2921737/2020', '2921738/2020', '2921739/2020', '292174/2020', '2921740/2020', '2921741/2020', '2921742/2020', '2921743/2019/1', '2921743/2019/2', '2921743/2020', '2921744/2020', '2921745/2020', '2921746/2016/1/A', '2921746/2016/2/A', '2921746/2020', '2921747/2020', '2921748/2020', '2921749/2020', '292175/2020', '292175/2020/1', '292175/2020/2', '2921750/2020', '2921751/2020', '2921752/2020', '2921753/2020', '2921754/2020', '2921755/2020', '2921756/2018/2/A', '2921756/2020', '2921757/2020', '2921758/2020', '2921759/2020', '292176/2020', '2921760/2020', '2921761/2020', '2921762/2020', '2921763/2020', '2921764/2020', '2921765/2020', '2921766/2020', '2921767/2020', '2921768/2020', '2921769/2020', '292177/2020', '2921770/2020', '2921771/2020', '2921772/2020', '2921773/2020', '2921774/2020', '2921775/2020', '2921776/2020', '2921777/2020', '2921778/2020', '2921779/2020', '2921780/2020', '2921781/2020', '2921782/2020', '2921783/2020', '2921784/2020', '2921785/2020', '2921786/2020', '2921787/2020', '2921788/2020', '2921789/2020', '292179/2020', '2921790/2020', '2921791/2020', '2921792/2020', '2921793/2020', '2921794/2020', '2921795/2020', '2921796/2020', '2921797/2020', '2921798/2020', '2921799/2020', '29218/2020', '292180/2020', '2921800/2020', '2921801/2020', '2921802/2020', '2921803/2020', '2921804/2020', '2921805/2020', '2921806/2020', '2921807/2020', '2921808/2020', '2921809/2020', '292181/2020', '2921810/2020', '2921811/2017/A', '2921811/2020', '2921812/2020', '2921813/2020', '2921814/2020', '2921815/2020', '2921816/2020', '2921817/2020', '2921818/2020', '2921819/2020', '292182/2020', '2921820/2020', '2921821/2020', '2921822/2020', '2921823/2020', '2921824/2020', '2921825/2020', '2921826/2020', '2921827/2020', '2921828/2020', '2921829/2020', '292183/2020', '2921830/2020', '2921831/2020', '2921832/2020', '2921833/2020', '2921834/2020', '2921835/2019/A', '2921835/2020', '2921836/2020', '2921837/2020', '2921838/2020', '2921839/2020', '292184/2020', '2921840/2020', '2921841/2020', '2921842/2020', '2921843/2020', '2921844/2020', '2921845/2020', '2921846/2020', '2921847/2020', '2921848/2020', '2921848/2020/1', '2921849/2020', '292185/2020', '2921850/2020', '2921851/2020', '2921852/2020', '2921853/2020', '2921854/2020', '2921855/2020', '2921856/2020', '2921857/2020', '2921858/2020', '2921859/2020', '292186/2020', '2921860/2020', '2921861/2020', '2921862/2020', '2921863/2020', '2921864/2020', '2921865/2019/1', '2921865/2019/2', '2921865/2020', '2921866/2020', '2921867/2020', '2921868/2020', '2921869/2020', '292187/2020', '2921870/2020', '2921871/2020', '2921872/2020', '2921873/2017/A', '2921873/2020', '2921874/2020', '2921875/2020', '2921876/2020', '2921877/2020', '2921878/2020', '2921879/2020', '292188/2020', '2921880/2020', '2921881/2020', '2921882/2020', '2921883/2020', '2921884/2019/1', '2921884/2019/2', '2921884/2020', '2921885/2020', '2921886/2020', '2921887/2020', '2921888/2020', '2921889/2020', '292189/2020', '2921890/2020', '2921891/2020', '2921892/2020', '2921893/2020', '2921894/2020', '2921895/2020', '2921896/2020', '2921897/2020', '2921898/2020', '2921899/2020', '29219/2012/A', '29219/2020', '292190/2020', '2921900/2020', '2921901/2020', '2921902/2020', '2921903/2020', '2921904/2020', '2921905/2020', '2921906/2020', '2921907/2020', '2921908/2020', '2921909/2020', '292191/2020', '2921910/2020', '2921911/2020', '2921912/2020', '2921913/2020', '2921914/2020', '2921915/2020', '2921916/2019/1', '2921916/2020', '2921917/2019/1', '2921917/2020', '2921918/2020', '2921919/2020', '292192/2020', '2921920/2020', '2921921/2020', '2921922/2020', '2921923/2020', '2921924/2020', '2921925/2020', '2921926/2020', '2921927/2020', '2921928/2020', '2921929/2020', '292193/2020', '2921930/2020', '2921931/2020', '2921932/2020', '2921933/2020', '2921934/2020', '2921935/2020', '2921936/2020', '2921937/2020', '2921938/2020', '2921939/2020', '292194/2020', '2921940/2020', '2921941/2020', '2921942/2020', '2921943/2020', '2921944/2020', '2921945/2020', '2921946/2020', '2921947/2020', '2921948/2020', '2921949/2020', '292195/2020', '2921950/2020', '2921951/2020', '2921952/2020', '2921953/2020', '2921954/2020', '2921955/2020', '2921956/2020', '2921957/2020', '2921958/2020', '2921959/2020', '292196/2020', '2921960/2020', '2921961/2020', '2921962/2020', '2921963/2020', '2921964/2020', '2921965/2020', '2921966/2020', '2921967/2020', '2921968/2020', '2921969/2020', '292197/2020', '2921970/2020', '2921971/2020', '2921972/2020', '2921973/2020', '2921974/2020', '2921975/2020', '2921976/2020', '2921977/2020', '2921978/2020', '2921979/2020', '292198/2020', '2921980/2020', '2921981/2020', '2921982/2020', '2921983/2020', '2921984/2020', '2921985/2020', '2921986/2020', '2921987/2020', '2921988/2020', '2921989/2020', '292199/2020', '2921990/2020', '2921991/2020', '2921992/2020', '2921993/2019/1', '2921993/2019/A', '2921993/2020', '2921994/2020', '2921995/2020', '2921996/2020', '2921997/2020', '2921998/2020', '2921999/2020', '2922/2020', '29220/2020', '292200/2020', '2922000/2020', '2922001/2020', '2922002/2020', '2922003/2020', '2922004/2020', '2922005/2020', '2922006/2020', '2922007/2020', '2922008/2020', '2922009/2020', '292201/2020', '2922010/2020', '2922011/2020', '2922012/2020', '2922013/2020', '2922014/2020', '2922015/2020', '2922016/2020', '2922017/2020', '2922018/2020', '2922019/2020', '292202/2020', '2922020/2020', '2922021/2020', '2922022/2020', '2922023/2020', '2922024/2020', '2922026/2020', '2922027/2020', '2922028/2020', '2922029/2020', '292203/2020', '2922030/2020', '2922031/2020', '2922032/2020', '2922033/2020', '2922034/2020', '2922035/2020', '2922036/2020', '2922037/2020', '2922038/2020', '2922039/2020', '292204/2020', '2922040/2020', '2922041/2020', '2922042/2020', '2922043/2020', '2922044/2020', '2922045/2020', '2922046/2020', '2922047/2020', '2922048/2020', '2922049/2020', '292205/2020', '2922050/2020', '2922051/2020', '2922052/2020', '2922053/2020', '2922054/2020', '2922055/2020', '2922056/2020', '2922057/2020', '2922058/2020', '2922059/2020', '292206/2020', '2922060/2020', '2922061/2020', '2922062/2020', '2922063/2020', '2922064/2020', '2922065/2020', '2922066/2020', '2922067/2020', '2922068/2020', '2922069/2020', '292207/2020', '2922070/2020', '2922071/2020', '2922072/2020', '2922073/2020', '2922074/2020', '2922075/2020', '2922076/2020', '2922077/2020', '2922078/2020', '2922079/2020', '292208/2020', '2922080/2020', '2922081/2020', '2922082/2020', '2922083/2020', '2922084/2020', '2922085/2020', '2922086/2020', '2922087/2020', '2922088/2020', '2922089/2020', '292209/2020', '2922090/2020', '2922091/2020', '2922092/2020', '2922093/2020', '2922094/2020', '2922095/2020', '2922096/2020', '2922097/2020', '2922098/2020', '2922099/2020', '29221/2020', '292210/2020', '2922100/2020', '2922101/2020', '2922102/2020', '2922103/2020', '2922104/2020', '2922105/2020', '2922106/2020', '2922107/2020', '2922108/2020', '2922109/2020', '292211/2020', '2922110/2020', '2922111/2020', '2922112/2020', '2922113/2020', '2922114/2020', '2922115/2020', '2922116/2020', '2922117/2020', '2922118/2020', '2922119/2020', '292212/2020', '2922120/2020', '2922121/2020', '2922122/2020', '2922123/2020', '2922124/2020', '2922125/2020', '2922126/2020', '2922127/2020', '2922128/2020', '2922129/2020', '292213/2020', '2922130/2020', '2922131/2020', '2922132/2020', '2922133/2020', '2922134/2020', '2922135/2020', '2922136/2020', '2922137/2020', '2922138/2020', '2922139/2020', '292214/2020', '2922140/2020', '2922141/2020', '2922142/2020', '2922143/2020', '2922144/2020', '2922145/2020', '2922146/2020', '2922147/2020', '2922148/2020', '2922149/2020', '292215/2020', '2922150/2020', '2922151/2020', '2922152/2020', '2922153/2020', '2922154/2020', '2922155/2020', '2922156/2020', '2922157/2020', '2922158/2020', '2922159/2020', '292216/2020', '2922160/2020', '2922161/2020', '2922162/2020', '2922163/2020', '2922164/2020', '2922165/2020', '2922166/2020', '2922167/2020', '2922168/2020', '2922169/2020', '2922170/2020', '2922171/2020', '2922172/2020', '2922173/2020', '2922174/2020', '2922175/2020', '2922176/2020', '2922177/2020', '2922178/2020', '2922179/2020', '292218/2020', '2922180/2020', '2922181/2020', '2922182/2020', '2922183/2020', '2922184/2020', '2922185/2020', '2922186/2020', '2922187/2020', '2922188/2020', '2922189/2020', '292219/2020', '2922190/2020', '2922191/2020', '2922192/2020', '2922193/2020', '2922194/2020', '2922195/2020', '2922196/2020', '2922197/2020', '2922198/2020', '2922199/2020', '29222/2020', '292220/2020', '2922200/2020', '2922201/2020', '2922202/2020', '2922203/2020', '2922204/2020', '2922205/2020', '2922206/2020', '2922207/2020', '2922208/2020', '2922209/2020', '292221/2020', '2922210/2020', '2922211/2020', '2922212/2020', '2922213/2020', '2922214/2020', '2922215/2020', '2922216/2020', '2922217/2020', '2922218/2020', '2922219/2020', '292222/2020', '2922220/2020', '2922221/2020', '2922222/2020', '2922223/2020', '2922224/2020', '2922225/2020', '2922226/2020', '2922227/2020', '2922229/2020', '292223/2020', '2922230/2020', '2922231/2020', '2922232/2020', '2922233/2020', '2922234/2020', '2922235/2020', '2922236/2020', '2922237/2020', '2922238/2020', '2922239/2020', '292224/2020', '2922240/2020', '2922241/2020', '2922242/2020', '2922243/2020', '2922244/2020', '2922245/2020', '2922246/2020', '2922247/2020', '2922248/2020', '2922249/2020', '292225/2020', '2922250/2020', '2922251/2020', '2922252/2020', '2922253/2020', '2922254/2020', '2922255/2020', '2922256/2020', '2922257/2020', '2922258/2020', '2922259/2020', '292226/2020', '2922260/2020', '2922261/2020', '2922262/2020', '2922263/2020', '2922264/2020', '2922265/2020', '2922266/2020', '2922267/2020', '2922268/2020', '2922269/2020', '292227/2020', '2922270/2020', '2922271/2020', '2922272/2020', '2922273/2020', '2922274/2020', '2922275/2020', '2922276/2020', '2922277/2020', '2922278/2020', '2922279/2020', '292228/2020', '2922280/2020', '2922281/2020', '2922282/2020', '2922283/2020', '2922284/2020', '2922285/2020', '2922286/2020', '2922287/2020', '2922288/2020', '2922289/2020', '292229/2020', '2922290/2020', '2922291/2020', '2922292/2020', '2922293/2020', '2922294/2020', '2922295/2020', '2922296/2020', '2922297/2020', '2922298/2020', '2922299/2020', '29223/2020', '292230/2020', '2922300/2020', '2922301/2020', '2922302/2020', '2922303/2020', '2922304/2020', '2922305/2020', '2922306/2020', '2922307/2020', '2922308/2020', '2922309/2020', '292231/2020', '2922310/2020', '2922311/2020', '2922312/2020', '2922313/2020', '2922314/2020', '2922315/2020', '2922316/2020', '2922317/2020', '2922318/2020', '2922319/2020', '292232/2020', '2922320/2020', '2922321/2020', '2922322/2020', '2922323/2020', '2922324/2020', '2922325/2020', '2922326/2020', '2922327/2020', '2922328/2020', '2922329/2020', '292233/2020', '2922330/2020', '2922331/2020', '2922332/2020', '2922333/2020', '2922334/2020', '2922335/2020', '2922336/2020', '2922337/2020', '2922338/2020', '2922339/2020', '292234/2020', '2922340/2020', '2922341/2020', '2922342/2020', '2922343/2020', '2922344/2020', '2922345/2020', '2922346/2020', '2922347/2020', '2922348/2020', '2922349/2020', '292235/2020', '2922350/2020', '2922351/2020', '2922352/2020', '2922353/2020', '2922354/2020', '2922355/2020', '2922356/2020', '2922357/2020', '2922358/2020', '2922359/2020', '292236/2020', '2922360/2020', '2922361/2020', '2922362/2020', '2922363/2020', '2922364/2020', '2922365/2020', '2922366/2020', '2922367/2020', '2922368/2020', '2922369/2020', '292237/2020', '2922370/2020', '2922371/2020', '2922372/2020', '2922373/2020', '2922374/2020', '2922375/2020', '2922376/2020', '2922377/2020', '2922378/2020', '2922379/2020', '292238/2020', '2922380/2020', '2922381/2020', '2922382/2020', '2922383/2020', '2922384/2020', '2922385/2020', '2922386/2020', '2922387/2020', '2922388/2020', '2922389/2020', '292239/2017/A', '292239/2020', '2922390/2020', '2922391/2020', '2922392/2020', '2922393/2020', '2922394/2020', '2922395/2020', '2922396/2020', '2922397/2020', '2922398/2020', '2922399/2020', '29224/2020', '292240/2020', '292240/2020/A', '2922400/2020', '2922401/2020', '2922402/2020', '2922403/2020', '2922404/2020', '2922405/2020', '2922406/2020', '2922407/2020', '2922408/2020', '2922409/2020', '292241/2020', '2922410/2020', '2922411/2020', '2922412/2020', '2922413/2020', '2922414/2020', '2922415/2020', '2922416/2020', '2922417/2020', '2922418/2020', '2922419/2020', '292242/2020', '2922420/2020', '2922421/2020', '2922422/2020', '2922423/2020', '2922424/2020', '2922425/2020', '2922426/2020', '2922427/2020', '2922428/2020', '2922429/2020', '292243/2020', '2922430/2020', '2922431/2020', '2922432/2020', '2922433/2020', '2922434/2020', '2922435/2020', '2922436/2020', '2922437/2020', '2922438/2020', '2922439/2020', '292244/2020', '2922440/2020', '2922441/2020', '2922442/2020', '2922443/2020', '2922444/2020', '2922445/2020', '2922446/2020', '2922447/2020', '2922448/2020', '2922449/2020', '292245/2020', '2922450/2020', '2922451/2020', '2922452/2020', '2922453/2020', '2922454/2020', '2922455/2020', '2922456/2020', '2922457/2020', '2922458/2020', '2922459/2020', '292246/2020', '2922460/2020', '2922461/2020', '2922462/2020', '2922463/2020', '2922464/2020', '2922465/2020', '2922466/2020', '2922467/2020', '2922468/2020', '2922469/2020', '292247/2020', '2922470/2020', '2922471/2020', '2922472/2020', '2922473/2020', '2922474/2020', '2922475/2020', '2922476/2020', '2922477/2020', '2922478/2020', '2922479/2020', '292248/2020', '2922480/2020', '2922481/2020', '2922482/2020', '2922483/2020', '2922484/2020', '2922485/2020', '2922486/2020', '2922487/2020', '2922488/2020', '2922489/2020', '292249/2020', '2922490/2020', '2922491/2020', '2922492/2020', '2922493/2020', '2922494/2020', '2922495/2020', '2922496/2020', '2922497/2020', '2922498/2020', '2922499/2020', '29225/2020', '292250/2020', '2922500/2020', '2922501/2020', '2922502/2020', '2922503/2020', '2922504/2020', '2922505/2020', '2922506/2020', '2922507/2020', '2922508/2020', '2922509/2020', '292251/2020', '2922510/2020', '2922511/2020', '2922512/2020', '2922513/2020', '2922514/2020', '2922515/2020', '2922516/2020', '2922517/2020', '2922518/2020', '2922519/2020', '292252/2020', '2922520/2020', '2922521/2020', '2922522/2020', '2922523/2020', '2922524/2020', '2922525/2020', '2922526/2020', '2922527/2020', '2922528/2020', '2922529/2020', '292253/2020', '2922530/2020', '2922531/2020', '2922532/2020', '2922533/2020', '2922534/2020', '2922535/2020', '2922536/2020', '2922537/2020', '2922538/2020', '2922539/2020', '292254/2020', '2922540/2020', '2922541/2020', '2922542/2020', '2922543/2020', '2922544/2020', '2922545/2020', '2922546/2020', '2922547/2020', '2922548/2020', '2922549/2020', '292255/2020', '2922550/2020', '2922551/2020', '2922552/2020', '2922553/2020', '2922554/2020', '2922555/2020', '2922556/2020', '2922557/2020', '2922558/2020', '2922559/2020', '292256/2020', '2922560/2020', '2922561/2020', '2922562/2020', '2922563/2020', '2922564/2020', '2922565/2020', '2922566/2020', '2922567/2020', '2922568/2020', '2922569/2020', '292257/2020', '2922570/2020', '2922571/2020', '2922572/2020', '2922573/2020', '2922574/2020', '2922575/2020', '2922576/2020', '2922577/2020', '2922578/2020', '2922579/2020', '292258/2020', '2922580/2020', '2922581/2020', '2922582/2020', '2922583/2020', '2922584/2020', '2922585/2020', '2922586/2020', '2922587/2020', '2922588/2020', '2922589/2020', '292259/2020', '2922590/2020', '2922591/2020', '2922592/2020', '2922593/2020', '2922594/2020', '2922595/2020', '2922596/2020', '2922597/2020', '2922598/2020', '2922599/2020', '29226/2020', '292260/2020', '2922600/2020', '2922601/2020', '2922602/2020', '2922603/2020', '2922604/2020', '2922605/2020', '2922606/2020', '2922607/2020', '2922608/2020', '2922609/2020', '292261/2020', '2922610/2020', '2922611/2020', '2922612/2020', '2922613/2020', '2922614/2020', '2922615/2020', '2922616/2020', '2922617/2020', '2922618/2020', '2922619/2020', '292262/2020', '2922620/2020', '2922621/2020', '2922622/2020', '2922623/2020', '2922624/2020', '2922625/2020', '2922626/2020', '2922627/2020', '2922628/2020', '2922629/2020', '292263/2020', '2922630/2020', '2922631/2020', '2922632/2020', '2922633/2020', '2922634/2020', '2922635/2020', '2922636/2020', '2922637/2020', '292264/2020', '292265/2020', '292266/2020', '292267/2020', '292268/2020', '292269/2020', '29227/2020', '292270/2020', '292271/2020', '292272/2020', '292273/2020', '292274/2020', '292275/2020', '292276/2020', '292277/2020', '292278/2020', '292279/2020', '29228/2020', '292280/2020', '292281/2020', '292282/2020', '292283/2020', '292284/2020', '292286/2020', '292287/2020', '292288/2016/2', '292288/2016/3', '292289/2020', '29229/2020', '292290/2016/1/C', '292290/2020', '292291/2020', '292292/2020', '292293/2020', '292294/2020', '292295/2020', '292296/2020', '292297/2020', '292298/2020', '292299/2019/A', '292299/2020', '2923/2020', '292300/2020', '292301/2020', '292302/2020', '292303/2020', '292304/2020', '292305/2020', '292306/2020', '292307/2020', '292308/2020', '292309/2020', '292310/2020', '292311/2020', '292312/2018/2', '292312/2020', '292313/2020', '292314/2020', '292315/2020', '292316/2020', '292317/2020', '292318/2020', '292319/2020', '29232/2020', '292320/2020', '292321/2020', '292322/2020', '292323/2020', '292324/2020', '292325/2020', '292326/2020', '292327/2020', '292328/2020', '292329/2020', '29233/2020', '292330/2020', '292331/2020', '292332/2020', '292333/2020', '292334/2020', '292335/2020', '292336/2020', '292337/2020', '292338/2020', '292338/2020/1', '292338/2020/2', '292339/2020', '29234/2020', '292340/2020', '292341/2020', '292341/2020/A', '292342/2020', '292343/2020', '292344/2020', '292345/2020', '292346/2020', '292347/2020', '292348/2019/1', '292348/2019/2', '292348/2020', '292349/2020', '29235/2020', '292350/2020', '292351/2020', '292352/2020', '292353/2020', '292354/2020', '292355/2020', '292356/2020', '292357/2020', '292358/2019/1/A', '292358/2020', '292359/2020', '29236/2018/A', '29236/2020', '292360/2020', '292361/2020', '292362/2020', '292363/2020', '292364/2020', '292365/2020', '292366/2020', '292367/2020', '292368/2020', '292369/2020', '29237/2020', '292370/2020', '292371/2020', '292372/2020', '292373/2020', '292374/2020', '292375/2020', '292376/2020', '292378/2020', '292379/2020', '29238/2020', '292380/2020', '292381/2020', '292382/2020', '292383/2020', '292384/2020', '292385/2020', '292386/2020', '292387/2020', '292388/2020', '292389/2020', '29239/2020', '292390/2020', '292391/2020', '292392/2020', '292393/2020', '292394/2020', '292395/2020', '292396/2020', '292397/2020', '292398/2020', '292399/2020', '2924/2020', '29240/2020', '292400/2007/A', '292400/2020', '292401/2020', '292402/2020', '292403/2020', '292404/2020', '292405/2020', '292406/2020', '292407/2020', '292408/2020', '292409/2020', '29241/2020', '292410/2020', '292411/2020', '292412/2020', '292413/2020', '292414/2020', '292415/2020', '292416/2020', '292417/2020', '292418/2020', '292419/2020', '29242/2020', '292420/2020', '292421/2020', '292422/2020', '292423/2020', '292424/2020', '292426/2020', '292427/2020', '292428/2020', '292429/2020', '29243/2020', '292430/2020', '292431/2020', </t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -707,7 +707,7 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>25/11/2020 12:00:00 AM</t>
+          <t>5/12/2020 12:00:00 AM</t>
         </is>
       </c>
       <c r="T3" t="n">
@@ -725,14 +725,14 @@
         <v>0</v>
       </c>
       <c r="X3" t="n">
-        <v>56360</v>
+        <v>63073</v>
       </c>
       <c r="Y3" t="n">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>['1/04/2020 12:00:00 AM', '1/05/2020 12:00:00 AM', '1/06/2020 12:00:00 AM', '1/07/2020 12:00:00 AM', '1/09/2020 12:00:00 AM', '1/10/2020 12:00:00 AM', '10/01/2020 12:00:00 AM', '10/02/2020 12:00:00 AM', '10/03/2020 12:00:00 AM', '10/06/2020 12:00:00 AM', '10/07/2020 12:00:00 AM', '10/08/2020 12:00:00 AM', '10/09/2020 12:00:00 AM', '10/11/2020 12:00:00 AM', '11/02/2020 12:00:00 AM', '11/03/2020 12:00:00 AM', '11/05/2020 12:00:00 AM', '11/06/2020 12:00:00 AM', '11/08/2020 12:00:00 AM', '11/09/2020 12:00:00 AM', '11/11/2020 12:00:00 AM', '12/02/2020 12:00:00 AM', '12/03/2020 12:00:00 AM', '12/05/2020 12:00:00 AM', '12/06/2020 12:00:00 AM', '12/08/2020 12:00:00 AM', '12/09/2020 12:00:00 AM', '12/10/2020 12:00:00 AM', '12/11/2020 12:00:00 AM', '13/01/2020 12:00:00 AM', '13/02/2020 12:00:00 AM', '13/03/2020 12:00:00 AM', '13/05/2020 12:00:00 AM', '13/07/2020 12:00:00 AM', '13/08/2020 12:00:00 AM', '13/10/2020 12:00:00 AM', '13/11/2020 12:00:00 AM', '14/01/2020 12:00:00 AM', '14/02/2020 12:00:00 AM', '14/04/2020 12:00:00 AM', '14/05/2020 12:00:00 AM', '14/07/2020 12:00:00 AM', '14/08/2020 12:00:00 AM', '14/09/2020 12:00:00 AM', '14/10/2020 12:00:00 AM', '15/01/2020 12:00:00 AM', '15/04/2020 12:00:00 AM', '15/05/2020 12:00:00 AM', '15/06/2020 12:00:00 AM', '15/07/2020 12:00:00 AM', '15/08/2020 12:00:00 AM', '15/09/2020 12:00:00 AM', '15/10/2020 12:00:00 AM', '16/01/2020 12:00:00 AM', '16/03/2020 12:00:00 AM', '16/04/2020 12:00:00 AM', '16/06/2020 12:00:00 AM', '16/07/2020 12:00:00 AM', '16/09/2020 12:00:00 AM', '16/10/2020 12:00:00 AM', '16/11/2020 12:00:00 AM', '17/01/2020 12:00:00 AM', '17/02/2020 12:00:00 AM', '17/03/2020 12:00:00 AM', '17/04/2020 12:00:00 AM', '17/05/2020 12:00:00 AM', '17/06/2020 12:00:00 AM', '17/07/2020 12:00:00 AM', '17/08/2020 12:00:00 AM', '17/09/2020 12:00:00 AM', '17/10/2020 12:00:00 AM', '17/11/2020 12:00:00 AM', '18/02/2020 12:00:00 AM', '18/03/2020 12:00:00 AM', '18/05/2020 12:00:00 AM', '18/06/2020 12:00:00 AM', '18/08/2020 12:00:00 AM', '18/09/2020 12:00:00 AM', '18/11/2020 12:00:00 AM', '19/02/2020 12:00:00 AM', '19/03/2020 12:00:00 AM', '19/05/2020 12:00:00 AM', '19/06/2020 12:00:00 AM', '19/07/2020 12:00:00 AM', '19/08/2020 12:00:00 AM', '19/10/2020 12:00:00 AM', '19/11/2020 12:00:00 AM', '2/01/2020 12:00:00 AM', '2/03/2020 12:00:00 AM', '2/04/2020 12:00:00 AM', '2/06/2020 12:00:00 AM', '2/07/2020 12:00:00 AM', '2/08/2020 12:00:00 AM', '2/09/2020 12:00:00 AM', '2/10/2020 12:00:00 AM', '2/11/2020 12:00:00 AM', '20/01/2020 12:00:00 AM', '20/02/2020 12:00:00 AM', '20/03/2020 12:00:00 AM', '20/04/2020 12:00:00 AM', '20/05/2020 12:00:00 AM', '20/07/2020 12:00:00 AM', '20/08/2020 12:00:00 AM', '20/10/2020 12:00:00 AM', '21/01/2020 12:00:00 AM', '21/02/2020 12:00:00 AM', '21/03/2020 12:00:00 AM', '21/04/2020 12:00:00 AM', '21/05/2020 12:00:00 AM', '21/06/2020 12:00:00 AM', '21/07/2020 12:00:00 AM', '21/08/2020 12:00:00 AM', '21/09/2020 12:00:00 AM', '21/10/2020 12:00:00 AM', '22/01/2020 12:00:00 AM', '22/04/2020 12:00:00 AM', '22/05/2020 12:00:00 AM', '22/06/2020 12:00:00 AM', '22/07/2020 12:00:00 AM', '22/08/2020 12:00:00 AM', '22/09/2020 12:00:00 AM', '22/10/2020 12:00:00 AM', '23/01/2020 12:00:00 AM', '23/02/2020 12:00:00 AM', '23/03/2020 12:00:00 AM', '23/04/2020 12:00:00 AM', '23/06/2020 12:00:00 AM', '23/07/2020 12:00:00 AM', '23/09/2020 12:00:00 AM', '23/10/2020 12:00:00 AM', '23/11/2020 12:00:00 AM', '24/01/2020 12:00:00 AM', '24/02/2020 12:00:00 AM', '24/03/2020 12:00:00 AM', '24/04/2020 12:00:00 AM', '24/06/2020 12:00:00 AM', '24/07/2020 12:00:00 AM', '24/08/2020 12:00:00 AM', '24/09/2020 12:00:00 AM', '24/11/2020 12:00:00 AM', '25/02/2020 12:00:00 AM', '25/03/2020 12:00:00 AM', '25/05/2020 12:00:00 AM', '25/06/2020 12:00:00 AM', '25/08/2020 12:00:00 AM', '25/09/2020 12:00:00 AM', '25/11/2020 12:00:00 AM', '26/02/2020 12:00:00 AM', '26/03/2020 12:00:00 AM', '26/05/2020 12:00:00 AM', '26/06/2020 12:00:00 AM', '26/07/2020 12:00:00 AM', '26/08/2020 12:00:00 AM', '26/10/2020 12:00:00 AM', '26/11/2020 12:00:00 AM', '27/02/2020 12:00:00 AM', '27/03/2020 12:00:00 AM', '27/04/2020 12:00:00 AM', '27/05/2020 12:00:00 AM', '27/07/2020 12:00:00 AM', '27/08/2020 12:00:00 AM', '27/10/2020 12:00:00 AM', '28/01/2020 12:00:00 AM', '28/02/2020 12:00:00 AM', '28/04/2020 12:00:00 AM', '28/05/2020 12:00:00 AM', '28/07/2020 12:00:00 AM', '28/08/2020 12:00:00 AM', '28/09/2020 12:00:00 AM', '28/10/2020 12:00:00 AM', '29/01/2020 12:00:00 AM', '29/04/2020 12:00:00 AM', '29/05/2020 12:00:00 AM', '29/06/2020 12:00:00 AM', '29/07/2020 12:00:00 AM', '29/09/2020 12:00:00 AM', '29/10/2020 12:00:00 AM', '3/01/2020 12:00:00 AM', '3/02/2020 12:00:00 AM', '3/03/2020 12:00:00 AM', '3/04/2020 12:00:00 AM', '3/05/2020 12:00:00 AM', '3/06/2020 12:00:00 AM', '3/07/2020 12:00:00 AM', '3/08/2020 12:00:00 AM', '3/09/2020 12:00:00 AM', '3/11/2020 12:00:00 AM', '30/01/2020 12:00:00 AM', '30/03/2020 12:00:00 AM', '30/04/2020 12:00:00 AM', '30/05/2020 12:00:00 AM', '30/06/2020 12:00:00 AM', '30/07/2020 12:00:00 AM', '30/09/2020 12:00:00 AM', '30/10/2020 12:00:00 AM', '31/01/2020 12:00:00 AM', '31/03/2020 12:00:00 AM', '31/07/2020 12:00:00 AM', '31/08/2020 12:00:00 AM', '4/02/2020 12:00:00 AM', '4/03/2020 12:00:00 AM', '4/05/2020 12:00:00 AM', '4/06/2020 12:00:00 AM', '4/08/2020 12:00:00 AM', '4/09/2020 12:00:00 AM', '4/10/2020 12:00:00 AM', '4/11/2020 12:00:00 AM', '5/02/2020 12:00:00 AM', '5/03/2020 12:00:00 AM', '5/05/2020 12:00:00 AM', '5/06/2020 12:00:00 AM', '5/08/2020 12:00:00 AM', '5/11/2020 12:00:00 AM', '6/01/2020 12:00:00 AM', '6/02/2020 12:00:00 AM', '6/03/2020 12:00:00 AM', '6/04/2020 12:00:00 AM', '6/05/2020 12:00:00 AM', '6/06/2020 12:00:00 AM', '6/07/2020 12:00:00 AM', '6/08/2020 12:00:00 AM', '6/10/2020 12:00:00 AM', '6/11/2020 12:00:00 AM', '7/01/2020 12:00:00 AM', '7/02/2020 12:00:00 AM', '7/04/2020 12:00:00 AM', '7/05/2020 12:00:00 AM', '7/07/2020 12:00:00 AM', '7/08/2020 12:00:00 AM', '7/09/2020 12:00:00 AM', '7/10/2020 12:00:00 AM', '8/01/2020 12:00:00 AM', '8/04/2020 12:00:00 AM', '8/05/2020 12:00:00 AM', '8/07/2020 12:00:00 AM', '8/08/2020 12:00:00 AM', '8/09/2020 12:00:00 AM', '8/10/2020 12:00:00 AM', '9/01/2020 12:00:00 AM', '9/03/2020 12:00:00 AM', '9/04/2020 12:00:00 AM', '9/06/2020 12:00:00 AM', '9/07/2020 12:00:00 AM', '9/09/2020 12:00:00 AM', '9/10/2020 12:00:00 AM', '9/11/2020 12:00:00 AM']</t>
+          <t>['1/04/2020 12:00:00 AM', '1/05/2020 12:00:00 AM', '1/06/2020 12:00:00 AM', '1/07/2020 12:00:00 AM', '1/09/2020 12:00:00 AM', '1/10/2020 12:00:00 AM', '1/12/2020 12:00:00 AM', '10/01/2020 12:00:00 AM', '10/02/2020 12:00:00 AM', '10/03/2020 12:00:00 AM', '10/06/2020 12:00:00 AM', '10/07/2020 12:00:00 AM', '10/08/2020 12:00:00 AM', '10/09/2020 12:00:00 AM', '10/11/2020 12:00:00 AM', '10/12/2020 12:00:00 AM', '11/02/2020 12:00:00 AM', '11/03/2020 12:00:00 AM', '11/05/2020 12:00:00 AM', '11/06/2020 12:00:00 AM', '11/08/2020 12:00:00 AM', '11/09/2020 12:00:00 AM', '11/11/2020 12:00:00 AM', '11/12/2020 12:00:00 AM', '12/02/2020 12:00:00 AM', '12/03/2020 12:00:00 AM', '12/05/2020 12:00:00 AM', '12/06/2020 12:00:00 AM', '12/08/2020 12:00:00 AM', '12/09/2020 12:00:00 AM', '12/10/2020 12:00:00 AM', '12/11/2020 12:00:00 AM', '13/01/2020 12:00:00 AM', '13/02/2020 12:00:00 AM', '13/03/2020 12:00:00 AM', '13/05/2020 12:00:00 AM', '13/07/2020 12:00:00 AM', '13/08/2020 12:00:00 AM', '13/10/2020 12:00:00 AM', '13/11/2020 12:00:00 AM', '14/01/2020 12:00:00 AM', '14/02/2020 12:00:00 AM', '14/04/2020 12:00:00 AM', '14/05/2020 12:00:00 AM', '14/07/2020 12:00:00 AM', '14/08/2020 12:00:00 AM', '14/09/2020 12:00:00 AM', '14/10/2020 12:00:00 AM', '14/12/2020 12:00:00 AM', '15/01/2020 12:00:00 AM', '15/04/2020 12:00:00 AM', '15/05/2020 12:00:00 AM', '15/06/2020 12:00:00 AM', '15/07/2020 12:00:00 AM', '15/08/2020 12:00:00 AM', '15/09/2020 12:00:00 AM', '15/10/2020 12:00:00 AM', '15/12/2020 12:00:00 AM', '16/01/2020 12:00:00 AM', '16/03/2020 12:00:00 AM', '16/04/2020 12:00:00 AM', '16/06/2020 12:00:00 AM', '16/07/2020 12:00:00 AM', '16/09/2020 12:00:00 AM', '16/10/2020 12:00:00 AM', '16/11/2020 12:00:00 AM', '16/12/2020 12:00:00 AM', '17/01/2020 12:00:00 AM', '17/02/2020 12:00:00 AM', '17/03/2020 12:00:00 AM', '17/04/2020 12:00:00 AM', '17/05/2020 12:00:00 AM', '17/06/2020 12:00:00 AM', '17/07/2020 12:00:00 AM', '17/08/2020 12:00:00 AM', '17/09/2020 12:00:00 AM', '17/10/2020 12:00:00 AM', '17/11/2020 12:00:00 AM', '17/12/2020 12:00:00 AM', '18/02/2020 12:00:00 AM', '18/03/2020 12:00:00 AM', '18/05/2020 12:00:00 AM', '18/06/2020 12:00:00 AM', '18/08/2020 12:00:00 AM', '18/09/2020 12:00:00 AM', '18/11/2020 12:00:00 AM', '18/12/2020 12:00:00 AM', '19/02/2020 12:00:00 AM', '19/03/2020 12:00:00 AM', '19/05/2020 12:00:00 AM', '19/06/2020 12:00:00 AM', '19/07/2020 12:00:00 AM', '19/08/2020 12:00:00 AM', '19/10/2020 12:00:00 AM', '19/11/2020 12:00:00 AM', '2/01/2020 12:00:00 AM', '2/03/2020 12:00:00 AM', '2/04/2020 12:00:00 AM', '2/06/2020 12:00:00 AM', '2/07/2020 12:00:00 AM', '2/08/2020 12:00:00 AM', '2/09/2020 12:00:00 AM', '2/10/2020 12:00:00 AM', '2/11/2020 12:00:00 AM', '2/12/2020 12:00:00 AM', '20/01/2020 12:00:00 AM', '20/02/2020 12:00:00 AM', '20/03/2020 12:00:00 AM', '20/04/2020 12:00:00 AM', '20/05/2020 12:00:00 AM', '20/07/2020 12:00:00 AM', '20/08/2020 12:00:00 AM', '20/10/2020 12:00:00 AM', '21/01/2020 12:00:00 AM', '21/02/2020 12:00:00 AM', '21/03/2020 12:00:00 AM', '21/04/2020 12:00:00 AM', '21/05/2020 12:00:00 AM', '21/06/2020 12:00:00 AM', '21/07/2020 12:00:00 AM', '21/08/2020 12:00:00 AM', '21/09/2020 12:00:00 AM', '21/10/2020 12:00:00 AM', '21/12/2020 12:00:00 AM', '22/01/2020 12:00:00 AM', '22/04/2020 12:00:00 AM', '22/05/2020 12:00:00 AM', '22/06/2020 12:00:00 AM', '22/07/2020 12:00:00 AM', '22/08/2020 12:00:00 AM', '22/09/2020 12:00:00 AM', '22/10/2020 12:00:00 AM', '22/12/2020 12:00:00 AM', '23/01/2020 12:00:00 AM', '23/02/2020 12:00:00 AM', '23/03/2020 12:00:00 AM', '23/04/2020 12:00:00 AM', '23/06/2020 12:00:00 AM', '23/07/2020 12:00:00 AM', '23/09/2020 12:00:00 AM', '23/10/2020 12:00:00 AM', '23/11/2020 12:00:00 AM', '23/12/2020 12:00:00 AM', '24/01/2020 12:00:00 AM', '24/02/2020 12:00:00 AM', '24/03/2020 12:00:00 AM', '24/04/2020 12:00:00 AM', '24/06/2020 12:00:00 AM', '24/07/2020 12:00:00 AM', '24/08/2020 12:00:00 AM', '24/09/2020 12:00:00 AM', '24/11/2020 12:00:00 AM', '25/02/2020 12:00:00 AM', '25/03/2020 12:00:00 AM', '25/05/2020 12:00:00 AM', '25/06/2020 12:00:00 AM', '25/08/2020 12:00:00 AM', '25/09/2020 12:00:00 AM', '25/11/2020 12:00:00 AM', '26/02/2020 12:00:00 AM', '26/03/2020 12:00:00 AM', '26/05/2020 12:00:00 AM', '26/06/2020 12:00:00 AM', '26/07/2020 12:00:00 AM', '26/08/2020 12:00:00 AM', '26/10/2020 12:00:00 AM', '26/11/2020 12:00:00 AM', '27/02/2020 12:00:00 AM', '27/03/2020 12:00:00 AM', '27/04/2020 12:00:00 AM', '27/05/2020 12:00:00 AM', '27/07/2020 12:00:00 AM', '27/08/2020 12:00:00 AM', '27/10/2020 12:00:00 AM', '27/11/2020 12:00:00 AM', '28/01/2020 12:00:00 AM', '28/02/2020 12:00:00 AM', '28/04/2020 12:00:00 AM', '28/05/2020 12:00:00 AM', '28/07/2020 12:00:00 AM', '28/08/2020 12:00:00 AM', '28/09/2020 12:00:00 AM', '28/10/2020 12:00:00 AM', '29/01/2020 12:00:00 AM', '29/04/2020 12:00:00 AM', '29/05/2020 12:00:00 AM', '29/06/2020 12:00:00 AM', '29/07/2020 12:00:00 AM', '29/09/2020 12:00:00 AM', '29/10/2020 12:00:00 AM', '3/01/2020 12:00:00 AM', '3/02/2020 12:00:00 AM', '3/03/2020 12:00:00 AM', '3/04/2020 12:00:00 AM', '3/05/2020 12:00:00 AM', '3/06/2020 12:00:00 AM', '3/07/2020 12:00:00 AM', '3/08/2020 12:00:00 AM', '3/09/2020 12:00:00 AM', '3/11/2020 12:00:00 AM', '3/12/2020 12:00:00 AM', '30/01/2020 12:00:00 AM', '30/03/2020 12:00:00 AM', '30/04/2020 12:00:00 AM', '30/05/2020 12:00:00 AM', '30/06/2020 12:00:00 AM', '30/07/2020 12:00:00 AM', '30/09/2020 12:00:00 AM', '30/10/2020 12:00:00 AM', '30/11/2020 12:00:00 AM', '31/01/2020 12:00:00 AM', '31/03/2020 12:00:00 AM', '31/07/2020 12:00:00 AM', '31/08/2020 12:00:00 AM', '4/02/2020 12:00:00 AM', '4/03/2020 12:00:00 AM', '4/05/2020 12:00:00 AM', '4/06/2020 12:00:00 AM', '4/08/2020 12:00:00 AM', '4/09/2020 12:00:00 AM', '4/10/2020 12:00:00 AM', '4/11/2020 12:00:00 AM', '4/12/2020 12:00:00 AM', '5/02/2020 12:00:00 AM', '5/03/2020 12:00:00 AM', '5/05/2020 12:00:00 AM', '5/06/2020 12:00:00 AM', '5/08/2020 12:00:00 AM', '5/11/2020 12:00:00 AM', '5/12/2020 12:00:00 AM', '6/01/2020 12:00:00 AM', '6/02/2020 12:00:00 AM', '6/03/2020 12:00:00 AM', '6/04/2020 12:00:00 AM', '6/05/2020 12:00:00 AM', '6/06/2020 12:00:00 AM', '6/07/2020 12:00:00 AM', '6/08/2020 12:00:00 AM', '6/10/2020 12:00:00 AM', '6/11/2020 12:00:00 AM', '7/01/2020 12:00:00 AM', '7/02/2020 12:00:00 AM', '7/04/2020 12:00:00 AM', '7/05/2020 12:00:00 AM', '7/07/2020 12:00:00 AM', '7/08/2020 12:00:00 AM', '7/09/2020 12:00:00 AM', '7/10/2020 12:00:00 AM', '7/12/2020 12:00:00 AM', '8/01/2020 12:00:00 AM', '8/04/2020 12:00:00 AM', '8/05/2020 12:00:00 AM', '8/07/2020 12:00:00 AM', '8/08/2020 12:00:00 AM', '8/09/2020 12:00:00 AM', '8/10/2020 12:00:00 AM', '8/12/2020 12:00:00 AM', '9/01/2020 12:00:00 AM', '9/03/2020 12:00:00 AM', '9/04/2020 12:00:00 AM', '9/06/2020 12:00:00 AM', '9/07/2020 12:00:00 AM', '9/09/2020 12:00:00 AM', '9/10/2020 12:00:00 AM', '9/11/2020 12:00:00 AM', '9/12/2020 12:00:00 AM']</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -784,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="O4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
@@ -799,7 +799,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Ms T L Pascoe</t>
+          <t>Mr A D Wallis</t>
         </is>
       </c>
       <c r="T4" t="n">
@@ -811,20 +811,20 @@
         </is>
       </c>
       <c r="V4" t="n">
-        <v>384</v>
+        <v>451</v>
       </c>
       <c r="W4" t="n">
         <v>0</v>
       </c>
       <c r="X4" t="n">
-        <v>55385</v>
+        <v>62840</v>
       </c>
       <c r="Y4" t="n">
-        <v>841</v>
+        <v>907</v>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>['365 Studio Pty Ltd', '3MT Solutions Pty Ltd', '41 Barfield Pty Ltd', '43 Barfield Pty Ltd', 'A Asteris', 'A Bragg', 'A Horn', 'A L Russell', 'A Morgado', 'A Robertson', 'A Sapic', 'A Sharma', 'A Smith', 'A Tebyanyan', 'A V Jennings', 'A V Jennings Pty Ltd', 'A Valiff', 'AAT Building', 'ABC Homes Pty Ltd', 'AH Design &amp; Drafting', 'APM Plumbing', 'Access SDM Pty Ltd', 'Actium Land Developments Pty Ltd', 'Adelaide Builders Pty Ltd', 'Adelaide Building Consulting', 'Adelaide Designer Homes Pty Ltd', 'Adelaide Insurance Builders', 'Adelaide Nominees Pty Ltd', 'Adelaide Retaining Walls', 'Aerobic Tech Pty Ltd', 'Ahrens Engineering', 'Albury Wodonga Community College', 'Aldinga Home Improvements', 'Alete Homes Pty Ltd', 'Alexander Symonds Pty Ltd', 'Alif Homes', 'All Sites Welding Services', 'Alpha Industries', 'Alpha Industries - Glandore', 'Andrash Commercial Pty Ltd', 'Andrew Evans Plumbing', 'Anglicare SA Housing Ltd', 'Anthony Donato Architects', 'Apalie Drive Pty Ltd', 'Apex Greenhouses', 'Apex Greenhouses Aust Pty Ltd', 'Apex Home Improvements', 'Aspire Homes SA Pty Ltd', 'Astrad Pty Ltd', 'Atelier 18 Pty Ltd', 'Attica Homes', 'Aust Child Care Career', 'Aust Outdoor Living', 'Australian Building Company', 'Australian Outdoor Living', 'Australian Workplace Training', 'B A Mebberson', 'B Cox', 'B Goyal', 'B Pring', 'B Thomas and Bargain Steel Centre', 'B Van Groesen', 'Ballavarra Pty Ltd', 'Baracuda Holdings Pty Ltd', 'Bargain Steel Centre', 'Barossa Pergolas &amp; Outdoor Concepts', 'Beechwood Homes', 'Bella Build &amp; Design', 'Better Built Industries', 'Big Difference Home Improvement', 'Botanic Dreams Pty Ltd', 'Bovpap Pty Ltd', 'Bradford Homes', 'Brightspace Homes', 'Brookmont Property Developments Pty Ltd', 'Brooks Development Services', 'Brooks Development Services Pty Ltd', 'Budget Built Home Additions', 'Burbank Aust (SA) Pty Ltd', 'Burton Demolition Pty Ltd', 'C Biven', 'C Grimaldi', 'C Liebeknecht', 'C Stevenson', 'C Stock', 'C Yu', 'CT Group Properties No 4 Pty Ltd', 'Cafcakis Nominees and Mr E Cafcakis', 'Catholic Archdiocese of Adelaide', 'Century North Pty Ltd', 'Changhui Construction Pty Ltd', 'Checkpoint Building Surveyors', 'City of Playford', 'City of Playford Sports &amp; Property Team', 'Classic Pools &amp; Spas', 'Cocercan Pty Ltd', 'Colcon (NT) Pty Ltd', 'Collins Adelaide', 'Collins Transport', 'Comfresh Pty Ltd', 'Construction Services Aust Pty Ltd', 'Creative Outdoors', 'Crisio Investments Pty Ltd', 'D Clarke', 'D Harris', 'D Lobbe', 'D Martyr', 'D Rawat', 'D Turnbull', 'D W Rogers', 'D2c Services', 'DMV Outdoor Solutions', 'DPTI Rail Commissioner', 'Dechellis Homes', 'Department for Education', 'Department for Education - Das Studio', 'Department of Education/Tesa', 'Dept for Infrastructure &amp; Transport', 'Design Constructive Pty Ltd', 'Detail Studio Pty Ltd', 'Diamanti Design Development', 'Dimension Design Studio', 'Distinctive Homes Pty Ltd', 'Dominion Homes', 'Drug &amp; Alcohol Services SA', 'E Bidhendi', 'Elite Pools &amp; Landscapes', 'Elizabeth RSL', 'Emmett Property Pty Ltd', 'Everclear Pool Solutions', 'Exquisite Brows Pty Ltd', 'F Ahmadi', 'Faculty Design', 'Fairland Homes Group Pty Ltd', 'Fairmont Homes Group Pty Ltd', 'Fairmont Land Holdings Pty Ltd', 'Farrago Interiors', 'First Choice Verandahs &amp; Carports', 'Format Homes Pty Ltd', 'Fortune Living', 'Frank Nesci Homes', 'Freedom Pools', 'Frenchys Fix It', 'Fyfe Pty Ltd', "G D'Agostino", 'G P Forensic', 'G Smith', 'Garrad Plumbing &amp; Civil', 'Gawler Pergola &amp; Timber Supplies', 'Genis Steel', 'Giudel Developments Pty Ltd', 'Goostrey Smith Design', 'Grove Concepts', 'H Vo', 'HBB Property', 'Hawke &amp; Co Pty Ltd', 'Haywood Carpentry', 'Henley Arch Pty Ltd', 'Holmes Dyer', 'Homecorp Constructions SA', 'Homestyle Living Outdoors', 'Hot Property Group', 'Hunter Property Solutions Pty Ltd', 'Hyde Park Projects Pty Ltd', 'I Singh', 'IJ Projects', 'Iconic Roofing', 'Impressive Patios', 'Inception Design', 'Inspire Design Studio', 'J &amp; S Pergola Installations', 'J A Alexander', 'J A Lewis Nominees Pty Ltd', 'J Barbis', 'J Cabangal', 'J D Water Pty Ltd', 'J Harvey', 'J Hayes', 'J J J Services Pty Ltd', 'J Mead', 'J Palmer', 'J Pugh', 'J Rullo', 'J S Hales', 'JVT Holdings Pty Ltd', "Joe's Golden Gasoline Classic Imports Pty Ltd", 'K A Yovan', 'K Ahmadi', 'K Enoka', 'K Ferguson and Mr S A Ferguson', 'K G Drafting &amp; Development Services', 'K Gourlay', 'K Humphreys', 'K P Cherayaramal', 'K Singh', 'K Sokhom', 'Keeping Up Appearances Group Pty Ltd', 'Klhp Family Trust', 'L Abalos', 'L Pawar', 'Lake Maintenance', 'Lamato Property Holdings Pty Ltd', 'Lanser Communities Pty Ltd', 'Leipzig Aust Property Pty Ltd', 'Leipzig Australia Property Trust 2', 'Level Earthworx', 'Levett Engineering Pty Ltd', 'Lifestyle Pergolas', 'Lodge Construction &amp; Building Pty Ltd', 'Lofty Building Group', 'Longridge Group Pty Ltd', 'Louvre House (SA)', 'M A Najafi', 'M Branch', 'M C Pergolas', 'M Galinato', 'M Garnett', 'M Irwin', 'M King', 'M L Schories', 'M Mickan', 'M N Salehi', 'M Pavic', 'M Rani', 'M Schwientek', 'M Wilson and Anglicare SA', 'M2 Architectural Design', 'M2A2 Hillier Pty Ltd', 'Magill Demolition', 'Mahogany Homes', 'Maiden Estate Pty Ltd', 'Mark Willis Excavations', 'Master Homes of Adelaide Pty Ltd', 'Masterplan SA Pty Ltd', 'Matthews Architects', 'Maybach Property Group', 'Metal As Anything (Kadina)', 'Metricon Homes Pty Ltd', 'Metro (SA) Housing Pty Ltd', 'Minister for Infrastructure &amp; Transport', 'Miravale Joint Venture', 'Miss A Karagozlu', 'Miss G R Badea', 'Miss J Fittes', 'Miss V L Kilsby', 'Mitolo Group Pty Ltd', 'Mojo Outdoor Constructions Pty Ltd', 'Mr A A Clarke', 'Mr A A Lombardi', 'Mr A A Paul and Mrs E M Paul', 'Mr A Almas', 'Mr A B Dube and Ms A V Forwood', 'Mr A B Todd', 'Mr A Bhamra', 'Mr A F Johnson', 'Mr A G Kruse', 'Mr A H Krieger', 'Mr A J Bossy', 'Mr A J C Swyghuizen', 'Mr A J Kley', 'Mr A J Kovarik', 'Mr A J Lord', 'Mr A J Sharp', 'Mr A J Stunell', 'Mr A L Xanthopoulos', 'Mr A Lediaev', 'Mr A M Alimi', 'Mr A M Cottrell', 'Mr A M Elliott', 'Mr A N Scutcheon', "Mr A O'Leary", 'Mr A R Borhani', 'Mr A R Tiedau', 'Mr A Ragno', 'Mr A Romaniuk', 'Mr A Russell-Price and Mr T Robinson', 'Mr A S Minopoulos', 'Mr A S Pickett', 'Mr A Sorrenti', 'Mr A T Preen', 'Mr A Taneja', 'Mr A V Coniglio', 'Mr A V Manno and Mrs K Manno', 'Mr A V Vadnere', 'Mr A W Dix', 'Mr A W Mohring', 'Mr B A Singlewood', 'Mr B C Crook', 'Mr B C Day', 'Mr B C Nikou', 'Mr B Coppock', 'Mr B D Wastell', 'Mr B E Goddard', 'Mr B G Hudson', 'Mr B J Woodrow', 'Mr B M Arnold', 'Mr B M Ellis', 'Mr B N Jensen', 'Mr B Newman', 'Mr B P Jamieson', 'Mr B R Prior', 'Mr B Round', 'Mr B S Danzic', 'Mr B Stjepanovic', 'Mr B Vertudaches', 'Mr C A Dawe', 'Mr C A Knowles', 'Mr C D Bishop', 'Mr C D Thornton', 'Mr C H Noble', 'Mr C I Deuter', 'Mr C J Duff', 'Mr C J Eckberg', 'Mr C J Hopgood', 'Mr C J Larson', 'Mr C L Green', 'Mr C Laftsis', 'Mr C M Barrett', 'Mr C M Gutteridge', 'Mr C Petris', 'Mr C Puccini', 'Mr C R Wild', 'Mr D A Beverley', 'Mr D B To', 'Mr D Barton and Mrs J A Barton', 'Mr D Bjelja', 'Mr D Brealey', 'Mr D C Hoppo', 'Mr D E Craddock', 'Mr D Green', 'Mr D J Bastiras', 'Mr D J Kirby', 'Mr D J Launer', 'Mr D J McAnoy', 'Mr D L Boyce', 'Mr D L Goddard', 'Mr D L Van Der Meer', 'Mr D M Peel', 'Mr D M R Pregarz', 'Mr D N Bubner', 'Mr D P Tregenza', 'Mr D R Cockburn', 'Mr D S Dutschke', 'Mr D S R Williams', 'Mr D S Smith', 'Mr D S Zalewski', 'Mr D Shinakis', 'Mr D Spavin', 'Mr D Teurer and Ms A Teurer', 'Mr D W Fleming', 'Mr D Welch', 'Mr D X Ly', 'Mr E J McQueer', 'Mr E K Rendell', 'Mr E Napoli', 'Mr F R Smith', 'Mr F S Catanzariti', 'Mr G A Howarth and Ms K L Gittus', 'Mr G A Jamieson', 'Mr G C Muscat', 'Mr G Hick', 'Mr G J Davis', 'Mr G Marsh', 'Mr G N Willey', 'Mr G P Coy', 'Mr G R Page and Mrs L A Page', 'Mr G W Kercher', 'Mr H Antoniou', 'Mr H D Tonkin', 'Mr H J McLean', 'Mr H Tran', 'Mr I Alrefae', 'Mr I Dichiera', 'Mr I Duncan', 'Mr I Ozdemir', 'Mr I Panetta', 'Mr I W Matthews', 'Mr J A Comelli', 'Mr J A Johnston', 'Mr J B Dearing', 'Mr J B Thorogood', 'Mr J C Muke', 'Mr J D Goldfinch', 'Mr J D Moloney', 'Mr J D Watson', 'Mr J Duffy', 'Mr J Grima', 'Mr J Iacopetta', 'Mr J Imin', 'Mr J J McCormack', 'Mr J K Elliott', 'Mr J K Hutchinson', 'Mr J L Nichols', 'Mr J L Saunders', 'Mr J Maiolo', 'Mr J McGilvray', 'Mr J P Abraham', 'Mr J P Knevitt', 'Mr J P Snoad', 'Mr J P W Henkel', 'Mr J R Settre', 'Mr J S Kavasi', 'Mr J T Purdie and Mrs C A Purdie', 'Mr J Thomas', 'Mr J W Buhagiar', 'Mr J W Prince and Ms E E Prince', 'Mr J W Spong', 'Mr J Yin', 'Mr K A Cussion', 'Mr K Bridger', 'Mr K C Fischer', 'Mr K D Van Schaijik', 'Mr K H Bruns', 'Mr K H Schaefer', 'Mr K K Carypidis', 'Mr K M Thompson', 'Mr K S Aung', 'Mr K W Menadue', 'Mr L A Sanchez', 'Mr L Behn', 'Mr L D Trenorden', 'Mr L Dimanno', 'Mr L Doubleday', 'Mr L I Hardy', 'Mr L J Cooper', 'Mr L J Matthews and Ms L R Matthews', 'Mr L Mayes', 'Mr L Piscioneri', 'Mr L S Duke-Smith', 'Mr L W Bentley', 'Mr M A B Shiddik', 'Mr M A Hutchens', 'Mr M A Owen', 'Mr M Boyle', 'Mr M Brady', 'Mr M C J Nudo', 'Mr M D Campbell', 'Mr M D Hood', 'Mr M Dawson', 'Mr M E Turner', 'Mr M Egel', 'Mr M G Moss', 'Mr M H Krieger', 'Mr M Hatungimana', 'Mr M J Cane', 'Mr M J Fletcher', 'Mr M J Haywood', 'Mr M J Hughes', 'Mr M J Jacka', 'Mr M J Lawrence', 'Mr M J Loechel', 'Mr M J Palmer', 'Mr M J Palmer and Barkleigh Homes', 'Mr M J Press', 'Mr M J Ryan', 'Mr M Jarmyn', 'Mr M M Tebyanyan', 'Mr M Mangiola', 'Mr M Miljevic', 'Mr M Mohammadi', 'Mr M Nocera', 'Mr M P Millar', 'Mr M Pilcher', 'Mr M Radakovitch', 'Mr M T Hall', 'Mr M W Baker', 'Mr M W Hoy', 'Mr N Cavuoto', 'Mr N Cooke', 'Mr N D White', 'Mr N Goulding', 'Mr N Im', 'Mr N J Hall', 'Mr N J Lock', 'Mr N J Staker', 'Mr N K Grabowski', 'Mr N Karantonis', 'Mr N R Wooster', 'Mr N S Zeunert and Ms T M Staines', 'Mr O B Baltazar', 'Mr P B Brentson', 'Mr P Chan', 'Mr P D Corbin', 'Mr P D Farrow', 'Mr P D Reed', 'Mr P G Dezen', 'Mr P H Buch', 'Mr P I Daly', 'Mr P J Bain', 'Mr P J Cannell and Mrs M D Cannell', 'Mr P K Engel and Ms L Engel', 'Mr P L J Baulderstone', 'Mr P L Jeffs', 'Mr P N Gambranis', 'Mr P Nhanh', 'Mr P P J Corbran', 'Mr P R Ellis', 'Mr P Reynolds', 'Mr P S Brar', 'Mr P S Morris', 'Mr P Suchocki', 'Mr R A Barker', 'Mr R Brooks', 'Mr R C Gonzales', 'Mr R C Martin', 'Mr R C Page', 'Mr R C Pilgrim and Ms M Pilgrim', 'Mr R C Wendelborn', 'Mr R D Barrett', 'Mr R D Strehler', 'Mr R Deborsey', 'Mr R E Day', 'Mr R F De Bortoli', 'Mr R F Hussey', 'Mr R Fimmano', 'Mr R G Ellis', 'Mr R G Wilkes and Mrs Y A Wilkes', 'Mr R Hill', 'Mr R Iannella', 'Mr R J Duffield', 'Mr R J Kennedy', 'Mr R J Sharp', 'Mr R J Vast', 'Mr R J Winter', 'Mr R J Young and Miss D K Young', 'Mr R K Bandtock', 'Mr R K Williams', 'Mr R L Damiani and Olympic Industries', 'Mr R Lal', 'Mr R M A Owens', 'Mr R Monti', 'Mr R Muir', 'Mr R Pepper', 'Mr R Rende', 'Mr R V Jordan', 'Mr R Varacalli', 'Mr R W Hill', 'Mr R W Jameson', 'Mr R Winfield', 'Mr R Zwezerijnen', 'Mr S A Ashby', 'Mr S A Jenke', 'Mr S A M Woods', 'Mr S A M Woodward', 'Mr S A Wotton', 'Mr S C Smith', 'Mr S Casey', 'Mr S D Johnson', 'Mr S D Morris', 'Mr S D Newitt', 'Mr S D Sefton', 'Mr S Du Preez', 'Mr S F M Blott', 'Mr S G Osborne', 'Mr S Ibrahimi', 'Mr S J Barlow', 'Mr S J Coward', 'Mr S J Cryer', 'Mr S J Morgan', 'Mr S J Passmore', 'Mr S J Rankine', 'Mr S J Selley', 'Mr S J Wicik', 'Mr S J Y Chan and Ms H K W Li', 'Mr S Kafantaris', 'Mr S Kirkwood', 'Mr S Koulianos', 'Mr S L Long', 'Mr S L Nicol', 'Mr S L Tonellato', 'Mr S M Kimongo', 'Mr S M Norton', 'Mr S M Thomas', 'Mr S Noto', 'Mr S P Arbon', 'Mr S P Kilpatrick', 'Mr S Peregi', 'Mr S R Powney', 'Mr S Schutt', 'Mr S Syrianos', 'Mr S T Walters', 'Mr S Wearing-Smith', 'Mr T A Bodycote', 'Mr T Cambareri', 'Mr T Jones', 'Mr T K Margitich', 'Mr T N Minett', 'Mr T P Wasley', 'Mr T Phillips', 'Mr T R Subedi', 'Mr T Shannon', 'Mr T Song', 'Mr T T Kontos', 'Mr T T Nguyen', 'Mr T Treverton', 'Mr V Bzikadze', 'Mr V J Callus', 'Mr V V Badea', 'Mr W A Wilson', 'Mr W King', 'Mr W L Birch', 'Mr W L Stevens', 'Mr W Lennon', 'Mr W T Davey', 'Mrs A L Walters and Mr S T Walters', 'Mrs A M Ferres', 'Mrs A S McGuffie', 'Mrs A Virgara and Mr A Virgara', "Mrs B C D'Arcy", 'Mrs C E Stewart-Watt', 'Mrs C Enalanga', 'Mrs C M Shoumack', 'Mrs D A J McDonagh', 'Mrs D L Giorgio', 'Mrs D M Moir', 'Mrs D Ryder and Mr A J Ryder', 'Mrs E F Hanauer', 'Mrs E J Chandler', 'Mrs E K Whale', 'Mrs E L Whiteley', "Mrs E M O'Donovan", 'Mrs E Teligiannidis', 'Mrs G D Randall', 'Mrs J K Campbell', 'Mrs J L Silvestri', 'Mrs K Johnston', 'Mrs K W Pilgrim', 'Mrs L A Dezen', 'Mrs M E Costello', 'Mrs N Luke', 'Mrs R J Jones', 'Mrs R M Suell', 'Mrs S C Taylor', 'Mrs S Halteh', 'Mrs S J Lotts', 'Mrs T Cianci', 'Mrs T L Pezzaniti and Mr J A Pezzaniti', 'Mrs T R Sears', 'Mrs Y D Matthews', 'Ms A C Pitman-Purdie', 'Ms A D Pengilly', 'Ms A L Greenwood', 'Ms A M Abela', 'Ms A Reed', 'Ms B Smith', 'Ms C E Boyle', 'Ms C E Dunand', 'Ms C H Ruscoe', 'Ms C J Slager', 'Ms C L Brown', 'Ms C L Waite', 'Ms C Lai', 'Ms C Prak', 'Ms C S Herbert', 'Ms C Snook', 'Ms D H Stratton', 'Ms D M Rush and Mr G T Evans', 'Ms E J Carr', 'Ms F Nazari', 'Ms H M Hewitt', 'Ms J A Pascoe', 'Ms J J Valentijn', 'Ms J L Cox', 'Ms J M Gull', 'Ms J M Zielinski', 'Ms J Sutton', 'Ms J Whitlock', 'Ms K A Ritonja', 'Ms K E Keane', 'Ms K H Lee', 'Ms K L McInnes', 'Ms K Laverty', 'Ms L A Treloar', 'Ms L K D Prosser', 'Ms L K Scott', 'Ms M Ellis', 'Ms M J Tonkin', 'Ms M L Ralph', 'Ms M R Johnson', 'Ms M R Zollo', 'Ms N M French', 'Ms N R Costello and Mr A Maurici', 'Ms N Viant', 'Ms P A Johnson', 'Ms R G Freeman', 'Ms R L Allen', 'Ms R L Damiani', 'Ms S Biacca', 'Ms S J Maschotta', 'Ms S J Morse', 'Ms S J Western and Mr S W Bradshaw', 'Ms S L Payne', 'Ms S M Lavery', 'Ms S N Mells', 'Ms S Paltridge', 'Ms T J Truscott', 'Ms T L Pascoe', 'Ms T Sare', 'Ms V Howson', 'Ms W S Eyers', 'Multichoice Building Services', 'Murfman6 Pty Ltd', 'My Dezign Exteriors', 'My Health Engine Pty Ltd', 'My Living Outdoors', 'N Paiva and A Hussaini', 'N Prak', 'N Yangnovong', 'Network Carports &amp; Verandahs', 'Nevarc Constructions Pty Ltd', 'Nevarc Constructions Pty Ltd and Oakford Homes', 'Ngen Design', 'North MP East Holdings Pty Ltd', 'Northern Shed Works', 'Northern Verandah Supplies', 'Northwest Healthcare Aust Propery Pty Ltd', 'Number One Nominees Pty Ltd', 'Oakford Homes', 'Oakford Homes and Nevarc Constructions Pty Ltd', 'Olympic Industries', 'One SA Pty Ltd', 'P B S Aust', 'P Geracitano', 'P Herbert', 'P McIver', 'P Singlewood', 'P Thwaites', 'P Whittaker and Gannon Lifestyle Pty Ltd', 'PC Infrastructure Pty Ltd', 'Palumbo Building Pty Ltd', 'Palumbo Pty Ltd', 'Panel Homes SA', 'Peats Group', 'Penfield Complex Pty Ltd', 'Pergolas of Distinction', 'Peters Property Group', 'Planning Solutions (Aust) Pty Ltd', 'Premium Home Improvements', 'Premium Roofing &amp; Patios', 'Prestige Pools SA Pty Ltd', 'Pro Form Pergolas Pty Ltd', 'Pro-Form Pergolas', 'R &amp; F M Varacalli Pty Ltd', 'R &amp; M Timber Pty Ltd', 'R B Hill', 'R Gordon', 'R Hanna', 'R M &amp; R C Pty Ltd', 'R Pye', 'Regent Homes', 'Rendition Group', 'Renewal SA', 'Renovus Pty Ltd', 'Revolution Roofing', 'Right Price Roofing', 'Rivergum Homes', 'Rivergum Homes Pty Ltd', 'Riverina Pools &amp; Spas', 'Rossdale Homes Pty Ltd', 'Rotundas &amp; Pergolas of Adelaide', 'Royal Park Salvage', 'Russell Consulting Engineers', 'S Barbieri', 'S Bishop', 'S Fakkas', 'S Ihnatiuc', 'S J Castledine', 'S J Sperrin', 'S Khan', 'S Khun', 'S Lee', 'S McClelland', 'S Nguyen', 'S Rajsekharan', 'S Stallard', 'S T A Bayati', 'S Votino', 'SA Housing Authority', 'SA Housing Trust', 'SA Pergolas', 'SA Power Networks', 'SA Quality Home Improvements', 'SA Ultimate Home Improvements', 'SA Water - Liveability', 'Sagle Constructions Pty Ltd', 'Scouts Australia SA Branch', 'Selecta Homes &amp; Building Co Pty Ltd', 'Sfeer Building Design', 'Shadeform Sailshades', 'Shreenarayan Holdings Pty Ltd', 'Shutta Ya Place', 'Simonds Homes SA', 'Sky Construction &amp; Development', 'Softwoods Timberyards', 'Softwoods Timberyards Pty Ltd', 'Solarlab Pty Ltd', 'South Central Renovations', 'Spa Mart', 'Spartan Plans &amp; Building Services', 'Spectra Building Designers', 'Sri Krishna Investors Pty Ltd', 'State Surveys', 'Statewide Pools', 'Steps Building Services', 'Sterling Homes Pty Ltd', 'Subdivision Solutions', 'Superb Pergolas N Decks', 'T Graham', 'T Hang', 'T Kosmidis', 'T Nguyen', 'T Smith', 'TAFE SA - Elizabeth Campus', 'TMK Consulting Engineers', 'Taking Care of Trees', 'Talent Plumbing', 'The 2a Architectural Studio', 'The Galvin Group', 'The Pergola Man', 'The Trademan', 'Total Space Design Pty Ltd', 'Trinity College Gawler Inc', 'UPM Plumbing &amp; Excavations', 'Unitech Building', 'Urban Renewal Authority', 'Urban3', 'Utter Gutters', 'V Maraviya', 'V N Vuppalapati', 'Vergola Pty Ltd', 'WG Developments Pty Ltd', 'Water Technology', 'Watt Preah Puth Mean Chey Assoc Inc', 'Watusi LJ Pty Ltd', 'Weathersafe Shades Pty Ltd', 'Webb Constructions (SA) Pty Ltd', 'Weeks Building Group', 'Welcome Home Enterprises', 'Z Cai', 'Z Yin', 'Zappall Family Trust']</t>
+          <t>['365 Studio Pty Ltd', '3MT Solutions Pty Ltd', '41 Barfield Pty Ltd', '43 Barfield Pty Ltd', 'A Asteris', 'A Bragg', 'A Breeze', 'A Horn', 'A L Russell', 'A Morgado', 'A Robertson', 'A Sapic', 'A Sharma', 'A Sims', 'A Smith', 'A Tebyanyan', 'A V Jennings', 'A V Jennings Pty Ltd', 'A Valiff', 'AAT Building', 'ABC Homes Pty Ltd', 'ACH Group', 'AH Design &amp; Drafting', 'APM Plumbing', 'Abel Home Improvements', 'Access SDM Pty Ltd', 'Actium Land Developments Pty Ltd', 'Adelaide Builders Pty Ltd', 'Adelaide Building Consulting', 'Adelaide Designer Homes Pty Ltd', 'Adelaide Insurance Builders', 'Adelaide Nominees Pty Ltd', 'Adelaide Retaining Walls', 'Aerobic Tech Pty Ltd', 'Ahrens Engineering', 'Albury Wodonga Community College', 'Aldinga Home Improvements', 'Alete Homes Pty Ltd', 'Alexander Symonds Pty Ltd', 'Alif Homes', 'All Sites Welding Services', 'Alpha Industries', 'Alpha Industries - Glandore', 'Andrash Commercial Pty Ltd', 'Andrew Evans Plumbing', 'Anglicare SA Housing Ltd', 'Anthony Donato Architects', 'Apalie Drive Pty Ltd', 'Apex Greenhouses', 'Apex Greenhouses Aust Pty Ltd', 'Apex Home Improvements', 'Aspire Homes SA Pty Ltd', 'Astrad Pty Ltd', 'Atelier 18 Pty Ltd', 'Attica Homes', 'Aust Child Care Career', 'Aust Outdoor Living', 'Australian Building Company', 'Australian Outdoor Living', 'Australian Workplace Training', 'B A Mebberson', 'B Cox', 'B Goyal', 'B Pring', 'B Thomas and Bargain Steel Centre', 'B Van Groesen', 'Ballavarra Pty Ltd', 'Baracuda Holdings Pty Ltd', 'Bargain Steel Centre', 'Barossa Pergolas &amp; Outdoor Concepts', 'Beechwood Homes', 'Bella Build &amp; Design', 'Better Built Industries', 'Big Difference Home Improvement', 'Botanic Dreams Pty Ltd', 'Bovpap Pty Ltd', 'Bradford Homes', 'Brightspace Homes', 'Brookmont Property Developments Pty Ltd', 'Brooks Development Services', 'Brooks Development Services Pty Ltd', 'Budget Built Home Additions', 'Burbank Aust (SA) Pty Ltd', 'Burns for Blinds', 'Burton Demolition Pty Ltd', 'C Biven', 'C Grimaldi', 'C Liebeknecht', 'C R Hansford', 'C Stevenson', 'C Stock', 'C Yu', 'CT Group Properties No 4 Pty Ltd', 'Cafcakis Nominees and Mr E Cafcakis', 'Catholic Archdiocese of Adelaide', 'Catholic Education SA', 'Century North Pty Ltd', 'Changhui Construction Pty Ltd', 'Chapley Nominees Pty Ltd', 'Checkpoint Building Surveyors', 'City of Playford', 'City of Playford Sports &amp; Property Team', 'Classic Pools &amp; Spas', 'Cocercan Pty Ltd', 'Colcon (NT) Pty Ltd', 'Collins Adelaide', 'Collins Transport', 'Comfresh Pty Ltd', 'Construction Services Aust Pty Ltd', 'Creative Outdoors', 'Crisio Investments Pty Ltd', 'D Clarke', 'D Harris', 'D Knezic', 'D Lobbe', 'D Martyr', 'D Rawat', 'D Turnbull', 'D W Rogers', 'D2c Services', 'DMV Outdoor Solutions', 'DPTI Rail Commissioner', 'Dechellis Homes', 'Department for Education', 'Department for Education - Das Studio', 'Department of Education/Tesa', 'Dept for Education', 'Dept for Infrastructure &amp; Transport', 'Design Constructive Pty Ltd', 'Detail Studio Pty Ltd', 'Diamanti Design Development', 'Dimension Design Studio', 'Distinctive Homes Pty Ltd', 'Dominion Homes', 'Dominos Pizza Enterprises', 'Drug &amp; Alcohol Services SA', 'E Bidhendi', 'Eco Construction &amp; Project Management', 'Elite Pools &amp; Landscapes', 'Elizabeth RSL', 'Emmett JV Pty Ltd', 'Emmett Property Pty Ltd', 'Est Late Mr V Bzikadze', 'Everclear Pool Solutions', 'Exquisite Brows Pty Ltd', 'F Ahmadi', 'F Condelli', 'Faculty Design', 'Fairland Homes Group Pty Ltd', 'Fairmont Homes Group Pty Ltd', 'Fairmont Land Holdings Pty Ltd', 'Farrago Interiors', 'First Choice Verandahs &amp; Carports', 'Format Homes Pty Ltd', 'Fortune Living', 'Frank Nesci Homes', 'Freedom Pools', 'Frenchys Fix It', 'Fyfe Pty Ltd', "G D'Agostino", 'G P Forensic', 'G Smith', 'Garrad Plumbing &amp; Civil', 'Gawler Pergola &amp; Timber Supplies', 'Genis Steel', 'Giudel Developments Pty Ltd', 'Goostrey Smith Design', 'Grove Concepts', 'H Hinrichsen', 'H Li', 'H Sheridan', 'H Vo', 'HBB Property', 'Hawke &amp; Co Pty Ltd', 'Hayden Sheriden', 'Haywood Carpentry', 'Henley Arch Pty Ltd', 'Holmes Dyer', 'Homecorp Constructions SA', 'Homestart Finance Ltd', 'Homestyle Living Outdoors', 'Hot Property Group', 'Hunter Property Solutions Pty Ltd', 'Hyde Park Projects Pty Ltd', 'I Singh', 'IJ Projects', 'Iconic Roofing', 'Impressive Patios', 'Inception Design', 'Inspire Design Studio', 'J &amp; S Pergola Installations', 'J A Alexander', 'J A Lewis Nominees Pty Ltd', 'J Barbis', 'J Brimer', 'J Cabangal', 'J D Water Pty Ltd', 'J Harvey', 'J Hayes', 'J J J Services Pty Ltd', 'J Mead', 'J Palmer', 'J Pugh', 'J Rullo', 'J S Hales', 'JVT Holdings Pty Ltd', "Joe's Golden Gasoline Classic Imports Pty Ltd", 'K A Yovan', 'K Ahmadi', 'K Enoka', 'K Ferguson and Mr S A Ferguson', 'K G Drafting &amp; Development Services', 'K Gourlay', 'K Humphreys', 'K P Cherayaramal', 'K Singh', 'K Sokhom', 'Keeping Up Appearances Group Pty Ltd', 'Klhp Family Trust', 'L Abalos', 'L Pawar', 'Lake Maintenance', 'Lamato Property Holdings Pty Ltd', 'Lanser Communities Pty Ltd', 'Leipzig Aust Property Pty Ltd', 'Leipzig Australia Property Trust 2', 'Level Earthworx', 'Levett Engineering Pty Ltd', 'Lifestyle Pergolas', 'Lionsgate Elizabeth (Pelligra) Pty Ltd', 'Lodge Construction &amp; Building Pty Ltd', 'Lofty Building Group', 'Longridge Group Pty Ltd', 'Louvre House (SA)', 'M A Najafi', 'M Branch', 'M C Pergolas', 'M Dench', 'M Galinato', 'M Garnett', 'M Irwin', 'M King', 'M L Schories', 'M Mickan', 'M N Salehi', 'M Pavic', 'M Rani', 'M Schwientek', 'M Wilson and Anglicare SA', 'M2 Architectural Design', 'M2A2 Hillier Pty Ltd', 'Magill Demolition', 'Mahogany Homes', 'Maiden Estate Pty Ltd', 'Mark Willis Excavations', 'Master Homes of Adelaide Pty Ltd', 'Masterplan SA Pty Ltd', 'Matthews Architects', 'Maybach Property Group', 'Metal As Anything (Kadina)', 'Metricon Homes Pty Ltd', 'Metro (SA) Housing Pty Ltd', 'Metro Homes SA', 'Minister for Infrastructure &amp; Transport', 'Miravale Joint Venture', 'Miss A Karagozlu', 'Miss G R Badea', 'Miss J Fittes', 'Miss V L Kilsby', 'Mitolo Group Pty Ltd', 'Mojo Outdoor Constructions Pty Ltd', 'Mr A A Clarke', 'Mr A A Lombardi', 'Mr A A Paul and Mrs E M Paul', 'Mr A Almas', 'Mr A B Dube and Ms A V Forwood', 'Mr A B Todd', 'Mr A Bhamra', 'Mr A D Wallis', 'Mr A F Johnson', 'Mr A G Clarke', 'Mr A G Kruse', 'Mr A H Krieger', 'Mr A J Bossy', 'Mr A J C Swyghuizen', 'Mr A J Kley', 'Mr A J Kovarik', 'Mr A J Lord', 'Mr A J Sharp', 'Mr A J Stunell', 'Mr A L Xanthopoulos', 'Mr A Lediaev', 'Mr A M Alimi', 'Mr A M Cottrell', 'Mr A M Elliott', 'Mr A N Scutcheon', "Mr A O'Leary", 'Mr A R Borhani', 'Mr A R Tiedau', 'Mr A Ragno', 'Mr A Romaniuk', 'Mr A Russell-Price and Mr T Robinson', 'Mr A S Minopoulos', 'Mr A S Pickett', 'Mr A Sorrenti', 'Mr A T Preen', 'Mr A Taneja', 'Mr A V Coniglio', 'Mr A V Manno and Mrs K Manno', 'Mr A V Vadnere', 'Mr A W Dix', 'Mr A W Mohring', 'Mr A Zummo', 'Mr B A Singlewood', 'Mr B C Crook', 'Mr B C Day', 'Mr B C Nikou', 'Mr B Coppock', 'Mr B D Wastell', 'Mr B E Goddard', 'Mr B G Hudson', 'Mr B J Woodrow', 'Mr B M Arnold', 'Mr B M Ellis', 'Mr B N Jensen', 'Mr B Newman', 'Mr B P Jamieson', 'Mr B R Prior', 'Mr B Round', 'Mr B S Danzic', 'Mr B Stjepanovic', 'Mr B Vertudaches', 'Mr C A Dawe', 'Mr C A Knowles', 'Mr C D Bishop', 'Mr C D Thornton', 'Mr C H Noble', 'Mr C I Deuter', 'Mr C J Duff', 'Mr C J Eckberg', 'Mr C J Hopgood', 'Mr C J Larson', 'Mr C L Green', 'Mr C Laftsis', 'Mr C M Barrett', 'Mr C M Gutteridge', 'Mr C Petris', 'Mr C Puccini', 'Mr C R Wild', 'Mr D A Beverley', 'Mr D B To', 'Mr D Barton and Mrs J A Barton', 'Mr D Bjelja', 'Mr D Brealey', 'Mr D C Hoppo', 'Mr D E Craddock', 'Mr D Green', 'Mr D J Bastiras', 'Mr D J Kirby', 'Mr D J Launer', 'Mr D J McAnoy', 'Mr D L Boyce', 'Mr D L Goddard', 'Mr D L Van Der Meer', 'Mr D M Peel', 'Mr D M R Pregarz', 'Mr D N Bubner', 'Mr D P Tregenza', 'Mr D R Cockburn', 'Mr D S Dutschke', 'Mr D S R Williams', 'Mr D S Smith', 'Mr D S Zalewski', 'Mr D Shinakis', 'Mr D Spavin', 'Mr D Teurer and Ms A Teurer', 'Mr D W Fenner', 'Mr D W Fleming', 'Mr D Welch', 'Mr D X Ly', 'Mr E J McQueer', 'Mr E K Rendell', 'Mr E Napoli', 'Mr F R Smith', 'Mr F S Catanzariti', 'Mr G A Howarth and Ms K L Gittus', 'Mr G A Jamieson', 'Mr G C Muscat', 'Mr G Hick', 'Mr G J Davis', 'Mr G Marsh', 'Mr G N Willey', 'Mr G Nichinonni', 'Mr G P Coy', 'Mr G R Page and Mrs L A Page', 'Mr G W Kercher', 'Mr H Antoniou', 'Mr H D Tonkin', 'Mr H J McLean', 'Mr H Tran', 'Mr I Alrefae', 'Mr I Dichiera', 'Mr I Duncan', 'Mr I Ozdemir', 'Mr I Panetta', 'Mr I W Matthews', 'Mr J A Comelli', 'Mr J A Johnston', 'Mr J B Dearing', 'Mr J B T Scheepens and Mrs M Scheepens', 'Mr J B Thorogood', 'Mr J C Muke', 'Mr J D Goldfinch', 'Mr J D Moloney', 'Mr J D Watson', 'Mr J Duffy', 'Mr J Grima', 'Mr J Iacopetta', 'Mr J Imin', 'Mr J J McCormack', 'Mr J K Elliott', 'Mr J K Hutchinson', 'Mr J L Nichols', 'Mr J L Saunders', 'Mr J Maiolo', 'Mr J McGilvray', 'Mr J P Abraham', 'Mr J P Knevitt', 'Mr J P Snoad', 'Mr J P W Henkel', 'Mr J R Settre', 'Mr J S Kavasi', 'Mr J T Purdie and Mrs C A Purdie', 'Mr J Thomas', 'Mr J W Buhagiar', 'Mr J W Prince and Ms E E Prince', 'Mr J W Spong', 'Mr J Yin', 'Mr K A Cussion', 'Mr K Barlow', 'Mr K Bridger', 'Mr K C Fischer', 'Mr K D Van Schaijik', 'Mr K E A D Nicholls', 'Mr K H Bruns', 'Mr K H Schaefer', 'Mr K K Carypidis', 'Mr K M Thompson', 'Mr K S Aung', 'Mr K W Menadue', 'Mr L A Sanchez', 'Mr L Behn', 'Mr L D Trenorden', 'Mr L Dimanno', 'Mr L Doubleday', 'Mr L I Hardy', 'Mr L J Cooper', 'Mr L J Matthews and Ms L R Matthews', 'Mr L Mayes', 'Mr L Piscioneri', 'Mr L S Duke-Smith', 'Mr L Thomas', 'Mr L W Bentley', 'Mr M A B Shiddik', 'Mr M A Hutchens', 'Mr M A Owen', 'Mr M Borg', 'Mr M Boyle', 'Mr M Brady', 'Mr M C J Nudo', 'Mr M C Pocock', 'Mr M D Campbell', 'Mr M D Hood', 'Mr M Dawson', 'Mr M E Turner', 'Mr M Egel', 'Mr M G Moss', 'Mr M H Krieger', 'Mr M Hatungimana', 'Mr M J Cane', 'Mr M J Fletcher', 'Mr M J Haywood', 'Mr M J Hughes', 'Mr M J Jacka', 'Mr M J Lawrence', 'Mr M J Loechel', 'Mr M J Palmer', 'Mr M J Palmer and Barkleigh Homes', 'Mr M J Press', 'Mr M J Ryan', 'Mr M Jarmyn', 'Mr M M Tebyanyan', 'Mr M Mangiola', 'Mr M Miljevic', 'Mr M Mohammadi', 'Mr M Nocera', 'Mr M P Millar', 'Mr M Pilcher', 'Mr M Radakovitch', 'Mr M T Hall', 'Mr M W Baker', 'Mr M W Hoy', 'Mr N Cavuoto', 'Mr N Cooke', 'Mr N D White', 'Mr N Goulding', 'Mr N Im', 'Mr N J Allen', 'Mr N J Hall', 'Mr N J Lock', 'Mr N J Staker', 'Mr N K Grabowski', 'Mr N Karantonis', 'Mr N R Wooster', 'Mr N S Zeunert and Ms T M Staines', 'Mr O B Baltazar', 'Mr P B Brentson', 'Mr P Chan', 'Mr P D Corbin', 'Mr P D Farrow', 'Mr P D Reed', 'Mr P G Dezen', 'Mr P H Buch', 'Mr P I Daly', 'Mr P J Bain', 'Mr P J Cannell and Mrs M D Cannell', 'Mr P J Day', 'Mr P K Engel and Ms L Engel', 'Mr P L J Baulderstone', 'Mr P L Jeffs', 'Mr P N Gambranis', 'Mr P Nhanh', 'Mr P P J Corbran', 'Mr P R Ellis', 'Mr P Reynolds', 'Mr P S Brar', 'Mr P S Morris', 'Mr P Suchocki', 'Mr R A Barker', 'Mr R Brooks', 'Mr R C Gonzales', 'Mr R C Martin', 'Mr R C Page', 'Mr R C Pilgrim and Ms M Pilgrim', 'Mr R C Wendelborn', 'Mr R D Barrett', 'Mr R D Strehler', 'Mr R Deborsey', 'Mr R E Day', 'Mr R F De Bortoli', 'Mr R F Hussey', 'Mr R Fimmano', 'Mr R G Ellis', 'Mr R G Wilkes and Mrs Y A Wilkes', 'Mr R Hill', 'Mr R Iannella', 'Mr R J Duffield', 'Mr R J Kennedy', 'Mr R J Sharp', 'Mr R J Vast', 'Mr R J White', 'Mr R J Winter', 'Mr R J Young and Miss D K Young', 'Mr R K Bandtock', 'Mr R K Williams', 'Mr R L Damiani and Olympic Industries', 'Mr R Lal', 'Mr R M A Owens', 'Mr R Maiolo and Mr F Maiolo', 'Mr R Monti', 'Mr R Muir', 'Mr R Pepper', 'Mr R Rende', 'Mr R V Jordan', 'Mr R V Kirkham', 'Mr R Varacalli', 'Mr R W Hill', 'Mr R W Jameson', 'Mr R Winfield', 'Mr R Zwezerijnen', 'Mr S A Ashby', 'Mr S A Hosseini', 'Mr S A Jenke', 'Mr S A M Woods', 'Mr S A M Woodward', 'Mr S A Valiff', 'Mr S A Wotton', 'Mr S C Smith', 'Mr S Casey', 'Mr S D Johnson', 'Mr S D Laming', 'Mr S D Morris', 'Mr S D Newitt', 'Mr S D Sefton', 'Mr S Du Preez', 'Mr S F M Blott', 'Mr S G Osborne', 'Mr S Ghyas', 'Mr S Ibrahimi', 'Mr S J Barlow', 'Mr S J Coward', 'Mr S J Cryer', 'Mr S J Morgan', 'Mr S J Passmore', 'Mr S J Rankine', 'Mr S J Selley', 'Mr S J Wicik', 'Mr S J Y Chan and Ms H K W Li', 'Mr S K Cahill', 'Mr S Kafantaris', 'Mr S Kirkwood', 'Mr S Koulianos', 'Mr S L Long', 'Mr S L Nicol', 'Mr S L Tonellato', 'Mr S M Kimongo', 'Mr S M Norton', 'Mr S M Thomas', 'Mr S Noto', 'Mr S P Arbon', 'Mr S P Kilpatrick', 'Mr S Peregi', 'Mr S R Powney', 'Mr S Schutt', 'Mr S Syrianos', 'Mr S T Walters', 'Mr S W Duncan', 'Mr S Wearing-Smith', 'Mr T A Bodycote', 'Mr T Cambareri', 'Mr T Jones', 'Mr T K Margitich', 'Mr T N Minett', 'Mr T P Wasley', 'Mr T Phillips', 'Mr T R Subedi', 'Mr T Shannon', 'Mr T Song', 'Mr T T Kontos', 'Mr T T Nguyen', 'Mr T Treverton', 'Mr V J Callus', 'Mr V V Badea', 'Mr W A Wilson', 'Mr W King', 'Mr W L Birch', 'Mr W L Stevens', 'Mr W Lennon', 'Mr W T Davey', 'Mrs A L Walters and Mr S T Walters', 'Mrs A M Ferres', 'Mrs A S McGuffie', 'Mrs A Virgara and Mr A Virgara', "Mrs B C D'Arcy", 'Mrs C E Stewart-Watt', 'Mrs C Enalanga', 'Mrs C M Shoumack', 'Mrs D A J McDonagh', 'Mrs D L Giorgio', 'Mrs D M Moir', 'Mrs D M Tipping', 'Mrs D Ryder and Mr A J Ryder', 'Mrs E F Hanauer', 'Mrs E J Chandler', 'Mrs E K Whale', 'Mrs E L Whiteley', "Mrs E M O'Donovan", 'Mrs E Teligiannidis', 'Mrs F M Ryan', 'Mrs G D Randall', 'Mrs J K Campbell', 'Mrs J L Silvestri', 'Mrs K Johnston', 'Mrs K W Pilgrim', 'Mrs L A Dezen', 'Mrs M A Parletta', 'Mrs M E Costello', 'Mrs N Luke', 'Mrs R J Jones', 'Mrs R M Suell', 'Mrs S C Taylor', 'Mrs S Halteh', 'Mrs S J Lotts', 'Mrs T Cianci', 'Mrs T Jones', 'Mrs T L Pezzaniti and Mr J A Pezzaniti', 'Mrs T R Sears', 'Mrs Y D Matthews', 'Ms A C Pitman-Purdie', 'Ms A D Pengilly', 'Ms A L Greenwood', 'Ms A M Abela', 'Ms A Reed', 'Ms B Smith', 'Ms C E Boyle', 'Ms C E Dunand', 'Ms C H Ruscoe', 'Ms C J Slager', 'Ms C L Brown', 'Ms C L Waite', 'Ms C Lai', 'Ms C Prak', 'Ms C S Herbert', 'Ms C Snook', 'Ms D H Stratton', 'Ms D M Rush and Mr G T Evans', 'Ms E J Carr', 'Ms F Delaney', 'Ms F Nazari', 'Ms H M Hewitt', 'Ms J A Pascoe', 'Ms J F Adamson', 'Ms J J Valentijn', 'Ms J L Cox', 'Ms J M Gull', 'Ms J M Zielinski', 'Ms J Sutton', 'Ms J Whitlock', 'Ms K A Ritonja', 'Ms K E Keane', 'Ms K H Lee', 'Ms K L McInnes', 'Ms K Laverty', 'Ms L A Treloar', 'Ms L K D Prosser', 'Ms L K Scott', 'Ms M Ellis', 'Ms M J Tonkin', 'Ms M L Ralph', 'Ms M R Johnson', 'Ms M R Zollo', 'Ms N M French', 'Ms N R Costello and Mr A Maurici', 'Ms N Viant', 'Ms P A Johnson', 'Ms R G Freeman', 'Ms R L Allen', 'Ms R L Damiani', 'Ms S Biacca', 'Ms S J Fleming', 'Ms S J Maschotta', 'Ms S J Morse', 'Ms S J Western and Mr S W Bradshaw', 'Ms S L Payne', 'Ms S M Lavery', 'Ms S N Mells', 'Ms S Paltridge', 'Ms T J Truscott', 'Ms T L Pascoe', 'Ms T Sare', 'Ms V Howson', 'Ms W S Eyers', 'Multichoice Building Services', 'Murfman6 Pty Ltd', 'My Dezign Exteriors', 'My Health Engine Pty Ltd', 'My Living Outdoors', 'N Paiva and A Hussaini', 'N Prak', 'N Yangnovong', 'Network Carports &amp; Verandahs', 'Nevarc Constructions Pty Ltd', 'Nevarc Constructions Pty Ltd and Oakford Homes', 'Ngen Design', 'Nguyen SA', 'North MP East Holdings Pty Ltd', 'Northern Shed Works', 'Northern Verandah Supplies', 'Northwest Healthcare Aust Propery Pty Ltd', 'Number One Nominees Pty Ltd', 'Oakford Homes', 'Oakford Homes and Nevarc Constructions Pty Ltd', 'Olympic Industries', 'One SA Pty Ltd', 'P B S Aust', 'P Geracitano', 'P Herbert', 'P McIver', 'P Singlewood', 'P Thwaites', 'P Whittaker and Gannon Lifestyle Pty Ltd', 'PC Infrastructure Pty Ltd', 'Palumbo Building Pty Ltd', 'Palumbo Pty Ltd', 'Panel Homes SA', 'Peats Group', 'Penfield Complex Pty Ltd', 'Pergolas of Distinction', 'Peters Property Group', 'Planning Solutions (Aust) Pty Ltd', 'Playford Primary School', 'Premium Home Improvements', 'Premium Roofing &amp; Patios', 'Prestige Pools SA Pty Ltd', 'Pro Form Pergolas Pty Ltd', 'Pro-Form Pergolas', 'R &amp; F M Varacalli Pty Ltd', 'R &amp; M Timber Pty Ltd', 'R B Hill', 'R Gilbert', 'R Gordon', 'R Hanna', 'R M &amp; R C Pty Ltd', 'R Pye', 'Reach Energy Storage Co', 'Regent Homes', 'Rendition Group', 'Rendition Homes', 'Renewal SA', 'Renovus Pty Ltd', 'Revolution Roofing', 'Right Price Roofing', 'Rivergum Homes', 'Rivergum Homes Pty Ltd', 'Riverina Pools &amp; Spas', 'Rossdale Homes Pty Ltd', 'Rotundas &amp; Pergolas of Adelaide', 'Royal Park Salvage', 'Russell Consulting Engineers', 'S Barbieri', 'S Bishop', 'S Fakkas', 'S Furqan', 'S Ihnatiuc', 'S J Castledine', 'S J Sperrin', 'S K Maybury', 'S Khan', 'S Khun', 'S Lee', 'S McClelland', 'S Nguyen', 'S Rajsekharan', 'S Stallard', 'S T A Bayati', 'S Votino', 'SA Housing Authority', 'SA Housing Trust', 'SA Pergolas', 'SA Power Networks', 'SA Quality Home Improvements', 'SA Ultimate Home Improvements', 'SA Water - Liveability', 'Sagle Constructions Pty Ltd', 'Scouts Australia SA Branch', 'Selecta Homes &amp; Building Co Pty Ltd', 'Sfeer Building Design', 'Shade SA', 'Shadeform Sailshades', 'Shreenarayan Holdings Pty Ltd', 'Shutta Ya Place', 'Simonds Homes SA', 'Sketch &amp; Build Pty Ltd', 'Sky Construction &amp; Development', 'Softwoods Timberyards', 'Softwoods Timberyards Pty Ltd', 'Solarlab Pty Ltd', 'South Central Renovations', 'Spa Mart', 'Spartan Plans &amp; Building Services', 'Spectra Building Designers', 'Sri Krishna Investors Pty Ltd', 'State Surveys', 'Statewide Pools', 'Steps Building Services', 'Sterling Homes Pty Ltd', 'Subdivision Solutions', 'Superb Pergolas N Decks', 'T Graham', 'T Hang', 'T Kosmidis', 'T Nguyen', 'T Smith', 'TAFE SA - Elizabeth Campus', 'TMK Consulting Engineers', 'Taking Care of Trees', 'Talent Plumbing', 'Tecon Aust Pty Ltd', 'The 2a Architectural Studio', 'The Galvin Group', 'The Pergola Man', 'The Trademan', 'Think Architects', 'Total Space Design Pty Ltd', 'Trinity College Gawler Inc', 'UPM Plumbing', 'UPM Plumbing &amp; Excavations', 'Unitech Building', 'Urban Renewal Authority', 'Urban3', 'Utter Gutters', 'V Maraviya', 'V N Vuppalapati', 'Vergola Pty Ltd', 'WG Developments Pty Ltd', 'Water Technology', 'Watt Preah Puth Mean Chey Assoc Inc', 'Watusi LJ Pty Ltd', 'Weathersafe Shades Pty Ltd', 'Webb Constructions (SA) Pty Ltd', 'Weeks Building Group', 'Welcome Home Enterprises', 'Z Cai', 'Z Yin', 'Zappall Family Trust', 'Zappia Consulting Pty Ltd', 'Zummo Design']</t>
         </is>
       </c>
     </row>
@@ -843,7 +843,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -876,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
@@ -891,7 +891,7 @@
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>Ms T L Pascoe</t>
+          <t>Mr A D Wallis</t>
         </is>
       </c>
       <c r="T5" t="n">
@@ -903,20 +903,20 @@
         </is>
       </c>
       <c r="V5" t="n">
-        <v>384</v>
+        <v>451</v>
       </c>
       <c r="W5" t="n">
         <v>0</v>
       </c>
       <c r="X5" t="n">
-        <v>55420</v>
+        <v>62875</v>
       </c>
       <c r="Y5" t="n">
-        <v>840</v>
+        <v>906</v>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>['********** PRIVATE **********', '365 Studio Pty Ltd', '3MT Solutions Pty Ltd', '41 Barfield Pty Ltd', '43 Barfield Pty Ltd', 'A Asteris', 'A Bragg', 'A Horn', 'A L Russell', 'A Morgado', 'A Robertson', 'A Sapic', 'A Sharma', 'A Smith', 'A Tebyanyan', 'A V Jennings', 'A V Jennings Pty Ltd', 'A Valiff', 'AAT Building', 'ABC Homes Pty Ltd', 'AH Design &amp; Drafting', 'APM Plumbing', 'Access SDM Pty Ltd', 'Actium Land Developments Pty Ltd', 'Adelaide Builders Pty Ltd', 'Adelaide Building Consulting', 'Adelaide Designer Homes Pty Ltd', 'Adelaide Insurance Builders', 'Adelaide Nominees Pty Ltd', 'Adelaide Retaining Walls', 'Aerobic Tech Pty Ltd', 'Ahrens Engineering', 'Albury Wodonga Community College', 'Aldinga Home Improvements', 'Alete Homes Pty Ltd', 'Alexander Symonds Pty Ltd', 'Alif Homes', 'All Sites Welding Services', 'Alpha Industries', 'Alpha Industries - Glandore', 'Andrash Commercial Pty Ltd', 'Andrew Evans Plumbing', 'Anglicare SA Housing Ltd', 'Anthony Donato Architects', 'Apalie Drive Pty Ltd', 'Apex Greenhouses', 'Apex Greenhouses Aust Pty Ltd', 'Apex Home Improvements', 'Aspire Homes SA Pty Ltd', 'Astrad Pty Ltd', 'Atelier 18 Pty Ltd', 'Attica Homes', 'Aust Child Care Career', 'Aust Outdoor Living', 'Australian Building Company', 'Australian Outdoor Living', 'Australian Workplace Training', 'B A Mebberson', 'B Cox', 'B Goyal', 'B Pring', 'B Thomas and Bargain Steel Centre', 'B Van Groesen', 'Ballavarra Pty Ltd', 'Baracuda Holdings Pty Ltd', 'Bargain Steel Centre', 'Barossa Pergolas &amp; Outdoor Concepts', 'Beechwood Homes', 'Bella Build &amp; Design', 'Better Built Industries', 'Big Difference Home Improvement', 'Botanic Dreams Pty Ltd', 'Bovpap Pty Ltd', 'Bradford Homes', 'Brightspace Homes', 'Brookmont Property Developments Pty Ltd', 'Brooks Development Services', 'Brooks Development Services Pty Ltd', 'Budget Built Home Additions', 'Burbank Aust (SA) Pty Ltd', 'Burton Demolition Pty Ltd', 'C Biven', 'C Grimaldi', 'C Liebeknecht', 'C Stevenson', 'C Stock', 'C Yu', 'CT Group Properties No 4 Pty Ltd', 'Cafcakis Nominees and Mr E Cafcakis', 'Catholic Archdiocese of Adelaide', 'Century North Pty Ltd', 'Changhui Construction Pty Ltd', 'Checkpoint Building Surveyors', 'City of Playford', 'City of Playford Sports &amp; Property Team', 'Classic Pools &amp; Spas', 'Cocercan Pty Ltd', 'Colcon (NT) Pty Ltd', 'Collins Adelaide', 'Collins Transport', 'Comfresh Pty Ltd', 'Construction Services Aust Pty Ltd', 'Creative Outdoors', 'Crisio Investments Pty Ltd', 'D Clarke', 'D Harris', 'D Lobbe', 'D Martyr', 'D Rawat', 'D Turnbull', 'D W Rogers', 'D2c Services', 'DMV Outdoor Solutions', 'DPTI Rail Commissioner', 'Dechellis Homes', 'Department for Education', 'Department for Education - Das Studio', 'Department of Education/Tesa', 'Dept for Infrastructure &amp; Transport', 'Design Constructive Pty Ltd', 'Detail Studio Pty Ltd', 'Diamanti Design Development', 'Dimension Design Studio', 'Distinctive Homes Pty Ltd', 'Dominion Homes', 'Drug &amp; Alcohol Services SA', 'E Bidhendi', 'Elite Pools &amp; Landscapes', 'Elizabeth RSL', 'Emmett Property Pty Ltd', 'Everclear Pool Solutions', 'Exquisite Brows Pty Ltd', 'F Ahmadi', 'Faculty Design', 'Fairland Homes Group Pty Ltd', 'Fairmont Homes Group Pty Ltd', 'Fairmont Land Holdings Pty Ltd', 'Farrago Interiors', 'First Choice Verandahs &amp; Carports', 'Format Homes Pty Ltd', 'Fortune Living', 'Frank Nesci Homes', 'Freedom Pools', 'Frenchys Fix It', 'Fyfe Pty Ltd', "G D'Agostino", 'G P Forensic', 'G Smith', 'Garrad Plumbing &amp; Civil', 'Gawler Pergola &amp; Timber Supplies', 'Genis Steel', 'Giudel Developments Pty Ltd', 'Goostrey Smith Design', 'Grove Concepts', 'H Vo', 'HBB Property', 'Hawke &amp; Co Pty Ltd', 'Haywood Carpentry', 'Henley Arch Pty Ltd', 'Holmes Dyer', 'Homecorp Constructions SA', 'Homestyle Living Outdoors', 'Hot Property Group', 'Hunter Property Solutions Pty Ltd', 'Hyde Park Projects Pty Ltd', 'I Singh', 'IJ Projects', 'Iconic Roofing', 'Impressive Patios', 'Inception Design', 'Inspire Design Studio', 'J &amp; S Pergola Installations', 'J A Alexander', 'J A Lewis Nominees Pty Ltd', 'J Barbis', 'J Cabangal', 'J D Water Pty Ltd', 'J Harvey', 'J Hayes', 'J J J Services Pty Ltd', 'J Mead', 'J Palmer', 'J Pugh', 'J Rullo', 'J S Hales', 'JVT Holdings Pty Ltd', "Joe's Golden Gasoline Classic Imports Pty Ltd", 'K A Yovan', 'K Ahmadi', 'K Enoka', 'K Ferguson and Mr S A Ferguson', 'K G Drafting &amp; Development Services', 'K Gourlay', 'K Humphreys', 'K P Cherayaramal', 'K Singh', 'K Sokhom', 'Keeping Up Appearances Group Pty Ltd', 'Klhp Family Trust', 'L Abalos', 'L Pawar', 'Lake Maintenance', 'Lamato Property Holdings Pty Ltd', 'Lanser Communities Pty Ltd', 'Leipzig Aust Property Pty Ltd', 'Leipzig Australia Property Trust 2', 'Level Earthworx', 'Levett Engineering Pty Ltd', 'Lifestyle Pergolas', 'Lodge Construction &amp; Building Pty Ltd', 'Lofty Building Group', 'Longridge Group Pty Ltd', 'Louvre House (SA)', 'M A Najafi', 'M Branch', 'M C Pergolas', 'M Galinato', 'M Garnett', 'M Irwin', 'M King', 'M L Schories', 'M Mickan', 'M N Salehi', 'M Pavic', 'M Rani', 'M Schwientek', 'M Wilson and Anglicare SA', 'M2 Architectural Design', 'M2A2 Hillier Pty Ltd', 'Magill Demolition', 'Mahogany Homes', 'Maiden Estate Pty Ltd', 'Mark Willis Excavations', 'Master Homes of Adelaide Pty Ltd', 'Masterplan SA Pty Ltd', 'Matthews Architects', 'Maybach Property Group', 'Metal As Anything (Kadina)', 'Metricon Homes Pty Ltd', 'Metro (SA) Housing Pty Ltd', 'Minister for Infrastructure &amp; Transport', 'Miravale Joint Venture', 'Miss A Karagozlu', 'Miss G R Badea', 'Miss J Fittes', 'Miss V L Kilsby', 'Mitolo Group Pty Ltd', 'Mojo Outdoor Constructions Pty Ltd', 'Mr A A Clarke', 'Mr A A Lombardi', 'Mr A A Paul and Mrs E M Paul', 'Mr A Almas', 'Mr A B Dube and Ms A V Forwood', 'Mr A B Todd', 'Mr A Bhamra', 'Mr A F Johnson', 'Mr A G Kruse', 'Mr A H Krieger', 'Mr A J Bossy', 'Mr A J C Swyghuizen', 'Mr A J Kley', 'Mr A J Kovarik', 'Mr A J Sharp', 'Mr A J Stunell', 'Mr A L Xanthopoulos', 'Mr A Lediaev', 'Mr A M Alimi', 'Mr A M Cottrell', 'Mr A M Elliott', 'Mr A N Scutcheon', "Mr A O'Leary", 'Mr A R Borhani', 'Mr A R Tiedau', 'Mr A Ragno', 'Mr A Romaniuk', 'Mr A Russell-Price and Mr T Robinson', 'Mr A S Minopoulos', 'Mr A S Pickett', 'Mr A Sorrenti', 'Mr A T Preen', 'Mr A Taneja', 'Mr A V Coniglio', 'Mr A V Manno and Mrs K Manno', 'Mr A V Vadnere', 'Mr A W Dix', 'Mr A W Mohring', 'Mr B A Singlewood', 'Mr B C Crook', 'Mr B C Day', 'Mr B C Nikou', 'Mr B Coppock', 'Mr B D Wastell', 'Mr B E Goddard', 'Mr B G Hudson', 'Mr B J Woodrow', 'Mr B M Arnold', 'Mr B M Ellis', 'Mr B N Jensen', 'Mr B Newman', 'Mr B P Jamieson', 'Mr B R Prior', 'Mr B Round', 'Mr B S Danzic', 'Mr B Stjepanovic', 'Mr B Vertudaches', 'Mr C A Dawe', 'Mr C A Knowles', 'Mr C D Bishop', 'Mr C D Thornton', 'Mr C H Noble', 'Mr C I Deuter', 'Mr C J Duff', 'Mr C J Eckberg', 'Mr C J Hopgood', 'Mr C J Larson', 'Mr C L Green', 'Mr C Laftsis', 'Mr C M Barrett', 'Mr C M Gutteridge', 'Mr C Petris', 'Mr C Puccini', 'Mr C R Wild', 'Mr D A Beverley', 'Mr D B To', 'Mr D Barton and Mrs J A Barton', 'Mr D Bjelja', 'Mr D Brealey', 'Mr D C Hoppo', 'Mr D E Craddock', 'Mr D Green', 'Mr D J Bastiras', 'Mr D J Kirby', 'Mr D J Launer', 'Mr D J McAnoy', 'Mr D L Boyce', 'Mr D L Goddard', 'Mr D L Van Der Meer', 'Mr D M Peel', 'Mr D M R Pregarz', 'Mr D N Bubner', 'Mr D P Tregenza', 'Mr D R Cockburn', 'Mr D S Dutschke', 'Mr D S R Williams', 'Mr D S Smith', 'Mr D S Zalewski', 'Mr D Shinakis', 'Mr D Spavin', 'Mr D Teurer and Ms A Teurer', 'Mr D W Fleming', 'Mr D Welch', 'Mr D X Ly', 'Mr E J McQueer', 'Mr E K Rendell', 'Mr E Napoli', 'Mr F R Smith', 'Mr F S Catanzariti', 'Mr G A Howarth and Ms K L Gittus', 'Mr G A Jamieson', 'Mr G C Muscat', 'Mr G Hick', 'Mr G J Davis', 'Mr G Marsh', 'Mr G N Willey', 'Mr G P Coy', 'Mr G R Page and Mrs L A Page', 'Mr G W Kercher', 'Mr H Antoniou', 'Mr H D Tonkin', 'Mr H J McLean', 'Mr H Tran', 'Mr I Alrefae', 'Mr I Dichiera', 'Mr I Duncan', 'Mr I Ozdemir', 'Mr I Panetta', 'Mr I W Matthews', 'Mr J A Comelli', 'Mr J A Johnston', 'Mr J B Dearing', 'Mr J B Thorogood', 'Mr J C Muke', 'Mr J D Goldfinch', 'Mr J D Moloney', 'Mr J D Watson', 'Mr J Duffy', 'Mr J Grima', 'Mr J Iacopetta', 'Mr J Imin', 'Mr J J McCormack', 'Mr J K Elliott', 'Mr J K Hutchinson', 'Mr J L Nichols', 'Mr J L Saunders', 'Mr J Maiolo', 'Mr J McGilvray', 'Mr J P Abraham', 'Mr J P Knevitt', 'Mr J P Snoad', 'Mr J P W Henkel', 'Mr J R Settre', 'Mr J S Kavasi', 'Mr J T Purdie and Mrs C A Purdie', 'Mr J Thomas', 'Mr J W Buhagiar', 'Mr J W Prince and Ms E E Prince', 'Mr J W Spong', 'Mr J Yin', 'Mr K A Cussion', 'Mr K Bridger', 'Mr K C Fischer', 'Mr K D Van Schaijik', 'Mr K H Bruns', 'Mr K H Schaefer', 'Mr K K Carypidis', 'Mr K M Thompson', 'Mr K S Aung', 'Mr K W Menadue', 'Mr L A Sanchez', 'Mr L Behn', 'Mr L D Trenorden', 'Mr L Dimanno', 'Mr L Doubleday', 'Mr L I Hardy', 'Mr L J Cooper', 'Mr L J Matthews and Ms L R Matthews', 'Mr L Mayes', 'Mr L Piscioneri', 'Mr L S Duke-Smith', 'Mr L W Bentley', 'Mr M A B Shiddik', 'Mr M A Hutchens', 'Mr M A Owen', 'Mr M Boyle', 'Mr M Brady', 'Mr M C J Nudo', 'Mr M D Campbell', 'Mr M D Hood', 'Mr M Dawson', 'Mr M E Turner', 'Mr M Egel', 'Mr M G Moss', 'Mr M H Krieger', 'Mr M Hatungimana', 'Mr M J Cane', 'Mr M J Fletcher', 'Mr M J Haywood', 'Mr M J Hughes', 'Mr M J Jacka', 'Mr M J Lawrence', 'Mr M J Loechel', 'Mr M J Palmer', 'Mr M J Palmer and Barkleigh Homes', 'Mr M J Press', 'Mr M J Ryan', 'Mr M Jarmyn', 'Mr M M Tebyanyan', 'Mr M Mangiola', 'Mr M Miljevic', 'Mr M Mohammadi', 'Mr M Nocera', 'Mr M P Millar', 'Mr M Pilcher', 'Mr M Radakovitch', 'Mr M T Hall', 'Mr M W Baker', 'Mr M W Hoy', 'Mr N Cavuoto', 'Mr N Cooke', 'Mr N D White', 'Mr N Goulding', 'Mr N Im', 'Mr N J Hall', 'Mr N J Lock', 'Mr N J Staker', 'Mr N K Grabowski', 'Mr N Karantonis', 'Mr N R Wooster', 'Mr N S Zeunert and Ms T M Staines', 'Mr O B Baltazar', 'Mr P B Brentson', 'Mr P Chan', 'Mr P D Corbin', 'Mr P D Farrow', 'Mr P D Reed', 'Mr P G Dezen', 'Mr P H Buch', 'Mr P I Daly', 'Mr P J Bain', 'Mr P J Cannell and Mrs M D Cannell', 'Mr P K Engel and Ms L Engel', 'Mr P L J Baulderstone', 'Mr P L Jeffs', 'Mr P N Gambranis', 'Mr P Nhanh', 'Mr P P J Corbran', 'Mr P R Ellis', 'Mr P Reynolds', 'Mr P S Brar', 'Mr P S Morris', 'Mr P Suchocki', 'Mr R A Barker', 'Mr R Brooks', 'Mr R C Gonzales', 'Mr R C Martin', 'Mr R C Page', 'Mr R C Pilgrim and Ms M Pilgrim', 'Mr R C Wendelborn', 'Mr R D Barrett', 'Mr R D Strehler', 'Mr R Deborsey', 'Mr R E Day', 'Mr R F De Bortoli', 'Mr R F Hussey', 'Mr R Fimmano', 'Mr R G Ellis', 'Mr R G Wilkes and Mrs Y A Wilkes', 'Mr R Hill', 'Mr R Iannella', 'Mr R J Duffield', 'Mr R J Kennedy', 'Mr R J Sharp', 'Mr R J Vast', 'Mr R J Winter', 'Mr R J Young and Miss D K Young', 'Mr R K Bandtock', 'Mr R K Williams', 'Mr R L Damiani and Olympic Industries', 'Mr R Lal', 'Mr R M A Owens', 'Mr R Monti', 'Mr R Muir', 'Mr R Pepper', 'Mr R Rende', 'Mr R V Jordan', 'Mr R Varacalli', 'Mr R W Hill', 'Mr R W Jameson', 'Mr R Winfield', 'Mr R Zwezerijnen', 'Mr S A Ashby', 'Mr S A Jenke', 'Mr S A M Woods', 'Mr S A M Woodward', 'Mr S A Wotton', 'Mr S C Smith', 'Mr S Casey', 'Mr S D Johnson', 'Mr S D Morris', 'Mr S D Newitt', 'Mr S D Sefton', 'Mr S Du Preez', 'Mr S F M Blott', 'Mr S G Osborne', 'Mr S Ibrahimi', 'Mr S J Barlow', 'Mr S J Coward', 'Mr S J Cryer', 'Mr S J Morgan', 'Mr S J Passmore', 'Mr S J Rankine', 'Mr S J Selley', 'Mr S J Wicik', 'Mr S J Y Chan and Ms H K W Li', 'Mr S Kafantaris', 'Mr S Kirkwood', 'Mr S Koulianos', 'Mr S L Long', 'Mr S L Nicol', 'Mr S L Tonellato', 'Mr S M Kimongo', 'Mr S M Norton', 'Mr S M Thomas', 'Mr S Noto', 'Mr S P Arbon', 'Mr S P Kilpatrick', 'Mr S Peregi', 'Mr S R Powney', 'Mr S Schutt', 'Mr S Syrianos', 'Mr S T Walters', 'Mr S Wearing-Smith', 'Mr T A Bodycote', 'Mr T Cambareri', 'Mr T Jones', 'Mr T K Margitich', 'Mr T N Minett', 'Mr T P Wasley', 'Mr T Phillips', 'Mr T R Subedi', 'Mr T Shannon', 'Mr T Song', 'Mr T T Kontos', 'Mr T T Nguyen', 'Mr T Treverton', 'Mr V Bzikadze', 'Mr V J Callus', 'Mr V V Badea', 'Mr W A Wilson', 'Mr W King', 'Mr W L Birch', 'Mr W L Stevens', 'Mr W Lennon', 'Mr W T Davey', 'Mrs A L Walters and Mr S T Walters', 'Mrs A M Ferres', 'Mrs A S McGuffie', 'Mrs A Virgara and Mr A Virgara', "Mrs B C D'Arcy", 'Mrs C E Stewart-Watt', 'Mrs C Enalanga', 'Mrs C M Shoumack', 'Mrs D A J McDonagh', 'Mrs D L Giorgio', 'Mrs D M Moir', 'Mrs D Ryder and Mr A J Ryder', 'Mrs E F Hanauer', 'Mrs E J Chandler', 'Mrs E K Whale', 'Mrs E L Whiteley', "Mrs E M O'Donovan", 'Mrs E Teligiannidis', 'Mrs G D Randall', 'Mrs J K Campbell', 'Mrs J L Silvestri', 'Mrs K Johnston', 'Mrs K W Pilgrim', 'Mrs L A Dezen', 'Mrs M E Costello', 'Mrs N Luke', 'Mrs R J Jones', 'Mrs R M Suell', 'Mrs S C Taylor', 'Mrs S Halteh', 'Mrs S J Lotts', 'Mrs T Cianci', 'Mrs T L Pezzaniti and Mr J A Pezzaniti', 'Mrs T R Sears', 'Mrs Y D Matthews', 'Ms A C Pitman-Purdie', 'Ms A D Pengilly', 'Ms A L Greenwood', 'Ms A M Abela', 'Ms A Reed', 'Ms B Smith', 'Ms C E Dunand', 'Ms C H Ruscoe', 'Ms C J Slager', 'Ms C L Brown', 'Ms C L Waite', 'Ms C Lai', 'Ms C Prak', 'Ms C S Herbert', 'Ms C Snook', 'Ms D H Stratton', 'Ms D M Rush and Mr G T Evans', 'Ms E J Carr', 'Ms F Nazari', 'Ms H M Hewitt', 'Ms J A Pascoe', 'Ms J J Valentijn', 'Ms J L Cox', 'Ms J M Gull', 'Ms J M Zielinski', 'Ms J Sutton', 'Ms J Whitlock', 'Ms K A Ritonja', 'Ms K E Keane', 'Ms K H Lee', 'Ms K L McInnes', 'Ms K Laverty', 'Ms L A Treloar', 'Ms L K D Prosser', 'Ms L K Scott', 'Ms M Ellis', 'Ms M J Tonkin', 'Ms M L Ralph', 'Ms M R Johnson', 'Ms M R Zollo', 'Ms N M French', 'Ms N R Costello and Mr A Maurici', 'Ms N Viant', 'Ms P A Johnson', 'Ms R G Freeman', 'Ms R L Allen', 'Ms R L Damiani', 'Ms S Biacca', 'Ms S J Maschotta', 'Ms S J Morse', 'Ms S J Western and Mr S W Bradshaw', 'Ms S L Payne', 'Ms S M Lavery', 'Ms S N Mells', 'Ms S Paltridge', 'Ms T J Truscott', 'Ms T L Pascoe', 'Ms T Sare', 'Ms V Howson', 'Ms W S Eyers', 'Multichoice Building Services', 'Murfman6 Pty Ltd', 'My Dezign Exteriors', 'My Health Engine Pty Ltd', 'My Living Outdoors', 'N Paiva and A Hussaini', 'N Prak', 'N Yangnovong', 'Network Carports &amp; Verandahs', 'Nevarc Constructions Pty Ltd', 'Nevarc Constructions Pty Ltd and Oakford Homes', 'Ngen Design', 'North MP East Holdings Pty Ltd', 'Northern Shed Works', 'Northern Verandah Supplies', 'Northwest Healthcare Aust Propery Pty Ltd', 'Number One Nominees Pty Ltd', 'Oakford Homes', 'Oakford Homes and Nevarc Constructions Pty Ltd', 'Olympic Industries', 'One SA Pty Ltd', 'P B S Aust', 'P Geracitano', 'P Herbert', 'P McIver', 'P Singlewood', 'P Thwaites', 'P Whittaker and Gannon Lifestyle Pty Ltd', 'PC Infrastructure Pty Ltd', 'Palumbo Building Pty Ltd', 'Palumbo Pty Ltd', 'Panel Homes SA', 'Peats Group', 'Penfield Complex Pty Ltd', 'Pergolas of Distinction', 'Peters Property Group', 'Planning Solutions (Aust) Pty Ltd', 'Premium Home Improvements', 'Premium Roofing &amp; Patios', 'Prestige Pools SA Pty Ltd', 'Pro Form Pergolas Pty Ltd', 'Pro-Form Pergolas', 'R &amp; F M Varacalli Pty Ltd', 'R &amp; M Timber Pty Ltd', 'R B Hill', 'R Gordon', 'R Hanna', 'R M &amp; R C Pty Ltd', 'R Pye', 'Regent Homes', 'Rendition Group', 'Renewal SA', 'Renovus Pty Ltd', 'Revolution Roofing', 'Right Price Roofing', 'Rivergum Homes', 'Rivergum Homes Pty Ltd', 'Riverina Pools &amp; Spas', 'Rossdale Homes Pty Ltd', 'Rotundas &amp; Pergolas of Adelaide', 'Royal Park Salvage', 'Russell Consulting Engineers', 'S Barbieri', 'S Bishop', 'S Fakkas', 'S Ihnatiuc', 'S J Castledine', 'S J Sperrin', 'S Khan', 'S Khun', 'S Lee', 'S McClelland', 'S Nguyen', 'S Rajsekharan', 'S Stallard', 'S T A Bayati', 'S Votino', 'SA Housing Authority', 'SA Housing Trust', 'SA Pergolas', 'SA Power Networks', 'SA Quality Home Improvements', 'SA Ultimate Home Improvements', 'SA Water - Liveability', 'Sagle Constructions Pty Ltd', 'Scouts Australia SA Branch', 'Selecta Homes &amp; Building Co Pty Ltd', 'Sfeer Building Design', 'Shadeform Sailshades', 'Shreenarayan Holdings Pty Ltd', 'Shutta Ya Place', 'Simonds Homes SA', 'Sky Construction &amp; Development', 'Softwoods Timberyards', 'Softwoods Timberyards Pty Ltd', 'Solarlab Pty Ltd', 'South Central Renovations', 'Spa Mart', 'Spartan Plans &amp; Building Services', 'Spectra Building Designers', 'Sri Krishna Investors Pty Ltd', 'State Surveys', 'Statewide Pools', 'Steps Building Services', 'Sterling Homes Pty Ltd', 'Subdivision Solutions', 'Superb Pergolas N Decks', 'T Graham', 'T Hang', 'T Kosmidis', 'T Nguyen', 'T Smith', 'TAFE SA - Elizabeth Campus', 'TMK Consulting Engineers', 'Taking Care of Trees', 'Talent Plumbing', 'The 2a Architectural Studio', 'The Galvin Group', 'The Pergola Man', 'The Trademan', 'Total Space Design Pty Ltd', 'Trinity College Gawler Inc', 'UPM Plumbing &amp; Excavations', 'Unitech Building', 'Urban Renewal Authority', 'Urban3', 'Utter Gutters', 'V Maraviya', 'V N Vuppalapati', 'Vergola Pty Ltd', 'WG Developments Pty Ltd', 'Water Technology', 'Watt Preah Puth Mean Chey Assoc Inc', 'Watusi LJ Pty Ltd', 'Weathersafe Shades Pty Ltd', 'Webb Constructions (SA) Pty Ltd', 'Weeks Building Group', 'Welcome Home Enterprises', 'Z Cai', 'Z Yin', 'Zappall Family Trust']</t>
+          <t>['********** PRIVATE **********', '365 Studio Pty Ltd', '3MT Solutions Pty Ltd', '41 Barfield Pty Ltd', '43 Barfield Pty Ltd', 'A Asteris', 'A Bragg', 'A Breeze', 'A Horn', 'A L Russell', 'A Morgado', 'A Robertson', 'A Sapic', 'A Sharma', 'A Sims', 'A Smith', 'A Tebyanyan', 'A V Jennings', 'A V Jennings Pty Ltd', 'A Valiff', 'AAT Building', 'ABC Homes Pty Ltd', 'ACH Group', 'AH Design &amp; Drafting', 'APM Plumbing', 'Abel Home Improvements', 'Access SDM Pty Ltd', 'Actium Land Developments Pty Ltd', 'Adelaide Builders Pty Ltd', 'Adelaide Building Consulting', 'Adelaide Designer Homes Pty Ltd', 'Adelaide Insurance Builders', 'Adelaide Nominees Pty Ltd', 'Adelaide Retaining Walls', 'Aerobic Tech Pty Ltd', 'Ahrens Engineering', 'Albury Wodonga Community College', 'Aldinga Home Improvements', 'Alete Homes Pty Ltd', 'Alexander Symonds Pty Ltd', 'Alif Homes', 'All Sites Welding Services', 'Alpha Industries', 'Alpha Industries - Glandore', 'Andrash Commercial Pty Ltd', 'Andrew Evans Plumbing', 'Anglicare SA Housing Ltd', 'Anthony Donato Architects', 'Apalie Drive Pty Ltd', 'Apex Greenhouses', 'Apex Greenhouses Aust Pty Ltd', 'Apex Home Improvements', 'Aspire Homes SA Pty Ltd', 'Astrad Pty Ltd', 'Atelier 18 Pty Ltd', 'Attica Homes', 'Aust Child Care Career', 'Aust Outdoor Living', 'Australian Building Company', 'Australian Outdoor Living', 'Australian Workplace Training', 'B A Mebberson', 'B Cox', 'B Goyal', 'B Pring', 'B Thomas and Bargain Steel Centre', 'B Van Groesen', 'Ballavarra Pty Ltd', 'Baracuda Holdings Pty Ltd', 'Bargain Steel Centre', 'Barossa Pergolas &amp; Outdoor Concepts', 'Beechwood Homes', 'Bella Build &amp; Design', 'Better Built Industries', 'Big Difference Home Improvement', 'Botanic Dreams Pty Ltd', 'Bovpap Pty Ltd', 'Bradford Homes', 'Brightspace Homes', 'Brookmont Property Developments Pty Ltd', 'Brooks Development Services', 'Brooks Development Services Pty Ltd', 'Budget Built Home Additions', 'Burbank Aust (SA) Pty Ltd', 'Burns for Blinds', 'Burton Demolition Pty Ltd', 'C Biven', 'C Grimaldi', 'C Liebeknecht', 'C R Hansford', 'C Stevenson', 'C Stock', 'C Yu', 'CT Group Properties No 4 Pty Ltd', 'Cafcakis Nominees and Mr E Cafcakis', 'Catholic Archdiocese of Adelaide', 'Catholic Education SA', 'Century North Pty Ltd', 'Changhui Construction Pty Ltd', 'Chapley Nominees Pty Ltd', 'Checkpoint Building Surveyors', 'City of Playford', 'City of Playford Sports &amp; Property Team', 'Classic Pools &amp; Spas', 'Cocercan Pty Ltd', 'Colcon (NT) Pty Ltd', 'Collins Adelaide', 'Collins Transport', 'Comfresh Pty Ltd', 'Construction Services Aust Pty Ltd', 'Creative Outdoors', 'Crisio Investments Pty Ltd', 'D Clarke', 'D Harris', 'D Knezic', 'D Lobbe', 'D Martyr', 'D Rawat', 'D Turnbull', 'D W Rogers', 'D2c Services', 'DMV Outdoor Solutions', 'DPTI Rail Commissioner', 'Dechellis Homes', 'Department for Education', 'Department for Education - Das Studio', 'Department of Education/Tesa', 'Dept for Education', 'Dept for Infrastructure &amp; Transport', 'Design Constructive Pty Ltd', 'Detail Studio Pty Ltd', 'Diamanti Design Development', 'Dimension Design Studio', 'Distinctive Homes Pty Ltd', 'Dominion Homes', 'Dominos Pizza Enterprises', 'Drug &amp; Alcohol Services SA', 'E Bidhendi', 'Eco Construction &amp; Project Management', 'Elite Pools &amp; Landscapes', 'Elizabeth RSL', 'Emmett JV Pty Ltd', 'Emmett Property Pty Ltd', 'Est Late Mr V Bzikadze', 'Everclear Pool Solutions', 'Exquisite Brows Pty Ltd', 'F Ahmadi', 'F Condelli', 'Faculty Design', 'Fairland Homes Group Pty Ltd', 'Fairmont Homes Group Pty Ltd', 'Fairmont Land Holdings Pty Ltd', 'Farrago Interiors', 'First Choice Verandahs &amp; Carports', 'Format Homes Pty Ltd', 'Fortune Living', 'Frank Nesci Homes', 'Freedom Pools', 'Frenchys Fix It', 'Fyfe Pty Ltd', "G D'Agostino", 'G P Forensic', 'G Smith', 'Garrad Plumbing &amp; Civil', 'Gawler Pergola &amp; Timber Supplies', 'Genis Steel', 'Giudel Developments Pty Ltd', 'Goostrey Smith Design', 'Grove Concepts', 'H Hinrichsen', 'H Li', 'H Sheridan', 'H Vo', 'HBB Property', 'Hawke &amp; Co Pty Ltd', 'Hayden Sheriden', 'Haywood Carpentry', 'Henley Arch Pty Ltd', 'Holmes Dyer', 'Homecorp Constructions SA', 'Homestart Finance Ltd', 'Homestyle Living Outdoors', 'Hot Property Group', 'Hunter Property Solutions Pty Ltd', 'Hyde Park Projects Pty Ltd', 'I Singh', 'IJ Projects', 'Iconic Roofing', 'Impressive Patios', 'Inception Design', 'Inspire Design Studio', 'J &amp; S Pergola Installations', 'J A Alexander', 'J A Lewis Nominees Pty Ltd', 'J Barbis', 'J Brimer', 'J Cabangal', 'J D Water Pty Ltd', 'J Harvey', 'J Hayes', 'J J J Services Pty Ltd', 'J Mead', 'J Palmer', 'J Pugh', 'J Rullo', 'J S Hales', 'JVT Holdings Pty Ltd', "Joe's Golden Gasoline Classic Imports Pty Ltd", 'K A Yovan', 'K Ahmadi', 'K Enoka', 'K Ferguson and Mr S A Ferguson', 'K G Drafting &amp; Development Services', 'K Gourlay', 'K Humphreys', 'K P Cherayaramal', 'K Singh', 'K Sokhom', 'Keeping Up Appearances Group Pty Ltd', 'Klhp Family Trust', 'L Abalos', 'L Pawar', 'Lake Maintenance', 'Lamato Property Holdings Pty Ltd', 'Lanser Communities Pty Ltd', 'Leipzig Aust Property Pty Ltd', 'Leipzig Australia Property Trust 2', 'Level Earthworx', 'Levett Engineering Pty Ltd', 'Lifestyle Pergolas', 'Lionsgate Elizabeth (Pelligra) Pty Ltd', 'Lodge Construction &amp; Building Pty Ltd', 'Lofty Building Group', 'Longridge Group Pty Ltd', 'Louvre House (SA)', 'M A Najafi', 'M Branch', 'M C Pergolas', 'M Dench', 'M Galinato', 'M Garnett', 'M Irwin', 'M King', 'M L Schories', 'M Mickan', 'M N Salehi', 'M Pavic', 'M Rani', 'M Schwientek', 'M Wilson and Anglicare SA', 'M2 Architectural Design', 'M2A2 Hillier Pty Ltd', 'Magill Demolition', 'Mahogany Homes', 'Maiden Estate Pty Ltd', 'Mark Willis Excavations', 'Master Homes of Adelaide Pty Ltd', 'Masterplan SA Pty Ltd', 'Matthews Architects', 'Maybach Property Group', 'Metal As Anything (Kadina)', 'Metricon Homes Pty Ltd', 'Metro (SA) Housing Pty Ltd', 'Metro Homes SA', 'Minister for Infrastructure &amp; Transport', 'Miravale Joint Venture', 'Miss A Karagozlu', 'Miss G R Badea', 'Miss J Fittes', 'Miss V L Kilsby', 'Mitolo Group Pty Ltd', 'Mojo Outdoor Constructions Pty Ltd', 'Mr A A Clarke', 'Mr A A Lombardi', 'Mr A A Paul and Mrs E M Paul', 'Mr A Almas', 'Mr A B Dube and Ms A V Forwood', 'Mr A B Todd', 'Mr A Bhamra', 'Mr A D Wallis', 'Mr A F Johnson', 'Mr A G Clarke', 'Mr A G Kruse', 'Mr A H Krieger', 'Mr A J Bossy', 'Mr A J C Swyghuizen', 'Mr A J Kley', 'Mr A J Kovarik', 'Mr A J Sharp', 'Mr A J Stunell', 'Mr A L Xanthopoulos', 'Mr A Lediaev', 'Mr A M Alimi', 'Mr A M Cottrell', 'Mr A M Elliott', 'Mr A N Scutcheon', "Mr A O'Leary", 'Mr A R Borhani', 'Mr A R Tiedau', 'Mr A Ragno', 'Mr A Romaniuk', 'Mr A Russell-Price and Mr T Robinson', 'Mr A S Minopoulos', 'Mr A S Pickett', 'Mr A Sorrenti', 'Mr A T Preen', 'Mr A Taneja', 'Mr A V Coniglio', 'Mr A V Manno and Mrs K Manno', 'Mr A V Vadnere', 'Mr A W Dix', 'Mr A W Mohring', 'Mr A Zummo', 'Mr B A Singlewood', 'Mr B C Crook', 'Mr B C Day', 'Mr B C Nikou', 'Mr B Coppock', 'Mr B D Wastell', 'Mr B E Goddard', 'Mr B G Hudson', 'Mr B J Woodrow', 'Mr B M Arnold', 'Mr B M Ellis', 'Mr B N Jensen', 'Mr B Newman', 'Mr B P Jamieson', 'Mr B R Prior', 'Mr B Round', 'Mr B S Danzic', 'Mr B Stjepanovic', 'Mr B Vertudaches', 'Mr C A Dawe', 'Mr C A Knowles', 'Mr C D Bishop', 'Mr C D Thornton', 'Mr C H Noble', 'Mr C I Deuter', 'Mr C J Duff', 'Mr C J Eckberg', 'Mr C J Hopgood', 'Mr C J Larson', 'Mr C L Green', 'Mr C Laftsis', 'Mr C M Barrett', 'Mr C M Gutteridge', 'Mr C Petris', 'Mr C Puccini', 'Mr C R Wild', 'Mr D A Beverley', 'Mr D B To', 'Mr D Barton and Mrs J A Barton', 'Mr D Bjelja', 'Mr D Brealey', 'Mr D C Hoppo', 'Mr D E Craddock', 'Mr D Green', 'Mr D J Bastiras', 'Mr D J Kirby', 'Mr D J Launer', 'Mr D J McAnoy', 'Mr D L Boyce', 'Mr D L Goddard', 'Mr D L Van Der Meer', 'Mr D M Peel', 'Mr D M R Pregarz', 'Mr D N Bubner', 'Mr D P Tregenza', 'Mr D R Cockburn', 'Mr D S Dutschke', 'Mr D S R Williams', 'Mr D S Smith', 'Mr D S Zalewski', 'Mr D Shinakis', 'Mr D Spavin', 'Mr D Teurer and Ms A Teurer', 'Mr D W Fenner', 'Mr D W Fleming', 'Mr D Welch', 'Mr D X Ly', 'Mr E J McQueer', 'Mr E K Rendell', 'Mr E Napoli', 'Mr F R Smith', 'Mr F S Catanzariti', 'Mr G A Howarth and Ms K L Gittus', 'Mr G A Jamieson', 'Mr G C Muscat', 'Mr G Hick', 'Mr G J Davis', 'Mr G Marsh', 'Mr G N Willey', 'Mr G Nichinonni', 'Mr G P Coy', 'Mr G R Page and Mrs L A Page', 'Mr G W Kercher', 'Mr H Antoniou', 'Mr H D Tonkin', 'Mr H J McLean', 'Mr H Tran', 'Mr I Alrefae', 'Mr I Dichiera', 'Mr I Duncan', 'Mr I Ozdemir', 'Mr I Panetta', 'Mr I W Matthews', 'Mr J A Comelli', 'Mr J A Johnston', 'Mr J B Dearing', 'Mr J B T Scheepens and Mrs M Scheepens', 'Mr J B Thorogood', 'Mr J C Muke', 'Mr J D Goldfinch', 'Mr J D Moloney', 'Mr J D Watson', 'Mr J Duffy', 'Mr J Grima', 'Mr J Iacopetta', 'Mr J Imin', 'Mr J J McCormack', 'Mr J K Elliott', 'Mr J K Hutchinson', 'Mr J L Nichols', 'Mr J L Saunders', 'Mr J Maiolo', 'Mr J McGilvray', 'Mr J P Abraham', 'Mr J P Knevitt', 'Mr J P Snoad', 'Mr J P W Henkel', 'Mr J R Settre', 'Mr J S Kavasi', 'Mr J T Purdie and Mrs C A Purdie', 'Mr J Thomas', 'Mr J W Buhagiar', 'Mr J W Prince and Ms E E Prince', 'Mr J W Spong', 'Mr J Yin', 'Mr K A Cussion', 'Mr K Barlow', 'Mr K Bridger', 'Mr K C Fischer', 'Mr K D Van Schaijik', 'Mr K E A D Nicholls', 'Mr K H Bruns', 'Mr K H Schaefer', 'Mr K K Carypidis', 'Mr K M Thompson', 'Mr K S Aung', 'Mr K W Menadue', 'Mr L A Sanchez', 'Mr L Behn', 'Mr L D Trenorden', 'Mr L Dimanno', 'Mr L Doubleday', 'Mr L I Hardy', 'Mr L J Cooper', 'Mr L J Matthews and Ms L R Matthews', 'Mr L Mayes', 'Mr L Piscioneri', 'Mr L S Duke-Smith', 'Mr L Thomas', 'Mr L W Bentley', 'Mr M A B Shiddik', 'Mr M A Hutchens', 'Mr M A Owen', 'Mr M Borg', 'Mr M Boyle', 'Mr M Brady', 'Mr M C J Nudo', 'Mr M C Pocock', 'Mr M D Campbell', 'Mr M D Hood', 'Mr M Dawson', 'Mr M E Turner', 'Mr M Egel', 'Mr M G Moss', 'Mr M H Krieger', 'Mr M Hatungimana', 'Mr M J Cane', 'Mr M J Fletcher', 'Mr M J Haywood', 'Mr M J Hughes', 'Mr M J Jacka', 'Mr M J Lawrence', 'Mr M J Loechel', 'Mr M J Palmer', 'Mr M J Palmer and Barkleigh Homes', 'Mr M J Press', 'Mr M J Ryan', 'Mr M Jarmyn', 'Mr M M Tebyanyan', 'Mr M Mangiola', 'Mr M Miljevic', 'Mr M Mohammadi', 'Mr M Nocera', 'Mr M P Millar', 'Mr M Pilcher', 'Mr M Radakovitch', 'Mr M T Hall', 'Mr M W Baker', 'Mr M W Hoy', 'Mr N Cavuoto', 'Mr N Cooke', 'Mr N D White', 'Mr N Goulding', 'Mr N Im', 'Mr N J Allen', 'Mr N J Hall', 'Mr N J Lock', 'Mr N J Staker', 'Mr N K Grabowski', 'Mr N Karantonis', 'Mr N R Wooster', 'Mr N S Zeunert and Ms T M Staines', 'Mr O B Baltazar', 'Mr P B Brentson', 'Mr P Chan', 'Mr P D Corbin', 'Mr P D Farrow', 'Mr P D Reed', 'Mr P G Dezen', 'Mr P H Buch', 'Mr P I Daly', 'Mr P J Bain', 'Mr P J Cannell and Mrs M D Cannell', 'Mr P J Day', 'Mr P K Engel and Ms L Engel', 'Mr P L J Baulderstone', 'Mr P L Jeffs', 'Mr P N Gambranis', 'Mr P Nhanh', 'Mr P P J Corbran', 'Mr P R Ellis', 'Mr P Reynolds', 'Mr P S Brar', 'Mr P S Morris', 'Mr P Suchocki', 'Mr R A Barker', 'Mr R Brooks', 'Mr R C Gonzales', 'Mr R C Martin', 'Mr R C Page', 'Mr R C Pilgrim and Ms M Pilgrim', 'Mr R C Wendelborn', 'Mr R D Barrett', 'Mr R D Strehler', 'Mr R Deborsey', 'Mr R E Day', 'Mr R F De Bortoli', 'Mr R F Hussey', 'Mr R Fimmano', 'Mr R G Ellis', 'Mr R G Wilkes and Mrs Y A Wilkes', 'Mr R Hill', 'Mr R Iannella', 'Mr R J Duffield', 'Mr R J Kennedy', 'Mr R J Sharp', 'Mr R J Vast', 'Mr R J White', 'Mr R J Winter', 'Mr R J Young and Miss D K Young', 'Mr R K Bandtock', 'Mr R K Williams', 'Mr R L Damiani and Olympic Industries', 'Mr R Lal', 'Mr R M A Owens', 'Mr R Maiolo and Mr F Maiolo', 'Mr R Monti', 'Mr R Muir', 'Mr R Pepper', 'Mr R Rende', 'Mr R V Jordan', 'Mr R V Kirkham', 'Mr R Varacalli', 'Mr R W Hill', 'Mr R W Jameson', 'Mr R Winfield', 'Mr R Zwezerijnen', 'Mr S A Ashby', 'Mr S A Hosseini', 'Mr S A Jenke', 'Mr S A M Woods', 'Mr S A M Woodward', 'Mr S A Valiff', 'Mr S A Wotton', 'Mr S C Smith', 'Mr S Casey', 'Mr S D Johnson', 'Mr S D Laming', 'Mr S D Morris', 'Mr S D Newitt', 'Mr S D Sefton', 'Mr S Du Preez', 'Mr S F M Blott', 'Mr S G Osborne', 'Mr S Ghyas', 'Mr S Ibrahimi', 'Mr S J Barlow', 'Mr S J Coward', 'Mr S J Cryer', 'Mr S J Morgan', 'Mr S J Passmore', 'Mr S J Rankine', 'Mr S J Selley', 'Mr S J Wicik', 'Mr S J Y Chan and Ms H K W Li', 'Mr S K Cahill', 'Mr S Kafantaris', 'Mr S Kirkwood', 'Mr S Koulianos', 'Mr S L Long', 'Mr S L Nicol', 'Mr S L Tonellato', 'Mr S M Kimongo', 'Mr S M Norton', 'Mr S M Thomas', 'Mr S Noto', 'Mr S P Arbon', 'Mr S P Kilpatrick', 'Mr S Peregi', 'Mr S R Powney', 'Mr S Schutt', 'Mr S Syrianos', 'Mr S T Walters', 'Mr S W Duncan', 'Mr S Wearing-Smith', 'Mr T A Bodycote', 'Mr T Cambareri', 'Mr T Jones', 'Mr T K Margitich', 'Mr T N Minett', 'Mr T P Wasley', 'Mr T Phillips', 'Mr T R Subedi', 'Mr T Shannon', 'Mr T Song', 'Mr T T Kontos', 'Mr T T Nguyen', 'Mr T Treverton', 'Mr V J Callus', 'Mr V V Badea', 'Mr W A Wilson', 'Mr W King', 'Mr W L Birch', 'Mr W L Stevens', 'Mr W Lennon', 'Mr W T Davey', 'Mrs A L Walters and Mr S T Walters', 'Mrs A M Ferres', 'Mrs A S McGuffie', 'Mrs A Virgara and Mr A Virgara', "Mrs B C D'Arcy", 'Mrs C E Stewart-Watt', 'Mrs C Enalanga', 'Mrs C M Shoumack', 'Mrs D A J McDonagh', 'Mrs D L Giorgio', 'Mrs D M Moir', 'Mrs D M Tipping', 'Mrs D Ryder and Mr A J Ryder', 'Mrs E F Hanauer', 'Mrs E J Chandler', 'Mrs E K Whale', 'Mrs E L Whiteley', "Mrs E M O'Donovan", 'Mrs E Teligiannidis', 'Mrs F M Ryan', 'Mrs G D Randall', 'Mrs J K Campbell', 'Mrs J L Silvestri', 'Mrs K Johnston', 'Mrs K W Pilgrim', 'Mrs L A Dezen', 'Mrs M A Parletta', 'Mrs M E Costello', 'Mrs N Luke', 'Mrs R J Jones', 'Mrs R M Suell', 'Mrs S C Taylor', 'Mrs S Halteh', 'Mrs S J Lotts', 'Mrs T Cianci', 'Mrs T Jones', 'Mrs T L Pezzaniti and Mr J A Pezzaniti', 'Mrs T R Sears', 'Mrs Y D Matthews', 'Ms A C Pitman-Purdie', 'Ms A D Pengilly', 'Ms A L Greenwood', 'Ms A M Abela', 'Ms A Reed', 'Ms B Smith', 'Ms C E Dunand', 'Ms C H Ruscoe', 'Ms C J Slager', 'Ms C L Brown', 'Ms C L Waite', 'Ms C Lai', 'Ms C Prak', 'Ms C S Herbert', 'Ms C Snook', 'Ms D H Stratton', 'Ms D M Rush and Mr G T Evans', 'Ms E J Carr', 'Ms F Delaney', 'Ms F Nazari', 'Ms H M Hewitt', 'Ms J A Pascoe', 'Ms J F Adamson', 'Ms J J Valentijn', 'Ms J L Cox', 'Ms J M Gull', 'Ms J M Zielinski', 'Ms J Sutton', 'Ms J Whitlock', 'Ms K A Ritonja', 'Ms K E Keane', 'Ms K H Lee', 'Ms K L McInnes', 'Ms K Laverty', 'Ms L A Treloar', 'Ms L K D Prosser', 'Ms L K Scott', 'Ms M Ellis', 'Ms M J Tonkin', 'Ms M L Ralph', 'Ms M R Johnson', 'Ms M R Zollo', 'Ms N M French', 'Ms N R Costello and Mr A Maurici', 'Ms N Viant', 'Ms P A Johnson', 'Ms R G Freeman', 'Ms R L Allen', 'Ms R L Damiani', 'Ms S Biacca', 'Ms S J Fleming', 'Ms S J Maschotta', 'Ms S J Morse', 'Ms S J Western and Mr S W Bradshaw', 'Ms S L Payne', 'Ms S M Lavery', 'Ms S N Mells', 'Ms S Paltridge', 'Ms T J Truscott', 'Ms T L Pascoe', 'Ms T Sare', 'Ms V Howson', 'Ms W S Eyers', 'Multichoice Building Services', 'Murfman6 Pty Ltd', 'My Dezign Exteriors', 'My Health Engine Pty Ltd', 'My Living Outdoors', 'N Paiva and A Hussaini', 'N Prak', 'N Yangnovong', 'Network Carports &amp; Verandahs', 'Nevarc Constructions Pty Ltd', 'Nevarc Constructions Pty Ltd and Oakford Homes', 'Ngen Design', 'Nguyen SA', 'North MP East Holdings Pty Ltd', 'Northern Shed Works', 'Northern Verandah Supplies', 'Northwest Healthcare Aust Propery Pty Ltd', 'Number One Nominees Pty Ltd', 'Oakford Homes', 'Oakford Homes and Nevarc Constructions Pty Ltd', 'Olympic Industries', 'One SA Pty Ltd', 'P B S Aust', 'P Geracitano', 'P Herbert', 'P McIver', 'P Singlewood', 'P Thwaites', 'P Whittaker and Gannon Lifestyle Pty Ltd', 'PC Infrastructure Pty Ltd', 'Palumbo Building Pty Ltd', 'Palumbo Pty Ltd', 'Panel Homes SA', 'Peats Group', 'Penfield Complex Pty Ltd', 'Pergolas of Distinction', 'Peters Property Group', 'Planning Solutions (Aust) Pty Ltd', 'Playford Primary School', 'Premium Home Improvements', 'Premium Roofing &amp; Patios', 'Prestige Pools SA Pty Ltd', 'Pro Form Pergolas Pty Ltd', 'Pro-Form Pergolas', 'R &amp; F M Varacalli Pty Ltd', 'R &amp; M Timber Pty Ltd', 'R B Hill', 'R Gilbert', 'R Gordon', 'R Hanna', 'R M &amp; R C Pty Ltd', 'R Pye', 'Reach Energy Storage Co', 'Regent Homes', 'Rendition Group', 'Rendition Homes', 'Renewal SA', 'Renovus Pty Ltd', 'Revolution Roofing', 'Right Price Roofing', 'Rivergum Homes', 'Rivergum Homes Pty Ltd', 'Riverina Pools &amp; Spas', 'Rossdale Homes Pty Ltd', 'Rotundas &amp; Pergolas of Adelaide', 'Royal Park Salvage', 'Russell Consulting Engineers', 'S Barbieri', 'S Bishop', 'S Fakkas', 'S Furqan', 'S Ihnatiuc', 'S J Castledine', 'S J Sperrin', 'S K Maybury', 'S Khan', 'S Khun', 'S Lee', 'S McClelland', 'S Nguyen', 'S Rajsekharan', 'S Stallard', 'S T A Bayati', 'S Votino', 'SA Housing Authority', 'SA Housing Trust', 'SA Pergolas', 'SA Power Networks', 'SA Quality Home Improvements', 'SA Ultimate Home Improvements', 'SA Water - Liveability', 'Sagle Constructions Pty Ltd', 'Scouts Australia SA Branch', 'Selecta Homes &amp; Building Co Pty Ltd', 'Sfeer Building Design', 'Shade SA', 'Shadeform Sailshades', 'Shreenarayan Holdings Pty Ltd', 'Shutta Ya Place', 'Simonds Homes SA', 'Sketch &amp; Build Pty Ltd', 'Sky Construction &amp; Development', 'Softwoods Timberyards', 'Softwoods Timberyards Pty Ltd', 'Solarlab Pty Ltd', 'South Central Renovations', 'Spa Mart', 'Spartan Plans &amp; Building Services', 'Spectra Building Designers', 'Sri Krishna Investors Pty Ltd', 'State Surveys', 'Statewide Pools', 'Steps Building Services', 'Sterling Homes Pty Ltd', 'Subdivision Solutions', 'Superb Pergolas N Decks', 'T Graham', 'T Hang', 'T Kosmidis', 'T Nguyen', 'T Smith', 'TAFE SA - Elizabeth Campus', 'TMK Consulting Engineers', 'Taking Care of Trees', 'Talent Plumbing', 'Tecon Aust Pty Ltd', 'The 2a Architectural Studio', 'The Galvin Group', 'The Pergola Man', 'The Trademan', 'Think Architects', 'Total Space Design Pty Ltd', 'Trinity College Gawler Inc', 'UPM Plumbing', 'UPM Plumbing &amp; Excavations', 'Unitech Building', 'Urban Renewal Authority', 'Urban3', 'Utter Gutters', 'V Maraviya', 'V N Vuppalapati', 'Vergola Pty Ltd', 'WG Developments Pty Ltd', 'Water Technology', 'Watt Preah Puth Mean Chey Assoc Inc', 'Watusi LJ Pty Ltd', 'Weathersafe Shades Pty Ltd', 'Webb Constructions (SA) Pty Ltd', 'Weeks Building Group', 'Welcome Home Enterprises', 'Z Cai', 'Z Yin', 'Zappall Family Trust', 'Zappia Consulting Pty Ltd', 'Zummo Design']</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -968,7 +968,7 @@
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P6" t="n">
         <v>0</v>
@@ -983,7 +983,7 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>15 Abelia Street</t>
+          <t>881 Main North Road</t>
         </is>
       </c>
       <c r="T6" t="n">
@@ -995,20 +995,20 @@
         </is>
       </c>
       <c r="V6" t="n">
-        <v>385</v>
+        <v>452</v>
       </c>
       <c r="W6" t="n">
         <v>0</v>
       </c>
       <c r="X6" t="n">
-        <v>40391</v>
+        <v>45289</v>
       </c>
       <c r="Y6" t="n">
-        <v>782</v>
+        <v>838</v>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>['*****************************', '1 Bain Street', '1 Crace Court', '1 Crown Street', '1 Fergusson Bowl', '1 Grampain Street', '1 Joes Court', '1 Lisa Court', '1 Rhus Avenue', '1 Tarana Court', '1 Tatura Court', '1 Westbury Court', '1-3 Dewer Avenue', '1/ Lot 72 Paxton Street', '1/121 Angle Vale Road', '1/18-22 Provident Avenue', '1/198 Greenhill Road', '1/28 Chellaston Road', '1/280 Payneham Road', '1/52 Ron Parkison Crescent', '1/8 Deuter Road', '10 Africaine Avenue', '10 Alderwood Court', '10 Bracken Avenue', '10 Breamore Street', '10 Brookfield Street', '10 Cartwright Drive', '10 Christine Avenue', '10 Epsom Street', '10 Goddard Drive', '10 Karinga Crescent', '10 Keysley Street', '10 Liebrooke Boulevard', '10 Magnolia Crescent', '10 Marles Court', '10 Pendolino Road', '10 Shah Place', '10 Strawson Road', '10 Ward Street', '101 Port Road', '103 Halsey Road', '104/19 Holdfast Promenade', '104a Muller Road', '106 Halifax Street', '108-110 Mooringe Avenue', '1097 Stebonheath Road', '10a Chardonnay Court', '11 Litchfield Avenue', '11 Metcalfe Avenue', '11 North Street', '11 Pendolino Road', '11 William Street', '110-114 Grange Road', '111 Viney Drive', '114-116 Heaslip Road', '115 Crittenden Road', '115 Sampson Road', '116 Botting Street', '11d Metro Parade', '12 Beatrix Drive', '12 Bishopstone Road', '12 Black Top Road', '12 Cameron Road', '12 Dana Street', '12 Elm Drive', '12 Epsom Street', '12 Federation Close', '12 Fowler Street', '12 Oleander Drive', '12 Palmer Road', '12 Sharrad Court', '12 Stock Road', '12 Sunrise Court', '120 Salisbury Highway', '122 Womma West Road', '125 Galway Avenue', '125-129 Commercial Road', '126b Payneham Road', '13 Brittania Drive', '13 Brock Street', '13 Hughes Avenue', '13 Prelude Circuit', '13 Prosperity Way', '13 Stone Road', '13 Swan Crescent', '13 Treleaven Way', '131 Gawler River Road', '132 Payneham Road', '133 Main South Road', '134 Fullarton Road', '134 Tyeka Drive', '136 McKenzie Road', '137 Angle Vale Road', '138 Penfield Road', '138 Supple Road', '139 Kentish Road', '14 Carmela Avenue', '14 Charlson Street', '14 Clover Court', '14 Crisp Road', '14 Dana Street', '14 Durrington Road', '14 Greenhood Crescent', '14 Hancock Road', '14 Jordon Street', '14 Kapoola Avenue', '14 Lynton Avenue', '14 Mary Street', '14 Prosperity Way', '14 Raymond Road', '14 Talbot Street', '14 Yarnbrook Street', '1415 Main North Road', '143 Lakeside Drive', '144 Halsey Road', '147 Goodman Road', '149 Douglas Drive', '149 Tyeka Drive', '15 Abelia Street', '15 Adams Road', '15 Bailey Road', '15 Bubner Street', '15 Coach House Mews', '15 Collins Street', '15 Hermitage Drive', '15 Jenolan Crescent', '15 Kernel Road', '15 Lawder Road', '15 Penley Avenue', '15 Southern Avenue', '15 Spruance Road', '15 Waterford Circuit', '158 Railway Terrace', '159 Port Road', '15a Fife Street', '15b King William Street', '16 Alderwood Court', '16 Breamore Street', '16 Cameron Road', '16 Honeysuckle Drive', '16 Illawarra Court', '16 Karinga Crescent', '16 Lister Avenue', '16 Michael Crescent', '16 Palari Crescent', '16 Sharrad Court', '16 The Greenway', '16 Tindara Avenue', '16 Warren Road', '1602 Two Wells Road', '161 Brunswick Street', '162 Greenhill Road', '168 Grand Junction Road', '168 Julian Road', '17 Alexander Road', '17 Ariadne Crescent', '17 Bastow Road', '17 Benham Street', '17 Boettcher Road', '17 Dawkins Avenue', '17 Elder Court', '17 Falcon Drive', '17 Fradd Road', '17 Mosterton Road', '17 The Circuit', '17/21 Heaslip Road', '170 Greenhill Road', '18 Bogan Road', '18 Carob Crescent', '18 Elmwood Circuit', '18 Fantasia Drive', '18 Green Crescent', '18 Laburnum Gardens', '18 Lorna Court', '18 Oregon Avenue', '18 Perthville Court', '18 Rosetta Street', '18 Warragal Court', '18 Yarnbrook Street', '180 Peachey Road', '182 Gilles Street', '182 Humbug Scrub Road', '183 OG Road', '189 Wingate Road', '18b Gould Road', '19 Ascot Avenue', '19 Bundarra Court', '19 Dawn Close', '19 Hawker Crescent', '19 Marleycombe Road', '19 Palari Crescent', '19 St Clair Avenue', '19 Stanley Street', '19 Stuckey Avenue', '19 Winklebury Road', '19 Wolsten Drive', '190 Williams Road', '193-195 Port Road', '194 Petherton Road', '195 Midway Road', '19a Bartlett Street', '1a Gosfield Crescent', '2 Alvis Crescent', '2 Ballard Street', '2 Bastow Road', '2 Bellview Street', '2 Burke Circuit', '2 Fyfield Street', '2 Heysen Court', '2 Howegate Lane', '2 Martha Way', '2 Railway Terrace', '2 Smith Place', '2 Sturt Court', '2 Walter Street', '2 Westbury Court', '2 Woodford Road', '2/123 Old Adelaide Road', '2/3 Peacock Road', '2/32 Heggaton Terrace', '20 Bollen Street', '20 Bridport Street', '20 Gladman Close', '20 Highland Circuit', '20 Karrawirra Close', '20 Keevil Street', '20 Olivia Court', '20 Rollison Road', '20b Marybank Terrace', '21 Castle Court', '21 Chateau Avenue', '21 Elly Drive', '21 Glasshouse Road', '21 Grace Boulevard', '21 Jacobsen Crescent', '21 Lewis Drive', '21 Magnolia Crescent', '21 Range Road', '21 Scott Street', '211 Lower Athelstone Road', '212 Grange Road', '22 Alawoona Road', '22 Bagalowie Crescent', '22 Dillon Street', '22 Dundee Road', '22 Jane Street', '22 Mapleton Circuit', '22 Max Fatchen Drive', '22 Riverglen Court', '22 Varacalli Way', '22 Wahroonga Drive', '225 Fullarton Road', '23 Banksia Crescent', '23 Bimini Crescent', '23 Carolan Crescent', '23 Castle Avenue', '23 Cavenagh Street', '23 Charleston Crescent', '23 Deptford Street', '23 Huon Road', '23 Magor Street', '23 Secombe Street', '23 Short Road', '234 Prospect', '234 Prospect Road', '238 Black Top Road', '23a David Avenue', '24 Fantasia Drive', '24 The Avenue', '24 Traminer Drive', '24 Westbury Street', '24a Norongo Street', '25 Bell Street', '25 Bellchambers Road', '25 Chiselbury Road', '25 Hedgerow Drive', '25 Lancaster Court', '25 North Terrace', '25 Patterson Road', '252 Grange Road', '253 Salisbury Highway', '26 Flinders Parade', '26 Lorna Court', '26 Minchington Road', '26 The Terrace', '261a Waymouth Street', '262 Melbourne Street', '27 Burnett Drive', '27 Chellaston Road', '27 Higgins Terrace', '27 Ina Close', '27 Stockton Street', '270 The Parade', '274 Anzac Highway', '278 Flinders Street', '28 Burke Circuit', '28 Jeffries Road', '28 Laxton Road', '28 Newhaven Terrace', '28 Penfold Road', '280 Pulteney Street', '281 Stebonheath Road', '28a Perre Drive', '28b Mavros Road', '29 Baldina Crescent', '29 Max Fatchen Drive', '29 Old Sarum Road', '292 Findon Road', '299-301 Henley Beach Road', '3 Arthur Street', '3 Binara Court', '3 Catalonia Avenue', '3 Colombo Court', '3 Eighth Street', '3 Elmwood Circuit', '3 Mantilla Street', '3 Olivia Court', '3 Peachey Road', '3 Princess Street', '3 Reunion Lane', '3 The Grove', '3 Turnworth Street', '3 Virgara Court', '3-5 Price Street', '3/10 Gateway Drive', '3/11-13 Bremen Drive', '3/18 Davidson Road', '3/46 Queen Street', '3/76 Muller Road', '30 Bain Road', '30 Benham Street', '30 Green Court', '30 Mapleton Circuit', '30 Mavros Road', '30 McKenzie Road', '30 McPherson Grove', '300 Glen Osmond Road', '302 Glen Osmond Road', '31 Bennett Avenue', '31 Collingbourne Drive', '31 Flinders Street', '31 Kernel Road', '31 Palomino Drive', '32 Chaddenwick Road', '32 Farnham Road', '32 Fourth Street', '32 Uley Road', '32a Sunbeam Road', '33 Adelaide Street', '33 Brisbane Drive', '33 Broadmeadows Road', '33 Carrington Street', '33 Filsell Terrace', '33 McKay Road', '33 Naweena Road', '33 Omega Drive', '33 Tulloch Drive', '34 Green Court', '34 Heysen Court', '34 Whitford Road', '35 Mayfair Drive', '35 Stevens Drive', '352 Alexander Avenue', '36 Clementine Avenue', '36 Como Road', '36 Fullarton Road', '36 Jordan Drive', '36 Moir Street', '36 Radiata Grove', '36 Robert Road', '366 Craigmore Road', '366 Unley Road', '37 Bassnet Road', '37 Green Crescent', '37 Yarnbrook Street', '378 Payneham Road', '38 Bagot Road', '38 Hamilton Road', '38 Windsor Street', '39 Chellaston Road', '39 Fantasia Drive', '39 Green Ridge', '39 Samuel Street', '39 Yarnbury Road', '395 Ferntree Gully Road', '39a Anderson Walk', '4 Cathy Mews', '4 Chellaston Road', '4 De Luca Court', '4 Fradd Court', '4 Grovely Street', '4 Hamptworth Street', '4 John Shultz Court', '4 Levant Street', '4 Little Para Street', '4 Lorenzo Court', '4 Mary Court', '4 Oxford Drive', '4 Pix Road', '4 Teakle Court', '4 Whitehart Close', '4 Willowood Drive', '4/25 Sheridan Street', '4/66 Rundle Street', '40 Athol Street', '40 Cambridge Terrace', '40 Manchester Circuit', '40 Raglan Avenue', '405 Craigmore Road', '41 Amberdale Road', '41 Fantasia Drive', '41 Nilpena Court', '410 Grand Junction Road', '43 Dartmouth Street', '43 Innes Street', '43 Mayfair Drive', '43 Seavington Road', '44 Alawoona Road', '45 Collins Parade', '45 First Street', '45 Riesling Crescent', '45 Southbank Boulevard', '45 Vine Street', '45 Willison Road', '457 Grange Road', '46 Clement Terrace', '465b South Road', '47 Mahood Street', '47 Pipkin Road', '475 Torrens Road', '48 Coppleridge Drive', '48 Coratina Road', '48 Hamblynn Road', '48 Uley Road', '49 Alicante Avenue', '497 North East Road', '5 Carabeen Crescent', '5 Collingbourne Drive', '5 De Luca Court', '5 Elm Court', '5 Jacaranda Drive', '5 Lewis Court', '5 Orchard Grove', '5 Orietta Court', '5 Palmer Road', '5 Rhodes Court', '5 Riverview Drive', '5 Rody Court', '5 Second Street', '5 Sedgemoor Road', '5 Walsh Avenue', '5 Warner Road', '5-7 Taminga Street', '5/19-21 Metro Parade', '5/59 Fullarton Road', '5/9 Baxter Avenue', '50 Christine Avenue', '500 North East Road', '503 Lower North East Road', '51 Beulah Road', '51 Loftis Road', '516 Western Branch Road', '519 Torrens Road', '52 Jeffries Road', '52 Jordan Drive', '53 Greenfields Drive', '54 Alawoona Road', '54 Minchington Road', '553 Womma Road', '55b Railway Terrace', '56 Waterside Drive', '566 Craigmore Road', '573 Port Road', '59-63 Saints Road', '6 Arabella Court', '6 Bloomfield Crescent', '6 Bressington Drive', '6 Burns Avenue', '6 Kavanagh Court', '6 Maple Leaf Court', '6 Pegglome Court', '6 Rositano Drive', '6 Stanley Street', '6 The Parkway', '6 Woodcutts Road', '6/221 Martins Road', '607 Marion Road', '64 Halifax Street', '641 North East Road', '65 Charles Street', '65 Gawler Road', '66 Balmoral Circuit', '68 Redbanks Road', '7 Colombo Court', '7 Dulkara Avenue', '7 George Avenue', '7 Longleat Road', '7 McLaren Court', '7 Reordan Drive', '7 Tobruk Drive', '7 Varney Court', '7/34 Millicent Street', '7/9 OG Road', '70 Liberator Drive', '70 Midway Road', '70 Peachey Road', '71 Faulding Avenue', '712 South Road', '72 President Avenue', '72 Strathaird Boulevard', '73 Douglas Drive', '73 Glen Osmond Road', '73 Stanford Road', '736 North East Road', '74 Grange Road', '75 Magill Road', '76 McLaren Street', '78 North Terrace', '79 Beatrice Street', '79 Hamblynn Road', '79 Peachey Road', '8 Angle Vale Road', '8 Arrow Crescent', '8 Blue Lake Drive', '8 Blue Wren Circuit', '8 Church Street', '8 Kent Place', '8 Kentish Road', '8 Lovelock Road', '8 Luis Drive', '8 Luvera Drive', '8 Milan Street', '8 Tangelo Court', '8 Wahroonga Drive', '8/25 Harbour Village Parade', '8/5 Kintore Avenue', '805 South Road', '805-807 South Road', '806/147 Pirie Street', '81 President Avenue', '82 Gibson Street', '83 Heaslip Road', '84 North Terrace', '86 Fullarton Road', '86 Whitington Road', '86-88 Main North Road', '877 Grand Junction Road', '89 Douglas Drive', '89 Forrestall Road', '89 Talbot Road', '9 Anzac Highway', '9 Armiger Court', '9 Baron Road', '9 Bluebell Lane', '9 Crown Court', '9 Fellows Street', '9 Fisher Place', '9 George Street', '9 Tallowwood Way', '9 Torrens Street', '91 Halifax Street', '91a Chellaston Road', '92 Light Avenue', '92 McGilp Road', '93 Angle Vale Road', '94 Whitington Road', '95 Johns Road', '95 Womma Road', '97a Reservoir Road', '98 Lakeside Drive', '997 Black Top Road', '9b John Street', 'C/', 'C/ 360 Surveying', 'C/ Adelaide Concrete', 'C/ Alexander Symonds', 'C/ Alexander Symonds Pty Ltd', 'C/ Bargain Steel Centre', 'C/ Bdc', 'C/ Bleeze Neale Surveyors Pty Ltd', 'C/ Elite Land Solutions', 'C/ Erin Dare,Trice', 'C/ Fyfe Pty Ltd', 'C/ Heynen Planning Consultants', 'C/ Jeffrey Fudge &amp; Associates', 'C/ John C Bested &amp; Associates Pty Ltd', 'C/ Lock Surveys', 'C/ Masterplan (SA) Pty Ltd', 'C/ Masterplan SA', 'C/ Mattsson &amp; Martyn', 'C/ Mayfair Property Services', 'C/ Mayfairi Property Services', 'C/ PBS Aust', 'C/ Pbs Australia', 'C/ Pbs Australia Pty Ltd', 'C/ Pennino &amp; Associates', 'C/ Pyper Leaker Surveying Services Pty Ltd', 'C/ Pyper Leaker Surveyng Services Pty Ltd', 'C/ Reality Commercial Projects', 'C/ Rivergum Homes', 'C/ Stock Land Division', 'C/ Swanbury Penglase', 'C/ TK Building Design', 'C/ Transport Project Delivery', 'C/ Visionstream', 'C/-', 'C/- 360 Conveyancing', 'C/- Adelaide Retaining Walls', 'C/- Aecom', 'C/- Alexander Symonds', 'C/- Alexander Symonds Pty Ltd', 'C/- BDC', 'C/- Bleeze Neale Surveyors', 'C/- Botten Levinson Lawyers', 'C/- Cavallo Forest &amp; Assoc', 'C/- Cavallo Forest &amp; Associates', 'C/- City of Playford', 'C/- Colin Davies', 'C/- Department for Child Protection', 'C/- Dept of Planning Transport &amp; Infrastructure', 'C/- Dr Sadiq Assafi', 'C/- Ekistics', 'C/- Elite Land Solutions', 'C/- Future Urban', 'C/- Fyfe Pty Ltd', 'C/- Homebush Business Village', 'C/- J &amp; S Pergola Installations', 'C/- Lanser', 'C/- Lanser Communities', 'C/- MRS Pty Ltd', 'C/- Masterplan SA Pty Ltd', 'C/- Multi Design', 'C/- PBS', 'C/- PBS Aust', 'C/- PBS Australia', 'C/- Pennino &amp; Assoc Pty Ltd', 'C/- Phillips Pilkington Architects', 'C/- Pinksterboer Property', 'C/- Planning Chambers', 'C/- Playford City Hotel Pty Ltd', 'C/- Pyper Leaker Surveying Services', 'C/- Pyper Leaker Surveying Services Pty Ltd', 'C/- Reality Commercial Projects', 'C/- Remo Contractors Pty Ltd', 'C/- Retail Asset Management Pty Ltd', 'C/- SA Water', 'C/- Spectra Group Pty Ltd - Ground Floor', 'C/- Stimson Consulting', 'C/- Studio Nine Architects', 'C/- The Elms', 'C/- Zummo Design', 'C/-Urps Pty Ltd', 'C\\- Alexander Symonds Pty Ltd', 'GPO Box 1533', 'GPO Box 292', 'GPO Box 698', 'Level 1, 124 South Terrace', 'Level 1, 40 Greenhill Road', 'Level 3 142 North Terrace', 'Level 3 Suite 37 799 Springvale Road', 'Level 6, 100 Pirie Street', 'Level 9, 19 North Terrace', 'Lot 151b Seaview Road', 'Lot 198 Andrews Road', 'Lot 28 Andrews Road', 'Lot 3 Gawler-One Tree Hill Road', 'PO Box 1000', 'PO Box 1018', 'PO Box 1029', 'PO Box 108', 'PO Box 1085', 'PO Box 1088', 'PO Box 119', 'PO Box 1210', 'PO Box 1227', 'PO Box 129', 'PO Box 131', 'PO Box 14', 'PO Box 140', 'PO Box 141', 'PO Box 145', 'PO Box 1465', 'PO Box 1506', 'PO Box 151', 'PO Box 153', 'PO Box 1536', 'PO Box 158', 'PO Box 1598', 'PO Box 17', 'PO Box 1700', 'PO Box 1757', 'PO Box 180', 'PO Box 185', 'PO Box 1863', 'PO Box 187', 'PO Box 189', 'PO Box 191', 'PO Box 193', 'PO Box 195', 'PO Box 2', 'PO Box 20', 'PO Box 2005', 'PO Box 2017', 'PO Box 2075', 'PO Box 208', 'PO Box 213', 'PO Box 221', 'PO Box 2218', 'PO Box 234', 'PO Box 2343', 'PO Box 237', 'PO Box 242', 'PO Box 25', 'PO Box 258', 'PO Box 2601', 'PO Box 268', 'PO Box 27', 'PO Box 2709', 'PO Box 273', 'PO Box 28', 'PO Box 283', 'PO Box 285', 'PO Box 296', 'PO Box 30', 'PO Box 3019', 'PO Box 303', 'PO Box 3074', 'PO Box 313 Centre Plaza', 'PO Box 350', 'PO Box 356', 'PO Box 357', 'PO Box 360', 'PO Box 371', 'PO Box 388', 'PO Box 391', 'PO Box 42', 'PO Box 424', 'PO Box 45', 'PO Box 453', 'PO Box 46', 'PO Box 487', 'PO Box 501', 'PO Box 520', 'PO Box 526', 'PO Box 535', 'PO Box 537', 'PO Box 55', 'PO Box 551', 'PO Box 595', 'PO Box 6037', 'PO Box 616', 'PO Box 630', 'PO Box 654', 'PO Box 656', 'PO Box 66', 'PO Box 662', 'PO Box 68', 'PO Box 693', 'PO Box 7002', 'PO Box 71', 'PO Box 712', 'PO Box 7165 Hutt Street', 'PO Box 736', 'PO Box 798', 'PO Box 811', 'PO Box 818', 'PO Box 831', 'PO Box 838', 'PO Box 84', 'PO Box 841', 'PO Box 848', 'PO Box 89', 'PO Box 894', 'PO Box 905', 'PO Box 909', 'PO Box 911', 'PO Box 916', 'PO Box 97', 'PO Box 988', 'Spud, 67 Lipson Street', 'Suite 5', 'Unknown']</t>
+          <t>['*****************************', '1 Bain Street', '1 Crace Court', '1 Crown Street', '1 Everglade Court', '1 Fergusson Bowl', '1 Grampain Street', '1 Grampian Street', '1 Joes Court', '1 Lisa Court', '1 Parkwood Lane', '1 Rhus Avenue', '1 Tarana Court', '1 Tatura Court', '1 Westbury Court', '1-3 Dewer Avenue', '1/ Lot 72 Paxton Street', '1/121 Angle Vale Road', '1/16 Kingstag Crescent', '1/18-22 Provident Avenue', '1/198 Greenhill Road', '1/28 Chellaston Road', '1/280 Payneham Road', '1/52 Ron Parkison Crescent', '1/8 Deuter Road', '10 Africaine Avenue', '10 Alderwood Court', '10 Bracken Avenue', '10 Breamore Street', '10 Brookfield Street', '10 Cartwright Drive', '10 Christine Avenue', '10 Epsom Street', '10 Goddard Drive', '10 Karinga Crescent', '10 Keysley Street', '10 Liebrooke Boulevard', '10 Magnolia Crescent', '10 Marles Court', '10 Pendolino Road', '10 Ronan Court', '10 Shah Place', '10 Strawson Road', '10 Ward Street', '101 Port Road', '103 Halsey Road', '104/19 Holdfast Promenade', '104a Muller Road', '108-110 Mooringe Avenue', '1097 Stebonheath Road', '10a Chardonnay Court', '11 Aistrope Avenue', '11 Litchfield Avenue', '11 Metcalfe Avenue', '11 North Street', '11 Pendolino Road', '11 William Street', '110-114 Grange Road', '111 Viney Drive', '114-116 Heaslip Road', '115 Crittenden Road', '115 Sampson Road', '116 Botting Street', '11d Metro Parade', '12 Beatrix Drive', '12 Bishopstone Road', '12 Black Top Road', '12 Cameron Road', '12 Dana Street', '12 Elm Drive', '12 Epsom Street', '12 Federation Close', '12 Fowler Street', '12 Miller Street', '12 Oleander Drive', '12 Palmer Road', '12 Sharrad Court', '12 Stock Road', '12 Sunrise Court', '120 Salisbury Highway', '122 Womma West Road', '125 Galway Avenue', '125-129 Commercial Road', '126b Payneham Road', '13 Brittania Drive', '13 Brock Street', '13 Hughes Avenue', '13 Prelude Circuit', '13 Prosperity Way', '13 Stone Road', '13 Swan Crescent', '13 Treleaven Way', '131 Gawler River Road', '132 Payneham Road', '133 Main South Road', '134 Fullarton Road', '134 Tyeka Drive', '136 McKenzie Road', '137 Angle Vale Road', '138 Penfield Road', '138 Supple Road', '139 Kentish Road', '14 Carmela Avenue', '14 Charlson Street', '14 Clover Court', '14 Crisp Road', '14 Dana Street', '14 Durrington Road', '14 Greenhood Crescent', '14 Hancock Road', '14 Jordon Street', '14 Kapoola Avenue', '14 Lynton Avenue', '14 Mary Street', '14 Prosperity Way', '14 Raymond Road', '14 Talbot Street', '14 Yarnbrook Street', '1415 Main North Road', '143 Lakeside Drive', '144 Halsey Road', '147 Goodman Road', '149 Douglas Drive', '149 Tyeka Drive', '15 Abelia Street', '15 Adams Road', '15 Bailey Road', '15 Bubner Street', '15 Coach House Mews', '15 Collins Street', '15 Hermitage Drive', '15 Jenolan Crescent', '15 Kernel Road', '15 Lawder Road', '15 Penley Avenue', '15 Southern Avenue', '15 Spruance Road', '15 Waterford Circuit', '150 Williams Road', '158 Railway Terrace', '159 Port Road', '15a Fife Street', '15b King William Street', '16 Alderwood Court', '16 Breamore Street', '16 Cameron Road', '16 Honeysuckle Drive', '16 Illawarra Court', '16 Karinga Crescent', '16 Lawder Road', '16 Lister Avenue', '16 Michael Crescent', '16 Palari Crescent', '16 Sharrad Court', '16 The Greenway', '16 Tindara Avenue', '16 Warren Road', '1602 Two Wells Road', '161 Brunswick Street', '162 Greenhill Road', '168 Grand Junction Road', '168 Julian Road', '17 Alexander Road', '17 Ariadne Crescent', '17 Ballard Street', '17 Bastow Road', '17 Benham Street', '17 Boettcher Road', '17 Dawkins Avenue', '17 Elder Court', '17 Falcon Drive', '17 Fradd Road', '17 Mosterton Road', '17 Stanley Street', '17/21 Heaslip Road', '170 Greenhill Road', '179 Gilles Street', '18 Bogan Road', '18 Bubner Road', '18 Carob Crescent', '18 Elmwood Circuit', '18 Fantasia Drive', '18 Green Crescent', '18 Laburnum Gardens', '18 Lorna Court', '18 Oregon Avenue', '18 Perthville Court', '18 Pineridge Drive', '18 Richard Street', '18 Rosetta Street', '18 Warragal Court', '18 Yarnbrook Street', '180 Peachey Road', '182 Gilles Street', '182 Humbug Scrub Road', '183 OG Road', '189 Wingate Road', '18b Gould Road', '19 Ascot Avenue', '19 Bundarra Court', '19 Dawn Close', '19 Hawker Crescent', '19 Marleycombe Road', '19 Palari Crescent', '19 St Clair Avenue', '19 Stanley Street', '19 Stuckey Avenue', '19 Swallow Drive', '19 Winklebury Road', '19 Wolsten Drive', '190 Williams Road', '193-195 Port Road', '194 Petherton Road', '195 Midway Road', '19a Bartlett Street', '1a Gosfield Crescent', '2 Alvis Crescent', '2 Ballard Street', '2 Bastow Road', '2 Bellview Street', '2 Burke Circuit', '2 Fyfield Street', '2 Heysen Court', '2 Howegate Lane', '2 Martha Way', '2 Railway Terrace', '2 Smith Place', '2 Sturt Court', '2 Walter Street', '2 Westbury Court', '2 Woodford Road', '2/123 Old Adelaide Road', '2/3 Peacock Road', '2/32 Heggaton Terrace', '20 Bollen Street', '20 Bridport Street', '20 Gladman Close', '20 Highland Circuit', '20 Karrawirra Close', '20 Keevil Street', '20 Olivia Court', '20 Rollison Road', '206 Magill Road', '20b Marybank Terrace', '21 Castle Court', '21 Chateau Avenue', '21 Elly Drive', '21 Glasshouse Road', '21 Grace Boulevard', '21 Jacobsen Crescent', '21 Lewis Drive', '21 Magnolia Crescent', '21 Range Road', '21 Scott Street', '211 Lower Athelstone Road', '212 Grange Road', '216-220 Adams Road', '22 Alawoona Road', '22 Bagalowie Crescent', '22 Dillon Street', '22 Dundee Road', '22 Jane Street', '22 Mapleton Circuit', '22 Max Fatchen Drive', '22 Priority Court', '22 Riverglen Court', '22 Varacalli Way', '22 Wahroonga Drive', '225 Fullarton Road', '23 Banksia Crescent', '23 Bimini Crescent', '23 Carolan Crescent', '23 Castle Avenue', '23 Cavenagh Street', '23 Charleston Crescent', '23 Deptford Street', '23 Huon Road', '23 Magor Street', '23 Secombe Street', '23 Short Road', '234 Prospect', '234 Prospect Road', '238 Black Top Road', '23a David Avenue', '24 Fantasia Drive', '24 The Avenue', '24 Traminer Drive', '24 Westbury Street', '24a Norongo Street', '25 Bell Street', '25 Bellchambers Road', '25 Chiselbury Road', '25 Hedgerow Drive', '25 Lancaster Court', '25 North Terrace', '25 Patterson Road', '252 Grange Road', '253 Salisbury Highway', '26 Flinders Parade', '26 Lorna Court', '26 Minchington Road', '26 The Terrace', '261a Waymouth Street', '262 Melbourne Street', '27 Burnett Drive', '27 Chellaston Road', '27 Higgins Terrace', '27 Ina Close', '27 Stockton Street', '270 The Parade', '274 Anzac Highway', '278 Flinders Street', '28 Burke Circuit', '28 Jeffries Road', '28 Laxton Road', '28 Newhaven Terrace', '28 Penfold Road', '28 Telowie Avenue', '280 Pulteney Street', '281 Stebonheath Road', '28a Perre Drive', '28b Mavros Road', '29 Baldina Crescent', '29 Max Fatchen Drive', '29 Old Sarum Road', '292 Findon Road', '299-301 Henley Beach Road', '3 Arthur Street', '3 Binara Court', '3 Catalonia Avenue', '3 Colombo Court', '3 Eighth Street', '3 Elmwood Circuit', '3 Mantilla Street', '3 Olivia Court', '3 Peachey Road', '3 Princess Street', '3 Reunion Lane', '3 The Grove', '3 Turnworth Street', '3 Virgara Court', '3-5 Price Street', '3/10 Gateway Drive', '3/11-13 Bremen Drive', '3/18 Davidson Road', '3/4 Adelaide Terrace', '3/46 Queen Street', '3/76 Muller Road', '30 Bain Road', '30 Benham Street', '30 Green Court', '30 Mapleton Circuit', '30 Mavros Road', '30 McKenzie Road', '30 McPherson Grove', '300 Glen Osmond Road', '302 Glen Osmond Road', '31 Bennett Avenue', '31 Collingbourne Drive', '31 Flinders Street', '31 Kernel Road', '31 Palomino Drive', '32 Chaddenwick Road', '32 Farnham Road', '32 Fourth Street', '32 Reservoir Road', '32 Uley Road', '32a Mary Street', '32a Sunbeam Road', '33 Adelaide Street', '33 Brisbane Drive', '33 Broadmeadows Road', '33 Carrington Street', '33 Filsell Terrace', '33 McKay Road', '33 Naweena Road', '33 Omega Drive', '33 Tulloch Drive', '34 Cascades Drive', '34 Green Court', '34 Heysen Court', '34 Hogarth Road', '34 Whitford Road', '35 Mayfair Drive', '35 Portrush Road', '35 Stevens Drive', '352 Alexander Avenue', '36 Clementine Avenue', '36 Como Road', '36 Fullarton Road', '36 Jordan Drive', '36 Leonis Avenue', '36 Moir Street', '36 Radiata Grove', '36 Robert Road', '366 Craigmore Road', '366 Unley Road', '37 Bassnet Road', '37 Green Crescent', '37 Yarnbrook Street', '378 Payneham Road', '38 Bagot Road', '38 Hamilton Road', '38 Lamorna Parade', '38 Windsor Street', '39 Chellaston Road', '39 Fantasia Drive', '39 Green Ridge', '39 Samuel Street', '39 Yarnbury Road', '390 Alexander Avenue', '395 Ferntree Gully Road', '39a Anderson Walk', '4 Bice Street', '4 Cathy Mews', '4 Chellaston Road', '4 De Luca Court', '4 Fradd Court', '4 Grovely Street', '4 Hamptworth Street', '4 John Shultz Court', '4 Levant Street', '4 Little Para Street', '4 Lorenzo Court', '4 Mary Court', '4 Oxford Drive', '4 Pix Road', '4 Teakle Court', '4 Whitehart Close', '4 Willowood Drive', '4/25 Sheridan Street', '4/66 Rundle Street', '40 Athol Street', '40 Cambridge Terrace', '40 Manchester Circuit', '40 Raglan Avenue', '405 Craigmore Road', '41 Amberdale Road', '41 Fantasia Drive', '41 Nilpena Court', '41/155 Brebner Drive', '410 Grand Junction Road', '43 Dartmouth Street', '43 Innes Street', '43 Mayfair Drive', '43 Seavington Road', '44 Alawoona Road', '44a Nilpena Avenue', '45 Collins Parade', '45 First Street', '45 Riesling Crescent', '45 Southbank Boulevard', '45 Vine Street', '45 Willison Road', '457 Grange Road', '46 Clement Terrace', '465b South Road', '47 Mahood Street', '47 Pipkin Road', '475 Torrens Road', '48 Coppleridge Drive', '48 Coratina Road', '48 Hamblynn Road', '48 Uley Road', '49 Alicante Avenue', '497 North East Road', '4b Mantissa Road', '5 Carabeen Crescent', '5 Collingbourne Drive', '5 De Luca Court', '5 Elm Court', '5 Jacaranda Drive', '5 Lewis Court', '5 Matthew Street', '5 Orchard Grove', '5 Orietta Court', '5 Overlander Way', '5 Palmer Road', '5 Rhodes Court', '5 Riverview Drive', '5 Rody Court', '5 Second Street', '5 Sedgemoor Road', '5 Walsh Avenue', '5 Warner Road', '5-7 Taminga Street', '5/126 Carrington Street', '5/19-21 Metro Parade', '5/59 Fullarton Road', '5/9 Baxter Avenue', '50 Christine Avenue', '500 North East Road', '503 Lower North East Road', '51 Beulah Road', '51 Loftis Road', '516 Western Branch Road', '519 Torrens Road', '52 Jeffries Road', '52 Jordan Drive', '53 Greenfields Drive', '54 Alawoona Road', '54 Derrick Road', '54 Minchington Road', '553 Womma Road', '55b Railway Terrace', '56 Waterside Drive', '566 Craigmore Road', '573 Port Road', '59-63 Saints Road', '6 Arabella Court', '6 Bloomfield Crescent', '6 Bressington Drive', '6 Burns Avenue', '6 Kavanagh Court', '6 Maple Leaf Court', '6 Pegglome Court', '6 Rositano Drive', '6 Stanley Street', '6 The Parkway', '6 Woodcutts Road', '6/221 Martins Road', '607 Marion Road', '64 Halifax Street', '641 North East Road', '65 Charles Street', '65 Gawler Road', '66 Balmoral Circuit', '68 Redbanks Road', '7 Colombo Court', '7 Dulkara Avenue', '7 George Avenue', '7 Longleat Road', '7 McLaren Court', '7 Ranee Court', '7 Reordan Drive', '7 Tobruk Drive', '7 Varney Court', '7/34 Millicent Street', '7/9 OG Road', '70 Liberator Drive', '70 Midway Road', '71 Faulding Avenue', '712 South Road', '72 President Avenue', '72 Strathaird Boulevard', '73 Douglas Drive', '73 Glen Osmond Road', '73 Stanford Road', '736 North East Road', '74 Grange Road', '75 Kew Drive', '75 Magill Road', '76 McLaren Street', '78 North Terrace', '79 Beatrice Street', '79 Hamblynn Road', '79 Peachey Road', '8 Angle Vale Road', '8 Arrow Crescent', '8 Blue Lake Drive', '8 Blue Wren Circuit', '8 Church Street', '8 Kent Place', '8 Kentish Road', '8 Lovelock Road', '8 Luis Drive', '8 Luvera Drive', '8 Milan Street', '8 Tangelo Court', '8 Wahroonga Drive', '8/25 Harbour Village Parade', '8/5 Kintore Avenue', '805 South Road', '805-807 South Road', '806/147 Pirie Street', '81 President Avenue', '82 Gibson Street', '83 Heaslip Road', '84 Gulf View Drive', '84 North Terrace', '86 Fullarton Road', '86 Whitington Road', '86-88 Main North Road', '877 Grand Junction Road', '881 Main North Road', '89 Douglas Drive', '89 Forrestall Road', '89 Talbot Road', '9 Anzac Highway', '9 Armiger Court', '9 Baron Road', '9 Bluebell Lane', '9 Crown Court', '9 Fellows Street', '9 Fisher Place', '9 George Street', '9 Madrid Court', '9 Pipkin Road', '9 Tallowwood Way', '9 Torrens Street', '91 Halifax Street', '91a Chellaston Road', '92 Light Avenue', '92 McGilp Road', '93 Angle Vale Road', '94 Whitington Road', '95 Johns Road', '95 Womma Road', '953 Stebonheath Road', '97a Reservoir Road', '98 Lakeside Drive', '98a Muller Road', '997 Black Top Road', '9b John Street', 'C/', 'C/ 360 Surveying', 'C/ Adelaide Concrete', 'C/ Alexander Symonds', 'C/ Alexander Symonds Pty Ltd', 'C/ Bargain Steel Centre', 'C/ Bdc', 'C/ Bleeze Neale Surveyors Pty Ltd', 'C/ Elite Land Solutions', 'C/ Erin Dare,Trice', 'C/ Fyfe Pty Ltd', 'C/ Heynen Planning Consultants', 'C/ Jeffrey Fudge &amp; Associates', 'C/ John C Bested &amp; Associates Pty Ltd', 'C/ Lock Surveys', 'C/ Masterplan (SA) Pty Ltd', 'C/ Masterplan SA', 'C/ Masterplan SA Pty Ltd', 'C/ Mattsson &amp; Martyn', 'C/ Mayfair Property Services', 'C/ Mayfairi Property Services', 'C/ PBS Aust', 'C/ Pbs Australia', 'C/ Pbs Australia Pty Ltd', 'C/ Pennino &amp; Associates', 'C/ Pyper Leaker Surveying Services Pty Ltd', 'C/ Pyper Leaker Surveyng Services Pty Ltd', 'C/ Reality Commercial Projects', 'C/ Rivergum Homes', 'C/ Stock Land Division', 'C/ Swanbury Penglase', 'C/ TK Building Design', 'C/ Transport Project Delivery', 'C/ Visionstream', 'C/-', 'C/- 360 Conveyancing', 'C/- Adelaide Retaining Walls', 'C/- Aecom', 'C/- Alexander Symonds', 'C/- Alexander Symonds Pty Ltd', 'C/- BDC', 'C/- Bleeze Neale Surveyors', 'C/- Botten Levinson Lawyers', 'C/- Cavallo Forest &amp; Assoc', 'C/- Cavallo Forest &amp; Associates', 'C/- City of Playford', 'C/- Colin Davies', 'C/- Department for Child Protection', 'C/- Dept of Planning Transport &amp; Infrastructure', 'C/- Dr Sadiq Assafi', 'C/- Ekistics', 'C/- Elite Land Solutions', 'C/- Future Urban', 'C/- Future Urban Pty Ltd', 'C/- Fyfe Pty Ltd', 'C/- Grieve Gillett Andersen', 'C/- Homebush Business Village', 'C/- J &amp; S Pergola Installations', 'C/- Jones Lang Lasalle (SA)', 'C/- Lanser', 'C/- Lanser Communities', 'C/- Little Hearts Child Care Centre', 'C/- MRS Pty Ltd', 'C/- Masterplan SA Pty Ltd', 'C/- Multi Design', 'C/- PBS', 'C/- PBS Aust', 'C/- PBS Australia', 'C/- Pba', 'C/- Pennino &amp; Assoc Pty Ltd', 'C/- Phillips Pilkington Architects', 'C/- Pinksterboer Property', 'C/- Planning Chambers', 'C/- Playford City Hotel Pty Ltd', 'C/- Pyper Leaker Surveying Services', 'C/- Pyper Leaker Surveying Services Pty Ltd', 'C/- Reality Commercial Projects', 'C/- Remo Contractors Pty Ltd', 'C/- Retail Asset Management Pty Ltd', 'C/- SA Water', 'C/- Spectra Group Pty Ltd - Ground Floor', 'C/- Stimson Consulting', 'C/- Studio Nine Architects', 'C/- The Elms', 'C/- Zummo Design', 'C/-Urps Pty Ltd', 'C/Alexander Symonds Pty Ltd', 'C\\- Alexander Symonds Pty Ltd', 'GPO Box 1266', 'GPO Box 1533', 'GPO Box 292', 'GPO Box 698', 'Level 1, 124 South Terrace', 'Level 1, 40 Greenhill Road', 'Level 16  461 Bourke Street', 'Level 3 142 North Terrace', 'Level 3 Suite 37 799 Springvale Road', 'Level 5', 'Level 6, 100 Pirie Street', 'Level 9, 19 North Terrace', 'Lot 151b Seaview Road', 'Lot 198 Andrews Road', 'Lot 28 Andrews Road', 'Lot 3 Gawler-One Tree Hill Road', 'Multi Design', 'PO Box 1000', 'PO Box 1018', 'PO Box 1029', 'PO Box 108', 'PO Box 1085', 'PO Box 1088', 'PO Box 119', 'PO Box 1210', 'PO Box 1227', 'PO Box 129', 'PO Box 131', 'PO Box 14', 'PO Box 140', 'PO Box 141', 'PO Box 145', 'PO Box 1465', 'PO Box 1506', 'PO Box 151', 'PO Box 153', 'PO Box 1536', 'PO Box 158', 'PO Box 1598', 'PO Box 17', 'PO Box 170', 'PO Box 1700', 'PO Box 1757', 'PO Box 180', 'PO Box 185', 'PO Box 1863', 'PO Box 187', 'PO Box 189', 'PO Box 191', 'PO Box 193', 'PO Box 195', 'PO Box 2', 'PO Box 20', 'PO Box 2005', 'PO Box 2017', 'PO Box 2075', 'PO Box 208', 'PO Box 213', 'PO Box 221', 'PO Box 2218', 'PO Box 234', 'PO Box 2343', 'PO Box 237', 'PO Box 24', 'PO Box 242', 'PO Box 25', 'PO Box 258', 'PO Box 2601', 'PO Box 268', 'PO Box 27', 'PO Box 2709', 'PO Box 273', 'PO Box 28', 'PO Box 283', 'PO Box 285', 'PO Box 296', 'PO Box 30', 'PO Box 3019', 'PO Box 303', 'PO Box 3074', 'PO Box 313 Centre Plaza', 'PO Box 350', 'PO Box 356', 'PO Box 357', 'PO Box 359', 'PO Box 371', 'PO Box 388', 'PO Box 391', 'PO Box 405', 'PO Box 42', 'PO Box 424', 'PO Box 45', 'PO Box 453', 'PO Box 46', 'PO Box 487', 'PO Box 501', 'PO Box 520', 'PO Box 526', 'PO Box 535', 'PO Box 537', 'PO Box 55', 'PO Box 551', 'PO Box 595', 'PO Box 6037', 'PO Box 616', 'PO Box 630', 'PO Box 654', 'PO Box 656', 'PO Box 66', 'PO Box 662', 'PO Box 68', 'PO Box 693', 'PO Box 7002', 'PO Box 71', 'PO Box 712', 'PO Box 7165 Hutt Street', 'PO Box 736', 'PO Box 798', 'PO Box 811', 'PO Box 818', 'PO Box 831', 'PO Box 838', 'PO Box 84', 'PO Box 841', 'PO Box 848', 'PO Box 89', 'PO Box 894', 'PO Box 905', 'PO Box 909', 'PO Box 911', 'PO Box 916', 'PO Box 97', 'PO Box 988', 'Spud, 67 Lipson Street', 'Suite 5', 'Unknown']</t>
         </is>
       </c>
     </row>
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -1060,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>WODONGA  VIC  3690</t>
+          <t>26 Wakenham Street</t>
         </is>
       </c>
       <c r="T7" t="n">
@@ -1087,20 +1087,20 @@
         </is>
       </c>
       <c r="V7" t="n">
-        <v>387</v>
+        <v>454</v>
       </c>
       <c r="W7" t="n">
         <v>0.289</v>
       </c>
       <c r="X7" t="n">
-        <v>49663</v>
+        <v>55674</v>
       </c>
       <c r="Y7" t="n">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>['*****************************', '1 Coglin Street', '1 Victoria Terrace', '10 Barfield Crescent', '10/230 Main South Road', '1002 Grand Junction Road', '11/11-21 Underwood Road', '12 Bishopstone Road', '15 Fullarton Road', '16 Aristotto Close', '16-18 Ann Street', '165 MacKinnon Parade', '214 Gilbert Street', '219 Old Mt Barker Road', '220 Henley Beach Road', '225 Fullarton Road', '25 Hardys Road', '250 Victoria Square', '27 19th Street', '3/11-13 Bremen Drive', '32a Mary Street', '33 Carrington Street', '362 Magill Road', '387-391 South Road', '4/66 Rundle Street', '50 Peachey Road', '6 Todd Street', '607 Marion Road', '78 Goodwood Road', '87 Springbank Road', '9 George Street', '9 Kalka Crescent', '9 King William Street', '95 Harrison Road', 'ADELAIDE  SA  5000', 'ADELAIDE  SA  5001', 'ALBERT PARK  SA  5014', 'ALDGATE  SA  5154', 'ALDINGA BEACH  SA  5173', 'ALEXANDRIA  NSW  2015', 'ALLENBY GARDENS  SA  5009', 'ANDREWS FARM  SA  5114', 'ANGLE VALE  SA  5114', 'ANGLE VALE  SA  5117', 'ATHELSTONE  SA  5076', 'ATHOL PARK  SA  5012', 'BALGOWLAH HEIGHTS  NSW  2093', 'BANKSIA PARK  SA  5091', 'BEAUMONT HILLS  NSW  2155', 'BELLIS CREEK  QLD  4551', 'BIBARINGA  SA  5118', 'BLACKWOOD  SA  5051', 'BLAIR ATHOL  SA  5084', 'BLAKEVIEW  SA  5114', 'BOWDEN  SA  5007', 'BRIGHTON  SA  5048', 'BROADVIEW  SA  5083', 'BROOKLYN PARK  SA  5032', 'BURTON  SA  5110', 'CAMPBELLTOWN  SA  5074', 'CARRUM DOWNS  VIC  3201', 'CAVAN  SA  5094', 'CHRISTIES BEACH  SA  5165', 'CLARENCE GARDENS  SA  5039', 'CLEARVIEW  SA  5085', 'CLOISTERS SQUARE  WA  6850', 'COCKATOO VALLEY  SA  5351', 'COOMERA WATERS  QLD  4209', 'CRAIGMORE  SA  5114', 'CROYDON  SA  5008', 'DAVOREN PARK  SA  5113', 'DAVOREN PARK SOUTH  SA  5113', 'DAW PARK  SA  5041', 'DIREK  SA  5110', 'DOVER GARDENS  SA  5048', 'EASTWOOD  SA  5063', 'EDINBURGH NORTH  SA  5113', 'EDWARDSTOWN  SA  5039', 'ELIZABETH  SA  5112', 'ELIZABETH DOWNS  SA  5113', 'ELIZABETH EAST  SA  5112', 'ELIZABETH GROVE  SA  5112', 'ELIZABETH NORTH  SA  5113', 'ELIZABETH PARK  SA  5113', 'ELIZABETH SOUTH  SA  5112', 'ELIZABETH VALE  SA  5112', 'EVANSTON  SA  5116', 'EVANSTON PARK  SA  5116', 'EYRE  SA  5121', 'FINDON  SA  5023', 'FLINDERS PARK  SA  5025', 'FORTITUDE VALLEY  QLD  4006', 'FULLARTON  SA  5063', 'GAWLER  SA  5118', 'GAWLER EAST  SA  5118', 'GAWLER RIVER  SA  5118', 'GAWLER SOUTH  SA  5118', 'GILLES PLAINS  SA  5086', 'GLANDORE  SA  5037', 'GLENELG  SA  5045', 'GLYNDE  SA  5070', 'GOLDEN GROVE  SA  5125', 'GOULD CREEK  SA  5114', 'GPO Box 1533', 'GPO Box 2450', 'GREENACRES  SA  5086', 'GREENWITH  SA  5125', 'GULFVIEW HEIGHTS  SA  5096', 'HACKHAM  SA  5163', 'HACKNEY  SA  5069', 'HAMPSTEAD GARDENS  SA  5086', 'HENLEY BEACH  SA  5022', 'HEWETT  SA  5118', 'HILLBANK  SA  5112', 'HILLCREST  SA  5086', 'HILLIER  SA  5116', 'HINDMARSH  SA  5007', 'HOLDEN HILL  SA  5088', 'HOPE VALLEY  SA  5090', 'HUGHESDALE  VIC  3166', 'HUMBUG SCRUB  SA  5114', 'KADINA  SA  5554', 'KALBEEBA  SA  5118', 'KAPUNDA  SA  5373', 'KENSINGTON PARK  SA  5068', 'KENT TOWN  SA  5067', 'KENT TOWN  SA  5071', 'KERSBROOK  SA  5231', 'KESWICK  SA  5035', 'KLEMZIG  SA  5087', 'L28  91 King William Road', 'LARGS BAY  SA  5016', 'LEWISTON  SA  5501', 'LIGHTSVIEW  SA  5085', 'LILYDALE  VIC  3140', 'LONSDALE  SA  5160', 'Level 1', 'Level 1 74 Pirie Street', 'Locked Bag 4001', 'Lot 10 Heaslip Road', 'MACDONALD PARK  SA  5121', 'MAGILL  SA  5072', 'MANNINGHAM  SA  5086', 'MANSFIELD PARK  SA  5012', 'MARDEN  SA  5070', 'MARLESTON  SA  5033', 'MAWSON LAKES  SA  5095', 'MAYLAND  SA  5069', 'MELROSE PARK  SA  5039', 'MIDDLETON  SA  5213', 'MILDURA  VIC  3501', 'MILE END  SA  5031', 'MILLSWOOD  SA  5034', 'MITCHELL PARK  SA  5043', 'MODBURY  SA  5092', 'MODBURY HEIGHTS  SA  5092', 'MORPHETTVILLE  SA  5045', 'MOUNT BARKER  SA  5251', 'MOUNT OMMANEY  QLD  4074', 'MOUNT WAVERLEY  VIC  3149', 'MULGRAVE  VIC  3170', 'MUNNO PARA  SA  5115', 'MUNNO PARA DOWNS  SA  5115', 'MUNNO PARA WEST  SA  5115', 'MURRAY BRIDGE  SA  5254', 'NAIRNE  SA  5252', 'NEDLANDS  WA  6909', 'NEWTON  SA  5074', 'NORTH ADELAIDE  SA  5006', 'NORTH HAVEN  SA  5018', 'NORTH PLYMPTON  SA  5037', 'NORTHFIELD  SA  5085', 'NORWOOD  SA  5067', 'NURIOOTPA  SA  5355', "O'HALLORAN HILL  SA  5158", "O'SULLIVAN BEACH  SA  5166", 'ONE TREE HILL  SA  5114', 'PARA HILLS  SA  5096', 'PARA HILLS WEST  SA  5096', 'PARA VISTA  SA  5093', 'PARADISE  SA  5075', 'PARAFIELD GARDENS  SA  5107', 'PARALOWIE  SA  5108', 'PARKSIDE  SA  5063', 'PASADENA  SA  5042', 'PAYNEHAM  SA  5070', 'PENFIELD  SA  5121', 'PENNINGTON  SA  5013', 'PLYMPTON  SA  5038', 'PO Box 1000', 'PO Box 227', 'PO Box 235', 'PO Box 248', 'PO Box 302', 'PO Box 3131', 'PO Box 32', 'PO Box 358', 'PO Box 4015', 'PO Box 523', 'PO Box 6', 'PO Box 603', 'PO Box 6196', 'PO Box 662', 'PO Box 849', 'PO Box 917', 'POORAKA  SA  5095', 'PORT ADELAIDE  SA  5015', 'PROSPECT  SA  5082', 'PROSPECT EAST  SA  5082', 'REDWOOD PARK  SA  5097', 'REGENCY PARK  SA  5010', 'REGENCY PARK  SA  5942', 'RIDGEHAVEN  SA  5097', 'ROBINA  QLD  4226', 'ROSE PARK  SA  5067', 'ROSEWORTHY  SA  5371', 'SALISBURY  SA  5108', 'SALISBURY DOWNS  SA  5108', 'SALISBURY EAST  SA  5109', 'SALISBURY HEIGHTS  SA  5109', 'SALISBURY NORTH  SA  5108', 'SALISBURY PARK  SA  5109', 'SALISBURY PLAIN  SA  5109', 'SALISBURY SOUTH  SA  5106', 'SEATON  SA  5023', 'SEAVIEW DOWNS  SA  5049', 'SEFTON PARK  SA  5083', 'SHEA-OAK LOG  SA  5371', 'SHEIDOW PARK  SA  5158', 'SMITHFIELD  SA  5114', 'SMITHFIELD PLAINS  SA  5114', 'SOUTH PLYMPTON  SA  5038', 'ST AGNES  SA  5097', 'ST CLAIR  SA  5011', 'ST MARYS  SA  5042', 'STEPNEY  SA  5069', 'SURREY DOWNS  SA  5126', 'Suite 1/159 Port Road', 'Suite 12,154 Fullarton Road', 'TANUNDA  SA  5352', 'TEA TREE GULLY  SA  5091', 'THEBARTON  SA  5031', 'THORNTON  NSW  2322', 'TORRENSVILLE PLAZA  SA  5031', 'TWO WELLS  SA  5501', 'ULEYBURY  SA  5114', 'UNDERDALE  SA  5032', 'UNLEY PARK  SA  5061', 'VALE PARK  SA  5081', 'VALLEY VIEW  SA  5093', 'VIRGINIA  SA  5120', 'VISTA  SA  5091', 'WALKLEY HEIGHTS  SA  5098', 'WATERLOO CORNER  SA  5110', 'WAYVILLE  SA  5034', 'WELLAND  SA  5007', 'WEST CROYDON  SA  5008', 'WEST LAKES  SA  5021', 'WILLASTON  SA  5118', 'WILLIAMSTOWN  SA  5351', 'WILLUNGA  SA  5172', 'WINDSOR GARDENS  SA  5087', 'WINGFIELD  SA  5013', 'WODONGA  VIC  3690', 'WOODSIDE  SA  5244', 'WOODVILLE  SA  5011', 'WOODVILLE NORTH  SA  5012', 'WOODVILLE SOUTH  SA  5011', 'WYNN VALE  SA  5127', 'YATTALUNGA  SA  5114']</t>
+          <t>['*****************************', '1 Coglin Street', '1 Victoria Terrace', '10 Barfield Crescent', '10/230 Main South Road', '1002 Grand Junction Road', '11/11-21 Underwood Road', '12 Bishopstone Road', '13 Whitford Road', '15 Fullarton Road', '16 Aristotto Close', '16-18 Ann Street', '165 MacKinnon Parade', '214 Gilbert Street', '219 Old Mt Barker Road', '220 Henley Beach Road', '225 Fullarton Road', '243 Pirie Street', '25 Hardys Road', '250 Victoria Square', '26 Wakenham Street', '27 19th Street', '3/11-13 Bremen Drive', '32a Mary Street', '33 Carrington Street', '362 Magill Road', '387-391 South Road', '4/66 Rundle Street', '50 Peachey Road', '6 Todd Street', '607 Marion Road', '78 Goodwood Road', '87 Springbank Road', '9 George Street', '9 Kalka Crescent', '9 King William Street', '95 Harrison Road', 'ADELAIDE  SA  5000', 'ADELAIDE  SA  5001', 'ALBERT PARK  SA  5014', 'ALDGATE  SA  5154', 'ALDINGA BEACH  SA  5173', 'ALEXANDRIA  NSW  2015', 'ALLENBY GARDENS  SA  5009', 'ANDREWS FARM  SA  5114', 'ANGLE VALE  SA  5114', 'ANGLE VALE  SA  5117', 'ATHELSTONE  SA  5076', 'ATHOL PARK  SA  5012', 'BALGOWLAH HEIGHTS  NSW  2093', 'BANKSIA PARK  SA  5091', 'BEAUMONT HILLS  NSW  2155', 'BELLIS CREEK  QLD  4551', 'BIBARINGA  SA  5118', 'BLACKWOOD  SA  5051', 'BLAIR ATHOL  SA  5084', 'BLAKEVIEW  SA  5114', 'BOWDEN  SA  5007', 'BRIGHTON  SA  5048', 'BROADVIEW  SA  5083', 'BROOKLYN PARK  SA  5032', 'BURTON  SA  5110', 'CAMPBELLTOWN  SA  5074', 'CARRUM DOWNS  VIC  3201', 'CAVAN  SA  5094', 'CHRISTIES BEACH  SA  5165', 'CLARENCE GARDENS  SA  5039', 'CLEARVIEW  SA  5085', 'CLOISTERS SQUARE  WA  6850', 'COCKATOO VALLEY  SA  5351', 'COOMERA WATERS  QLD  4209', 'CRAIGMORE  SA  5114', 'CROYDON  SA  5008', 'DAVOREN PARK  SA  5113', 'DAVOREN PARK SOUTH  SA  5113', 'DAW PARK  SA  5041', 'DIREK  SA  5110', 'DOVER GARDENS  SA  5048', 'EASTWOOD  SA  5063', 'EDINBURGH NORTH  SA  5113', 'EDWARDSTOWN  SA  5039', 'ELIZABETH  SA  5112', 'ELIZABETH DOWNS  SA  5113', 'ELIZABETH EAST  SA  5112', 'ELIZABETH GROVE  SA  5112', 'ELIZABETH NORTH  SA  5113', 'ELIZABETH PARK  SA  5113', 'ELIZABETH SOUTH  SA  5112', 'ELIZABETH VALE  SA  5112', 'EVANSTON  SA  5116', 'EVANSTON PARK  SA  5116', 'EYRE  SA  5121', 'FINDON  SA  5023', 'FLINDERS PARK  SA  5025', 'FORTITUDE VALLEY  QLD  4006', 'FULLARTON  SA  5063', 'GAWLER  SA  5118', 'GAWLER EAST  SA  5118', 'GAWLER RIVER  SA  5118', 'GAWLER SOUTH  SA  5118', 'GILLES PLAINS  SA  5086', 'GLANDORE  SA  5037', 'GLENELG  SA  5045', 'GLYNDE  SA  5070', 'GOLDEN GROVE  SA  5125', 'GOULD CREEK  SA  5114', 'GPO Box 1533', 'GPO Box 2450', 'GREENACRES  SA  5086', 'GREENWITH  SA  5125', 'GULFVIEW HEIGHTS  SA  5096', 'HACKHAM  SA  5163', 'HACKNEY  SA  5069', 'HAMPSTEAD GARDENS  SA  5086', 'HENLEY BEACH  SA  5022', 'HEWETT  SA  5118', 'HILLBANK  SA  5112', 'HILLCREST  SA  5086', 'HILLIER  SA  5116', 'HINDMARSH  SA  5007', 'HOLDEN HILL  SA  5088', 'HOPE VALLEY  SA  5090', 'HUGHESDALE  VIC  3166', 'HUMBUG SCRUB  SA  5114', 'KADINA  SA  5554', 'KALBEEBA  SA  5118', 'KAPUNDA  SA  5373', 'KENSINGTON PARK  SA  5068', 'KENT TOWN  SA  5067', 'KENT TOWN  SA  5071', 'KERSBROOK  SA  5231', 'KESWICK  SA  5035', 'KLEMZIG  SA  5087', 'Ksd1', 'L28  91 King William Road', 'LARGS BAY  SA  5016', 'LEWISTON  SA  5501', 'LIGHTSVIEW  SA  5085', 'LILYDALE  VIC  3140', 'LONSDALE  SA  5160', 'Level 1', 'Level 1 74 Pirie Street', 'Level 1/74 Pirie Street', 'Level 18/25 Grenfell Street', 'Locked Bag 4001', 'Lot 10 Heaslip Road', 'MACDONALD PARK  SA  5121', 'MAGILL  SA  5072', 'MANNINGHAM  SA  5086', 'MANSFIELD PARK  SA', 'MANSFIELD PARK  SA  5012', 'MARDEN  SA  5070', 'MARLESTON  SA  5033', 'MAWSON LAKES  SA  5095', 'MAYLAND  SA  5069', 'MELBOURNE  VIC  4000', 'MELROSE PARK  SA  5039', 'MIDDLETON  SA  5213', 'MILDURA  VIC  3501', 'MILE END  SA  5031', 'MILLSWOOD  SA  5034', 'MITCHELL PARK  SA  5043', 'MODBURY  SA  5092', 'MODBURY HEIGHTS  SA  5092', 'MODBURY NORTH  SA  5092', 'MORPHETT VALE  SA  5162', 'MORPHETTVILLE  SA  5045', 'MOUNT BARKER  SA  5251', 'MOUNT OMMANEY  QLD  4074', 'MOUNT WAVERLEY  VIC  3149', 'MULGRAVE  VIC  3170', 'MUNNO PARA  SA  5115', 'MUNNO PARA DOWNS  SA  5115', 'MUNNO PARA WEST  SA  5115', 'MURRAY BRIDGE  SA  5254', 'NAIRNE  SA  5252', 'NEDLANDS  WA  6909', 'NEWTON  SA  5074', 'NORTH ADELAIDE  SA  5006', 'NORTH HAVEN  SA  5018', 'NORTH PLYMPTON  SA  5037', 'NORTHFIELD  SA  5085', 'NORWOOD  SA  5067', 'NURIOOTPA  SA  5355', "O'HALLORAN HILL  SA  5158", "O'SULLIVAN BEACH  SA  5166", 'OAKDEN  SA  5086', 'ONE TREE HILL  SA  5114', 'PARA HILLS  SA  5096', 'PARA HILLS WEST  SA  5096', 'PARA VISTA  SA  5093', 'PARADISE  SA  5075', 'PARAFIELD GARDENS  SA  5107', 'PARALOWIE  SA  5108', 'PARKSIDE  SA  5063', 'PASADENA  SA  5042', 'PAYNEHAM  SA  5070', 'PENFIELD  SA  5121', 'PENNINGTON  SA  5013', 'PLYMPTON  SA  5038', 'PO Box 1000', 'PO Box 227', 'PO Box 235', 'PO Box 248', 'PO Box 302', 'PO Box 3131', 'PO Box 32', 'PO Box 358', 'PO Box 4015', 'PO Box 523', 'PO Box 6', 'PO Box 603', 'PO Box 6196', 'PO Box 662', 'PO Box 849', 'PO Box 917', 'POORAKA  SA  5095', 'PORT ADELAIDE  SA  5015', 'PROSPECT  SA  5082', 'PROSPECT EAST  SA  5082', 'REDWOOD PARK  SA  5097', 'REGENCY PARK  SA  5010', 'REGENCY PARK  SA  5942', 'RIDGEHAVEN  SA  5097', 'ROBINA  QLD  4226', 'ROSE PARK  SA  5067', 'ROSEWORTHY  SA  5371', 'SALISBURY  SA  5108', 'SALISBURY DOWNS  SA  5108', 'SALISBURY EAST  SA  5109', 'SALISBURY HEIGHTS  SA  5109', 'SALISBURY NORTH  SA  5108', 'SALISBURY PARK  SA  5109', 'SALISBURY PLAIN  SA  5109', 'SALISBURY SOUTH  SA  5106', 'SEATON  SA  5023', 'SEAVIEW DOWNS  SA  5049', 'SEFTON PARK  SA  5083', 'SHEA-OAK LOG  SA  5371', 'SHEIDOW PARK  SA  5158', 'SMITHFIELD  SA  5114', 'SMITHFIELD PLAINS  SA  5114', 'SOUTH PLYMPTON  SA  5038', 'ST AGNES  SA  5097', 'ST CLAIR  SA  5011', 'ST MARYS  SA  5039', 'ST MARYS  SA  5042', 'STEPNEY  SA  5069', 'SURREY DOWNS  SA  5126', 'Suite 1/159 Port Road', 'Suite 12,154 Fullarton Road', 'TANUNDA  SA  5352', 'TEA TREE GULLY  SA  5091', 'THEBARTON  SA  5031', 'THORNTON  NSW  2322', 'TORRENSVILLE PLAZA  SA  5031', 'TWO WELLS  SA  5501', 'ULEYBURY  SA  5114', 'UNDERDALE  SA  5032', 'UNLEY PARK  SA  5061', 'VALE PARK  SA  5081', 'VALLEY VIEW  SA  5093', 'VIRGINIA  SA  5120', 'VISTA  SA  5091', 'WAIKERIE  SA  5330', 'WATERLOO CORNER  SA  5110', 'WAYVILLE  SA  5034', 'WELLAND  SA  5007', 'WEST CROYDON  SA  5008', 'WEST LAKES  SA  5021', 'WILLASTON  SA  5118', 'WILLIAMSTOWN  SA  5351', 'WILLUNGA  SA  5172', 'WINDSOR GARDENS  SA  5087', 'WINGFIELD  SA  5013', 'WODONGA  VIC  3690', 'WOODSIDE  SA  5244', 'WOODVILLE  SA  5011', 'WOODVILLE NORTH  SA  5012', 'WOODVILLE SOUTH  SA  5011', 'WYNN VALE  SA  5127', 'YATTALUNGA  SA  5114']</t>
         </is>
       </c>
     </row>
@@ -1119,7 +1119,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -1152,7 +1152,7 @@
         <v>0</v>
       </c>
       <c r="O8" t="n">
-        <v>2187</v>
+        <v>2466</v>
       </c>
       <c r="P8" t="n">
         <v>0</v>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>WALKERVILLE  SA  5081</t>
+          <t>ELIZABETH SOUTH  SA  5112</t>
         </is>
       </c>
       <c r="T8" t="n">
@@ -1175,20 +1175,20 @@
       </c>
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="n">
-        <v>2187</v>
+        <v>2466</v>
       </c>
       <c r="W8" t="n">
         <v>0</v>
       </c>
       <c r="X8" t="n">
-        <v>8049</v>
+        <v>8650</v>
       </c>
       <c r="Y8" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>['28 Franklin Street', 'ADELAIDE', 'ADELAIDE  SA  5000', 'ADELAIDE  SA  5001', 'ALDGATE  SA  5154', 'BROMPTON  SA  5007', 'BURTON  SA  5110', 'CLAPHAM  SA  5062', 'DAVOREN PARK  SA  5113', 'DUDLEY PARK  SA  5008', 'EASTWOOD  SA  5063', 'EDINBURGH NORTH  SA  5113', 'GAWLER  SA  5118', 'GAWLER SOUTH  SA  5118', 'GOLDEN GROVE  SA  5125', 'GOODWOOD  SA  5034', 'HINDMARSH  SA  5007', 'HOLDEN HILL  SA  5088', 'HOMEBUSH  NSW  2140', 'KENSINGTON PARK  SA  5068', 'KENT TOWN  SA  5067', 'KENT TOWN  SA  5071', 'MAGILL  SA  5072', 'MARDEN  SA  5070', 'MILE END SOUTH  SA  5031', 'MOORABBIN  VIC  3189', 'MORPHETT VALE  SA  5162', 'NEWTON  SA  5074', 'NORTH ADELAIDE  SA  5006', 'PASADENA  SA  5042', 'PORT ADELAIDE  SA  5015', 'PROSPECT  SA  5082', 'PROSPECT EAST  SA  5082', 'ROSE PARK  SA  5067', 'RUNDLE MALL  SA  5000', 'SALISBURY  SA  5108', 'SALISBURY SOUTH  SA  5106', 'SEATON  SA  5023', 'SOUTH PLYMPTON  SA  5038', 'TORRENSVILLE  SA  5031', 'UNDERDALE  SA  5032', 'WALKERVILLE  SA  5081', 'WAYVILLE  SA  5034']</t>
+          <t>['28 Franklin Street', '485 Kingsford Smith Drive', 'ADELAIDE', 'ADELAIDE  SA  5000', 'ADELAIDE  SA  5001', 'ALDGATE  SA  5154', 'BROMPTON  SA  5007', 'BURTON  SA  5110', 'CLAPHAM  SA  5062', 'DAVOREN PARK  SA  5113', 'DUDLEY PARK  SA  5008', 'EASTWOOD  SA  5063', 'EDINBURGH NORTH  SA  5113', 'ELIZABETH SOUTH  SA  5112', 'GAWLER  SA  5118', 'GAWLER SOUTH  SA  5118', 'GOLDEN GROVE  SA  5125', 'GOODWOOD  SA  5034', 'HINDMARSH  SA  5007', 'HOLDEN HILL  SA  5088', 'HOMEBUSH  NSW  2140', 'KENSINGTON PARK  SA  5068', 'KENT TOWN  SA  5067', 'KENT TOWN  SA  5071', 'MAGILL  SA  5072', 'MARDEN  SA  5070', 'MILE END SOUTH  SA  5031', 'MOORABBIN  VIC  3189', 'MORPHETT VALE  SA  5162', 'NEWTON  SA  5074', 'NORTH ADELAIDE  SA  5006', 'PASADENA  SA  5042', 'PORT ADELAIDE  SA  5015', 'PROSPECT  SA  5082', 'PROSPECT EAST  SA  5082', 'ROSE PARK  SA  5067', 'RUNDLE MALL  SA  5000', 'SALISBURY  SA  5108', 'SALISBURY SOUTH  SA  5106', 'SEATON  SA  5023', 'SOUTH PLYMPTON  SA  5038', 'TORRENSVILLE  SA  5031', 'UNDERDALE  SA  5032', 'WALKERVILLE  SA  5081', 'WAYVILLE  SA  5034']</t>
         </is>
       </c>
     </row>
@@ -1207,7 +1207,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -1231,10 +1231,10 @@
         <v>-1</v>
       </c>
       <c r="L9" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M9" t="n">
-        <v>401</v>
+        <v>504</v>
       </c>
       <c r="N9" t="n">
         <v>0</v>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>Renovation of kitchen and removal of walls - Sch-1A</t>
+          <t>Construction of a verandah - sch 1a</t>
         </is>
       </c>
       <c r="T9" t="n">
@@ -1267,20 +1267,20 @@
         </is>
       </c>
       <c r="V9" t="n">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="W9" t="n">
         <v>0.167</v>
       </c>
       <c r="X9" t="n">
-        <v>146566</v>
+        <v>164277</v>
       </c>
       <c r="Y9" t="n">
-        <v>1051</v>
+        <v>1164</v>
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t xml:space="preserve">['292/V026/20- Removal of 14 Regulated trees (4 Significant)  and major pruning of 22 Regulated trees( 10 Significant) in conjunction with Gawler Rail electrification', '?Eyre Stage 4A2 ? ENGINEERING', 'A change of use to consulting rooms with an ancillary store, including an internal fit out and addition to an existing building and alterations to an existing car park and the provision of landscaping, the commencement of advertising and demolition of a shed', 'ALMOND GROVE STAGE 9B ? ENGINEERING', 'Addition &amp; Alterations to existing McDonalds Restaurant', 'Addition to existing verandah', 'Additions &amp; Alterations to existing dwelling', 'Additions &amp; alterations to existing dwelling including a new verandah &amp; replacement of a domestic outbuilding &amp; carport', 'Additions and alterations to an existing detached dwelling comprising internal alterations and a partial change of use of an existing outbuilding', 'Additions and alterations to existing dwelling including a two storey addition as well as construction of a domestic outbuilding and retaining walls', 'Additions to an existing carport', 'Aerobic Waste System', 'Aerobic Wasterwater System', 'Aerobic Wastewater System', 'Aerobic Wastewater System - Pressurised Sub-Surface Soakage Bed', 'Aerobic Wastewater System - RiCycle EP20', 'Aerobic Wastewater system', 'Aerobic wastewater system', 'Alteration of a dwelling (install strutting beam) - Sch-1A reference to 292/662/2018', 'Alteration to Irrigation Area', 'Alteration to Septic Soakage Trench', 'Alteration to Underfloor Plumbing', 'Alteration to a road for the construction of a driveway onto an Arterial Road (Womma Road, Edinburgh North) and alterations to existing car parking', 'Alteration to existing Light Industry building in the form of ancillary offices and amenities', 'Alteration to existing Light Industry building in the form of ancillary transportable office building', 'Alteration to existing dwelling - replacement of existing window with a sliding door', 'Alteration to existing soakage', 'Alteration to existing system', 'Alteration to existing wastewater', 'Alteration to existing wastewater plumbing', 'Alteration to existing wastewater system', 'Alteration to irrigation area', 'Alteration to septic soakage trench', 'Alteration to under floor plumbing', 'Alteration to underfloor plumbing', 'Alteration to wastewater system', 'Alterations and additions to an existing dwelling -Withdrawn', 'Alterations and additions to an existing dwelling and retaining wall', 'Alterations and additions to an existing dwelling for the purposes of supported accommodation', 'Alterations and additions to an existing educational establishment and the construction of a car park.', 'Alterations and additions to existing building for the purposes of general industry and the construction of an associated office.\n\nSTAGE 3: Completed Factory Building and Services', 'Alterations and additions to existing dwelling', 'Alterations and additions to existing dwelling and construction of a deck and verandah', 'Alterations and additions to existing fitness centre building and alterations to existing carparking', 'Alterations and additions to existing single storey detached dwelling', 'Alterations to Stage 2 of division:  Amended plan of division to provide 6 additional allotments and amended SMP.\nTorrens title land division 2 into 66 (292/D090/15)', 'Alterations to an existing service station including fa?ade upgrades, internal alterations and signage including pylon sign', 'Alterations to existing dwelling and the construction of a carport and verandah', 'Alterations to existing dwelling and the construction of a verandah and deck', 'Alterations to existing under floor plumbing', 'Amendment to swimming pool safety barriers and increase to boundary fence (maximum hieght 2.5m)', 'Application for a holding tank', 'Application lodged on 292/1788/2020', 'BROOKMONT - ENGINEERING STAGE 5', 'BROOKMONT - ENGINEERING STAGE 6', 'BURGUNDY ESTATE Stage 2B &amp; 3 ? ENGINEERING', 'Boundary Realignment two allotments into two (D017/20)', 'Boundary re-alignment two allotments into two (292/D023/20)', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20.\n\nStage 1: Siteworks and Footings', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20.\n\nStage 2: Structure excluding internal work', 'CHIVELL GROVE STAGE 2 ? ENGINEERING', 'CONSTRUCTION OF A VERANDAH - RESCODE', 'Change of Use from Dwelling to office', 'Change of Use to a Takeaway Shop', 'Change of land use to a restaurant, internal fit out, internal and external alterations to existing shop and associated signage (5076- Zitto)', 'Change of land use to a restaurant, internal fit out, internal and external alterations to existing shop and associated signage (5076- Zitto) \n\nStage 1: Change of class &amp; internal fitout', 'Change of land use to a restaurant, internal fit out, internal and external alterations to existing shop and associated signage (5076- Zitto) \n\nStage 2: External works &amp; associated signage', 'Change of land use to a waste storage facility- FURTHER INFO EMAILED 26/10', 'Change of land use to horticulture and the construction of three glasshouses, a warehouse and packing shed, loading canopy, three dams, staff room and amenities building, four maintenance sheds, six water tanks, staff car park and landscaping', 'Change of land use to horticulture comprising structures (twelve greenhouses) and the construction of an ancillary packing and implement shed, dam and carpark and the placement of rainwater tanks.', 'Change of land use to light industry in the form of sheet metal fabrication, the construction of a canopy and advertising signage and the placement of a shipping container', 'Change of use and conversion of a residential dwelling to a medical clinic and consulting room with associated carparking - WITHDRAWN', 'Change of use and internal and external alterations to an existing building for self storage units', 'Change of use from Storage of Automotive parts to General Industry', 'Change of use from community centre to a multiple dwelling, the construction of a detached transportable unit, installation of three (3) shipping containers and additions and alterations to the existing building', 'Change of use from domestic outbuilding to Place of Worship', 'Change of use from outbuilding to temporary place of worship &amp; proposing marquee installed to be temporarily used for worship and celebrations', 'Change of use to a restaurant', 'Change of use to a training facility and internal alterations', 'Change of use to consulting rooms including alterations and additions of existing building with associated advertising signage, car parking and demolition of existing outbuildings at 24 Siddall Road (Stage 1), alterations to existing car park at 28 &amp; 30 Oldham Road (Stage 2), demolition of dwellings and associated outbuildings and change of use to at grade car park at 28 &amp; 30 Siddall Road (Stage 2)', 'Change of use to disability services with associated car parking', 'Change of use to dog grooming salon', 'Change of use to educational room and associated offices - Australia Workplace Training (Raleigh Chambers)', 'Change of use to include crushing of asphalt waste onsite', 'Change of use to office and assocciated fit-out (HS07C)', 'Change of use to office and supported accommodation', 'Change of use to special events space', 'Change of use to waste processing station in the form of a wrecking yard', 'Community Land Division 1 in to 2  (Existing dwelling to remain ) 292/C025/20 - rescode DPC', 'Con struction of a verandah - Rescode certified', 'Constrtuction of a carport', 'Constructioin of detached dwelling with garage UMR', 'Construction a detached dwelling with attached verandah and a freestanding carport', 'Construction of  a Verandah', 'Construction of  a detached dwelling with garage UMR- withdraw', 'Construction of  verandah - rescode', 'Construction of 2 Retaining Walls with a fence above 2.1 metres in total height.', 'Construction of 2 domestic outbuildings', 'Construction of 2 verandahs', 'Construction of 2 x verandah', 'Construction of 2 x verandahs', 'Construction of 2 x verandahs Sch1a', 'Construction of 3 Verandahs', 'Construction of 3 x dwellings with attached carports', 'Construction of 3x shade sails in association with an existing child care centre', 'Construction of 4 x two storey dwellings', 'Construction of 4x single storey dwelling - rescode certified', 'Construction of 5 green houses and dam with ancillary store, carparking and amenities', 'Construction of 7 x Greenhouses &amp; a Dam', 'Construction of 9 single storey dwellings', 'Construction of Detached Dwelling with a Garage under the main roof', 'Construction of Green House', 'Construction of Greenhouses', 'Construction of Horticulture Structures (Greenhouses) and a Dam', 'Construction of Verandah', 'Construction of Verandah ( Schedule 1A)', 'Construction of Verandah (Schedule 1a)', 'Construction of a 2 storey detached dwelling with attached garage  and verandah', 'Construction of a 2 verandahs', 'Construction of a 66kV Transmission Line - 292/V031/20', 'Construction of a Boundary fence to 2.7m high', 'Construction of a Carport', 'Construction of a Carport &amp; Verandah', 'Construction of a Carport &amp; two x Verandahs', 'Construction of a Carport - Rescode certified', 'Construction of a Carport - SCH1A', 'Construction of a Carport - Sch 1a', 'Construction of a Carport to existing Dwelling &amp; the construction of Storage/Packing Shed with attached verandah', 'Construction of a Carport- Sch1A', 'Construction of a Commerical Storage Shed', 'Construction of a Detached Dwelling', 'Construction of a Detached Dwelling - Res code Certifiied', 'Construction of a Detached Dwelling with Garage Locataed Under Main Roof', 'Construction of a Detached Dwelling with Garage Located Under Main Roof', 'Construction of a Detached Dwelling with Garage Under Main Roof', 'Construction of a Domestic Outbuilding- sch1a', 'Construction of a Domestic outbuilding', 'Construction of a Dwelling - Rescode certified', 'Construction of a Farm building &amp; Greenhouses', 'Construction of a Garage- Sch 1a', 'Construction of a Implement Shed (Farm Building)', 'Construction of a Rumpus Room and Sleep Out', 'Construction of a Shade Sail', 'Construction of a Swimming Pool &amp; Associated Safety Barrier.', 'Construction of a Swimming Pool &amp; Associated Safety Barrier/Fence', 'Construction of a Swimming Pool &amp; safety barrier', 'Construction of a Verandah', 'Construction of a Verandah &amp; Carport', 'Construction of a Verandah &amp; Deck', 'Construction of a Verandah ( Shedule 1A)', 'Construction of a Verandah -  Sch1A', 'Construction of a Verandah - Complying', 'Construction of a Verandah - RESCODE', 'Construction of a Verandah - Rescode certified', 'Construction of a Verandah - SCH1A', 'Construction of a Verandah - Sch1A', 'Construction of a Verandah - rescode certfied', 'Construction of a Verandah - sch1a', 'Construction of a Verandah, Carport &amp; External Dwelling Addition (Rumpus Room)', 'Construction of a Verandah- SCH1A', 'Construction of a Verandah- SCHEDULE 1A', 'Construction of a Verandah- sch1A', 'Construction of a Verandah- sch1a', 'Construction of a Verandah-Sch1A', 'Construction of a boundary fence (western) to a height of 2.6 metres', 'Construction of a canopy', 'Construction of a carport', 'Construction of a carport - SCH1A', 'Construction of a carport - Sch 1A', 'Construction of a carport - Sch 1a', 'Construction of a carport - Sch-1A', 'Construction of a carport - Sch1A', 'Construction of a carport - Schedule 1A', 'Construction of a carport - rescode', 'Construction of a carport - rescode certfied', 'Construction of a carport - sch 1a', 'Construction of a carport and domestic outbuilding - email &amp; letter sent 26/10/2020', 'Construction of a carport and garage', 'Construction of a carport and verandah', 'Construction of a carport attached to existing dependent accommodation', 'Construction of a carport attached to existing outbuilding', 'Construction of a carport, verandah and freestanding domestic outbuilding (shed)', 'Construction of a carport- Sch1A', 'Construction of a carpot - Sch-1A', 'Construction of a childcare centre with associated advertising, car park resulting in tree damaging activity, fencing, retaining walls, masonry entry wall, storage sheds and landscaping', 'Construction of a commercial  shed', 'Construction of a commercial/industrial shed', 'Construction of a dam and associated pump shed with surrounding fence', 'Construction of a deatched dwelling with a garage under the main roof', 'Construction of a deatched two storey dwelling with garage UMR', 'Construction of a deck', 'Construction of a detached Dwelling with Garage Located Under Main Roof', 'Construction of a detached dweling with verandah and garage under main roof', 'Construction of a detached dwelling', 'Construction of a detached dwelling  - rescode certified', 'Construction of a detached dwelling ( Lot 119 Parkvale Drive)', 'Construction of a detached dwelling ( Lot 128 Parkvale Drive)', 'Construction of a detached dwelling ( Res Code  Certified)', 'Construction of a detached dwelling (Lot 102 Parkvale Drive)', 'Construction of a detached dwelling (Lot 105 Damien Street)', 'Construction of a detached dwelling (Lot 110 Damien street)', 'Construction of a detached dwelling (Res Code Certifed)', 'Construction of a detached dwelling (Res Code Certified)', 'Construction of a detached dwelling -  Rescode certified', 'Construction of a detached dwelling - Rescode Certified', 'Construction of a detached dwelling - Rescode certified', 'Construction of a detached dwelling - Rescode certified- WITHDRAWN', 'Construction of a detached dwelling - Schedule 4 1(1)a (Complying)', 'Construction of a detached dwelling - Withdrawn', 'Construction of a detached dwelling - rescode', 'Construction of a detached dwelling - rescode - WITHDRAWN', 'Construction of a detached dwelling - rescode certified', 'Construction of a detached dwelling a with garage under the main roof', 'Construction of a detached dwelling and outbuilding and  placement of a water tank', 'Construction of a detached dwelling and retaining walls (Lot 1081 Highview drive)', 'Construction of a detached dwelling to be used as a display home (Lot 100 Parkvale drive)', 'Construction of a detached dwelling to be used as a display home (Lot 101  Parkvale drive)', 'Construction of a detached dwelling to be used as a display home for a period of up to 5 years', 'Construction of a detached dwelling to be used as a display home for a period of up to 5 years and associated signage', 'Construction of a detached dwelling wiith a garage under the main roof', 'Construction of a detached dwelling with a garage and alfresco under main roof', 'Construction of a detached dwelling with a garage and alfresco under the main roof', 'Construction of a detached dwelling with a garage and terrace under main roof', 'Construction of a detached dwelling with a garage and verandah under main roof', 'Construction of a detached dwelling with a garage under main roof', 'Construction of a detached dwelling with a garage under the main roof', 'Construction of a detached dwelling with a garage under the main roof  and associated retaining walls', 'Construction of a detached dwelling with a garage under the main roof - WITHDRAWN', 'Construction of a detached dwelling with a garage under the main roof and an associated retaining wall', 'Construction of a detached dwelling with a garage under the main roof and retaining walls', 'Construction of a detached dwelling with a garage, alfresco and verandah under main roof and associated retaining wall', 'Construction of a detached dwelling with an attached garage and two verandahs', 'Construction of a detached dwelling with attached carport and verandah', 'Construction of a detached dwelling with attached carport and verandah - Awaiting Civil Plans- WITHDRAWN', 'Construction of a detached dwelling with attached garage', 'Construction of a detached dwelling with attached garage  to be used as a temporary display home with associated office and advertising displays.', 'Construction of a detached dwelling with attached garage - (Lot 3120, Reel Tce)', 'Construction of a detached dwelling with attached garage - Awaiting CT', 'Construction of a detached dwelling with attached garage and freestanding carport', 'Construction of a detached dwelling with attached garage and veradahs', 'Construction of a detached dwelling with attached garage and verandah', 'Construction of a detached dwelling with attached garage and verandah (temporary display home)', 'Construction of a detached dwelling with attached garage and verandah - Awaiting Civil Plan- WITH DRAWN', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary display home with associated office and advertising display.', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary display home with associated office and signage\n\nStage 1: Footings Only', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary display home with associated office and signage\n\nStage 2: Final', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary sales &amp; project office', 'Construction of a detached dwelling with attached garage and verandah under main roof and associated retaining walls', 'Construction of a detached dwelling with attached garage and verandahs', 'Construction of a detached dwelling with attached garage and verandahs - WITHDRAWN', 'Construction of a detached dwelling with attached garage and verandahs to be used as a temporary display home with associated office and signage\n\nStage 1: construction of display building and associated display office (only)', 'Construction of a detached dwelling with attached garage and verandahs- WITHDRAWN', 'Construction of a detached dwelling with attached garage and vernadah - Waiting on civil/stormwater plan- WITHDRAWN', 'Construction of a detached dwelling with attached garage and verndah', 'Construction of a detached dwelling with attached garage to be used as a temporary display home with associated advertising displays.', 'Construction of a detached dwelling with attached garage, verandah and associated retaining wall', 'Construction of a detached dwelling with attached garage, verandah and associated retaining wall -', 'Construction of a detached dwelling with attached garage, verandah and associated retaining wall - (Lot 25 Highview Drive)', 'Construction of a detached dwelling with attached garage.', 'Construction of a detached dwelling with attached verandah', 'Construction of a detached dwelling with attached verandah and a freestanding carport', 'Construction of a detached dwelling with attached verandah and carport', 'Construction of a detached dwelling with carport UMR', 'Construction of a detached dwelling with garage &amp; verandah UMR', 'Construction of a detached dwelling with garage - temporary display home', 'Construction of a detached dwelling with garage UMR', 'Construction of a detached dwelling with garage UMR ( House 1)', 'Construction of a detached dwelling with garage UMR ( House 2)', 'Construction of a detached dwelling with garage UMR ( lot 2031 Lindgren Avenue', 'Construction of a detached dwelling with garage UMR ( lot 2032 Lindgren Avenue', 'Construction of a detached dwelling with garage UMR (Res Code)', 'Construction of a detached dwelling with garage UMR- LODGED IN ERROR', 'Construction of a detached dwelling with garage UMR- WITHDRAWN', 'Construction of a detached dwelling with garage and alfresco under main roof', 'Construction of a detached dwelling with garage and veranda under main roof', 'Construction of a detached dwelling with garage and verandah under main roof', 'Construction of a detached dwelling with garage and verandah under main roof and retaining walls to a maximum height of 3.5m', 'Construction of a detached dwelling with garage and verandahs under main roof', 'Construction of a detached dwelling with garage located under main roof', 'Construction of a detached dwelling with garage located under main roof - Lot 797 Philip Avenue, Angle Vale', 'Construction of a detached dwelling with garage to be used as a temporary display home', 'Construction of a detached dwelling with garage umr', 'Construction of a detached dwelling with garage under main roof', 'Construction of a detached dwelling with garage under main roof ( Lot 87 Parkvale Drive)', 'Construction of a detached dwelling with garage under main roof - WITHDRAWN', 'Construction of a detached dwelling with garage under main roof and a verandah', 'Construction of a detached dwelling with garage under main roof.', 'Construction of a detached dwelling with garage under the main roof', 'Construction of a detached dwelling with garage under the main roof ( Lot 109 Damien Street)', 'Construction of a detached dwelling with garage under the main roof - Lot 111 Damien Street', 'Construction of a detached dwelling with garage under the main roof.', 'Construction of a detached dwelling with garage underthe main roof ( Lot 127 Parkvale Drive)', 'Construction of a detached dwelling with the garage under the main roof', 'Construction of a detached dwelling with the garage under the main roof.', 'Construction of a detached dwelling with verandah and garage (Lot 170 Damien street)', 'Construction of a detached dwelling with verandah and garage under main roof', 'Construction of a detached dwelling with verandah and garage under main roof (Lot 2022 Lindgren Avenue)', 'Construction of a detached dwelling with verandah and garage under main roof (Lot 2023 Lindgren Avenue)', 'Construction of a detached dwelling with verandah and garage under main roof - WITHDRAWN', 'Construction of a detached dwelling with verandah and garage under mian roof', 'Construction of a detached dwelling with verandah, porch and  garage under main roof', 'Construction of a detached dwelling with verandahs and garage under main roof', 'Construction of a detached dwelling with verandahs and garage under main roof (Lot 117 Damien street)', 'Construction of a detached dwelling- Rescode certified', 'Construction of a detached dwelling- WITHDRAWN', 'Construction of a detached dwelling- rescode certified', 'Construction of a detached dwelling- rescode certified WITHDRAWN', 'Construction of a detached dwelling-WITHDRAWN', 'Construction of a detached dwellng with garage UMR', 'Construction of a disability toilet - Fremont Park', 'Construction of a domesetic outbuilding (shed)', 'Construction of a domestic garage', 'Construction of a domestic out building - Sch1a', 'Construction of a domestic out building - sch 1a', 'Construction of a domestic out building - sch1a', 'Construction of a domestic out building and verandah', 'Construction of a domestic outbuilding', 'Construction of a domestic outbuilding  - Sch1A', 'Construction of a domestic outbuilding &amp; a Verandah', 'Construction of a domestic outbuilding (garage)', 'Construction of a domestic outbuilding (garage), 1.8m high masonary fence, pool equipment shed and verandah\n\nStage 1: Domestic outbuilding (garage) and 1.8m high masonary fence', 'Construction of a domestic outbuilding (garage), 1.8m high masonary fence, pool equipment shed and verandah\nStage 1: Domestic outbuilding (garage) and 1.8m high masonary fence\nStage 2: Pool equipment shed and verandah', 'Construction of a domestic outbuilding (partially enclosed verandah)', 'Construction of a domestic outbuilding (shed)', 'Construction of a domestic outbuilding (shed) &amp; verandah', 'Construction of a domestic outbuilding (workshop &amp; garage)', 'Construction of a domestic outbuilding - Rescode certified', 'Construction of a domestic outbuilding - SCH1A', 'Construction of a domestic outbuilding - Sch 1a', 'Construction of a domestic outbuilding - Sch1A', 'Construction of a domestic outbuilding - Sch1a', 'Construction of a domestic outbuilding - Schedule 1A', 'Construction of a domestic outbuilding - Shed', 'Construction of a domestic outbuilding - rescode certified', 'Construction of a domestic outbuilding - sch 1a', 'Construction of a domestic outbuilding - sch1a', 'Construction of a domestic outbuilding -Sch1a', 'Construction of a domestic outbuilding and carport', 'Construction of a domestic outbuilding and two verandahs', 'Construction of a domestic outbuilding and verandahs', 'Construction of a domestic outbuilding- SCH1A', 'Construction of a domestic outbuilding- Sch 1a', 'Construction of a domestic outbuilding- Sch1A', 'Construction of a domestic outbuilding- sch1a', 'Construction of a domestic shed - Sch1A', 'Construction of a double storey detached dwelling - rescode certified', 'Construction of a dwelliing (Res Code Certified )', 'Construction of a dwelling ( Lot 238 Greenhood)', 'Construction of a dwelling ( Lot 240 Greenhood)', 'Construction of a dwelling ( Lot 241 Greenhood)', 'Construction of a dwelling ( Res Code Certified)', 'Construction of a dwelling (Lot 239 Greenhood)', 'Construction of a dwelling (Res Code Certifed)', 'Construction of a dwelling (Res Code Certified)', 'Construction of a dwelling (Res Code)', 'Construction of a dwelling (lot 206)', 'Construction of a dwelling -  rescode certified', 'Construction of a dwelling - -rescode certified', 'Construction of a dwelling - ResCode Certified', 'Construction of a dwelling - Rescode Certfied', 'Construction of a dwelling - Rescode Certified', 'Construction of a dwelling - Rescode certifed', 'Construction of a dwelling - Rescode certified', 'Construction of a dwelling - Rescode certified - (Lot 2)', 'Construction of a dwelling - rescode certifed', 'Construction of a dwelling - rescode certified', 'Construction of a dwelling - rescode certified - WITHDRAWN', 'Construction of a dwelling - rescode certified- WITHDRAWN', 'Construction of a dwelling - resocde certified', 'Construction of a dwelling addition - Rescode certified', 'Construction of a dwelling addition, verandahs and deck', 'Construction of a dwelling and a carport', 'Construction of a dwelling extension (bathroom extension)', 'Construction of a dwelling extension - rescode certified', 'Construction of a dwelling extension, verandah and installation of a pool', 'Construction of a dwelling for the purposes of supported accomodation ( Lot 2)', 'Construction of a dwelling for the purposes of supported accomodation (Lot 1)', 'Construction of a dwelling in the form of dependent accommodation', 'Construction of a dwelling with attached garage - WITHDRAWN', 'Construction of a dwelling with attached garage and verandah', 'Construction of a dwelling with attached garage and verandah- WITHDRAWN', 'Construction of a dwelling with carport - Site 207', 'Construction of a dwelling with carport - Site 213', 'Construction of a dwelling with carport - Site 214', 'Construction of a dwelling with detached carport', 'Construction of a dwelling with garage - Rescode certified', 'Construction of a dwelling with garage under main roof', 'Construction of a dwelling, carport and deck (lot 212 )', 'Construction of a dwelling- Rescode Certified', 'Construction of a dwelling- Rescode certified', 'Construction of a dwelling- Rescode certified - WITHDRAWN', 'Construction of a dwelling- rescode certified', 'Construction of a dwelling. RES CODE certified', 'Construction of a farm building', 'Construction of a farm building and fence', 'Construction of a farm implement shed', 'Construction of a freestanding gable verandah', 'Construction of a freestanding verandah (Site 41)', 'Construction of a gable verandah ( Schedule 1A)', 'Construction of a garage and demolition of existing carport', 'Construction of a glasshouse\n\nStage 2: Final', 'Construction of a greenhouse with associated dam and carparking', 'Construction of a horse shelter', 'Construction of a implement shed', 'Construction of a implement shed for use in association with existing farming operations', 'Construction of a light industrial building (caravan repairs) with associated carparking and landscaping', 'Construction of a masonry fence with  signage', 'Construction of a new dwelling - Rescode certified', 'Construction of a new entry and crossover- refferal from SCAP for Council to provide comment', 'Construction of a new glass balustrade - Level 1 Building 7', 'Construction of a outbuilding', 'Construction of a outbuilding with attached verandah', 'Construction of a packing shed', 'Construction of a pump and storage shed in association with existing horticulture', 'Construction of a replacement fence (2.19m high) on existing retaining wall', 'Construction of a retaining wall', 'Construction of a retaining wall (1m) with a total fence height of 2.8m', 'Construction of a retaining wall (Stage 3 &amp; 4 Evergreen Estate)', 'Construction of a retaining wall (maximum height 750mm) and fence (1.8m)', 'Construction of a retaining wall and fence', 'Construction of a rumpus room', 'Construction of a second dwelling in the form of dependent accomodation', 'Construction of a shade sail', 'Construction of a shade sail ( Fremont park)', 'Construction of a shade sail structure', 'Construction of a shed', 'Construction of a shed - Sch1a', 'Construction of a sign - park reserve (Parkview Walk)\nSchedule 3, Part 2(e) ? buildings in a recreation area- Withdrawn', 'Construction of a sign - park reserve (Perre Reserve)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve (Ramsay Park)', 'Construction of a sign - park reserve (Secombe Street)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve (Virginia Oval-Sign 2)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve (Virginia Oval-sign 1)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve sign (California Reserve)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve sign (Honeysuckle Reserve)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - reserve sign (Smithfield Memorial Garden)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - reserve sign (Smithfield Oval)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - reserve sign (Uley Reserve West)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - reserve sign (Uley Reserve)\nSchedule 3, Part 2(e) ? buildings in a recreation area', 'Construction of a sign - suburb sign (Andrews Farm)', 'Construction of a sign - suburb sign (Davoren Park)', 'Construction of a sign - suburb sign (Elizabeth Downs)', 'Construction of a single storey additions to existing dwelling', 'Construction of a single storey detached dwelling', 'Construction of a single storey detached dwelling\n\nStage 1: Footings Only', 'Construction of a single storey detached dwelling\n\nStage 2: Final', 'Construction of a single storey detached dwelling (transportable)', 'Construction of a single storey detached dwelling - WITHDRAWN', 'Construction of a single storey detached dwelling - rescode', 'Construction of a single storey detached dwelling and associated retaining walls up to a height of 1.0 metre', 'Construction of a single storey detached dwelling and freestanding carport', 'Construction of a single storey detached dwelling with garage under main roof', 'Construction of a single storey detached dwelling- WITHDRAWN', 'Construction of a single storey detached dwelling- rescode certified', 'Construction of a single storey dwelling', 'Construction of a single storey dwelling (Lot 229 Greenhood)', 'Construction of a single storey dwelling (Lot 230 Greenhood)', 'Construction of a single storey dwelling (Lot 231 Greenhood)', 'Construction of a single storey dwelling (Lot 232 Greenhood)', 'Construction of a single storey dwelling - Rescode certified', 'Construction of a single storey dwelling addition', 'Construction of a single storey dwelling with detached carport', 'Construction of a single storey dwelling with garage - Rescode certified', 'Construction of a single storey dwelling with garage - rescode certified', 'Construction of a sleepout- Rescode Certified', 'Construction of a spa and associated safety barrier and decking surrounding the spa', 'Construction of a </t>
+          <t>['292/V026/20- Removal of 14 Regulated trees (4 Significant)  and major pruning of 22 Regulated trees( 10 Significant) in conjunction with Gawler Rail electrification', '?Eyre Stage 4A2 ? ENGINEERING', 'A change of use to consulting rooms with an ancillary store, including an internal fit out and addition to an existing building and alterations to an existing car park and the provision of landscaping, the commencement of advertising and demolition of a shed', 'ALMOND GROVE STAGE 9B ? ENGINEERING', 'Addition &amp; Alterations to existing McDonalds Restaurant', 'Addition to existing verandah', 'Additions &amp; Alterations to existing dwelling', 'Additions &amp; alterations to existing dwelling', 'Additions &amp; alterations to existing dwelling including a new verandah &amp; replacement of a domestic outbuilding &amp; carport', 'Additions and alterations to an existing detached dwelling comprising internal alterations and a partial change of use of an existing outbuilding', 'Additions and alterations to existing dwelling including a two storey addition as well as construction of a domestic outbuilding and retaining walls', 'Additions to an existing carport', 'Aerobic Waste System', 'Aerobic Wasterwater System', 'Aerobic Wastewater System', 'Aerobic Wastewater System - Pressurised Sub-Surface Soakage Bed', 'Aerobic Wastewater System - RiCycle EP20', 'Aerobic Wastewater system', 'Aerobic wastewater system', 'Alteration of a dwelling (install strutting beam) - Sch-1A reference to 292/662/2018', 'Alteration to Irrigation Area', 'Alteration to Septic Soakage Trench', 'Alteration to Underfloor Plumbing', 'Alteration to a road for the construction of a driveway onto an Arterial Road (Womma Road, Edinburgh North) and alterations to existing car parking', 'Alteration to an existing wastewater system', 'Alteration to existing Light Industry building in the form of ancillary offices and amenities', 'Alteration to existing Light Industry building in the form of ancillary transportable office building', 'Alteration to existing dwelling - replacement of existing window with a sliding door', 'Alteration to existing soakage', 'Alteration to existing system', 'Alteration to existing wastewater', 'Alteration to existing wastewater plumbing', 'Alteration to existing wastewater system', 'Alteration to irrigation', 'Alteration to irrigation area', 'Alteration to septic soakage trench', 'Alteration to under floor plumbing', 'Alteration to underfloor plumbing', 'Alteration to wastewater system', 'Alterations and additions to an existing dwelling -Withdrawn', 'Alterations and additions to an existing dwelling and retaining wall', 'Alterations and additions to an existing dwelling for the purposes of supported accommodation', 'Alterations and additions to an existing educational establishment and the construction of a car park.', 'Alterations and additions to existing building for the purposes of general industry and the construction of an associated office.\n\nSTAGE 3: Completed Factory Building and Services', 'Alterations and additions to existing dwelling', 'Alterations and additions to existing dwelling and construction of a deck and verandah', 'Alterations and additions to existing fitness centre building and alterations to existing carparking', 'Alterations and additions to existing single storey detached dwelling', 'Alterations to Stage 2 of division:  Amended plan of division to provide 6 additional allotments and amended SMP.\nTorrens title land division 2 into 66 (292/D090/15)', 'Alterations to an existing retail showroom', 'Alterations to an existing service station including fa?ade upgrades, internal alterations and signage including pylon sign', 'Alterations to existing dwelling and the construction of a carport and verandah', 'Alterations to existing dwelling and the construction of a verandah and deck', 'Alterations to existing under floor plumbing', 'Alterations to existing verandah', 'Amendment to swimming pool safety barriers and increase to boundary fence (maximum hieght 2.5m)', 'Application for a holding tank', 'Application lodged on 292/1788/2020', 'BROOKMONT - ENGINEERING STAGE 5', 'BROOKMONT - ENGINEERING STAGE 6', 'BURGUNDY ESTATE Stage 2B &amp; 3 ? ENGINEERING', 'Boundary Realignment two allotments into two (D017/20)', 'Boundary re-alignment two allotments into two (292/D023/20)', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20.\n\nStage 1: Siteworks and Footings', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20.\n\nStage 2: Structure excluding internal work', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20.\n\nStage 3: Additional 3 bays structure excluding internal work', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20.\n\nStage 4: Remainder of work', 'CHIVELL GROVE STAGE 2 ? ENGINEERING', 'CONSTRUCTION OF A VERANDAH - RESCODE', 'Change of Use from Dwelling to office', 'Change of Use to a Takeaway Shop', 'Change of land use to a restaurant, internal fit out, internal and external alterations to existing shop and associated signage (5076- Zitto)', 'Change of land use to a restaurant, internal fit out, internal and external alterations to existing shop and associated signage (5076- Zitto) \n\nStage 1: Change of class &amp; internal fitout', 'Change of land use to a restaurant, internal fit out, internal and external alterations to existing shop and associated signage (5076- Zitto) \n\nStage 2: External works &amp; associated signage', 'Change of land use to a waste storage facility- FURTHER INFO EMAILED 26/10', 'Change of land use to horticulture and the construction of fourteen greenhouses, a packing shed, two rainwater tanks, a stormwater dam and associated car parking', 'Change of land use to horticulture and the construction of three glasshouses, a warehouse and packing shed, loading canopy, three dams, staff room and amenities building, four maintenance sheds, six water tanks, staff car park and landscaping - WITHDRAWN', 'Change of land use to horticulture comprising structures (twelve greenhouses) and the construction of an ancillary packing and implement shed, dam and carpark and the placement of rainwater tanks.', 'Change of land use to light industry in the form of sheet metal fabrication, the construction of a canopy and advertising signage and the placement of a shipping container', 'Change of use and conversion of a residential dwelling to a medical clinic and consulting room with associated carparking - WITHDRAWN', 'Change of use and internal and external alterations to an existing building for self storage units', 'Change of use from Storage of Automotive parts to General Industry', 'Change of use from community centre to a multiple dwelling, the construction of a detached transportable unit, installation of three (3) shipping containers and additions and alterations to the existing building', 'Change of use from domestic outbuilding to Place of Worship', 'Change of use from outbuilding to temporary place of worship &amp; proposing marquee installed to be temporarily used for worship and celebrations', 'Change of use from shop to customer service centre (office) (Tenancy HS07)', 'Change of use to a restaurant', 'Change of use to a showroom with associated fit out &amp; carpark', 'Change of use to a training facility and internal alterations', 'Change of use to consulting rooms including alterations and additions of existing building with associated advertising signage, car parking and demolition of existing outbuildings at 24 Siddall Road (Stage 1), alterations to existing car park at 28 &amp; 30 Oldham Road (Stage 2), demolition of dwellings and associated outbuildings and change of use to at grade car park at 28 &amp; 30 Siddall Road (Stage 2)', 'Change of use to disability services with associated car parking', 'Change of use to dog grooming salon', 'Change of use to educational room and associated offices - Australia Workplace Training (Raleigh Chambers)', 'Change of use to include crushing of asphalt waste onsite', 'Change of use to office &amp; associated fitout - cancelled', 'Change of use to office and assocciated fit-out (HS07C)', 'Change of use to office and supported accommodation', 'Change of use to special events space', 'Change of use to waste processing station in the form of a wrecking yard', 'Community Land Division 1 in to 2  (Existing dwelling to remain ) 292/C025/20 - rescode DPC', 'Con struction of a verandah - Rescode certified', 'Constrtuction of a carport', 'Constructioin of detached dwelling with verandah and garage under main roof', 'Construction a detached dwelling with attached verandah and a freestanding carport', 'Construction a single storey detached dwelling', 'Construction of  a Verandah', 'Construction of  a detached dwelling with garage UMR- withdraw', 'Construction of  verandah - rescode', 'Construction of 2 Retaining Walls with a fence above 2.1 metres in total height.', 'Construction of 2 domestic outbuildings', 'Construction of 2 verandahs', 'Construction of 2 x dependant accommodation', 'Construction of 2 x verandah', 'Construction of 2 x verandahs', 'Construction of 2 x verandahs Sch1a', 'Construction of 2x Verandahs', 'Construction of 3 Verandahs', 'Construction of 3 x dwellings with attached carports', 'Construction of 3x shade sails in association with an existing child care centre', 'Construction of 4 x two storey dwellings', 'Construction of 4x single storey dwelling - rescode certified', 'Construction of 5 green houses and dam with ancillary store, carparking and amenities', 'Construction of 7 x Greenhouses &amp; a Dam', 'Construction of 9 single storey dwellings', 'Construction of Aged living &amp; associated support facilities - staged consent', 'Construction of Detached Dwelling with a Garage under the main roof', 'Construction of Green Houses', 'Construction of Green house', 'Construction of Greenhouses', 'Construction of Horticulture Structures (Greenhouses) and a Dam', 'Construction of Verandah', 'Construction of Verandah ( Schedule 1A)', 'Construction of Verandah (Schedule 1a)', 'Construction of a 2 storey detached dwelling with attached garage  and verandah', 'Construction of a 2 verandahs', 'Construction of a 66kV Transmission Line - 292/V031/20', 'Construction of a Boundary fence to 2.7m high', 'Construction of a Carport', 'Construction of a Carport &amp; Verandah', 'Construction of a Carport &amp; two x Verandahs', 'Construction of a Carport - Rescode certified', 'Construction of a Carport - SCH1A', 'Construction of a Carport - Sch 1a', 'Construction of a Carport to existing Dwelling &amp; the construction of Storage/Packing Shed with attached verandah', 'Construction of a Carport- Sch1A', 'Construction of a Carport- sch1a', 'Construction of a Commerical Storage Shed', 'Construction of a Deck &amp; Verandah', 'Construction of a Dependent Accommodation Building Comprising Bedroom, Rumpas Room and Amenities (Retrospective)', 'Construction of a Detached Dwelling', 'Construction of a Detached Dwelling - Res code Certifiied', 'Construction of a Detached Dwelling with Garage Located Under Main Roof', 'Construction of a Domestic Outbuilding- sch1a', 'Construction of a Domestic outbuilding', 'Construction of a Dwelling - Rescode Certified', 'Construction of a Dwelling - Rescode certified', 'Construction of a Farm building &amp; Greenhouses', 'Construction of a Garage- Sch 1a', 'Construction of a Granny Flat', 'Construction of a Implement Shed (Farm Building)', 'Construction of a Packing Shed', 'Construction of a Shade Sail', 'Construction of a Swimming Pool &amp; Associated Safety Barrier.', 'Construction of a Swimming Pool &amp; Associated Safety Barrier/Fence', 'Construction of a Swimming Pool &amp; safety barrier', 'Construction of a Verandah', 'Construction of a Verandah &amp; Carport', 'Construction of a Verandah &amp; Deck', 'Construction of a Verandah ( Shedule 1A)', 'Construction of a Verandah -  Sch1A', 'Construction of a Verandah - Complying', 'Construction of a Verandah - RESCODE', 'Construction of a Verandah - Rescode certified', 'Construction of a Verandah - SCH1A', 'Construction of a Verandah - Sch1A', 'Construction of a Verandah - rescode certfied', 'Construction of a Verandah - sch1a', 'Construction of a Verandah, Carport &amp; External Dwelling Addition (Rumpus Room)', 'Construction of a Verandah- SCH1A', 'Construction of a Verandah- SCHEDULE 1A', 'Construction of a Verandah- sch1A', 'Construction of a Verandah- sch1a', 'Construction of a Verandah-Sch1A', 'Construction of a an outbuilding', 'Construction of a boundary fence (western) to a height of 2.6 metres', 'Construction of a canopy', 'Construction of a carport', 'Construction of a carport - SCH1A', 'Construction of a carport - Sch 1A', 'Construction of a carport - Sch 1a', 'Construction of a carport - Sch-1A', 'Construction of a carport - Sch1A', 'Construction of a carport - Schedule 1A', 'Construction of a carport - rescode', 'Construction of a carport - rescode certfied', 'Construction of a carport - sch 1a', 'Construction of a carport and domestic outbuilding - email &amp; letter sent 26/10/2020', 'Construction of a carport and garage', 'Construction of a carport and verandah', 'Construction of a carport attached to existing dependent accommodation', 'Construction of a carport attached to existing outbuilding', 'Construction of a carport, verandah and freestanding domestic outbuilding (shed)', 'Construction of a carport- Sch1A', 'Construction of a carpot - Sch-1A', 'Construction of a childcare centre with associated advertising, car park resulting in tree damaging activity, fencing, retaining walls, masonry entry wall, storage sheds and landscaping', 'Construction of a commercial  shed', 'Construction of a commercial/industrial shed', 'Construction of a dam in association with horticulture with a surrounding fence and associated building used as a pump shed and irrigation store', 'Construction of a deatched dwelling with a garage under the main roof', 'Construction of a deatched two storey dwelling', 'Construction of a deck', 'Construction of a detached Dwelling', 'Construction of a detached dweling with verandah and garage under main roof', 'Construction of a detached dwelling', 'Construction of a detached dwelling  - rescode certified', 'Construction of a detached dwelling ( Lot 119 Parkvale Drive)', 'Construction of a detached dwelling ( Lot 128 Parkvale Drive)', 'Construction of a detached dwelling ( Res Code  Certified)', 'Construction of a detached dwelling ( Res Code Certifed)', 'Construction of a detached dwelling (Lot 102 Parkvale Drive)', 'Construction of a detached dwelling (Lot 105 Damien Street)', 'Construction of a detached dwelling (Lot 110 Damien street)', 'Construction of a detached dwelling (Res Code Ceretifed)', 'Construction of a detached dwelling (Res Code Certifed)', 'Construction of a detached dwelling (Res Code Certified)', 'Construction of a detached dwelling (Res Code)', 'Construction of a detached dwelling -  Rescode certified', 'Construction of a detached dwelling - Rescode Certified', 'Construction of a detached dwelling - Rescode certified', 'Construction of a detached dwelling - Rescode certified- WITHDRAWN', 'Construction of a detached dwelling - Schedule 4 1(1)a (Complying)', 'Construction of a detached dwelling - WITHDRAWN', 'Construction of a detached dwelling - Withdrawn', 'Construction of a detached dwelling - rescode', 'Construction of a detached dwelling - rescode - WITHDRAWN', 'Construction of a detached dwelling - rescode certified', 'Construction of a detached dwelling - rescode certified - WITHDRAWN', 'Construction of a detached dwelling a with garage under the main roof', 'Construction of a detached dwelling addition', 'Construction of a detached dwelling and associated retaining wall and fence totalling 3.1m in height', 'Construction of a detached dwelling and detached carport', 'Construction of a detached dwelling and outbuilding and  placement of a water tank', 'Construction of a detached dwelling and retaining walls (Lot 1081 Highview drive) WITHDRAWN', 'Construction of a detached dwelling for temporary use as a display home for a period of 3 years', 'Construction of a detached dwelling to be used as a display home (Lot 100 Parkvale drive)', 'Construction of a detached dwelling to be used as a display home (Lot 101  Parkvale drive)', 'Construction of a detached dwelling to be used as a display home for a period of up to 5 years', 'Construction of a detached dwelling to be used as a display home for a period of up to 5 years and associated signage', 'Construction of a detached dwelling to be used as a temporary display home for a period of up to 4 years', 'Construction of a detached dwelling wiith a garage under the main roof', 'Construction of a detached dwelling with a garage and alfresco under main roof', 'Construction of a detached dwelling with a garage and alfresco under the main roof', 'Construction of a detached dwelling with a garage and terrace under main roof', 'Construction of a detached dwelling with a garage and verandah under main roof', 'Construction of a detached dwelling with a garage under main roof', 'Construction of a detached dwelling with a garage under the main roof', 'Construction of a detached dwelling with a garage under the main roof  and associated retaining walls', 'Construction of a detached dwelling with a garage under the main roof - WITHDRAWN', 'Construction of a detached dwelling with a garage under the main roof and an associated retaining wall', 'Construction of a detached dwelling with a garage under the main roof and retaining walls', 'Construction of a detached dwelling with a garage, alfresco and verandah under main roof and associated retaining wall', 'Construction of a detached dwelling with an attached garage and two verandahs', 'Construction of a detached dwelling with associated retaining walls and colorbond fencing (maximum hieght 3.6m)', 'Construction of a detached dwelling with attached carport and verandah', 'Construction of a detached dwelling with attached carport and verandah - Awaiting Civil Plans- WITHDRAWN', 'Construction of a detached dwelling with attached garage', 'Construction of a detached dwelling with attached garage  to be used as a temporary display home with associated office and advertising displays.', 'Construction of a detached dwelling with attached garage - (Lot 3120, Reel Tce)', 'Construction of a detached dwelling with attached garage and freestanding carport', 'Construction of a detached dwelling with attached garage and veradahs', 'Construction of a detached dwelling with attached garage and verandah', 'Construction of a detached dwelling with attached garage and verandah (temporary display home)', 'Construction of a detached dwelling with attached garage and verandah - Awaiting Civil Plan- WITH DRAWN', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary display home with associated office and advertising display.', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary display home with associated office and signage\n\nStage 1: Footings Only', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary display home with associated office and signage\n\nStage 2: Final', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary sales &amp; project office', 'Construction of a detached dwelling with attached garage and verandah under main roof', 'Construction of a detached dwelling with attached garage and verandahs', 'Construction of a detached dwelling with attached garage and verandahs - WITHDRAWN', 'Construction of a detached dwelling with attached garage and verandahs to be used as a temporary display home with associated office and signage\n\nStage 1: construction of display building and associated display office (only)', 'Construction of a detached dwelling with attached garage and verandahs- WITHDRAWN', 'Construction of a detached dwelling with attached garage and vernadah - Waiting on civil/stormwater plan- WITHDRAWN', 'Construction of a detached dwelling with attached garage and verndah', 'Construction of a detached dwelling with attached garage to be used as a temporary display home with associated advertising displays.', 'Construction of a detached dwelling with attached garage, verandah and associated retaining wall', 'Construction of a detached dwelling with attached garage, verandah and associated retaining wall -', 'Construction of a detached dwelling with attached garage, verandah and associated retaining wall - (Lot 25 Highview Drive)', 'Construction of a detached dwelling with attached garage.', 'Construction of a detached dwelling with attached verandah', 'Construction of a detached dwelling with attached verandah and a freestanding carport', 'Construction of a detached dwelling with carport UMR', 'Construction of a detached dwelling with carport under main roof', 'Construction of a detached dwelling with garage', 'Construction of a detached dwelling with garage UMR', 'Construction of a detached dwelling with garage UMR ( lot 2031 Lindgren Avenue', 'Construction of a detached dwelling with garage UMR ( lot 2032 Lindgren Avenue', 'Construction of a detached dwelling with garage UMR (Lot 15 Heysen Circuit)', 'Construction of a detached dwelling with garage UMR (Res Code)', 'Construction of a detached dwelling with garage UMR - WITHDRAWN', 'Construction of a detached dwelling with garage UMR- LODGED IN ERROR', 'Construction of a detached dwelling with garage UMR- WITHDRAWN', 'Construction of a detached dwelling with garage UMR- WITHDRAWN- COUNCIL ERROR', 'Construction of a detached dwelling with garage UMR- awaiting civil plan 8/12', 'Construction of a detached dwelling with garage and alfresco under main roof', 'Construction of a detached dwelling with garage and alfresco under main roof and associated retaining walls', 'Construction of a detached dwelling with garage and veranda under main roof', 'Construction of a detached dwelling with garage and verandah under main roof', 'Construction of a detached dwelling with garage and verandah under main roof and retaining walls to a maximum height of 3.5m', 'Construction of a detached dwelling with garage and verandahs under main roof', 'Construction of a detached dwelling with garage located under main roof', 'Construction of a detached dwelling with garage under main roof', 'Construction of a detached dwelling with garage under main roof ( Lot 87 Parkvale Drive)', 'Construction of a detached dwelling with garage under main roof - WITHDRAWN', 'Construction of a detached dwelling with garage under main roof and a verandah', 'Construction of a detached dwelling with garage under main roof.', 'Construction of a detached dwelling with garage under the main roof', 'Construction of a detached dwelling with garage under the main roof ( Lot 109 Damien Street)', 'Construction of a detached dwelling with garage under the main roof - Lot 111 Damien Street', 'Construction of a detached dwelling with garage under the main roof.', 'Construction of a detached dwelling with garage underthe main roof ( Lot 127 Parkvale Drive)', 'Construction of a detached dwelling with the garage under the main roof', 'Construction of a detached dwelling with the garage under the main roof.', 'Construction of a detached dwelling with verandah and garage (Lot 170 Damien street)', 'Construction of a detached dwelling with verandah and garage under main roof', 'Construction of a detached dwelling with verandah and garage under main roof (Lot 2022 Lindgren Avenue)', 'Construction of a detached dwelling with verandah and garage under main roof (Lot 2023 Lindgren Avenue)', 'Construction of a detached dwelling with verandah and garage under main roof - WITHDRAWN', 'Construction of a detached dwelling with verandah and garage under mian roof', 'Construction of a detached dwelling with verandah, porch and  garage under main roof', 'Construction of a detached dwelling with verandahs and garage under main roof', 'Construction of a detached dwelling with verandahs and garage under main roof (Lot 117 Damien street)', 'Construction of a detached dwelling- Rescode certified', 'Construction of a detached dwelling- WITHDRAWN', 'Construction of a detached dwelling- rescode certified', 'Construction of a detached dwelling- rescode certified WITHDRAWN', 'Construction of a detached dwelling-WITHDRAWN', 'Construction of a detached dwelling.', 'Construction of a detached dwellng with garage UMR', 'Construction of a disability toilet - Fremont Park', 'Construction of a domesetic outbuilding (shed)', 'Construction of a domestic garage', 'Construction of a domestic out building - Sch1a', 'Construction of a domestic out building - sch 1a', 'Construction of a domestic out building - sch1a', 'Construction of a domestic out building and verandah', 'Construction of a domestic outbuilding', 'Construction of a domestic outbuilding  - Sch1A', 'Construction of a domestic outbuilding &amp; a Verandah', 'Construction of a domestic outbuilding (garage)', 'Construction of a domestic outbuilding (garage), 1.8m high masonary fence, pool equipment shed and verandah\n\nStage 1: Domestic outbuilding (garage) and 1.8m high masonary fence', 'Construction of a domestic outbuilding (garage), 1.8m high masonary fence, pool equipment shed and verandah\nStage 1: Domestic outbuilding (garage) and 1.8m high masonary fence\nStage 2: Pool equipment shed and verandah', 'Construction of a domestic outbuilding (partially enclosed verandah)', 'Construction of a domestic outbuilding (shed)', 'Construction of a domestic outbuilding (shed) &amp; verandah', 'Construction of a domestic outbuilding (workshop &amp; garage)', 'Construction of a domestic outbuilding - Rescode certified', 'Construction of a domestic outbuilding - SCH1A', 'Construction of a domestic outbuilding - Sch 1a', 'Construction of a domestic outbuilding - Sch1A', 'Construction of a domestic outbuilding - Sch1a', 'Construction of a domestic outbuilding - Schedule 1A', 'Construction of a domestic outbuilding - Shed', 'Construction of a domestic outbuilding - rescode certified', 'Construction of a domestic outbuilding - sch 1a', 'Construction of a domestic outbuilding - sch1a', 'Construction of a domestic outbuilding -Sch1a', 'Construction of a domestic outbuilding and carport', 'Construction of a domestic outbuilding and the temporary placement of three shipping containers for a period of 12 months', 'Construction of a domestic outbuilding and two verandahs', 'Construction of a domestic outbuilding and verandahs', 'Construction of a domestic outbuilding- SCH1A', 'Construction of a domestic outbuilding- Sch 1a', 'Construction of a domestic outbuilding- Sch1A', 'Construction of a domestic outbuilding- sch1a', 'Construction of a domestic shed - Sch1A', 'Construction of a double storey detached dwelling - rescode certified', 'Construction of a dwelliing (Res Code Certified )', 'Construction of a dwelling', 'Construction of a dwelling ( Lot 238 Greenhood)', 'Construction of a dwelling ( Lot 240 Greenhood)', 'Construction of a dwelling ( Lot 241 Greenhood)', 'Construction of a dwelling ( Res Code Certified)', 'Construction of a dwelling (Lot 239 Greenhood)', 'Construction of a dwelling (Res Code Certifed)', 'Construction of a dwelling (Res Code Certified)', 'Construction of a dwelling (Res Code)', 'Construction of a dwelling (lot 206)', 'Construction of a dwelling -  rescode certified', 'Construction of a dwelling - -rescode certified', 'Construction of a dwelling - ResCode Certified', 'Construction of a dwelling - Rescode Certfied', 'Construction of a dwelling - Rescode Certified', 'Construction of a dwelling - Rescode certifed', 'Construction of a dwelling - Rescode certified', 'Construction of a dwelling - Rescode certified - (Lot 2)', 'Construction of a dwelling - rescode certifed', 'Construction of a dwelling - rescode certified', 'Construction of a dwelling - rescode certified - WITHDRAWN', 'Construction of a dwelling - rescode certified- WITHDRAWN', 'Construction of a dwelling - resocde certified', 'Construction of a dwelling -Res Code Certifed', 'Construction of a dwelling -Rescode certified', 'Construction of a dwelling addition - Rescode certified', 'Construction of a dwelling addition, verandahs and deck', 'Construction of a dwelling and a carport', 'Construction of a dwelling extension', 'Construction of a dwelling extension (bathroom extension)', 'Construction of a dwelling extension - rescode certified', 'Construction of a dwelling extension, verandah and installation of a pool', 'Construction of a dwelling for the purposes of supported accomodation ( Lot 2)', 'Construction of a dwelling for the purposes of supported accomodation (Lot 1)', 'Construction of a dwelling in the form of dependent accommodation', 'Construction of a dwelling with attached garage - WITHDRAWN', 'Construction of a dwelling with attached garage and verandah', 'Construction of a dwelling with attached garage and verandah- WITHDRAWN', 'Construction of a dwelling with detached carport', 'Construction of a dwelling with garage - Rescode certified', 'Construction of a dwelling with garage UMR', 'Construction of a dwelling with garage under main roof', 'Construction of a dwelling with retaining walls', 'Construction of a dwelling, carport and deck (lot 212 )', 'Construction of a dwelling- Rescode Certified', 'Construction of a dwelling- Rescode certified', 'Construction of a dwelling- Rescode certified - WITHDRAWN', 'Construction of a dwelling- rescode certified', 'Construction of a dwelling. RES CODE certified', 'Construction of a farm building', 'Construction of a farm building and fence', 'Construction of a farm implement shed', 'Construction of a fence 2.5m - Brookmont Stage 5 perimeter fence', 'Construction of a freestanding gable verandah', 'Construction of a freestanding verandah (Site 41)', 'Construction of a front fence', 'Construction of a gable verandah ( Schedule 1A)', 'Construction of a garage and demolition of existing carport', 'Construction of a glasshouse\n\nStage 2: Final', 'Construction of a greenhouse with associated dam and carparking', 'Construction of a horse shelter', 'Construction of a implement shed', 'Construction of a implement shed and rainwater tank', 'Construction of a implement shed for use in association with existing farming operations', 'Construction of a light industrial building (caravan repairs) with associated carparking and landscaping', 'Construction of a masonry fence with  signage', 'Construction of a new dwelling - Rescode certified', 'Construction of a new entry and crossover- refferal from SCAP for Council to provide comment', 'Construction of a new glass balustrade - Level 1 Building 7', 'Construction of a outbuilding', 'Construction of a outbuilding with attached verandah', 'Construction of a packing shed', 'Construction of a partially enclosed verandah', 'Construction of a pump and storage shed in association with existing horticulture', 'Construction of a replacement fence (2.19m high) on existing retaining wall', 'Construction of a retaining wall', 'Construction of a retaining wall (1m) with a total fence height of 2.8m', 'Construction of a retaining wall (Stage 3 &amp; 4 Evergreen Estate)', 'Construction of a retaining wall (maximum height 750mm) and fence (1.8m)', 'Construction of a retaining wall and fence', 'Construction of a rumpus room', 'Construction of a second dwelling in the form of dependent accomodation', 'Construction of a shade sail', 'Construction of a shade sail ( Fremont park)', 'Construction of a shade sail structure', 'Construction of a shed', 'Construction of a shed - Sch 1a', 'Construction of a shed - Sch1a', 'Construction of a sign - park reserve (Parkview Walk)\nSchedule 3, Part 2(e) ? buildings in a recreation area- Withdrawn', 'Construction of a sign - park reserve (Perre Reserve)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve (Ramsay Park)', 'Construction of a sign - park reserve (Secombe Street)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve (Virginia Oval-Sign 2)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve (Virginia Oval-sign 1)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve sign (California Reserve)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn</t>
         </is>
       </c>
     </row>
@@ -1299,7 +1299,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -1359,13 +1359,13 @@
         </is>
       </c>
       <c r="V10" t="n">
-        <v>1840</v>
+        <v>2083</v>
       </c>
       <c r="W10" t="n">
         <v>1</v>
       </c>
       <c r="X10" t="n">
-        <v>80186</v>
+        <v>89838</v>
       </c>
       <c r="Y10" t="n">
         <v>14</v>
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P11" t="n">
         <v>0</v>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>31  John Circuit</t>
+          <t>71  Yelki Road</t>
         </is>
       </c>
       <c r="T11" t="n">
@@ -1447,20 +1447,20 @@
       </c>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="W11" t="n">
         <v>0</v>
       </c>
       <c r="X11" t="n">
-        <v>45403</v>
+        <v>50812</v>
       </c>
       <c r="Y11" t="n">
-        <v>2207</v>
+        <v>2469</v>
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>['1  Alessia Lane', '1  Anderson Walk', '1  Apsley Close', '1  Bauera Place', '1  Bayer Road', '1  Beaumont Road', '1  Blatchford Road', '1  Botany Drive', '1  Bracken Avenue', '1  Bright Court', '1  Brodie Circuit', '1  Burwood Road', '1  Catalonia Avenue', '1  Charlie Street', '1  Clementine Avenue', '1  Crostan Close', '1  Cumbria Way', '1  Damien Street', '1  Dayman Street', '1  Deverill Street', '1  Edmund Avenue', '1  English Court', '1  Fergusson Bowl', '1  Fortana Lane', '1  Hanne Street', '1  Highview Drive', '1  Inwood Road', '1  Kendell Lane', '1  Kerrie Avenue', '1  Lorikeet Place', '1  Lucca Close', '1  Luis Drive', '1  Majella Way', '1  Mary Close', '1  Mira Road', '1  Olive Grove', '1  Olsen Way', '1  Oraton Court', '1  Ormsby Road', '1  Parkvale Drive', '1  Pinda Court', '1  Rhus Avenue', '1  Riverview Drive', '1  Roxburgh Crescent', '1  Stocklinch Crescent', '1  Varney Court', '1  Walpole Street', '1  Warburton Street', '1  Westbury Court', '1  Wolsten Drive', '1-3  Odgers Road', '1-5/ 2  Anderson Walk', '10  Alderwood Court', '10  Anderson Street', '10  Barfield Crescent', '10  Bracken Avenue', '10  Breamore Street', '10  Bridport Street', '10  Brookfield Street', '10  Carric Court', '10  Cartwright Drive', '10  Charlie Street', '10  Cooper Place', '10  Damien Street', '10  Darling Street', '10  Dauntless Crescent', '10  Drimpton Street', '10  Dulcis Circuit', '10  Epsom Street', '10  Forest Court', '10  George Avenue', '10  Goulburn Street', '10  Greenhood Crescent', '10  Isabel Road', '10  Jenkins Road', '10  Karinga Crescent', '10  Kerrie Avenue', '10  Keysley Street', '10  Lakes Entrance', '10  Lawder Road', '10  Liebrooke Boulevard', '10  Lily Court', '10  Lindgren Avenue', '10  Magnolia Crescent', '10  Mary Close', '10  McInerney Court', '10  McNamara Way', '10  Melbury Street', '10  Michael Road', '10  Murcia Avenue', '10  Myrta Avenue', '10  Myrtle Avenue', '10  Oakwood Circuit', '10  Parkvale Drive', '10  Peacemarsh Road', '10  Pendolino Road', '10  Ranger Street', '10  Reel Terrace', '10  Rivitalo Avenue', '10  Samphire Avenue', '10  Scoular Road', '10  Tony Street', '10  Union Avenue', '10  Ward Street', '10  Wood Crescent', '10  Woodfalls Road', '100  Johnson Road', '100-106  Chellaston Road', '101  Park Terrace', '1027  Stebonheath Road', '103  Halsey Road', '103  Juniper Boulevard', '103  Keane Avenue', '104  Johns Road', '104  Keane Avenue', '104  Precolumb Road', '105  Keane Avenue', '1064  Old Port Wakefield Road', '107  Beckham Rise', '107  Juniper Boulevard', '107  Keane Avenue', '107  Womma Road', '1072  Gawler-One Tree Hill Road', '108  Douglas Drive', '108  Keane Avenue', '108  McKenzie Road', '1080  Andrews Road', '109  Juniper Boulevard', '109  Keane Avenue', '1097  Stebonheath Road', '10A  Chardonnay Court', '10A  Perre Drive', '10B  Burke Circuit', '11  Alex Street', '11  Arbequina Road', '11  Argyle Walk', '11  Ashwin Street', '11  Bastow Road', '11  Bauera Place', '11  Begonia Drive', '11  Belanger Court', '11  Berwick Rise', '11  Bracken Avenue', '11  Brodie Circuit', '11  Brunswick Terrace', '11  Carman Close', '11  Charlie Street', '11  Dimasi Court', '11  Dulcis Circuit', '11  Eucalyptus Crescent', '11  Gold Street', '11  Grainger Road', '11  Grandview Drive', '11  Grove Avenue', '11  Gunther Street', '11  Hanorah Avenue', '11  Hewitt Road', '11  Jane Street', '11  Kendell Lane', '11  Lindgren Avenue', '11  Litchfield Avenue', '11  Luis Drive', '11  Manston Street', '11  McNamara Way', '11  Parkinson Street', '11  Parkvale Drive', '11  Pendolino Road', '11  Peridot Loop', '11  Pioneer Way', '11  Prunus Court', '11  Ridgeway Road', '11  Rivitalo Avenue', '11  Sam Circuit', '11  Shaftesbury Road', '11  Tony Street', '11  Waratah Avenue', '11  Wyong Crescent', '11  Yamuna Avenue', '110  Douglas Drive', '110  Keane Avenue', '110  Yorktown Road', '111  Flinders Road', '111  Johnson Road', '111  Keane Avenue', '111  Viney Drive', '112  Coventry Road', '112  Karwin Road', '112  Keane Avenue', '112  Tyeka Drive', '113  Keane Avenue', '114-116  Heaslip Road', '115  Crittenden Road', '115  Sampson Road', '1159  Stebonheath Road', '1161  Stebonheath Road', '1163  Stebonheath Road', '1165  Stebonheath Road', '1167  Stebonheath Road', '1169  Stebonheath Road', '117  Forrestall Road', '117-119  Heaslip Road', '1184  Stebonheath Road', '119  Keane Avenue', '119  Kelly Hill Road', '12  Apple Close', '12  Baker Court', '12  Beatrix Drive', '12  Black Top Road', '12  Bracken Avenue', '12  Bradpole Road', '12  Cameron Road', '12  Charleston Terrace', '12  Charlie Street', '12  Chivell Road', '12  Cleveland Road', '12  Cooper Place', '12  Coulter Street', '12  Damien Street', '12  Dana Street', '12  Dulcis Circuit', '12  Edward Avenue', '12  Elm Drive', '12  Epsom Street', '12  Esperance Drive', '12  Eucalyptus Crescent', '12  Federation Close', '12  Fradd Road', '12  Fruin Close', '12  Greenhood Crescent', '12  Hanorah Avenue', '12  Hewittson Road', '12  Isabel Road', '12  Kathleen Crescent', '12  Lawder Road', '12  Lindgren Avenue', '12  Luis Drive', '12  Mandel Street', '12  Martha Way', '12  McNamara Way', '12  Myrta Avenue', '12  Myrtle Avenue', '12  Natasha Avenue', '12  Noble Road', '12  Olsen Way', '12  Palmer Road', '12  Parkvale Drive', '12  Peacemarsh Road', '12  Pine Avenue', '12  Reel Terrace', '12  Rivitalo Avenue', '12  Sam Circuit', '12  Samphire Avenue', '12  Sasha Drive', '12  Sharrad Court', '12  Sturt Circuit', '12  Wolsten Drive', '120  Coventry Road', '1200  Andrews Road', '1201  Heaslip Road', '121  Keane Avenue', '121  Philip Highway', '121-129  Heaslip Road', '1219  Heaslip Road', '122  Crittenden Road', '123  Hogarth Road', '123  Keane Avenue', '123  McEvoy Road', '124  Douglas Drive', '125  Womma West Road', '1278  Gawler-One Tree Hill Road', '12A  Figsbury Street', '12B  Redwood Avenue', '13  Alex Street', '13  Bastow Road', '13  Bauera Place', '13  Brodie Circuit', '13  Burnett Drive', '13  Davalan Drive', '13  Eucalypt Circuit', '13  Eucalyptus Crescent', '13  Forest Court', '13  Geoff Road', '13  George Avenue', '13  Grant Street', '13  Hanorah Avenue', '13  Harris Road', '13  Horrie Knight Crescent', '13  John Circuit', '13  Kendell Lane', '13  Lawder Road', '13  Luis Drive', '13  McNamara Way', '13  McPherson Grove', '13  Myrta Avenue', '13  Natasha Avenue', '13  Oxford Terrace', '13  Parham Street', '13  Parkvale Drive', '13  Pedlar Close', '13  Prelude Circuit', '13  Prosperity Way', '13  Ranger Street', '13  Rivitalo Avenue', '13  Sam Circuit', '13  Stone Road', '13  Swan Crescent', '13  Waratah Avenue', '13  Wolsten Drive', '130  Haydown Road', '130  Willison Road', '1304  Angle Vale Road', '133  Keane Avenue', '134  Tyeka Drive', '1349  Stebonheath Road', '135  Keane Avenue', '136  McKenzie Road', '136  Penfield Road', '137  Angle Vale Road', '138  Supple Road', '138  Yorktown Road', '139  Kentish Road', '139  Lakeside Drive', '13A  Salerno Court', '14  Allington Street', '14  Boucaut Avenue', '14  Brandis Road', '14  Bridget Court', '14  Carmela Avenue', '14  Charleston Terrace', '14  Charlson Street', '14  Cleveland Road', '14  Clover Court', '14  Coonawarra Avenue', '14  Cruikshank Street', '14  Damien Street', '14  Dana Street', '14  Darling Street', '14  Dulcis Circuit', '14  Durrington Road', '14  Edmund Avenue', '14  Emerald Drive', '14  Eucalyptus Crescent', '14  Fradd Road', '14  Fruin Close', '14  George Avenue', '14  Green Court', '14  Greenhood Crescent', '14  Hughes Court', '14  John Rice Avenue', '14  Jordon Street', '14  Kathleen Crescent', '14  Knighton Road', '14  Lawder Road', '14  Lindgren Avenue', '14  Lomandra Crescent', '14  Luis Drive', '14  Mary Close', '14  McNamara Way', '14  Michael Road', '14  Myrta Avenue', '14  Myrtle Avenue', '14  Olsen Way', '14  Priority Court', '14  Prosperity Way', '14  Reel Terrace', '14  Rivitalo Avenue', '14  Sam Circuit', '14  Sissman Street', '14  Talbot Street', '14  Union Avenue', '14  Willys Street', '14  Wolsten Drive', '14  Yarnbrook Street', '14  Yorktown Road', '14-16  Heard Street', '140  Woodford Road', '141  Woodford Road', '143  Heaslip Road', '143  Lakeside Drive', '144  Halsey Road', '144  King Road', '147  Goodman Road', '149  Douglas Drive', '149  Frisby Road', '149  Tyeka Drive', '15  Abelia Street', '15  Adams Road', '15  Alex Street', '15  Bailey Road', '15  Beckham Rise', '15  Brodie Circuit', '15  Bubner Street', '15  Carioca Drive', '15  Coach House Mews', '15  Collins Street', '15  Crown Court', '15  Dulcis Circuit', '15  Edmund Avenue', '15  Epsom Street', '15  Eucalyptus Crescent', '15  Featherstone Street', '15  George Avenue', '15  Hermitage Drive', '15  Highview Drive', '15  Jenolan Crescent', '15  John Circuit', '15  Kernel Road', '15  Kingsbury Street', '15  Lafitte Way', '15  Lindgren Avenue', '15  Mary Close', '15  Myrta Avenue', '15  Nautilus Road', '15  Needlewood Court', '15  Parkvale Drive', '15  Peachey Road', '15  Portland Road', '15  Prominent Rise', '15  Rivitalo Avenue', '15  Rosewood Avenue', '15  Samphire Avenue', '15  Shandon Drive', '15  Sissman Street', '15  Southan Street', '15  Spruance Road', '15  St Clair Avenue', '15  St Leonard Crescent', '15  Webster Street', '15  Yorktown Road', '151  Douglas Drive', '152  Goulds Creek Road', '153  Angle Vale Road', '153  Carmelo Road', '154  Huxtable Road', '158  Penfield Road', '16  Alderwood Court', '16  Beatrix Drive', '16  Bentley Road', '16  Berkeley Way', '16  Breamore Street', '16  Cameron Road', '16  Charleston Terrace', '16  Damien Street', '16  Darling Street', '16  Dawn Close', '16  Dulcis Circuit', '16  Edward John Parade', '16  Elm Drive', '16  Emerald Drive', '16  Eucalyptus Crescent', '16  Figsbury Street', '16  Fradd Road', '16  George Avenue', '16  Grandview Place', '16  Hawick Avenue', '16  Hayles Road', '16  Highgate Mews', '16  Honeysuckle Drive', '16  Illawarra Court', '16  Karinga Crescent', '16  Kendell Lane', '16  Lawder Road', '16  Lindgren Avenue', '16  Lorna Court', '16  Michael Crescent', '16  Michael Road', '16  Murcia Avenue', '16  Myrta Avenue', '16  Myrtle Avenue', '16  Natasha Avenue', '16  Neagle Road', '16  Palari Crescent', '16  Pine Avenue', '16  Portland Road', '16  Ramsay Road', '16  Reel Terrace', '16  Rivitalo Avenue', '16  Sam Circuit', '16  Samphire Avenue', '16  Sharrad Court', '16  Sissman Street', '16  The Greenway', '16  Union Avenue', '16  Winkfield Street', '16  Wolsten Drive', '16  Wootton Street', '162  Philip Highway', '164  Harvey Road', '165  Ridley Road', '168  Julian Road', '168  Newton Boulevard', '16A  Redwood Avenue', '17  Alex Street', '17  Alexander Road', '17  Bastow Road', '17  Belanger Court', '17  Benham Street', '17  Birmingham Drive', '17  Brittlewood Drive', '17  Brodie Circuit', '17  Burley Griffin Drive', '17  Carey Street', '17  Charleston Terrace', '17  Charta Circuit', '17  Claret Avenue', '17  Cleveland Road', '17  Darling Street', '17  Drupe Street', '17  Dulcis Circuit', '17  Eucalyptus Crescent', '17  Featherstone Street', '17  Fradd Road', '17  Geoff Road', '17  George Avenue', '17  Harry Court', '17  Innes Street', '17  Kingsbury Street', '17  Lawder Road', '17  Lewis Drive', '17  Lindgren Avenue', '17  Longbridge Road', '17  Luis Drive', '17  Manya Crescent', '17  McNamara Way', '17  Mosterton Road', '17  Myrta Avenue', '17  Olivia Court', '17  Olsen Way', '17  Palari Crescent', '17  Parkvale Drive', '17  Rivitalo Avenue', '17  Rose Circuit', '17  Sam Circuit', '17  Samphire Avenue', '17  Scott Road', '17  Sissman Street', '17  St Leonard Crescent', '17  Tareena Street', '17  Tuggarah Street', '17  Varacalli Way', '17  Village Terrace', '17  Webster Street', '17  Wolsten Drive', '17  Wyong Crescent', '173  Woodford Road', '175  Williams Road', '17A  Everleigh Road', '18  Alawoona Road', '18  Applecross Drive', '18  Argent Street', '18  Bastow Road', '18  Bogan Road', '18  Bracken Avenue', '18  Bubner Road', '18  Carob Crescent', '18  Cawrse Street', '18  Charleston Terrace', '18  Darling Street', '18  Edmonds Road', '18  Edmund Avenue', '18  Emerald Drive', '18  Fantasia Drive', '18  Finnis Street', '18  George Avenue', '18  Green Crescent', '18  Harvest Court', '18  John Circuit', '18  Jordan Drive', '18  Keevil Street', '18  Lawder Road', '18  Lewis Drive', '18  Lorna Court', '18  Luis Drive', '18  Myrtle Avenue', '18  Ontario Crescent', '18  Oregon Avenue', '18  Pendolino Road', '18  Preston Street', '18  Reel Terrace', '18  Rivitalo Avenue', '18  Sam Circuit', '18  Samphire Avenue', '18  Sampson Road', '18  Sissman Street', '18  Union Avenue', '18  Varacalli Way', '18  Warragal Court', '18  Winkfield Street', '18  Yarnbrook Street', '18-20  Charlotte Street', '18-22  Anderson Walk', '180  Philip Highway', '182  Humbug Scrub Road', '185  Hannaford Hump Road', '185  Philip Highway', '185  Yorktown Road', '186  Ryan Road', '187  Hannaford Hump Road', '189  Philip Highway', '18B  Gould Road', '19  Alexander Road', '19  Banksia Crescent', '19  Bastow Road', '19  Bedchester Road', '19  Brodie Circuit', '19  Bundarra Court', '19  Carey Street', '19  Cleveland Road', '19  Cockshell Street', '19  Crisp Road', '19  Dawn Close', '19  Edmund Avenue', '19  Epsom Street', '19  Eucalyptus Crescent', '19  George Avenue', '19  Hambridge Road', '19  John Circuit', '19  Jordon Street', '19  Lakeside Drive', '19  Lawder Road', '19  Lewis Drive', '19  Lindgren Avenue', '19  Luis Drive', '19  Marleycombe Road', '19  Mary Close', '19  McNamara Way', '19  Myrta Avenue', '19  Parkvale Drive', '19  Ridgeway Road', '19  Rivitalo Avenue', '19  Sam Circuit', '19  Samphire Avenue', '19  Scoular Road', '19  Secombe Street', '19  Sissman Street', '19  St Clair Avenue', '19  Sturt Circuit', '19  Toorak Drive', '19  Winklebury Road', '19  Wolsten Drive', '19  Wyong Crescent', '190  Taylors Road', '190  Williams Road', '194  Petherton Road', '195  Midway Road', '197  Curnow Road', '198  President Avenue', '19A  Bartlett Street', '1A  Lawder Road', '1B  Lawder Road', '2  Ballard Street', '2  Bastow Road', '2  Blackham Crescent', '2  Blatchford Road', '2  Blunden Court', '2  Burdett Street', '2  Burke Circuit', '2  Carric Court', '2  Cooper Place', '2  Davey Street', '2  Fyfield Street', '2  Hanne Street', '2  Howegate Lane', '2  Innes Street', '2  Kerrie Avenue', '2  Kerry Close', '2  MacFarlane Way', '2  Madison Street', '2  Martha Way', '2  McLean Street', '2  McNamara Way', '2  Michael Road', '2  Mission Court', '2  Morris Street', '2  Parker Road', '2  Parkvale Drive', '2  Peachey Road', '2  Prominent Rise', '2  Reel Terrace', '2  Sam Circuit', '2  Saverio Boulevard', '2  Smith Place', '2  Sturt Circuit', '2  Sussex Court', '2  Teofilo Street', '2  Wills Court', '2  Yamuna Avenue', '2-4  Priority Court', '2/ 17  Bellchambers Road', '20  Ascot Avenue', '20  Ashfield Road', '20  Ashwin Street', '20  Balmoral Circuit', '20  Briar Road', '20  Bridport Street', '20  Brookmont Boulevard', '20  Cleveland Road', '20  Darling Street', '20  Emerald Drive', '20  Esperance Drive', '20  Fradd Road', '20  Gladman Close', '20  Highland Circuit', '20  Justinian Street', '20  Karrawirra Close', '20  Lawder Road', '20  Lindgren Avenue', '20  Lonsdale Crescent', '20  Luis Drive', '20  Magnolia Crescent', '20  Manningford Road', '20  McGilp Road', '20  McNamara Way', '20  Murcia Avenue', '20  Myrtle Avenue', '20  Olivia Court', '20  Priority Court', '20  Reel Terrace', '20  Rivitalo Avenue', '20  Rowe Street', '20  Sam Circuit', '20  Samphire Avenue', '20  Sampson Road', '20  Toorak Drive', '20  Tyalla Court', '20  Union Avenue', '20  Waratah Avenue', '20  Woodford Road', '200  Thompson Road', '201  Symes Road', '202  President Avenue', '203  Main North Road', '204  President Avenue', '206  Petherton Road', '206  President Avenue', '21  Baron Road', '21  Bracken Avenue', '21  Brodie Circuit', '21  Castle Court', '21  Cork Avenue', '21  Drupe Street', '21  Dulcis Circuit', '21  Elly Drive', '21  Eucalyptus Crescent', '21  Fyfield Street', '21  George Avenue', '21  Grace Boulevard', '21  John Circuit', '21  Lewis Drive', '21  Lindgren Avenue', '21  Loftis Road', '21  Luis Drive', '21  Magnolia Crescent', '21  Maplewood Drive', '21  McNamara Way', '21  Mendota Avenue', '21  Parkvale Drive', '21  Peachey Road', '21  Rivitalo Avenue', '21  Rockbourne Street', '21  Sam Circuit', '21  Samphire Avenue', '21  Serenity Way', '21  Sissman Street', '21  Stanley Road', '21  Wanbi Court', '21  Waratah Avenue', '21  Webster Street', '21  Wolsten Drive', '21  Wyong Crescent', '210  Newton Boulevard', '210  President Avenue', '212  Newton Boulevard', '212  President Avenue', '213  Yorktown Road', '22  Alawoona Road', '22  Angove Drive', '22  Ashwin Street', '22  Bagalowie Crescent', '22  Booyong Drive', '22  Broadacres Drive', '22  Burnlea Parade', '22  Cleveland Road', '22  Dowie Way', '22  Emerald Drive', '22  Esperance Drive', '22  Eucalyptus Crescent', '22  Fantasia Drive', '22  Geoff Road', '22  Greenhood Crescent', '22  Hambridge Road', '22  Jane Street', '22  Kilsby Street', '22  Langford Drive', '22  Lindgren Avenue', '22  Luis Drive', '22  Max Fatchen Drive', '22  McNamara Way', '22  Murcia Avenue', '22  Myrtle Avenue', '22  Natasha Avenue', '22  Olinda Street', '22  Oxford Drive', '22  Patterson Road', '22  Riverglen Court', '22  Rivitalo Avenue', '22  Rushall Crescent', '22  Sam Circuit', '22  Samphire Avenue', '22  Senna Avenue', '22  Southan Street', '22  Traminer Drive', '22  Union Avenue', '22  Varacalli Way', '22  Wahroonga Drive', '22  Wolsten Drive', '222  President Avenue', '23  Banksia Crescent', '23  Bartlett Street', '23  Bridport Street', '23  Brodie Circuit', '23  Burley Road', '23  Cambridge Terrace', '23  Catalonia Avenue', '23  Cavenagh Street', '23  Charleston Crescent', '23  Chicklade Street', '23  Cleveland Road', '23  Crosby Road', '23  Deptford Street', '23  Dulcis Circuit', '23  Edmund Avenue', '23  Eucalyptus Crescent', '23  Geoff Road', '23  George Avenue', '23  Green Crescent', '23  Hanson Road', '23  Huon Road', '23  Jarvis Road', '23  John Circuit', '23  Lewis Drive', '23  Loftis Road', '23  Luis Drive', '23  Magor Street', '23  McNamara Way', '23  Parkvale Drive', '23  Rockbourne Street', '23  Sam Circuit', '23  Samphire Avenue', '23  Secombe Street', '23  Short Road', '23  Sissman Street', '23  Smitham Street', '23  Waratah Avenue', '23  Webster Street', '23  Wolsten Drive', '23  Wood Crescent', '23  Woodbridge Drive', '23  Wyong Crescent', '233  Curtis Road', '234  President Avenue', '238  Black Top Road', '238  Curtis Road', '24  Booyong Drive', '24  Broadwater Place', '24  Castleton Street', '24  Cleveland Road', '24  Emerald Drive', '24  Enterprise Circuit', '24  Esperance Drive', '24  Eucalyptus Crescent', '24  George Avenue', '24  Grandview Drive', '24  Hambridge Road', '24  John Circuit', '24  Kalamata Court', '24  Lewis Drive', '24  Luis Drive', '24  Max Fatchen Drive', '24  McNamara Way', '24  Murcia Avenue', '24  Myrtle Avenue', '24  Natasha Avenue', '24  Ontario Crescent', '24  Saint Germain Avenue', '24  Sam Circuit', '24  Senna Avenue', '24  Siddall Road', '24  Telowie Avenue', '24  The Avenue', '24  Traminer Drive', '24  Trinity Way', '24  Union Avenue', '24  Waratah Avenue', '24-30  Durrington Road', '244  Curtis Road', '245  Alexander Avenue', '247  Hogarth Road', '25  Bell Street', '25  Bellchambers Road', '25  Bressington Drive', '25  Cambridge Terrace', '25  Catalonia Avenue', '25  Chiselbury Road', '25  Clark Road', '25  Cleveland Road', '25  Dulcis Circuit', '25  Elizabeth Way', '25  Geoff Road', '25  George Avenue', '25  Horrie Knight Crescent', '25  John Circuit', '25  Kerrie Avenue', '25  Lancaster Court', '25  Lewis Drive', '25  McNamara Way', '25  Midlow Road', '25  Palmer Road', '25  Patterson Road', '25  Pedlar Close', '25  Sam Circuit', '25  Samphire Avenue', '25  Tudor Crescent', '25  Waratah Avenue', '25  Wood Crescent', '25  Wyong Crescent', '252  Midway Road', '255  Womma West Road', '258  Riggs Road', '259  Fradd East Road', '25A  Sissman Street', '25B  Sissman Street', '26  Alawoona Road', '26  Alexandrina Crescent', '26  Amberdale Road', '26  Burley Griffin Drive', '26  Cavenagh Street', '26  Cleveland Road', '26  Edmonds Road', '26  Edmund Avenue', '26  Emerald Drive', '26  Esperance Drive', '26  Eucalyptus Crescent', '26  Flannery Crescent', '26  Hodgson Road', '26  John Circuit', '26  Justinian Street', '26  Kingsbury Street', '26  Liebrooke Boulevard', '26  Lorna Court', '26  McNamara Way', '26  Minchington Road', '26  Murcia Avenue', '26  Odgers Road', '26  Sam Circuit', '26  Senna Avenue', '26  Siddall Road', '26  Union Avenue', '260  Carclew Road', '261  Midway Road', '267  Riggs Road', '268  Midway Road', '26B  Redwood Avenue', '26C  Redwood Avenue', '27  Booyong Drive', '27  Burnett Drive', '27  Catalonia Avenue', '27  Chellaston Road', '27  Dulcis Circuit', '27  George Avenue', '27  Ina Close', '27  John Circuit', '27  Jordan Drive', '27  Kentish Road', '27  Kernel Road', '27  Lewis Drive', '27  Parkvale Drive', '27  Sam Circuit', '27  Telowie Avenue', '27  Waratah Avenue', '27  Wyong Crescent', '270  Moloney Road', '272  Curtis Road', '28  Ballard Road', '28  Brittlewood Drive', '28  Burke Circuit', '28  Castleton Street', '28  Emerald Drive', '28  Esperance Drive', '28  Greenhood Crescent', '28  Harvest Court', '28  John Circuit', '28  Laxton Road', '28  Levant Street', '28  Lewis Drive', '28  Luis Drive', '28  McNamara Way', '28  Oldham Road', '28  Penfold Road', '28  Sam Circuit', '28  Saverio Boulevard', '28  Senna Avenue', '28  Siddall Road', '28  Tollerdown Street', '28  Union Avenue', '28  Zurich Road', '281  Stebonheath Road', '283  Stebonheath Road', '286  Craigmore Road', '287  Carmelo Road', '287  Fradd East Road', '28B  Mavros Road', '29  Ashwin Street', '29  Baldina Crescent', '29  Birchdale Circuit', '29  Booyong Drive', '29  Brimsdown Road', '29  Carrama Crescent', '29  Catalonia Avenue', '29  Dowie Way', '29  Lewis Drive', '29  Librandi Street', '29  Luis Drive', '29  Max Fatchen Drive', '29  McNamara Way', '29  Old Sarum Road', '29  Oxford Court', '29  Parkvale Drive', '29  Sam Circuit', '29  Samphire Avenue', '29  Sissman Street', '29  Waratah Avenue', '29  Wyong Crescent', '3  Adams Road', '3  Alessia Lane', '3  Apsley Close', '3  Augusta Square', '3  Bastow Road', '3  Bauera Place', '3  Baxter Avenue', '3  Begonia Drive', '3  Brodie Circuit', '3  Catalonia Avenue', '3  Cleveland Road', '3  Colombo Court', '3  Cooper Place', '3  Damien Street', '3  Darling Street', '3  Drupe Street', '3  English Court', '3  Forde Street', '3  Fortana Lane', '3  George Avenue', '3  Glory Road', '3  Grand Road', '3  Hannah Road', '3  Hanorah Avenue', '3  John Circuit', '3  Kensington Mews', '3  Kerrie Avenue', '3  Lauren Lane', '3  Lindgren Avenue', '3  Longstaff Lane', '3  Lucca Close', '3  Luis Drive', '3  MacPharlin Court', '3  Majella Way', '3  Martha Way', '3  Mary Close', '3  Midlow Road', '3  Mira Road', '3  Myrta Avenue', '3  Natalia Road', '3  Olivia Court', '3  Ormsby Road', '3  Oxford Terrace', '3  Parkvale Drive', '3  Peridot Loop', '3  Prosperity Way', '3  Riverview Drive', '3  Rivitalo Avenue', '3  Russell Court', '3  Seavington Road', '3  Sienna Road', '3  Silk Road', '3  Spratt Street', '3  Stocklinch Crescent', '3  Sturt Circuit', '3  Tea Tree Drive', '3  The Grove', '3  Tilshead Road', '3  Tony Street', '3  Torrens Street', '3  Trinity Way', '3  Virgara Court', '3  Warburton Street', '3  Willison Road', '3  Wolsten Drive', '3  Yamuna Avenue', '3/ 4  Fletcher Road', '30  Benham Street', '30  Brittlewood Drive', '30  Clover Court', '30  Elly Drive', '30  Emerald Drive', '30  Esperance Drive', '30  Faulding Avenue', '30  Green Court', '30  Highview Drive', '30  John Circuit', '30  Kerrie Avenue', '30  Levant Street', '30  Lewis Drive', '30  Luis Drive', '30  Mavros Road', '30  McGilp Road', '30  McKenzie Road', '30  McNamara Way', '30  McPherson Grove', '30  Odgers Road', '30  Oldham Road', '30  Sam Circuit', '30  Senna Avenue', '30  Siddall Road', '30  Stockton Street', '30  Waratah Avenue', '30  William Drive', '306  Taylors Road', '31  Ashwin Street', '31  Ballard Road', '31  Chateau Avenue', '31  Collingbourne Drive', '31  Edmund Avenue', '31  Harris Road', '31  Huon Road', '31  John Circuit', '31  Kernel Road', '31  Luis Drive', '31  McNamara Way', '31  Paginton Crescent', '31  Parkvale Drive', '31  Pedlar Close', '31  Sam Circuit', '31  Southan Street', '31  Telowie Avenue', '31  Waratah Avenue', '31  Wyong Crescent', '31A  Kentish Road', '32  Brookmont Boulevard', '32  Castleton Street', '32  Chaddenwick Road', '32  Highview Drive', '32  John Circuit', '32  McNamara Way', '32  Murcia Avenue', '32  Odgers Road', '32  Sam Circuit', '32  Scoular Road', '32  Sheedy Road', '32  Uley Road', '32  Waratah Avenue', '321  Tozer Road', '323  Peachey Road', '329  Peachey Road', '329  Stebonheath Road', '33  Angle Vale Road', '33  Baldina Crescent', '33  Bellchambers Road', '33  Broadmeadows Road', '33  Catalonia Avenue', '33  Davey Street', '33  Edmund Avenue', '33  Hambridge Road', '33  Highview Drive', '33  Kerrie Avenue', '33  Mayfair Drive', '33  McKay Road', '33  McNamara Way', '33  Megunya Crescent', '33  Moloney Road', '33  Parkvale Drive', '33  Pix Road', '33  Scott Road', '33  Telowie Avenue', '33  Vincent Road', '33  Vokes Road', '33  Waratah Avenue', '33  Woodbridge Drive', '331  Peachey Road', '331  Stebonheath Road', '333  Peachey Road', '333  Stebonheath Road', '335  Stebonheath Road', '337  Stebonheath Road', '339  Stebonheath Road', '34  Ascot Avenue', '34  Burwood Road', '34  Emerald Circuit', '34  Green Court', '34  Heysen Court', '34  Highview Drive', '34  John Circuit', '34  Luis Drive', '34  Plane Tree Drive', '34  Richardson Road', '34  Sam Circuit', '34  Waratah Avenue', '34  Whitford Road', '341  Peachey Road', '343  Peachey Road', '343  Stebonheath Road', '345  Stebonheath Road', '347  Peachey Road', '347  Stebonheath Road', '34B  Ballard Road', '34B  Hooper Road', '35  Andrews Road', '35  Bailey Road', '35  Catalonia Avenue', '35  Edmund Avenue', '35  Elizabeth Way', '35  Homington Road', '35  Lewis Drive', '35  Linger Crescent', '35  Luis Drive', '35  Mayfair Drive', '35  Parkvale Drive', '35  Pedlar Close', '35  Seavington Road', '35  Stevens Drive', '35  Waratah Avenue', '35  Woodbridge Drive', '352  Alexander Avenue', '354  Fradd East Road', '357  Stebonheath Road', '36  Clementine Avenue', '36  Highview Drive', '36  Jordan Drive', '36  Luis Drive', '36  McKay Road', '36  McNamara Way', '36  Moir Street', '36  Robert Road', '36  Sam Circuit', '36  Saverio Boulevard', '36  Waratah Avenue', '36  West Parkway', '36-40  John Rice Avenue', '361  Stebonheath Road', '363  Stebonheath Road', '36C  Halsey Road', '37  Bassnet Road', '37  Browne Circuit', '37  Catalonia Avenue', '37  Green Crescent', '37  Kerrie Avenue', '37  Lewis Drive', '37  Luis Drive', '37  McNamara Way', '37  Olive Grove', '37  Oxford Terrace', '37  Pedlar Close', '37  Rosewood Avenue', '37  Spruance Road', '37  Stevens Drive', '37  Vincent Road', '37  Waratah Avenue', '37  Yarnbrook Street', '37A  Kinkaid Road', '37A  Nautilus Road', '37B  Oxford Terrace', '38  Bagot Road', '38  Chellaston Road', '38  Greenhood Crescent', '38  John Circuit', '38  Kakuna Crescent', '38  McNamara Way', '38  Sam Circuit', '38  Waratah Avenue', '38  West Parkway', '39  Bellchambers Road', '39  Catalonia Avenue', '39  Chellaston Road', '39  Coratina Road', '39  Davoren Road', '39  Edmonds Road', '39  Edmund Avenue', '39  Fantasia Drive', '39  Haydown Road', '39  Lewis Drive', '39  McNamara Way', '39  Pedlar Close', '39  Ramnet Circuit', '39  Waratah Avenue', '39  Yarnbury Road', '390  Fradd East Road', '394  Fradd East Road', '39A  Ballard Road', '39B  Ballard Road', '3A  Kilsby Street', '3A  Lawder Road', '3B  Willison Road', '4  Angel Street', '4  Ash Place', '4  Ashwin Street', '4  Barossa Drive', '4  Begonia Drive', '4  Blatchford Road', '4  Brodie Circuit', '4  Burnett Drive', '4  Burra Street', '4  Cadillac Street', '4  Carric Court', '4  Castor Avenue', '4  Cathy Mews', '4  Charlie Street', '4  Charlson Street', '4  Charmouth Road', '4  Chellaston Road', '4  Chowilla Court', '4  Colins Court', '4  Damien Street', '4  De Luca Court', '4  Dulcis Circuit', '4  Dylan Close', '4  Emerald Drive', '4  English Court', '4  Forest Court', '4  Fradd Court', '4  Fradd Road', '4  Fruin Close', '4  George Avenue', '4  Glory Road', '4  Goulburn Street', '4  Grovely Street', '4  Hamptworth Street', '4  Hanne Street', '4  Harris Road', '4  Highgrove Court', '4  Joseph Court', '4  Kathleen Crescent', '4  Kendell Lane', '4  Kerry Close', '4  Kingsbury Street', '4  Lambrook Street', '4  Larkhill Road', '4  Levant Street', '4  Lewis Drive', '4  Librandi Street', '4  Lindgren Avenue', '4  Luis Drive', '4  Madison Street', '4  Mary Court', '4  Matthew Rise', '4  Michael Road', '4  Morris Street', '4  Myrtle Avenue', '4  Noble Road', '4  Oxford Drive', '4  Parkvale Drive', '4  Pix Road', '4  Platten Avenue', '4  Playford Boulevard', '4  Prunus Court', '4  Reel Terrace', '4  Rivitalo Avenue', '4  Salway Street', '4  Saverio Boulevard', '4  Sissman Street', '4  Smith Place', '4  Stapleton Street', '4  Teakle Court', '4  Vitana Court', '4  Vokes Road', '4  Waratah Avenue', '4  Warburton Street', '4  Whitehart Close', '4  Wills Court', '4  Windsor Court', '40  Angove Drive', '40  Cambridge Terrace', '40  John Rice Avenue', '40  Jordan Drive', '40  Luis Drive', '40  Olympic Way', '40  Pacific Boulevard', '40  Philip Highway', '40  Portland Road', '40  Serpentine Circuit', '40  Waratah Avenue', '40  West Parkway', '405  Craigmore Road', '407  Hillier Road', '41  Ballard Road', '41  Barfield Crescent', '41  Belanger Court', '41  Catalonia Avenue', '41  Clementine Avenue', '41  Crabb Road', '41  Fantasia Drive', '41  Grandview Drive', '41  Jenkins Road', '41  Lakeside Drive', '41  Lomalinda Drive', '41  Luis Drive', '41  Nilpena Court', '41  Pedlar Close', '41  Waratah Avenue', '412  Hillier Road', '41A  Johnston Road', '42  Elly Drive', '42  Greenhood Crescent', '42  Highview Drive', '42  Keane Avenue', '42  Olympic Way', '42  Park Terrace', '42  Saverio Boulevard', '42  Waratah Avenue', '42  West Parkway', '422  Alexander Avenue', '425  Hillier Road', '43  Barfield Crescent', '43  Catalonia Avenue', '43  Dartmouth Street', '43  Emerald Circuit', '43  Gooronga Drive', '43  Highview Drive', '43  Innes Street', '43  Keane Avenue', '43  Lewis Drive', '43  Mayfair Drive', '43  McNamara Way', '43  Olympic Way', '43  Pedlar Close', '43  Saverio Boulevard', '43  Secombe Street', '43  Yeovil Circuit', '435  Coventry Road', '437  Coventry Road', '43A  Johnston Road', '44  Alawoona Road', '44  Clark Road', '44  Halsey Road', '44  Highview Drive', '44  John Circuit', '44  John Rice Avenue', '44  Olympic Way', '44  Saverio Boulevard', '44  Waratah Avenue', '44  West Parkway', '45  Catalonia Avenue', '45  Emerald Circuit', '45  Highview Drive', '45  Johnston Road', '45  Peachey Road', '45  Pedlar Close', '45  Riesling Crescent', '45  Saverio Boulevard', '45  Waratah Avenue', '45  Willison Road', '46  Baxter Avenue', '46  Brookmont Boulevard', '46  Grenadier Road', '46  Gunther Street', '46  Highfield Drive', '46  Highview Drive', '46  John Circuit', '46  John Rice Avenue', '46  Luis Drive', '46  Olympic Way', '46  Park Terrace', '46  Saverio Boulevard', '46  Waratah Avenue', '46  West Parkway', '461  Coventry Road', '47  Ascot Avenue', '47  Emerald Circuit', '47  Galda Way', '47  Mahood Street', '47  Pedlar Close', '47  Pipkin Road', '47  Sturt Circuit', '47  Waratah Avenue', '48  Coppleridge Drive', '48  Coratina Road', '48  Galda Way', '48  Hamblynn Road', '48  Highview Drive', '48  John Circuit', '48  Jordan Drive', '48  Marshalsea Road', '48  Morialta Drive', '48  Olympic Way', '48  Peachey Road', '48  Saverio Boulevard', '48  Uley Road', '48  Vincent Road', '48  Waratah Avenue', '48  West Parkway', '48B  Pix Road', '49  Ascot Avenue', '49  Emerald Circuit', '49  Fantasia Drive', '49  Highview Drive', '49  Pedlar Close', '49  Saverio Boulevard', '49  Vincent Road', '49  Waratah Avenue', '492  Robert Road', '4A  Davey Street', '4B  Davey Street', '5  Alessia Lane', '5  Alex Street', '5  Atlanta Street', '5  Barbon Lane', '5  Baron Road', '5  Bastow Road', '5  Bauera Place', '5  Belanger Court', '5  Botany Drive', '5  Bracken Avenue', '5  Broadwater Place', '5  Carabeen Crescent', '5  Charlie Street', '5  Collingbourne Drive', '5  Conmurra Court', '5  Cooper Place', '5  Coventry Road', '5  Crockerton Road', '5  De Luca Court', '5  Dulcis Circuit', '5  Eucalyptus Crescent', '5  Fleetwood Drive', '5  Forest Court', '5  Fortana Lane', '5  Fruin Close', '5  Geoff Road', '5  Geor</t>
+          <t xml:space="preserve">['1  Alessia Lane', '1  Anderson Walk', '1  Apsley Close', '1  Bauera Place', '1  Bayer Road', '1  Beaumont Road', '1  Birch Grove', '1  Blatchford Road', '1  Botany Drive', '1  Bracken Avenue', '1  Bright Court', '1  Brodie Circuit', '1  Burwood Road', '1  Catalonia Avenue', '1  Chang Place', '1  Charlie Street', '1  Clementine Avenue', '1  Crostan Close', '1  Cumbria Way', '1  Damien Street', '1  Dayman Street', '1  Deverill Street', '1  Edmund Avenue', '1  English Court', '1  Fergusson Bowl', '1  Fiore Way', '1  Fortana Lane', '1  Hanne Street', '1  Highview Drive', '1  Inwood Road', '1  Joseph Court', '1  Kendell Lane', '1  Kerrie Avenue', '1  Lorikeet Place', '1  Lucca Close', '1  Luis Drive', '1  Majella Way', '1  Mary Close', '1  Mira Road', '1  Olive Grove', '1  Olsen Way', '1  Oraton Court', '1  Ormsby Road', '1  Parkvale Drive', '1  Parkwood Lane', '1  Pinda Court', '1  Rhus Avenue', '1  Riverview Drive', '1  Roxburgh Crescent', '1  Stocklinch Crescent', '1  Sussex Court', '1  Varney Court', '1  Walpole Street', '1  Warburton Street', '1  Westbury Court', '1  Wolsten Drive', '1-3  Odgers Road', '1-5/ 2  Anderson Walk', '10  Alderwood Court', '10  Anderson Street', '10  Barfield Crescent', '10  Bracken Avenue', '10  Breamore Street', '10  Bridport Street', '10  Brookfield Street', '10  Brookmont Boulevard', '10  Calabria Court', '10  Caloria Street', '10  Carric Court', '10  Cartwright Drive', '10  Charlie Street', '10  Cooper Place', '10  Damien Street', '10  Darling Street', '10  Dauntless Crescent', '10  Drimpton Street', '10  Dulcis Circuit', '10  Edmund Avenue', '10  Epsom Street', '10  Eucalyptus Crescent', '10  Forest Court', '10  George Avenue', '10  Goulburn Street', '10  Greenhood Crescent', '10  Isabel Road', '10  Jenkins Road', '10  Karinga Crescent', '10  Kendell Lane', '10  Kerrie Avenue', '10  Keysley Street', '10  Lakes Entrance', '10  Lawder Road', '10  Liebrooke Boulevard', '10  Lily Court', '10  Lindgren Avenue', '10  Magnolia Crescent', '10  Mary Close', '10  McInerney Court', '10  McNamara Way', '10  Melbury Street', '10  Michael Road', '10  Murcia Avenue', '10  Myrta Avenue', '10  Myrtle Avenue', '10  Oakwood Circuit', '10  Parkvale Drive', '10  Peacemarsh Road', '10  Pendolino Road', '10  Philip Avenue', '10  Ranger Street', '10  Reel Terrace', '10  Rivitalo Avenue', '10  Samphire Avenue', '10  Scoular Road', '10  Sienna Road', '10  Springvale Drive', '10  Terry Street', '10  Tony Street', '10  Union Avenue', '10  Ward Street', '10  Wood Crescent', '10  Woodfalls Road', '100  Johnson Road', '100-106  Chellaston Road', '101  Park Terrace', '102  Keane Avenue', '1027  Stebonheath Road', '103  Halsey Road', '103  Juniper Boulevard', '103  Keane Avenue', '104  Johns Road', '104  Keane Avenue', '104  Precolumb Road', '105  Keane Avenue', '1064  Old Port Wakefield Road', '107  Beckham Rise', '107  Juniper Boulevard', '107  Keane Avenue', '107  Womma Road', '1072  Gawler-One Tree Hill Road', '108  Douglas Drive', '108  Keane Avenue', '108  McKenzie Road', '1080  Andrews Road', '109  Juniper Boulevard', '109  Keane Avenue', '1097  Stebonheath Road', '10A  Chardonnay Court', '10A  Perre Drive', '10B  Burke Circuit', '10B  Charlson Street', '11  Albero Street', '11  Alex Street', '11  Arbequina Road', '11  Argyle Walk', '11  Ashwin Street', '11  Bastow Road', '11  Bauera Place', '11  Begonia Drive', '11  Belanger Court', '11  Berwick Rise', '11  Bracken Avenue', '11  Brodie Circuit', '11  Brunswick Terrace', '11  Carman Close', '11  Chang Place', '11  Charlie Street', '11  Darling Street', '11  Dimasi Court', '11  Dulcis Circuit', '11  Eucalyptus Crescent', '11  Gold Street', '11  Grainger Road', '11  Grandview Drive', '11  Grove Avenue', '11  Gunther Street', '11  Hanorah Avenue', '11  Hewitt Road', '11  Jane Street', '11  Kendell Lane', '11  Lindgren Avenue', '11  Litchfield Avenue', '11  Luis Drive', '11  Manston Street', '11  McNamara Way', '11  Parkinson Street', '11  Parkvale Drive', '11  Pendolino Road', '11  Peridot Loop', '11  Philip Avenue', '11  Pioneer Way', '11  Prunus Court', '11  Reel Terrace', '11  Ridgeway Road', '11  Rivitalo Avenue', '11  Sam Circuit', '11  Shaftesbury Road', '11  Sussex Court', '11  Tony Street', '11  Waratah Avenue', '11  Wyong Crescent', '11  Yamuna Avenue', '110  Douglas Drive', '110  Keane Avenue', '110  Yorktown Road', '111  Flinders Road', '111  Johnson Road', '111  Keane Avenue', '111  Viney Drive', '112  Coventry Road', '112  Karwin Road', '112  Keane Avenue', '112  Tyeka Drive', '1122  Old Port Wakefield Road', '113  Gerald Boulevard', '113  Keane Avenue', '114-116  Heaslip Road', '115  Crittenden Road', '115  Keane Avenue', '115  Sampson Road', '1159  Stebonheath Road', '116  Gulf View Drive', '1161  Stebonheath Road', '1163  Stebonheath Road', '1165  Stebonheath Road', '1167  Stebonheath Road', '1169  Stebonheath Road', '117  Forrestall Road', '117  Philip Highway', '117-119  Heaslip Road', '1184  Stebonheath Road', '119  Keane Avenue', '119  Kelly Hill Road', '12  Apple Close', '12  Baker Court', '12  Beatrix Drive', '12  Bishopstone Road', '12  Black Top Road', '12  Bracken Avenue', '12  Bradpole Road', '12  Cameron Road', '12  Charleston Terrace', '12  Charlie Street', '12  Charlson Street', '12  Chivell Road', '12  Cleveland Road', '12  Cooper Place', '12  Coulter Street', '12  Damien Street', '12  Dana Street', '12  Dulcis Circuit', '12  Edward Avenue', '12  Elm Drive', '12  Epsom Street', '12  Esperance Drive', '12  Eucalyptus Crescent', '12  Federation Close', '12  Forest Court', '12  Fradd Road', '12  Fruin Close', '12  Greenhood Crescent', '12  Hanorah Avenue', '12  Hermitage Drive', '12  Hewittson Road', '12  Isabel Road', '12  Kathleen Crescent', '12  Kendell Lane', '12  Lawder Road', '12  Lindgren Avenue', '12  Luis Drive', '12  Mandel Street', '12  Martha Way', '12  Mary Close', '12  McNamara Way', '12  Murcia Avenue', '12  Myrta Avenue', '12  Myrtle Avenue', '12  Natasha Avenue', '12  Noble Road', '12  Norway Avenue', '12  Olsen Way', '12  Palmer Road', '12  Parkvale Drive', '12  Peacemarsh Road', '12  Pine Avenue', '12  Reel Terrace', '12  Rivitalo Avenue', '12  Sam Circuit', '12  Samphire Avenue', '12  Sasha Drive', '12  Sharrad Court', '12  Sturt Circuit', '12  Union Avenue', '12  Wolsten Drive', '120  Coventry Road', '1200  Andrews Road', '1201  Heaslip Road', '121  Keane Avenue', '121  Philip Highway', '121-129  Heaslip Road', '1219  Heaslip Road', '122  Crittenden Road', '123  Hogarth Road', '123  Keane Avenue', '123  McEvoy Road', '124  Douglas Drive', '125  Womma West Road', '127  Keane Avenue', '1278  Gawler-One Tree Hill Road', '129  Keane Avenue', '12A  Figsbury Street', '12B  Redwood Avenue', '13  Alex Street', '13  Bastow Road', '13  Bauera Place', '13  Blight Street', '13  Brodie Circuit', '13  Burnett Drive', '13  Calabria Court', '13  Chang Place', '13  Davalan Drive', '13  Eucalypt Circuit', '13  Eucalyptus Crescent', '13  Forest Court', '13  Geoff Road', '13  George Avenue', '13  Grant Street', '13  Hanorah Avenue', '13  Harris Road', '13  Horrie Knight Crescent', '13  John Circuit', '13  Kendell Lane', '13  Lawder Road', '13  Luis Drive', '13  McNamara Way', '13  McPherson Grove', '13  Myrta Avenue', '13  Natasha Avenue', '13  Oxford Terrace', '13  Parham Street', '13  Parkvale Drive', '13  Pedlar Close', '13  Prelude Circuit', '13  Prominent Rise', '13  Prosperity Way', '13  Ranger Street', '13  Reel Terrace', '13  Rivitalo Avenue', '13  Sam Circuit', '13  Stone Road', '13  Swan Crescent', '13  Waratah Avenue', '13  Whitford Road', '13  Wolsten Drive', '130  Haydown Road', '130  Willison Road', '1304  Angle Vale Road', '131  Keane Avenue', '133  Keane Avenue', '134  Tyeka Drive', '1347  Stebonheath Road', '1349  Stebonheath Road', '135  Keane Avenue', '136  McKenzie Road', '136  Penfield Road', '137  Angle Vale Road', '138  Supple Road', '138  Yorktown Road', '139  Kentish Road', '139  Lakeside Drive', '13A  Salerno Court', '13A  Webster Street', '14  Allington Street', '14  Boucaut Avenue', '14  Brandis Road', '14  Bridget Court', '14  Carmela Avenue', '14  Charleston Terrace', '14  Charlson Street', '14  Cleveland Road', '14  Clover Court', '14  Colombo Court', '14  Coonawarra Avenue', '14  Coorara Court', '14  Cruikshank Street', '14  Damien Street', '14  Dana Street', '14  Darling Street', '14  Dulcis Circuit', '14  Durrington Road', '14  Edmund Avenue', '14  Emerald Drive', '14  Eucalyptus Crescent', '14  Fradd Road', '14  Fruin Close', '14  George Avenue', '14  Green Court', '14  Greenhood Crescent', '14  Hanorah Avenue', '14  Hughes Court', '14  John Rice Avenue', '14  Jordon Street', '14  Kathleen Crescent', '14  Kendell Lane', '14  Knighton Road', '14  Lawder Road', '14  Lindgren Avenue', '14  Lomandra Crescent', '14  Luis Drive', '14  Mary Close', '14  McNamara Way', '14  Michael Road', '14  Murcia Avenue', '14  Myrta Avenue', '14  Myrtle Avenue', '14  Olsen Way', '14  Priority Court', '14  Prosperity Way', '14  Reel Terrace', '14  Rivitalo Avenue', '14  Sam Circuit', '14  Sissman Street', '14  Talbot Street', '14  Union Avenue', '14  Willys Street', '14  Wolsten Drive', '14  Yarnbrook Street', '14  Yorktown Road', '14-16  Heard Street', '140  Woodford Road', '141  Woodford Road', '143  Heaslip Road', '143  Lakeside Drive', '144  Halsey Road', '144  King Road', '147  Goodman Road', '149  Douglas Drive', '149  Frisby Road', '149  Tyeka Drive', '14B  Redwood Avenue', '15  Abelia Street', '15  Adams Road', '15  Alex Street', '15  Bailey Road', '15  Beckham Rise', '15  Brodie Circuit', '15  Bubner Street', '15  Carioca Drive', '15  Chang Place', '15  Coach House Mews', '15  Collins Street', '15  Crown Court', '15  Dulcis Circuit', '15  Edmund Avenue', '15  Epsom Street', '15  Eucalyptus Crescent', '15  Featherstone Street', '15  George Avenue', '15  Hermitage Drive', '15  Highview Drive', '15  Jenolan Crescent', '15  John Circuit', '15  Kernel Road', '15  Kingsbury Street', '15  Lafitte Way', '15  Lindgren Avenue', '15  Mary Close', '15  Myrta Avenue', '15  Natasha Avenue', '15  Nautilus Road', '15  Needlewood Court', '15  Parkvale Drive', '15  Peachey Road', '15  Portland Road', '15  Prominent Rise', '15  Reel Terrace', '15  Rivitalo Avenue', '15  Rosewood Avenue', '15  Samphire Avenue', '15  Shandon Drive', '15  Sissman Street', '15  Southan Street', '15  Spruance Road', '15  St Clair Avenue', '15  St Leonard Crescent', '15  Webster Street', '15  Yorktown Road', '151  Douglas Drive', '151  Julian Road', '152  Goulds Creek Road', '153  Angle Vale Road', '153  Carmelo Road', '154  Huxtable Road', '158  Penfield Road', '16  Alderwood Court', '16  Beatrix Drive', '16  Bentley Road', '16  Berkeley Way', '16  Breamore Street', '16  Burnlea Parade', '16  Caloria Street', '16  Cameron Road', '16  Charleston Terrace', '16  Coratina Road', '16  Damien Street', '16  Darling Street', '16  Dawn Close', '16  Dulcis Circuit', '16  Edward John Parade', '16  Elm Drive', '16  Emerald Drive', '16  Eucalyptus Crescent', '16  Figsbury Street', '16  Forest Court', '16  Fradd Road', '16  George Avenue', '16  Grandview Place', '16  Hawick Avenue', '16  Hayles Road', '16  Highgate Mews', '16  Honeysuckle Drive', '16  Illawarra Court', '16  Karinga Crescent', '16  Kendell Lane', '16  Lawder Road', '16  Lindgren Avenue', '16  Lorna Court', '16  Mary Close', '16  Michael Crescent', '16  Michael Road', '16  Murcia Avenue', '16  Myrta Avenue', '16  Myrtle Avenue', '16  Natasha Avenue', '16  Neagle Road', '16  Palari Crescent', '16  Pine Avenue', '16  Portland Road', '16  Ramsay Road', '16  Reel Terrace', '16  Rivitalo Avenue', '16  Sam Circuit', '16  Samphire Avenue', '16  Sharrad Court', '16  Sissman Street', '16  The Greenway', '16  Union Avenue', '16  Winkfield Street', '16  Wolsten Drive', '16  Wootton Street', '162  Philip Highway', '164  Harvey Road', '165  Ridley Road', '168  Julian Road', '168  Newton Boulevard', '16A  Redwood Avenue', '17  Alex Street', '17  Alexander Road', '17  Ballard Street', '17  Bastow Road', '17  Belanger Court', '17  Benham Street', '17  Birmingham Drive', '17  Bracken Avenue', '17  Brittlewood Drive', '17  Brodie Circuit', '17  Burley Griffin Drive', '17  Carey Street', '17  Charleston Terrace', '17  Charta Circuit', '17  Claret Avenue', '17  Cleveland Road', '17  Darling Street', '17  Drupe Street', '17  Dulcis Circuit', '17  Eucalyptus Crescent', '17  Featherstone Street', '17  Fradd Road', '17  Geoff Road', '17  George Avenue', '17  Harry Court', '17  Innes Street', '17  Kingsbury Street', '17  Lawder Road', '17  Lewis Drive', '17  Lindgren Avenue', '17  Longbridge Road', '17  Luis Drive', '17  Manya Crescent', '17  Mary Close', '17  McNamara Way', '17  Mosterton Road', '17  Myrta Avenue', '17  Olivia Court', '17  Olsen Way', '17  Palari Crescent', '17  Parkvale Drive', '17  Reel Terrace', '17  Rivitalo Avenue', '17  Rose Circuit', '17  Sam Circuit', '17  Samphire Avenue', '17  Scott Road', '17  Sissman Street', '17  St Leonard Crescent', '17  Stanley Street', '17  Tareena Street', '17  Tuggarah Street', '17  Varacalli Way', '17  Village Terrace', '17  Webster Street', '17  Wolsten Drive', '17  Wyong Crescent', '173  Woodford Road', '175  Williams Road', '17A  Everleigh Road', '18  Alawoona Road', '18  Applecross Drive', '18  Argent Street', '18  Bastow Road', '18  Bogan Road', '18  Bracken Avenue', '18  Bubner Road', '18  Burnlea Parade', '18  Cambridge Terrace', '18  Carob Crescent', '18  Cawrse Street', '18  Charleston Terrace', '18  Darling Street', '18  Dulcis Circuit', '18  Edmonds Road', '18  Edmund Avenue', '18  Emerald Drive', '18  Eucalyptus Crescent', '18  Fantasia Drive', '18  Finnis Street', '18  George Avenue', '18  Green Crescent', '18  Harvest Court', '18  John Circuit', '18  Jordan Drive', '18  Keevil Street', '18  Koongarra Crescent', '18  Lawder Road', '18  Lewis Drive', '18  Lindgren Avenue', '18  Lorna Court', '18  Luis Drive', '18  Myrtle Avenue', '18  Ontario Crescent', '18  Oregon Avenue', '18  Pendolino Road', '18  Pineridge Drive', '18  Preston Street', '18  Reel Terrace', '18  Rivitalo Avenue', '18  Sam Circuit', '18  Samphire Avenue', '18  Sampson Road', '18  Sissman Street', '18  Union Avenue', '18  Varacalli Way', '18  Warragal Court', '18  Winkfield Street', '18  Yarnbrook Street', '18-20  Charlotte Street', '18-22  Anderson Walk', '180  Philip Highway', '182  Humbug Scrub Road', '185  Hannaford Hump Road', '185  Philip Highway', '185  Yorktown Road', '186  Ryan Road', '187  Hannaford Hump Road', '189  Philip Highway', '18B  Gould Road', '18B  Redwood Avenue', '19  Alexander Road', '19  Banksia Crescent', '19  Bastow Road', '19  Bedchester Road', '19  Brodie Circuit', '19  Bundarra Court', '19  Carey Street', '19  Cleveland Road', '19  Cockshell Street', '19  Crisp Road', '19  Dawn Close', '19  Edmund Avenue', '19  Epsom Street', '19  Eucalyptus Crescent', '19  George Avenue', '19  Hambridge Road', '19  Harradine Court', '19  John Circuit', '19  Jordon Street', '19  Lakeside Drive', '19  Lawder Road', '19  Lewis Drive', '19  Lindgren Avenue', '19  Luis Drive', '19  Marleycombe Road', '19  Mary Close', '19  McNamara Way', '19  Myrta Avenue', '19  Parkvale Drive', '19  Reel Terrace', '19  Ridgeway Road', '19  Rivitalo Avenue', '19  Sam Circuit', '19  Samphire Avenue', '19  Scoular Road', '19  Secombe Street', '19  Sissman Street', '19  St Clair Avenue', '19  Sturt Circuit', '19  Toorak Drive', '19  Winklebury Road', '19  Wolsten Drive', '19  Wyong Crescent', '190  Taylors Road', '190  Williams Road', '194  Petherton Road', '195  Midway Road', '197  Curnow Road', '198  President Avenue', '19A  Bartlett Street', '19B  Butterfield Road', '1A  Lawder Road', '1B  Lawder Road', '2  Ballard Street', '2  Bastow Road', '2  Blackham Crescent', '2  Blatchford Road', '2  Blunden Court', '2  Burdett Street', '2  Burke Circuit', '2  Carric Court', '2  Castor Avenue', '2  Cooper Place', '2  Davey Street', '2  Fyfield Street', '2  Hanne Street', '2  Homington Road', '2  Howegate Lane', '2  Innes Street', '2  Kerrie Avenue', '2  Kerry Close', '2  MacFarlane Way', '2  Madison Street', '2  Martha Way', '2  McLean Street', '2  McNamara Way', '2  Michael Road', '2  Mission Court', '2  Morris Street', '2  Murcia Avenue', '2  Parker Road', '2  Parkvale Drive', '2  Peachey Road', '2  Prominent Rise', '2  Reel Terrace', '2  Sam Circuit', '2  Saverio Boulevard', '2  Smith Place', '2  Sturt Circuit', '2  Sussex Court', '2  Teofilo Street', '2  Valle Close', '2  Wills Court', '2  Yamuna Avenue', '2-4  Priority Court', '2/ 17  Bellchambers Road', '20  Ascot Avenue', '20  Ashfield Road', '20  Ashwin Street', '20  Balmoral Circuit', '20  Briar Road', '20  Bridport Street', '20  Brookmont Boulevard', '20  Burnlea Parade', '20  Cleveland Road', '20  Darling Street', '20  Emerald Drive', '20  Esperance Drive', '20  Eucalyptus Crescent', '20  Fradd Road', '20  Gladman Close', '20  Golfview Drive', '20  Highland Circuit', '20  Justinian Street', '20  Karrawirra Close', '20  Lawder Road', '20  Lindgren Avenue', '20  Lonsdale Crescent', '20  Luis Drive', '20  Magnolia Crescent', '20  Manningford Road', '20  McGilp Road', '20  McNamara Way', '20  Murcia Avenue', '20  Myrtle Avenue', '20  Natasha Avenue', '20  Olivia Court', '20  Priority Court', '20  Reel Terrace', '20  Rivitalo Avenue', '20  Rowe Street', '20  Sam Circuit', '20  Samphire Avenue', '20  Sampson Road', '20  Toorak Drive', '20  Tyalla Court', '20  Union Avenue', '20  Waratah Avenue', '20  Woodford Road', '200  Thompson Road', '201  Symes Road', '202  President Avenue', '203  Main North Road', '204  President Avenue', '206  Petherton Road', '206  President Avenue', '20A  Redwood Avenue', '20B  Redwood Avenue', '21  Baron Road', '21  Bracken Avenue', '21  Brodie Circuit', '21  Castle Court', '21  Cork Avenue', '21  Drupe Street', '21  Dulcis Circuit', '21  Edmund Avenue', '21  Elly Drive', '21  Eucalyptus Crescent', '21  Featherstone Street', '21  Fyfield Street', '21  George Avenue', '21  Grace Boulevard', '21  John Circuit', '21  Lewis Drive', '21  Lindgren Avenue', '21  Loftis Road', '21  Luis Drive', '21  Magnolia Crescent', '21  Maplewood Drive', '21  McNamara Way', '21  Mendota Avenue', '21  Parkvale Drive', '21  Peachey Road', '21  Rivitalo Avenue', '21  Rockbourne Street', '21  Sam Circuit', '21  Samphire Avenue', '21  Serenity Way', '21  Sissman Street', '21  Stanley Road', '21  Wanbi Court', '21  Waratah Avenue', '21  Webster Street', '21  Wolsten Drive', '21  Wyong Crescent', '210  Newton Boulevard', '210  President Avenue', '212  Newton Boulevard', '212  President Avenue', '213  Yorktown Road', '216-220  Adams Road', '22  Alawoona Road', '22  Angove Drive', '22  Ashwin Street', '22  Bagalowie Crescent', '22  Booyong Drive', '22  Broadacres Drive', '22  Burnlea Parade', '22  Cleveland Road', '22  Dowie Way', '22  Emerald Drive', '22  Esperance Drive', '22  Eucalyptus Crescent', '22  Fantasia Drive', '22  Fradd Road', '22  Geoff Road', '22  Greenhood Crescent', '22  Hambridge Road', '22  Jane Street', '22  Kilsby Street', '22  Langford Drive', '22  Lindgren Avenue', '22  Luis Drive', '22  Max Fatchen Drive', '22  McNamara Way', '22  Murcia Avenue', '22  Myrtle Avenue', '22  Natasha Avenue', '22  North Way', '22  Olinda Street', '22  Olsen Way', '22  Oxford Drive', '22  Patterson Road', '22  Priority Court', '22  Riverglen Court', '22  Rivitalo Avenue', '22  Rushall Crescent', '22  Sam Circuit', '22  Samphire Avenue', '22  Senna Avenue', '22  Southan Street', '22  Traminer Drive', '22  Union Avenue', '22  Varacalli Way', '22  Wahroonga Drive', '22  Wolsten Drive', '222  President Avenue', '22A  Redwood Avenue', '22B  Redwood Avenue', '23  Banksia Crescent', '23  Bartlett Street', '23  Bridport Street', '23  Brodie Circuit', '23  Burley Road', '23  Cambridge Terrace', '23  Catalonia Avenue', '23  Cavenagh Street', '23  Charleston Crescent', '23  Chicklade Street', '23  Cleveland Road', '23  Crosby Road', '23  Deptford Street', '23  Dulcis Circuit', '23  Edmund Avenue', '23  Eucalyptus Crescent', '23  Geoff Road', '23  George Avenue', '23  Green Crescent', '23  Hanorah Avenue', '23  Hanson Road', '23  Huon Road', '23  Jarvis Road', '23  John Circuit', '23  Lewis Drive', '23  Loftis Road', '23  Luis Drive', '23  Magor Street', '23  McNamara Way', '23  Parkvale Drive', '23  Rockbourne Street', '23  Sam Circuit', '23  Samphire Avenue', '23  Secombe Street', '23  Short Road', '23  Sissman Street', '23  Smitham Street', '23  Waratah Avenue', '23  Webster Street', '23  Wolsten Drive', '23  Wood Crescent', '23  Woodbridge Drive', '23  Wyong Crescent', '233  Curtis Road', '234  President Avenue', '238  Black Top Road', '238  Curtis Road', '24  Booyong Drive', '24  Broadwater Place', '24  Castleton Street', '24  Cleveland Road', '24  Emerald Drive', '24  Enterprise Circuit', '24  Esperance Drive', '24  Eucalyptus Crescent', '24  George Avenue', '24  Grandview Drive', '24  Hambridge Road', '24  John Circuit', '24  Kalamata Court', '24  Lewis Drive', '24  Luis Drive', '24  Max Fatchen Drive', '24  McNamara Way', '24  Murcia Avenue', '24  Myrtle Avenue', '24  Natasha Avenue', '24  Ontario Crescent', '24  Saint Germain Avenue', '24  Sam Circuit', '24  Senna Avenue', '24  Siddall Road', '24  Telowie Avenue', '24  The Avenue', '24  Traminer Drive', '24  Trinity Way', '24  Union Avenue', '24  Waratah Avenue', '24-30  Durrington Road', '240  Petherton Road', '244  Curtis Road', '245  Alexander Avenue', '247  Hogarth Road', '24A  Redwood Avenue', '24B  Redwood Avenue', '25  Bell Street', '25  Bellchambers Road', '25  Bressington Drive', '25  Cambridge Terrace', '25  Catalonia Avenue', '25  Chiselbury Road', '25  Clark Road', '25  Cleveland Road', '25  Dulcis Circuit', '25  Elizabeth Way', '25  Geoff Road', '25  George Avenue', '25  Horrie Knight Crescent', '25  John Circuit', '25  Kerrie Avenue', '25  Lancaster Court', '25  Lewis Drive', '25  McNamara Way', '25  Midlow Road', '25  Palmer Road', '25  Patterson Road', '25  Pedlar Close', '25  Sam Circuit', '25  Samphire Avenue', '25  Tudor Crescent', '25  Waratah Avenue', '25  Wood Crescent', '25  Wyong Crescent', '252  Midway Road', '255  Womma West Road', '258  Riggs Road', '259  Fradd East Road', '25A  Sissman Street', '25B  Sissman Street', '26  Alawoona Road', '26  Alexander Road', '26  Alexandrina Crescent', '26  Amberdale Road', '26  Burley Griffin Drive', '26  Carob Crescent', '26  Cavenagh Street', '26  Cleveland Road', '26  Edmonds Road', '26  Edmund Avenue', '26  Emerald Drive', '26  Esperance Drive', '26  Eucalyptus Crescent', '26  Flannery Crescent', '26  Hodgson Road', '26  John Circuit', '26  Justinian Street', '26  Kingsbury Street', '26  Liebrooke Boulevard', '26  Lorna Court', '26  McNamara Way', '26  Minchington Road', '26  Murcia Avenue', '26  Odgers Road', '26  Sam Circuit', '26  Senna Avenue', '26  Siddall Road', '26  St Georges Way', '26  Union Avenue', '260  Carclew Road', '261  Midway Road', '267  Riggs Road', '268  Midway Road', '26A  Redwood Avenue', '26B  Redwood Avenue', '26C  Redwood Avenue', '27  Booyong Drive', '27  Burnett Drive', '27  Catalonia Avenue', '27  Chellaston Road', '27  Dulcis Circuit', '27  George Avenue', '27  Ina Close', '27  John Circuit', '27  Jordan Drive', '27  Kentish Road', '27  Kernel Road', '27  Lewis Drive', '27  McNamara Way', '27  Parkvale Drive', '27  Sam Circuit', '27  Samphire Avenue', '27  Telowie Avenue', '27  Waratah Avenue', '27  Wyong Crescent', '270  Moloney Road', '272  Curtis Road', '28  Ballard Road', '28  Brittlewood Drive', '28  Burke Circuit', '28  Castleton Street', '28  Emerald Drive', '28  Esperance Drive', '28  Eucalyptus Crescent', '28  Greenhood Crescent', '28  Harvest Court', '28  Highview Drive', '28  John Circuit', '28  Laxton Road', '28  Levant Street', '28  Lewis Drive', '28  Luis Drive', '28  McNamara Way', '28  Oldham Road', '28  Penfold Road', '28  Sam Circuit', '28  Saverio Boulevard', '28  Senna Avenue', '28  Siddall Road', '28  Telowie Avenue', '28  Tollerdown Street', '28  Union Avenue', '28  Zurich Road', '281  Stebonheath Road', '283  Stebonheath Road', '286  Craigmore Road', '287  Carmelo Road', '287  Fradd East Road', '28B  Mavros Road', '29  Ashwin Street', '29  Baldina Crescent', '29  Birchdale Circuit', '29  Booyong Drive', '29  Brimsdown Road', '29  Carrama Crescent', '29  Catalonia Avenue', '29  Dowie Way', '29  Lewis Drive', '29  Librandi Street', '29  Luis Drive', '29  Max Fatchen Drive', '29  McNamara Way', '29  Old Sarum Road', '29  Oxford Court', '29  Parkvale Drive', '29  Sam Circuit', '29  Samphire Avenue', '29  Sissman Street', '29  Thyer Road', '29  Waratah Avenue', '29  Wyong Crescent', '3  Adams Road', '3  Alessia Lane', '3  Apsley Close', '3  Augusta Square', '3  Bastow Road', '3  Bauera Place', '3  Baxter Avenue', '3  Begonia Drive', '3  Blakeview Boulevard', '3  Brodie Circuit', '3  Calabria Court', '3  Catalonia Avenue', '3  Chang Place', '3  Charlie Street', '3  Cleveland Road', '3  Colombo Court', '3  Cooper Place', '3  Damien Street', '3  Darling Street', '3  Drupe Street', '3  Dulcis Circuit', '3  English Court', '3  Forde Street', '3  Fortana Lane', '3  Fruin Close', '3  George Avenue', '3  Glory Road', '3  Grand Road', '3  Hannah Road', '3  Hanorah Avenue', '3  John Circuit', '3  Kensington Mews', '3  Kerrie Avenue', '3  Lauren Lane', '3  Lindgren Avenue', '3  Longstaff Lane', '3  Lucca Close', '3  Luis Drive', '3  MacPharlin Court', '3  Majella Way', '3  Martha Way', '3  Mary Close', '3  Midlow Road', '3  Mira Road', '3  Myrta Avenue', '3  Natalia Road', '3  Olivia Court', '3  Ormsby Road', '3  Oxford Terrace', '3  Parkvale Drive', '3  Peridot Loop', '3  Philip Avenue', '3  Prosperity Way', '3  Reel Terrace', '3  Riverview Drive', '3  Rivitalo Avenue', '3  Russell Court', '3  Sam Circuit', '3  Seavington Road', '3  Sienna Road', '3  Silk Road', '3  Spratt Street', '3  Stocklinch Crescent', '3  Sturt Circuit', '3  Tea Tree Drive', '3  The Grove', '3  Tilshead Road', '3  Tony Street', '3  Torrens Street', '3  Trinity Way', '3  Virgara Court', '3  Warburton Street', '3  Willison Road', '3  Wolsten Drive', '3  Yamuna Avenue', '3/ 4  Fletcher Road', '30  Bain Road', '30  Benham Street', '30  Brittlewood Drive', '30  Clover Court', '30  Elly Drive', '30  Emerald Drive', '30  Esperance Drive', '30  Faulding Avenue', '30  Green Court', '30  Highview Drive', '30  John Circuit', '30  Kerrie Avenue', '30  Levant Street', '30  Lewis Drive', '30  Luis Drive', '30  Mavros Road', '30  McGilp Road', '30  McKenzie Road', '30  McNamara Way', '30  McPherson Grove', '30  Murcia Avenue', '30  Odgers Road', '30  Oldham Road', '30  Sam Circuit', '30  Senna Avenue', '30  Siddall Road', '30  Stockton Street', '30  Waratah Avenue', '30  William Drive', '306  Taylors Road', '31  Ashwin Street', '31  Ballard Road', '31  Chateau Avenue', '31  Collingbourne Drive', '31  Edmund Avenue', '31  Harris Road', '31  Haynes Street', '31  Huon Road', '31  John Circuit', '31  Kernel Road', '31  Luis Drive', '31  McNamara Way', '31  Paginton Crescent', '31  Parkvale Drive', '31  Pedlar Close', '31  Sam Circuit', '31  Samphire Avenue', '31  Southan Street', '31  Telowie Avenue', '31  Waratah Avenue', '31  Wyong Crescent', '31A  Kentish Road', '32  Brookmont Boulevard', '32  Castleton Street', '32  Chaddenwick Road', '32  Highview Drive', '32  John Circuit', '32  Loftis Road', '32  Luis Drive', '32  McNamara Way', '32  Murcia Avenue', '32  Odgers Road', '32  Sam Circuit', '32  Scoular Road', '32  Sheedy Road', '32  Uley Road', '32  Waratah Avenue', '321  Tozer Road', '323  Peachey Road', '329  Peachey Road', '329  Stebonheath Road', '33  Angle Vale Road', '33  Baldina Crescent', '33  Bellchambers Road', '33  Broadmeadows Road', '33  Catalonia Avenue', '33  Davey Street', '33  Edmund Avenue', '33  Hambridge Road', '33  Highview Drive', '33  Kerrie Avenue', '33  Mayfair Drive', '33  McKay Road', '33  McNamara Way', '33  Megunya Crescent', '33  Moloney Road', '33  Parkvale Drive', '33  Pix Road', '33  Scott Road', '33  Telowie Avenue', '33  Vincent Road', '33  Vokes Road', '33  Waratah Avenue', '33  Woodbridge Drive', '331  Peachey Road', '331  Stebonheath Road', '333  Peachey Road', '333  Stebonheath Road', '335  Stebonheath Road', '337  Stebonheath Road', '339  Peachey Road', '339  Stebonheath Road', '34  Ascot Avenue', '34  Burwood Road', '34  Emerald Circuit', '34  Fradd Road', '34  Green Court', '34  Heysen Court', '34  Highview Drive', '34  Hogarth Road', '34  John Circuit', '34  Luis Drive', '34  McNamara Way', '34  Plane Tree Drive', '34  Richardson Road', '34  Sam Circuit', '34  Scarlet Avenue', '34  Waratah Avenue', '34  Whitford Road', '341  Peachey Road', '341  Stebonheath Road', '343  Peachey Road', '343  Stebonheath Road', '345  Stebonheath Road', '347  Peachey Road', '347  Stebonheath Road', '34A  Ballard Road', '34B  Ballard Road', '34B  Hooper Road', '35  Andrews Road', '35  Bailey Road', '35  Catalonia Avenue', '35  Dover Place', '35  Edmund Avenue', '35  Elizabeth Way', '35  Homington Road', '35  Lewis Drive', '35  Linger Crescent', '35  Luis Drive', '35  Mayfair Drive', '35  Parkvale Drive', '35  Pedlar Close', '35  Seavington Road', '35  Stevens Drive', '35  Waratah Avenue', '35  Woodbridge Drive', '352  Alexander Avenue', '354  Fradd East Road', '355  Stebonheath Road', '357  Stebonheath Road', '359  Stebonheath Road', '35A  Pix Road', '36  Clementine Avenue', '36  Highview Drive', '36  John Circuit', '36  Jordan Drive', '36  Luis Drive', '36  McKay Road', '36  McNamara Way', '36  Moir Street', '36  Robert Road', '36  Sam Circuit', '36  Saverio Boulevard', '36  Waratah Avenue', '36  West Parkway', '36-40  John Rice Avenue', '361  Stebonheath Road', '363  Stebonheath Road', '36C  Halsey Road', '37  Bassnet Road', '37  Browne Circuit', '37  Catalonia Avenue', '37  Green Crescent', '37  Kerrie Avenue', '37  Lewis Drive', '37  Luis Drive', '37  McNamara Way', '37  Olive Grove', '37  Oxford Terrace', '37  Pedlar Close', '37  Rosewood Avenue', '37  Spruance Road', '37  Stevens Drive', '37  Vincent Road', '37  Waratah Avenue', '37  Yarnbrook Street', '37A  Kinkaid Road', '37A  Nautilus Road', '37B  Oxford Terrace', '38  Bagot Road', '38  Chellaston Road', '38  Greenhood Crescent', '38  Hanorah Avenue', '38  John Circuit', '38  Kakuna Crescent', '38  McNamara Way', '38  Sam Circuit', '38  Saverio Boulevard', '38  Waratah Avenue', '38  West Parkway', '38A  Hogarth Road', '39  Bellchambers Road', '39  Catalonia Avenue', '39  Chellaston Road', '39  Coratina Road', '39  Davoren Road', '39  Edmonds Road', '39  Edmund Avenue', '39  Fantasia Drive', '39  Gunther Street', '39  Hanorah Avenue', '39  Haydown Road', '39  Lewis Drive', '39  McNamara Way', '39  Pedlar Close', '39  Ramnet Circuit', '39  Waratah Avenue', '39  Yarnbury Road', '390  Alexander Avenue', '390  Fradd East Road', '394  Fradd East Road', '39A  Ballard Road', '39B  Ballard Road', '3A  Kilsby Street', '3A  Lawder Road', '3B  Lawder Road', '3B  Willison Road', '4  Angel Street', '4  Ash Place', '4  Ashwin Street', '4  Barossa Drive', '4  Begonia Drive', '4  Blatchford Road', '4  Botany Drive', '4  Brodie Circuit', '4  Burnett Drive', '4  Burra Street', '4  Cadillac Street', '4  Calabria Court', '4  Caloria Street', '4  Carric Court', '4  Castor Avenue', '4  Cathy Mews', '4  Charlie Street', '4  Charlson Street', '4  Charmouth Road', '4  Chellaston Road', '4  Chowilla Court', '4  Colins Court', '4  Damien Street', '4  De Luca Court', '4  Dulcis Circuit', '4  Dylan Close', '4  Emerald Drive', '4  English Court', '4  Eucalyptus Crescent', '4  Fiore Way', '4  Forest Court', '4  Fradd Court', '4  Fradd Road', '4  Fruin Close', '4  George Avenue', '4  Glory Road', '4  Goulburn Street', '4  Grovely Street', '4  Hamptworth Street', '4  Hanne Street', '4  Harris Road', '4  Highgrove Court', '4  Joseph Court', '4  Kathleen Crescent', '4  Kendell Lane', '4  Kerrie Avenue', '4  Kerry Close', '4  Kingsbury Street', '4  Lambrook Street', '4  Larkhill Road', '4  Levant Street', '4  Lewis Drive', '4  Librandi Street', '4  Lindgren Avenue', '4  Luis Drive', '4  Madison Street', '4  Mary Court', '4  Matthew Rise', '4  McNamara Way', '4  Michael Road', '4  Morris Street', '4  Myrtle Avenue', '4  Noble Road', '4  Oxford Drive', '4  Parkvale Drive', '4  Philip Avenue', '4  Pix Road', '4  Platten Avenue', '4  Playford Boulevard', '4  Prunus Court', '4  Ranger Street', '4  Reel Terrace', '4  Rivitalo Avenue', '4  Salway Street', '4  Saverio Boulevard', '4  Sissman Street', '4  Smith Place', '4  Stapleton Street', '4  Teakle Court', '4  Valle Close', '4  Vitana Court', '4  Vokes Road', '4  Waratah Avenue', '4  Warburton Street', '4  Whitehart Close', '4  Wills Court', '4  Windsor Court', '4  Yamuna </t>
         </is>
       </c>
     </row>
@@ -1479,7 +1479,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -1512,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P12" t="n">
         <v>0</v>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>MUNNO PARA DOWNS  SA  5115</t>
+          <t>EDINBURGH NORTH SA 5113</t>
         </is>
       </c>
       <c r="T12" t="n">
@@ -1539,20 +1539,20 @@
         </is>
       </c>
       <c r="V12" t="n">
-        <v>383</v>
+        <v>448</v>
       </c>
       <c r="W12" t="n">
         <v>0.289</v>
       </c>
       <c r="X12" t="n">
-        <v>53557</v>
+        <v>60056</v>
       </c>
       <c r="Y12" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>['ANDREWS FARM  SA  5114', 'ANDREWS FARM SA 5114', 'ANGLE VALE  SA', 'ANGLE VALE  SA  5117', 'ANGLE VALE SA 5117', 'BIBARINGA  SA  5118', 'BIBARINGA SA 5118', 'BLAKEVIEW  SA  5114', 'BLAKEVIEW SA 5114', 'BUCKLAND PARK  SA  5120', 'BUCKLAND PARK SA 5120', 'CRAIGMORE  SA  5114', 'CRAIGMORE SA 5114', 'DAVOREN PARK  SA  5113', 'DAVOREN PARK SA 5113', 'EDINBURGH NORTH  SA  5113', 'ELIZABETH  SA  5112', 'ELIZABETH DOWNS  SA', 'ELIZABETH DOWNS  SA  5113', 'ELIZABETH DOWNS SA 5113', 'ELIZABETH EAST  SA  5112', 'ELIZABETH GROVE  SA  5112', 'ELIZABETH NORTH  SA  5113', 'ELIZABETH NORTH SA 5113', 'ELIZABETH PARK  SA  5113', 'ELIZABETH PARK SA 5113', 'ELIZABETH SA 5112', 'ELIZABETH SOUTH  SA', 'ELIZABETH SOUTH  SA  5112', 'ELIZABETH SOUTH SA 5112', 'ELIZABETH VALE  SA  5112', 'ELIZABETH VALE SA 5112', 'EVANSTON PARK  SA  5116', 'EYRE  SA  5121', 'EYRE SA 5121', 'GOULD CREEK  SA  5114', 'HILLBANK  SA  5112', 'HILLBANK SA 5112', 'HILLIER  SA  5116', 'HUMBUG SCRUB  SA  5114', 'MACDONALD PARK  SA  5121', 'MACDONALD PARK SA 5121', 'MUNNO PARA  SA  5115', 'MUNNO PARA DOWNS  SA  5115', 'MUNNO PARA DOWNS SA 5115', 'MUNNO PARA SA 5115', 'MUNNO PARA WEST  SA  5115', 'MUNNO PARA WEST SA 5115', 'ONE TREE HILL  SA  5114', 'ONE TREE HILL SA 5114', 'PENFIELD  SA  5121', 'PENFIELD GARDENS  SA  5121', 'PENFIELD GARDENS SA 5121', 'PENFIELD SA 5121', 'SAMPSON FLAT  SA  5114', 'SAMPSON FLAT SA 5114', 'SMITHFIELD  SA  5114', 'SMITHFIELD PLAINS  SA  5114', 'SMITHFIELD PLAINS SA 5114', 'ULEYBURY  SA  5114', 'VIRGINIA  SA  5120', 'VIRGINIA SA 5120', 'WATERLOO CORNER  SA  5110', 'WATERLOO CORNER SA 5110', 'YATTALUNGA  SA  5114']</t>
+          <t>['ANDREWS FARM  SA  5114', 'ANDREWS FARM SA 5114', 'ANGLE VALE  SA', 'ANGLE VALE  SA  5117', 'ANGLE VALE SA 5117', 'BIBARINGA  SA  5118', 'BIBARINGA SA 5118', 'BLAKEVIEW  SA  5114', 'BLAKEVIEW SA 5114', 'BUCKLAND PARK  SA  5120', 'BUCKLAND PARK SA 5120', 'CRAIGMORE  SA  5114', 'CRAIGMORE SA 5114', 'DAVOREN PARK  SA  5113', 'DAVOREN PARK SA 5113', 'EDINBURGH NORTH  SA  5113', 'EDINBURGH NORTH SA 5113', 'ELIZABETH  SA  5112', 'ELIZABETH DOWNS  SA', 'ELIZABETH DOWNS  SA  5113', 'ELIZABETH DOWNS SA 5113', 'ELIZABETH EAST  SA  5112', 'ELIZABETH GROVE  SA  5112', 'ELIZABETH NORTH  SA  5113', 'ELIZABETH NORTH SA 5113', 'ELIZABETH PARK  SA  5113', 'ELIZABETH PARK SA 5113', 'ELIZABETH SA 5112', 'ELIZABETH SOUTH  SA', 'ELIZABETH SOUTH  SA  5112', 'ELIZABETH SOUTH SA 5112', 'ELIZABETH VALE  SA  5112', 'ELIZABETH VALE SA 5112', 'EVANSTON PARK  SA  5116', 'EYRE  SA  5121', 'EYRE SA 5121', 'GOULD CREEK  SA  5114', 'HILLBANK  SA  5112', 'HILLBANK SA 5112', 'HILLIER  SA  5116', 'HUMBUG SCRUB  SA  5114', 'HUMBUG SCRUB SA 5114', 'MACDONALD PARK  SA  5121', 'MACDONALD PARK SA 5121', 'MUNNO PARA  SA  5115', 'MUNNO PARA DOWNS  SA  5115', 'MUNNO PARA DOWNS SA 5115', 'MUNNO PARA SA 5115', 'MUNNO PARA WEST  SA  5115', 'MUNNO PARA WEST SA 5115', 'ONE TREE HILL  SA  5114', 'ONE TREE HILL SA 5114', 'PENFIELD  SA  5121', 'PENFIELD GARDENS  SA  5121', 'PENFIELD GARDENS SA 5121', 'PENFIELD SA 5121', 'SAMPSON FLAT  SA  5114', 'SAMPSON FLAT SA 5114', 'SMITHFIELD  SA  5114', 'SMITHFIELD PLAINS  SA  5114', 'SMITHFIELD PLAINS SA 5114', 'ULEYBURY  SA  5114', 'VIRGINIA  SA  5120', 'VIRGINIA SA 5120', 'WATERLOO CORNER  SA  5110', 'WATERLOO CORNER SA 5110', 'YATTALUNGA  SA  5114']</t>
         </is>
       </c>
     </row>
@@ -1571,7 +1571,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1604,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>2553</v>
+        <v>2862</v>
       </c>
       <c r="P13" t="n">
         <v>0</v>
@@ -1627,13 +1627,13 @@
       </c>
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="n">
-        <v>2553</v>
+        <v>2862</v>
       </c>
       <c r="W13" t="n">
         <v>0</v>
       </c>
       <c r="X13" t="n">
-        <v>584</v>
+        <v>612</v>
       </c>
       <c r="Y13" t="n">
         <v>4</v>
@@ -1659,7 +1659,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -1692,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>2553</v>
+        <v>2862</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
@@ -1715,13 +1715,13 @@
       </c>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="n">
-        <v>2553</v>
+        <v>2862</v>
       </c>
       <c r="W14" t="n">
         <v>0</v>
       </c>
       <c r="X14" t="n">
-        <v>584</v>
+        <v>612</v>
       </c>
       <c r="Y14" t="n">
         <v>4</v>
@@ -1747,7 +1747,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1780,7 +1780,7 @@
         <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>2553</v>
+        <v>2862</v>
       </c>
       <c r="P15" t="n">
         <v>0</v>
@@ -1803,13 +1803,13 @@
       </c>
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="n">
-        <v>2553</v>
+        <v>2862</v>
       </c>
       <c r="W15" t="n">
         <v>0</v>
       </c>
       <c r="X15" t="n">
-        <v>838</v>
+        <v>878</v>
       </c>
       <c r="Y15" t="n">
         <v>2</v>
@@ -1835,7 +1835,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1868,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>2553</v>
+        <v>2862</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
@@ -1891,13 +1891,13 @@
       </c>
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="n">
-        <v>2553</v>
+        <v>2862</v>
       </c>
       <c r="W16" t="n">
         <v>0</v>
       </c>
       <c r="X16" t="n">
-        <v>804</v>
+        <v>842</v>
       </c>
       <c r="Y16" t="n">
         <v>2</v>
@@ -1923,7 +1923,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1956,7 +1956,7 @@
         <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>2555</v>
+        <v>2864</v>
       </c>
       <c r="P17" t="n">
         <v>0</v>
@@ -1975,17 +1975,17 @@
         </is>
       </c>
       <c r="T17" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="U17" t="inlineStr"/>
       <c r="V17" t="n">
-        <v>2555</v>
+        <v>2864</v>
       </c>
       <c r="W17" t="n">
         <v>0</v>
       </c>
       <c r="X17" t="n">
-        <v>880</v>
+        <v>924</v>
       </c>
       <c r="Y17" t="n">
         <v>1</v>
@@ -2011,7 +2011,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -2059,7 +2059,7 @@
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>Development Application Refused</t>
+          <t>Under Construction Engineering</t>
         </is>
       </c>
       <c r="T18" t="n">
@@ -2071,20 +2071,20 @@
         </is>
       </c>
       <c r="V18" t="n">
-        <v>1309</v>
+        <v>1459</v>
       </c>
       <c r="W18" t="n">
         <v>1</v>
       </c>
       <c r="X18" t="n">
-        <v>71482</v>
+        <v>80324</v>
       </c>
       <c r="Y18" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>['Application Under Assessment', 'Approved', 'Cancelled', 'Development Application Approved', 'Development Application Refused', 'Development Application Withdrawn', 'Engineering Consent Granted', 'Incomplete Application Further Information Require', 'Lodged', 'Pending Additional Information Building', 'Pending Additional Information Planning', 'Pending Building Assessment', 'Pending Building Fire Safety Inspection', 'Pending Building Private Certifier Assessment', 'Pending CDAP Decision', 'Pending External Referral', 'Pending Further Information', 'Pending Internal Referral', 'Pending Planning Assessment', 'Planning Consent Granted', 'Public Consultation - Category 2', 'Public Consultation - Category 3', 'Referral of Calculations to Building Surveyor', 'Under Assessment Building', 'Under Assessment Planning', 'Under Construction Engineering', 'Variation Requested', 'Withdrawn', 'Work Commenced', 'Work Completed']</t>
+          <t>['Application Under Assessment', 'Approved', 'Cancelled', 'Development Application Approved', 'Development Application Refused', 'Development Application Withdrawn', 'Engineering Consent Granted', 'Incomplete Application Further Information Require', 'Lodged', 'Pending Additional Information Building', 'Pending Additional Information Planning', 'Pending Building Assessment', 'Pending Building Fire Safety Inspection', 'Pending Building Private Certifier Assessment', 'Pending External Referral', 'Pending Further Information', 'Pending Internal Referral', 'Pending Planning Assessment', 'Planning Consent Granted', 'Public Consultation - Category 2', 'Referral of Calculations to Building Surveyor', 'Under Assessment Building', 'Under Assessment Planning', 'Under Construction Engineering', 'Variation Requested', 'Withdrawn', 'Work Commenced', 'Work Completed']</t>
         </is>
       </c>
     </row>
@@ -2103,7 +2103,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -2136,7 +2136,7 @@
         <v>0</v>
       </c>
       <c r="O19" t="n">
-        <v>827</v>
+        <v>890</v>
       </c>
       <c r="P19" t="n">
         <v>0</v>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>26/11/2020 3:38:59 PM</t>
+          <t>23/12/2020 4:18:23 PM</t>
         </is>
       </c>
       <c r="T19" t="n">
@@ -2159,20 +2159,20 @@
       </c>
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="n">
-        <v>827</v>
+        <v>890</v>
       </c>
       <c r="W19" t="n">
         <v>0</v>
       </c>
       <c r="X19" t="n">
-        <v>37312</v>
+        <v>42537</v>
       </c>
       <c r="Y19" t="n">
-        <v>1717</v>
+        <v>1957</v>
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>['1/04/2020 10:56:58 AM', '1/04/2020 11:49:55 AM', '1/04/2020 1:55:40 PM', '1/04/2020 3:39:57 PM', '1/04/2020 9:41:47 AM', '1/05/2020 11:53:11 AM', '1/05/2020 12:52:38 PM', '1/05/2020 1:07:00 PM', '1/05/2020 1:55:58 PM', '1/05/2020 4:21:36 PM', '1/05/2020 5:31:51 PM', '1/06/2020 10:07:53 AM', '1/06/2020 10:21:10 AM', '1/06/2020 10:38:43 AM', '1/06/2020 11:35:14 AM', '1/06/2020 12:20:15 PM', '1/06/2020 12:39:25 PM', '1/06/2020 4:39:51 PM', '1/06/2020 9:29:50 AM', '1/06/2020 9:56:26 AM', '1/07/2020 10:08:53 AM', '1/07/2020 10:36:35 AM', '1/07/2020 10:40:39 AM', '1/07/2020 2:17:38 PM', '1/07/2020 2:51:36 PM', '1/07/2020 3:39:08 PM', '1/07/2020 3:40:38 PM', '1/07/2020 9:35:15 AM', '1/09/2020 10:31:47 AM', '1/09/2020 10:46:55 AM', '1/09/2020 11:08:06 AM', '1/09/2020 12:18:48 PM', '1/09/2020 1:19:10 PM', '1/09/2020 1:54:52 PM', '1/09/2020 2:09:57 PM', '1/09/2020 3:44:49 PM', '1/09/2020 4:17:39 PM', '1/09/2020 9:05:32 AM', '1/09/2020 9:29:18 AM', '1/10/2020 10:38:28 AM', '1/10/2020 10:51:28 AM', '1/10/2020 11:15:15 AM', '1/10/2020 11:43:34 AM', '1/10/2020 12:15:02 PM', '1/10/2020 12:23:10 PM', '1/10/2020 12:32:54 PM', '1/10/2020 1:21:07 PM', '1/10/2020 2:03:34 PM', '1/10/2020 3:45:02 PM', '1/10/2020 3:54:49 PM', '1/10/2020 4:45:18 PM', '1/10/2020 9:30:15 AM', '10/02/2020 12:35:03 PM', '10/02/2020 1:20:27 PM', '10/02/2020 2:29:16 PM', '10/02/2020 5:23:12 PM', '10/02/2020 9:15:15 AM', '10/02/2020 9:58:29 AM', '10/03/2020 10:41:01 AM', '10/03/2020 11:22:40 AM', '10/03/2020 2:25:02 PM', '10/03/2020 3:18:02 PM', '10/03/2020 3:36:51 PM', '10/03/2020 4:47:34 PM', '10/06/2020 10:32:38 AM', '10/06/2020 10:55:12 AM', '10/06/2020 12:06:03 PM', '10/06/2020 1:44:11 PM', '10/06/2020 2:14:09 PM', '10/06/2020 2:35:32 PM', '10/06/2020 2:51:53 PM', '10/06/2020 3:38:08 PM', '10/06/2020 3:53:16 PM', '10/06/2020 4:18:04 PM', '10/06/2020 9:25:13 AM', '10/06/2020 9:32:46 AM', '10/07/2020 11:59:23 AM', '10/07/2020 1:38:50 PM', '10/07/2020 4:32:12 PM', '10/07/2020 4:52:45 PM', '10/07/2020 9:23:48 AM', '10/07/2020 9:37:12 AM', '10/08/2020 10:26:48 AM', '10/08/2020 10:41:27 AM', '10/08/2020 11:11:22 AM', '10/08/2020 11:38:07 AM', '10/08/2020 1:52:59 PM', '10/08/2020 2:54:03 PM', '10/08/2020 3:18:34 PM', '10/08/2020 3:41:35 PM', '10/08/2020 4:29:32 PM', '10/08/2020 4:38:59 PM', '10/08/2020 5:14:51 PM', '10/09/2020 10:35:18 AM', '10/09/2020 11:24:12 AM', '10/09/2020 12:21:53 PM', '10/09/2020 3:25:16 PM', '10/09/2020 3:39:04 PM', '10/09/2020 3:43:13 PM', '10/09/2020 3:56:49 PM', '10/09/2020 9:36:29 AM', '10/09/2020 9:50:06 AM', '10/09/2020 9:59:43 AM', '10/11/2020 12:38:33 PM', '10/11/2020 2:47:02 PM', '10/11/2020 4:16:49 PM', '10/11/2020 4:20:10 PM', '10/11/2020 9:38:16 AM', '10/11/2020 9:55:50 AM', '11/02/2020 1:45:45 PM', '11/02/2020 3:58:22 PM', '11/03/2020 11:35:43 AM', '11/03/2020 11:56:26 AM', '11/03/2020 12:08:09 PM', '11/03/2020 12:45:27 PM', '11/03/2020 1:52:00 PM', '11/03/2020 2:01:09 PM', '11/03/2020 2:43:34 PM', '11/03/2020 4:53:10 PM', '11/03/2020 9:15:30 AM', '11/05/2020 11:04:46 AM', '11/05/2020 11:51:16 AM', '11/05/2020 12:43:50 PM', '11/05/2020 3:31:28 PM', '11/05/2020 3:47:29 PM', '11/05/2020 9:09:33 AM', '11/06/2020 10:39:04 AM', '11/06/2020 11:39:44 AM', '11/06/2020 11:42:01 AM', '11/06/2020 11:57:42 AM', '11/06/2020 12:11:56 PM', '11/06/2020 1:55:01 PM', '11/06/2020 3:04:08 PM', '11/06/2020 3:35:02 PM', '11/06/2020 3:51:00 PM', '11/06/2020 5:08:05 PM', '11/06/2020 9:28:31 AM', '11/06/2020 9:29:13 PM', '11/08/2020 10:08:29 AM', '11/08/2020 10:45:40 AM', '11/08/2020 11:01:23 AM', '11/08/2020 11:16:12 AM', '11/08/2020 3:45:35 PM', '11/08/2020 4:36:35 PM', '11/08/2020 8:56:12 AM', '11/08/2020 9:35:01 AM', '11/08/2020 9:53:16 AM', '11/09/2020 10:39:29 AM', '11/09/2020 3:11:32 PM', '11/09/2020 3:12:28 PM', '11/09/2020 3:54:14 PM', '11/09/2020 3:57:31 PM', '11/11/2020 10:35:33 AM', '11/11/2020 10:49:52 AM', '11/11/2020 11:10:10 AM', '11/11/2020 11:24:26 AM', '11/11/2020 12:05:16 PM', '11/11/2020 12:28:49 PM', '11/11/2020 12:55:18 PM', '11/11/2020 1:15:28 PM', '11/11/2020 2:24:13 PM', '11/11/2020 2:35:04 PM', '11/11/2020 2:35:58 PM', '11/11/2020 2:43:26 PM', '11/11/2020 3:06:24 PM', '11/11/2020 3:13:03 PM', '11/11/2020 3:53:48 PM', '11/11/2020 4:34:43 PM', '11/11/2020 4:42:19 PM', '12/02/2020 1:32:41 PM', '12/02/2020 1:55:28 PM', '12/02/2020 3:23:37 PM', '12/02/2020 3:48:10 PM', '12/02/2020 4:47:12 PM', '12/02/2020 9:41:36 AM', '12/03/2020 12:43:27 PM', '12/03/2020 2:29:42 PM', '12/03/2020 4:11:56 PM', '12/05/2020 10:22:54 AM', '12/05/2020 11:58:18 AM', '12/05/2020 12:32:50 PM', '12/05/2020 9:48:13 AM', '12/06/2020 10:49:12 AM', '12/06/2020 10:51:31 AM', '12/06/2020 11:30:25 AM', '12/06/2020 12:00:45 PM', '12/06/2020 12:42:18 PM', '12/06/2020 2:18:14 PM', '12/06/2020 3:28:57 PM', '12/06/2020 3:52:17 PM', '12/08/2020 10:12:51 AM', '12/08/2020 10:22:47 AM', '12/08/2020 10:45:08 AM', '12/08/2020 11:45:22 AM', '12/08/2020 1:08:28 PM', '12/08/2020 2:00:16 PM', '12/08/2020 2:22:44 PM', '12/08/2020 3:05:34 PM', '12/08/2020 3:15:21 PM', '12/08/2020 3:38:48 PM', '12/08/2020 9:27:12 AM', '12/08/2020 9:41:11 AM', '12/08/2020 9:57:47 AM', '12/10/2020 11:56:41 AM', '12/10/2020 12:17:00 PM', '12/10/2020 1:58:18 PM', '12/10/2020 3:02:27 PM', '12/10/2020 3:18:57 PM', '12/10/2020 3:36:03 PM', '12/10/2020 3:38:02 PM', '12/10/2020 4:17:50 PM', '12/11/2020 10:57:07 AM', '12/11/2020 1:22:46 PM', '12/11/2020 2:23:57 PM', '12/11/2020 2:34:55 PM', '12/11/2020 2:48:45 PM', '12/11/2020 3:18:17 PM', '12/11/2020 3:27:52 PM', '12/11/2020 3:42:46 PM', '12/11/2020 4:04:31 PM', '12/11/2020 4:16:49 PM', '12/11/2020 4:41:14 PM', '12/11/2020 9:48:30 AM', '13/02/2020 11:49:00 AM', '13/02/2020 11:49:45 AM', '13/02/2020 11:59:50 AM', '13/02/2020 12:01:09 PM', '13/02/2020 12:11:19 PM', '13/02/2020 12:25:18 PM', '13/02/2020 2:43:51 PM', '13/02/2020 3:36:21 PM', '13/03/2020 10:19:33 AM', '13/03/2020 11:00:05 AM', '13/03/2020 11:53:53 AM', '13/03/2020 1:44:33 PM', '13/03/2020 2:17:28 PM', '13/03/2020 3:03:59 PM', '13/03/2020 4:12:10 PM', '13/03/2020 4:32:44 PM', '13/03/2020 5:06:27 PM', '13/03/2020 5:28:15 PM', '13/05/2020 1:49:10 PM', '13/07/2020 10:26:06 AM', '13/07/2020 11:20:52 AM', '13/07/2020 11:43:46 AM', '13/07/2020 11:47:20 AM', '13/07/2020 12:21:56 PM', '13/07/2020 2:24:32 PM', '13/07/2020 2:56:37 PM', '13/07/2020 9:45:18 AM', '13/08/2020 10:57:16 AM', '13/08/2020 11:19:06 AM', '13/08/2020 11:33:42 AM', '13/08/2020 11:56:20 AM', '13/08/2020 1:38:15 PM', '13/08/2020 2:04:21 PM', '13/08/2020 3:15:07 PM', '13/08/2020 4:00:32 PM', '13/08/2020 4:15:09 PM', '13/08/2020 4:27:04 PM', '13/08/2020 9:16:50 AM', '13/08/2020 9:58:56 AM', '13/10/2020 11:55:13 AM', '13/10/2020 2:36:29 PM', '13/10/2020 2:50:52 PM', '13/10/2020 3:01:39 PM', '13/10/2020 3:07:36 PM', '13/10/2020 4:16:56 PM', '13/11/2020 11:10:01 AM', '13/11/2020 12:31:02 PM', '13/11/2020 12:41:59 PM', '13/11/2020 4:07:31 PM', '13/11/2020 9:54:51 AM', '14/01/2020 4:46:53 PM', '14/02/2020 10:03:09 AM', '14/02/2020 12:39:33 PM', '14/02/2020 1:22:07 PM', '14/02/2020 1:44:28 PM', '14/02/2020 2:18:57 PM', '14/02/2020 3:09:22 PM', '14/02/2020 4:31:40 PM', '14/02/2020 9:20:55 AM', '14/02/2020 9:43:40 AM', '14/04/2020 12:33:18 PM', '14/04/2020 2:16:25 PM', '14/04/2020 4:31:49 PM', '14/04/2020 5:33:47 PM', '14/05/2020 10:01:08 AM', '14/05/2020 11:55:06 AM', '14/05/2020 2:58:35 PM', '14/05/2020 4:12:20 PM', '14/05/2020 4:14:50 PM', '14/05/2020 4:55:17 PM', '14/05/2020 9:23:33 AM', '14/05/2020 9:45:20 AM', '14/07/2020 10:38:46 AM', '14/07/2020 11:51:34 AM', '14/07/2020 3:27:23 PM', '14/07/2020 4:14:18 PM', '14/07/2020 4:36:48 PM', '14/07/2020 9:38:17 AM', '14/07/2020 9:46:20 AM', '14/08/2020 10:04:03 AM', '14/08/2020 11:10:25 AM', '14/08/2020 11:57:11 AM', '14/08/2020 12:48:02 PM', '14/08/2020 1:41:13 PM', '14/08/2020 4:00:46 PM', '14/08/2020 4:10:09 PM', '14/08/2020 4:49:03 PM', '14/08/2020 9:21:31 AM', '14/09/2020 10:37:52 AM', '14/09/2020 11:19:54 AM', '14/09/2020 9:35:38 AM', '14/10/2020 10:07:40 AM', '14/10/2020 10:42:21 AM', '14/10/2020 11:16:57 AM', '14/10/2020 11:37:33 AM', '14/10/2020 12:39:04 PM', '14/10/2020 12:49:39 PM', '14/10/2020 1:21:50 PM', '14/10/2020 1:29:04 PM', '14/10/2020 2:43:18 PM', '14/10/2020 9:20:31 AM', '15/01/2020 4:21:56 PM', '15/01/2020 9:59:45 AM', '15/04/2020 1:30:32 PM', '15/04/2020 4:18:28 PM', '15/05/2020 10:44:44 AM', '15/05/2020 10:59:29 AM', '15/05/2020 12:18:09 PM', '15/05/2020 2:03:54 PM', '15/05/2020 2:51:44 PM', '15/05/2020 3:17:15 PM', '15/05/2020 9:48:09 AM', '15/06/2020 10:13:16 AM', '15/06/2020 10:33:40 AM', '15/06/2020 12:08:55 PM', '15/06/2020 12:14:05 PM', '15/06/2020 12:45:43 PM', '15/06/2020 1:12:50 PM', '15/06/2020 2:08:20 PM', '15/06/2020 3:34:32 PM', '15/06/2020 4:20:00 PM', '15/06/2020 4:50:16 PM', '15/06/2020 4:50:47 PM', '15/07/2020 10:19:19 AM', '15/07/2020 10:45:38 AM', '15/07/2020 11:27:54 AM', '15/07/2020 12:55:11 PM', '15/07/2020 1:15:28 PM', '15/07/2020 1:58:29 PM', '15/07/2020 2:28:19 PM', '15/07/2020 2:35:41 PM', '15/07/2020 4:13:12 PM', '15/07/2020 9:30:59 AM', '15/09/2020 1:37:12 PM', '15/09/2020 2:10:27 PM', '15/09/2020 2:58:04 PM', '15/09/2020 3:18:28 PM', '15/10/2020 11:51:52 AM', '15/10/2020 11:59:42 AM', '15/10/2020 1:11:28 PM', '15/10/2020 2:21:42 PM', '15/10/2020 2:41:21 PM', '15/10/2020 2:57:22 PM', '16/01/2020 12:15:44 PM', '16/03/2020 11:34:04 AM', '16/03/2020 12:19:46 PM', '16/03/2020 2:01:19 PM', '16/03/2020 2:12:02 PM', '16/03/2020 2:24:15 PM', '16/03/2020 3:23:06 PM', '16/03/2020 3:47:23 PM', '16/03/2020 4:03:59 PM', '16/03/2020 4:24:12 PM', '16/03/2020 4:24:45 PM', '16/03/2020 4:39:51 PM', '16/03/2020 9:43:46 AM', '16/04/2020 10:30:25 AM', '16/04/2020 11:16:56 AM', '16/04/2020 11:42:50 AM', '16/04/2020 12:00:00 AM', '16/04/2020 12:01:00 PM', '16/04/2020 12:59:09 PM', '16/04/2020 1:39:34 PM', '16/04/2020 3:13:26 PM', '16/04/2020 3:37:29 PM', '16/04/2020 4:01:14 PM', '16/04/2020 9:52:24 AM', '16/06/2020 10:20:22 AM', '16/06/2020 1:06:38 PM', '16/06/2020 1:16:41 PM', '16/06/2020 3:11:38 PM', '16/06/2020 3:57:16 PM', '16/06/2020 4:09:53 PM', '16/06/2020 4:35:32 PM', '16/06/2020 5:01:32 PM', '16/06/2020 9:22:05 AM', '16/06/2020 9:49:36 AM', '16/07/2020 2:12:51 PM', '16/07/2020 3:05:34 PM', '16/07/2020 3:10:17 PM', '16/07/2020 4:05:22 PM', '16/07/2020 4:23:14 PM', '16/07/2020 4:28:39 PM', '16/09/2020 10:54:56 AM', '16/09/2020 11:03:50 AM', '16/09/2020 12:37:04 PM', '16/09/2020 2:16:39 PM', '16/09/2020 2:41:12 PM', '16/09/2020 3:28:17 PM', '16/09/2020 3:36:31 PM', '16/09/2020 3:44:58 PM', '16/09/2020 3:56:53 PM', '16/09/2020 4:06:59 PM', '16/09/2020 4:37:18 PM', '16/10/2020 10:45:47 AM', '16/10/2020 10:47:05 AM', '16/10/2020 10:56:54 AM', '16/10/2020 11:40:25 AM', '16/10/2020 12:03:21 PM', '16/10/2020 2:06:32 PM', '16/10/2020 3:40:40 PM', '16/10/2020 4:04:00 PM', '16/10/2020 9:08:41 AM', '16/10/2020 9:52:50 AM', '16/11/2020 11:02:21 AM', '16/11/2020 11:03:41 AM', '16/11/2020 11:20:51 AM', '16/11/2020 11:25:44 AM', '16/11/2020 11:40:50 AM', '16/11/2020 11:40:57 AM', '16/11/2020 12:12:15 PM', '16/11/2020 12:30:16 PM', '16/11/2020 12:43:11 PM', '16/11/2020 1:07:01 PM', '16/11/2020 1:51:59 PM', '16/11/2020 2:10:52 PM', '16/11/2020 2:14:32 PM', '16/11/2020 2:49:59 PM', '16/11/2020 3:02:53 PM', '16/11/2020 3:28:38 PM', '16/11/2020 3:28:48 PM', '16/11/2020 4:18:02 PM', '16/11/2020 5:05:59 PM', '16/11/2020 9:51:55 AM', '17/01/2020 11:32:17 AM', '17/01/2020 9:05:24 AM', '17/02/2020 10:26:01 AM', '17/02/2020 10:54:56 AM', '17/02/2020 2:36:08 PM', '17/02/2020 3:43:43 PM', '17/02/2020 4:05:34 PM', '17/04/2020 10:42:33 AM', '17/04/2020 11:53:18 AM', '17/04/2020 12:31:41 PM', '17/04/2020 3:35:32 PM', '17/04/2020 4:02:59 PM', '17/04/2020 4:13:41 PM', '17/04/2020 4:22:46 PM', '17/04/2020 4:37:13 PM', '17/04/2020 9:30:52 AM', '17/04/2020 9:45:41 AM', '17/06/2020 10:18:03 AM', '17/06/2020 10:23:40 AM', '17/06/2020 10:32:06 AM', '17/06/2020 11:01:33 AM', '17/06/2020 11:26:09 AM', '17/06/2020 11:26:18 AM', '17/06/2020 11:28:29 AM', '17/06/2020 12:20:31 PM', '17/06/2020 12:35:03 PM', '17/06/2020 12:38:04 PM', '17/06/2020 1:15:20 PM', '17/06/2020 5:22:13 PM', '17/06/2020 9:27:11 AM', '17/06/2020 9:58:57 AM', '17/07/2020 11:48:46 AM', '17/07/2020 2:43:38 PM', '17/07/2020 3:13:46 PM', '17/07/2020 4:33:28 PM', '17/08/2020 10:03:48 AM', '17/08/2020 10:41:19 AM', '17/08/2020 11:30:46 AM', '17/08/2020 12:02:23 PM', '17/08/2020 12:34:03 PM', '17/08/2020 1:45:09 PM', '17/08/2020 1:55:54 PM', '17/08/2020 2:37:12 PM', '17/08/2020 3:12:14 PM', '17/08/2020 5:33:50 PM', '17/09/2020 10:22:48 AM', '17/09/2020 10:49:51 AM', '17/09/2020 4:20:53 PM', '17/09/2020 5:49:54 PM', '17/09/2020 8:54:19 AM', '17/11/2020 10:28:38 AM', '17/11/2020 11:26:04 AM', '17/11/2020 11:26:11 AM', '17/11/2020 11:53:51 AM', '17/11/2020 12:05:24 PM', '17/11/2020 12:12:08 PM', '17/11/2020 12:33:36 PM', '17/11/2020 12:44:25 PM', '17/11/2020 12:58:52 PM', '17/11/2020 1:50:12 PM', '17/11/2020 2:32:02 PM', '17/11/2020 2:52:27 PM', '17/11/2020 3:15:25 PM', '17/11/2020 4:12:04 PM', '17/11/2020 4:19:07 PM', '17/11/2020 9:56:59 AM', '18/02/2020 1:57:46 PM', '18/02/2020 2:57:57 PM', '18/02/2020 4:29:53 PM', '18/02/2020 9:44:14 AM', '18/03/2020 10:55:23 AM', '18/03/2020 9:18:02 AM', '18/03/2020 9:39:08 AM', '18/05/2020 10:09:24 AM', '18/05/2020 10:26:09 AM', '18/05/2020 10:40:15 AM', '18/05/2020 11:43:08 AM', '18/05/2020 2:07:37 PM', '18/05/2020 2:21:25 PM', '18/05/2020 2:44:20 PM', '18/05/2020 3:55:57 PM', '18/05/2020 9:48:51 AM', '18/06/2020 10:35:51 AM', '18/06/2020 11:04:17 AM', '18/06/2020 11:33:03 AM', '18/06/2020 11:36:31 AM', '18/06/2020 11:52:07 AM', '18/06/2020 12:15:24 PM', '18/06/2020 2:03:24 PM', '18/06/2020 2:47:11 PM', '18/06/2020 3:54:26 PM', '18/06/2020 4:39:17 PM', '18/06/2020 4:48:17 PM', '18/08/2020 10:38:58 AM', '18/08/2020 10:42:06 AM', '18/08/2020 10:58:32 AM', '18/08/2020 12:18:35 PM', '18/08/2020 1:07:22 PM', '18/08/2020 2:23:20 PM', '18/08/2020 4:53:35 PM', '18/08/2020 9:59:59 AM', '18/09/2020 10:45:33 AM', '18/09/2020 12:06:24 PM', '18/09/2020 2:17:54 PM', '18/09/2020 2:40:15 PM', '18/09/2020 3:48:01 PM', '18/09/2020 3:58:06 PM', '18/09/2020 4:28:24 PM', '18/09/2020 4:29:34 PM', '18/09/2020 4:42:02 PM', '18/09/2020 4:53:58 PM', '18/09/2020 5:03:31 PM', '18/09/2020 9:51:23 AM', '18/11/2020 10:24:07 AM', '18/11/2020 10:41:00 AM', '18/11/2020 11:11:19 AM', '18/11/2020 11:43:33 AM', '18/11/2020 11:45:13 AM', '18/11/2020 12:02:14 PM', '18/11/2020 2:03:39 PM', '18/11/2020 3:10:56 PM', '18/11/2020 3:18:47 PM', '18/11/2020 3:30:54 PM', '18/11/2020 4:42:53 PM', '18/11/2020 4:49:20 PM', '18/11/2020 9:21:22 AM', '19/02/2020 10:34:28 AM', '19/02/2020 12:10:00 PM', '19/02/2020 12:48:00 PM', '19/02/2020 3:34:54 PM', '19/02/2020 9:20:46 AM', '19/02/2020 9:52:12 AM', '19/03/2020 10:09:33 AM', '19/03/2020 10:55:28 AM', '19/03/2020 11:21:17 AM', '19/03/2020 11:25:38 AM', '19/03/2020 11:39:21 AM', '19/03/2020 12:13:17 PM', '19/03/2020 12:28:02 PM', '19/03/2020 1:22:20 PM', '19/03/2020 1:32:36 PM', '19/03/2020 2:40:39 PM', '19/03/2020 3:09:14 PM', '19/03/2020 3:10:12 PM', '19/03/2020 5:01:50 PM', '19/03/2020 9:24:44 AM', '19/05/2020 10:00:13 AM', '19/05/2020 10:22:22 AM', '19/05/2020 10:41:18 PM', '19/05/2020 12:49:25 PM', '19/05/2020 1:15:51 PM', '19/05/2020 2:45:55 PM', '19/05/2020 2:57:45 PM', '19/05/2020 3:37:28 PM', '19/05/2020 3:51:12 PM', '19/05/2020 4:05:32 PM', '19/05/2020 4:31:24 PM', '19/06/2020 10:04:30 AM', '19/06/2020 10:24:33 AM', '19/06/2020 11:16:13 AM', '19/06/2020 11:36:53 AM', '19/06/2020 1:34:14 PM', '19/06/2020 1:45:32 PM', '19/06/2020 2:30:46 PM', '19/06/2020 3:19:20 PM', '19/06/2020 3:43:18 PM', '19/06/2020 4:03:05 PM', '19/06/2020 9:35:59 AM', '19/08/2020 10:11:19 AM', '19/08/2020 10:51:48 AM', '19/08/2020 11:31:22 AM', '19/08/2020 12:27:06 PM', '19/08/2020 1:58:29 PM', '19/08/2020 4:11:58 PM', '19/08/2020 9:03:29 AM', '19/08/2020 9:37:40 AM', '19/08/2020 9:46:42 AM', '19/10/2020 10:03:31 AM', '19/10/2020 10:29:11 AM', '19/10/2020 10:37:53 AM', '19/10/2020 11:35:07 AM', '19/10/2020 11:56:03 AM', '19/10/2020 2:38:11 PM', '19/10/2020 2:51:01 PM', '19/10/2020 4:52:46 PM', '19/10/2020 5:04:25 PM', '19/11/2020 10:15:20 AM', '19/11/2020 12:52:05 PM', '19/11/2020 1:22:23 PM', '2/01/2020 3:07:29 PM', '2/03/2020 11:10:36 AM', '2/03/2020 11:24:21 AM', '2/03/2020 11:48:04 AM', '2/03/2020 11:58:50 AM', '2/03/2020 1:33:51 PM', '2/03/2020 4:10:08 PM', '2/03/2020 4:11:30 PM', '2/03/2020 5:24:35 PM', '2/03/2020 9:20:43 AM', '2/03/2020 9:29:51 AM', '2/03/2020 9:39:40 AM', '2/04/2020 11:09:47 AM', '2/04/2020 12:00:03 PM', '2/04/2020 12:15:50 PM', '2/04/2020 1:33:18 PM', '2/07/2020 11:06:36 AM', '2/07/2020 11:34:28 AM', '2/07/2020 11:52:50 AM', '2/07/2020 11:54:00 AM', '2/07/2020 12:10:05 PM', '2/07/2020 1:20:08 PM', '2/07/2020 2:33:34 PM', '2/07/2020 4:47:47 PM', '2/07/2020 4:55:09 PM', '2/07/2020 9:21:05 AM', '2/09/2020 10:11:42 AM', '2/09/2020 10:42:18 AM', '2/09/2020 11:00:54 AM', '2/09/2020 11:22:04 AM', '2/09/2020 11:23:03 AM', '2/09/2020 11:32:15 AM', '2/09/2020 12:01:30 PM', '2/09/2020 12:10:51 PM', '2/09/2020 12:16:09 PM', '2/09/2020 12:29:12 PM', '2/09/2020 12:44:11 PM', '2/09/2020 1:11:06 PM', '2/09/2020 1:28:02 PM', '2/09/2020 1:39:22 PM', '2/09/2020 2:11:00 PM', '2/09/2020 2:31:09 PM', '2/09/2020 2:51:57 PM', '2/09/2020 3:11:32 PM', '2/09/2020 3:56:17 PM', '2/09/2020 9:51:29 AM', '2/10/2020 10:05:44 AM', '2/10/2020 10:24:47 AM', '2/10/2020 11:44:26 AM', '2/10/2020 12:33:53 PM', '2/10/2020 12:44:04 PM', '2/10/2020 3:25:17 PM', '2/10/2020 9:13:00 AM', '2/10/2020 9:50:20 AM', '2/10/2020 9:56:16 AM', '2/11/2020 11:51:21 AM', '2/11/2020 2:06:08 PM', '2/11/2020 2:21:04 PM', '2/11/2020 2:49:28 PM', '2/11/2020 3:20:11 PM', '2/11/2020 3:43:29 PM', '2/11/2020 4:13:17 PM', '2/11/2020 4:52:36 PM', '20/01/2020 10:18:49 AM', '20/01/2020 9:58:30 AM', '20/02/2020 10:04:18 AM', '20/02/2020 10:20:49 AM', '20/02/2020 10:27:40 AM', '20/02/2020 10:48:45 AM', '20/02/2020 10:50:10 AM', '20/02/2020 11:02:22 AM', '20/02/2020 11:16:44 AM', '20/02/2020 11:18:16 AM', '20/02/2020 12:02:42 PM', '20/02/2020 12:31:49 PM', '20/02/2020 1:29:19 PM', '20/02/2020 2:14:04 PM', '20/02/2020 2:36:19 PM', '20/02/2020 9:18:34 AM', '20/02/2020 9:51:50 AM', '20/03/2020 10:07:01 AM', '20/03/2020 10:18:08 AM', '20/03/2020 11:26:41 AM', '20/03/2020 11:37:05 AM', '20/03/2020 1:23:15 PM', '20/03/2020 1:48:35 PM', '20/03/2020 2:09:57 PM', '20/03/2020 2:33:05 PM', '20/03/2020 3:01:01 PM', '20/03/2020 3:42:21 PM', '20/03/2020 4:42:56 PM', '20/03/2020 9:45:31 AM', '20/03/2020 9:53:26 AM', '20/04/2020 11:05:23 AM', '20/04/2020 12:00:00 AM', '20/04/2020 12:05:23 PM', '20/04/2020 12:24:43 PM', '20/04/2020 2:16:16 PM', '20/04/2020 2:38:03 PM', '20/04/2020 4:51:52 PM', '20/04/2020 5:17:27 PM', '20/05/2020 10:21:11 AM', '20/05/2020 1:10:41 PM', '20/05/2020 2:33:16 PM', '20/05/2020 3:53:02 PM', '20/05/2020 9:54:10 AM', '20/07/2020 10:19:18 AM', '20/07/2020 10:45:16 AM', '20/07/2020 11:54:58 AM', '20/07/2020 2:14:06 PM', '20/08/2020 10:13:56 AM', '20/08/2020 11:46:49 AM', '20/08/2020 2:24:16 PM', '20/08/2020 2:59:58 PM', '20/08/2020 4:38:02 PM', '20/08/2020 9:48:28 AM', '20/08/2020 9:51:09 AM', '20/10/2020 12:51:14 PM', '20/10/2020 2:05:03 PM', '20/10/2020 9:22:36 AM', '20/11/2020 12:21:15 PM', '21/01/2020 12:19:29 PM', '21/01/2020 9:20:36 AM', '21/02/2020 10:59:53 AM', '21/02/2020 11:38:04 AM', '21/02/2020 11:59:06 AM', '21/02/2020 12:23:45 PM', '21/02/2020 12:45:57 PM', '21/02/2020 3:14:24 PM', '21/02/2020 3:25:06 PM', '21/02/2020 4:18:02 PM', '21/02/2020 4:31:11 PM', '21/02/2020 9:23:34 AM', '21/04/2020 10:06:36 AM', '21/04/2020 10:13:16 AM', '21/04/2020 12:56:28 PM', '21/04/2020 2:40:17 PM', '21/04/2020 3:49:53 PM', '21/04/2020 8:34:53 AM', '21/05/2020 10:15:55 AM', '21/05/2020 11:49:33 AM', '21/05/2020 12:31:16 PM', '21/05/2020 1:44:23 PM', '21/05/2020 1:53:20 PM', '21/05/2020 3:47:33 PM', '21/05/2020 3:55:31 PM', '21/05/2020 9:50:23 AM', '21/05/2020 9:59:45 AM', '21/07/2020 10:11:41 AM', '21/07/2020 3:52:01 PM', '21/07/2020 4:05:55 PM', '21/07/2020 4:46:59 PM', '21/08/2020 10:12:10 AM', '21/08/2020 10:42:34 AM', '21/08/2020 12:05:18 PM', '21/08/2020 12:16:55 PM', '21/08/2020 1:46:38 PM', '21/08/2020 3:12:18 PM', '21/08/2020 4:27:59 PM', '21/08/2020 4:52:11 PM', '21/09/2020 10:18:40 AM', '21/09/2020 11:05:40 AM', '21/09/2020 11:14:37 AM', '21/09/2020 11:22:16 AM', '21/09/2020 11:53:23 AM', '21/09/2020 12:00:06 PM', '21/09/2020 12:10:46 PM', '21/09/2020 12:42:51 PM', '21/09/2020 3:11:27 PM', '21/09/2020 3:34:12 PM', '21/09/2020 3:58:38 PM', '21/09/2020 4:03:08 PM', '21/09/2020 4:48:05 PM', '21/09/2020 9:07:02 AM', '21/09/2020 9:57:29 AM', '21/10/2020 11:12:24 AM', '21/10/2020 12:35:13 PM', '21/10/2020 12:45:52 PM', '21/10/2020 1:22:57 PM', '21/10/2020 2:08:00 PM', '21/10/2020 2:12:40 PM', '21/10/2020 2:51:08 PM', '21/10/2020 2:54:49 PM', '21/10/2020 3:04:40 PM', '21/10/2020 3:35:33 PM', '21/10/2020 3:59:03 PM', '21/10/2020 4:02:56 PM', '21/10/2020 4:36:06 PM', '22/04/2020 1:20:13 PM', '22/04/2020 1:55:52 PM', '22/04/2020 3:41:52 PM', '22/04/2020 4:10:06 PM', '22/05/2020 10:06:56 AM', '22/05/2020 10:32:13 AM', '22/05/2020 4:01:50 PM', '22/05/2020 4:11:59 PM', '22/05/2020 4:20:30 PM', '22/05/2020 5:45:02 PM', '22/06/2020 10:14:25 AM', '22/06/2020 10:36:19 AM', '22/06/2020 9:23:59 AM', '22/07/2020 10:51:44 AM', '22/07/2020 2:13:54 PM', '22/07/2020 2:26:32 PM', '22/07/2020 2:59:38 PM', '22/07/2020 3:15:32 PM', '22/07/2020 3:49:32 PM', '22/07/2020 9:19:36 AM', '22/07/2020 9:52:59 AM', '22/09/2020 12:11:44 PM', '22/09/2020 5:20:50 PM', '22/10/2020 12:48:48 PM', '22/10/2020 1:02:35 PM', '22/10/2020 1:11:41 PM', '22/10/2020 1:51:20 PM', '22/10/2020 2:02:27 PM', '22/10/2020 4:00:05 PM', '22/10/2020 4:23:01 PM', '23/01/2020 11:21:59 AM', '23/01/2020 4:40:44 PM', '23/03/2020 10:17:49 AM', '23/03/2020 10:20:30 AM', '23/03/2020 10:34:32 AM', '23/03/2020 12:45:17 PM', '23/03/2020 1:11:23 PM', '23/03/2020 3:29:52 PM', '23/03/2020 9:30:39 AM', '23/03/2020 9:57:29 AM', '23/04/2020 11:24:21 AM', '23/04/2020 1:28:03 PM', '23/06/2020 10:10:22 AM', '23/06/2020 11:03:27 AM', '23/06/2020 11:47:29 AM', '23/06/2020 3:19:49 PM', '23/06/2020 3:21:40 PM', '23/06/2020 4:05:21 PM', '23/06/2020 4:54:50 PM', '23/06/2020 9:56:26 AM', '23/07/2020 10:18:16 AM', '23/07/2020 1:57:12 PM', '23/07/2020 2:01:40 PM', '23/07/2020 2:49:21 PM', '23/07/2020 3:24:09 PM', '23/07/2020 3:36:36 PM', '23/07/2020 4:32:09 PM', '23/09/2020 10:07:26 AM', '23/09/2020 10:09:19 AM', '23/09/2020 10:15:26 AM', '23/09/2020 10:33:31 AM', '23/09/2020 11:22:22 AM', '23/09/2020 12:33:39 PM', '23/09/2020 12:45:05 PM', '23/09/2020 12:58:15 PM', '23/09/2020 2:00:54 PM', '23/09/2020 2:09:49 PM', '23/09/2020 2:14:27 PM', '23/09/2020 2:24:59 PM', '23/09/2020 3:13:55 PM', '23/09/2020 3:25:49 PM', '23/09/2020 3:52:16 PM', '23/09/2020 4:24:39 PM', '23/09/2020 9:19:42 AM', '23/10/2020 12:08:16 PM', '23/10/2020 12:30:20 PM', '23/10/2020 12:58:13 PM', '23/10/2020 1:08:29 PM', '23/10/2020 1:20:08 PM', '23/10/2020 1:36:09 PM', '23/10/2020 1:59:49 PM', '23/10/2020 2:30:14 PM', '23/10/2020 3:25:48 PM', '23/10/2020 3:51:39 PM', '23/10/2020 3:59:05 PM', '23/10/2020 4:04:49 PM', '23/10/2020 9:20:36 AM', '23/10/2020 9:56:35 AM', '23/11/2020 10:44:26 AM', '23/11/2020 11:14:48 AM', '23/11/2020 11:17:26 AM', '23/11/2020 12:02:25 PM', '23/11/2020 12:02:42 PM', '23/11/2020 12:31:13 PM', '23/11/2020 12:35:37 PM', '23/11/2020 12:56:55 PM', '23/11/2020 1:10:21 PM', '23/11/2020 1:58:58 PM', '23/11/2020 2:19:48 PM', '23/11/2020 3:03:47 PM', '23/11/2020 3:13:20 PM', '23/11/2020 3:23:57 PM', '23/11/2020 3:53:52 PM', '23/11/2020 4:40:05 PM', '23/11/2020 9:43:23 AM', '24/01/2020 10:44:54 AM', '24/01/2020 3:00:48 PM', '24/02/2020 10:15:58 AM', '24/02/2020 10:30:24 AM', '24/02/2020 11:14:45 AM', '24/02/2020 12:44:12 PM', '24/03/2020 3:54:32 PM', '24/03/2020 9:10:17 AM', '24/03/2020 9:33:58 AM', '24/04/2020 4:02:28 PM', '24/06/2020 10:07:24 AM', '24/06/2020 11:15:13 AM', '24/06/2020 11:19:07 AM', '24/06/2020 12:35:33 PM', '24/06/2020 1:08:55 PM', '24/06/2020 1:55:48 PM', '24/06/2020 2:28:01 PM', '24/06/2020 3:05:44 PM', '24/06/2020 3:09:47 PM', '24/06/2020 3:59:29 PM', '24/06/2020 4:05:23 PM', '24/06/2020 4:26:51 PM', '24/06/2020 4:34:55 PM', '24/06/2020 4:45:04 PM', '24/06/2020 9:35:46 AM', '24/06/2020 9:46:54 AM', '24/06/2020 9:48:35 AM', '24/07/2020 1:22:02 PM', '24/07/2020 1:44:33 PM', '24/07/2020 2:25:04 PM', '24/07/2020 3:04:03 PM', '24/07/2020 4:10:14 PM', '24/07/2020 9:05:06 AM', '24/08/2020 11:16:53 AM', '24/08/2020 12:07:05 PM', '24/08/2020 2:40:07 PM', '24/08/2020 2:46:24 PM', '24/08/2020 3:56:27 PM', '24/08/2020 4:22:06 PM', '24/08/2020 4:42:56 PM', '24/09/2020 10:21:57 AM', '24/09/2020 10:55:15 AM', '24/09/2020 11:37:34 AM', '24/09/2020 12:58:01 PM', '24/09/2020 1:23:37 PM', '24/09/2020 2:19:36 PM', '24/09/2020 2:42:11 PM', '24/09/2020 5:04:52 PM', '24/09/2020 9:27:10 AM', '24/09/2020 9:41:00 AM', '24/11/2020 10:14:05 AM', '24/11/2020 10:42:13 AM', '24/11/2020 11:00:50 AM', '24/11/2020 11:36:00 AM', '24/11/2020 11:47:58 AM', '24/11/2020 12:17:30 PM', '24/11/2020 2:41:02 PM', '24/11/2020 3:03:18 PM', '24/11/2020 4:02:58 PM', '24/11/2020 4:49:38 PM', '25/02/2020 12:55:26 PM', '25/02/2020 2:07:57 PM', '25/02/2020 9:32:36 AM', '25/03/2020 10:33:20 AM', '25/03/2020 3:22:58 PM', '25/03/2020 3:46:43 PM', '25/05/2020 2:51:08 PM', '25/05/2020 3:22:38 PM', '25/05/2020 8:53:47 AM', '25/05/2020 9:14:15 AM', '25/05/2020 9:47:46 AM', '25/06/2020 10:18:45 AM', '25/06/2020 10:34:03 AM', '25/06/2020 11:51:39 AM', '25/06/2020 12:52:05 PM', '25/06/2020 12:53:27 PM', '25/06/2020 2:06:06 PM', '25/06/2020 4:12:15 PM', '25/06/2020 4:53:13 PM', '25/06/2020 9:58:27 AM', '25/08/2020 11:41:37 AM', '25/08/2020 1:52:17 PM', '25/08/2020 3:15:22 PM', '25/08/2020 4:12:20 PM', '25/08/2020 4:29:14 PM', '25/08/2020 4:53:26 PM', '25/08/2020 5:17:51 PM', '25/08/2020 9:04:21 AM', '25/08/2020 9:32:42 AM', '25/09/2020 9:30:00 AM', '25/11/2020 10:16:51 AM', '25/11/2020 12:19:20 PM', '25/11/2020 12:50:20 PM', '25/11/2020 1:54:20 PM', '25/11/2020 3:13:47 PM', '25/11/2020 4:13:20 PM', '25/11/2020 9:30:34 AM', '26/02/2020 10:58:33 AM', '26/02/2020 9:22:51 AM', '26/03/2020 10:44:51 AM', '26/03/2020 10:58:14 AM', '26/03/2020 12:18:32 PM', '26/03/2020 1:29:39 PM', '26/03/2020 2:23:42 PM', '26/03/2020 3:01:10 PM', '26/03/2020 3:52:45 PM', '26/03/2020 4:45:35 PM', '26/03/2020 4:55:50 PM', '26/03/2020 9:14:03 AM', '26/03/2020 9:52:45 AM', '26/05/2020 10:58:56 AM', '26/05/2020 11:19:16 AM', '26/05/2020 1:19:11 PM', '26/05/2020 3:44:09 PM', '26/05/2020 8:55:15 AM', '26/05/2020 9:40:58 AM', '26/06/2020 11:13:21 AM', '26/06/2020 11:37:13 AM', '26/06/2020 12:53:20 PM', '26/06/2020 3:01:17 PM', '26/06/2020 3:12:16 PM', '26/06/2020 4:30:13 PM', '26/06/2020 4:40:50 PM', '26/06/2020 5:48:42 PM', '26/06/2020 9:29:02 AM', '26/06/2020 9:43:45 AM', '26/08/2020 10:12:17 AM', '26/08/2020 10:51:26 AM', '26/08/2020 11:21:05 AM', '26/08/2020 11:35:43 AM', '26/08/2020 11:43:28 AM', '26/08/2020 12:17:29 PM', '26/08/2020 12:43:34 PM', '26/08/2020 12:47:59 PM', '26/08/2020 1:48:05 PM', '26/08/2020 2:23:14 PM', '26/08/2020 3:42:48 PM', '26/08/2020 4:11:41 PM', '26/08/2020 4:42:23 PM', '26/08/2020 9:13:18 AM', '26/10/2020 11:11:28 AM', '26/10/2020 11:24:18 AM', '26/10/2020 12:01:59 PM', '26/10/2020 2:48:36 PM', '26/10/2020 3:18:22 PM', '26/10/2020 3:43:43 PM', '26/10/2020 4:36:42 PM', '26/11/2020 11:29:21 AM', '26/11/2020 12:03:54 PM', '26/11/2020 1:20:27 PM', '26/11/2020 3:38:59 PM', '27/02/2020 10:39:07 AM', '27/02/2020 10:58:09 AM', '27/02/2020 11:08:32 AM', '27/02/2020 11:53:04 AM', '27/02/2020 12:36:22 PM', '27/02/2020 3:23:36 PM', '27/02/2020 4:39:35 PM', '27/03/2020 9:34:01 AM', '27/04/2020 12:10:56 PM', '27/04/2020 2:25:31 PM', '27/04/2020 2:57:07 PM', '27/04/2020 3:19:29 PM', '27/04/2020 3:38:49 PM', '27/04/2020 4:33:47 PM', '27/04/2020 4:58:31 PM', '27/04/2020 9:24:07 AM', '27/04/2020 9:44:05 AM', '27/05/2020 11:01:10 AM', '27/05/2020 11:26:19 AM', '27/05/2020 11:29:56 AM', '27/05/2020 12:15:09 PM', '27/05/2020 9:33:37 AM', '27/05/2020 9:43:54 AM', '27/05/2020 9:52:44 AM', '27/07/2020 10:51:38 AM', '27/07/2020 12:44:33 PM', '27/07/2020 1:39:07 PM', '27/07/2020 4:04:59 PM', '27/07/2020 5:01:10 PM', '27/08/2020 10:35:56 AM', '27/08/2020 11:04:47 AM', '27/08/2020 11:49:07 AM', '27/08/2020 1:19:58 PM', '27/08/2020 1:49:23 PM', '27/08/2020 1:57:12 PM', '27/08/2020 2:36:21 PM', '27/08/2020 3:24:35 PM', '27/08/2020 3:30:36 PM', '27/08/2020 3:47:23 PM', '27/08/2020 9:48:28 AM', '27/10/2020 10:23:37 AM', '27/10/2020 10:37:33 AM', '27/10/2020 11:48:44 AM', '27/10/2020 2:43:36 PM', '27/10/2020 4:16:35 PM', '27/10/2020 4:31:01 PM', '27/10/2020 4:39:55 PM', '27/10/2020 9:38:47 AM', '27/10/2020 9:57:32 AM', '28/01/2020 3:32:55 PM', '28/01/2020 4:41:53 PM', '28/01/2020 9:18:11 AM', '28/01/2020 9:40:07 AM', '28/02/2020 10:13:36 AM', '28/02/2020 12:49:04 PM', '28/02/2020 1:09:09 PM', '28/02/2020 2:50:45 PM', '28/02/2020 3:39:39 PM', '28/02/2020 4:02:35 PM', '28/04/2020 11:32:04 AM', '28/04/2020 12:52:58 PM', '28/04/2020 4:15:15 PM', '28/04/2020 9:12:58 AM', '28/05/2020 10:10:23 AM', '28/05/2020 10:33:39 AM', '28/05/2020 11:12:17 AM', '28/05/2020 12:49:40 PM', '28/05/2020 2:11:23 PM', '28/05/2020 2:40:58 PM', '28/05/2020 3:35:21 PM', '28/05/2020 3:35:51 PM', '28/05/2020 3:42:43 PM', '28/05/2020 4:13:28 PM', '28/05/2020 4:15:36 PM', '28/05/2020 4:26:33 PM', '28/05/2020 9:41:15 AM', '28/06/2020 8:43:22 PM', '28/07/2020 11:16:05 AM', '28/07/2020 11:35:47 AM', '28/07/2020 12:16:07 PM', '28/07/2020 12:25:57 PM', '28/07/2020 12:36:23 PM', '28/07/2020 12:51:07 PM', '28/07/2020 2:09:21 PM', '28/07/2020 3:04:39 PM', '28/07/2020 3:06:18 PM', '28/08/2020 11:47:56 AM', '28/08/2020 1:32:58 PM', '28/08/2020 1:42:47 PM', '28/08/2020 1:53:26 PM', '28/08/2020 4:05:04 PM', '28/08/2020 4:21:56 PM', '28/08/2020 9:17:50 AM', '28/09/2020 10:05:55 AM', '28/09/2020 11:24:39 AM', '28/09/2020 11:35:47 AM', '28/09/2020 11:56:57 AM', '28/09/2020 11:59:52 AM', '28/09/2020 1:23:33 PM', '28/09/2020 2:21:10 PM', '28/09/2020 2:34:20 PM', '28/09/2020 3:01:49 PM', '28/09/2020 3:16:33 PM', '28/09/2020 3:26:43 PM', '28/09/2020 3:34:09 PM', '28/09/2020 3:47:23 PM', '28/09/2020 4:14:48 PM', '28/09/2020 5:23:49 PM', '28/09/2020 9:52:58 AM', '28/10/2020 10:18:38 AM', '28/10/2020 11:17:46 AM', '28/10/2020 11:44:28 AM', '28/10/2020 11:50:01 AM', '28/10/2020 11:51:49 AM', '28/10/2020 12:11:24 PM', '28/10/2020 12:11:33 PM', '28/10/2020 12:34:53 PM', '28/10/2020 12:35:10 PM', '28/10/2020 1:56:42 PM', '28/10/2020 2:19:44 PM', '28/10/2020 2:20:52 PM', '28/10/2020 2:21:44 PM', '28/10/2020 2:34:47 PM', '28/10/2020 4:46:02 PM', '28/10/2020 9:22:26 AM', '28/10/2020 9:26:07 AM', '28/10/2020 9:48:29 AM', '28/10/2020 9:57:34 AM', '29/01/2020 3:06:56 PM', '29/01/2020 3:35:31 PM', '29/01/2020 9:04:13 AM', '29/04/2020 10:05:38 AM', '29/04/2020 11:47:57 AM', '29/04/2020 12:45:35 PM', '29/04/2020 1:05:00 PM', '29/04/2020 2:02:41 PM', '29/04/2020 2:36:22 PM', '29/04/2020 4:06:44 PM', '29/04/2020 4:25:31 PM', '29/04/2020 5:11:26 PM', '29/04/2020 5:11:43 PM', '29/05/2020 10:58:35 AM', '29/05/2020 12:09:19 PM', '29/05/2020 12:36:39 PM', '29/05/2020 2:11:15 PM', '29/05/2020 2:25:24 PM', '29/05/2020 2:46:12 PM', '29/05/2020 2:59:22 PM', '29/05/2020 3:12:09 PM', '29/05/2020 3:21:44 PM', '29/05/2020 3:56:40 PM', '29/05/2020 4:04:20 PM', '29/05/2020 4:44:41 PM', '29/05/2020 9:07:28 AM', '29/06/2020 10:11:32 AM', '29/06/2020 10:30:30 AM', '29/06/2020 11:45:43 AM', '29/06/2020 12:08:39 PM', '29/06/2020 12:22:47 PM', '29/06/2020 1:58:41 PM', '29/06/2020 2:13:45 PM', '29/06/2020 2:23:48 PM', '29/06/2020 4:25:50 PM', '29/06/2020 4:37:04 PM', '29/06/2020 4:48:08 PM', '29/06/2020 8:45:17 PM', '29/06/2020 9:30:21 AM', '29/07/2020 10:31:02 AM', '29/07/2020 11:10:22 AM', '29/07/2020 11:49:08 AM', '29/07/2020 11:58:55 AM', '29/07/2020 12:26:54 PM', '29/07/2020 2:15:10 PM', '29/07/2020 2:29:37 PM', '29/07/2020 2:41:52 PM', '29/07/2020 3:35:46 PM', '29/07/2020 4:50:21 PM', '29/09/2020 10:47:57 AM', '29/09/2020 11:27:42 AM', '29/09/2020 11:44:50 AM', '29/09/2020 12:31:15 PM', '29/09/2020 1:37:55 PM', '29/09/2020 1:57:43 PM', '29/09/2020 3:33:21 PM', '29/09/2020 3:46:48 PM', '29/09/2020 4:06:51 PM', '29/09/2020 4:20:12 PM', '29/09/2020 4:28:45 PM', '29/09/2020 4:37:32 PM', '29/09/2020 9:37:01 AM', '29/10/2020 10:54:23 AM', '29/10/2020 11:26:15 AM', '29/10/2020 11:31:04 AM', '29/10/2020 12:28:29 PM', '29/10/2020 12:57:09 PM', '29/10/2020 12:59:22 PM', '29/10/2020 2:17:30 PM', '29/10/2020 2:17:33 PM', '29/10/2020 3:44:15 PM', '29/10/2020 4:15:09 PM', '29/10/2020 5:04:25 PM', '29/10/2020 9:49:59 AM', '3/01/2020 11:20:33 AM', '3/01/2020 9:38:47 AM', '3/02/2020 10:54:33 AM', '3/02/2020 11:37:33 AM', '3/02/2020 11:46:24 AM', '3/02/2020 12:53:44 PM', '3/02/2020 1:19:26 PM', '3/02/2020 2:55:30 PM', '3/02/2020 3:12:11 PM', '3/03/2020 10:29:32 AM', '3/03/2020 11:09:54 AM', '3/03/2020 12:18:24 PM', '3/03/2020 12:54:14 PM', '3/03/2020 2:09:3</t>
+          <t>['1/04/2020 10:56:58 AM', '1/04/2020 11:49:55 AM', '1/04/2020 1:55:40 PM', '1/04/2020 3:39:57 PM', '1/04/2020 9:41:47 AM', '1/05/2020 11:53:11 AM', '1/05/2020 12:52:38 PM', '1/05/2020 1:07:00 PM', '1/05/2020 1:55:58 PM', '1/05/2020 4:21:36 PM', '1/05/2020 5:31:51 PM', '1/06/2020 10:07:53 AM', '1/06/2020 10:21:10 AM', '1/06/2020 10:38:43 AM', '1/06/2020 11:35:14 AM', '1/06/2020 12:20:15 PM', '1/06/2020 12:39:25 PM', '1/06/2020 4:39:51 PM', '1/06/2020 9:29:50 AM', '1/06/2020 9:56:26 AM', '1/07/2020 10:08:53 AM', '1/07/2020 10:36:35 AM', '1/07/2020 10:40:39 AM', '1/07/2020 2:17:38 PM', '1/07/2020 2:51:36 PM', '1/07/2020 3:39:08 PM', '1/07/2020 3:40:38 PM', '1/07/2020 9:35:15 AM', '1/09/2020 10:31:47 AM', '1/09/2020 10:46:55 AM', '1/09/2020 11:08:06 AM', '1/09/2020 12:18:48 PM', '1/09/2020 1:19:10 PM', '1/09/2020 1:54:52 PM', '1/09/2020 2:09:57 PM', '1/09/2020 3:44:49 PM', '1/09/2020 4:17:39 PM', '1/09/2020 9:05:32 AM', '1/09/2020 9:29:18 AM', '1/10/2020 10:38:28 AM', '1/10/2020 10:51:28 AM', '1/10/2020 11:15:15 AM', '1/10/2020 11:43:34 AM', '1/10/2020 12:15:02 PM', '1/10/2020 12:23:10 PM', '1/10/2020 12:32:54 PM', '1/10/2020 1:21:07 PM', '1/10/2020 2:03:34 PM', '1/10/2020 3:45:02 PM', '1/10/2020 3:54:49 PM', '1/10/2020 4:45:18 PM', '1/10/2020 9:30:15 AM', '1/12/2020 1:57:55 PM', '1/12/2020 4:59:35 PM', '10/02/2020 12:35:03 PM', '10/02/2020 1:20:27 PM', '10/02/2020 2:29:16 PM', '10/02/2020 5:23:12 PM', '10/02/2020 9:15:15 AM', '10/02/2020 9:58:29 AM', '10/03/2020 10:41:01 AM', '10/03/2020 11:22:40 AM', '10/03/2020 2:25:02 PM', '10/03/2020 3:18:02 PM', '10/03/2020 3:36:51 PM', '10/03/2020 4:47:34 PM', '10/06/2020 10:32:38 AM', '10/06/2020 10:55:12 AM', '10/06/2020 12:06:03 PM', '10/06/2020 1:44:11 PM', '10/06/2020 2:14:09 PM', '10/06/2020 2:35:32 PM', '10/06/2020 2:51:53 PM', '10/06/2020 3:38:08 PM', '10/06/2020 3:53:16 PM', '10/06/2020 4:18:04 PM', '10/06/2020 9:25:13 AM', '10/06/2020 9:32:46 AM', '10/07/2020 11:59:23 AM', '10/07/2020 1:38:50 PM', '10/07/2020 4:32:12 PM', '10/07/2020 4:52:45 PM', '10/07/2020 9:23:48 AM', '10/07/2020 9:37:12 AM', '10/08/2020 10:26:48 AM', '10/08/2020 10:41:27 AM', '10/08/2020 11:11:22 AM', '10/08/2020 11:38:07 AM', '10/08/2020 1:52:59 PM', '10/08/2020 2:54:03 PM', '10/08/2020 3:18:34 PM', '10/08/2020 3:41:35 PM', '10/08/2020 4:29:32 PM', '10/08/2020 4:38:59 PM', '10/08/2020 5:14:51 PM', '10/09/2020 10:35:18 AM', '10/09/2020 11:24:12 AM', '10/09/2020 12:21:53 PM', '10/09/2020 3:25:16 PM', '10/09/2020 3:39:04 PM', '10/09/2020 3:43:13 PM', '10/09/2020 3:56:49 PM', '10/09/2020 9:36:29 AM', '10/09/2020 9:50:06 AM', '10/09/2020 9:59:43 AM', '10/11/2020 12:38:33 PM', '10/11/2020 2:47:02 PM', '10/11/2020 4:16:49 PM', '10/11/2020 4:20:10 PM', '10/11/2020 9:38:16 AM', '10/11/2020 9:55:50 AM', '10/12/2020 10:32:53 AM', '10/12/2020 10:53:14 AM', '10/12/2020 12:17:44 PM', '10/12/2020 1:01:54 PM', '10/12/2020 2:28:55 PM', '10/12/2020 2:30:29 PM', '10/12/2020 2:42:03 PM', '10/12/2020 3:59:12 PM', '10/12/2020 4:17:19 PM', '10/12/2020 4:44:05 PM', '10/12/2020 9:31:22 AM', '11/02/2020 1:45:45 PM', '11/02/2020 3:58:22 PM', '11/03/2020 11:35:43 AM', '11/03/2020 11:56:26 AM', '11/03/2020 12:08:09 PM', '11/03/2020 12:45:27 PM', '11/03/2020 1:52:00 PM', '11/03/2020 2:01:09 PM', '11/03/2020 2:43:34 PM', '11/03/2020 4:53:10 PM', '11/03/2020 9:15:30 AM', '11/05/2020 11:04:46 AM', '11/05/2020 11:51:16 AM', '11/05/2020 12:43:50 PM', '11/05/2020 3:31:28 PM', '11/05/2020 3:47:29 PM', '11/05/2020 9:09:33 AM', '11/06/2020 10:39:04 AM', '11/06/2020 11:39:44 AM', '11/06/2020 11:42:01 AM', '11/06/2020 11:57:42 AM', '11/06/2020 12:11:56 PM', '11/06/2020 1:55:01 PM', '11/06/2020 3:04:08 PM', '11/06/2020 3:35:02 PM', '11/06/2020 3:51:00 PM', '11/06/2020 5:08:05 PM', '11/06/2020 9:28:31 AM', '11/06/2020 9:29:13 PM', '11/08/2020 10:08:29 AM', '11/08/2020 10:45:40 AM', '11/08/2020 11:01:23 AM', '11/08/2020 11:16:12 AM', '11/08/2020 3:45:35 PM', '11/08/2020 4:36:35 PM', '11/08/2020 8:56:12 AM', '11/08/2020 9:35:01 AM', '11/08/2020 9:53:16 AM', '11/09/2020 10:39:29 AM', '11/09/2020 3:11:32 PM', '11/09/2020 3:12:28 PM', '11/09/2020 3:54:14 PM', '11/09/2020 3:57:31 PM', '11/11/2020 10:35:33 AM', '11/11/2020 10:49:52 AM', '11/11/2020 11:10:10 AM', '11/11/2020 11:24:26 AM', '11/11/2020 12:05:16 PM', '11/11/2020 12:28:49 PM', '11/11/2020 12:55:18 PM', '11/11/2020 1:15:28 PM', '11/11/2020 2:24:13 PM', '11/11/2020 2:35:04 PM', '11/11/2020 2:35:58 PM', '11/11/2020 2:43:26 PM', '11/11/2020 3:06:24 PM', '11/11/2020 3:13:03 PM', '11/11/2020 3:53:48 PM', '11/11/2020 4:34:43 PM', '11/11/2020 4:42:19 PM', '11/12/2020 11:15:44 AM', '11/12/2020 11:35:22 AM', '11/12/2020 11:46:11 AM', '11/12/2020 11:53:29 AM', '11/12/2020 12:06:29 PM', '11/12/2020 12:24:10 PM', '11/12/2020 1:39:28 PM', '11/12/2020 1:50:39 PM', '11/12/2020 2:05:59 PM', '11/12/2020 2:30:12 PM', '11/12/2020 2:42:58 PM', '11/12/2020 3:25:08 PM', '11/12/2020 4:16:54 PM', '11/12/2020 4:45:27 PM', '11/12/2020 4:58:15 PM', '12/02/2020 1:32:41 PM', '12/02/2020 1:55:28 PM', '12/02/2020 3:23:37 PM', '12/02/2020 3:48:10 PM', '12/02/2020 4:47:12 PM', '12/02/2020 9:41:36 AM', '12/03/2020 12:43:27 PM', '12/03/2020 2:29:42 PM', '12/03/2020 4:11:56 PM', '12/05/2020 10:22:54 AM', '12/05/2020 11:58:18 AM', '12/05/2020 12:32:50 PM', '12/05/2020 9:48:13 AM', '12/06/2020 10:49:12 AM', '12/06/2020 10:51:31 AM', '12/06/2020 11:30:25 AM', '12/06/2020 12:00:45 PM', '12/06/2020 12:42:18 PM', '12/06/2020 2:18:14 PM', '12/06/2020 3:28:57 PM', '12/06/2020 3:52:17 PM', '12/08/2020 10:12:51 AM', '12/08/2020 10:22:47 AM', '12/08/2020 10:45:08 AM', '12/08/2020 11:45:22 AM', '12/08/2020 1:08:28 PM', '12/08/2020 2:00:16 PM', '12/08/2020 2:22:44 PM', '12/08/2020 3:05:34 PM', '12/08/2020 3:15:21 PM', '12/08/2020 3:38:48 PM', '12/08/2020 9:27:12 AM', '12/08/2020 9:41:11 AM', '12/08/2020 9:57:47 AM', '12/10/2020 11:56:41 AM', '12/10/2020 12:17:00 PM', '12/10/2020 1:58:18 PM', '12/10/2020 3:02:27 PM', '12/10/2020 3:18:57 PM', '12/10/2020 3:36:03 PM', '12/10/2020 3:38:02 PM', '12/10/2020 4:17:50 PM', '12/11/2020 10:57:07 AM', '12/11/2020 1:22:46 PM', '12/11/2020 2:23:57 PM', '12/11/2020 2:34:55 PM', '12/11/2020 2:48:45 PM', '12/11/2020 3:18:17 PM', '12/11/2020 3:27:52 PM', '12/11/2020 3:42:46 PM', '12/11/2020 4:04:31 PM', '12/11/2020 4:16:49 PM', '12/11/2020 4:41:14 PM', '12/11/2020 9:48:30 AM', '13/02/2020 11:49:00 AM', '13/02/2020 11:49:45 AM', '13/02/2020 11:59:50 AM', '13/02/2020 12:01:09 PM', '13/02/2020 12:11:19 PM', '13/02/2020 12:25:18 PM', '13/02/2020 2:43:51 PM', '13/02/2020 3:36:21 PM', '13/03/2020 10:19:33 AM', '13/03/2020 11:00:05 AM', '13/03/2020 11:53:53 AM', '13/03/2020 1:44:33 PM', '13/03/2020 2:17:28 PM', '13/03/2020 3:03:59 PM', '13/03/2020 4:12:10 PM', '13/03/2020 4:32:44 PM', '13/03/2020 5:06:27 PM', '13/03/2020 5:28:15 PM', '13/05/2020 1:49:10 PM', '13/07/2020 10:26:06 AM', '13/07/2020 11:20:52 AM', '13/07/2020 11:43:46 AM', '13/07/2020 11:47:20 AM', '13/07/2020 12:21:56 PM', '13/07/2020 2:24:32 PM', '13/07/2020 2:56:37 PM', '13/07/2020 9:45:18 AM', '13/08/2020 10:57:16 AM', '13/08/2020 11:19:06 AM', '13/08/2020 11:33:42 AM', '13/08/2020 11:56:20 AM', '13/08/2020 1:38:15 PM', '13/08/2020 2:04:21 PM', '13/08/2020 3:15:07 PM', '13/08/2020 4:00:32 PM', '13/08/2020 4:15:09 PM', '13/08/2020 4:27:04 PM', '13/08/2020 9:16:50 AM', '13/08/2020 9:58:56 AM', '13/10/2020 11:55:13 AM', '13/10/2020 2:36:29 PM', '13/10/2020 2:50:52 PM', '13/10/2020 3:01:39 PM', '13/10/2020 3:07:36 PM', '13/10/2020 4:16:56 PM', '13/11/2020 11:10:01 AM', '13/11/2020 12:31:02 PM', '13/11/2020 12:41:59 PM', '13/11/2020 4:07:31 PM', '13/11/2020 9:54:51 AM', '14/01/2020 4:46:53 PM', '14/02/2020 10:03:09 AM', '14/02/2020 12:39:33 PM', '14/02/2020 1:22:07 PM', '14/02/2020 1:44:28 PM', '14/02/2020 2:18:57 PM', '14/02/2020 3:09:22 PM', '14/02/2020 4:31:40 PM', '14/02/2020 9:20:55 AM', '14/02/2020 9:43:40 AM', '14/04/2020 12:33:18 PM', '14/04/2020 2:16:25 PM', '14/04/2020 4:31:49 PM', '14/04/2020 5:33:47 PM', '14/05/2020 10:01:08 AM', '14/05/2020 11:55:06 AM', '14/05/2020 2:58:35 PM', '14/05/2020 4:12:20 PM', '14/05/2020 4:14:50 PM', '14/05/2020 4:55:17 PM', '14/05/2020 9:23:33 AM', '14/05/2020 9:45:20 AM', '14/07/2020 10:38:46 AM', '14/07/2020 11:51:34 AM', '14/07/2020 3:27:23 PM', '14/07/2020 4:14:18 PM', '14/07/2020 4:36:48 PM', '14/07/2020 9:38:17 AM', '14/07/2020 9:46:20 AM', '14/08/2020 10:04:03 AM', '14/08/2020 11:10:25 AM', '14/08/2020 11:57:11 AM', '14/08/2020 12:48:02 PM', '14/08/2020 1:41:13 PM', '14/08/2020 4:00:46 PM', '14/08/2020 4:10:09 PM', '14/08/2020 4:49:03 PM', '14/08/2020 9:21:31 AM', '14/09/2020 10:37:52 AM', '14/09/2020 11:19:54 AM', '14/09/2020 9:35:38 AM', '14/10/2020 10:07:40 AM', '14/10/2020 10:42:21 AM', '14/10/2020 11:16:57 AM', '14/10/2020 11:37:33 AM', '14/10/2020 12:39:04 PM', '14/10/2020 12:49:39 PM', '14/10/2020 1:21:50 PM', '14/10/2020 1:29:04 PM', '14/10/2020 2:43:18 PM', '14/10/2020 9:20:31 AM', '14/12/2020 10:02:53 AM', '14/12/2020 10:16:50 AM', '14/12/2020 10:27:55 AM', '14/12/2020 10:52:23 AM', '14/12/2020 10:57:30 AM', '14/12/2020 11:16:11 AM', '14/12/2020 11:26:51 AM', '14/12/2020 11:51:09 AM', '14/12/2020 2:12:24 PM', '14/12/2020 3:18:51 PM', '14/12/2020 4:54:41 PM', '14/12/2020 4:57:44 PM', '15/01/2020 4:21:56 PM', '15/01/2020 9:59:45 AM', '15/04/2020 1:30:32 PM', '15/04/2020 4:18:28 PM', '15/05/2020 10:44:44 AM', '15/05/2020 10:59:29 AM', '15/05/2020 12:18:09 PM', '15/05/2020 2:03:54 PM', '15/05/2020 2:51:44 PM', '15/05/2020 3:17:15 PM', '15/05/2020 9:48:09 AM', '15/06/2020 10:13:16 AM', '15/06/2020 10:33:40 AM', '15/06/2020 12:08:55 PM', '15/06/2020 12:14:05 PM', '15/06/2020 12:45:43 PM', '15/06/2020 1:12:50 PM', '15/06/2020 2:08:20 PM', '15/06/2020 3:34:32 PM', '15/06/2020 4:20:00 PM', '15/06/2020 4:50:16 PM', '15/06/2020 4:50:47 PM', '15/07/2020 10:19:19 AM', '15/07/2020 10:45:38 AM', '15/07/2020 11:27:54 AM', '15/07/2020 12:55:11 PM', '15/07/2020 1:15:28 PM', '15/07/2020 1:58:29 PM', '15/07/2020 2:28:19 PM', '15/07/2020 2:35:41 PM', '15/07/2020 4:13:12 PM', '15/07/2020 9:30:59 AM', '15/09/2020 1:37:12 PM', '15/09/2020 2:10:27 PM', '15/09/2020 2:58:04 PM', '15/09/2020 3:18:28 PM', '15/10/2020 11:51:52 AM', '15/10/2020 11:59:42 AM', '15/10/2020 1:11:28 PM', '15/10/2020 2:21:42 PM', '15/10/2020 2:41:21 PM', '15/10/2020 2:57:22 PM', '15/12/2020 11:08:52 AM', '15/12/2020 11:47:26 AM', '15/12/2020 11:56:20 AM', '15/12/2020 12:12:18 PM', '15/12/2020 1:29:50 PM', '15/12/2020 3:28:18 PM', '15/12/2020 3:39:13 PM', '15/12/2020 3:48:03 PM', '15/12/2020 3:48:10 PM', '15/12/2020 4:02:42 PM', '15/12/2020 4:12:52 PM', '16/01/2020 12:15:44 PM', '16/03/2020 11:34:04 AM', '16/03/2020 12:19:46 PM', '16/03/2020 2:01:19 PM', '16/03/2020 2:12:02 PM', '16/03/2020 2:24:15 PM', '16/03/2020 3:23:06 PM', '16/03/2020 3:47:23 PM', '16/03/2020 4:03:59 PM', '16/03/2020 4:24:12 PM', '16/03/2020 4:24:45 PM', '16/03/2020 4:39:51 PM', '16/03/2020 9:43:46 AM', '16/04/2020 10:30:25 AM', '16/04/2020 11:16:56 AM', '16/04/2020 11:42:50 AM', '16/04/2020 12:00:00 AM', '16/04/2020 12:01:00 PM', '16/04/2020 12:59:09 PM', '16/04/2020 1:39:34 PM', '16/04/2020 3:13:26 PM', '16/04/2020 3:37:29 PM', '16/04/2020 4:01:14 PM', '16/04/2020 9:52:24 AM', '16/06/2020 10:20:22 AM', '16/06/2020 1:06:38 PM', '16/06/2020 1:16:41 PM', '16/06/2020 3:11:38 PM', '16/06/2020 3:57:16 PM', '16/06/2020 4:09:53 PM', '16/06/2020 4:35:32 PM', '16/06/2020 5:01:32 PM', '16/06/2020 9:22:05 AM', '16/06/2020 9:49:36 AM', '16/07/2020 2:12:51 PM', '16/07/2020 3:05:34 PM', '16/07/2020 3:10:17 PM', '16/07/2020 4:05:22 PM', '16/07/2020 4:23:14 PM', '16/07/2020 4:28:39 PM', '16/09/2020 10:54:56 AM', '16/09/2020 11:03:50 AM', '16/09/2020 12:37:04 PM', '16/09/2020 2:16:39 PM', '16/09/2020 2:41:12 PM', '16/09/2020 3:28:17 PM', '16/09/2020 3:36:31 PM', '16/09/2020 3:44:58 PM', '16/09/2020 3:56:53 PM', '16/09/2020 4:06:59 PM', '16/09/2020 4:37:18 PM', '16/10/2020 10:45:47 AM', '16/10/2020 10:47:05 AM', '16/10/2020 10:56:54 AM', '16/10/2020 11:40:25 AM', '16/10/2020 12:03:21 PM', '16/10/2020 2:06:32 PM', '16/10/2020 3:40:40 PM', '16/10/2020 4:04:00 PM', '16/10/2020 9:08:41 AM', '16/10/2020 9:52:50 AM', '16/11/2020 11:02:21 AM', '16/11/2020 11:03:41 AM', '16/11/2020 11:20:51 AM', '16/11/2020 11:25:44 AM', '16/11/2020 11:40:50 AM', '16/11/2020 11:40:57 AM', '16/11/2020 12:12:15 PM', '16/11/2020 12:30:16 PM', '16/11/2020 12:43:11 PM', '16/11/2020 1:07:01 PM', '16/11/2020 1:51:59 PM', '16/11/2020 2:10:52 PM', '16/11/2020 2:14:32 PM', '16/11/2020 2:49:59 PM', '16/11/2020 3:02:53 PM', '16/11/2020 3:28:38 PM', '16/11/2020 3:28:48 PM', '16/11/2020 4:18:02 PM', '16/11/2020 5:05:59 PM', '16/11/2020 9:51:55 AM', '16/12/2020 10:11:24 AM', '16/12/2020 11:08:49 AM', '16/12/2020 11:16:19 AM', '16/12/2020 11:16:50 AM', '16/12/2020 11:21:00 AM', '16/12/2020 11:30:37 AM', '16/12/2020 11:52:02 AM', '16/12/2020 12:13:17 PM', '16/12/2020 12:30:30 PM', '16/12/2020 12:34:02 PM', '16/12/2020 1:12:33 PM', '16/12/2020 1:13:03 PM', '16/12/2020 1:46:34 PM', '16/12/2020 2:17:10 PM', '16/12/2020 3:04:42 PM', '16/12/2020 3:21:20 PM', '16/12/2020 3:34:32 PM', '16/12/2020 3:51:29 PM', '16/12/2020 4:09:39 PM', '16/12/2020 4:34:12 PM', '16/12/2020 5:18:30 PM', '17/01/2020 11:32:17 AM', '17/01/2020 9:05:24 AM', '17/02/2020 10:26:01 AM', '17/02/2020 10:54:56 AM', '17/02/2020 2:36:08 PM', '17/02/2020 3:43:43 PM', '17/02/2020 4:05:34 PM', '17/04/2020 10:42:33 AM', '17/04/2020 11:53:18 AM', '17/04/2020 12:31:41 PM', '17/04/2020 3:35:32 PM', '17/04/2020 4:02:59 PM', '17/04/2020 4:13:41 PM', '17/04/2020 4:22:46 PM', '17/04/2020 4:37:13 PM', '17/04/2020 9:30:52 AM', '17/04/2020 9:45:41 AM', '17/06/2020 10:18:03 AM', '17/06/2020 10:23:40 AM', '17/06/2020 10:32:06 AM', '17/06/2020 11:01:33 AM', '17/06/2020 11:26:09 AM', '17/06/2020 11:26:18 AM', '17/06/2020 11:28:29 AM', '17/06/2020 12:20:31 PM', '17/06/2020 12:35:03 PM', '17/06/2020 12:38:04 PM', '17/06/2020 1:15:20 PM', '17/06/2020 5:22:13 PM', '17/06/2020 9:27:11 AM', '17/06/2020 9:58:57 AM', '17/07/2020 11:48:46 AM', '17/07/2020 2:43:38 PM', '17/07/2020 3:13:46 PM', '17/07/2020 4:33:28 PM', '17/08/2020 10:03:48 AM', '17/08/2020 10:41:19 AM', '17/08/2020 11:30:46 AM', '17/08/2020 12:02:23 PM', '17/08/2020 12:34:03 PM', '17/08/2020 1:45:09 PM', '17/08/2020 1:55:54 PM', '17/08/2020 2:37:12 PM', '17/08/2020 3:12:14 PM', '17/08/2020 5:33:50 PM', '17/09/2020 10:22:48 AM', '17/09/2020 10:49:51 AM', '17/09/2020 4:20:53 PM', '17/09/2020 5:49:54 PM', '17/09/2020 8:54:19 AM', '17/11/2020 10:28:38 AM', '17/11/2020 11:26:04 AM', '17/11/2020 11:26:11 AM', '17/11/2020 11:53:51 AM', '17/11/2020 12:05:24 PM', '17/11/2020 12:12:08 PM', '17/11/2020 12:33:36 PM', '17/11/2020 12:44:25 PM', '17/11/2020 12:58:52 PM', '17/11/2020 1:50:12 PM', '17/11/2020 2:32:02 PM', '17/11/2020 2:52:27 PM', '17/11/2020 3:15:25 PM', '17/11/2020 4:12:04 PM', '17/11/2020 4:19:07 PM', '17/11/2020 9:56:59 AM', '17/12/2020 11:05:50 AM', '17/12/2020 1:32:19 PM', '17/12/2020 2:30:21 PM', '17/12/2020 2:48:28 PM', '17/12/2020 2:49:48 PM', '17/12/2020 3:27:28 PM', '17/12/2020 3:29:35 PM', '17/12/2020 3:31:21 PM', '17/12/2020 3:41:02 PM', '17/12/2020 4:01:49 PM', '17/12/2020 4:36:20 PM', '17/12/2020 4:54:38 PM', '17/12/2020 5:15:37 PM', '17/12/2020 9:10:15 AM', '18/02/2020 1:57:46 PM', '18/02/2020 2:57:57 PM', '18/02/2020 4:29:53 PM', '18/02/2020 9:44:14 AM', '18/03/2020 10:55:23 AM', '18/03/2020 9:18:02 AM', '18/03/2020 9:39:08 AM', '18/05/2020 10:09:24 AM', '18/05/2020 10:26:09 AM', '18/05/2020 10:40:15 AM', '18/05/2020 11:43:08 AM', '18/05/2020 2:07:37 PM', '18/05/2020 2:21:25 PM', '18/05/2020 2:44:20 PM', '18/05/2020 3:55:57 PM', '18/05/2020 9:48:51 AM', '18/06/2020 10:35:51 AM', '18/06/2020 11:04:17 AM', '18/06/2020 11:33:03 AM', '18/06/2020 11:36:31 AM', '18/06/2020 11:52:07 AM', '18/06/2020 12:15:24 PM', '18/06/2020 2:03:24 PM', '18/06/2020 2:47:11 PM', '18/06/2020 3:54:26 PM', '18/06/2020 4:39:17 PM', '18/06/2020 4:48:17 PM', '18/08/2020 10:38:58 AM', '18/08/2020 10:42:06 AM', '18/08/2020 10:58:32 AM', '18/08/2020 12:18:35 PM', '18/08/2020 1:07:22 PM', '18/08/2020 2:23:20 PM', '18/08/2020 4:53:35 PM', '18/08/2020 9:59:59 AM', '18/09/2020 10:45:33 AM', '18/09/2020 12:06:24 PM', '18/09/2020 2:17:54 PM', '18/09/2020 2:40:15 PM', '18/09/2020 3:48:01 PM', '18/09/2020 3:58:06 PM', '18/09/2020 4:28:24 PM', '18/09/2020 4:29:34 PM', '18/09/2020 4:42:02 PM', '18/09/2020 4:53:58 PM', '18/09/2020 5:03:31 PM', '18/09/2020 9:51:23 AM', '18/11/2020 10:24:07 AM', '18/11/2020 10:41:00 AM', '18/11/2020 11:11:19 AM', '18/11/2020 11:43:33 AM', '18/11/2020 11:45:13 AM', '18/11/2020 12:02:14 PM', '18/11/2020 2:03:39 PM', '18/11/2020 3:10:56 PM', '18/11/2020 3:18:47 PM', '18/11/2020 3:30:54 PM', '18/11/2020 4:42:53 PM', '18/11/2020 4:49:20 PM', '18/11/2020 9:21:22 AM', '18/12/2020 10:01:25 AM', '18/12/2020 10:03:31 AM', '18/12/2020 10:09:05 AM', '18/12/2020 10:48:02 AM', '18/12/2020 11:04:57 AM', '18/12/2020 11:16:36 AM', '18/12/2020 11:17:52 AM', '18/12/2020 11:37:55 AM', '18/12/2020 11:46:24 AM', '18/12/2020 12:17:29 PM', '18/12/2020 9:53:00 AM', '19/02/2020 10:34:28 AM', '19/02/2020 12:10:00 PM', '19/02/2020 12:48:00 PM', '19/02/2020 3:34:54 PM', '19/02/2020 9:20:46 AM', '19/02/2020 9:52:12 AM', '19/03/2020 10:09:33 AM', '19/03/2020 10:55:28 AM', '19/03/2020 11:21:17 AM', '19/03/2020 11:25:38 AM', '19/03/2020 11:39:21 AM', '19/03/2020 12:13:17 PM', '19/03/2020 12:28:02 PM', '19/03/2020 1:22:20 PM', '19/03/2020 1:32:36 PM', '19/03/2020 2:40:39 PM', '19/03/2020 3:09:14 PM', '19/03/2020 3:10:12 PM', '19/03/2020 5:01:50 PM', '19/03/2020 9:24:44 AM', '19/05/2020 10:00:13 AM', '19/05/2020 10:22:22 AM', '19/05/2020 10:41:18 PM', '19/05/2020 12:49:25 PM', '19/05/2020 1:15:51 PM', '19/05/2020 2:45:55 PM', '19/05/2020 2:57:45 PM', '19/05/2020 3:37:28 PM', '19/05/2020 3:51:12 PM', '19/05/2020 4:05:32 PM', '19/05/2020 4:31:24 PM', '19/06/2020 10:04:30 AM', '19/06/2020 10:24:33 AM', '19/06/2020 11:16:13 AM', '19/06/2020 11:36:53 AM', '19/06/2020 1:34:14 PM', '19/06/2020 1:45:32 PM', '19/06/2020 2:30:46 PM', '19/06/2020 3:19:20 PM', '19/06/2020 3:43:18 PM', '19/06/2020 4:03:05 PM', '19/06/2020 9:35:59 AM', '19/08/2020 10:11:19 AM', '19/08/2020 10:51:48 AM', '19/08/2020 11:31:22 AM', '19/08/2020 12:27:06 PM', '19/08/2020 1:58:29 PM', '19/08/2020 4:11:58 PM', '19/08/2020 9:03:29 AM', '19/08/2020 9:37:40 AM', '19/08/2020 9:46:42 AM', '19/10/2020 10:03:31 AM', '19/10/2020 10:29:11 AM', '19/10/2020 10:37:53 AM', '19/10/2020 11:35:07 AM', '19/10/2020 11:56:03 AM', '19/10/2020 2:38:11 PM', '19/10/2020 2:51:01 PM', '19/10/2020 4:52:46 PM', '19/10/2020 5:04:25 PM', '19/11/2020 10:15:20 AM', '19/11/2020 12:52:05 PM', '19/11/2020 1:22:23 PM', '2/01/2020 3:07:29 PM', '2/03/2020 11:10:36 AM', '2/03/2020 11:24:21 AM', '2/03/2020 11:48:04 AM', '2/03/2020 11:58:50 AM', '2/03/2020 1:33:51 PM', '2/03/2020 4:10:08 PM', '2/03/2020 4:11:30 PM', '2/03/2020 5:24:35 PM', '2/03/2020 9:20:43 AM', '2/03/2020 9:29:51 AM', '2/03/2020 9:39:40 AM', '2/04/2020 11:09:47 AM', '2/04/2020 12:00:03 PM', '2/04/2020 12:15:50 PM', '2/04/2020 1:33:18 PM', '2/07/2020 11:06:36 AM', '2/07/2020 11:34:28 AM', '2/07/2020 11:52:50 AM', '2/07/2020 11:54:00 AM', '2/07/2020 12:10:05 PM', '2/07/2020 1:20:08 PM', '2/07/2020 2:33:34 PM', '2/07/2020 4:47:47 PM', '2/07/2020 4:55:09 PM', '2/07/2020 9:21:05 AM', '2/09/2020 10:11:42 AM', '2/09/2020 10:42:18 AM', '2/09/2020 11:00:54 AM', '2/09/2020 11:22:04 AM', '2/09/2020 11:23:03 AM', '2/09/2020 11:32:15 AM', '2/09/2020 12:01:30 PM', '2/09/2020 12:10:51 PM', '2/09/2020 12:16:09 PM', '2/09/2020 12:29:12 PM', '2/09/2020 12:44:11 PM', '2/09/2020 1:11:06 PM', '2/09/2020 1:28:02 PM', '2/09/2020 1:39:22 PM', '2/09/2020 2:11:00 PM', '2/09/2020 2:31:09 PM', '2/09/2020 2:51:57 PM', '2/09/2020 3:11:32 PM', '2/09/2020 3:56:17 PM', '2/09/2020 9:51:29 AM', '2/10/2020 10:05:44 AM', '2/10/2020 10:24:47 AM', '2/10/2020 11:44:26 AM', '2/10/2020 12:33:53 PM', '2/10/2020 12:44:04 PM', '2/10/2020 3:25:17 PM', '2/10/2020 9:13:00 AM', '2/10/2020 9:50:20 AM', '2/10/2020 9:56:16 AM', '2/11/2020 11:51:21 AM', '2/11/2020 2:06:08 PM', '2/11/2020 2:21:04 PM', '2/11/2020 2:49:28 PM', '2/11/2020 3:20:11 PM', '2/11/2020 3:43:29 PM', '2/11/2020 4:13:17 PM', '2/11/2020 4:52:36 PM', '2/12/2020 10:05:43 AM', '2/12/2020 11:26:55 AM', '2/12/2020 1:13:07 PM', '2/12/2020 2:17:01 PM', '2/12/2020 2:40:23 PM', '2/12/2020 3:07:57 PM', '2/12/2020 3:39:00 PM', '2/12/2020 3:39:44 PM', '2/12/2020 3:50:43 PM', '2/12/2020 4:04:06 PM', '2/12/2020 4:28:05 PM', '2/12/2020 4:29:31 PM', '2/12/2020 4:44:21 PM', '2/12/2020 5:00:00 PM', '20/01/2020 10:18:49 AM', '20/01/2020 9:58:30 AM', '20/02/2020 10:04:18 AM', '20/02/2020 10:20:49 AM', '20/02/2020 10:27:40 AM', '20/02/2020 10:48:45 AM', '20/02/2020 10:50:10 AM', '20/02/2020 11:02:22 AM', '20/02/2020 11:16:44 AM', '20/02/2020 11:18:16 AM', '20/02/2020 12:02:42 PM', '20/02/2020 12:31:49 PM', '20/02/2020 1:29:19 PM', '20/02/2020 2:14:04 PM', '20/02/2020 2:36:19 PM', '20/02/2020 9:18:34 AM', '20/02/2020 9:51:50 AM', '20/03/2020 10:07:01 AM', '20/03/2020 10:18:08 AM', '20/03/2020 11:26:41 AM', '20/03/2020 11:37:05 AM', '20/03/2020 1:23:15 PM', '20/03/2020 1:48:35 PM', '20/03/2020 2:09:57 PM', '20/03/2020 2:33:05 PM', '20/03/2020 3:01:01 PM', '20/03/2020 3:42:21 PM', '20/03/2020 4:42:56 PM', '20/03/2020 9:45:31 AM', '20/03/2020 9:53:26 AM', '20/04/2020 11:05:23 AM', '20/04/2020 12:00:00 AM', '20/04/2020 12:05:23 PM', '20/04/2020 12:24:43 PM', '20/04/2020 2:16:16 PM', '20/04/2020 2:38:03 PM', '20/04/2020 4:51:52 PM', '20/04/2020 5:17:27 PM', '20/05/2020 10:21:11 AM', '20/05/2020 1:10:41 PM', '20/05/2020 2:33:16 PM', '20/05/2020 3:53:02 PM', '20/05/2020 9:54:10 AM', '20/07/2020 10:19:18 AM', '20/07/2020 10:45:16 AM', '20/07/2020 11:54:58 AM', '20/07/2020 2:14:06 PM', '20/08/2020 10:13:56 AM', '20/08/2020 11:46:49 AM', '20/08/2020 2:24:16 PM', '20/08/2020 2:59:58 PM', '20/08/2020 4:38:02 PM', '20/08/2020 9:48:28 AM', '20/08/2020 9:51:09 AM', '20/10/2020 12:51:14 PM', '20/10/2020 2:05:03 PM', '20/10/2020 9:22:36 AM', '20/11/2020 12:21:15 PM', '21/01/2020 12:19:29 PM', '21/01/2020 9:20:36 AM', '21/02/2020 10:59:53 AM', '21/02/2020 11:38:04 AM', '21/02/2020 11:59:06 AM', '21/02/2020 12:23:45 PM', '21/02/2020 12:45:57 PM', '21/02/2020 3:14:24 PM', '21/02/2020 3:25:06 PM', '21/02/2020 4:18:02 PM', '21/02/2020 4:31:11 PM', '21/02/2020 9:23:34 AM', '21/04/2020 10:06:36 AM', '21/04/2020 10:13:16 AM', '21/04/2020 12:56:28 PM', '21/04/2020 2:40:17 PM', '21/04/2020 3:49:53 PM', '21/04/2020 8:34:53 AM', '21/05/2020 10:15:55 AM', '21/05/2020 11:49:33 AM', '21/05/2020 12:31:16 PM', '21/05/2020 1:44:23 PM', '21/05/2020 1:53:20 PM', '21/05/2020 3:47:33 PM', '21/05/2020 3:55:31 PM', '21/05/2020 9:50:23 AM', '21/05/2020 9:59:45 AM', '21/07/2020 10:11:41 AM', '21/07/2020 3:52:01 PM', '21/07/2020 4:05:55 PM', '21/07/2020 4:46:59 PM', '21/08/2020 10:12:10 AM', '21/08/2020 10:42:34 AM', '21/08/2020 12:05:18 PM', '21/08/2020 12:16:55 PM', '21/08/2020 1:46:38 PM', '21/08/2020 3:12:18 PM', '21/08/2020 4:27:59 PM', '21/08/2020 4:52:11 PM', '21/09/2020 10:18:40 AM', '21/09/2020 11:05:40 AM', '21/09/2020 11:14:37 AM', '21/09/2020 11:22:16 AM', '21/09/2020 11:53:23 AM', '21/09/2020 12:00:06 PM', '21/09/2020 12:10:46 PM', '21/09/2020 12:42:51 PM', '21/09/2020 3:11:27 PM', '21/09/2020 3:34:12 PM', '21/09/2020 3:58:38 PM', '21/09/2020 4:03:08 PM', '21/09/2020 4:48:05 PM', '21/09/2020 9:07:02 AM', '21/09/2020 9:57:29 AM', '21/10/2020 11:12:24 AM', '21/10/2020 12:35:13 PM', '21/10/2020 12:45:52 PM', '21/10/2020 1:22:57 PM', '21/10/2020 2:08:00 PM', '21/10/2020 2:12:40 PM', '21/10/2020 2:51:08 PM', '21/10/2020 2:54:49 PM', '21/10/2020 3:04:40 PM', '21/10/2020 3:35:33 PM', '21/10/2020 3:59:03 PM', '21/10/2020 4:02:56 PM', '21/10/2020 4:36:06 PM', '21/12/2020 10:22:53 AM', '21/12/2020 10:29:25 AM', '21/12/2020 10:36:25 AM', '21/12/2020 10:39:08 AM', '21/12/2020 10:52:14 AM', '21/12/2020 11:55:46 AM', '21/12/2020 12:08:49 PM', '21/12/2020 3:50:17 PM', '21/12/2020 3:52:56 PM', '21/12/2020 4:26:21 PM', '21/12/2020 9:29:14 AM', '21/12/2020 9:38:43 AM', '22/04/2020 1:20:13 PM', '22/04/2020 1:55:52 PM', '22/04/2020 3:41:52 PM', '22/04/2020 4:10:06 PM', '22/05/2020 10:06:56 AM', '22/05/2020 10:32:13 AM', '22/05/2020 4:01:50 PM', '22/05/2020 4:11:59 PM', '22/05/2020 4:20:30 PM', '22/05/2020 5:45:02 PM', '22/06/2020 10:14:25 AM', '22/06/2020 10:36:19 AM', '22/06/2020 9:23:59 AM', '22/07/2020 10:51:44 AM', '22/07/2020 2:13:54 PM', '22/07/2020 2:26:32 PM', '22/07/2020 2:59:38 PM', '22/07/2020 3:15:32 PM', '22/07/2020 3:49:32 PM', '22/07/2020 9:19:36 AM', '22/07/2020 9:52:59 AM', '22/09/2020 12:11:44 PM', '22/09/2020 5:20:50 PM', '22/10/2020 12:48:48 PM', '22/10/2020 1:02:35 PM', '22/10/2020 1:11:41 PM', '22/10/2020 1:51:20 PM', '22/10/2020 2:02:27 PM', '22/10/2020 4:00:05 PM', '22/10/2020 4:23:01 PM', '22/12/2020 10:25:54 AM', '22/12/2020 10:47:24 AM', '22/12/2020 12:40:05 PM', '22/12/2020 3:53:46 PM', '22/12/2020 4:15:22 PM', '22/12/2020 4:49:37 PM', '22/12/2020 9:00:46 AM', '22/12/2020 9:40:12 AM', '22/12/2020 9:59:52 AM', '23/01/2020 11:21:59 AM', '23/01/2020 4:40:44 PM', '23/03/2020 10:17:49 AM', '23/03/2020 10:20:30 AM', '23/03/2020 10:34:32 AM', '23/03/2020 12:45:17 PM', '23/03/2020 1:11:23 PM', '23/03/2020 3:29:52 PM', '23/03/2020 9:30:39 AM', '23/03/2020 9:57:29 AM', '23/04/2020 11:24:21 AM', '23/04/2020 1:28:03 PM', '23/06/2020 10:10:22 AM', '23/06/2020 11:03:27 AM', '23/06/2020 11:47:29 AM', '23/06/2020 3:19:49 PM', '23/06/2020 3:21:40 PM', '23/06/2020 4:05:21 PM', '23/06/2020 4:54:50 PM', '23/06/2020 9:56:26 AM', '23/07/2020 10:18:16 AM', '23/07/2020 1:57:12 PM', '23/07/2020 2:01:40 PM', '23/07/2020 2:49:21 PM', '23/07/2020 3:24:09 PM', '23/07/2020 3:36:36 PM', '23/07/2020 4:32:09 PM', '23/09/2020 10:07:26 AM', '23/09/2020 10:09:19 AM', '23/09/2020 10:15:26 AM', '23/09/2020 10:33:31 AM', '23/09/2020 11:22:22 AM', '23/09/2020 12:33:39 PM', '23/09/2020 12:45:05 PM', '23/09/2020 12:58:15 PM', '23/09/2020 2:00:54 PM', '23/09/2020 2:09:49 PM', '23/09/2020 2:14:27 PM', '23/09/2020 2:24:59 PM', '23/09/2020 3:13:55 PM', '23/09/2020 3:25:49 PM', '23/09/2020 3:52:16 PM', '23/09/2020 4:24:39 PM', '23/09/2020 9:19:42 AM', '23/10/2020 12:08:16 PM', '23/10/2020 12:30:20 PM', '23/10/2020 12:58:13 PM', '23/10/2020 1:08:29 PM', '23/10/2020 1:20:08 PM', '23/10/2020 1:36:09 PM', '23/10/2020 1:59:49 PM', '23/10/2020 2:30:14 PM', '23/10/2020 3:25:48 PM', '23/10/2020 3:51:39 PM', '23/10/2020 3:59:05 PM', '23/10/2020 4:04:49 PM', '23/10/2020 9:20:36 AM', '23/10/2020 9:56:35 AM', '23/11/2020 10:44:26 AM', '23/11/2020 11:14:48 AM', '23/11/2020 11:17:26 AM', '23/11/2020 12:02:25 PM', '23/11/2020 12:02:42 PM', '23/11/2020 12:31:13 PM', '23/11/2020 12:35:37 PM', '23/11/2020 12:56:55 PM', '23/11/2020 1:10:21 PM', '23/11/2020 1:58:58 PM', '23/11/2020 2:19:48 PM', '23/11/2020 3:03:47 PM', '23/11/2020 3:13:20 PM', '23/11/2020 3:23:57 PM', '23/11/2020 3:53:52 PM', '23/11/2020 4:40:05 PM', '23/11/2020 9:43:23 AM', '23/12/2020 10:00:46 AM', '23/12/2020 10:42:51 AM', '23/12/2020 10:51:16 AM', '23/12/2020 12:10:10 PM', '23/12/2020 12:26:22 PM', '23/12/2020 12:44:10 PM', '23/12/2020 1:12:49 PM', '23/12/2020 1:18:35 PM', '23/12/2020 1:57:48 PM', '23/12/2020 2:12:44 PM', '23/12/2020 2:52:50 PM', '23/12/2020 3:20:35 PM', '23/12/2020 4:18:23 PM', '23/12/2020 4:34:35 PM', '23/12/2020 4:41:21 PM', '23/12/2020 4:48:20 PM', '23/12/2020 9:21:56 AM', '23/12/2020 9:45:24 AM', '23/12/2020 9:46:21 AM', '24/01/2020 10:44:54 AM', '24/01/2020 3:00:48 PM', '24/02/2020 10:15:58 AM', '24/02/2020 10:30:24 AM', '24/02/2020 11:14:45 AM', '24/02/2020 12:44:12 PM', '24/03/2020 3:54:32 PM', '24/03/2020 9:10:17 AM', '24/03/2020 9:33:58 AM', '24/04/2020 4:02:28 PM', '24/06/2020 10:07:24 AM', '24/06/2020 11:15:13 AM', '24/06/2020 11:19:07 AM', '24/06/2020 12:35:33 PM', '24/06/2020 1:08:55 PM', '24/06/2020 1:55:48 PM', '24/06/2020 2:28:01 PM', '24/06/2020 3:05:44 PM', '24/06/2020 3:09:47 PM', '24/06/2020 3:59:29 PM', '24/06/2020 4:05:23 PM', '24/06/2020 4:26:51 PM', '24/06/2020 4:34:55 PM', '24/06/2020 4:45:04 PM', '24/06/2020 9:35:46 AM', '24/06/2020 9:46:54 AM', '24/06/2020 9:48:35 AM', '24/07/2020 1:22:02 PM', '24/07/2020 1:44:33 PM', '24/07/2020 2:25:04 PM', '24/07/2020 3:04:03 PM', '24/07/2020 4:10:14 PM', '24/07/2020 9:05:06 AM', '24/08/2020 11:16:53 AM', '24/08/2020 12:07:05 PM', '24/08/2020 2:40:07 PM', '24/08/2020 2:46:24 PM', '24/08/2020 3:56:27 PM', '24/08/2020 4:22:06 PM', '24/08/2020 4:42:56 PM', '24/09/2020 10:21:57 AM', '24/09/2020 10:55:15 AM', '24/09/2020 11:37:34 AM', '24/09/2020 12:58:01 PM', '24/09/2020 1:23:37 PM', '24/09/2020 2:19:36 PM', '24/09/2020 2:42:11 PM', '24/09/2020 5:04:52 PM', '24/09/2020 9:27:10 AM', '24/09/2020 9:41:00 AM', '24/11/2020 10:14:05 AM', '24/11/2020 10:42:13 AM', '24/11/2020 11:00:50 AM', '24/11/2020 11:36:00 AM', '24/11/2020 11:47:58 AM', '24/11/2020 12:17:30 PM', '24/11/2020 2:41:02 PM', '24/11/2020 3:03:18 PM', '24/11/2020 4:02:58 PM', '24/11/2020 4:49:38 PM', '25/02/2020 12:55:26 PM', '25/02/2020 2:07:57 PM', '25/02/2020 9:32:36 AM', '25/03/2020 10:33:20 AM', '25/03/2020 3:22:58 PM', '25/03/2020 3:46:43 PM', '25/05/2020 2:51:08 PM', '25/05/2020 3:22:38 PM', '25/05/2020 8:53:47 AM', '25/05/2020 9:14:15 AM', '25/05/2020 9:47:46 AM', '25/06/2020 10:18:45 AM', '25/06/2020 10:34:03 AM', '25/06/2020 11:51:39 AM', '25/06/2020 12:52:05 PM', '25/06/2020 12:53:27 PM', '25/06/2020 2:06:06 PM', '25/06/2020 4:12:15 PM', '25/06/2020 4:53:13 PM', '25/06/2020 9:58:27 AM', '25/08/2020 11:41:37 AM', '25/08/2020 1:52:17 PM', '25/08/2020 3:15:22 PM', '25/08/2020 4:12:20 PM', '25/08/2020 4:29:14 PM', '25/08/2020 4:53:26 PM', '25/08/2020 5:17:51 PM', '25/08/2020 9:04:21 AM', '25/08/2020 9:32:42 AM', '25/09/2020 9:30:00 AM', '25/11/2020 10:16:51 AM', '25/11/2020 12:19:20 PM', '25/11/2020 12:50:20 PM', '25/11/2020 1:44:27 PM', '25/11/2020 1:54:20 PM', '25/11/2020 3:13:47 PM', '25/11/2020 4:13:20 PM', '25/11/2020 9:30:34 AM', '26/02/2020 10:58:33 AM', '26/02/2020 9:22:51 AM', '26/03/2020 10:44:51 AM', '26/03/2020 10:58:14 AM', '26/03/2020 12:18:32 PM', '26/03/2020 1:29:39 PM', '26/03/2020 2:23:42 PM', '26/03/2020 3:01:10 PM', '26/03/2020 3:52:45 PM', '26/03/2020 4:45:35 PM', '26/03/2020 4:55:50 PM', '26/03/2020 9:14:03 AM', '26/03/2020 9:52:45 AM', '26/05/2020 10:58:56 AM', '26/05/2020 11:19:16 AM', '26/05/2020 1:19:11 PM', '26/05/2020 3:44:09 PM', '26/05/2020 8:55:15 AM', '26/05/2020 9:40:58 AM', '26/06/2020 11:13:21 AM', '26/06/2020 11:37:13 AM', '26/06/2020 12:53:20 PM', '26/06/2020 3:01:17 PM', '26/06/2020 3:12:16 PM', '26/06/2020 4:30:13 PM', '26/06/2020 4:40:50 PM', '26/06/2020 5:48:42 PM', '26/06/2020 9:29:02 AM', '26/06/2020 9:43:45 AM', '26/08/2020 10:12:17 AM', '26/08/2020 10:51:26 AM', '26/08/2020 11:21:05 AM', '26/08/2020 11:35:43 AM', '26/08/2020 11:43:28 AM', '26/08/2020 12:17:29 PM', '26/08/2020 12:43:34 PM', '26/08/2020 12:47:59 PM', '26/08/2020 1:48:05 PM', '26/08/2020 2:23:14 PM', '26/08/2020 3:42:48 PM', '26/08/2020 4:11:41 PM', '26/08/2020 4:42:23 PM', '26/08/2020 9:13:18 AM', '26/10/2020 11:11:28 AM', '26/10/2020 11:24:18 AM', '26/10/2020 12:01:59 PM', '26/10/2020 2:48:36 PM', '26/10/2020 3:18:22 PM', '26/10/2020 3:43:43 PM', '26/10/2020 4:36:42 PM', '26/11/2020 11:29:21 AM', '26/11/2020 12:03:54 PM', '26/11/2020 1:20:27 PM', '26/11/2020 3:38:59 PM', '27/02/2020 10:39:07 AM', '27/02/2020 10:58:09 AM', '27/02/2020 11:08:32 AM', '27/02/2020 11:53:04 AM', '27/02/2020 12:36:22 PM', '27/02/2020 3:23:36 PM', '27/02/2020 4:39:35 PM', '27/03/2020 9:34:01 AM', '27/04/2020 12:10:56 PM', '27/04/2020 2:25:31 PM', '27/04/2020 2:57:07 PM', '27/04/2020 3:19:29 PM', '27/04/2020 3:38:49 PM', '27/04/2020 4:33:47 PM', '27/04/2020 4:58:31 PM', '27/04/2020 9:24:07 AM', '27/04/2020 9:44:05 AM', '27/05/2020 11:01:10 AM', '27/05/2020 11:26:19 AM', '27/05/2020 11:29:56 AM', '27/05/2020 12:15:09 PM', '27/05/2020 9:33:37 AM', '27/05/2020 9:43:54 AM', '27/05/2020 9:52:44 AM', '27/07/2020 10:51:38 AM', '27/07/2020 12:44:33 PM', '27/07/2020 1:39:07 PM', '27/07/2020 4:04:59 PM', '27/07/2020 5:01:10 PM', '27/08/2020 10:35:56 AM', '27/08/2020 11:04:47 AM', '27/08/2020 11:49:07 AM', '27/08/2020 1:19:58 PM', '27/08/2020 1:49:23 PM', '27/08/2020 1:57:12 PM', '27/08/2020 2:36:21 PM', '27/08/2020 3:24:35 PM', '27/08/2020 3:30:36 PM', '27/08/2020 3:47:23 PM', '27/08/2020 9:48:28 AM', '27/10/2020 10:23:37 AM', '27/10/2020 10:37:33 AM', '27/10/2020 11:48:44 AM', '27/10/2020 2:43:36 PM', '27/10/2020 4:16:35 PM', '27/10/2020 4:31:01 PM', '27/10/2020 4:39:55 PM', '27/10/2020 9:38:47 AM', '27/10/2020 9:57:32 AM', '27/11/2020 11:47:34 AM', '27/11/2020 12:11:37 PM', '27/11/2020 12:27:25 PM', '27/11/2020 1:31:49 PM', '27/11/2020 2:18:50 PM', '27/11/2020 2:24:40 PM', '27/11/2020 2:30:33 PM', '28/01/2020 3:32:55 PM', '28/01/2020 4:41:53 PM', '28/01/2020 9:18:11 AM', '28/01/2020 9:40:07 AM', '28/02/2020 10:13:36 AM', '28/02/2020 12:49:04 PM', '28/02/2020 1:09:09 PM', '28/02/2020 2:50:45</t>
         </is>
       </c>
     </row>
@@ -2191,7 +2191,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -2224,7 +2224,7 @@
         <v>0</v>
       </c>
       <c r="O20" t="n">
-        <v>819</v>
+        <v>869</v>
       </c>
       <c r="P20" t="n">
         <v>0</v>
@@ -2243,7 +2243,7 @@
         </is>
       </c>
       <c r="T20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
@@ -2251,13 +2251,13 @@
         </is>
       </c>
       <c r="V20" t="n">
-        <v>1729</v>
+        <v>1986</v>
       </c>
       <c r="W20" t="n">
         <v>1</v>
       </c>
       <c r="X20" t="n">
-        <v>12768</v>
+        <v>14595</v>
       </c>
       <c r="Y20" t="n">
         <v>4</v>
@@ -2283,7 +2283,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -2335,7 +2335,7 @@
         </is>
       </c>
       <c r="T21" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="U21" t="inlineStr">
         <is>
@@ -2343,13 +2343,13 @@
         </is>
       </c>
       <c r="V21" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="W21" t="n">
         <v>1</v>
       </c>
       <c r="X21" t="n">
-        <v>38925</v>
+        <v>43590</v>
       </c>
       <c r="Y21" t="n">
         <v>1</v>
@@ -2375,22 +2375,22 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E22" t="n">
-        <v>1020614.69</v>
+        <v>1200865.82</v>
       </c>
       <c r="F22" t="n">
-        <v>393.3004585741812</v>
+        <v>413.2366896077082</v>
       </c>
       <c r="G22" t="n">
-        <v>320.1</v>
+        <v>323.5</v>
       </c>
       <c r="H22" t="n">
-        <v>1399.134371236428</v>
+        <v>1475.166681710265</v>
       </c>
       <c r="I22" t="n">
-        <v>1957576.988775156</v>
+        <v>2176116.738828074</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>491.40</t>
+          <t>26145.50</t>
         </is>
       </c>
       <c r="T22" t="n">
@@ -2435,20 +2435,20 @@
         </is>
       </c>
       <c r="V22" t="n">
-        <v>232</v>
+        <v>253</v>
       </c>
       <c r="W22" t="n">
         <v>0</v>
       </c>
       <c r="X22" t="n">
-        <v>15144</v>
+        <v>16978</v>
       </c>
       <c r="Y22" t="n">
-        <v>909</v>
+        <v>1029</v>
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>['0.00', '1003.84', '1006.88', '1009.50', '1026.50', '1043.41', '1060.89', '1079.03', '108.75', '1086.00', '1106.35', '1108.50', '111.00', '1140.00', '1157.67', '1161.94', '1172.08', '1185.78', '122.50', '1247.00', '125.00', '1258.37', '1262.30', '1321.00', '1327.25', '1335.00', '134.00', '136.00', '13719.30', '1395.50', '140.00', '1419.82', '142.50', '143.00', '145.00', '145.05', '145.50', '1454.00', '1500.18', '1509.95', '1578.00', '1580.28', '165.00', '1661.68', '175.75', '177.25', '179.50', '181.75', '184.25', '185.50', '188.00', '189.50', '191.00', '193.50', '1933.82', '195.50', '197.50', '198.00', '199.50', '202.00', '2020.50', '2022.00', '207.25', '209.50', '2103.52', '214.00', '215.50', '2190.49', '220.00', '224.75', '228.94', '2361.50', '237.55', '239.00', '243.00', '248.75', '250.25', '251.25', '251.30', '2511.50', '252.75', '255.30', '256.50', '257.25', '261.50', '262.50', '264.00', '265.00', '265.42', '270.50', '270.65', '271.00', '272.53', '273.73', '273.97', '273.99', '276.41', '276.50', '280.56', '284.91', '285.57', '289.03', '289.09', '289.50', '290.69', '290.88', '2926.50', '295.04', '296.75', '298.04', '299.00', '300.75', '300.81', '303.00', '303.62', '303.98', '307.33', '308.75', '309.31', '310.53', '312.25', '312.75', '314.51', '317.35', '3185.84', '320.10', '320.74', '321.26', '322.50', '323.10', '323.50', '324.25', '325.00', '326.04', '326.80', '328.25', '329.00', '329.50', '330.00', '330.14', '331.00', '331.80', '332.30', '333.00', '333.83', '334.25', '334.51', '334.97', '336.00', '336.40', '336.62', '338.76', '338.86', '339.14', '339.62', '339.90', '340.57', '341.06', '345.25', '345.50', '346.76', '346.97', '346.98', '348.05', '349.70', '352.55', '352.69', '353.17', '353.62', '354.31', '355.00', '355.38', '356.25', '357.96', '358.65', '359.00', '359.22', '359.50', '360.25', '361.12', '362.75', '362.89', '364.00', '365.00', '365.69', '365.75', '366.90', '367.50', '368.75', '370.22', '370.28', '371.00', '371.26', '371.75', '372.00', '372.78', '373.37', '373.76', '373.81', '374.48', '374.54', '376.16', '376.20', '376.50', '377.39', '378.27', '381.06', '383.05', '384.50', '385.03', '386.10', '386.12', '386.49', '388.08', '388.25', '388.50', '389.00', '389.50', '389.88', '389.89', '390.75', '391.49', '392.88', '39205.69', '393.00', '393.01', '394.78', '395.44', '395.50', '395.68', '396.50', '396.75', '397.00', '397.58', '397.62', '397.79', '398.50', '398.65', '398.75', '399.21', '400.46', '401.50', '402.13', '402.60', '403.22', '403.50', '404.67', '404.84', '404.94', '406.00', '406.89', '407.38', '408.13', '409.44', '409.50', '409.54', '409.75', '410.66', '410.75', '410.97', '411.08', '411.56', '413.44', '413.78', '414.00', '414.83', '414.87', '414.91', '415.26', '416.82', '416.89', '417.00', '417.14', '417.50', '417.52', '417.91', '418.04', '419.12', '419.86', '420.10', '420.12', '420.28', '420.41', '420.47', '421.21', '421.41', '422.27', '422.50', '422.75', '423.60', '424.50', '424.62', '425.18', '425.25', '425.40', '425.48', '425.80', '425.86', '425.87', '425.96', '426.29', '426.50', '427.30', '430.00', '430.26', '430.75', '430.76', '430.90', '431.97', '432.36', '432.62', '432.84', '433.51', '433.87', '433.93', '4334.50', '434.06', '434.33', '434.42', '434.50', '434.55', '435.01', '435.11', '435.28', '435.66', '435.87', '436.80', '437.31', '437.50', '437.86', '438.06', '438.72', '438.99', '439.00', '439.37', '439.50', '439.53', '439.64', '439.70', '440.03', '440.25', '440.39', '441.00', '441.56', '441.66', '442.00', '442.19', '442.21', '442.22', '442.31', '442.50', '442.70', '443.04', '443.12', '443.38', '443.75', '444.82', '445.25', '445.53', '445.80', '446.00', '447.25', '447.63', '447.73', '447.84', '4478.00', '448.00', '448.07', '448.13', '448.43', '448.55', '4486.00', '449.00', '449.10', '449.21', '449.31', '449.41', '450.02', '450.50', '450.58', '451.30', '451.40', '451.50', '451.55', '451.86', '451.92', '451.93', '452.00', '452.37', '452.60', '452.71', '452.77', '452.91', '453.12', '453.25', '453.60', '453.68', '454.00', '454.32', '455.16', '455.29', '455.80', '456.15', '456.47', '456.58', '457.00', '457.42', '457.58', '457.69', '458.02', '458.06', '458.15', '458.37', '459.16', '459.38', '459.39', '459.44', '459.50', '459.84', '460.11', '460.35', '460.44', '460.75', '461.37', '461.45', '461.60', '462.58', '462.79', '463.00', '463.25', '463.26', '4636.50', '464.00', '464.04', '464.09', '464.10', '464.19', '464.45', '465.50', '465.75', '465.77', '465.87', '466.08', '466.10', '466.39', '467.06', '467.23', '467.75', '467.87', '468.12', '468.25', '468.32', '468.43', '468.51', '468.72', '469.50', '469.54', '469.96', '469.99', '470.25', '470.50', '470.87', '470.99', '471.50', '471.89', '471.98', '472.00', '472.36', '472.39', '472.75', '472.86', '472.98', '473.23', '473.25', '473.73', '473.82', '474.40', '474.50', '475.10', '475.35', '475.39', '475.44', '475.62', '475.71', '475.79', '476.03', '476.07', '476.29', '476.38', '476.41', '476.44', '476.96', '476.98', '476.99', '477.15', '477.83', '477.92', '478.06', '478.12', '478.18', '478.25', '478.58', '478.94', '479.47', '479.63', '479.81', '480.33', '480.50', '480.69', '481.02', '481.04', '481.50', '482.00', '482.28', '482.49', '482.65', '482.75', '482.81', '483.25', '483.27', '483.58', '483.76', '484.13', '484.50', '484.87', '484.96', '485.01', '485.05', '485.36', '485.50', '486.00', '486.41', '487.00', '487.10', '487.22', '487.37', '487.52', '487.91', '488.18', '488.36', '489.00', '489.03', '489.52', '489.86', '490.12', '490.25', '490.39', '490.54', '490.63', '491.00', '491.04', '491.33', '491.37', '491.40', '491.50', '491.56', '491.87', '493.56', '494.24', '494.60', '494.79', '494.81', '495.03', '495.12', '495.25', '495.92', '496.17', '496.26', '496.59', '496.70', '496.87', '497.00', '497.31', '497.81', '498.20', '499.00', '499.25', '499.36', '499.37', '499.41', '499.47', '499.69', '500.76', '501.06', '501.23', '501.33', '501.50', '501.60', '501.75', '501.97', '502.09', '502.29', '502.56', '502.70', '502.75', '503.17', '503.32', '503.53', '504.04', '504.20', '504.72', '505.21', '506.25', '506.81', '507.10', '507.12', '507.24', '507.62', '507.64', '507.72', '507.75', '507.88', '508.55', '509.20', '509.36', '509.50', '509.61', '510.61', '510.72', '511.30', '511.51', '511.76', '512.11', '512.23', '512.25', '512.34', '512.48', '512.61', '512.99', '513.02', '513.37', '513.95', '514.62', '514.63', '514.83', '514.88', '515.27', '515.44', '515.50', '515.56', '515.75', '515.83', '516.03', '516.11', '516.19', '516.22', '516.56', '516.59', '516.86', '516.99', '518.17', '518.23', '518.42', '518.63', '518.65', '518.88', '519.41', '519.47', '519.64', '520.25', '520.63', '520.85', '521.06', '521.23', '521.26', '521.75', '522.00', '522.07', '522.22', '522.57', '522.61', '522.75', '523.00', '523.02', '523.87', '523.97', '524.25', '524.38', '524.66', '525.32', '525.75', '525.95', '526.50', '526.79', '526.80', '527.47', '528.42', '529.10', '529.50', '529.61', '529.68', '529.91', '530.73', '531.18', '532.47', '532.58', '534.00', '534.50', '535.20', '535.51', '536.10', '537.10', '537.74', '538.53', '538.76', '539.00', '539.36', '539.44', '539.45', '540.00', '540.25', '541.10', '541.24', '541.61', '541.97', '542.68', '542.75', '542.76', '542.91', '542.92', '543.23', '543.78', '543.80', '544.40', '545.30', '545.44', '546.07', '546.60', '546.78', '548.38', '548.65', '548.87', '549.49', '549.68', '549.80', '550.07', '550.54', '550.59', '550.61', '551.65', '552.01', '552.72', '553.25', '553.46', '553.74', '555.44', '555.50', '557.13', '557.53', '557.75', '558.12', '558.27', '558.41', '558.43', '559.50', '559.94', '560.42', '562.00', '562.53', '563.12', '563.28', '564.37', '565.16', '565.61', '565.87', '565.94', '566.33', '566.34', '566.50', '567.75', '568.21', '569.00', '569.06', '569.20', '569.49', '569.70', '572.75', '573.00', '573.50', '574.00', '574.25', '575.03', '575.51', '576.10', '576.25', '576.28', '577.87', '579.52', '579.61', '579.93', '580.00', '581.63', '583.69', '584.50', '584.62', '584.90', '585.59', '589.00', '590.68', '592.42', '593.01', '595.50', '596.50', '598.00', '601.50', '602.61', '603.68', '607.23', '608.92', '611.50', '613.18', '614.37', '615.55', '617.27', '621.35', '624.86', '624.98', '625.66', '629.96', '630.07', '630.56', '632.20', '633.00', '633.83', '636.59', '637.19', '639.00', '640.59', '641.50', '644.50', '646.44', '650.14', '654.25', '654.75', '656.36', '661.83', '665.25', '665.40', '666.32', '666.70', '67.00', '670.25', '671.46', '678.12', '678.51', '68.50', '680.08', '681.68', '685.82', '686.12', '686.50', '686.78', '698.66', '700.97', '706.36', '707.00', '708.00', '709.00', '710.91', '711.00', '713.18', '720.63', '725.54', '727.10', '7323.50', '733.24', '736.07', '738.81', '740.25', '744.50', '754.41', '758.52', '7594.70', '766.75', '773.28', '773.60', '776.50', '780.51', '793.10', '793.20', '795.43', '837.22', '839.00', '841.62', '848.19', '850.18', '852.86', '864.75', '877.02', '901.50', '909.50', '922.17', '932.75', '935.50', '942.30', '948.62', '950.00', '950.85', '951.50', '952.44', '955.00', '957.00', '959.36', '959.50', '959.90', '964.00', '981.93', '987.04', '989.57']</t>
+          <t>['0.00', '1003.84', '1006.88', '1009.50', '1022.09', '1026.50', '1043.41', '1060.89', '1079.03', '108.75', '1086.00', '1106.35', '1108.50', '111.00', '1125.48', '1139.50', '1140.00', '115.00', '1157.67', '1161.94', '1172.08', '1185.78', '1207.59', '122.50', '1247.00', '125.00', '1258.37', '1262.30', '1321.00', '1327.25', '1335.00', '134.00', '136.00', '1371.19', '13719.30', '1395.50', '140.00', '1419.82', '142.50', '143.00', '145.00', '145.05', '145.50', '1454.00', '1500.18', '1509.95', '1578.00', '1580.28', '15886.50', '1714.00', '175.75', '177.25', '179.50', '181.75', '184.25', '185.50', '185.75', '188.00', '189.50', '191.00', '193.50', '1933.82', '195.50', '197.50', '198.00', '199.50', '202.00', '2020.50', '2022.00', '207.25', '209.50', '2103.52', '214.00', '215.50', '2190.49', '220.00', '224.75', '228.94', '2361.50', '237.55', '239.00', '243.00', '248.75', '250.25', '251.25', '251.30', '2511.50', '252.75', '255.30', '256.50', '257.25', '261.50', '26145.50', '262.50', '264.00', '265.00', '265.42', '269.10', '270.50', '270.65', '271.00', '272.53', '273.73', '273.97', '273.99', '276.41', '276.50', '279.90', '280.56', '284.91', '285.57', '288.00', '289.03', '289.09', '289.50', '290.69', '290.88', '2926.50', '295.04', '296.75', '297.00', '298.04', '299.00', '300.75', '300.81', '303.00', '303.62', '303.98', '307.33', '308.75', '309.31', '310.53', '312.25', '312.75', '314.51', '317.35', '3185.84', '320.10', '320.20', '320.74', '321.26', '322.50', '323.10', '323.50', '324.25', '325.00', '326.04', '326.80', '328.25', '329.00', '329.50', '330.00', '330.14', '331.00', '331.80', '332.30', '333.00', '333.83', '3339.00', '334.25', '334.51', '334.97', '336.00', '336.40', '336.62', '338.76', '338.86', '339.14', '339.62', '339.90', '340.57', '341.06', '345.25', '345.50', '346.76', '346.97', '346.98', '348.05', '349.70', '352.55', '352.69', '353.17', '353.62', '354.31', '355.00', '355.38', '356.25', '356.50', '357.96', '358.65', '359.00', '359.22', '359.50', '360.25', '361.12', '362.75', '362.89', '364.00', '365.00', '365.69', '365.75', '366.76', '366.90', '367.50', '368.66', '368.75', '369.41', '370.22', '370.28', '371.00', '371.26', '371.75', '372.00', '372.78', '373.37', '373.76', '373.81', '374.48', '374.54', '376.16', '376.20', '376.50', '377.39', '378.27', '379.00', '379.38', '381.06', '383.05', '384.50', '385.03', '386.10', '386.12', '386.49', '387.72', '388.08', '388.25', '388.50', '389.00', '389.50', '389.88', '389.89', '390.75', '391.49', '391.50', '392.88', '39205.69', '393.00', '393.01', '393.72', '394.78', '395.44', '395.50', '395.68', '396.37', '396.50', '396.75', '3964.00', '397.00', '397.50', '397.58', '397.62', '397.79', '398.50', '398.65', '398.75', '399.21', '400.46', '401.50', '402.13', '402.60', '403.22', '403.50', '404.67', '404.84', '404.87', '404.94', '406.00', '406.89', '407.38', '408.13', '409.44', '409.50', '409.54', '409.75', '410.66', '410.75', '410.97', '411.08', '411.56', '412.45', '413.44', '413.78', '414.00', '414.03', '414.05', '414.25', '414.83', '414.87', '414.91', '415.26', '416.82', '416.89', '417.00', '417.14', '417.50', '417.52', '417.91', '418.04', '418.36', '419.12', '419.86', '420.10', '420.12', '420.25', '420.28', '420.41', '420.47', '421.41', '422.27', '422.50', '422.75', '423.60', '424.50', '424.62', '425.18', '425.25', '425.40', '425.41', '425.48', '425.80', '425.86', '425.87', '425.96', '426.29', '426.50', '426.99', '427.30', '430.00', '430.26', '430.75', '430.76', '430.90', '431.97', '432.36', '432.62', '432.84', '432.91', '433.51', '433.78', '433.87', '433.93', '4334.50', '434.06', '434.18', '434.33', '434.42', '434.50', '434.55', '435.01', '435.11', '435.28', '435.66', '435.87', '436.80', '436.94', '436.96', '437.31', '437.50', '437.68', '437.86', '438.06', '438.72', '438.99', '439.00', '439.37', '439.50', '439.53', '439.64', '439.70', '440.03', '440.25', '441.00', '441.56', '441.66', '442.00', '442.19', '442.21', '442.22', '442.31', '442.45', '442.50', '442.61', '442.70', '443.04', '443.12', '443.38', '443.75', '444.04', '444.08', '444.82', '445.05', '445.25', '445.53', '445.80', '446.00', '446.50', '447.25', '447.63', '447.73', '447.84', '4478.00', '448.00', '448.07', '448.13', '448.43', '448.55', '448.75', '4486.00', '449.00', '449.10', '449.21', '449.31', '449.41', '450.02', '450.50', '450.58', '451.30', '451.40', '451.50', '451.55', '451.86', '451.92', '451.93', '452.00', '452.37', '452.60', '452.71', '452.77', '452.91', '453.12', '453.25', '453.60', '453.68', '454.00', '454.32', '454.52', '455.16', '455.29', '455.46', '455.80', '456.15', '456.47', '456.50', '456.58', '457.00', '457.42', '457.58', '457.69', '458.02', '458.06', '458.15', '458.37', '459.16', '459.38', '459.39', '459.44', '459.50', '459.84', '460.10', '460.11', '460.35', '460.44', '460.75', '460.85', '461.37', '461.45', '461.50', '461.60', '462.58', '462.79', '463.00', '463.25', '463.26', '463.32', '463.75', '4636.50', '464.00', '464.04', '464.09', '464.10', '464.19', '464.45', '465.00', '465.50', '465.72', '465.75', '465.77', '465.87', '466.00', '466.08', '466.10', '466.39', '466.40', '466.97', '467.06', '467.23', '467.75', '467.79', '467.87', '468.12', '468.25', '468.32', '468.43', '468.51', '468.72', '469.50', '469.54', '469.94', '469.96', '469.99', '470.25', '470.87', '470.99', '471.49', '471.50', '471.89', '471.98', '472.00', '472.36', '472.39', '472.61', '472.75', '472.86', '472.98', '473.23', '473.25', '473.73', '473.82', '474.40', '474.50', '474.59', '475.10', '475.39', '475.44', '475.62', '475.71', '475.79', '476.00', '476.03', '476.07', '476.29', '476.38', '476.41', '476.44', '476.96', '476.98', '476.99', '477.15', '477.83', '477.92', '478.06', '478.12', '478.18', '478.25', '478.58', '478.82', '478.94', '479.47', '479.63', '479.81', '480.33', '480.48', '480.50', '480.69', '481.02', '481.04', '481.50', '482.00', '482.28', '482.49', '482.65', '482.75', '482.81', '483.25', '483.27', '483.58', '483.76', '483.96', '484.13', '484.50', '484.87', '484.96', '485.01', '485.05', '485.36', '485.50', '485.86', '486.00', '486.41', '486.95', '487.00', '487.10', '487.22', '487.37', '487.52', '487.62', '487.77', '487.91', '488.18', '488.36', '488.61', '489.00', '489.03', '489.52', '489.71', '489.86', '490.12', '490.25', '490.39', '490.54', '490.63', '491.00', '491.02', '491.04', '491.33', '491.37', '491.40', '491.50', '491.56', '491.80', '491.87', '493.56', '494.24', '494.60', '494.79', '494.81', '494.93', '495.03', '495.12', '495.25', '495.92', '496.17', '496.26', '496.59', '496.70', '496.87', '497.00', '497.31', '497.44', '497.81', '498.20', '498.75', '499.00', '499.25', '499.36', '499.37', '499.41', '499.47', '499.69', '500.64', '500.76', '501.06', '501.23', '501.33', '501.50', '501.60', '501.75', '501.97', '502.09', '502.29', '502.56', '502.70', '502.75', '503.11', '503.17', '503.32', '503.53', '504.04', '504.20', '504.72', '505.21', '506.25', '506.81', '507.10', '507.12', '507.24', '507.62', '507.64', '507.72', '507.75', '507.88', '508.51', '508.55', '508.89', '509.20', '509.36', '509.50', '509.61', '510.61', '510.72', '511.30', '511.41', '511.51', '511.76', '512.11', '512.23', '512.25', '512.34', '512.48', '512.61', '512.99', '513.02', '513.37', '513.95', '514.62', '514.63', '514.83', '514.88', '515.27', '515.35', '515.40', '515.44', '515.50', '515.56', '515.75', '515.78', '515.83', '516.03', '516.11', '516.19', '516.22', '516.42', '516.56', '516.59', '516.79', '516.86', '516.99', '518.17', '518.23', '518.42', '518.63', '518.65', '518.88', '519.41', '519.47', '519.64', '520.21', '520.25', '520.50', '520.63', '520.70', '520.85', '521.06', '521.23', '521.26', '521.75', '522.00', '522.07', '522.22', '522.57', '522.61', '522.75', '522.96', '523.00', '523.02', '523.87', '523.97', '524.00', '524.25', '524.38', '524.66', '525.32', '525.75', '525.95', '526.50', '526.79', '526.80', '527.47', '528.42', '528.88', '529.10', '529.50', '529.61', '529.68', '529.91', '530.00', '530.73', '531.18', '532.47', '532.49', '532.58', '534.00', '534.50', '534.58', '535.20', '535.51', '536.10', '537.10', '537.68', '537.74', '538.53', '538.76', '539.00', '539.36', '539.44', '539.45', '540.00', '540.25', '541.10', '541.11', '541.24', '541.61', '541.97', '542.68', '542.75', '542.76', '542.91', '542.92', '543.23', '543.78', '543.80', '543.85', '544.40', '545.30', '545.44', '546.07', '546.60', '548.38', '548.65', '548.87', '548.88', '549.49', '549.68', '549.80', '550.07', '550.23', '550.54', '550.59', '550.61', '551.65', '552.01', '552.72', '553.25', '553.46', '553.74', '555.44', '555.50', '557.13', '557.53', '557.75', '558.12', '558.27', '558.41', '558.43', '559.50', '559.94', '560.42', '560.49', '561.45', '561.78', '562.00', '562.53', '563.12', '563.28', '564.37', '565.16', '565.21', '565.61', '565.87', '565.94', '566.33', '566.34', '566.50', '567.75', '567.83', '568.21', '569.00', '569.06', '569.20', '569.49', '569.70', '572.75', '573.00', '573.50', '574.00', '574.25', '575.03', '575.51', '576.10', '576.25', '576.28', '577.87', '579.52', '579.61', '579.93', '580.00', '580.53', '581.63', '583.69', '584.50', '584.62', '584.90', '585.00', '585.59', '586.50', '589.00', '590.68', '592.42', '593.01', '595.50', '596.50', '598.00', '601.50', '602.61', '603.68', '605.69', '607.23', '608.92', '611.50', '613.18', '614.37', '615.28', '615.55', '617.27', '621.35', '624.86', '624.98', '625.66', '629.96', '630.07', '630.56', '632.20', '633.00', '633.83', '636.59', '637.19', '638.87', '639.00', '640.59', '641.50', '644.50', '646.44', '650.08', '650.14', '651.50', '654.25', '654.75', '656.36', '658.08', '661.83', '662.96', '665.25', '665.40', '666.32', '666.70', '67.00', '670.25', '671.46', '678.12', '678.51', '68.50', '680.08', '681.68', '685.82', '686.12', '686.50', '686.78', '696.39', '698.66', '700.97', '702.77', '706.36', '707.00', '708.00', '709.00', '710.91', '711.00', '713.18', '720.63', '725.54', '727.10', '7323.50', '733.24', '736.07', '738.81', '740.25', '744.50', '754.41', '758.52', '766.75', '773.28', '773.60', '776.50', '7770.50', '780.51', '793.10', '793.20', '795.43', '8350.70', '837.22', '839.00', '841.62', '848.19', '850.18', '852.86', '864.75', '877.02', '890.58', '901.50', '909.50', '922.17', '932.75', '935.50', '942.30', '948.62', '950.00', '950.85', '951.50', '952.44', '955.00', '957.00', '959.36', '959.50', '959.90', '964.00', '981.93', '986.35', '987.04', '989.57']</t>
         </is>
       </c>
     </row>
@@ -2467,7 +2467,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -2500,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="O23" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="P23" t="n">
         <v>0</v>
@@ -2515,11 +2515,11 @@
       </c>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="U23" t="inlineStr"/>
       <c r="V23" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="W23" t="n">
         <v>0</v>
@@ -2551,7 +2551,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>25/11/2020 12:00:00 AM</t>
+          <t>5/12/2020 12:00:00 AM</t>
         </is>
       </c>
       <c r="T24" t="n">
@@ -2617,14 +2617,14 @@
         <v>0</v>
       </c>
       <c r="X24" t="n">
-        <v>56354</v>
+        <v>63068</v>
       </c>
       <c r="Y24" t="n">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>['1/04/2020 12:00:00 AM', '1/05/2020 12:00:00 AM', '1/06/2020 12:00:00 AM', '1/07/2020 12:00:00 AM', '1/09/2020 12:00:00 AM', '1/10/2020 12:00:00 AM', '10/01/2020 12:00:00 AM', '10/02/2020 12:00:00 AM', '10/03/2020 12:00:00 AM', '10/06/2020 12:00:00 AM', '10/07/2020 12:00:00 AM', '10/08/2020 12:00:00 AM', '10/09/2020 12:00:00 AM', '10/11/2020 12:00:00 AM', '11/02/2020 12:00:00 AM', '11/03/2020 12:00:00 AM', '11/05/2020 12:00:00 AM', '11/06/2020 12:00:00 AM', '11/08/2020 12:00:00 AM', '11/09/2020 12:00:00 AM', '11/11/2020 12:00:00 AM', '12/02/2020 12:00:00 AM', '12/03/2020 12:00:00 AM', '12/05/2020 12:00:00 AM', '12/06/2020 12:00:00 AM', '12/08/2020 12:00:00 AM', '12/09/2020 12:00:00 AM', '12/10/2020 12:00:00 AM', '12/11/2020 12:00:00 AM', '13/01/2020 12:00:00 AM', '13/02/2020 12:00:00 AM', '13/03/2020 12:00:00 AM', '13/05/2020 12:00:00 AM', '13/07/2020 12:00:00 AM', '13/08/2020 12:00:00 AM', '13/10/2020 12:00:00 AM', '13/11/2020 12:00:00 AM', '14/01/2020 12:00:00 AM', '14/02/2020 12:00:00 AM', '14/04/2020 12:00:00 AM', '14/05/2020 12:00:00 AM', '14/07/2020 12:00:00 AM', '14/08/2020 12:00:00 AM', '14/09/2020 12:00:00 AM', '14/10/2020 12:00:00 AM', '15/01/2020 12:00:00 AM', '15/04/2020 12:00:00 AM', '15/05/2020 12:00:00 AM', '15/06/2020 12:00:00 AM', '15/07/2020 12:00:00 AM', '15/08/2020 12:00:00 AM', '15/09/2020 12:00:00 AM', '15/10/2020 12:00:00 AM', '16/01/2020 12:00:00 AM', '16/03/2020 12:00:00 AM', '16/04/2020 12:00:00 AM', '16/06/2020 12:00:00 AM', '16/07/2020 12:00:00 AM', '16/09/2020 12:00:00 AM', '16/10/2020 12:00:00 AM', '16/11/2020 12:00:00 AM', '17/01/2020 12:00:00 AM', '17/02/2020 12:00:00 AM', '17/03/2020 12:00:00 AM', '17/04/2020 12:00:00 AM', '17/05/2020 12:00:00 AM', '17/06/2020 12:00:00 AM', '17/07/2020 12:00:00 AM', '17/08/2020 12:00:00 AM', '17/09/2020 12:00:00 AM', '17/10/2020 12:00:00 AM', '17/11/2020 12:00:00 AM', '18/02/2020 12:00:00 AM', '18/03/2020 12:00:00 AM', '18/05/2020 12:00:00 AM', '18/06/2020 12:00:00 AM', '18/08/2020 12:00:00 AM', '18/09/2020 12:00:00 AM', '18/11/2020 12:00:00 AM', '19/02/2020 12:00:00 AM', '19/03/2020 12:00:00 AM', '19/05/2020 12:00:00 AM', '19/06/2020 12:00:00 AM', '19/07/2020 12:00:00 AM', '19/08/2020 12:00:00 AM', '19/10/2020 12:00:00 AM', '19/11/2020 12:00:00 AM', '2/01/2020 12:00:00 AM', '2/03/2020 12:00:00 AM', '2/04/2020 12:00:00 AM', '2/06/2020 12:00:00 AM', '2/07/2020 12:00:00 AM', '2/08/2020 12:00:00 AM', '2/09/2020 12:00:00 AM', '2/10/2020 12:00:00 AM', '2/11/2020 12:00:00 AM', '20/01/2020 12:00:00 AM', '20/02/2020 12:00:00 AM', '20/03/2020 12:00:00 AM', '20/04/2020 12:00:00 AM', '20/05/2020 12:00:00 AM', '20/07/2020 12:00:00 AM', '20/08/2020 12:00:00 AM', '20/10/2020 12:00:00 AM', '21/01/2020 12:00:00 AM', '21/02/2020 12:00:00 AM', '21/03/2020 12:00:00 AM', '21/04/2020 12:00:00 AM', '21/05/2020 12:00:00 AM', '21/06/2020 12:00:00 AM', '21/07/2020 12:00:00 AM', '21/08/2020 12:00:00 AM', '21/09/2020 12:00:00 AM', '21/10/2020 12:00:00 AM', '22/01/2020 12:00:00 AM', '22/04/2020 12:00:00 AM', '22/05/2020 12:00:00 AM', '22/06/2020 12:00:00 AM', '22/07/2020 12:00:00 AM', '22/08/2020 12:00:00 AM', '22/09/2020 12:00:00 AM', '22/10/2020 12:00:00 AM', '23/01/2020 12:00:00 AM', '23/02/2020 12:00:00 AM', '23/03/2020 12:00:00 AM', '23/04/2020 12:00:00 AM', '23/06/2020 12:00:00 AM', '23/07/2020 12:00:00 AM', '23/09/2020 12:00:00 AM', '23/10/2020 12:00:00 AM', '23/11/2020 12:00:00 AM', '24/01/2020 12:00:00 AM', '24/02/2020 12:00:00 AM', '24/03/2020 12:00:00 AM', '24/04/2020 12:00:00 AM', '24/06/2020 12:00:00 AM', '24/07/2020 12:00:00 AM', '24/08/2020 12:00:00 AM', '24/09/2020 12:00:00 AM', '24/11/2020 12:00:00 AM', '25/02/2020 12:00:00 AM', '25/03/2020 12:00:00 AM', '25/05/2020 12:00:00 AM', '25/06/2020 12:00:00 AM', '25/08/2020 12:00:00 AM', '25/09/2020 12:00:00 AM', '25/11/2020 12:00:00 AM', '26/02/2020 12:00:00 AM', '26/03/2020 12:00:00 AM', '26/05/2020 12:00:00 AM', '26/06/2020 12:00:00 AM', '26/07/2020 12:00:00 AM', '26/08/2020 12:00:00 AM', '26/10/2020 12:00:00 AM', '26/11/2020 12:00:00 AM', '27/02/2020 12:00:00 AM', '27/03/2020 12:00:00 AM', '27/04/2020 12:00:00 AM', '27/05/2020 12:00:00 AM', '27/07/2020 12:00:00 AM', '27/08/2020 12:00:00 AM', '27/10/2020 12:00:00 AM', '28/01/2020 12:00:00 AM', '28/02/2020 12:00:00 AM', '28/04/2020 12:00:00 AM', '28/05/2020 12:00:00 AM', '28/07/2020 12:00:00 AM', '28/08/2020 12:00:00 AM', '28/09/2020 12:00:00 AM', '28/10/2020 12:00:00 AM', '29/01/2020 12:00:00 AM', '29/04/2020 12:00:00 AM', '29/05/2020 12:00:00 AM', '29/06/2020 12:00:00 AM', '29/07/2020 12:00:00 AM', '29/09/2020 12:00:00 AM', '29/10/2020 12:00:00 AM', '3/01/2020 12:00:00 AM', '3/02/2020 12:00:00 AM', '3/03/2020 12:00:00 AM', '3/04/2020 12:00:00 AM', '3/05/2020 12:00:00 AM', '3/06/2020 12:00:00 AM', '3/07/2020 12:00:00 AM', '3/08/2020 12:00:00 AM', '3/09/2020 12:00:00 AM', '3/11/2020 12:00:00 AM', '30/01/2020 12:00:00 AM', '30/03/2020 12:00:00 AM', '30/04/2020 12:00:00 AM', '30/05/2020 12:00:00 AM', '30/06/2020 12:00:00 AM', '30/07/2020 12:00:00 AM', '30/09/2020 12:00:00 AM', '30/10/2020 12:00:00 AM', '31/01/2020 12:00:00 AM', '31/03/2020 12:00:00 AM', '31/07/2020 12:00:00 AM', '31/08/2020 12:00:00 AM', '4/02/2020 12:00:00 AM', '4/03/2020 12:00:00 AM', '4/05/2020 12:00:00 AM', '4/06/2020 12:00:00 AM', '4/08/2020 12:00:00 AM', '4/09/2020 12:00:00 AM', '4/10/2020 12:00:00 AM', '4/11/2020 12:00:00 AM', '5/02/2020 12:00:00 AM', '5/03/2020 12:00:00 AM', '5/05/2020 12:00:00 AM', '5/06/2020 12:00:00 AM', '5/08/2020 12:00:00 AM', '5/09/2020 12:00:00 AM', '5/11/2020 12:00:00 AM', '6/01/2020 12:00:00 AM', '6/02/2020 12:00:00 AM', '6/03/2020 12:00:00 AM', '6/04/2020 12:00:00 AM', '6/05/2020 12:00:00 AM', '6/06/2020 12:00:00 AM', '6/07/2020 12:00:00 AM', '6/08/2020 12:00:00 AM', '6/10/2020 12:00:00 AM', '6/11/2020 12:00:00 AM', '7/01/2020 12:00:00 AM', '7/02/2020 12:00:00 AM', '7/04/2020 12:00:00 AM', '7/05/2020 12:00:00 AM', '7/07/2020 12:00:00 AM', '7/08/2020 12:00:00 AM', '7/09/2020 12:00:00 AM', '7/10/2020 12:00:00 AM', '8/01/2020 12:00:00 AM', '8/04/2020 12:00:00 AM', '8/05/2020 12:00:00 AM', '8/07/2020 12:00:00 AM', '8/08/2020 12:00:00 AM', '8/09/2020 12:00:00 AM', '8/10/2020 12:00:00 AM', '9/01/2020 12:00:00 AM', '9/03/2020 12:00:00 AM', '9/04/2020 12:00:00 AM', '9/06/2020 12:00:00 AM', '9/07/2020 12:00:00 AM', '9/08/2020 12:00:00 AM', '9/09/2020 12:00:00 AM', '9/10/2020 12:00:00 AM', '9/11/2020 12:00:00 AM']</t>
+          <t>['1/04/2020 12:00:00 AM', '1/05/2020 12:00:00 AM', '1/06/2020 12:00:00 AM', '1/07/2020 12:00:00 AM', '1/09/2020 12:00:00 AM', '1/10/2020 12:00:00 AM', '1/12/2020 12:00:00 AM', '10/01/2020 12:00:00 AM', '10/02/2020 12:00:00 AM', '10/03/2020 12:00:00 AM', '10/06/2020 12:00:00 AM', '10/07/2020 12:00:00 AM', '10/08/2020 12:00:00 AM', '10/09/2020 12:00:00 AM', '10/11/2020 12:00:00 AM', '10/12/2020 12:00:00 AM', '11/02/2020 12:00:00 AM', '11/03/2020 12:00:00 AM', '11/05/2020 12:00:00 AM', '11/06/2020 12:00:00 AM', '11/08/2020 12:00:00 AM', '11/09/2020 12:00:00 AM', '11/11/2020 12:00:00 AM', '11/12/2020 12:00:00 AM', '12/02/2020 12:00:00 AM', '12/03/2020 12:00:00 AM', '12/05/2020 12:00:00 AM', '12/06/2020 12:00:00 AM', '12/08/2020 12:00:00 AM', '12/09/2020 12:00:00 AM', '12/10/2020 12:00:00 AM', '12/11/2020 12:00:00 AM', '13/01/2020 12:00:00 AM', '13/02/2020 12:00:00 AM', '13/03/2020 12:00:00 AM', '13/05/2020 12:00:00 AM', '13/07/2020 12:00:00 AM', '13/08/2020 12:00:00 AM', '13/10/2020 12:00:00 AM', '13/11/2020 12:00:00 AM', '14/01/2020 12:00:00 AM', '14/02/2020 12:00:00 AM', '14/04/2020 12:00:00 AM', '14/05/2020 12:00:00 AM', '14/07/2020 12:00:00 AM', '14/08/2020 12:00:00 AM', '14/09/2020 12:00:00 AM', '14/10/2020 12:00:00 AM', '14/12/2020 12:00:00 AM', '15/01/2020 12:00:00 AM', '15/04/2020 12:00:00 AM', '15/05/2020 12:00:00 AM', '15/06/2020 12:00:00 AM', '15/07/2020 12:00:00 AM', '15/08/2020 12:00:00 AM', '15/09/2020 12:00:00 AM', '15/10/2020 12:00:00 AM', '15/12/2020 12:00:00 AM', '16/01/2020 12:00:00 AM', '16/03/2020 12:00:00 AM', '16/04/2020 12:00:00 AM', '16/06/2020 12:00:00 AM', '16/07/2020 12:00:00 AM', '16/09/2020 12:00:00 AM', '16/10/2020 12:00:00 AM', '16/11/2020 12:00:00 AM', '16/12/2020 12:00:00 AM', '17/01/2020 12:00:00 AM', '17/02/2020 12:00:00 AM', '17/03/2020 12:00:00 AM', '17/04/2020 12:00:00 AM', '17/05/2020 12:00:00 AM', '17/06/2020 12:00:00 AM', '17/07/2020 12:00:00 AM', '17/08/2020 12:00:00 AM', '17/09/2020 12:00:00 AM', '17/10/2020 12:00:00 AM', '17/11/2020 12:00:00 AM', '17/12/2020 12:00:00 AM', '18/02/2020 12:00:00 AM', '18/03/2020 12:00:00 AM', '18/05/2020 12:00:00 AM', '18/06/2020 12:00:00 AM', '18/08/2020 12:00:00 AM', '18/09/2020 12:00:00 AM', '18/11/2020 12:00:00 AM', '18/12/2020 12:00:00 AM', '19/02/2020 12:00:00 AM', '19/03/2020 12:00:00 AM', '19/05/2020 12:00:00 AM', '19/06/2020 12:00:00 AM', '19/07/2020 12:00:00 AM', '19/08/2020 12:00:00 AM', '19/10/2020 12:00:00 AM', '19/11/2020 12:00:00 AM', '2/01/2020 12:00:00 AM', '2/03/2020 12:00:00 AM', '2/04/2020 12:00:00 AM', '2/06/2020 12:00:00 AM', '2/07/2020 12:00:00 AM', '2/08/2020 12:00:00 AM', '2/09/2020 12:00:00 AM', '2/10/2020 12:00:00 AM', '2/11/2020 12:00:00 AM', '2/12/2020 12:00:00 AM', '20/01/2020 12:00:00 AM', '20/02/2020 12:00:00 AM', '20/03/2020 12:00:00 AM', '20/04/2020 12:00:00 AM', '20/05/2020 12:00:00 AM', '20/07/2020 12:00:00 AM', '20/08/2020 12:00:00 AM', '20/10/2020 12:00:00 AM', '21/01/2020 12:00:00 AM', '21/02/2020 12:00:00 AM', '21/03/2020 12:00:00 AM', '21/04/2020 12:00:00 AM', '21/05/2020 12:00:00 AM', '21/06/2020 12:00:00 AM', '21/07/2020 12:00:00 AM', '21/08/2020 12:00:00 AM', '21/09/2020 12:00:00 AM', '21/10/2020 12:00:00 AM', '21/12/2020 12:00:00 AM', '22/01/2020 12:00:00 AM', '22/04/2020 12:00:00 AM', '22/05/2020 12:00:00 AM', '22/06/2020 12:00:00 AM', '22/07/2020 12:00:00 AM', '22/08/2020 12:00:00 AM', '22/09/2020 12:00:00 AM', '22/10/2020 12:00:00 AM', '22/12/2020 12:00:00 AM', '23/01/2020 12:00:00 AM', '23/02/2020 12:00:00 AM', '23/03/2020 12:00:00 AM', '23/04/2020 12:00:00 AM', '23/06/2020 12:00:00 AM', '23/07/2020 12:00:00 AM', '23/09/2020 12:00:00 AM', '23/10/2020 12:00:00 AM', '23/11/2020 12:00:00 AM', '23/12/2020 12:00:00 AM', '24/01/2020 12:00:00 AM', '24/02/2020 12:00:00 AM', '24/03/2020 12:00:00 AM', '24/04/2020 12:00:00 AM', '24/06/2020 12:00:00 AM', '24/07/2020 12:00:00 AM', '24/08/2020 12:00:00 AM', '24/09/2020 12:00:00 AM', '24/11/2020 12:00:00 AM', '25/02/2020 12:00:00 AM', '25/03/2020 12:00:00 AM', '25/05/2020 12:00:00 AM', '25/06/2020 12:00:00 AM', '25/08/2020 12:00:00 AM', '25/09/2020 12:00:00 AM', '25/11/2020 12:00:00 AM', '26/02/2020 12:00:00 AM', '26/03/2020 12:00:00 AM', '26/05/2020 12:00:00 AM', '26/06/2020 12:00:00 AM', '26/07/2020 12:00:00 AM', '26/08/2020 12:00:00 AM', '26/10/2020 12:00:00 AM', '26/11/2020 12:00:00 AM', '27/02/2020 12:00:00 AM', '27/03/2020 12:00:00 AM', '27/04/2020 12:00:00 AM', '27/05/2020 12:00:00 AM', '27/07/2020 12:00:00 AM', '27/08/2020 12:00:00 AM', '27/10/2020 12:00:00 AM', '27/11/2020 12:00:00 AM', '28/01/2020 12:00:00 AM', '28/02/2020 12:00:00 AM', '28/04/2020 12:00:00 AM', '28/05/2020 12:00:00 AM', '28/07/2020 12:00:00 AM', '28/08/2020 12:00:00 AM', '28/09/2020 12:00:00 AM', '28/10/2020 12:00:00 AM', '29/01/2020 12:00:00 AM', '29/04/2020 12:00:00 AM', '29/05/2020 12:00:00 AM', '29/06/2020 12:00:00 AM', '29/07/2020 12:00:00 AM', '29/09/2020 12:00:00 AM', '29/10/2020 12:00:00 AM', '3/01/2020 12:00:00 AM', '3/02/2020 12:00:00 AM', '3/03/2020 12:00:00 AM', '3/04/2020 12:00:00 AM', '3/05/2020 12:00:00 AM', '3/06/2020 12:00:00 AM', '3/07/2020 12:00:00 AM', '3/08/2020 12:00:00 AM', '3/09/2020 12:00:00 AM', '3/11/2020 12:00:00 AM', '3/12/2020 12:00:00 AM', '30/01/2020 12:00:00 AM', '30/03/2020 12:00:00 AM', '30/04/2020 12:00:00 AM', '30/05/2020 12:00:00 AM', '30/06/2020 12:00:00 AM', '30/07/2020 12:00:00 AM', '30/09/2020 12:00:00 AM', '30/10/2020 12:00:00 AM', '30/11/2020 12:00:00 AM', '31/01/2020 12:00:00 AM', '31/03/2020 12:00:00 AM', '31/07/2020 12:00:00 AM', '31/08/2020 12:00:00 AM', '4/02/2020 12:00:00 AM', '4/03/2020 12:00:00 AM', '4/05/2020 12:00:00 AM', '4/06/2020 12:00:00 AM', '4/08/2020 12:00:00 AM', '4/09/2020 12:00:00 AM', '4/10/2020 12:00:00 AM', '4/11/2020 12:00:00 AM', '4/12/2020 12:00:00 AM', '5/02/2020 12:00:00 AM', '5/03/2020 12:00:00 AM', '5/05/2020 12:00:00 AM', '5/06/2020 12:00:00 AM', '5/08/2020 12:00:00 AM', '5/09/2020 12:00:00 AM', '5/11/2020 12:00:00 AM', '5/12/2020 12:00:00 AM', '6/01/2020 12:00:00 AM', '6/02/2020 12:00:00 AM', '6/03/2020 12:00:00 AM', '6/04/2020 12:00:00 AM', '6/05/2020 12:00:00 AM', '6/06/2020 12:00:00 AM', '6/07/2020 12:00:00 AM', '6/08/2020 12:00:00 AM', '6/10/2020 12:00:00 AM', '6/11/2020 12:00:00 AM', '7/01/2020 12:00:00 AM', '7/02/2020 12:00:00 AM', '7/04/2020 12:00:00 AM', '7/05/2020 12:00:00 AM', '7/07/2020 12:00:00 AM', '7/08/2020 12:00:00 AM', '7/09/2020 12:00:00 AM', '7/10/2020 12:00:00 AM', '7/12/2020 12:00:00 AM', '8/01/2020 12:00:00 AM', '8/04/2020 12:00:00 AM', '8/05/2020 12:00:00 AM', '8/07/2020 12:00:00 AM', '8/08/2020 12:00:00 AM', '8/09/2020 12:00:00 AM', '8/10/2020 12:00:00 AM', '8/12/2020 12:00:00 AM', '9/01/2020 12:00:00 AM', '9/03/2020 12:00:00 AM', '9/04/2020 12:00:00 AM', '9/06/2020 12:00:00 AM', '9/07/2020 12:00:00 AM', '9/08/2020 12:00:00 AM', '9/09/2020 12:00:00 AM', '9/10/2020 12:00:00 AM', '9/11/2020 12:00:00 AM', '9/12/2020 12:00:00 AM']</t>
         </is>
       </c>
     </row>
@@ -2643,7 +2643,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -2676,7 +2676,7 @@
         <v>0</v>
       </c>
       <c r="O25" t="n">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="P25" t="n">
         <v>0</v>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>Private Certified Building Rules Consent Granted (17/11/2020)</t>
+          <t>Private Certified Planning Consent Granted (22/12/2020), Private Certified Building Rules Consent Required</t>
         </is>
       </c>
       <c r="T25" t="n">
@@ -2703,20 +2703,20 @@
         </is>
       </c>
       <c r="V25" t="n">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="W25" t="n">
         <v>0.802</v>
       </c>
       <c r="X25" t="n">
-        <v>220259</v>
+        <v>248775</v>
       </c>
       <c r="Y25" t="n">
-        <v>1547</v>
+        <v>1749</v>
       </c>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>['Building Rules Consent Granted (01/05/2020)', 'Building Rules Consent Granted (01/07/2020)', 'Building Rules Consent Granted (01/09/2020)', 'Building Rules Consent Granted (01/10/2020)', 'Building Rules Consent Granted (02/07/2020)', 'Building Rules Consent Granted (02/09/2020)', 'Building Rules Consent Granted (02/11/2020)', 'Building Rules Consent Granted (03/02/2020)', 'Building Rules Consent Granted (03/03/2020), Development Plan Consent Required', 'Building Rules Consent Granted (03/08/2020)', 'Building Rules Consent Granted (03/11/2020)', 'Building Rules Consent Granted (04/02/2020)', 'Building Rules Consent Granted (04/06/2020)', 'Building Rules Consent Granted (04/11/2020)', 'Building Rules Consent Granted (05/02/2020)', 'Building Rules Consent Granted (05/06/2020)', 'Building Rules Consent Granted (05/08/2020)', 'Building Rules Consent Granted (05/11/2020)', 'Building Rules Consent Granted (06/02/2020)', 'Building Rules Consent Granted (06/05/2020)', 'Building Rules Consent Granted (06/07/2020)', 'Building Rules Consent Granted (06/11/2020)', 'Building Rules Consent Granted (07/02/2020)', 'Building Rules Consent Granted (07/04/2020)', 'Building Rules Consent Granted (07/09/2020)', 'Building Rules Consent Granted (07/10/2020)', 'Building Rules Consent Granted (07/10/2020), Development Plan Consent Required', 'Building Rules Consent Granted (08/07/2020)', 'Building Rules Consent Granted (08/07/2020), Development Plan Consent Required', 'Building Rules Consent Granted (08/09/2020)', 'Building Rules Consent Granted (09/09/2020)', 'Building Rules Consent Granted (09/10/2020)', 'Building Rules Consent Granted (10/03/2020)', 'Building Rules Consent Granted (10/06/2020)', 'Building Rules Consent Granted (10/08/2020)', 'Building Rules Consent Granted (10/09/2020)', 'Building Rules Consent Granted (11/02/2020)', 'Building Rules Consent Granted (11/11/2020)', 'Building Rules Consent Granted (12/05/2020)', 'Building Rules Consent Granted (12/06/2020)', 'Building Rules Consent Granted (12/08/2020)', 'Building Rules Consent Granted (12/10/2020)', 'Building Rules Consent Granted (12/11/2020)', 'Building Rules Consent Granted (13/02/2020)', 'Building Rules Consent Granted (13/03/2020)', 'Building Rules Consent Granted (13/07/2020)', 'Building Rules Consent Granted (13/08/2020)', 'Building Rules Consent Granted (13/10/2020)', 'Building Rules Consent Granted (14/04/2020)', 'Building Rules Consent Granted (14/05/2020)', 'Building Rules Consent Granted (14/07/2020)', 'Building Rules Consent Granted (15/05/2020), Development Plan Consent Required', 'Building Rules Consent Granted (15/07/2020)', 'Building Rules Consent Granted (16/03/2020)', 'Building Rules Consent Granted (16/03/2020), Development Plan Consent Required', 'Building Rules Consent Granted (16/04/2020), Development Plan Consent Required', 'Building Rules Consent Granted (16/09/2020)', 'Building Rules Consent Granted (16/11/2020)', 'Building Rules Consent Granted (17/01/2020)', 'Building Rules Consent Granted (17/02/2020)', 'Building Rules Consent Granted (17/06/2020)', 'Building Rules Consent Granted (17/08/2020)', 'Building Rules Consent Granted (17/09/2020)', 'Building Rules Consent Granted (18/09/2020)', 'Building Rules Consent Granted (18/11/2020)', 'Building Rules Consent Granted (19/02/2020)', 'Building Rules Consent Granted (19/03/2020)', 'Building Rules Consent Granted (19/08/2020)', 'Building Rules Consent Granted (19/11/2020)', 'Building Rules Consent Granted (20/02/2020)', 'Building Rules Consent Granted (20/10/2020)', 'Building Rules Consent Granted (21/04/2020)', 'Building Rules Consent Granted (21/05/2020)', 'Building Rules Consent Granted (21/05/2020), Development Plan Consent Required', 'Building Rules Consent Granted (21/07/2020)', 'Building Rules Consent Granted (21/09/2020)', 'Building Rules Consent Granted (22/04/2020)', 'Building Rules Consent Granted (22/07/2020)', 'Building Rules Consent Granted (22/10/2020)', 'Building Rules Consent Granted (23/03/2020)', 'Building Rules Consent Granted (23/06/2020)', 'Building Rules Consent Granted (23/10/2020)', 'Building Rules Consent Granted (23/11/2020)', 'Building Rules Consent Granted (24/04/2020)', 'Building Rules Consent Granted (24/06/2020)', 'Building Rules Consent Granted (24/07/2020)', 'Building Rules Consent Granted (24/11/2020)', 'Building Rules Consent Granted (25/02/2020)', 'Building Rules Consent Granted (25/06/2020)', 'Building Rules Consent Granted (25/11/2020)', 'Building Rules Consent Granted (26/03/2020)', 'Building Rules Consent Granted (26/05/2020)', 'Building Rules Consent Granted (26/06/2020)', 'Building Rules Consent Granted (26/08/2020)', 'Building Rules Consent Granted (27/02/2020)', 'Building Rules Consent Granted (27/04/2020)', 'Building Rules Consent Granted (27/05/2020)', 'Building Rules Consent Granted (27/08/2020)', 'Building Rules Consent Granted (27/10/2020)', 'Building Rules Consent Granted (28/01/2020)', 'Building Rules Consent Granted (28/05/2020)', 'Building Rules Consent Granted (28/10/2020)', 'Building Rules Consent Granted (29/05/2020)', 'Building Rules Consent Granted (29/07/2020)', 'Building Rules Consent Granted (29/09/2020)', 'Building Rules Consent Granted (29/10/2020)', 'Building Rules Consent Granted (30/09/2020)', 'Building Rules Consent Granted (30/10/2020)', 'Building Rules Consent Granted (31/03/2020)', 'Building Rules Consent Required', 'Building Rules Consent Required, Development Plan Consent Required', 'Development Application Withdrawn (01/09/2020), Private Certified Building Rules Consent Required', 'Development Application Withdrawn (02/09/2020), Development Application Withdrawn (02/09/2020)', 'Development Application Withdrawn (03/03/2020), Development Application Withdrawn (03/03/2020)', 'Development Application Withdrawn (06/02/2020), Development Application Withdrawn (06/02/2020)', 'Development Application Withdrawn (08/04/2020)', 'Development Application Withdrawn (11/09/2020)', 'Development Application Withdrawn (11/09/2020), Development Application Withdrawn (11/09/2020)', 'Development Application Withdrawn (11/11/2020), Development Application Withdrawn (11/11/2020)', 'Development Application Withdrawn (12/10/2020)', 'Development Application Withdrawn (14/04/2020)', 'Development Application Withdrawn (15/01/2020)', 'Development Application Withdrawn (16/09/2020), Development Application Withdrawn (16/09/2020)', 'Development Application Withdrawn (17/07/2020)', 'Development Application Withdrawn (21/09/2020)', 'Development Application Withdrawn (22/07/2020), Development Application Withdrawn (22/07/2020)', 'Development Application Withdrawn (23/07/2020), Development Application Withdrawn (23/07/2020)', 'Development Application Withdrawn (23/09/2020)', 'Development Application Withdrawn (24/04/2020)', 'Development Application Withdrawn (25/05/2020)', 'Development Application Withdrawn (25/11/2020)', 'Development Application Withdrawn (26/11/2020), Development Application Withdrawn (26/11/2020)', 'Development Application Withdrawn (28/02/2020)', 'Development Application Withdrawn (29/07/2020), Development Application Withdrawn (29/07/2020)', 'Development Application Withdrawn (30/09/2020)', 'Development Plan Consent Granted (01/04/2020), Building Rules Consent Granted (11/06/2020)', 'Development Plan Consent Granted (01/04/2020), Building Rules Consent Required', 'Development Plan Consent Granted (01/06/2007), Building Rules Consent Granted (05/12/2007), Building Rules Consent Granted (29/05/2008), Development Plan Consent Granted (29/09/2020)', 'Development Plan Consent Granted (01/06/2020), Private Certified Building Rules Consent Granted (26/06/2020)', 'Development Plan Consent Granted (01/09/2020), Building Rules Consent Granted (03/09/2020)', 'Development Plan Consent Granted (01/09/2020), Building Rules Consent Granted (11/09/2020)', 'Development Plan Consent Granted (01/09/2020), Building Rules Consent Granted (20/10/2020)', 'Development Plan Consent Granted (01/09/2020), Private Certified Building Rules Consent Granted (06/10/2020)', 'Development Plan Consent Granted (01/09/2020), Private Certified Building Rules Consent Granted (07/09/2020)', 'Development Plan Consent Granted (01/09/2020), Private Certified Building Rules Consent Granted (09/10/2020)', 'Development Plan Consent Granted (01/09/2020), Private Certified Building Rules Consent Granted (13/09/2020)', 'Development Plan Consent Granted (01/09/2020), Private Certified Building Rules Consent Granted (17/10/2020)', 'Development Plan Consent Granted (01/10/2020), Building Rules Consent Granted (02/10/2020)', 'Development Plan Consent Granted (01/10/2020), Building Rules Consent Granted (03/11/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Granted (07/10/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Granted (08/10/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Granted (16/10/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Granted (22/10/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Granted (23/10/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (02/03/2020)', 'Development Plan Consent Granted (02/04/2020)', 'Development Plan Consent Granted (02/04/2020), Building Rules Consent Granted (05/05/2020)', 'Development Plan Consent Granted (02/04/2020), Building Rules Consent Granted (12/05/2020)', 'Development Plan Consent Granted (02/04/2020), Private Certified Building Rules Consent Granted (08/04/2020)', 'Development Plan Consent Granted (02/06/2020), Building Rules Consent Granted (07/07/2020)', 'Development Plan Consent Granted (02/06/2020), Private Certified Building Rules Consent Granted (04/06/2020)', 'Development Plan Consent Granted (02/06/2020), Private Certified Building Rules Consent Granted (16/06/2020)', 'Development Plan Consent Granted (02/07/2020), Building Rules Consent Granted (10/08/2020)', 'Development Plan Consent Granted (02/07/2020), Building Rules Consent Granted (21/08/2020)', 'Development Plan Consent Granted (02/07/2020), Building Rules Consent Granted (29/07/2020)', 'Development Plan Consent Granted (02/09/2020), Building Rules Consent Granted (24/09/2020)', 'Development Plan Consent Granted (02/09/2020), Building Rules Consent Required', 'Development Plan Consent Granted (02/09/2020), Land Division Consent Granted (02/09/2020)', 'Development Plan Consent Granted (02/09/2020), Private Certified Building Rules Consent Granted (07/09/2020)', 'Development Plan Consent Granted (02/09/2020), Private Certified Building Rules Consent Granted (10/09/2020)', 'Development Plan Consent Granted (02/09/2020), Private Certified Building Rules Consent Granted (16/09/2020)', 'Development Plan Consent Granted (02/09/2020), Private Certified Building Rules Consent Granted (25/10/2020)', 'Development Plan Consent Granted (02/10/2020), Building Rules Consent Granted (03/11/2020)', 'Development Plan Consent Granted (02/10/2020), Building Rules Consent Granted (20/10/2020)', 'Development Plan Consent Granted (02/10/2020), Building Rules Consent Granted (22/10/2020)', 'Development Plan Consent Granted (02/10/2020), Building Rules Consent Granted (23/11/2020)', 'Development Plan Consent Granted (02/10/2020), Building Rules Consent Granted (28/10/2020)', 'Development Plan Consent Granted (02/10/2020), Building Rules Consent Required', 'Development Plan Consent Granted (02/10/2020), Land Division Consent Granted (02/10/2020)', 'Development Plan Consent Granted (02/10/2020), Private Certified Building Rules Consent Granted (12/10/2020)', 'Development Plan Consent Granted (02/10/2020), Private Certified Building Rules Consent Granted (21/10/2020)', 'Development Plan Consent Granted (02/11/2020), Private Certified Building Rules Consent Granted (04/11/2020)', 'Development Plan Consent Granted (02/11/2020), Private Certified Building Rules Consent Granted (06/11/2020)', 'Development Plan Consent Granted (02/11/2020), Private Certified Building Rules Consent Granted (12/11/2020)', 'Development Plan Consent Granted (02/11/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (02/12/2019), Building Rules Consent Granted (10/08/2020)', 'Development Plan Consent Granted (02/12/2019), Building Rules Consent Granted (30/04/2020)', 'Development Plan Consent Granted (03/01/2020), Private Certified Building Rules Consent Granted (30/07/2020)', 'Development Plan Consent Granted (03/02/2020), Private Certified Building Rules Consent Granted (25/02/2020)', 'Development Plan Consent Granted (03/03/2020), Building Rules Consent Granted (16/03/2020)', 'Development Plan Consent Granted (03/03/2020), Private Certified Building Rules Consent Granted (12/03/2020)', 'Development Plan Consent Granted (03/03/2020), Private Certified Building Rules Consent Granted (18/06/2020)', 'Development Plan Consent Granted (03/03/2020), Private Certified Building Rules Consent Granted (20/04/2020)', 'Development Plan Consent Granted (03/03/2020), Private Certified Building Rules Consent Granted (23/03/2020)', 'Development Plan Consent Granted (03/04/2020), Private Certified Building Rules Consent Granted (15/05/2020)', 'Development Plan Consent Granted (03/06/2020), Building Rules Consent Granted (13/10/2020)', 'Development Plan Consent Granted (03/06/2020), Building Rules Consent Granted (24/06/2020)', 'Development Plan Consent Granted (03/06/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (03/07/2020)', 'Development Plan Consent Granted (03/07/2020), Building Rules Consent Granted (07/08/2020)', 'Development Plan Consent Granted (03/08/2020), Building Rules Consent Granted (10/08/2020)', 'Development Plan Consent Granted (03/08/2020), Private Certified Building Rules Consent Granted (07/09/2020)', 'Development Plan Consent Granted (03/08/2020), Private Certified Building Rules Consent Granted (12/08/2020)', 'Development Plan Consent Granted (03/09/2020), Building Rules Consent Granted (02/10/2020)', 'Development Plan Consent Granted (03/09/2020), Building Rules Consent Granted (14/10/2020)', 'Development Plan Consent Granted (03/09/2020), Building Rules Consent Granted (16/11/2020)', 'Development Plan Consent Granted (03/09/2020), Building Rules Consent Granted (23/09/2020)', 'Development Plan Consent Granted (03/09/2020), Building Rules Consent Granted (29/10/2020)', 'Development Plan Consent Granted (03/09/2020), Building Rules Consent Granted (30/09/2020)', 'Development Plan Consent Granted (03/09/2020), Private Certified Building Rules Consent Granted (03/11/2020)', 'Development Plan Consent Granted (03/09/2020), Private Certified Building Rules Consent Granted (08/09/2020)', 'Development Plan Consent Granted (03/09/2020), Private Certified Building Rules Consent Granted (20/10/2020)', 'Development Plan Consent Granted (03/09/2020), Private Certified Building Rules Consent Granted (22/09/2020)', 'Development Plan Consent Granted (03/09/2020), Private Certified Building Rules Consent Granted (29/09/2020)', 'Development Plan Consent Granted (03/09/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (03/10/2020), Private Certified Building Rules Consent Granted (19/11/2020)', 'Development Plan Consent Granted (03/10/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (04/02/2020), Building Rules Consent Granted (07/04/2020)', 'Development Plan Consent Granted (04/02/2020), Building Rules Consent Granted (20/02/2020)', 'Development Plan Consent Granted (04/02/2020), Private Certified Building Rules Consent Granted (10/02/2020)', 'Development Plan Consent Granted (04/02/2020), Private Certified Building Rules Consent Granted (12/02/2020)', 'Development Plan Consent Granted (04/02/2020), Private Certified Building Rules Consent Granted (18/02/2020)', 'Development Plan Consent Granted (04/02/2020), Private Certified Building Rules Consent Granted (19/02/2020)', 'Development Plan Consent Granted (04/02/2020), Private Certified Building Rules Consent Granted (31/03/2020)', 'Development Plan Consent Granted (04/03/2020), Building Rules Consent Granted (16/03/2020)', 'Development Plan Consent Granted (04/03/2020), Building Rules Consent Granted (23/04/2020)', 'Development Plan Consent Granted (04/03/2020), Private Certified Building Rules Consent Granted (10/03/2020)', 'Development Plan Consent Granted (04/03/2020), Private Certified Building Rules Consent Granted (11/05/2020)', 'Development Plan Consent Granted (04/03/2020), Private Certified Building Rules Consent Granted (11/09/2020)', 'Development Plan Consent Granted (04/03/2020), Private Certified Building Rules Consent Granted (19/03/2020)', 'Development Plan Consent Granted (04/05/2020), Private Certified Building Rules Consent Granted (14/05/2020)', 'Development Plan Consent Granted (04/06/2020), Building Rules Consent Granted (11/06/2020)', 'Development Plan Consent Granted (04/06/2020), Building Rules Consent Granted (17/07/2020)', 'Development Plan Consent Granted (04/06/2020), Private Certified Building Rules Consent Granted (09/06/2020)', 'Development Plan Consent Granted (04/06/2020), Private Certified Building Rules Consent Granted (11/06/2020)', 'Development Plan Consent Granted (04/06/2020), Private Certified Building Rules Consent Granted (12/06/2020)', 'Development Plan Consent Granted (04/08/2020), Building Rules Consent Granted (07/09/2020)', 'Development Plan Consent Granted (04/08/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (04/09/2020), Building Rules Consent Granted (05/11/2020)', 'Development Plan Consent Granted (04/09/2020), Building Rules Consent Granted (09/11/2020)', 'Development Plan Consent Granted (04/09/2020), Building Rules Consent Granted (21/10/2020)', 'Development Plan Consent Granted (04/09/2020), Land Division Consent Granted (04/09/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Granted (09/09/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Granted (15/09/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Granted (18/09/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Granted (24/09/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Granted (24/10/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Granted (29/10/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (04/11/2020)', 'Development Plan Consent Granted (04/11/2020), Building Rules Consent Granted (23/11/2020)', 'Development Plan Consent Granted (04/11/2020), Building Rules Consent Required', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (11/11/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (12/11/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (13/11/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (16/11/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (17/11/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (04/12/2019), Private Certified Building Rules Consent Granted (20/12/2020)', 'Development Plan Consent Granted (05/02/2020), Building Rules Consent Granted (20/02/2020)', 'Development Plan Consent Granted (05/02/2020), Building Rules Consent Granted (27/04/2020)', 'Development Plan Consent Granted (05/02/2020), Private Certified Building Rules Consent Granted (10/02/2020)', 'Development Plan Consent Granted (05/02/2020), Private Certified Building Rules Consent Granted (11/02/2020)', 'Development Plan Consent Granted (05/02/2020), Private Certified Building Rules Consent Granted (12/02/2020)', 'Development Plan Consent Granted (05/02/2020), Private Certified Building Rules Consent Granted (13/02/2020)', 'Development Plan Consent Granted (05/02/2020), Private Certified Building Rules Consent Granted (28/02/2020)', 'Development Plan Consent Granted (05/03/2020), Private Certified Building Rules Consent Granted (11/03/2020)', 'Development Plan Consent Granted (05/03/2020), Private Certified Building Rules Consent Granted (12/03/2020)', 'Development Plan Consent Granted (05/03/2020), Private Certified Building Rules Consent Granted (16/03/2020)', 'Development Plan Consent Granted (05/03/2020), Private Certified Building Rules Consent Granted (26/08/2020)', 'Development Plan Consent Granted (05/05/2017), Land Division Consent Required', 'Development Plan Consent Granted (05/05/2020)', 'Development Plan Consent Granted (05/05/2020), Private Certified Building Rules Consent Granted (07/05/2020)', 'Development Plan Consent Granted (05/05/2020), Private Certified Building Rules Consent Granted (17/06/2020)', 'Development Plan Consent Granted (05/05/2020), Private Certified Building Rules Consent Granted (18/06/2020)', 'Development Plan Consent Granted (05/06/2020), Building Rules Consent Granted (19/08/2020)', 'Development Plan Consent Granted (05/06/2020), Private Certified Building Rules Consent Granted (05/06/2020)', 'Development Plan Consent Granted (05/06/2020), Private Certified Building Rules Consent Granted (10/06/2020)', 'Development Plan Consent Granted (05/06/2020), Private Certified Building Rules Consent Granted (13/07/2020)', 'Development Plan Consent Granted (05/06/2020), Private Certified Building Rules Consent Granted (19/06/2020)', 'Development Plan Consent Granted (05/07/2019), Private Certified Building Rules Consent Granted (29/01/2020)', 'Development Plan Consent Granted (05/08/2020), Building Rules Consent Granted (30/09/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (02/09/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (06/08/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (08/09/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (09/10/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (16/09/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (17/09/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (18/09/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (21/08/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (24/10/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (25/09/2020)', 'Development Plan Consent Granted (05/11/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (06/02/2020), Building Rules Consent Granted (20/02/2020)', 'Development Plan Consent Granted (06/02/2020), Private Certified Building Rules Consent Granted (13/03/2020)', 'Development Plan Consent Granted (06/02/2020), Private Certified Building Rules Consent Granted (19/02/2020)', 'Development Plan Consent Granted (06/04/2020), Building Rules Consent Granted (06/05/2020)', 'Development Plan Consent Granted (06/05/2020), Building Rules Consent Granted (11/06/2020)', 'Development Plan Consent Granted (06/05/2020), Private Certified Building Rules Consent Granted (06/05/2020)', 'Development Plan Consent Granted (06/05/2020), Private Certified Building Rules Consent Granted (07/05/2020)', 'Development Plan Consent Granted (06/05/2020), Private Certified Building Rules Consent Granted (08/05/2020)', 'Development Plan Consent Granted (06/05/2020), Private Certified Building Rules Consent Granted (15/06/2020)', 'Development Plan Consent Granted (06/05/2020), Private Certified Building Rules Consent Granted (23/06/2020)', 'Development Plan Consent Granted (06/05/2020), Private Certified Building Rules Consent Granted (24/06/2020)', 'Development Plan Consent Granted (06/07/2020)', 'Development Plan Consent Granted (06/08/2020), Building Rules Consent Granted (17/09/2020)', 'Development Plan Consent Granted (06/08/2020), Building Rules Consent Granted (25/08/2020)', 'Development Plan Consent Granted (06/08/2020), Building Rules Consent Granted (30/09/2020)', 'Development Plan Consent Granted (06/08/2020), Private Certified Building Rules Consent Granted (13/08/2020)', 'Development Plan Consent Granted (06/08/2020), Private Certified Building Rules Consent Granted (18/08/2020)', 'Development Plan Consent Granted (06/08/2020), Private Certified Building Rules Consent Granted (21/08/2020)', 'Development Plan Consent Granted (06/08/2020), Private Certified Building Rules Consent Granted (21/10/2020)', 'Development Plan Consent Granted (06/10/2020), Building Rules Consent Granted (23/10/2020)', 'Development Plan Consent Granted (06/10/2020), Building Rules Consent Granted (29/10/2020)', 'Development Plan Consent Granted (06/10/2020), Private Certified Building Rules Consent Granted (07/10/2020)', 'Development Plan Consent Granted (06/10/2020), Private Certified Building Rules Consent Granted (15/10/2020)', 'Development Plan Consent Granted (06/10/2020), Private Certified Building Rules Consent Granted (17/11/2020)', 'Development Plan Consent Granted (06/11/2020)', 'Development Plan Consent Granted (06/11/2020), Building Rules Consent Required', 'Development Plan Consent Granted (06/11/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (07/02/2020)', 'Development Plan Consent Granted (07/02/2020), Building Rules Consent Granted (20/02/2020)', 'Development Plan Consent Granted (07/02/2020), Private Certified Building Rules Consent Granted (11/02/2020)', 'Development Plan Consent Granted (07/02/2020), Private Certified Building Rules Consent Granted (20/02/2020)', 'Development Plan Consent Granted (07/02/2020), Private Certified Building Rules Consent Granted (24/06/2020)', 'Development Plan Consent Granted (07/02/2020), Private Certified Building Rules Consent Granted (28/02/2020)', 'Development Plan Consent Granted (07/04/2020), Private Certified Building Rules Consent Granted (20/04/2020)', 'Development Plan Consent Granted (07/04/2020), Private Certified Building Rules Consent Granted (23/04/2020)', 'Development Plan Consent Granted (07/05/2020), Building Rules Consent Granted (07/05/2020)', 'Development Plan Consent Granted (07/05/2020), Land Division Consent Granted (07/05/2020)', 'Development Plan Consent Granted (07/05/2020), Private Certified Building Rules Consent Granted (18/05/2020)', 'Development Plan Consent Granted (07/05/2020), Private Certified Building Rules Consent Granted (29/06/2020)', 'Development Plan Consent Granted (07/06/2020), Private Certified Building Rules Consent Granted (10/06/2020)', 'Development Plan Consent Granted (07/08/2020), Building Rules Consent Granted (08/09/2020)', 'Development Plan Consent Granted (07/08/2020), Building Rules Consent Granted (18/09/2020)', 'Development Plan Consent Granted (07/08/2020), Building Rules Consent Granted (21/09/2020)', 'Development Plan Consent Granted (07/08/2020), Building Rules Consent Granted (25/08/2020)', 'Development Plan Consent Granted (07/08/2020), Private Certified Building Rules Consent Granted (02/09/2020)', 'Development Plan Consent Granted (07/08/2020), Private Certified Building Rules Consent Granted (13/08/2020)', 'Development Plan Consent Granted (07/08/2020), Private Certified Building Rules Consent Granted (18/08/2020)', 'Development Plan Consent Granted (07/08/2020), Private Certified Building Rules Consent Granted (29/10/2020)', 'Development Plan Consent Granted (07/09/2020), Building Rules Consent Granted (19/10/2020)', 'Development Plan Consent Granted (07/09/2020), Land Division Consent Granted (07/09/2020)', 'Development Plan Consent Granted (07/09/2020), Private Certified Building Rules Consent Granted (14/10/2020)', 'Development Plan Consent Granted (07/09/2020), Private Certified Building Rules Consent Granted (16/09/2020)', 'Development Plan Consent Granted (07/09/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (07/10/2020), Land Division Consent Granted (07/10/2020)', 'Development Plan Consent Granted (07/10/2020), Private Certified Building Rules Consent Granted (12/10/2020)', 'Development Plan Consent Granted (07/10/2020), Private Certified Building Rules Consent Granted (13/10/2020)', 'Development Plan Consent Granted (07/10/2020), Private Certified Building Rules Consent Granted (16/10/2020)', 'Development Plan Consent Granted (07/10/2020), Private Certified Building Rules Consent Granted (18/11/2020)', 'Development Plan Consent Granted (07/10/2020), Private Certified Building Rules Consent Granted (20/10/2020)', 'Development Plan Consent Granted (07/10/2020), Private Certified Building Rules Consent Granted (21/10/2020)', 'Development Plan Consent Granted (07/10/2020), Private Certified Building Rules Consent Granted (29/10/2020)', 'Development Plan Consent Granted (07/10/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (08/04/2020), Building Rules Consent Granted (06/05/2020)', 'Development Plan Consent Granted (08/04/2020), Land Division Consent Granted (08/04/2020)', 'Development Plan Consent Granted (08/04/2020), Private Certified Building Rules Consent Granted (17/04/2020)', 'Development Plan Consent Granted (08/05/2020)', 'Development Plan Consent Granted (08/05/2020), Building Rules Consent Granted (14/07/2020)', 'Development Plan Consent Granted (08/05/2020), Building Rules Consent Granted (28/05/2020)', 'Development Plan Consent Granted (08/05/2020), Private Certified Building Rules Consent Granted (06/07/2020)', 'Development Plan Consent Granted (08/05/2020), Private Certified Building Rules Consent Granted (10/07/2020)', 'Development Plan Consent Granted (08/05/2020), Private Certified Building Rules Consent Granted (14/05/2020)', 'Development Plan Consent Granted (08/05/2020), Private Certified Building Rules Consent Granted (15/05/2020)', 'Development Plan Consent Granted (08/05/2020), Private Certified Building Rules Consent Granted (16/06/2020)', 'Development Plan Consent Granted (08/05/2020), Private Certified Building Rules Consent Granted (18/05/2020)', 'Development Plan Consent Granted (08/05/2020), Private Certified Building Rules Consent Granted (20/05/2020)', 'Development Plan Consent Granted (08/05/2020), Private Certified Building Rules Consent Granted (22/05/2020)', 'Development Plan Consent Granted (08/05/2020), Private Certified Building Rules Consent Granted (25/06/2020)', 'Development Plan Consent Granted (08/06/2020), Building Rules Consent Granted (01/07/2020)', 'Development Plan Consent Granted (08/06/2020), Private Certified Building Rules Consent Granted (11/06/2020)', 'Development Plan Consent Granted (08/06/2020), Private Certified Building Rules Consent Granted (16/06/2020)', 'Development Plan Consent Granted (08/06/2020), Private Certified Building Rules Consent Granted (22/06/2020)', 'Development Plan Consent Granted (08/06/2020), Private Certified Building Rules Consent Granted (23/06/2020)', 'Development Plan Consent Granted (08/07/2020)', 'Development Plan Consent Granted (08/09/2020), Land Division Consent Granted (08/09/2020)', 'Development Plan Consent Granted (08/10/2020), Building Rules Consent Granted (28/10/2020)', 'Development Plan Consent Granted (08/10/2020), Building Rules Consent Required', 'Development Plan Consent Granted (08/10/2020), Private Certified Building Rules Consent Granted (16/11/2020)', 'Development Plan Consent Granted (08/10/2020), Private Certified Building Rules Consent Granted (21/10/2020)', 'Development Plan Consent Granted (08/10/2020), Private Certified Building Rules Consent Granted (23/10/2020)', 'Development Plan Consent Granted (08</t>
+          <t>['Building Rules Consent Granted (01/05/2020)', 'Building Rules Consent Granted (01/07/2020)', 'Building Rules Consent Granted (01/09/2020)', 'Building Rules Consent Granted (01/10/2020)', 'Building Rules Consent Granted (02/07/2020)', 'Building Rules Consent Granted (02/09/2020)', 'Building Rules Consent Granted (02/11/2020)', 'Building Rules Consent Granted (02/12/2020)', 'Building Rules Consent Granted (03/02/2020)', 'Building Rules Consent Granted (03/03/2020), Development Plan Consent Required', 'Building Rules Consent Granted (03/08/2020)', 'Building Rules Consent Granted (03/11/2020)', 'Building Rules Consent Granted (03/12/2020)', 'Building Rules Consent Granted (04/02/2020)', 'Building Rules Consent Granted (04/06/2020)', 'Building Rules Consent Granted (04/11/2020)', 'Building Rules Consent Granted (04/12/2020)', 'Building Rules Consent Granted (05/02/2020)', 'Building Rules Consent Granted (05/06/2020)', 'Building Rules Consent Granted (05/08/2020)', 'Building Rules Consent Granted (05/11/2020)', 'Building Rules Consent Granted (06/02/2020)', 'Building Rules Consent Granted (06/05/2020)', 'Building Rules Consent Granted (06/07/2020)', 'Building Rules Consent Granted (06/11/2020)', 'Building Rules Consent Granted (07/02/2020)', 'Building Rules Consent Granted (07/04/2020)', 'Building Rules Consent Granted (07/09/2020)', 'Building Rules Consent Granted (07/10/2020)', 'Building Rules Consent Granted (07/10/2020), Development Plan Consent Required', 'Building Rules Consent Granted (07/12/2020)', 'Building Rules Consent Granted (08/07/2020)', 'Building Rules Consent Granted (08/07/2020), Development Plan Consent Required', 'Building Rules Consent Granted (08/09/2020)', 'Building Rules Consent Granted (09/09/2020)', 'Building Rules Consent Granted (09/10/2020)', 'Building Rules Consent Granted (09/12/2020)', 'Building Rules Consent Granted (10/03/2020)', 'Building Rules Consent Granted (10/06/2020)', 'Building Rules Consent Granted (10/08/2020)', 'Building Rules Consent Granted (10/09/2020)', 'Building Rules Consent Granted (10/12/2020)', 'Building Rules Consent Granted (11/02/2020)', 'Building Rules Consent Granted (11/11/2020)', 'Building Rules Consent Granted (12/05/2020)', 'Building Rules Consent Granted (12/06/2020)', 'Building Rules Consent Granted (12/08/2020)', 'Building Rules Consent Granted (12/10/2020)', 'Building Rules Consent Granted (12/11/2020)', 'Building Rules Consent Granted (13/02/2020)', 'Building Rules Consent Granted (13/03/2020)', 'Building Rules Consent Granted (13/07/2020)', 'Building Rules Consent Granted (13/08/2020)', 'Building Rules Consent Granted (13/10/2020)', 'Building Rules Consent Granted (14/04/2020)', 'Building Rules Consent Granted (14/05/2020)', 'Building Rules Consent Granted (14/07/2020)', 'Building Rules Consent Granted (14/12/2020)', 'Building Rules Consent Granted (15/05/2020), Development Plan Consent Required', 'Building Rules Consent Granted (15/07/2020)', 'Building Rules Consent Granted (16/03/2020)', 'Building Rules Consent Granted (16/03/2020), Development Plan Consent Required', 'Building Rules Consent Granted (16/04/2020), Development Plan Consent Required', 'Building Rules Consent Granted (16/09/2020)', 'Building Rules Consent Granted (16/11/2020)', 'Building Rules Consent Granted (16/12/2020)', 'Building Rules Consent Granted (17/01/2020)', 'Building Rules Consent Granted (17/02/2020)', 'Building Rules Consent Granted (17/06/2020)', 'Building Rules Consent Granted (17/08/2020)', 'Building Rules Consent Granted (17/09/2020)', 'Building Rules Consent Granted (17/12/2020)', 'Building Rules Consent Granted (18/09/2020)', 'Building Rules Consent Granted (18/11/2020)', 'Building Rules Consent Granted (18/12/2020)', 'Building Rules Consent Granted (19/02/2020)', 'Building Rules Consent Granted (19/03/2020)', 'Building Rules Consent Granted (19/08/2020)', 'Building Rules Consent Granted (19/11/2020)', 'Building Rules Consent Granted (20/02/2020)', 'Building Rules Consent Granted (20/10/2020)', 'Building Rules Consent Granted (21/04/2020)', 'Building Rules Consent Granted (21/05/2020)', 'Building Rules Consent Granted (21/05/2020), Development Plan Consent Required', 'Building Rules Consent Granted (21/07/2020)', 'Building Rules Consent Granted (21/09/2020)', 'Building Rules Consent Granted (21/12/2020)', 'Building Rules Consent Granted (22/04/2020)', 'Building Rules Consent Granted (22/07/2020)', 'Building Rules Consent Granted (22/10/2020)', 'Building Rules Consent Granted (23/03/2020)', 'Building Rules Consent Granted (23/06/2020)', 'Building Rules Consent Granted (23/10/2020)', 'Building Rules Consent Granted (23/11/2020)', 'Building Rules Consent Granted (23/12/2020)', 'Building Rules Consent Granted (24/04/2020)', 'Building Rules Consent Granted (24/06/2020)', 'Building Rules Consent Granted (24/07/2020)', 'Building Rules Consent Granted (24/11/2020)', 'Building Rules Consent Granted (25/02/2020)', 'Building Rules Consent Granted (25/06/2020)', 'Building Rules Consent Granted (25/11/2020)', 'Building Rules Consent Granted (26/03/2020)', 'Building Rules Consent Granted (26/05/2020)', 'Building Rules Consent Granted (26/06/2020)', 'Building Rules Consent Granted (26/08/2020)', 'Building Rules Consent Granted (27/02/2020)', 'Building Rules Consent Granted (27/04/2020)', 'Building Rules Consent Granted (27/05/2020)', 'Building Rules Consent Granted (27/08/2020)', 'Building Rules Consent Granted (27/10/2020)', 'Building Rules Consent Granted (27/11/2020)', 'Building Rules Consent Granted (28/01/2020)', 'Building Rules Consent Granted (28/05/2020)', 'Building Rules Consent Granted (28/10/2020)', 'Building Rules Consent Granted (29/05/2020)', 'Building Rules Consent Granted (29/07/2020)', 'Building Rules Consent Granted (29/09/2020)', 'Building Rules Consent Granted (29/10/2020)', 'Building Rules Consent Granted (30/09/2020)', 'Building Rules Consent Granted (30/10/2020)', 'Building Rules Consent Granted (31/03/2020)', 'Building Rules Consent Required', 'Building Rules Consent Required, Development Plan Consent Required', 'Development Application Withdrawn (01/09/2020), Private Certified Building Rules Consent Required', 'Development Application Withdrawn (01/12/2020), Development Application Withdrawn (01/12/2020)', 'Development Application Withdrawn (02/09/2020), Development Application Withdrawn (02/09/2020)', 'Development Application Withdrawn (03/03/2020), Development Application Withdrawn (03/03/2020)', 'Development Application Withdrawn (06/02/2020), Development Application Withdrawn (06/02/2020)', 'Development Application Withdrawn (08/04/2020)', 'Development Application Withdrawn (08/12/2020), Private Certified Building Rules Consent Required', 'Development Application Withdrawn (11/09/2020)', 'Development Application Withdrawn (11/09/2020), Development Application Withdrawn (11/09/2020)', 'Development Application Withdrawn (11/11/2020), Development Application Withdrawn (11/11/2020)', 'Development Application Withdrawn (12/10/2020)', 'Development Application Withdrawn (14/04/2020)', 'Development Application Withdrawn (14/12/2020), Building Rules Consent Required', 'Development Application Withdrawn (14/12/2020), Development Application Withdrawn (14/12/2020)', 'Development Application Withdrawn (15/01/2020)', 'Development Application Withdrawn (16/09/2020), Development Application Withdrawn (16/09/2020)', 'Development Application Withdrawn (16/12/2020), Development Application Withdrawn (16/12/2020)', 'Development Application Withdrawn (17/07/2020)', 'Development Application Withdrawn (21/09/2020)', 'Development Application Withdrawn (22/07/2020), Development Application Withdrawn (22/07/2020)', 'Development Application Withdrawn (23/07/2020), Development Application Withdrawn (23/07/2020)', 'Development Application Withdrawn (23/09/2020)', 'Development Application Withdrawn (24/04/2020)', 'Development Application Withdrawn (25/05/2020)', 'Development Application Withdrawn (25/11/2020)', 'Development Application Withdrawn (26/11/2020), Development Application Withdrawn (26/11/2020)', 'Development Application Withdrawn (28/02/2020)', 'Development Application Withdrawn (29/07/2020), Development Application Withdrawn (29/07/2020)', 'Development Application Withdrawn (30/09/2020)', 'Development Plan Consent Granted (01/04/2020), Building Rules Consent Granted (11/06/2020)', 'Development Plan Consent Granted (01/04/2020), Building Rules Consent Required', 'Development Plan Consent Granted (01/06/2007), Building Rules Consent Granted (05/12/2007), Building Rules Consent Granted (29/05/2008), Development Plan Consent Granted (29/09/2020)', 'Development Plan Consent Granted (01/06/2020), Private Certified Building Rules Consent Granted (26/06/2020)', 'Development Plan Consent Granted (01/09/2020), Building Rules Consent Granted (03/09/2020)', 'Development Plan Consent Granted (01/09/2020), Building Rules Consent Granted (11/09/2020)', 'Development Plan Consent Granted (01/09/2020), Building Rules Consent Granted (20/10/2020)', 'Development Plan Consent Granted (01/09/2020), Private Certified Building Rules Consent Granted (06/10/2020)', 'Development Plan Consent Granted (01/09/2020), Private Certified Building Rules Consent Granted (07/09/2020)', 'Development Plan Consent Granted (01/09/2020), Private Certified Building Rules Consent Granted (09/10/2020)', 'Development Plan Consent Granted (01/09/2020), Private Certified Building Rules Consent Granted (13/09/2020)', 'Development Plan Consent Granted (01/09/2020), Private Certified Building Rules Consent Granted (17/10/2020)', 'Development Plan Consent Granted (01/10/2020), Building Rules Consent Granted (02/10/2020)', 'Development Plan Consent Granted (01/10/2020), Building Rules Consent Granted (03/11/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Granted (03/12/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Granted (07/10/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Granted (08/10/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Granted (16/10/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Granted (22/10/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Granted (23/10/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Granted (25/11/2020)', 'Development Plan Consent Granted (01/10/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (01/12/2020), Private Certified Building Rules Consent Granted (01/12/2020)', 'Development Plan Consent Granted (01/12/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (02/03/2020)', 'Development Plan Consent Granted (02/04/2020)', 'Development Plan Consent Granted (02/04/2020), Building Rules Consent Granted (05/05/2020)', 'Development Plan Consent Granted (02/04/2020), Building Rules Consent Granted (12/05/2020)', 'Development Plan Consent Granted (02/04/2020), Private Certified Building Rules Consent Granted (08/04/2020)', 'Development Plan Consent Granted (02/06/2020), Building Rules Consent Granted (07/07/2020)', 'Development Plan Consent Granted (02/06/2020), Private Certified Building Rules Consent Granted (04/06/2020)', 'Development Plan Consent Granted (02/06/2020), Private Certified Building Rules Consent Granted (16/06/2020)', 'Development Plan Consent Granted (02/07/2020), Building Rules Consent Granted (10/08/2020)', 'Development Plan Consent Granted (02/07/2020), Building Rules Consent Granted (21/08/2020)', 'Development Plan Consent Granted (02/07/2020), Building Rules Consent Granted (29/07/2020)', 'Development Plan Consent Granted (02/09/2020), Building Rules Consent Granted (24/09/2020)', 'Development Plan Consent Granted (02/09/2020), Building Rules Consent Required', 'Development Plan Consent Granted (02/09/2020), Land Division Consent Granted (02/09/2020)', 'Development Plan Consent Granted (02/09/2020), Private Certified Building Rules Consent Granted (07/09/2020)', 'Development Plan Consent Granted (02/09/2020), Private Certified Building Rules Consent Granted (10/09/2020)', 'Development Plan Consent Granted (02/09/2020), Private Certified Building Rules Consent Granted (16/09/2020)', 'Development Plan Consent Granted (02/09/2020), Private Certified Building Rules Consent Granted (25/10/2020)', 'Development Plan Consent Granted (02/10/2020), Building Rules Consent Granted (03/11/2020)', 'Development Plan Consent Granted (02/10/2020), Building Rules Consent Granted (20/10/2020)', 'Development Plan Consent Granted (02/10/2020), Building Rules Consent Granted (22/10/2020)', 'Development Plan Consent Granted (02/10/2020), Building Rules Consent Granted (23/11/2020)', 'Development Plan Consent Granted (02/10/2020), Building Rules Consent Granted (28/10/2020)', 'Development Plan Consent Granted (02/10/2020), Building Rules Consent Required', 'Development Plan Consent Granted (02/10/2020), Land Division Consent Granted (02/10/2020)', 'Development Plan Consent Granted (02/10/2020), Private Certified Building Rules Consent Granted (12/10/2020)', 'Development Plan Consent Granted (02/10/2020), Private Certified Building Rules Consent Granted (21/10/2020)', 'Development Plan Consent Granted (02/11/2020), Private Certified Building Rules Consent Granted (04/11/2020)', 'Development Plan Consent Granted (02/11/2020), Private Certified Building Rules Consent Granted (04/12/2020)', 'Development Plan Consent Granted (02/11/2020), Private Certified Building Rules Consent Granted (06/11/2020)', 'Development Plan Consent Granted (02/11/2020), Private Certified Building Rules Consent Granted (12/11/2020)', 'Development Plan Consent Granted (02/11/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (02/12/2019), Building Rules Consent Granted (10/08/2020)', 'Development Plan Consent Granted (02/12/2019), Building Rules Consent Granted (30/04/2020)', 'Development Plan Consent Granted (02/12/2020), Private Certified Building Rules Consent Granted (03/12/2020)', 'Development Plan Consent Granted (02/12/2020), Private Certified Building Rules Consent Granted (10/12/2020)', 'Development Plan Consent Granted (02/12/2020), Private Certified Building Rules Consent Granted (18/12/2020)', 'Development Plan Consent Granted (02/12/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (03/01/2020), Private Certified Building Rules Consent Granted (30/07/2020)', 'Development Plan Consent Granted (03/02/2020), Private Certified Building Rules Consent Granted (25/02/2020)', 'Development Plan Consent Granted (03/03/2020), Building Rules Consent Granted (16/03/2020)', 'Development Plan Consent Granted (03/03/2020), Private Certified Building Rules Consent Granted (12/03/2020)', 'Development Plan Consent Granted (03/03/2020), Private Certified Building Rules Consent Granted (18/06/2020)', 'Development Plan Consent Granted (03/03/2020), Private Certified Building Rules Consent Granted (20/04/2020)', 'Development Plan Consent Granted (03/03/2020), Private Certified Building Rules Consent Granted (23/03/2020)', 'Development Plan Consent Granted (03/04/2020), Private Certified Building Rules Consent Granted (15/05/2020)', 'Development Plan Consent Granted (03/06/2020), Building Rules Consent Granted (13/10/2020)', 'Development Plan Consent Granted (03/06/2020), Building Rules Consent Granted (24/06/2020)', 'Development Plan Consent Granted (03/06/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (03/07/2020)', 'Development Plan Consent Granted (03/07/2020), Building Rules Consent Granted (07/08/2020)', 'Development Plan Consent Granted (03/08/2020), Building Rules Consent Granted (10/08/2020)', 'Development Plan Consent Granted (03/08/2020), Private Certified Building Rules Consent Granted (07/09/2020)', 'Development Plan Consent Granted (03/08/2020), Private Certified Building Rules Consent Granted (12/08/2020)', 'Development Plan Consent Granted (03/09/2020), Building Rules Consent Granted (02/10/2020)', 'Development Plan Consent Granted (03/09/2020), Building Rules Consent Granted (14/10/2020)', 'Development Plan Consent Granted (03/09/2020), Building Rules Consent Granted (16/11/2020)', 'Development Plan Consent Granted (03/09/2020), Building Rules Consent Granted (23/09/2020)', 'Development Plan Consent Granted (03/09/2020), Building Rules Consent Granted (29/10/2020)', 'Development Plan Consent Granted (03/09/2020), Building Rules Consent Granted (30/09/2020)', 'Development Plan Consent Granted (03/09/2020), Private Certified Building Rules Consent Granted (03/11/2020)', 'Development Plan Consent Granted (03/09/2020), Private Certified Building Rules Consent Granted (08/09/2020)', 'Development Plan Consent Granted (03/09/2020), Private Certified Building Rules Consent Granted (20/10/2020)', 'Development Plan Consent Granted (03/09/2020), Private Certified Building Rules Consent Granted (22/09/2020)', 'Development Plan Consent Granted (03/09/2020), Private Certified Building Rules Consent Granted (29/09/2020)', 'Development Plan Consent Granted (03/09/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (03/10/2020), Private Certified Building Rules Consent Granted (19/11/2020)', 'Development Plan Consent Granted (03/10/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (03/12/2020), Building Rules Consent Granted (18/12/2020)', 'Development Plan Consent Granted (03/12/2020), Building Rules Consent Required', 'Development Plan Consent Granted (03/12/2020), Private Certified Building Rules Consent Granted (08/12/2020)', 'Development Plan Consent Granted (03/12/2020), Private Certified Building Rules Consent Granted (09/12/2020)', 'Development Plan Consent Granted (03/12/2020), Private Certified Building Rules Consent Granted (11/12/2020)', 'Development Plan Consent Granted (03/12/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (04/02/2020), Building Rules Consent Granted (07/04/2020)', 'Development Plan Consent Granted (04/02/2020), Building Rules Consent Granted (20/02/2020)', 'Development Plan Consent Granted (04/02/2020), Private Certified Building Rules Consent Granted (10/02/2020)', 'Development Plan Consent Granted (04/02/2020), Private Certified Building Rules Consent Granted (12/02/2020)', 'Development Plan Consent Granted (04/02/2020), Private Certified Building Rules Consent Granted (18/02/2020)', 'Development Plan Consent Granted (04/02/2020), Private Certified Building Rules Consent Granted (19/02/2020)', 'Development Plan Consent Granted (04/02/2020), Private Certified Building Rules Consent Granted (31/03/2020)', 'Development Plan Consent Granted (04/03/2020), Building Rules Consent Granted (16/03/2020)', 'Development Plan Consent Granted (04/03/2020), Building Rules Consent Granted (23/04/2020)', 'Development Plan Consent Granted (04/03/2020), Private Certified Building Rules Consent Granted (10/03/2020)', 'Development Plan Consent Granted (04/03/2020), Private Certified Building Rules Consent Granted (11/05/2020)', 'Development Plan Consent Granted (04/03/2020), Private Certified Building Rules Consent Granted (11/09/2020)', 'Development Plan Consent Granted (04/03/2020), Private Certified Building Rules Consent Granted (19/03/2020)', 'Development Plan Consent Granted (04/05/2020), Private Certified Building Rules Consent Granted (14/05/2020)', 'Development Plan Consent Granted (04/06/2020), Building Rules Consent Granted (11/06/2020)', 'Development Plan Consent Granted (04/06/2020), Building Rules Consent Granted (17/07/2020)', 'Development Plan Consent Granted (04/06/2020), Private Certified Building Rules Consent Granted (09/06/2020)', 'Development Plan Consent Granted (04/06/2020), Private Certified Building Rules Consent Granted (11/06/2020)', 'Development Plan Consent Granted (04/06/2020), Private Certified Building Rules Consent Granted (12/06/2020)', 'Development Plan Consent Granted (04/08/2020), Building Rules Consent Granted (07/09/2020)', 'Development Plan Consent Granted (04/08/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (04/09/2020), Building Rules Consent Granted (05/11/2020)', 'Development Plan Consent Granted (04/09/2020), Building Rules Consent Granted (09/11/2020)', 'Development Plan Consent Granted (04/09/2020), Building Rules Consent Granted (21/10/2020)', 'Development Plan Consent Granted (04/09/2020), Land Division Consent Granted (04/09/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Granted (09/09/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Granted (15/09/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Granted (18/09/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Granted (24/09/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Granted (24/10/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Granted (29/10/2020)', 'Development Plan Consent Granted (04/09/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (04/11/2020), Building Rules Consent Granted (02/12/2020)', 'Development Plan Consent Granted (04/11/2020), Building Rules Consent Granted (14/12/2020)', 'Development Plan Consent Granted (04/11/2020), Building Rules Consent Granted (23/11/2020)', 'Development Plan Consent Granted (04/11/2020), Building Rules Consent Granted (30/11/2020)', 'Development Plan Consent Granted (04/11/2020), Building Rules Consent Required', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (07/12/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (11/11/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (12/11/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (13/11/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (13/12/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (14/12/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (16/11/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (17/11/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (17/12/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Granted (30/11/2020)', 'Development Plan Consent Granted (04/11/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (04/12/2019), Private Certified Building Rules Consent Granted (20/12/2020)', 'Development Plan Consent Granted (05/02/2020), Building Rules Consent Granted (20/02/2020)', 'Development Plan Consent Granted (05/02/2020), Building Rules Consent Granted (27/04/2020)', 'Development Plan Consent Granted (05/02/2020), Private Certified Building Rules Consent Granted (10/02/2020)', 'Development Plan Consent Granted (05/02/2020), Private Certified Building Rules Consent Granted (11/02/2020)', 'Development Plan Consent Granted (05/02/2020), Private Certified Building Rules Consent Granted (12/02/2020)', 'Development Plan Consent Granted (05/02/2020), Private Certified Building Rules Consent Granted (13/02/2020)', 'Development Plan Consent Granted (05/02/2020), Private Certified Building Rules Consent Granted (28/02/2020)', 'Development Plan Consent Granted (05/03/2020), Private Certified Building Rules Consent Granted (11/03/2020)', 'Development Plan Consent Granted (05/03/2020), Private Certified Building Rules Consent Granted (12/03/2020)', 'Development Plan Consent Granted (05/03/2020), Private Certified Building Rules Consent Granted (16/03/2020)', 'Development Plan Consent Granted (05/03/2020), Private Certified Building Rules Consent Granted (26/08/2020)', 'Development Plan Consent Granted (05/05/2017), Land Division Consent Required', 'Development Plan Consent Granted (05/05/2020)', 'Development Plan Consent Granted (05/05/2020), Private Certified Building Rules Consent Granted (07/05/2020)', 'Development Plan Consent Granted (05/05/2020), Private Certified Building Rules Consent Granted (17/06/2020)', 'Development Plan Consent Granted (05/05/2020), Private Certified Building Rules Consent Granted (18/06/2020)', 'Development Plan Consent Granted (05/06/2020), Building Rules Consent Granted (19/08/2020)', 'Development Plan Consent Granted (05/06/2020), Private Certified Building Rules Consent Granted (05/06/2020)', 'Development Plan Consent Granted (05/06/2020), Private Certified Building Rules Consent Granted (10/06/2020)', 'Development Plan Consent Granted (05/06/2020), Private Certified Building Rules Consent Granted (13/07/2020)', 'Development Plan Consent Granted (05/06/2020), Private Certified Building Rules Consent Granted (19/06/2020)', 'Development Plan Consent Granted (05/07/2019), Private Certified Building Rules Consent Granted (29/01/2020)', 'Development Plan Consent Granted (05/08/2020), Building Rules Consent Granted (30/09/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (02/09/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (06/08/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (08/09/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (09/10/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (16/09/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (17/09/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (18/09/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (21/08/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (24/10/2020)', 'Development Plan Consent Granted (05/08/2020), Private Certified Building Rules Consent Granted (25/09/2020)', 'Development Plan Consent Granted (05/11/2020), Private Certified Building Rules Consent Granted (10/12/2020)', 'Development Plan Consent Granted (05/11/2020), Private Certified Building Rules Consent Granted (15/12/2020)', 'Development Plan Consent Granted (05/11/2020), Private Certified Building Rules Consent Granted (16/12/2020)', 'Development Plan Consent Granted (05/11/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (06/02/2020), Building Rules Consent Granted (20/02/2020)', 'Development Plan Consent Granted (06/02/2020), Private Certified Building Rules Consent Granted (13/03/2020)', 'Development Plan Consent Granted (06/02/2020), Private Certified Building Rules Consent Granted (19/02/2020)', 'Development Plan Consent Granted (06/04/2020), Building Rules Consent Granted (06/05/2020)', 'Development Plan Consent Granted (06/05/2020), Building Rules Consent Granted (11/06/2020)', 'Development Plan Consent Granted (06/05/2020), Private Certified Building Rules Consent Granted (06/05/2020)', 'Development Plan Consent Granted (06/05/2020), Private Certified Building Rules Consent Granted (07/05/2020)', 'Development Plan Consent Granted (06/05/2020), Private Certified Building Rules Consent Granted (08/05/2020)', 'Development Plan Consent Granted (06/05/2020), Private Certified Building Rules Consent Granted (15/06/2020)', 'Development Plan Consent Granted (06/05/2020), Private Certified Building Rules Consent Granted (23/06/2020)', 'Development Plan Consent Granted (06/05/2020), Private Certified Building Rules Consent Granted (24/06/2020)', 'Development Plan Consent Granted (06/07/2020)', 'Development Plan Consent Granted (06/08/2020), Building Rules Consent Granted (17/09/2020)', 'Development Plan Consent Granted (06/08/2020), Building Rules Consent Granted (25/08/2020)', 'Development Plan Consent Granted (06/08/2020), Building Rules Consent Granted (30/09/2020)', 'Development Plan Consent Granted (06/08/2020), Private Certified Building Rules Consent Granted (13/08/2020)', 'Development Plan Consent Granted (06/08/2020), Private Certified Building Rules Consent Granted (18/08/2020)', 'Development Plan Consent Granted (06/08/2020), Private Certified Building Rules Consent Granted (21/08/2020)', 'Development Plan Consent Granted (06/08/2020), Private Certified Building Rules Consent Granted (21/10/2020)', 'Development Plan Consent Granted (06/10/2020), Building Rules Consent Granted (23/10/2020)', 'Development Plan Consent Granted (06/10/2020), Building Rules Consent Granted (29/10/2020)', 'Development Plan Consent Granted (06/10/2020), Private Certified Building Rules Consent Granted (07/10/2020)', 'Development Plan Consent Granted (06/10/2020), Private Certified Building Rules Consent Granted (15/10/2020)', 'Development Plan Consent Granted (06/10/2020), Private Certified Building Rules Consent Granted (17/11/2020)', 'Development Plan Consent Granted (06/11/2020)', 'Development Plan Consent Granted (06/11/2020), Building Rules Consent Granted (09/12/2020)', 'Development Plan Consent Granted (06/11/2020), Private Certified Building Rules Consent Required', 'Development Plan Consent Granted (07/02/2020)', 'Development Plan Consent Granted (07/02/2020), Building Rules Consent Granted (20/02/2020)', 'Development Plan Consent Granted (07/02/2020), Private Certified Building Rules Consent Granted (11/02/2020)', 'Development Plan Consent Granted (07/02/2020), Private Certified Building Rules Consent Granted (20/02/2020)', 'Development Plan Consent Granted (07/02/2020), Private Certified Building Rules Consent Granted (24/06/2020)', 'Development Plan Consent Granted (07/02/2020), Private Certified Building Rules Consent Granted (28/02/2020)', 'Development Plan Consent Granted (07/04/2020), Private Certified Building Rules Consent Granted (20/04/2020)', 'Development Plan Consent Granted (07/04/2020), Private Certified Building Rules Consent Granted (23/04/2020)', 'Development Plan Consent Granted (07/05/2020), Building Rules Consent Granted (07/05/2020)', 'Development Plan Consent Granted (07/05/2020), Land Division Consent Granted (07/05/2020)', 'Development Plan Consent Granted (07/05/2020), Private Certified Building Rules Consent Granted (18/05/2020)', 'Development Plan Consent Granted (07/05/2020), Private Certified Building Rules Consent Granted (29/06/2020)', 'Development Plan Consent Granted (07/06/2020), Private Certified Building Rules Consent Granted (10/06/2020)', 'Development Plan Consent Granted (07/08/2020), Building Rules Consent Granted (08/09/2020)', 'Development Plan Consent Granted (07/08/2020), Building Rules Consent Granted (18/09/2020)', 'Development Plan Consent Granted (07/08/2020), Building Rules Consent Granted (21/09/2020)', 'Development Plan Consent Granted (07/08/2020), Building Rules Consent Granted (25/08/2020)', 'Development Plan Consent Granted (07/08/2020), Private Certified Building Rules Consent Granted (02/09/2020)', 'Development Plan Consent Granted (07/08/2020), Private Certified Building Rules Consent Granted (13/08/2020)', 'Development Plan Consent Granted (07/08/2020), Private Certified Building Rules Consent Granted (18/08/2020)', 'Development Plan Consent Granted (07/08/2020), Private Certified Building Rules Consent Granted (29/10/2020)', 'Development Plan Consent Granted (07/09/2020), Building Rules Consent Granted (19/10/2020)', 'Development Plan Consent Granted (07/09/2020), Land Division Consent Granted (07/09/2020)', 'Development Plan Consent Granted (07/09/2020), Private Certified Building Rules Consent Granted (14/10/2020)', 'Development Plan Consent Granted (07/09/2020), Private Certified Building Rules Consent Granted (16/09/2020)', 'Development Plan Consent Gr</t>
         </is>
       </c>
     </row>
@@ -2735,7 +2735,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="O26" t="n">
-        <v>1480</v>
+        <v>1639</v>
       </c>
       <c r="P26" t="n">
         <v>0</v>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>Salisbury Development Services and Katnich Dodd</t>
+          <t>BCA Concepts</t>
         </is>
       </c>
       <c r="T26" t="n">
@@ -2791,20 +2791,20 @@
       </c>
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="n">
-        <v>1480</v>
+        <v>1639</v>
       </c>
       <c r="W26" t="n">
         <v>0</v>
       </c>
       <c r="X26" t="n">
-        <v>27711</v>
+        <v>31426</v>
       </c>
       <c r="Y26" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>['B S G M Consulting Building Surveyors', 'Bdc', 'Bdc and Building Development Certifier', 'Blueprint Certifiers &amp; Designers Pty Ltd', 'Building Certification Approvals (SA) Pty Ltd', 'Building Development Certifier', 'Building Rules Consent Private Certifiers Pty Ltd', 'Buildsurv', 'Carlo Scinto &amp; Assoc Pty Ltd', 'George Capetanakis Building Surveyor', 'Giordano Certification', 'Hendry Group', 'KBS Consultants', 'KBS Consultants and \nProfessional Building Services Aust Pty Ltd', 'KBS Consultants and Salisbury Development Services', 'Katnich Dodd', 'Ms B Douflias', 'Nikias Certification', 'P B S Aust', 'Professional Building Services Aust Pty Ltd', 'Professional Building Services Aust Pty Ltd and \nP B S Aust', 'Project Building Certifiers Pty Ltd', 'SA Building Approvals &amp; Consultants', 'Salisbury Development Services', 'Salisbury Development Services and \nBuilding Certification Approvals (SA) Pty Ltd', 'Salisbury Development Services and Katnich Dodd', 'Softwoods Timberyards Pty Ltd', 'Tecon Aust Pty Ltd', 'Tonkin Consulting', 'Trento Fuller Pty Ltd', 'Urban Planning &amp; Design', 'Willmott Building Certification']</t>
+          <t>['B S G M Consulting Building Surveyors', 'BCA Concepts', 'Bdc', 'Bdc and Building Development Certifier', 'Blueprint Certifiers &amp; Designers Pty Ltd', 'Building Certification Approvals (SA) Pty Ltd', 'Building Development Certifier', 'Building Rules Consent Private Certifiers Pty Ltd', 'Buildsurv', 'Carlo Scinto &amp; Assoc Pty Ltd', 'George Capetanakis Building Surveyor', 'Giordano Certification', 'Hendry Group', 'KBS Consultants', 'KBS Consultants and \nProfessional Building Services Aust Pty Ltd', 'KBS Consultants and Salisbury Development Services', 'Katnich Dodd', 'Mr R Ciancio', 'Ms B Douflias', 'Nikias Certification', 'P B S Aust', 'Professional Building Services Aust Pty Ltd', 'Professional Building Services Aust Pty Ltd and \nP B S Aust', 'Project Building Certifiers Pty Ltd', 'SA Building Approvals &amp; Consultants', 'Salisbury Development Services', 'Salisbury Development Services and \nBuilding Certification Approvals (SA) Pty Ltd', 'Softwoods Timberyards Pty Ltd', 'Tecon Aust Pty Ltd', 'Tonkin Consulting', 'Trento Fuller Pty Ltd', 'Urban Planning &amp; Design', 'Willmott Building Certification']</t>
         </is>
       </c>
     </row>
@@ -2823,7 +2823,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -2856,7 +2856,7 @@
         <v>0</v>
       </c>
       <c r="O27" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="P27" t="n">
         <v>0</v>
@@ -2871,11 +2871,11 @@
       </c>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="W27" t="n">
         <v>0</v>
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
@@ -2940,7 +2940,7 @@
         <v>0</v>
       </c>
       <c r="O28" t="n">
-        <v>1787</v>
+        <v>1968</v>
       </c>
       <c r="P28" t="n">
         <v>0</v>
@@ -2955,7 +2955,7 @@
       </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>23/11/2020 3:33:42 PM</t>
+          <t>10/12/2020 9:55:58 AM</t>
         </is>
       </c>
       <c r="T28" t="n">
@@ -2963,20 +2963,20 @@
       </c>
       <c r="U28" t="inlineStr"/>
       <c r="V28" t="n">
-        <v>1787</v>
+        <v>1968</v>
       </c>
       <c r="W28" t="n">
         <v>0</v>
       </c>
       <c r="X28" t="n">
-        <v>17120</v>
+        <v>19880</v>
       </c>
       <c r="Y28" t="n">
-        <v>789</v>
+        <v>919</v>
       </c>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>['1/05/2020 2:15:32 PM', '1/06/2020 10:01:54 AM', '1/06/2020 11:25:01 AM', '1/06/2020 11:27:17 AM', '1/06/2020 11:28:43 AM', '1/07/2020 11:38:37 AM', '1/07/2020 11:42:37 AM', '1/07/2020 11:58:55 AM', '1/07/2020 12:00:19 PM', '1/07/2020 12:02:16 PM', '1/07/2020 12:03:44 PM', '1/07/2020 4:50:05 PM', '1/09/2020 9:34:20 AM', '1/09/2020 9:43:55 AM', '1/10/2020 10:28:10 AM', '1/10/2020 12:45:38 PM', '1/10/2020 1:43:16 PM', '1/10/2020 4:38:00 PM', '10/02/2020 11:06:40 AM', '10/02/2020 4:46:19 PM', '10/02/2020 4:47:35 PM', '10/03/2020 10:06:32 AM', '10/03/2020 9:08:28 AM', '10/03/2020 9:57:02 AM', '10/06/2020 3:19:37 PM', '10/07/2020 11:11:39 AM', '10/07/2020 11:19:59 AM', '10/07/2020 2:09:18 PM', '10/08/2020 10:20:57 AM', '10/08/2020 10:25:40 AM', '10/08/2020 10:30:56 AM', '10/08/2020 10:42:07 AM', '10/08/2020 10:43:30 AM', '10/08/2020 12:00:27 PM', '10/08/2020 12:11:40 PM', '10/08/2020 9:31:56 AM', '10/11/2020 4:57:42 PM', '10/11/2020 5:04:27 PM', '10/11/2020 5:05:46 PM', '10/11/2020 5:07:08 PM', '10/11/2020 5:17:57 PM', '11/03/2020 1:42:50 PM', '11/03/2020 8:51:56 AM', '11/03/2020 8:52:43 AM', '11/05/2020 9:48:12 AM', '11/05/2020 9:48:48 AM', '11/06/2020 10:03:25 AM', '11/06/2020 10:05:06 AM', '11/06/2020 10:26:37 AM', '11/06/2020 12:56:07 PM', '11/06/2020 5:31:16 PM', '11/08/2020 10:26:42 AM', '11/08/2020 10:27:40 AM', '11/08/2020 11:43:35 AM', '11/08/2020 11:44:07 AM', '11/09/2020 10:12:19 AM', '11/09/2020 9:53:11 AM', '11/09/2020 9:58:09 AM', '11/11/2020 10:43:39 AM', '12/05/2020 4:22:31 PM', '12/06/2020 2:05:22 PM', '12/06/2020 8:05:04 AM', '12/08/2020 5:14:39 PM', '12/08/2020 5:17:57 PM', '12/10/2020 10:47:56 AM', '12/10/2020 11:09:05 AM', '12/10/2020 11:10:15 AM', '12/10/2020 11:11:50 AM', '12/10/2020 11:12:59 AM', '12/10/2020 11:14:15 AM', '12/10/2020 11:15:46 AM', '12/10/2020 11:16:57 AM', '12/10/2020 11:18:05 AM', '12/10/2020 11:32:36 AM', '12/10/2020 3:44:41 PM', '13/02/2020 11:01:00 AM', '13/05/2020 10:50:49 AM', '13/05/2020 10:51:46 AM', '13/05/2020 12:00:00 AM', '13/07/2020 10:45:28 AM', '13/10/2020 10:58:33 AM', '13/10/2020 10:59:55 AM', '13/10/2020 11:01:02 AM', '13/10/2020 11:07:30 AM', '13/10/2020 11:08:31 AM', '13/10/2020 11:10:13 AM', '13/10/2020 11:12:22 AM', '13/10/2020 11:14:22 AM', '13/10/2020 11:15:41 AM', '13/10/2020 11:21:10 AM', '13/10/2020 11:22:37 AM', '13/10/2020 11:23:32 AM', '13/10/2020 11:26:05 AM', '13/10/2020 12:14:15 PM', '13/10/2020 5:11:31 PM', '13/10/2020 9:58:52 AM', '13/11/2020 10:57:23 AM', '13/11/2020 9:25:17 AM', '13/11/2020 9:32:31 AM', '13/11/2020 9:37:32 AM', '13/11/2020 9:47:49 AM', '14/02/2020 11:53:21 AM', '14/04/2020 10:56:28 AM', '14/04/2020 3:25:38 PM', '14/04/2020 3:59:27 PM', '14/04/2020 4:00:14 PM', '14/07/2020 10:07:53 AM', '14/07/2020 10:11:29 AM', '14/07/2020 10:24:24 AM', '14/07/2020 10:27:19 AM', '14/07/2020 10:29:28 AM', '14/07/2020 10:31:23 AM', '14/07/2020 10:33:12 AM', '14/07/2020 10:34:52 AM', '14/07/2020 10:36:17 AM', '14/07/2020 10:38:38 AM', '14/07/2020 10:40:14 AM', '14/07/2020 10:41:50 AM', '14/07/2020 10:43:19 AM', '14/07/2020 10:47:23 AM', '14/07/2020 10:49:05 AM', '14/07/2020 10:50:49 AM', '14/07/2020 11:41:49 AM', '14/07/2020 5:12:52 PM', '14/07/2020 5:20:49 PM', '14/07/2020 9:09:12 AM', '14/09/2020 10:16:21 AM', '14/09/2020 10:34:58 AM', '14/09/2020 10:36:07 AM', '14/09/2020 10:37:13 AM', '14/09/2020 10:38:37 AM', '14/09/2020 1:56:35 PM', '14/09/2020 1:57:19 PM', '14/09/2020 3:30:12 PM', '14/09/2020 9:30:28 AM', '14/10/2020 10:05:40 AM', '14/10/2020 12:48:07 PM', '14/10/2020 5:03:05 PM', '14/10/2020 9:08:08 AM', '15/05/2020 10:12:04 AM', '15/05/2020 4:29:37 PM', '15/06/2020 11:14:24 AM', '15/06/2020 11:25:03 AM', '15/06/2020 11:26:59 AM', '15/07/2020 1:09:54 PM', '15/07/2020 1:12:18 PM', '15/07/2020 1:15:05 PM', '15/07/2020 5:02:58 PM', '15/07/2020 5:04:41 PM', '15/09/2020 3:06:32 PM', '15/09/2020 9:03:52 AM', '15/09/2020 9:05:19 AM', '15/09/2020 9:28:09 AM', '15/10/2020 11:29:55 AM', '15/10/2020 12:17:26 PM', '15/10/2020 12:22:18 PM', '15/10/2020 1:16:42 PM', '15/10/2020 5:01:14 PM', '16/03/2020 10:26:40 AM', '16/04/2020 11:58:14 AM', '16/04/2020 12:17:35 PM', '16/06/2020 11:39:13 AM', '16/06/2020 12:45:33 PM', '16/06/2020 12:53:21 PM', '16/09/2020 10:59:32 AM', '16/09/2020 9:11:19 AM', '16/10/2020 10:37:49 AM', '16/10/2020 12:00:08 PM', '16/10/2020 12:54:55 PM', '16/10/2020 1:00:18 PM', '16/10/2020 1:02:24 PM', '16/10/2020 1:04:18 PM', '16/10/2020 1:06:31 PM', '16/10/2020 1:50:17 PM', '16/10/2020 4:29:56 PM', '16/11/2020 10:27:47 AM', '16/11/2020 10:28:50 AM', '16/11/2020 10:29:55 AM', '16/11/2020 10:32:49 AM', '16/11/2020 2:50:48 PM', '16/11/2020 9:58:34 AM', '17/02/2020 1:38:15 PM', '17/02/2020 4:33:40 PM', '17/02/2020 5:16:29 PM', '17/02/2020 5:16:53 PM', '17/03/2020 10:28:20 AM', '17/04/2020 2:59:33 PM', '17/06/2020 10:06:15 AM', '17/06/2020 10:08:39 AM', '17/06/2020 10:27:49 AM', '17/06/2020 3:41:22 PM', '17/06/2020 3:50:11 PM', '17/06/2020 9:39:34 AM', '17/07/2020 10:59:43 AM', '17/07/2020 2:00:10 PM', '17/07/2020 3:51:53 PM', '17/08/2020 11:32:40 AM', '17/08/2020 11:45:48 AM', '17/08/2020 11:48:09 AM', '17/08/2020 11:49:29 AM', '17/08/2020 11:52:30 AM', '17/08/2020 11:53:48 AM', '17/08/2020 11:55:00 AM', '17/08/2020 11:56:12 AM', '17/08/2020 12:17:52 PM', '17/08/2020 2:57:49 PM', '17/08/2020 4:05:01 PM', '17/08/2020 4:40:19 PM', '17/09/2020 11:19:07 AM', '17/09/2020 4:05:04 PM', '17/09/2020 4:09:22 PM', '17/09/2020 9:14:15 AM', '17/11/2020 9:29:54 AM', '17/11/2020 9:39:00 AM', '17/11/2020 9:42:27 AM', '17/11/2020 9:47:03 AM', '17/11/2020 9:48:27 AM', '18/02/2020 1:44:43 PM', '18/02/2020 1:45:23 PM', '18/02/2020 2:19:19 PM', '18/02/2020 9:48:00 AM', '18/05/2020 12:19:52 PM', '18/05/2020 12:38:29 PM', '18/06/2020 12:33:37 PM', '18/06/2020 12:45:23 PM', '18/06/2020 12:49:21 PM', '18/06/2020 12:50:41 PM', '18/06/2020 12:51:39 PM', '18/06/2020 12:52:32 PM', '18/06/2020 12:53:27 PM', '18/06/2020 12:54:30 PM', '18/06/2020 1:01:31 PM', '18/06/2020 1:02:25 PM', '18/06/2020 1:03:15 PM', '18/06/2020 1:04:04 PM', '18/06/2020 1:05:04 PM', '18/06/2020 1:06:07 PM', '18/06/2020 1:07:25 PM', '18/06/2020 1:08:37 PM', '18/06/2020 1:12:09 PM', '18/06/2020 1:16:29 PM', '18/06/2020 1:18:34 PM', '18/06/2020 1:20:24 PM', '18/06/2020 2:24:04 PM', '18/06/2020 2:26:21 PM', '18/06/2020 2:28:40 PM', '18/06/2020 2:31:04 PM', '18/06/2020 2:32:51 PM', '18/06/2020 2:34:02 PM', '18/06/2020 2:40:05 PM', '18/06/2020 3:00:08 PM', '18/08/2020 10:35:19 AM', '18/08/2020 11:04:38 AM', '18/08/2020 3:54:07 PM', '18/09/2020 2:17:11 PM', '18/11/2020 10:37:51 AM', '18/11/2020 12:04:10 PM', '18/11/2020 2:16:06 PM', '18/11/2020 9:46:55 AM', '19/03/2020 10:02:11 AM', '19/03/2020 3:16:51 PM', '19/05/2020 12:00:00 AM', '19/05/2020 12:26:22 PM', '19/06/2020 12:16:53 PM', '19/06/2020 4:08:26 PM', '19/08/2020 1:07:47 PM', '19/08/2020 9:07:34 AM', '19/10/2020 3:40:02 PM', '19/10/2020 3:41:35 PM', '19/10/2020 3:56:31 PM', '19/10/2020 3:56:57 PM', '19/10/2020 4:46:55 PM', '2/03/2020 10:20:09 AM', '2/03/2020 3:37:36 PM', '2/06/2020 10:03:23 AM', '2/06/2020 10:05:18 AM', '2/06/2020 10:07:21 AM', '2/06/2020 10:53:23 AM', '2/06/2020 4:21:52 PM', '2/06/2020 9:37:49 AM', '2/06/2020 9:51:22 AM', '2/07/2020 11:35:17 AM', '2/07/2020 12:19:34 PM', '2/09/2020 10:26:52 AM', '2/09/2020 11:31:00 AM', '2/09/2020 11:37:55 AM', '2/09/2020 11:38:14 AM', '2/09/2020 4:59:33 PM', '2/09/2020 5:00:42 PM', '2/09/2020 5:02:40 PM', '2/09/2020 5:04:28 PM', '2/09/2020 5:06:04 PM', '2/09/2020 5:06:49 PM', '2/09/2020 5:08:00 PM', '2/09/2020 5:11:38 PM', '2/10/2020 12:00:00 AM', '2/11/2020 12:12:50 PM', '20/03/2020 11:57:02 AM', '20/03/2020 1:48:21 PM', '20/03/2020 2:46:28 PM', '20/04/2020 9:15:34 AM', '20/05/2020 12:01:11 PM', '20/05/2020 3:55:06 PM', '20/07/2020 10:11:17 AM', '20/07/2020 10:17:15 AM', '20/07/2020 10:19:17 AM', '20/07/2020 10:21:16 AM', '20/07/2020 10:26:30 AM', '20/07/2020 10:29:11 AM', '20/07/2020 10:35:15 AM', '20/07/2020 12:27:04 PM', '20/07/2020 2:13:50 PM', '20/07/2020 2:27:51 PM', '20/07/2020 2:29:16 PM', '20/07/2020 2:52:05 PM', '20/11/2020 10:34:27 AM', '21/04/2020 12:49:55 PM', '21/04/2020 9:10:27 AM', '21/04/2020 9:12:33 AM', '21/04/2020 9:20:33 AM', '21/05/2020 10:01:46 AM', '21/05/2020 10:52:34 AM', '21/07/2020 10:32:47 AM', '21/08/2020 12:49:22 PM', '21/08/2020 1:55:29 PM', '21/08/2020 2:07:58 PM', '21/10/2020 10:17:42 AM', '21/10/2020 11:31:01 AM', '21/10/2020 11:35:15 AM', '21/10/2020 11:45:00 AM', '21/10/2020 11:47:15 AM', '21/10/2020 3:43:52 PM', '21/10/2020 3:46:47 PM', '21/10/2020 3:48:57 PM', '22/05/2020 10:02:31 AM', '22/05/2020 12:00:38 PM', '22/06/2020 11:27:08 AM', '22/06/2020 11:40:00 AM', '22/06/2020 11:49:47 AM', '22/06/2020 12:10:27 PM', '22/06/2020 12:12:46 PM', '22/06/2020 12:15:00 PM', '22/06/2020 12:16:24 PM', '22/06/2020 12:18:44 PM', '22/06/2020 12:20:30 PM', '22/06/2020 12:23:01 PM', '22/06/2020 12:27:36 PM', '22/06/2020 12:29:17 PM', '22/06/2020 12:35:46 PM', '22/06/2020 12:37:14 PM', '22/06/2020 12:39:05 PM', '22/06/2020 3:15:31 PM', '22/07/2020 10:27:03 AM', '22/07/2020 10:55:25 AM', '22/07/2020 11:42:32 AM', '22/07/2020 9:31:41 AM', '22/09/2020 10:29:02 AM', '22/09/2020 10:30:54 AM', '22/09/2020 10:34:22 AM', '22/09/2020 10:38:15 AM', '22/09/2020 12:42:54 PM', '22/09/2020 12:44:00 PM', '22/09/2020 12:44:58 PM', '22/09/2020 12:50:03 PM', '22/09/2020 12:51:08 PM', '22/09/2020 12:52:59 PM', '22/09/2020 2:14:04 PM', '22/09/2020 4:12:30 PM', '22/09/2020 4:25:23 PM', '22/09/2020 4:34:18 PM', '22/09/2020 4:35:40 PM', '22/09/2020 4:37:32 PM', '22/09/2020 4:45:44 PM', '22/09/2020 4:47:53 PM', '22/09/2020 4:48:57 PM', '22/09/2020 4:49:49 PM', '22/09/2020 4:51:31 PM', '22/10/2020 10:08:32 AM', '22/10/2020 10:21:05 AM', '22/10/2020 10:33:03 AM', '22/10/2020 12:00:00 AM', '22/10/2020 1:52:11 PM', '22/10/2020 9:59:20 AM', '23/03/2020 2:29:12 PM', '23/03/2020 9:23:18 AM', '23/03/2020 9:36:07 AM', '23/04/2020 4:53:45 PM', '23/06/2020 1:34:20 PM', '23/07/2020 9:45:05 AM', '23/09/2020 12:39:45 PM', '23/09/2020 4:27:24 PM', '23/10/2020 10:29:57 AM', '23/10/2020 10:34:35 AM', '23/10/2020 10:50:19 AM', '23/10/2020 12:40:15 PM', '23/10/2020 4:14:53 PM', '23/10/2020 4:23:01 PM', '23/11/2020 10:15:36 AM', '23/11/2020 2:30:59 PM', '23/11/2020 3:04:49 PM', '23/11/2020 3:25:40 PM', '23/11/2020 3:33:42 PM', '23/11/2020 3:34:57 PM', '23/11/2020 9:19:05 AM', '24/02/2020 12:11:26 PM', '24/02/2020 12:12:15 PM', '24/02/2020 12:33:59 PM', '24/03/2020 1:29:41 PM', '24/04/2020 12:00:00 AM', '24/04/2020 4:56:30 PM', '24/04/2020 5:02:25 PM', '24/07/2020 11:30:31 AM', '24/07/2020 11:32:53 AM', '24/07/2020 11:34:57 AM', '24/07/2020 11:36:42 AM', '24/07/2020 12:34:26 PM', '24/07/2020 3:13:42 PM', '24/08/2020 11:53:59 AM', '24/08/2020 11:55:18 AM', '24/08/2020 4:56:53 PM', '24/08/2020 9:28:55 AM', '24/09/2020 10:48:16 AM', '24/09/2020 10:50:09 AM', '24/11/2020 1:02:41 PM', '24/11/2020 1:04:44 PM', '24/11/2020 1:10:03 PM', '24/11/2020 1:11:31 PM', '24/11/2020 1:12:07 PM', '24/11/2020 1:12:46 PM', '24/11/2020 1:13:27 PM', '24/11/2020 1:14:04 PM', '24/11/2020 2:02:30 PM', '24/11/2020 2:03:49 PM', '24/11/2020 2:04:53 PM', '24/11/2020 2:05:46 PM', '24/11/2020 2:06:54 PM', '24/11/2020 2:10:35 PM', '24/11/2020 2:12:02 PM', '24/11/2020 2:15:26 PM', '24/11/2020 2:19:14 PM', '24/11/2020 2:20:40 PM', '24/11/2020 2:22:54 PM', '24/11/2020 2:23:42 PM', '24/11/2020 2:24:56 PM', '24/11/2020 2:25:30 PM', '24/11/2020 2:27:00 PM', '24/11/2020 2:28:24 PM', '24/11/2020 2:29:32 PM', '24/11/2020 2:30:55 PM', '24/11/2020 2:33:19 PM', '24/11/2020 2:36:20 PM', '24/11/2020 2:37:33 PM', '24/11/2020 2:38:42 PM', '24/11/2020 2:41:02 PM', '24/11/2020 2:41:42 PM', '24/11/2020 2:43:48 PM', '24/11/2020 2:53:38 PM', '24/11/2020 2:55:14 PM', '24/11/2020 2:56:15 PM', '24/11/2020 2:59:44 PM', '24/11/2020 3:58:46 PM', '24/11/2020 4:01:14 PM', '24/11/2020 4:04:35 PM', '24/11/2020 4:05:18 PM', '24/11/2020 4:10:57 PM', '24/11/2020 4:13:51 PM', '24/11/2020 5:06:42 PM', '24/11/2020 5:10:06 PM', '24/11/2020 5:11:41 PM', '24/11/2020 5:13:42 PM', '24/11/2020 5:15:41 PM', '24/11/2020 9:43:10 AM', '24/11/2020 9:49:50 AM', '25/02/2020 8:54:32 AM', '25/03/2020 12:13:41 PM', '25/03/2020 1:15:46 PM', '25/06/2020 10:06:57 AM', '25/08/2020 10:14:47 AM', '25/08/2020 3:14:24 PM', '25/08/2020 3:26:32 PM', '25/09/2020 10:16:49 AM', '25/09/2020 10:18:31 AM', '25/09/2020 9:20:48 AM', '25/11/2020 3:29:18 PM', '26/02/2020 11:56:52 AM', '26/02/2020 1:21:56 PM', '26/05/2020 11:47:23 AM', '26/05/2020 11:58:09 AM', '26/05/2020 3:14:45 PM', '26/05/2020 4:01:28 PM', '26/06/2020 2:23:30 PM', '26/06/2020 9:32:49 AM', '26/06/2020 9:34:47 AM', '26/08/2020 2:38:59 PM', '26/08/2020 2:39:07 PM', '26/08/2020 2:39:26 PM', '26/08/2020 3:03:58 PM', '26/08/2020 3:05:13 PM', '26/08/2020 9:49:49 AM', '26/10/2020 10:02:27 AM', '26/10/2020 10:03:56 AM', '26/10/2020 10:05:17 AM', '26/10/2020 10:06:33 AM', '26/10/2020 10:07:54 AM', '26/10/2020 10:09:10 AM', '26/10/2020 10:10:29 AM', '26/10/2020 10:11:56 AM', '26/10/2020 9:50:12 AM', '26/10/2020 9:53:24 AM', '27/02/2020 3:57:54 PM', '27/04/2020 12:39:33 PM', '27/05/2020 3:19:16 PM', '27/05/2020 3:32:22 PM', '27/07/2020 1:05:13 PM', '27/07/2020 4:55:54 PM', '27/07/2020 9:38:57 AM', '27/07/2020 9:56:29 AM', '27/10/2020 10:29:09 AM', '27/10/2020 10:31:00 AM', '27/10/2020 1:14:20 PM', '27/10/2020 2:36:43 PM', '27/10/2020 4:38:35 PM', '27/10/2020 9:51:33 AM', '28/02/2020 2:53:55 PM', '28/04/2020 12:00:00 AM', '28/04/2020 2:17:28 PM', '28/04/2020 2:18:41 PM', '28/05/2020 1:27:38 PM', '28/05/2020 9:19:56 AM', '28/05/2020 9:21:56 AM', '28/07/2020 10:06:25 AM', '28/08/2020 9:44:54 AM', '28/09/2020 10:17:15 AM', '28/09/2020 10:19:18 AM', '28/09/2020 10:20:31 AM', '28/09/2020 10:21:40 AM', '28/09/2020 10:22:46 AM', '28/09/2020 10:24:15 AM', '28/09/2020 10:25:22 AM', '28/09/2020 10:28:27 AM', '28/09/2020 5:13:44 PM', '28/09/2020 5:17:57 PM', '28/09/2020 9:42:08 AM', '28/09/2020 9:43:52 AM', '28/09/2020 9:50:58 AM', '28/09/2020 9:52:23 AM', '28/09/2020 9:59:50 AM', '28/10/2020 12:19:35 PM', '28/10/2020 1:59:52 PM', '28/10/2020 9:19:55 AM', '29/04/2020 4:11:01 PM', '29/05/2020 9:54:13 AM', '29/06/2020 3:37:31 PM', '29/06/2020 3:53:44 PM', '29/06/2020 3:55:34 PM', '29/07/2020 11:33:44 AM', '29/07/2020 11:40:35 AM', '29/09/2020 3:54:15 PM', '29/10/2020 2:29:03 PM', '29/10/2020 9:09:21 AM', '3/02/2020 12:00:00 AM', '3/02/2020 3:07:00 PM', '3/03/2020 2:25:16 PM', '3/03/2020 2:26:22 PM', '3/04/2020 9:39:58 AM', '3/06/2020 2:39:20 PM', '3/06/2020 3:49:54 PM', '3/06/2020 9:01:32 AM', '3/07/2020 11:42:35 AM', '3/07/2020 3:10:56 PM', '3/07/2020 4:05:10 PM', '3/07/2020 4:18:28 PM', '3/08/2020 12:43:51 PM', '3/08/2020 12:53:22 PM', '3/09/2020 10:23:24 AM', '3/09/2020 10:24:32 AM', '3/09/2020 10:25:42 AM', '3/09/2020 10:27:44 AM', '3/09/2020 10:32:44 AM', '3/09/2020 10:35:41 AM', '3/09/2020 10:39:16 AM', '3/09/2020 10:40:14 AM', '3/09/2020 10:42:07 AM', '3/09/2020 10:43:28 AM', '3/09/2020 10:44:41 AM', '3/09/2020 10:47:03 AM', '3/09/2020 10:59:45 AM', '3/09/2020 11:01:20 AM', '3/09/2020 11:03:33 AM', '3/09/2020 11:05:02 AM', '3/09/2020 11:05:52 AM', '3/09/2020 11:06:31 AM', '3/09/2020 11:08:07 AM', '3/09/2020 11:09:06 AM', '3/09/2020 11:15:08 AM', '3/09/2020 11:16:01 AM', '3/09/2020 11:20:32 AM', '3/09/2020 11:21:37 AM', '3/09/2020 11:22:33 AM', '3/09/2020 11:23:17 AM', '3/09/2020 11:24:17 AM', '3/09/2020 11:27:25 AM', '3/09/2020 11:28:35 AM', '3/09/2020 11:30:26 AM', '3/09/2020 11:34:12 AM', '3/09/2020 11:34:57 AM', '3/09/2020 11:36:29 AM', '3/09/2020 11:39:14 AM', '3/09/2020 11:40:11 AM', '3/09/2020 11:41:05 AM', '3/09/2020 11:42:30 AM', '3/09/2020 11:44:15 AM', '3/09/2020 11:44:58 AM', '3/09/2020 11:45:46 AM', '3/09/2020 12:21:55 PM', '3/11/2020 4:52:44 PM', '3/11/2020 9:12:41 AM', '3/11/2020 9:20:17 AM', '3/11/2020 9:39:18 AM', '30/03/2020 10:05:37 AM', '30/03/2020 8:54:19 AM', '30/03/2020 9:14:38 AM', '30/03/2020 9:15:35 AM', '30/03/2020 9:16:26 AM', '30/06/2020 11:43:28 AM', '30/06/2020 12:13:41 PM', '30/06/2020 12:14:53 PM', '30/06/2020 12:15:39 PM', '30/06/2020 12:16:27 PM', '30/06/2020 12:17:18 PM', '30/06/2020 12:21:12 PM', '30/06/2020 4:18:53 PM', '30/06/2020 4:22:23 PM', '30/07/2020 10:29:38 AM', '30/07/2020 3:18:34 PM', '30/07/2020 5:07:06 PM', '30/09/2020 11:18:24 AM', '30/09/2020 3:22:08 PM', '30/10/2020 9:46:00 AM', '31/03/2020 2:33:34 PM', '31/03/2020 2:50:33 PM', '31/03/2020 3:54:14 PM', '31/07/2020 1:00:07 PM', '31/07/2020 1:56:42 PM', '31/07/2020 3:37:17 PM', '31/08/2020 11:23:40 AM', '31/08/2020 11:25:07 AM', '31/08/2020 11:38:34 AM', '31/08/2020 11:40:07 AM', '31/08/2020 11:56:30 AM', '31/08/2020 9:26:49 AM', '31/08/2020 9:28:39 AM', '31/08/2020 9:39:34 AM', '4/02/2020 10:07:23 AM', '4/02/2020 1:46:43 PM', '4/05/2020 10:33:52 AM', '4/05/2020 3:14:29 PM', '4/05/2020 9:27:52 AM', '4/05/2020 9:28:31 AM', '4/05/2020 9:45:44 AM', '4/06/2020 2:12:50 PM', '4/06/2020 4:07:01 PM', '4/09/2020 9:27:04 AM', '4/11/2020 10:51:33 AM', '4/11/2020 10:54:30 AM', '4/11/2020 12:23:39 PM', '4/11/2020 2:48:47 PM', '4/11/2020 4:58:28 PM', '4/11/2020 9:07:07 AM', '4/11/2020 9:08:33 AM', '5/02/2020 9:05:52 AM', '5/05/2020 11:19:14 AM', '5/05/2020 12:27:12 PM', '5/08/2020 11:03:39 AM', '5/08/2020 11:41:50 AM', '5/08/2020 12:09:39 PM', '5/11/2020 9:52:36 AM', '6/04/2020 4:52:25 PM', '6/04/2020 9:57:43 AM', '6/04/2020 9:58:07 AM', '6/04/2020 9:58:52 AM', '6/07/2020 11:03:09 AM', '6/07/2020 1:03:53 PM', '6/07/2020 2:03:37 PM', '6/07/2020 2:05:29 PM', '6/07/2020 2:11:57 PM', '6/07/2020 2:35:27 PM', '6/07/2020 2:46:50 PM', '6/07/2020 2:47:57 PM', '6/08/2020 10:27:13 AM', '6/08/2020 10:29:11 AM', '6/10/2020 12:13:55 PM', '6/10/2020 12:15:07 PM', '6/10/2020 12:16:23 PM', '6/10/2020 12:17:41 PM', '6/10/2020 12:19:38 PM', '6/10/2020 12:31:22 PM', '6/10/2020 12:34:46 PM', '6/10/2020 12:35:29 PM', '6/10/2020 12:36:29 PM', '6/10/2020 12:38:00 PM', '6/10/2020 12:38:54 PM', '6/10/2020 12:40:57 PM', '6/10/2020 9:29:54 AM', '6/11/2020 1:06:41 PM', '6/11/2020 1:50:22 PM', '6/11/2020 9:32:44 AM', '6/11/2020 9:54:09 AM', '7/02/2020 1:16:27 PM', '7/05/2020 11:29:44 AM', '7/07/2020 12:24:01 PM', '7/08/2020 10:07:54 AM', '7/08/2020 9:47:39 AM', '7/08/2020 9:49:04 AM', '7/09/2020 10:20:45 AM', '7/09/2020 11:01:13 AM', '7/09/2020 11:08:18 AM', '7/09/2020 11:09:33 AM', '7/09/2020 11:10:41 AM', '7/09/2020 11:11:52 AM', '7/09/2020 11:29:55 AM', '7/09/2020 12:00:52 PM', '7/09/2020 12:22:23 PM', '7/09/2020 12:24:19 PM', '7/09/2020 12:26:58 PM', '7/09/2020 12:29:12 PM', '7/09/2020 12:32:25 PM', '7/09/2020 12:42:51 PM', '7/09/2020 12:43:47 PM', '7/09/2020 12:51:00 PM', '7/09/2020 12:51:41 PM', '7/09/2020 12:55:41 PM', '7/09/2020 1:02:46 PM', '7/09/2020 1:11:45 PM', '7/09/2020 1:14:07 PM', '7/09/2020 2:04:48 PM', '7/09/2020 2:06:31 PM', '7/09/2020 2:08:48 PM', '7/09/2020 2:11:15 PM', '7/09/2020 2:23:31 PM', '7/09/2020 2:28:07 PM', '7/09/2020 4:21:11 PM', '7/09/2020 9:15:55 AM', '7/09/2020 9:24:35 AM', '7/10/2020 12:07:00 PM', '7/10/2020 3:30:57 PM', '7/10/2020 9:33:46 AM', '7/10/2020 9:33:58 AM', '7/10/2020 9:34:12 AM', '7/10/2020 9:34:26 AM', '8/04/2020 9:19:15 AM', '8/05/2020 8:59:47 AM', '8/07/2020 11:11:16 AM', '8/07/2020 11:13:03 AM', '8/07/2020 12:12:16 PM', '8/07/2020 1:24:50 PM', '8/07/2020 9:53:03 AM', '8/10/2020 12:54:23 PM', '9/06/2020 11:17:31 AM', '9/06/2020 11:19:01 AM', '9/06/2020 11:23:17 AM', '9/06/2020 11:24:46 AM', '9/06/2020 11:26:54 AM', '9/06/2020 11:29:09 AM', '9/06/2020 11:30:53 AM', '9/06/2020 9:20:15 AM', '9/07/2020 9:22:30 AM', '9/07/2020 9:24:16 AM', '9/07/2020 9:26:54 AM', '9/07/2020 9:29:31 AM', '9/07/2020 9:30:58 AM', '9/09/2020 12:08:54 PM', '9/09/2020 1:49:02 PM', '9/09/2020 4:17:38 PM', '9/09/2020 4:19:14 PM', '9/09/2020 9:31:00 AM', '9/10/2020 4:56:20 PM', '9/10/2020 9:11:28 AM', '9/10/2020 9:19:11 AM', '9/11/2020 10:02:09 AM', '9/11/2020 10:03:10 AM', '9/11/2020 10:04:21 AM', '9/11/2020 10:05:26 AM', '9/11/2020 10:07:18 AM', '9/11/2020 10:08:25 AM', '9/11/2020 10:18:50 AM', '9/11/2020 2:11:22 PM', '9/11/2020 9:33:25 AM', '9/11/2020 9:54:43 AM']</t>
+          <t>['1/05/2020 2:15:32 PM', '1/06/2020 10:01:54 AM', '1/06/2020 11:25:01 AM', '1/06/2020 11:27:17 AM', '1/06/2020 11:28:43 AM', '1/07/2020 11:38:37 AM', '1/07/2020 11:42:37 AM', '1/07/2020 11:58:55 AM', '1/07/2020 12:00:19 PM', '1/07/2020 12:02:16 PM', '1/07/2020 12:03:44 PM', '1/07/2020 4:50:05 PM', '1/09/2020 9:34:20 AM', '1/09/2020 9:43:55 AM', '1/10/2020 10:28:10 AM', '1/10/2020 12:45:38 PM', '1/10/2020 1:43:16 PM', '1/10/2020 4:38:00 PM', '10/02/2020 11:06:40 AM', '10/02/2020 4:46:19 PM', '10/02/2020 4:47:35 PM', '10/03/2020 10:06:32 AM', '10/03/2020 9:08:28 AM', '10/03/2020 9:57:02 AM', '10/06/2020 3:19:37 PM', '10/07/2020 11:11:39 AM', '10/07/2020 11:19:59 AM', '10/07/2020 2:09:18 PM', '10/08/2020 10:20:57 AM', '10/08/2020 10:25:40 AM', '10/08/2020 10:30:56 AM', '10/08/2020 10:42:07 AM', '10/08/2020 10:43:30 AM', '10/08/2020 12:00:27 PM', '10/08/2020 12:11:40 PM', '10/08/2020 9:31:56 AM', '10/11/2020 4:57:42 PM', '10/11/2020 5:04:27 PM', '10/11/2020 5:05:46 PM', '10/11/2020 5:07:08 PM', '10/11/2020 5:17:57 PM', '10/12/2020 12:00:00 AM', '10/12/2020 9:33:22 AM', '10/12/2020 9:55:12 AM', '10/12/2020 9:55:34 AM', '10/12/2020 9:55:58 AM', '10/12/2020 9:56:13 AM', '10/12/2020 9:56:31 AM', '11/03/2020 1:42:50 PM', '11/03/2020 8:51:56 AM', '11/03/2020 8:52:43 AM', '11/05/2020 9:48:12 AM', '11/05/2020 9:48:48 AM', '11/06/2020 10:03:25 AM', '11/06/2020 10:05:06 AM', '11/06/2020 10:26:37 AM', '11/06/2020 12:56:07 PM', '11/06/2020 5:31:16 PM', '11/08/2020 10:26:42 AM', '11/08/2020 10:27:40 AM', '11/08/2020 11:43:35 AM', '11/08/2020 11:44:07 AM', '11/09/2020 10:12:19 AM', '11/09/2020 9:53:11 AM', '11/09/2020 9:58:09 AM', '11/11/2020 10:43:39 AM', '11/12/2020 10:33:16 AM', '11/12/2020 10:34:35 AM', '12/05/2020 4:22:31 PM', '12/06/2020 2:05:22 PM', '12/06/2020 8:05:04 AM', '12/08/2020 5:14:39 PM', '12/08/2020 5:17:57 PM', '12/10/2020 10:47:56 AM', '12/10/2020 11:09:05 AM', '12/10/2020 11:10:15 AM', '12/10/2020 11:11:50 AM', '12/10/2020 11:12:59 AM', '12/10/2020 11:14:15 AM', '12/10/2020 11:15:46 AM', '12/10/2020 11:16:57 AM', '12/10/2020 11:18:05 AM', '12/10/2020 11:32:36 AM', '12/10/2020 3:44:41 PM', '13/02/2020 11:01:00 AM', '13/05/2020 10:50:49 AM', '13/05/2020 10:51:46 AM', '13/05/2020 12:00:00 AM', '13/07/2020 10:45:28 AM', '13/10/2020 10:58:33 AM', '13/10/2020 10:59:55 AM', '13/10/2020 11:01:02 AM', '13/10/2020 11:07:30 AM', '13/10/2020 11:08:31 AM', '13/10/2020 11:10:13 AM', '13/10/2020 11:12:22 AM', '13/10/2020 11:14:22 AM', '13/10/2020 11:15:41 AM', '13/10/2020 11:21:10 AM', '13/10/2020 11:22:37 AM', '13/10/2020 11:23:32 AM', '13/10/2020 11:26:05 AM', '13/10/2020 12:14:15 PM', '13/10/2020 5:11:31 PM', '13/10/2020 9:58:52 AM', '13/11/2020 10:57:23 AM', '13/11/2020 9:25:17 AM', '13/11/2020 9:32:31 AM', '13/11/2020 9:37:32 AM', '13/11/2020 9:47:49 AM', '14/02/2020 11:53:21 AM', '14/04/2020 10:56:28 AM', '14/04/2020 3:25:38 PM', '14/04/2020 3:59:27 PM', '14/04/2020 4:00:14 PM', '14/07/2020 10:07:53 AM', '14/07/2020 10:11:29 AM', '14/07/2020 10:24:24 AM', '14/07/2020 10:27:19 AM', '14/07/2020 10:29:28 AM', '14/07/2020 10:31:23 AM', '14/07/2020 10:33:12 AM', '14/07/2020 10:34:52 AM', '14/07/2020 10:36:17 AM', '14/07/2020 10:38:38 AM', '14/07/2020 10:40:14 AM', '14/07/2020 10:41:50 AM', '14/07/2020 10:43:19 AM', '14/07/2020 10:47:23 AM', '14/07/2020 10:49:05 AM', '14/07/2020 10:50:49 AM', '14/07/2020 11:41:49 AM', '14/07/2020 5:12:52 PM', '14/07/2020 5:20:49 PM', '14/07/2020 9:09:12 AM', '14/09/2020 10:16:21 AM', '14/09/2020 10:34:58 AM', '14/09/2020 10:36:07 AM', '14/09/2020 10:37:13 AM', '14/09/2020 10:38:37 AM', '14/09/2020 1:56:35 PM', '14/09/2020 1:57:19 PM', '14/09/2020 3:30:12 PM', '14/09/2020 9:30:28 AM', '14/10/2020 10:05:40 AM', '14/10/2020 12:48:07 PM', '14/10/2020 5:03:05 PM', '14/10/2020 9:08:08 AM', '14/12/2020 12:03:04 PM', '14/12/2020 12:04:25 PM', '14/12/2020 12:09:02 PM', '14/12/2020 12:10:38 PM', '14/12/2020 12:13:21 PM', '14/12/2020 12:16:21 PM', '14/12/2020 12:17:29 PM', '14/12/2020 12:18:55 PM', '14/12/2020 12:20:57 PM', '14/12/2020 12:24:38 PM', '14/12/2020 12:25:51 PM', '14/12/2020 12:27:21 PM', '14/12/2020 12:28:29 PM', '14/12/2020 12:33:15 PM', '14/12/2020 12:44:26 PM', '14/12/2020 12:45:26 PM', '14/12/2020 12:46:50 PM', '14/12/2020 12:48:25 PM', '14/12/2020 12:49:56 PM', '14/12/2020 12:52:41 PM', '14/12/2020 12:54:36 PM', '14/12/2020 12:55:55 PM', '14/12/2020 12:57:00 PM', '14/12/2020 12:59:01 PM', '14/12/2020 12:59:53 PM', '14/12/2020 1:02:23 PM', '14/12/2020 1:03:47 PM', '14/12/2020 1:05:29 PM', '14/12/2020 1:07:09 PM', '14/12/2020 1:08:46 PM', '14/12/2020 1:12:06 PM', '14/12/2020 1:14:17 PM', '14/12/2020 1:18:56 PM', '14/12/2020 1:23:28 PM', '14/12/2020 1:27:49 PM', '14/12/2020 1:32:39 PM', '14/12/2020 2:13:52 PM', '14/12/2020 2:15:58 PM', '14/12/2020 2:17:44 PM', '14/12/2020 2:20:31 PM', '14/12/2020 2:37:20 PM', '14/12/2020 2:39:22 PM', '14/12/2020 2:42:02 PM', '14/12/2020 2:45:25 PM', '14/12/2020 2:46:43 PM', '14/12/2020 2:49:49 PM', '14/12/2020 2:51:22 PM', '14/12/2020 4:17:16 PM', '14/12/2020 9:10:46 AM', '14/12/2020 9:53:30 AM', '14/12/2020 9:54:47 AM', '14/12/2020 9:55:46 AM', '14/12/2020 9:56:50 AM', '14/12/2020 9:57:48 AM', '15/05/2020 10:12:04 AM', '15/05/2020 4:29:37 PM', '15/06/2020 11:14:24 AM', '15/06/2020 11:25:03 AM', '15/06/2020 11:26:59 AM', '15/07/2020 1:09:54 PM', '15/07/2020 1:12:18 PM', '15/07/2020 1:15:05 PM', '15/07/2020 5:02:58 PM', '15/07/2020 5:04:41 PM', '15/09/2020 3:06:32 PM', '15/09/2020 9:03:52 AM', '15/09/2020 9:05:19 AM', '15/09/2020 9:28:09 AM', '15/10/2020 11:29:55 AM', '15/10/2020 12:17:26 PM', '15/10/2020 1:16:42 PM', '15/10/2020 5:01:14 PM', '15/12/2020 10:29:44 AM', '15/12/2020 11:23:52 AM', '15/12/2020 11:33:14 AM', '15/12/2020 2:02:16 PM', '15/12/2020 2:36:09 PM', '15/12/2020 2:42:37 PM', '15/12/2020 3:14:31 PM', '15/12/2020 4:45:11 PM', '15/12/2020 5:00:10 PM', '15/12/2020 5:02:04 PM', '15/12/2020 5:03:57 PM', '15/12/2020 5:05:40 PM', '15/12/2020 5:07:40 PM', '15/12/2020 5:08:51 PM', '16/03/2020 10:26:40 AM', '16/04/2020 11:58:14 AM', '16/04/2020 12:17:35 PM', '16/06/2020 11:39:13 AM', '16/06/2020 12:45:33 PM', '16/06/2020 12:53:21 PM', '16/09/2020 10:59:32 AM', '16/09/2020 9:11:19 AM', '16/10/2020 10:37:49 AM', '16/10/2020 12:00:08 PM', '16/10/2020 12:54:55 PM', '16/10/2020 1:00:18 PM', '16/10/2020 1:02:24 PM', '16/10/2020 1:04:18 PM', '16/10/2020 1:06:31 PM', '16/10/2020 1:50:17 PM', '16/10/2020 4:29:56 PM', '16/11/2020 10:27:47 AM', '16/11/2020 10:28:50 AM', '16/11/2020 10:29:55 AM', '16/11/2020 10:32:49 AM', '16/11/2020 2:50:48 PM', '16/11/2020 9:58:34 AM', '16/12/2020 4:40:46 PM', '16/12/2020 9:34:46 AM', '17/02/2020 1:38:15 PM', '17/02/2020 4:33:40 PM', '17/02/2020 5:16:29 PM', '17/02/2020 5:16:53 PM', '17/03/2020 10:28:20 AM', '17/04/2020 2:59:33 PM', '17/06/2020 10:06:15 AM', '17/06/2020 10:08:39 AM', '17/06/2020 10:27:49 AM', '17/06/2020 3:41:22 PM', '17/06/2020 3:50:11 PM', '17/06/2020 9:39:34 AM', '17/07/2020 10:59:43 AM', '17/07/2020 2:00:10 PM', '17/07/2020 3:51:53 PM', '17/08/2020 11:32:40 AM', '17/08/2020 11:45:48 AM', '17/08/2020 11:48:09 AM', '17/08/2020 11:49:29 AM', '17/08/2020 11:52:30 AM', '17/08/2020 11:53:48 AM', '17/08/2020 11:55:00 AM', '17/08/2020 11:56:12 AM', '17/08/2020 12:17:52 PM', '17/08/2020 2:57:49 PM', '17/08/2020 4:05:01 PM', '17/08/2020 4:40:19 PM', '17/09/2020 11:19:07 AM', '17/09/2020 4:05:04 PM', '17/09/2020 4:09:22 PM', '17/09/2020 9:14:15 AM', '17/11/2020 9:29:54 AM', '17/11/2020 9:39:00 AM', '17/11/2020 9:42:27 AM', '17/11/2020 9:47:03 AM', '17/11/2020 9:48:27 AM', '17/12/2020 4:34:22 PM', '17/12/2020 8:31:24 AM', '18/02/2020 1:44:43 PM', '18/02/2020 1:45:23 PM', '18/02/2020 2:19:19 PM', '18/02/2020 9:48:00 AM', '18/05/2020 12:19:52 PM', '18/05/2020 12:38:29 PM', '18/06/2020 12:33:37 PM', '18/06/2020 12:45:23 PM', '18/06/2020 12:49:21 PM', '18/06/2020 12:50:41 PM', '18/06/2020 12:51:39 PM', '18/06/2020 12:52:32 PM', '18/06/2020 12:53:27 PM', '18/06/2020 12:54:30 PM', '18/06/2020 1:01:31 PM', '18/06/2020 1:02:25 PM', '18/06/2020 1:03:15 PM', '18/06/2020 1:04:04 PM', '18/06/2020 1:05:04 PM', '18/06/2020 1:06:07 PM', '18/06/2020 1:07:25 PM', '18/06/2020 1:08:37 PM', '18/06/2020 1:12:09 PM', '18/06/2020 1:16:29 PM', '18/06/2020 1:18:34 PM', '18/06/2020 1:20:24 PM', '18/06/2020 2:24:04 PM', '18/06/2020 2:26:21 PM', '18/06/2020 2:28:40 PM', '18/06/2020 2:31:04 PM', '18/06/2020 2:32:51 PM', '18/06/2020 2:34:02 PM', '18/06/2020 2:40:05 PM', '18/06/2020 3:00:08 PM', '18/08/2020 10:35:19 AM', '18/08/2020 11:04:38 AM', '18/08/2020 3:54:07 PM', '18/09/2020 2:17:11 PM', '18/11/2020 10:37:51 AM', '18/11/2020 12:04:10 PM', '18/11/2020 2:16:06 PM', '18/11/2020 9:46:55 AM', '18/12/2020 12:17:40 PM', '18/12/2020 9:38:33 AM', '19/03/2020 10:02:11 AM', '19/03/2020 3:16:51 PM', '19/05/2020 12:00:00 AM', '19/05/2020 12:26:22 PM', '19/06/2020 12:16:53 PM', '19/06/2020 4:08:26 PM', '19/08/2020 1:07:47 PM', '19/08/2020 9:07:34 AM', '19/10/2020 3:40:02 PM', '19/10/2020 3:41:35 PM', '19/10/2020 3:56:31 PM', '19/10/2020 3:56:57 PM', '19/10/2020 4:46:55 PM', '2/03/2020 10:20:09 AM', '2/03/2020 3:37:36 PM', '2/06/2020 10:03:23 AM', '2/06/2020 10:05:18 AM', '2/06/2020 10:07:21 AM', '2/06/2020 10:53:23 AM', '2/06/2020 4:21:52 PM', '2/06/2020 9:37:49 AM', '2/06/2020 9:51:22 AM', '2/07/2020 11:35:17 AM', '2/07/2020 12:19:34 PM', '2/09/2020 10:26:52 AM', '2/09/2020 11:31:00 AM', '2/09/2020 11:37:55 AM', '2/09/2020 11:38:14 AM', '2/09/2020 4:59:33 PM', '2/09/2020 5:00:42 PM', '2/09/2020 5:02:40 PM', '2/09/2020 5:04:28 PM', '2/09/2020 5:06:04 PM', '2/09/2020 5:06:49 PM', '2/09/2020 5:08:00 PM', '2/09/2020 5:11:38 PM', '2/10/2020 12:00:00 AM', '2/11/2020 12:12:50 PM', '2/12/2020 10:50:24 AM', '2/12/2020 10:57:52 AM', '2/12/2020 10:58:55 AM', '2/12/2020 10:59:57 AM', '2/12/2020 11:47:02 AM', '20/03/2020 11:57:02 AM', '20/03/2020 1:48:21 PM', '20/03/2020 2:46:28 PM', '20/04/2020 9:15:34 AM', '20/05/2020 12:01:11 PM', '20/05/2020 3:55:06 PM', '20/07/2020 10:11:17 AM', '20/07/2020 10:17:15 AM', '20/07/2020 10:19:17 AM', '20/07/2020 10:21:16 AM', '20/07/2020 10:26:30 AM', '20/07/2020 10:29:11 AM', '20/07/2020 10:35:15 AM', '20/07/2020 12:27:04 PM', '20/07/2020 2:13:50 PM', '20/07/2020 2:27:51 PM', '20/07/2020 2:29:16 PM', '20/07/2020 2:52:05 PM', '20/11/2020 10:34:27 AM', '21/04/2020 12:49:55 PM', '21/04/2020 9:10:27 AM', '21/04/2020 9:12:33 AM', '21/04/2020 9:20:33 AM', '21/05/2020 10:01:46 AM', '21/05/2020 10:52:34 AM', '21/07/2020 10:32:47 AM', '21/08/2020 12:49:22 PM', '21/08/2020 1:55:29 PM', '21/08/2020 2:07:58 PM', '21/10/2020 10:17:42 AM', '21/10/2020 11:31:01 AM', '21/10/2020 11:35:15 AM', '21/10/2020 11:45:00 AM', '21/10/2020 11:47:15 AM', '21/10/2020 3:43:52 PM', '21/10/2020 3:46:47 PM', '21/10/2020 3:48:57 PM', '22/05/2020 10:02:31 AM', '22/05/2020 12:00:38 PM', '22/06/2020 11:27:08 AM', '22/06/2020 11:40:00 AM', '22/06/2020 11:49:47 AM', '22/06/2020 12:10:27 PM', '22/06/2020 12:12:46 PM', '22/06/2020 12:15:00 PM', '22/06/2020 12:16:24 PM', '22/06/2020 12:18:44 PM', '22/06/2020 12:20:30 PM', '22/06/2020 12:23:01 PM', '22/06/2020 12:27:36 PM', '22/06/2020 12:29:17 PM', '22/06/2020 12:35:46 PM', '22/06/2020 12:37:14 PM', '22/06/2020 12:39:05 PM', '22/06/2020 3:15:31 PM', '22/07/2020 10:27:03 AM', '22/07/2020 10:55:25 AM', '22/07/2020 11:42:32 AM', '22/07/2020 9:31:41 AM', '22/09/2020 10:29:02 AM', '22/09/2020 10:30:54 AM', '22/09/2020 10:34:22 AM', '22/09/2020 10:38:15 AM', '22/09/2020 12:42:54 PM', '22/09/2020 12:44:00 PM', '22/09/2020 12:44:58 PM', '22/09/2020 12:50:03 PM', '22/09/2020 12:51:08 PM', '22/09/2020 12:52:59 PM', '22/09/2020 2:14:04 PM', '22/09/2020 4:12:30 PM', '22/09/2020 4:25:23 PM', '22/09/2020 4:34:18 PM', '22/09/2020 4:35:40 PM', '22/09/2020 4:37:32 PM', '22/09/2020 4:45:44 PM', '22/09/2020 4:47:53 PM', '22/09/2020 4:48:57 PM', '22/09/2020 4:49:49 PM', '22/09/2020 4:51:31 PM', '22/10/2020 10:08:32 AM', '22/10/2020 10:21:05 AM', '22/10/2020 10:33:03 AM', '22/10/2020 12:00:00 AM', '22/10/2020 1:52:11 PM', '22/10/2020 9:59:20 AM', '23/03/2020 2:29:12 PM', '23/03/2020 9:23:18 AM', '23/03/2020 9:36:07 AM', '23/04/2020 4:53:45 PM', '23/06/2020 1:34:20 PM', '23/07/2020 9:45:05 AM', '23/09/2020 12:39:45 PM', '23/09/2020 4:27:24 PM', '23/10/2020 10:29:57 AM', '23/10/2020 10:34:35 AM', '23/10/2020 10:50:19 AM', '23/10/2020 12:40:15 PM', '23/10/2020 4:14:53 PM', '23/10/2020 4:23:01 PM', '23/11/2020 10:15:36 AM', '23/11/2020 2:30:59 PM', '23/11/2020 3:04:49 PM', '23/11/2020 3:25:40 PM', '23/11/2020 3:33:42 PM', '23/11/2020 3:34:57 PM', '23/11/2020 9:19:05 AM', '23/12/2020 3:13:46 PM', '24/02/2020 12:11:26 PM', '24/02/2020 12:12:15 PM', '24/02/2020 12:33:59 PM', '24/03/2020 1:29:41 PM', '24/04/2020 12:00:00 AM', '24/04/2020 4:56:30 PM', '24/04/2020 5:02:25 PM', '24/07/2020 11:30:31 AM', '24/07/2020 11:32:53 AM', '24/07/2020 11:34:57 AM', '24/07/2020 11:36:42 AM', '24/07/2020 12:34:26 PM', '24/07/2020 3:13:42 PM', '24/08/2020 11:53:59 AM', '24/08/2020 11:55:18 AM', '24/08/2020 4:56:53 PM', '24/08/2020 9:28:55 AM', '24/09/2020 10:48:16 AM', '24/09/2020 10:50:09 AM', '24/11/2020 1:02:41 PM', '24/11/2020 1:04:44 PM', '24/11/2020 1:10:03 PM', '24/11/2020 1:11:31 PM', '24/11/2020 1:12:07 PM', '24/11/2020 1:12:46 PM', '24/11/2020 1:13:27 PM', '24/11/2020 1:14:04 PM', '24/11/2020 2:02:30 PM', '24/11/2020 2:03:49 PM', '24/11/2020 2:04:53 PM', '24/11/2020 2:05:46 PM', '24/11/2020 2:06:54 PM', '24/11/2020 2:10:35 PM', '24/11/2020 2:12:02 PM', '24/11/2020 2:15:26 PM', '24/11/2020 2:19:14 PM', '24/11/2020 2:20:40 PM', '24/11/2020 2:22:54 PM', '24/11/2020 2:23:42 PM', '24/11/2020 2:24:56 PM', '24/11/2020 2:25:30 PM', '24/11/2020 2:27:00 PM', '24/11/2020 2:28:24 PM', '24/11/2020 2:29:32 PM', '24/11/2020 2:30:55 PM', '24/11/2020 2:33:19 PM', '24/11/2020 2:36:20 PM', '24/11/2020 2:37:33 PM', '24/11/2020 2:38:42 PM', '24/11/2020 2:41:02 PM', '24/11/2020 2:41:42 PM', '24/11/2020 2:43:48 PM', '24/11/2020 2:53:38 PM', '24/11/2020 2:55:14 PM', '24/11/2020 2:56:15 PM', '24/11/2020 2:59:44 PM', '24/11/2020 3:58:46 PM', '24/11/2020 4:01:14 PM', '24/11/2020 4:04:35 PM', '24/11/2020 4:05:18 PM', '24/11/2020 4:10:57 PM', '24/11/2020 4:13:51 PM', '24/11/2020 5:06:42 PM', '24/11/2020 5:10:06 PM', '24/11/2020 5:11:41 PM', '24/11/2020 5:13:42 PM', '24/11/2020 5:15:41 PM', '24/11/2020 9:43:10 AM', '24/11/2020 9:49:50 AM', '25/02/2020 8:54:32 AM', '25/03/2020 12:13:41 PM', '25/03/2020 1:15:46 PM', '25/06/2020 10:06:57 AM', '25/08/2020 10:14:47 AM', '25/08/2020 3:14:24 PM', '25/08/2020 3:26:32 PM', '25/09/2020 10:16:49 AM', '25/09/2020 10:18:31 AM', '25/09/2020 9:20:48 AM', '25/11/2020 3:29:18 PM', '26/02/2020 11:56:52 AM', '26/02/2020 1:21:56 PM', '26/05/2020 11:47:23 AM', '26/05/2020 11:58:09 AM', '26/05/2020 3:14:45 PM', '26/05/2020 4:01:28 PM', '26/06/2020 2:23:30 PM', '26/06/2020 9:32:49 AM', '26/06/2020 9:34:47 AM', '26/08/2020 2:38:59 PM', '26/08/2020 2:39:07 PM', '26/08/2020 2:39:26 PM', '26/08/2020 3:03:58 PM', '26/08/2020 3:05:13 PM', '26/08/2020 9:49:49 AM', '26/10/2020 10:02:27 AM', '26/10/2020 10:03:56 AM', '26/10/2020 10:05:17 AM', '26/10/2020 10:06:33 AM', '26/10/2020 10:07:54 AM', '26/10/2020 10:09:10 AM', '26/10/2020 10:10:29 AM', '26/10/2020 10:11:56 AM', '26/10/2020 9:50:12 AM', '26/10/2020 9:53:24 AM', '27/02/2020 3:57:54 PM', '27/04/2020 12:39:33 PM', '27/05/2020 3:19:16 PM', '27/05/2020 3:32:22 PM', '27/07/2020 1:05:13 PM', '27/07/2020 4:55:54 PM', '27/07/2020 9:38:57 AM', '27/07/2020 9:56:29 AM', '27/10/2020 10:29:09 AM', '27/10/2020 10:31:00 AM', '27/10/2020 1:14:20 PM', '27/10/2020 2:36:43 PM', '27/10/2020 4:38:35 PM', '27/10/2020 9:51:33 AM', '27/11/2020 9:55:45 AM', '28/02/2020 2:53:55 PM', '28/04/2020 12:00:00 AM', '28/04/2020 2:17:28 PM', '28/04/2020 2:18:41 PM', '28/05/2020 1:27:38 PM', '28/05/2020 9:19:56 AM', '28/05/2020 9:21:56 AM', '28/07/2020 10:06:25 AM', '28/08/2020 9:44:54 AM', '28/09/2020 10:17:15 AM', '28/09/2020 10:19:18 AM', '28/09/2020 10:20:31 AM', '28/09/2020 10:21:40 AM', '28/09/2020 10:22:46 AM', '28/09/2020 10:24:15 AM', '28/09/2020 10:25:22 AM', '28/09/2020 10:28:27 AM', '28/09/2020 5:13:44 PM', '28/09/2020 5:17:57 PM', '28/09/2020 9:42:08 AM', '28/09/2020 9:43:52 AM', '28/09/2020 9:50:58 AM', '28/09/2020 9:52:23 AM', '28/09/2020 9:59:50 AM', '28/10/2020 12:19:35 PM', '28/10/2020 1:59:52 PM', '28/10/2020 9:19:55 AM', '29/04/2020 4:11:01 PM', '29/05/2020 9:54:13 AM', '29/06/2020 3:37:31 PM', '29/06/2020 3:53:44 PM', '29/06/2020 3:55:34 PM', '29/07/2020 11:33:44 AM', '29/07/2020 11:40:35 AM', '29/09/2020 3:54:15 PM', '29/10/2020 2:29:03 PM', '29/10/2020 9:09:21 AM', '3/02/2020 12:00:00 AM', '3/02/2020 3:07:00 PM', '3/03/2020 2:25:16 PM', '3/03/2020 2:26:22 PM', '3/04/2020 9:39:58 AM', '3/06/2020 2:39:20 PM', '3/06/2020 3:49:54 PM', '3/06/2020 9:01:32 AM', '3/07/2020 11:42:35 AM', '3/07/2020 3:10:56 PM', '3/07/2020 4:05:10 PM', '3/07/2020 4:18:28 PM', '3/08/2020 12:43:51 PM', '3/08/2020 12:53:22 PM', '3/09/2020 10:23:24 AM', '3/09/2020 10:24:32 AM', '3/09/2020 10:25:42 AM', '3/09/2020 10:27:44 AM', '3/09/2020 10:32:44 AM', '3/09/2020 10:35:41 AM', '3/09/2020 10:39:16 AM', '3/09/2020 10:40:14 AM', '3/09/2020 10:42:07 AM', '3/09/2020 10:43:28 AM', '3/09/2020 10:44:41 AM', '3/09/2020 10:47:03 AM', '3/09/2020 10:59:45 AM', '3/09/2020 11:01:20 AM', '3/09/2020 11:03:33 AM', '3/09/2020 11:05:02 AM', '3/09/2020 11:05:52 AM', '3/09/2020 11:06:31 AM', '3/09/2020 11:08:07 AM', '3/09/2020 11:09:06 AM', '3/09/2020 11:15:08 AM', '3/09/2020 11:16:01 AM', '3/09/2020 11:20:32 AM', '3/09/2020 11:21:37 AM', '3/09/2020 11:22:33 AM', '3/09/2020 11:23:17 AM', '3/09/2020 11:24:17 AM', '3/09/2020 11:27:25 AM', '3/09/2020 11:28:35 AM', '3/09/2020 11:30:26 AM', '3/09/2020 11:34:12 AM', '3/09/2020 11:34:57 AM', '3/09/2020 11:36:29 AM', '3/09/2020 11:39:14 AM', '3/09/2020 11:40:11 AM', '3/09/2020 11:41:05 AM', '3/09/2020 11:42:30 AM', '3/09/2020 11:44:15 AM', '3/09/2020 11:44:58 AM', '3/09/2020 11:45:46 AM', '3/09/2020 12:21:55 PM', '3/11/2020 4:52:44 PM', '3/11/2020 9:12:41 AM', '3/11/2020 9:20:17 AM', '3/11/2020 9:39:18 AM', '3/12/2020 10:25:23 AM', '3/12/2020 10:25:39 AM', '3/12/2020 10:32:30 AM', '3/12/2020 2:14:06 PM', '3/12/2020 5:17:16 PM', '30/03/2020 10:05:37 AM', '30/03/2020 8:54:19 AM', '30/03/2020 9:14:38 AM', '30/03/2020 9:15:35 AM', '30/03/2020 9:16:26 AM', '30/06/2020 11:43:28 AM', '30/06/2020 12:13:41 PM', '30/06/2020 12:14:53 PM', '30/06/2020 12:15:39 PM', '30/06/2020 12:16:27 PM', '30/06/2020 12:17:18 PM', '30/06/2020 12:21:12 PM', '30/06/2020 4:18:53 PM', '30/06/2020 4:22:23 PM', '30/07/2020 10:29:38 AM', '30/07/2020 3:18:34 PM', '30/07/2020 5:07:06 PM', '30/09/2020 11:18:24 AM', '30/09/2020 3:22:08 PM', '30/10/2020 9:46:00 AM', '30/11/2020 10:14:27 AM', '30/11/2020 10:42:10 AM', '30/11/2020 10:49:25 AM', '30/11/2020 11:18:50 AM', '30/11/2020 11:19:47 AM', '30/11/2020 11:20:47 AM', '30/11/2020 11:22:18 AM', '30/11/2020 11:23:22 AM', '30/11/2020 11:24:31 AM', '30/11/2020 9:32:26 AM', '31/03/2020 2:33:34 PM', '31/03/2020 2:50:33 PM', '31/03/2020 3:54:14 PM', '31/07/2020 1:00:07 PM', '31/07/2020 1:56:42 PM', '31/07/2020 3:37:17 PM', '31/08/2020 11:23:40 AM', '31/08/2020 11:25:07 AM', '31/08/2020 11:38:34 AM', '31/08/2020 11:40:07 AM', '31/08/2020 11:56:30 AM', '31/08/2020 9:26:49 AM', '31/08/2020 9:28:39 AM', '31/08/2020 9:39:34 AM', '4/02/2020 10:07:23 AM', '4/02/2020 1:46:43 PM', '4/05/2020 10:33:52 AM', '4/05/2020 3:14:29 PM', '4/05/2020 9:27:52 AM', '4/05/2020 9:28:31 AM', '4/05/2020 9:45:44 AM', '4/06/2020 2:12:50 PM', '4/06/2020 4:07:01 PM', '4/09/2020 9:27:04 AM', '4/11/2020 10:51:33 AM', '4/11/2020 10:54:30 AM', '4/11/2020 12:23:39 PM', '4/11/2020 2:48:47 PM', '4/11/2020 4:58:28 PM', '4/11/2020 9:07:07 AM', '4/11/2020 9:08:33 AM', '4/12/2020 11:27:06 AM', '4/12/2020 12:00:00 AM', '5/02/2020 9:05:52 AM', '5/05/2020 11:19:14 AM', '5/05/2020 12:27:12 PM', '5/08/2020 11:03:39 AM', '5/08/2020 11:41:50 AM', '5/08/2020 12:09:39 PM', '5/11/2020 9:52:36 AM', '6/04/2020 4:52:25 PM', '6/04/2020 9:57:43 AM', '6/04/2020 9:58:07 AM', '6/04/2020 9:58:52 AM', '6/07/2020 11:03:09 AM', '6/07/2020 1:03:53 PM', '6/07/2020 2:03:37 PM', '6/07/2020 2:05:29 PM', '6/07/2020 2:11:57 PM', '6/07/2020 2:35:27 PM', '6/07/2020 2:46:50 PM', '6/07/2020 2:47:57 PM', '6/08/2020 10:27:13 AM', '6/08/2020 10:29:11 AM', '6/10/2020 12:13:55 PM', '6/10/2020 12:15:07 PM', '6/10/2020 12:16:23 PM', '6/10/2020 12:17:41 PM', '6/10/2020 12:19:38 PM', '6/10/2020 12:31:22 PM', '6/10/2020 12:34:46 PM', '6/10/2020 12:35:29 PM', '6/10/2020 12:36:29 PM', '6/10/2020 12:38:00 PM', '6/10/2020 12:38:54 PM', '6/10/2020 12:40:57 PM', '6/10/2020 9:29:54 AM', '6/11/2020 1:06:41 PM', '6/11/2020 1:50:22 PM', '6/11/2020 9:32:44 AM', '6/11/2020 9:54:09 AM', '7/02/2020 1:16:27 PM', '7/05/2020 11:29:44 AM', '7/07/2020 12:24:01 PM', '7/08/2020 10:07:54 AM', '7/08/2020 9:47:39 AM', '7/08/2020 9:49:04 AM', '7/09/2020 10:20:45 AM', '7/09/2020 11:01:13 AM', '7/09/2020 11:08:18 AM', '7/09/2020 11:09:33 AM', '7/09/2020 11:10:41 AM', '7/09/2020 11:11:52 AM', '7/09/2020 11:29:55 AM', '7/09/2020 12:00:52 PM', '7/09/2020 12:22:23 PM', '7/09/2020 12:24:19 PM', '7/09/2020 12:26:58 PM', '7/09/2020 12:29:12 PM', '7/09/2020 12:32:25 PM', '7/09/2020 12:42:51 PM', '7/09/2020 12:43:47 PM', '7/09/2020 12:51:00 PM', '7/09/2020 12:51:41 PM', '7/09/2020 12:55:41 PM', '7/09/2020 1:02:46 PM', '7/09/2020 1:11:45 PM', '7/09/2020 1:14:07 PM', '7/09/2020 2:04:48 PM', '7/09/2020 2:06:31 PM', '7/09/2020 2:08:48 PM', '7/09/2020 2:11:15 PM', '7/09/2020 2:23:31 PM', '7/09/2020 2:28:07 PM', '7/09/2020 4:21:11 PM', '7/09/2020 9:15:55 AM', '7/09/2020 9:24:35 AM', '7/10/2020 12:07:00 PM', '7/10/2020 3:30:57 PM', '7/10/2020 9:33:46 AM', '7/10/2020 9:33:58 AM', '7/10/2020 9:34:12 AM', '7/10/2020 9:34:26 AM', '7/12/2020 10:18:18 AM', '7/12/2020 10:19:27 AM', '7/12/2020 10:22:39 AM', '7/12/2020 10:37:57 AM', '7/12/2020 10:56:03 AM', '7/12/2020 10:56:59 AM', '7/12/2020 10:57:52 AM', '7/12/2020 10:58:58 AM', '7/12/2020 10:59:52 AM', '7/12/2020 11:01:58 AM', '7/12/2020 11:02:57 AM', '7/12/2020 11:06:31 AM', '7/12/2020 11:07:40 AM', '7/12/2020 9:44:12 AM', '7/12/2020 9:53:41 AM', '8/04/2020 9:19:15 AM', '8/05/2020 8:59:47 AM', '8/07/2020 11:11:16 AM', '8/07/2020 11:13:03 AM', '8/07/2020 12:12:16 PM', '8/07/2020 1:24:50 PM', '8/07/2020 9:53:03 AM', '8/10/2020 12:54:23 PM', '8/12/2020 4:26:34 PM', '9/06/2020 11:17:31 AM', '9/06/2020 11:19:01 AM', '9/06/2020 11:23:17 AM', '9/06/2020 11:24:46 AM', '9/06/2020 11:26:54 AM', '9/06/2020 11:29:09 AM', '9/06/2020 11:30:53 AM', '9/06/2020 9:20:15 AM', '9/07/2020 9:22:30 AM', '9/07/2020 9:24:16 AM', '9/07/2020 9:26:54 AM', '9/07/2020 9:29:31 AM', '9/07/2020 9:30:58 AM', '9/09/2020 12:08:54 PM', '9/09/2020 1:49:02 PM', '9/09/2020 4:17:38 PM', '9/09/2020 4:19:14 PM', '9/09/2020 9:31:00 AM', '9/10/2020 4:56:20 PM', '9/10/2020 9:11:28 AM', '9/10/2020 9:19:11 AM', '9/11/2020 10:02:09 AM', '9/11/2020 10:03:10 AM', '9/11/2020 10:04:21 AM', '9/11/2020 10:05:26 AM', '9/11/2020 10:07:18 AM', '9/11/2020 10:08:25 AM', '9/11/2020 10:18:50 AM', '9/11/2020 2:11:22 PM', '9/11/2020 9:33:25 AM', '9/11/2020 9:54:43 AM', '9/12/2020 10:40:34 AM', '9/12/2020 10:41:47 AM', '9/12/2020 10:43:57 AM', '9/12/2020 2:34:47 PM', '9/12/2020 9:14:45 AM', '9/12/2020 9:22:19 AM', '9/12/2020 9:27:54 AM', '9/12/2020 9:40:11 AM']</t>
         </is>
       </c>
     </row>
@@ -2995,7 +2995,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -3028,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="O29" t="n">
-        <v>2280</v>
+        <v>2548</v>
       </c>
       <c r="P29" t="n">
         <v>0</v>
@@ -3043,7 +3043,7 @@
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>24/11/2020 4:27:11 PM</t>
+          <t>23/12/2020 3:14:01 PM</t>
         </is>
       </c>
       <c r="T29" t="n">
@@ -3051,20 +3051,20 @@
       </c>
       <c r="U29" t="inlineStr"/>
       <c r="V29" t="n">
-        <v>2280</v>
+        <v>2548</v>
       </c>
       <c r="W29" t="n">
         <v>0</v>
       </c>
       <c r="X29" t="n">
-        <v>6672</v>
+        <v>7582</v>
       </c>
       <c r="Y29" t="n">
-        <v>304</v>
+        <v>346</v>
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>['1/04/2020 10:29:59 AM', '1/04/2020 9:10:29 AM', '1/05/2020 11:13:07 AM', '1/05/2020 8:44:28 AM', '1/06/2020 10:25:51 AM', '1/06/2020 2:21:18 PM', '1/07/2020 1:50:37 PM', '1/07/2020 9:28:36 AM', '1/09/2020 1:28:44 PM', '1/09/2020 1:30:12 PM', '1/10/2020 4:29:58 PM', '1/10/2020 4:37:53 PM', '10/03/2020 9:58:09 AM', '10/07/2020 11:14:46 AM', '10/07/2020 2:15:04 PM', '10/07/2020 4:05:55 PM', '10/08/2020 10:14:03 AM', '10/08/2020 10:45:17 AM', '10/08/2020 9:24:06 AM', '10/09/2020 10:02:30 AM', '10/09/2020 10:51:22 AM', '10/09/2020 11:35:22 AM', '10/09/2020 5:02:23 PM', '11/05/2020 11:32:20 AM', '11/05/2020 12:41:12 PM', '11/05/2020 8:50:14 AM', '11/08/2020 10:22:51 AM', '11/08/2020 10:24:39 AM', '12/02/2020 12:25:07 PM', '12/02/2020 3:57:19 PM', '12/10/2020 11:03:36 AM', '12/10/2020 11:06:30 AM', '12/10/2020 2:12:42 PM', '12/10/2020 5:12:43 PM', '12/11/2020 12:13:33 PM', '12/11/2020 4:21:21 PM', '12/11/2020 4:25:50 PM', '12/11/2020 9:28:50 AM', '12/11/2020 9:33:34 AM', '12/11/2020 9:35:42 AM', '12/11/2020 9:38:18 AM', '13/05/2020 11:30:19 AM', '13/08/2020 9:31:41 AM', '13/10/2020 10:00:45 AM', '13/10/2020 11:33:55 AM', '13/10/2020 8:41:54 AM', '13/11/2020 10:51:44 AM', '13/11/2020 10:52:53 AM', '13/11/2020 10:59:47 AM', '13/11/2020 11:11:48 AM', '13/11/2020 3:26:05 PM', '13/11/2020 3:29:48 PM', '13/11/2020 3:33:04 PM', '13/11/2020 3:34:49 PM', '13/11/2020 3:50:50 PM', '13/11/2020 4:20:00 PM', '13/11/2020 9:28:26 AM', '14/04/2020 10:51:56 AM', '14/04/2020 4:13:35 PM', '14/05/2020 9:54:48 AM', '14/07/2020 12:05:22 PM', '14/07/2020 12:06:55 PM', '14/07/2020 9:35:27 AM', '14/09/2020 10:23:22 AM', '14/09/2020 10:27:13 AM', '14/09/2020 10:28:41 AM', '14/09/2020 10:31:28 AM', '14/09/2020 3:30:18 PM', '14/09/2020 9:31:59 AM', '14/10/2020 12:40:31 PM', '14/10/2020 12:41:39 PM', '14/10/2020 9:08:14 AM', '15/05/2020 12:47:10 PM', '15/05/2020 12:49:40 PM', '15/06/2020 5:00:44 PM', '15/09/2020 2:24:54 PM', '15/10/2020 12:11:24 PM', '15/10/2020 12:15:50 PM', '16/04/2020 11:58:58 AM', '16/04/2020 9:19:21 AM', '16/07/2020 10:30:06 AM', '16/07/2020 10:32:21 AM', '16/07/2020 10:34:24 AM', '16/07/2020 12:19:15 PM', '16/09/2020 10:48:52 AM', '16/10/2020 10:54:22 AM', '17/02/2020 10:43:41 AM', '17/03/2020 12:00:00 AM', '17/04/2020 3:02:59 PM', '17/04/2020 4:45:29 PM', '17/06/2020 10:17:40 AM', '17/06/2020 3:42:27 PM', '17/07/2020 11:05:29 AM', '17/08/2020 11:16:20 AM', '17/08/2020 12:15:19 PM', '17/08/2020 12:16:38 PM', '17/08/2020 12:24:52 PM', '17/09/2020 11:14:22 AM', '17/09/2020 11:15:45 AM', '17/09/2020 1:45:31 PM', '17/09/2020 3:56:38 PM', '17/11/2020 10:46:43 AM', '17/11/2020 11:26:36 AM', '17/11/2020 1:22:18 PM', '18/05/2020 11:36:39 AM', '18/05/2020 3:07:26 PM', '18/06/2020 3:07:51 PM', '18/08/2020 10:55:57 AM', '18/08/2020 10:57:38 AM', '18/08/2020 11:02:40 AM', '18/09/2020 9:30:09 AM', '18/11/2020 10:52:01 AM', '18/11/2020 12:00:00 AM', '18/11/2020 9:50:57 AM', '19/05/2020 12:00:00 AM', '19/05/2020 12:55:55 PM', '19/05/2020 1:05:56 PM', '19/06/2020 2:48:02 PM', '19/08/2020 12:56:53 PM', '19/08/2020 9:34:10 AM', '19/08/2020 9:35:35 AM', '19/08/2020 9:37:13 AM', '19/11/2020 12:09:50 PM', '2/07/2020 12:15:37 PM', '2/09/2020 10:07:53 AM', '2/09/2020 11:31:05 AM', '2/09/2020 1:54:11 PM', '2/09/2020 3:49:37 PM', '2/10/2020 11:28:55 AM', '2/11/2020 10:04:18 AM', '2/11/2020 11:49:04 AM', '2/11/2020 11:56:03 AM', '2/11/2020 11:57:30 AM', '2/11/2020 11:58:29 AM', '2/11/2020 11:59:23 AM', '2/11/2020 12:16:13 PM', '20/03/2020 12:57:06 PM', '20/03/2020 1:00:21 PM', '20/07/2020 9:15:03 AM', '20/08/2020 10:01:35 AM', '20/10/2020 12:12:13 PM', '20/10/2020 12:13:27 PM', '20/10/2020 12:16:57 PM', '21/04/2020 10:47:27 AM', '21/04/2020 9:13:19 AM', '21/04/2020 9:37:16 AM', '21/05/2020 10:39:15 AM', '21/05/2020 2:09:47 PM', '21/05/2020 8:59:52 AM', '21/07/2020 10:39:12 AM', '21/07/2020 5:26:56 PM', '21/08/2020 1:11:30 PM', '21/08/2020 2:04:32 PM', '21/09/2020 4:08:47 PM', '21/10/2020 11:27:37 AM', '22/04/2020 11:12:37 AM', '22/04/2020 4:52:50 PM', '22/06/2020 1:20:10 PM', '22/07/2020 10:24:23 AM', '22/09/2020 2:19:40 PM', '22/10/2020 12:16:19 PM', '22/10/2020 12:23:36 PM', '22/10/2020 12:24:48 PM', '22/10/2020 9:57:36 AM', '23/04/2020 10:05:09 AM', '23/04/2020 3:17:08 PM', '23/06/2020 10:49:17 AM', '23/06/2020 12:53:08 PM', '23/07/2020 10:29:30 AM', '23/07/2020 1:50:49 PM', '23/07/2020 9:45:14 AM', '23/09/2020 10:10:18 AM', '23/09/2020 4:12:09 PM', '23/09/2020 9:36:43 AM', '23/10/2020 10:32:32 AM', '23/10/2020 12:00:00 AM', '23/11/2020 10:18:03 AM', '24/03/2020 9:58:58 AM', '24/04/2020 4:50:17 PM', '24/06/2020 12:34:10 PM', '24/07/2020 11:21:57 AM', '24/07/2020 11:56:22 AM', '24/08/2020 12:20:55 PM', '24/08/2020 2:16:53 PM', '24/08/2020 5:04:22 PM', '24/11/2020 4:27:11 PM', '24/11/2020 4:52:12 PM', '24/11/2020 9:31:51 AM', '24/11/2020 9:39:12 AM', '24/11/2020 9:45:43 AM', '25/06/2020 10:02:50 AM', '25/06/2020 4:08:12 PM', '25/08/2020 12:09:20 PM', '25/08/2020 12:54:41 PM', '25/08/2020 3:19:44 PM', '25/08/2020 3:33:09 PM', '25/08/2020 9:54:43 AM', '25/09/2020 9:00:36 AM', '25/11/2020 12:02:44 PM', '26/05/2020 3:17:33 PM', '26/08/2020 2:39:12 PM', '26/10/2020 10:13:34 AM', '26/10/2020 9:55:22 AM', '26/11/2020 10:04:35 AM', '26/11/2020 10:20:17 AM', '27/03/2020 10:34:10 AM', '27/03/2020 9:04:05 AM', '27/07/2020 1:13:18 PM', '27/07/2020 4:55:59 PM', '27/08/2020 3:06:17 PM', '27/08/2020 3:27:19 PM', '27/08/2020 9:47:56 AM', '27/08/2020 9:49:00 AM', '27/10/2020 10:18:53 AM', '27/10/2020 10:27:09 AM', '27/10/2020 1:13:06 PM', '28/02/2020 9:06:54 AM', '28/05/2020 9:17:43 AM', '28/07/2020 2:09:47 PM', '28/09/2020 11:00:19 AM', '28/09/2020 3:46:32 PM', '28/09/2020 5:21:27 PM', '28/10/2020 12:25:13 PM', '28/10/2020 3:31:17 PM', '28/10/2020 9:25:14 AM', '29/04/2020 9:01:38 AM', '29/07/2020 9:22:14 AM', '29/09/2020 3:49:59 PM', '29/10/2020 2:47:51 PM', '29/10/2020 9:24:12 AM', '3/04/2020 11:40:26 AM', '3/06/2020 11:23:32 AM', '3/07/2020 3:08:35 PM', '3/07/2020 4:18:35 PM', '3/07/2020 4:19:49 PM', '3/08/2020 12:48:31 PM', '3/11/2020 12:00:00 AM', '3/11/2020 2:59:26 PM', '3/11/2020 4:55:57 PM', '3/11/2020 5:02:07 PM', '3/11/2020 9:23:48 AM', '3/11/2020 9:33:47 AM', '30/03/2020 9:12:46 AM', '30/09/2020 3:44:11 PM', '30/10/2020 1:44:01 PM', '30/10/2020 9:52:58 AM', '30/10/2020 9:54:12 AM', '31/03/2020 12:10:09 PM', '31/07/2020 1:00:16 PM', '31/07/2020 1:02:13 PM', '31/07/2020 1:04:50 PM', '31/08/2020 10:05:52 AM', '31/08/2020 11:43:01 AM', '4/03/2020 3:44:52 PM', '4/05/2020 8:56:34 AM', '4/06/2020 12:00:00 AM', '4/06/2020 2:15:27 PM', '4/11/2020 10:12:45 AM', '4/11/2020 10:31:09 AM', '4/11/2020 10:48:50 AM', '4/11/2020 3:47:22 PM', '4/11/2020 9:11:13 AM', '5/06/2020 2:06:44 PM', '5/08/2020 11:05:11 AM', '5/08/2020 11:36:12 AM', '5/08/2020 12:07:59 PM', '5/08/2020 4:13:14 PM', '5/08/2020 4:24:03 PM', '5/08/2020 9:42:13 AM', '5/11/2020 9:54:56 AM', '6/07/2020 9:18:16 AM', '6/10/2020 12:26:44 PM', '6/10/2020 12:33:21 PM', '6/10/2020 9:28:02 AM', '6/11/2020 10:02:18 AM', '6/11/2020 10:03:18 AM', '6/11/2020 10:04:32 AM', '6/11/2020 10:09:05 AM', '6/11/2020 1:43:09 PM', '7/04/2020 9:29:29 AM', '7/05/2020 1:00:51 PM', '7/09/2020 2:02:19 PM', '7/09/2020 2:16:26 PM', '7/09/2020 2:19:26 PM', '7/10/2020 9:41:08 AM', '8/05/2020 10:00:47 AM', '8/05/2020 11:04:06 AM', '8/07/2020 1:24:55 PM', '8/07/2020 1:53:05 PM', '8/07/2020 9:00:24 AM', '8/07/2020 9:03:57 AM', '8/09/2020 9:30:58 AM', '8/10/2020 12:54:48 PM', '8/10/2020 12:55:33 PM', '9/09/2020 11:55:36 AM', '9/09/2020 1:49:08 PM', '9/10/2020 11:14:47 AM', '9/10/2020 11:17:01 AM', '9/10/2020 3:56:00 PM', '9/11/2020 10:11:37 AM', '9/11/2020 10:12:39 AM', '9/11/2020 9:34:32 AM', '9/11/2020 9:52:20 AM', '9/11/2020 9:56:44 AM']</t>
+          <t>['1/04/2020 10:29:59 AM', '1/04/2020 9:10:29 AM', '1/05/2020 11:13:07 AM', '1/05/2020 8:44:28 AM', '1/06/2020 10:25:51 AM', '1/06/2020 2:21:18 PM', '1/07/2020 1:50:37 PM', '1/07/2020 9:28:36 AM', '1/09/2020 1:28:44 PM', '1/09/2020 1:30:12 PM', '1/10/2020 4:29:58 PM', '1/10/2020 4:37:53 PM', '10/03/2020 9:58:09 AM', '10/07/2020 11:14:46 AM', '10/07/2020 2:15:04 PM', '10/07/2020 4:05:55 PM', '10/08/2020 10:14:03 AM', '10/08/2020 10:45:17 AM', '10/08/2020 9:24:06 AM', '10/09/2020 10:02:30 AM', '10/09/2020 10:51:22 AM', '10/09/2020 11:35:22 AM', '10/09/2020 5:02:23 PM', '11/05/2020 11:32:20 AM', '11/05/2020 12:41:12 PM', '11/05/2020 8:50:14 AM', '11/08/2020 10:22:51 AM', '11/08/2020 10:24:39 AM', '11/12/2020 10:35:29 AM', '11/12/2020 12:49:01 PM', '11/12/2020 9:28:03 AM', '12/02/2020 12:25:07 PM', '12/02/2020 3:57:19 PM', '12/10/2020 11:03:36 AM', '12/10/2020 11:06:30 AM', '12/10/2020 2:12:42 PM', '12/10/2020 5:12:43 PM', '12/11/2020 12:13:33 PM', '12/11/2020 4:21:21 PM', '12/11/2020 4:25:50 PM', '12/11/2020 9:28:50 AM', '12/11/2020 9:33:34 AM', '12/11/2020 9:35:42 AM', '12/11/2020 9:38:18 AM', '13/05/2020 11:30:19 AM', '13/08/2020 9:31:41 AM', '13/10/2020 10:00:45 AM', '13/10/2020 11:33:55 AM', '13/10/2020 8:41:54 AM', '13/11/2020 10:51:44 AM', '13/11/2020 10:52:53 AM', '13/11/2020 10:59:47 AM', '13/11/2020 11:11:48 AM', '13/11/2020 3:26:05 PM', '13/11/2020 3:29:48 PM', '13/11/2020 3:33:04 PM', '13/11/2020 3:34:49 PM', '13/11/2020 3:50:50 PM', '13/11/2020 4:20:00 PM', '13/11/2020 9:28:26 AM', '14/04/2020 10:51:56 AM', '14/04/2020 4:13:35 PM', '14/05/2020 9:54:48 AM', '14/07/2020 12:05:22 PM', '14/07/2020 12:06:55 PM', '14/07/2020 9:35:27 AM', '14/09/2020 10:23:22 AM', '14/09/2020 10:27:13 AM', '14/09/2020 10:28:41 AM', '14/09/2020 10:31:28 AM', '14/09/2020 3:30:18 PM', '14/09/2020 9:31:59 AM', '14/10/2020 12:40:31 PM', '14/10/2020 12:41:39 PM', '14/10/2020 9:08:14 AM', '14/12/2020 10:43:29 AM', '14/12/2020 4:26:33 PM', '14/12/2020 4:27:23 PM', '14/12/2020 9:52:21 AM', '15/05/2020 12:47:10 PM', '15/05/2020 12:49:40 PM', '15/06/2020 5:00:44 PM', '15/09/2020 2:24:54 PM', '15/10/2020 12:11:24 PM', '15/10/2020 12:15:50 PM', '15/12/2020 5:11:51 PM', '16/04/2020 11:58:58 AM', '16/04/2020 9:19:21 AM', '16/07/2020 10:30:06 AM', '16/07/2020 10:32:21 AM', '16/07/2020 10:34:24 AM', '16/07/2020 12:19:15 PM', '16/09/2020 10:48:52 AM', '16/09/2020 12:00:00 AM', '16/10/2020 10:54:22 AM', '16/12/2020 9:31:18 AM', '16/12/2020 9:32:52 AM', '17/02/2020 10:43:41 AM', '17/03/2020 12:00:00 AM', '17/04/2020 3:02:59 PM', '17/04/2020 4:45:29 PM', '17/06/2020 10:17:40 AM', '17/06/2020 3:42:27 PM', '17/07/2020 11:05:29 AM', '17/08/2020 11:16:20 AM', '17/08/2020 12:15:19 PM', '17/08/2020 12:16:38 PM', '17/08/2020 12:24:52 PM', '17/09/2020 11:14:22 AM', '17/09/2020 11:15:45 AM', '17/09/2020 1:45:31 PM', '17/09/2020 3:56:38 PM', '17/11/2020 10:46:43 AM', '17/11/2020 11:26:36 AM', '17/11/2020 1:22:18 PM', '17/12/2020 2:37:12 PM', '17/12/2020 3:44:07 PM', '18/05/2020 11:36:39 AM', '18/05/2020 3:07:26 PM', '18/06/2020 3:07:51 PM', '18/08/2020 10:55:57 AM', '18/08/2020 10:57:38 AM', '18/08/2020 11:02:40 AM', '18/09/2020 9:30:09 AM', '18/11/2020 10:52:01 AM', '18/11/2020 12:00:00 AM', '18/11/2020 9:50:57 AM', '18/12/2020 10:18:25 AM', '18/12/2020 9:30:11 AM', '18/12/2020 9:48:19 AM', '18/12/2020 9:52:09 AM', '19/05/2020 12:00:00 AM', '19/05/2020 12:55:55 PM', '19/05/2020 1:05:56 PM', '19/06/2020 2:48:02 PM', '19/08/2020 12:56:53 PM', '19/08/2020 9:34:10 AM', '19/08/2020 9:35:35 AM', '19/08/2020 9:37:13 AM', '19/11/2020 12:09:50 PM', '2/07/2020 12:15:37 PM', '2/09/2020 10:07:53 AM', '2/09/2020 11:31:05 AM', '2/09/2020 1:54:11 PM', '2/09/2020 3:49:37 PM', '2/10/2020 11:28:55 AM', '2/11/2020 10:04:18 AM', '2/11/2020 11:49:04 AM', '2/11/2020 11:56:03 AM', '2/11/2020 11:57:30 AM', '2/11/2020 11:58:29 AM', '2/11/2020 11:59:23 AM', '2/11/2020 12:16:13 PM', '2/12/2020 10:41:32 AM', '2/12/2020 10:54:42 AM', '2/12/2020 10:55:49 AM', '2/12/2020 10:56:45 AM', '2/12/2020 11:34:26 AM', '20/03/2020 12:57:06 PM', '20/03/2020 1:00:21 PM', '20/07/2020 9:15:03 AM', '20/08/2020 10:01:35 AM', '20/10/2020 12:12:13 PM', '20/10/2020 12:13:27 PM', '20/10/2020 12:16:57 PM', '21/04/2020 10:47:27 AM', '21/04/2020 9:13:19 AM', '21/04/2020 9:37:16 AM', '21/05/2020 10:39:15 AM', '21/05/2020 2:09:47 PM', '21/05/2020 8:59:52 AM', '21/07/2020 10:39:12 AM', '21/07/2020 5:26:56 PM', '21/08/2020 1:11:30 PM', '21/08/2020 2:04:32 PM', '21/09/2020 4:08:47 PM', '21/10/2020 11:27:37 AM', '22/04/2020 11:12:37 AM', '22/04/2020 4:52:50 PM', '22/06/2020 1:20:10 PM', '22/07/2020 10:24:23 AM', '22/09/2020 2:19:40 PM', '22/10/2020 12:16:19 PM', '22/10/2020 12:23:36 PM', '22/10/2020 12:24:48 PM', '22/10/2020 9:57:36 AM', '22/12/2020 9:12:07 AM', '22/12/2020 9:15:48 AM', '22/12/2020 9:17:29 AM', '23/04/2020 10:05:09 AM', '23/04/2020 3:17:08 PM', '23/06/2020 10:49:17 AM', '23/06/2020 12:53:08 PM', '23/07/2020 10:29:30 AM', '23/07/2020 1:50:49 PM', '23/07/2020 9:45:14 AM', '23/09/2020 10:10:18 AM', '23/09/2020 4:12:09 PM', '23/09/2020 9:36:43 AM', '23/10/2020 10:32:32 AM', '23/10/2020 12:00:00 AM', '23/11/2020 10:18:03 AM', '23/12/2020 11:30:40 AM', '23/12/2020 3:10:27 PM', '23/12/2020 3:14:01 PM', '24/03/2020 9:58:58 AM', '24/04/2020 4:50:17 PM', '24/06/2020 12:34:10 PM', '24/07/2020 11:21:57 AM', '24/07/2020 11:56:22 AM', '24/08/2020 12:00:00 AM', '24/08/2020 12:20:55 PM', '24/08/2020 2:16:53 PM', '24/08/2020 5:04:22 PM', '24/11/2020 4:27:11 PM', '24/11/2020 4:52:12 PM', '24/11/2020 9:31:51 AM', '24/11/2020 9:39:12 AM', '24/11/2020 9:45:43 AM', '25/06/2020 10:02:50 AM', '25/06/2020 4:08:12 PM', '25/08/2020 12:09:20 PM', '25/08/2020 12:54:41 PM', '25/08/2020 3:19:44 PM', '25/08/2020 3:33:09 PM', '25/08/2020 9:54:43 AM', '25/09/2020 9:00:36 AM', '25/11/2020 12:02:44 PM', '26/05/2020 3:17:33 PM', '26/08/2020 2:39:12 PM', '26/10/2020 10:13:34 AM', '26/10/2020 9:55:22 AM', '26/11/2020 10:04:35 AM', '26/11/2020 10:20:17 AM', '27/03/2020 10:34:10 AM', '27/03/2020 9:04:05 AM', '27/07/2020 1:13:18 PM', '27/07/2020 4:55:59 PM', '27/08/2020 3:06:17 PM', '27/08/2020 3:27:19 PM', '27/08/2020 9:47:56 AM', '27/08/2020 9:49:00 AM', '27/10/2020 10:18:53 AM', '27/10/2020 10:27:09 AM', '27/10/2020 1:13:06 PM', '27/11/2020 9:38:22 AM', '27/11/2020 9:41:08 AM', '27/11/2020 9:45:52 AM', '27/11/2020 9:51:23 AM', '28/02/2020 9:06:54 AM', '28/05/2020 9:17:43 AM', '28/07/2020 2:09:47 PM', '28/09/2020 11:00:19 AM', '28/09/2020 3:46:32 PM', '28/09/2020 5:21:27 PM', '28/10/2020 12:25:13 PM', '28/10/2020 3:31:17 PM', '28/10/2020 9:25:14 AM', '29/04/2020 9:01:38 AM', '29/07/2020 9:22:14 AM', '29/09/2020 3:49:59 PM', '29/10/2020 2:47:51 PM', '29/10/2020 9:24:12 AM', '3/04/2020 11:40:26 AM', '3/06/2020 11:23:32 AM', '3/07/2020 3:08:35 PM', '3/07/2020 4:19:49 PM', '3/08/2020 12:48:31 PM', '3/11/2020 12:00:00 AM', '3/11/2020 2:59:26 PM', '3/11/2020 4:55:57 PM', '3/11/2020 5:02:07 PM', '3/11/2020 9:23:48 AM', '3/11/2020 9:33:47 AM', '3/12/2020 10:33:43 AM', '30/03/2020 9:12:46 AM', '30/09/2020 3:44:11 PM', '30/10/2020 1:44:01 PM', '30/10/2020 9:52:58 AM', '30/10/2020 9:54:12 AM', '31/03/2020 12:10:09 PM', '31/07/2020 1:00:16 PM', '31/07/2020 1:02:13 PM', '31/07/2020 1:04:50 PM', '31/08/2020 10:05:52 AM', '31/08/2020 11:43:01 AM', '4/03/2020 3:44:52 PM', '4/05/2020 8:56:34 AM', '4/06/2020 12:00:00 AM', '4/06/2020 2:15:27 PM', '4/11/2020 10:12:45 AM', '4/11/2020 10:31:09 AM', '4/11/2020 10:48:50 AM', '4/11/2020 3:47:22 PM', '4/11/2020 9:11:13 AM', '4/12/2020 12:00:00 AM', '4/12/2020 9:47:37 AM', '5/06/2020 2:06:44 PM', '5/08/2020 11:05:11 AM', '5/08/2020 11:36:12 AM', '5/08/2020 12:07:59 PM', '5/08/2020 4:13:14 PM', '5/08/2020 4:24:03 PM', '5/08/2020 9:42:13 AM', '5/11/2020 9:54:56 AM', '6/07/2020 9:18:16 AM', '6/10/2020 12:26:44 PM', '6/10/2020 12:33:21 PM', '6/10/2020 9:28:02 AM', '6/11/2020 10:02:18 AM', '6/11/2020 10:03:18 AM', '6/11/2020 10:04:32 AM', '6/11/2020 10:09:05 AM', '6/11/2020 1:43:09 PM', '7/04/2020 9:29:29 AM', '7/05/2020 1:00:51 PM', '7/09/2020 2:02:19 PM', '7/09/2020 2:16:26 PM', '7/09/2020 2:19:26 PM', '7/10/2020 9:41:08 AM', '7/12/2020 10:36:56 AM', '7/12/2020 10:55:08 AM', '7/12/2020 11:09:37 AM', '7/12/2020 11:16:05 AM', '7/12/2020 1:09:01 PM', '8/05/2020 10:00:47 AM', '8/05/2020 11:04:06 AM', '8/07/2020 1:24:55 PM', '8/07/2020 1:53:05 PM', '8/07/2020 9:00:24 AM', '8/07/2020 9:03:57 AM', '8/09/2020 9:30:58 AM', '8/10/2020 12:54:48 PM', '8/10/2020 12:55:33 PM', '9/09/2020 11:55:36 AM', '9/09/2020 1:49:08 PM', '9/10/2020 11:14:47 AM', '9/10/2020 11:17:01 AM', '9/10/2020 3:56:00 PM', '9/11/2020 10:11:37 AM', '9/11/2020 10:12:39 AM', '9/11/2020 9:34:32 AM', '9/11/2020 9:52:20 AM', '9/11/2020 9:56:44 AM', '9/12/2020 10:51:31 AM', '9/12/2020 10:58:53 AM']</t>
         </is>
       </c>
     </row>
@@ -3083,7 +3083,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
@@ -3116,7 +3116,7 @@
         <v>0</v>
       </c>
       <c r="O30" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="P30" t="n">
         <v>0</v>
@@ -3131,11 +3131,11 @@
       </c>
       <c r="S30" t="inlineStr"/>
       <c r="T30" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="U30" t="inlineStr"/>
       <c r="V30" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="W30" t="n">
         <v>0</v>
@@ -3167,7 +3167,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -3200,7 +3200,7 @@
         <v>0</v>
       </c>
       <c r="O31" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="P31" t="n">
         <v>0</v>
@@ -3215,11 +3215,11 @@
       </c>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="U31" t="inlineStr"/>
       <c r="V31" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="W31" t="n">
         <v>0</v>
@@ -3251,7 +3251,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -3284,7 +3284,7 @@
         <v>0</v>
       </c>
       <c r="O32" t="n">
-        <v>2594</v>
+        <v>2905</v>
       </c>
       <c r="P32" t="n">
         <v>0</v>
@@ -3307,7 +3307,7 @@
       </c>
       <c r="U32" t="inlineStr"/>
       <c r="V32" t="n">
-        <v>2594</v>
+        <v>2905</v>
       </c>
       <c r="W32" t="n">
         <v>0</v>
@@ -3339,7 +3339,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -3372,7 +3372,7 @@
         <v>0</v>
       </c>
       <c r="O33" t="n">
-        <v>2229</v>
+        <v>2499</v>
       </c>
       <c r="P33" t="n">
         <v>0</v>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>27/10/2020</t>
+          <t>11/11/2020</t>
         </is>
       </c>
       <c r="T33" t="n">
@@ -3395,20 +3395,20 @@
       </c>
       <c r="U33" t="inlineStr"/>
       <c r="V33" t="n">
-        <v>2229</v>
+        <v>2499</v>
       </c>
       <c r="W33" t="n">
         <v>0</v>
       </c>
       <c r="X33" t="n">
-        <v>629</v>
+        <v>706</v>
       </c>
       <c r="Y33" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>[',', ',           ,           ,           ,', '03/05/2020', '03/09/2020', '04/09/2020', '05/02/2020', '09/06/2020', '11/12/2017', '16/09/2020', '17/09/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']</t>
+          <t>[',', ',           ,           ,           ,', '03/05/2020', '03/09/2020', '04/09/2020', '05/02/2020', '06/11/2020', '09/06/2020', '11/11/2020', '11/12/2017', '14/10/2020', '16/09/2020', '17/09/2020', '18/08/2020', '19/05/2020', '23/01/2020', '27/10/2020', '29/09/2020,', '30/06/2020,']</t>
         </is>
       </c>
     </row>
@@ -3427,22 +3427,22 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E34" t="n">
-        <v>583449953.48</v>
+        <v>759597627.67</v>
       </c>
       <c r="F34" t="n">
-        <v>248065.4564115646</v>
+        <v>287617.4281219235</v>
       </c>
       <c r="G34" t="n">
-        <v>150000</v>
+        <v>156231</v>
       </c>
       <c r="H34" t="n">
-        <v>2504182.648527233</v>
+        <v>2616782.627464738</v>
       </c>
       <c r="I34" t="n">
-        <v>6270930737184.869</v>
+        <v>6847551319401.256</v>
       </c>
       <c r="J34" t="n">
         <v>0</v>
@@ -3460,7 +3460,7 @@
         <v>0</v>
       </c>
       <c r="O34" t="n">
-        <v>243</v>
+        <v>265</v>
       </c>
       <c r="P34" t="n">
         <v>0</v>
@@ -3475,7 +3475,7 @@
       </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>221925.000000</t>
+          <t>20800000.000000</t>
         </is>
       </c>
       <c r="T34" t="n">
@@ -3483,20 +3483,20 @@
       </c>
       <c r="U34" t="inlineStr"/>
       <c r="V34" t="n">
-        <v>243</v>
+        <v>265</v>
       </c>
       <c r="W34" t="n">
         <v>0</v>
       </c>
       <c r="X34" t="n">
-        <v>28794</v>
+        <v>32427</v>
       </c>
       <c r="Y34" t="n">
-        <v>1412</v>
+        <v>1580</v>
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>['0.000000', '1.000000', '1000.000000', '10000.000000', '100000.000000', '1000000.000000', '10001.000000', '100113.000000', '100500.000000', '10100.000000', '10110.000000', '101700.000000', '10195.000000', '10200.000000', '10325.910000', '10350.000000', '10360.000000', '104351534.000000', '10490.000000', '10500.000000', '105000.000000', '10510.000000', '105200.000000', '105250.000000', '10593.000000', '10600.000000', '10680.000000', '10775.000000', '10775.280000', '10790.000000', '10800.000000', '10845.000000', '10850.000000', '10864.000000', '10900.000000', '109000.000000', '10950.000000', '10966.930000', '11000.000000', '110500.000000', '110952.000000', '11100.000000', '11200.000000', '11250.000000', '11272.000000', '11300.000000', '11350.000000', '11361.000000', '113800.000000', '11400.000000', '11428.010000', '11452.000000', '11500.000000', '115000.000000', '115850.000000', '11600.000000', '116000.000000', '11680.000000', '11700.000000', '117000.000000', '11715.000000', '11720.000000', '11760.000000', '117700.000000', '11775.000000', '11780.000000', '11787.000000', '11800.000000', '11842.000000', '11860.000000', '11870.000000', '11880.000000', '11881.000000', '11890.000000', '11900.000000', '119000.000000', '119113.000000', '11922.000000', '11936.000000', '11972.000000', '11980.000000', '11990.000000', '11999.000000', '1200.000000', '12000.000000', '120000.000000', '1200000.000000', '12026.900000', '12140.000000', '12200.070000', '12280.000000', '12324.210000', '12331.420000', '12331.770000', '12390.000000', '12400.000000', '124980.000000', '12500.000000', '125000.000000', '12500000.000000', '12570.000000', '12577.890000', '12586.810000', '126900.000000', '127500.000000', '129758.000000', '1299.000000', '1300.000000', '13000.000000', '130000.000000', '131189.000000', '13200.000000', '13240.000000', '134315.000000', '1349.000000', '13500.000000', '13585.000000', '136272.000000', '13760.000000', '13772.000000', '137995.000000', '13800.000000', '13827.000000', '13950.000000', '13970.000000', '13980.860000', '14000.000000', '140000.000000', '140427.000000', '141300.000000', '141930.000000', '141990.000000', '14275.000000', '142896.000000', '14300.000000', '143000.000000', '14490.000000', '145000.000000', '1450000.000000', '145151.000000', '145347.000000', '146200.000000', '146709.000000', '146810.000000', '146860.000000', '14900.000000', '149788.000000', '14985.000000', '1500.000000', '15000.000000', '150000.000000', '1500000.000000', '150636.000000', '15070.000000', '150880.000000', '151000.000000', '151322.000000', '15133.370000', '151379.000000', '151570.000000', '151642.000000', '151768.000000', '1523.000000', '152766.000000', '15350.000000', '15358.000000', '15392.610000', '154105.000000', '154703.000000', '1547917.000000', '15500.000000', '155162.000000', '15525.000000', '155304.000000', '155308.000000', '155375.000000', '155766.000000', '155800.000000', '156270.000000', '156353.000000', '156431.000000', '156952.000000', '157421.000000', '157667.000000', '157860.000000', '158046.000000', '158387.000000', '158512.000000', '159000.000000', '159553.000000', '159824.000000', '159896.000000', '159950.000000', '1600.000000', '16000.000000', '160000.000000', '160197.000000', '160665.000000', '160930.000000', '16100.000000', '161000.000000', '161007.000000', '16151.000000', '161768.000000', '16187.620000', '162000.000000', '162111.000000', '162309.000000', '162719.000000', '163130.000000', '16319.320000', '163229.000000', '16360.000000', '164200.000000', '164328.000000', '164637.000000', '164692.000000', '164836.000000', '164900.000000', '1650.000000', '16500.000000', '165226.000000', '165283.000000', '165563.000000', '16590.000000', '166000.000000', '166111.000000', '166180.000000', '166287.000000', '166420.000000', '166620.000000', '166839.000000', '16700.000000', '167000.000000', '167699.000000', '1680000.000000', '168400.000000', '168485.000000', '168495.000000', '168628.000000', '168732.000000', '168737.000000', '168774.000000', '168801.000000', '169000.000000', '169185.000000', '169495.000000', '1695.000000', '169531.000000', '169705.000000', '169740.000000', '16990.000000', '169933.000000', '1700.000000', '17000.000000', '170000.000000', '170258.000000', '170274.000000', '170521.000000', '170805.000000', '170889.000000', '170931.000000', '171000.000000', '17145.000000', '17147.000000', '171981.000000', '17200.000000', '172225.000000', '172543.000000', '172722.000000', '172757.000000', '173000.000000', '173007.000000', '173044.000000', '173091.000000', '173168.000000', '173315.000000', '173350.000000', '173441.000000', '173518.000000', '174660.000000', '174900.000000', '175200.000000', '175290.000000', '175298.000000', '175401.000000', '175500.000000', '175610.000000', '175900.000000', '175908.000000', '176340.000000', '176402.000000', '176442.000000', '176885.000000', '176939.000000', '177000.000000', '177008.000000', '177021.000000', '177121.000000', '177285.000000', '177330.000000', '17750.000000', '177978.000000', '178000.000000', '178021.000000', '178034.000000', '178289.000000', '17830.000000', '178500.000000', '178675.000000', '17900.000000', '179092.000000', '179200.000000', '179249.000000', '179541.000000', '179551.000000', '179827.000000', '179863.000000', '179934.000000', '179992.000000', '180.000000', '1800.000000', '18000.000000', '180000.000000', '1800000.000000', '180346.000000', '180408.000000', '180773.000000', '180867.000000', '180934.000000', '181000.000000', '181083.000000', '181098.000000', '181232.000000', '181459.000000', '181529.000000', '181837.000000', '181915.000000', '182000.000000', '182003.000000', '182132.000000', '182223.000000', '182250.000000', '182336.000000', '18249.000000', '182575.000000', '182605.000000', '182645.000000', '182768.000000', '182800.000000', '182961.000000', '183052.000000', '183235.000000', '183294.000000', '183311.000000', '183380.000000', '183508.000000', '183894.000000', '183925.000000', '184000.000000', '184018.000000', '184026.000000', '184109.000000', '184114.000000', '184322.000000', '184426.000000', '184472.000000', '184500.000000', '184563.000000', '184657.000000', '184881.000000', '1850.000000', '18500.000000', '185000.000000', '185003.000000', '185119.000000', '185129.000000', '185438.000000', '185458.000000', '18572.000000', '185880.000000', '186000.000000', '186155.000000', '186165.000000', '186400.000000', '186662.000000', '186713.000000', '18683.000000', '186903.000000', '186988.000000', '18700.000000', '187109.000000', '187226.000000', '187258.000000', '187303.000000', '187544.000000', '187992.000000', '188000.000000', '188085.000000', '188172.000000', '188251.000000', '188598.000000', '188719.000000', '188720.000000', '188814.000000', '188835.000000', '189043.000000', '189265.000000', '189500.000000', '1896.000000', '189692.000000', '18990.000000', '189917.000000', '19000.000000', '190000.000000', '1900000.000000', '190044.000000', '190213.000000', '190337.000000', '190343.000000', '190476.000000', '190508.000000', '190672.000000', '190714.000000', '190972.000000', '19100.000000', '191014.000000', '191132.000000', '191297.000000', '191680.000000', '191926.000000', '191969.000000', '19200.000000', '192000.000000', '192045.000000', '192257.000000', '192417.000000', '192803.000000', '192828.000000', '192926.000000', '193000.000000', '193019.000000', '193442.000000', '193475.000000', '193500.000000', '193891.000000', '193977.000000', '194000.000000', '194067.000000', '194072.000000', '194297.000000', '194480.000000', '194739.000000', '194868.000000', '194900.000000', '19500.000000', '195000.000000', '195214.000000', '195223.000000', '195247.000000', '195348.000000', '195500.000000', '195780.000000', '196315.000000', '196375.000000', '196635.000000', '196673.000000', '196753.000000', '196890.000000', '197081.000000', '197253.000000', '197320.000000', '197612.000000', '197915.000000', '19794.000000', '197945.000000', '197957.000000', '197962.000000', '198000.000000', '198084.000000', '198550.000000', '198608.000000', '198861.000000', '198920.000000', '199000.000000', '199029.000000', '199074.000000', '199408.000000', '199481.000000', '199489.000000', '199503.000000', '19964.000000', '199732.000000', '199768.000000', '199900.000000', '199955.000000', '20.000000', '2000.000000', '20000.000000', '200000.000000', '200070.000000', '200080.000000', '200151.000000', '200360.000000', '200400.000000', '200496.000000', '200611.000000', '201000.000000', '201500.000000', '201664.000000', '201680.000000', '201916.000000', '20200.000000', '2020275.000000', '202312.000000', '202443.000000', '202445.000000', '202583.000000', '20278.000000', '203000.000000', '203132.000000', '203211.000000', '203297.000000', '203300.000000', '203500.000000', '203548.000000', '203634.000000', '203780.000000', '203800.000000', '204324.000000', '204543.000000', '204585.000000', '204696.000000', '204770.000000', '205000.000000', '205017.000000', '205087.000000', '205500.000000', '205558.000000', '205590.000000', '205765.000000', '206000.000000', '206315.000000', '206388.000000', '206524.000000', '206689.000000', '206693.000000', '206694.000000', '206775.000000', '206895.000000', '207000.000000', '207050.000000', '207058.000000', '207090.000000', '207182.000000', '207211.000000', '207234.000000', '207346.000000', '207384.000000', '2074.000000', '207443.000000', '207451.000000', '2079.000000', '2080.000000', '208000.000000', '208035.000000', '208146.000000', '208200.000000', '208395.000000', '209114.000000', '209116.000000', '209144.000000', '209146.000000', '209153.000000', '209178.000000', '209239.000000', '209295.000000', '209297.000000', '209370.000000', '209430.000000', '209625.000000', '20965.000000', '209656.000000', '209830.000000', '209907.000000', '209927.000000', '209956.000000', '2100.000000', '21000.000000', '210000.000000', '210174.000000', '210312.000000', '210368.000000', '210385.000000', '210393.000000', '210521.000000', '210609.000000', '211000.000000', '211064.000000', '211133.000000', '211250.000000', '211260.000000', '211344.000000', '211386.000000', '211457.000000', '211618.000000', '211665.000000', '211691.000000', '211730.000000', '211900.000000', '211923.000000', '211955.000000', '212000.000000', '212374.000000', '212453.000000', '212480.000000', '212546.000000', '212651.000000', '213065.000000', '213350.000000', '213500.000000', '21354.000000', '213604.000000', '213618.000000', '213632.000000', '213826.000000', '214000.000000', '214290.000000', '214790.000000', '214900.000000', '214919.000000', '2150.000000', '215000.000000', '215073.000000', '215115.000000', '215192.000000', '215390.000000', '215418.000000', '215497.000000', '216000.000000', '216106.000000', '216700.000000', '216843.000000', '217008.000000', '217200.000000', '217925.000000', '218000.000000', '218228.000000', '2184.000000', '218484.000000', '218504.000000', '218546.000000', '218579.000000', '218645.000000', '218694.000000', '218819.000000', '2190.000000', '219000.000000', '219126.000000', '219265.000000', '219341.000000', '219408.000000', '219457.000000', '219470.000000', '219488.000000', '219703.000000', '2200.000000', '22000.000000', '220000.000000', '220024.000000', '220237.000000', '220407.000000', '220566.000000', '2206.000000', '220692.000000', '220900.000000', '220990.000000', '221000.000000', '221111.000000', '221528.000000', '221612.000000', '221636.000000', '221900.000000', '221925.000000', '222000.000000', '222045.000000', '222296.000000', '22285.000000', '223098.000000', '223259.000000', '223650.000000', '22389.000000', '224015.000000', '224077.000000', '224192.000000', '224286.000000', '224290.000000', '224481.000000', '224631.000000', '224646.000000', '224825.000000', '224834.000000', '224900.000000', '224901.000000', '22500.000000', '225000.000000', '2253.420000', '225467.000000', '225813.000000', '22590.000000', '226074.000000', '226349.000000', '226650.000000', '226667.000000', '226692.000000', '226872.000000', '227026.000000', '228000.000000', '228035.000000', '228278.000000', '228291.000000', '228295.000000', '228329.000000', '228553.000000', '228597.000000', '228600.000000', '2290.000000', '229000.000000', '229133.000000', '229332.000000', '229333.000000', '229410.000000', '229486.000000', '229670.000000', '229729.000000', '229867.000000', '229900.000000', '2300.000000', '23000.000000', '230000.000000', '230107.000000', '230200.000000', '230375.000000', '230476.000000', '230513.000000', '23060.000000', '230635.000000', '230648.000000', '230849.000000', '230963.000000', '231000.000000', '231459.000000', '231500.000000', '231627.000000', '231800.000000', '231802.000000', '231975.000000', '232022.000000', '232033.000000', '232317.000000', '232617.000000', '232967.000000', '233250.000000', '233382.000000', '233500.000000', '2340.000000', '234482.000000', '234500.000000', '234563.000000', '234592.000000', '234900.000000', '234933.000000', '234976.000000', '235000.000000', '235103.000000', '235350.000000', '235424.000000', '235759.000000', '235909.000000', '236162.000000', '236181.000000', '236197.000000', '236291.000000', '236492.000000', '236512.000000', '236845.000000', '236904.000000', '2371.000000', '237169.000000', '237171.000000', '237287.000000', '237290.000000', '237378.000000', '237402.000000', '237423.000000', '237837.000000', '237851.000000', '237925.000000', '238007.000000', '238212.000000', '238487.000000', '238512.000000', '238602.000000', '238603.000000', '238675.000000', '238782.000000', '239191.000000', '239213.000000', '239229.000000', '239238.000000', '239496.000000', '239623.000000', '23965.000000', '239960.000000', '2400.000000', '24000.000000', '240000.000000', '240500.000000', '240667.000000', '240705.000000', '241000.000000', '241017.000000', '241213.000000', '241245.000000', '241621.000000', '241686.000000', '241750.000000', '241774.000000', '24202.000000', '242047.000000', '242076.000000', '242188.000000', '242208.000000', '242259.000000', '242291.000000', '242426.000000', '242444.000000', '242491.000000', '242621.000000', '242646.000000', '243337.000000', '243345.000000', '243363.000000', '243383.000000', '243533.000000', '24370.000000', '243705.000000', '243799.000000', '244098.000000', '244105.000000', '244326.000000', '244756.000000', '244987.000000', '245000.000000', '245131.000000', '245302.000000', '245479.000000', '245645.000000', '245811.000000', '245989.000000', '246085.000000', '246137.000000', '246454.000000', '246573.000000', '246855.000000', '246938.000000', '246999.000000', '247203.000000', '247219.000000', '247323.000000', '247501.000000', '247900.000000', '247975.000000', '247979.000000', '248110.000000', '248200.000000', '248308.000000', '249385.000000', '249563.000000', '249800.000000', '249988.000000', '2500.000000', '25000.000000', '250000.000000', '250234.000000', '250492.000000', '251322.000000', '251768.000000', '252000.000000', '252071.000000', '252125.000000', '252490.000000', '252543.000000', '25263.000000', '252659.000000', '252729.000000', '253000.000000', '253025.000000', '253152.000000', '253387.000000', '253749.000000', '25375.000000', '254377.000000', '254747.000000', '25480.000000', '254832.000000', '254869.000000', '2550.000000', '255133.000000', '255683.000000', '256930.000000', '256964.000000', '257680.000000', '25800.000000', '258374.000000', '258482.000000', '258809.000000', '258990.000000', '259373.000000', '259622.000000', '259809.000000', '259998.000000', '2600.000000', '26000.000000', '260000.000000', '260289.000000', '260351.000000', '260362.000000', '260807.000000', '261000.000000', '2611.650000', '261677.000000', '261797.000000', '262091.000000', '262375.000000', '2629.000000', '262944.000000', '262955.000000', '263000.000000', '263011.000000', '263050.000000', '263133.000000', '263382.000000', '263839.000000', '26400.000000', '264317.000000', '26499.000000', '265042.000000', '265156.000000', '265220.000000', '265657.000000', '265709.000000', '266084.000000', '267420.000000', '267502.000000', '267719.000000', '2678.000000', '267894.000000', '26800.000000', '268321.000000', '268637.000000', '268856.000000', '268965.000000', '269274.000000', '269276.000000', '269288.000000', '2700.000000', '27000.000000', '270000.000000', '270121.000000', '270243.000000', '270973.000000', '271566.000000', '271791.000000', '271995.000000', '272147.000000', '2725.000000', '272833.000000', '27290.000000', '2731.000000', '274011.000000', '274508.000000', '274822.000000', '27500.000000', '275000.000000', '275294.000000', '275527.000000', '275541.000000', '276729.000000', '276751.000000', '276753.000000', '277134.000000', '278826.000000', '279019.000000', '2800.000000', '28000.000000', '280000.000000', '280294.000000', '280351.000000', '281288.000000', '281500.000000', '281866.000000', '281874.000000', '282000.000000', '282900.000000', '283000.000000', '283022.000000', '2832.000000', '284050.000000', '284393.000000', '284525.000000', '284560.000000', '285154.000000', '286972.000000', '287000.000000', '287725.000000', '28780.000000', '288000.000000', '288157.000000', '288822.000000', '289206.000000', '289277.000000', '289680.000000', '289800.000000', '290.000000', '2900.000000', '29000.000000', '29169.000000', '292741.000000', '292973.000000', '293360.000000', '293422.000000', '294700.000000', '295020.000000', '29561.000000', '29568.000000', '295752.000000', '296000.000000', '296019.000000', '296088.000000', '296265.000000', '296347.000000', '297276.000000', '29731.000000', '297701.000000', '29800.000000', '29952.000000', '299974.000000', '3000.000000', '30000.000000', '300000.000000', '3000000.000000', '30000000.000000', '300094.000000', '300378.000000', '30060.000000', '301344.000000', '301565.000000', '30231350.000000', '303212.000000', '305941.000000', '306000.000000', '309010.000000', '30989.000000', '3100.000000', '310000.000000', '3102.000000', '310892.000000', '3111.000000', '311633.000000', '311746.000000', '311792.000000', '312956.000000', '314400.000000', '314546.000000', '314587.000000', '315939.000000', '31600.000000', '316855.000000', '318000.000000', '31880.000000', '319348.000000', '3200.000000', '320000.000000', '320300.000000', '321025.000000', '326220.000000', '32900.000000', '329325.000000', '329479.000000', '3300.000000', '3300000.000000', '332293.000000', '3323.000000', '332383.000000', '332858.000000', '333249.000000', '335171.000000', '335867.000000', '3382.000000', '338550.000000', '3400.000000', '34000.000000', '340000.000000', '34126.610000', '34132.000000', '341676.000000', '342000.000000', '344871.000000', '3450.000000', '34500.000000', '3480.000000', '3500.000000', '35000.000000', '350000.000000', '3500000.000000', '355000.000000', '356692.000000', '35800.000000', '358265.000000', '35879.000000', '3600.000000', '36000.000000', '361000.000000', '365000.000000', '365455.000000', '365764.000000', '36625.000000', '369568.000000', '3700.000000', '37000.000000', '371297.000000', '37130.000000', '37229.000000', '3725.000000', '37350.000000', '37460.000000', '37500.000000', '375208.000000', '3777.000000', '378000.000000', '37835.000000', '3793.000000', '3800.000000', '380000.000000', '381057.000000', '3826000.000000', '38500.000000', '38894.000000', '3900.000000', '39000.000000', '390000.000000', '391760.000000', '3926.510000', '39300.000000', '396000.000000', '39960.000000', '4000.000000', '40000.000000', '400000.000000', '4024.000000', '403040.000000', '4046.000000', '40577.000000', '4065.000000', '409230.000000', '4100.000000', '41000.000000', '4130.000000', '41400.000000', '4150.000000', '41700.000000', '4180.000000', '41800.000000', '4200.000000', '42000.000000', '421000.000000', '4235.000000', '4250.000000', '42500.000000', '4270.000000', '4275.000000', '4290.000000', '4300.000000', '43000.000000', '4350.000000', '43500.000000', '4352.000000', '43600.000000', '4400.000000', '444928.000000', '4450.000000', '445900.000000', '4490.000000', '4500.000000', '45000.000000', '450000.000000', '45570.000000', '45750.000000', '45800.000000', '458102.000000', '4590.000000', '4600.000000', '46000.000000', '463356.000000', '4641.000000', '465143.000000', '466157.000000', '466880.000000', '4690.000000', '46900.000000', '4700.000000', '4720.000000', '47436.000000', '47500.000000', '47800.000000', '4781.000000', '4790.000000', '4792.000000', '4800.000000', '4850.000000', '4865.000000', '4878.000000', '4888.000000', '48928.000000', '4893.000000', '4895.000000', '4900.000000', '4910.000000', '49170.000000', '4925.000000', '4930.000000', '4932.000000', '4950.000000', '4969.000000', '4985.000000', '4990.000000', '4995.000000', '4999.000000', '5000.000000', '50000.000000', '500000.000000', '5000000.000000', '50352.000000', '50586.000000', '5080.000000', '5090.000000', '5100.000000', '5140.000000', '51900.000000', '5200.000000', '5250.000000', '52760.000000', '5300.000000', '5316.000000', '5372.000000', '5400.000000', '5460.000000', '5500.000000', '550000.000000', '5580.000000', '5695.000000', '5700.000000', '575000.000000', '5760.000000', '5800.000000', '582645.000000', '5900.000000', '590000.000000', '593083.000000', '5942.000000', '5952.000000', '5980.000000', '599890.000000', '600.000000', '6000.000000', '60000.000000', '600000.000000', '6023.000000', '6038.000000', '6082.000000', '6100.000000', '61000.000000', '6109.000000', '6117.000000', '614347.000000', '6158.000000', '6200.000000', '62000.000000', '6210.000000', '6250.000000', '6300.000000', '6325.000000', '6370.000000', '6380.000000', '6400.000000', '640000.000000', '6500.000000', '65000.000000', '650000.000000', '6550.000000', '6572.000000', '6590.000000', '6600.000000', '663527.000000', '666863.000000', '6725.000000', '6740.000000', '6800.000000', '6820.000000', '6830.000000', '6870.000000', '6890.000000', '6900.000000', '6951.000000', '6990.000000', '700.000000', '7000.000000', '70000.000000', '700000.000000', '70190.000000', '70943.870000', '7098.000000', '71086.000000', '7114.000000', '7150.000000', '7170.000000', '7200.000000', '72485.000000', '7250.000000', '732312.000000', '7370.000000', '73746.000000', '7400.000000', '7410.000000', '7411.800000', '7428.000000', '7430.000000', '7435.000000', '7476.000000', '7484.000000', '7500.000000', '7523.910000', '7600.000000', '7670.000000', '7700.000000', '7772.000000', '7800.000000', '7850.000000', '7855.000000', '7870.000000', '7886.000000', '7900.000000', '7910.000000', '7947.000000', '7987.000000', '800.000000', '8000.000000', '80000.000000', '8050.000000', '80972.000000', '8100.000000', '8120.000000', '8190.000000', '8200.000000', '8205.000000', '8300.000000', '83400.000000', '8455.000000', '8500.000000', '850000.000000', '8600.000000', '86000.000000', '86197.000000', '862000.000000', '8700.000000', '8715.000000', '8794.000000', '8800.000000', '890.000000', '8900.000000', '8960.000000', '900.000000', '9000.000000', '90000.000000', '900000.000000', '9100.000000', '9200.000000', '9240.000000', '9300.000000', '9306.000000', '9330.000000', '9391.000000', '9400.000000', '9448.000000', '9500.000000', '95000.000000', '9600.000000', '9700.000000', '9721.000000', '9800.000000', '980000.000000', '9850.000000', '9870.000000', '9893.000000', '9900.000000', '99000.000000', '9930.000000', '9935.000000', '9950.000000', '9961.000000', '9990.000000']</t>
+          <t>['0.000000', '1.000000', '1000.000000', '10000.000000', '100000.000000', '1000000.000000', '10001.000000', '100113.000000', '100500.000000', '10100.000000', '10110.000000', '101700.000000', '10195.000000', '10200.000000', '10325.910000', '10350.000000', '10360.000000', '104351534.000000', '10490.000000', '10500.000000', '105000.000000', '10510.000000', '105200.000000', '105250.000000', '10593.000000', '10600.000000', '10680.000000', '10775.000000', '10775.280000', '10790.000000', '10800.000000', '10845.000000', '10850.000000', '10864.000000', '10900.000000', '109000.000000', '10950.000000', '10966.930000', '11000.000000', '110500.000000', '110952.000000', '11100.000000', '11200.000000', '11250.000000', '11272.000000', '11300.000000', '11350.000000', '11357.000000', '11361.000000', '113800.000000', '11400.000000', '114000.000000', '11428.010000', '11452.000000', '11500.000000', '115000.000000', '115850.000000', '11600.000000', '116000.000000', '11680.000000', '11700.000000', '117000.000000', '11715.000000', '11720.000000', '11760.000000', '117700.000000', '11775.000000', '11780.000000', '11787.000000', '11800.000000', '11842.000000', '11860.000000', '11870.000000', '11872.000000', '11880.000000', '11881.000000', '11890.000000', '11900.000000', '119000.000000', '119113.000000', '11922.000000', '11936.000000', '11972.000000', '11980.000000', '11990.000000', '11999.000000', '1200.000000', '12000.000000', '120000.000000', '1200000.000000', '12026.900000', '121200.000000', '12140.000000', '12200.070000', '12280.000000', '12324.210000', '12331.420000', '12331.770000', '12390.000000', '12400.000000', '124980.000000', '12500.000000', '125000.000000', '12500000.000000', '12570.000000', '12577.890000', '12586.810000', '126900.000000', '127500.000000', '129758.000000', '1299.000000', '1300.000000', '13000.000000', '130000.000000', '131189.000000', '13200.000000', '132000.000000', '13240.000000', '134315.000000', '1349.000000', '13500.000000', '13585.000000', '136272.000000', '13760.000000', '13772.000000', '137995.000000', '13800.000000', '13827.000000', '13950.000000', '13970.000000', '13980.860000', '14000.000000', '140000.000000', '140427.000000', '141300.000000', '141930.000000', '141990.000000', '142000.000000', '142386.000000', '14275.000000', '142896.000000', '14300.000000', '143000.000000', '14490.000000', '145000.000000', '1450000.000000', '145151.000000', '145347.000000', '146200.000000', '146709.000000', '146810.000000', '146860.000000', '14900.000000', '149788.000000', '14985.000000', '1500.000000', '15000.000000', '150000.000000', '1500000.000000', '150636.000000', '15070.000000', '150880.000000', '151000.000000', '151322.000000', '15133.370000', '151379.000000', '151570.000000', '151642.000000', '151768.000000', '15200.000000', '1523.000000', '152700.000000', '152766.000000', '15350.000000', '15358.000000', '15392.610000', '154105.000000', '154703.000000', '1547917.000000', '15500.000000', '155162.000000', '15525.000000', '155304.000000', '155308.000000', '155375.000000', '155766.000000', '155800.000000', '156231.000000', '156270.000000', '156353.000000', '156431.000000', '156952.000000', '157421.000000', '157667.000000', '157860.000000', '158046.000000', '158110.000000', '158387.000000', '158512.000000', '158759.000000', '159000.000000', '159553.000000', '159824.000000', '159896.000000', '159950.000000', '1600.000000', '16000.000000', '160000.000000', '160022.000000', '160038.000000', '160197.000000', '160665.000000', '160930.000000', '16100.000000', '161000.000000', '161007.000000', '16151.000000', '161768.000000', '16187.620000', '162000.000000', '162111.000000', '162309.000000', '162719.000000', '163130.000000', '163140.000000', '16319.320000', '163229.000000', '16336.000000', '163485.000000', '16360.000000', '164200.000000', '164328.000000', '164637.000000', '164692.000000', '164836.000000', '164883.000000', '164900.000000', '1650.000000', '16500.000000', '165000.000000', '165226.000000', '165243.000000', '165283.000000', '165563.000000', '16590.000000', '166000.000000', '166111.000000', '166180.000000', '166287.000000', '166329.000000', '166420.000000', '166620.000000', '166839.000000', '16700.000000', '167000.000000', '167699.000000', '1680000.000000', '168400.000000', '168485.000000', '168495.000000', '168628.000000', '168732.000000', '168737.000000', '168774.000000', '168801.000000', '169000.000000', '169126.000000', '169185.000000', '169495.000000', '1695.000000', '169530.000000', '169531.000000', '169705.000000', '169740.000000', '16990.000000', '169933.000000', '1700.000000', '17000.000000', '170000.000000', '170258.000000', '170274.000000', '170393.000000', '170521.000000', '170805.000000', '170889.000000', '170931.000000', '171000.000000', '17145.000000', '17147.000000', '171981.000000', '17200.000000', '172225.000000', '172333.000000', '172543.000000', '172722.000000', '172757.000000', '173000.000000', '173007.000000', '173044.000000', '173091.000000', '173168.000000', '173315.000000', '173350.000000', '173441.000000', '173518.000000', '174660.000000', '17485.000000', '174900.000000', '175132.000000', '175200.000000', '175290.000000', '175298.000000', '175401.000000', '175500.000000', '175610.000000', '175649.000000', '175825.000000', '175900.000000', '175908.000000', '176148.000000', '17618.000000', '176340.000000', '176402.000000', '176442.000000', '176885.000000', '176939.000000', '177000.000000', '177008.000000', '177011.000000', '177021.000000', '177121.000000', '177285.000000', '177330.000000', '17750.000000', '177600.000000', '177978.000000', '178000.000000', '178021.000000', '178034.000000', '178289.000000', '17830.000000', '178350.000000', '178500.000000', '178530.000000', '178675.000000', '17900.000000', '179092.000000', '179200.000000', '179249.000000', '179541.000000', '179551.000000', '179827.000000', '179863.000000', '179934.000000', '179992.000000', '180.000000', '1800.000000', '18000.000000', '180000.000000', '1800000.000000', '180346.000000', '180408.000000', '180773.000000', '180867.000000', '180934.000000', '181000.000000', '181083.000000', '181098.000000', '181232.000000', '181459.000000', '181529.000000', '181837.000000', '181915.000000', '182000.000000', '182003.000000', '182132.000000', '182223.000000', '182250.000000', '182336.000000', '18248.000000', '18249.000000', '182525.000000', '182575.000000', '182605.000000', '182645.000000', '182768.000000', '182800.000000', '182892.000000', '182961.000000', '183052.000000', '183235.000000', '183294.000000', '183311.000000', '183380.000000', '183508.000000', '183825.000000', '183894.000000', '183925.000000', '184000.000000', '184018.000000', '184026.000000', '184031.000000', '184067.000000', '184109.000000', '184114.000000', '184322.000000', '184426.000000', '184472.000000', '184495.000000', '184500.000000', '184550.000000', '184563.000000', '184657.000000', '184843.000000', '184881.000000', '1850.000000', '18500.000000', '185000.000000', '185003.000000', '185119.000000', '185129.000000', '185438.000000', '185458.000000', '18572.000000', '185880.000000', '186000.000000', '186155.000000', '186165.000000', '186400.000000', '186662.000000', '186713.000000', '18683.000000', '186903.000000', '186988.000000', '18700.000000', '187101.000000', '187109.000000', '187226.000000', '187258.000000', '187303.000000', '187544.000000', '187800.000000', '187992.000000', '188000.000000', '188085.000000', '188172.000000', '188251.000000', '188385.000000', '188598.000000', '188719.000000', '188720.000000', '188814.000000', '188835.000000', '189043.000000', '189265.000000', '189500.000000', '1896.000000', '189692.000000', '18990.000000', '189917.000000', '19000.000000', '190000.000000', '1900000.000000', '190044.000000', '190176.000000', '190213.000000', '190337.000000', '190343.000000', '190476.000000', '190508.000000', '190672.000000', '190714.000000', '190972.000000', '19100.000000', '191000.000000', '191014.000000', '191132.000000', '191297.000000', '191514.000000', '191680.000000', '191926.000000', '191969.000000', '19200.000000', '192000.000000', '192045.000000', '192257.000000', '192417.000000', '192420.000000', '192803.000000', '192828.000000', '192926.000000', '193000.000000', '193019.000000', '193172.000000', '193442.000000', '193475.000000', '193500.000000', '193777.000000', '193891.000000', '193977.000000', '194000.000000', '194067.000000', '194072.000000', '194297.000000', '194480.000000', '194531.000000', '194739.000000', '194868.000000', '194900.000000', '19500.000000', '195000.000000', '195214.000000', '195223.000000', '195247.000000', '195348.000000', '195500.000000', '195780.000000', '196315.000000', '196375.000000', '196620.000000', '196635.000000', '196673.000000', '196753.000000', '196879.000000', '196890.000000', '197081.000000', '197253.000000', '197320.000000', '197480.000000', '197612.000000', '197915.000000', '19794.000000', '197945.000000', '197957.000000', '197962.000000', '198000.000000', '198029.000000', '198084.000000', '198550.000000', '198580.000000', '198608.000000', '198721.000000', '198861.000000', '198920.000000', '199000.000000', '199029.000000', '199074.000000', '199408.000000', '199457.000000', '199481.000000', '199489.000000', '199503.000000', '19964.000000', '199732.000000', '199768.000000', '199801.000000', '199820.000000', '199900.000000', '199955.000000', '2.000000', '20.000000', '2000.000000', '20000.000000', '200000.000000', '200070.000000', '200080.000000', '200151.000000', '200360.000000', '200400.000000', '200496.000000', '200611.000000', '200694.000000', '200801.000000', '201000.000000', '201377.000000', '201500.000000', '201664.000000', '201680.000000', '201916.000000', '201918.000000', '20200.000000', '2020275.000000', '202312.000000', '202380.000000', '202443.000000', '202445.000000', '202583.000000', '20278.000000', '203000.000000', '203034.000000', '203132.000000', '203211.000000', '203297.000000', '203300.000000', '203500.000000', '203548.000000', '203634.000000', '203780.000000', '203800.000000', '204324.000000', '204543.000000', '204585.000000', '204696.000000', '204757.000000', '204770.000000', '205000.000000', '205017.000000', '205087.000000', '205500.000000', '205558.000000', '205590.000000', '205765.000000', '205993.000000', '206000.000000', '206315.000000', '206388.000000', '206524.000000', '206689.000000', '206693.000000', '206694.000000', '206775.000000', '206895.000000', '207000.000000', '207050.000000', '207058.000000', '207090.000000', '207182.000000', '207211.000000', '207234.000000', '207346.000000', '207384.000000', '2074.000000', '207443.000000', '207451.000000', '2079.000000', '2080.000000', '208000.000000', '20800000.000000', '208035.000000', '208146.000000', '208200.000000', '208395.000000', '208470.000000', '209114.000000', '209116.000000', '209144.000000', '209146.000000', '209153.000000', '209178.000000', '209239.000000', '209295.000000', '209297.000000', '209370.000000', '209430.000000', '209600.000000', '209625.000000', '20965.000000', '209656.000000', '209830.000000', '209907.000000', '209927.000000', '209956.000000', '2100.000000', '21000.000000', '210000.000000', '210174.000000', '210312.000000', '210368.000000', '210385.000000', '210393.000000', '210521.000000', '210609.000000', '211000.000000', '211064.000000', '211133.000000', '211250.000000', '211260.000000', '211344.000000', '211386.000000', '211457.000000', '211590.000000', '211618.000000', '211665.000000', '211691.000000', '211730.000000', '211857.000000', '211900.000000', '211923.000000', '211955.000000', '212000.000000', '212374.000000', '212453.000000', '212480.000000', '212546.000000', '212651.000000', '213000.000000', '213065.000000', '213184.000000', '213350.000000', '213500.000000', '21354.000000', '213604.000000', '213618.000000', '213632.000000', '213826.000000', '214000.000000', '214290.000000', '214790.000000', '214900.000000', '214919.000000', '2150.000000', '215000.000000', '215073.000000', '215115.000000', '215192.000000', '215390.000000', '215418.000000', '215497.000000', '215965.000000', '216000.000000', '216106.000000', '216700.000000', '216843.000000', '217008.000000', '217200.000000', '217493.000000', '217925.000000', '218000.000000', '218228.000000', '218358.000000', '2184.000000', '218484.000000', '218504.000000', '218546.000000', '218579.000000', '218645.000000', '218694.000000', '218819.000000', '218896.000000', '2190.000000', '219000.000000', '219014.000000', '219126.000000', '219265.000000', '219341.000000', '219408.000000', '219457.000000', '219470.000000', '219488.000000', '219690.000000', '219703.000000', '219951.000000', '2200.000000', '22000.000000', '220000.000000', '220024.000000', '220237.000000', '220407.000000', '220566.000000', '2206.000000', '220692.000000', '220900.000000', '220990.000000', '221000.000000', '221111.000000', '221528.000000', '221612.000000', '221613.000000', '221636.000000', '221900.000000', '221925.000000', '222000.000000', '222045.000000', '222296.000000', '22285.000000', '223098.000000', '223259.000000', '223650.000000', '22389.000000', '224015.000000', '224077.000000', '224192.000000', '224286.000000', '224290.000000', '224481.000000', '224631.000000', '224646.000000', '224743.000000', '224825.000000', '224834.000000', '224900.000000', '224901.000000', '2250.000000', '22500.000000', '225000.000000', '2253.420000', '225466.000000', '225467.000000', '225813.000000', '22590.000000', '226074.000000', '226349.000000', '226650.000000', '226667.000000', '226692.000000', '226750.000000', '226872.000000', '227026.000000', '227797.000000', '228000.000000', '228035.000000', '228278.000000', '228291.000000', '228295.000000', '228311.000000', '228329.000000', '228553.000000', '228597.000000', '228600.000000', '2290.000000', '229000.000000', '229133.000000', '229315.000000', '229332.000000', '229333.000000', '229410.000000', '229486.000000', '229670.000000', '229729.000000', '229867.000000', '229900.000000', '2300.000000', '23000.000000', '230000.000000', '230107.000000', '230200.000000', '230375.000000', '230476.000000', '230513.000000', '23060.000000', '230635.000000', '230648.000000', '230849.000000', '230963.000000', '231000.000000', '231287.000000', '231459.000000', '231500.000000', '231627.000000', '231800.000000', '231802.000000', '231975.000000', '232022.000000', '232033.000000', '232317.000000', '232323.000000', '232617.000000', '232967.000000', '233167.000000', '233250.000000', '233382.000000', '233500.000000', '233749.000000', '23380.000000', '2340.000000', '234482.000000', '234500.000000', '234563.000000', '234592.000000', '234900.000000', '234933.000000', '234976.000000', '235000.000000', '235103.000000', '235350.000000', '235424.000000', '235468.000000', '235610.000000', '235759.000000', '235821.000000', '235909.000000', '235977.000000', '236162.000000', '236181.000000', '236197.000000', '236291.000000', '236436.000000', '236492.000000', '236512.000000', '236845.000000', '236904.000000', '2371.000000', '237169.000000', '237171.000000', '237287.000000', '237290.000000', '237378.000000', '237402.000000', '237423.000000', '237837.000000', '237851.000000', '237925.000000', '237928.000000', '238007.000000', '238212.000000', '238487.000000', '238512.000000', '238602.000000', '238603.000000', '238675.000000', '238782.000000', '239191.000000', '239213.000000', '239229.000000', '239238.000000', '239496.000000', '239623.000000', '23965.000000', '239960.000000', '2400.000000', '24000.000000', '240000.000000', '240500.000000', '240667.000000', '240705.000000', '240800.000000', '241000.000000', '241017.000000', '241080.000000', '241120.000000', '241213.000000', '241245.000000', '241422.000000', '241621.000000', '241686.000000', '241750.000000', '241774.000000', '241934.000000', '242.000000', '24202.000000', '242047.000000', '242076.000000', '242188.000000', '242208.000000', '242231.000000', '242259.000000', '242291.000000', '242426.000000', '242444.000000', '242491.000000', '242621.000000', '242646.000000', '243337.000000', '243345.000000', '243363.000000', '243383.000000', '243533.000000', '24370.000000', '243705.000000', '243799.000000', '244098.000000', '244105.000000', '244326.000000', '244756.000000', '244822.000000', '244970.000000', '244987.000000', '245000.000000', '245131.000000', '245302.000000', '245360.000000', '245479.000000', '245645.000000', '245811.000000', '245989.000000', '246085.000000', '246137.000000', '246454.000000', '246573.000000', '246855.000000', '246938.000000', '246999.000000', '247170.000000', '247203.000000', '247219.000000', '247323.000000', '247501.000000', '247900.000000', '247975.000000', '247979.000000', '248000.000000', '248110.000000', '248200.000000', '248308.000000', '24900.000000', '249385.000000', '249563.000000', '249800.000000', '249988.000000', '24999.000000', '2500.000000', '25000.000000', '250000.000000', '2500000.000000', '250234.000000', '250492.000000', '251322.000000', '251768.000000', '251903.000000', '252000.000000', '252071.000000', '252125.000000', '252490.000000', '252543.000000', '25263.000000', '252659.000000', '252729.000000', '253000.000000', '253025.000000', '253152.000000', '253387.000000', '253749.000000', '25375.000000', '254377.000000', '254440.000000', '254747.000000', '254792.000000', '25480.000000', '254832.000000', '254869.000000', '2550.000000', '255133.000000', '255683.000000', '256467.000000', '256633.000000', '256930.000000', '256964.000000', '257680.000000', '25800.000000', '258374.000000', '258482.000000', '258809.000000', '258948.000000', '258990.000000', '259048.000000', '259373.000000', '259622.000000', '259809.000000', '259998.000000', '2600.000000', '26000.000000', '260000.000000', '2600000.000000', '260289.000000', '260351.000000', '260362.000000', '260807.000000', '261000.000000', '2611.650000', '261548.000000', '261677.000000', '261687.000000', '261797.000000', '2618.000000', '262091.000000', '262375.000000', '2629.000000', '262944.000000', '262955.000000', '263000.000000', '263011.000000', '263050.000000', '263133.000000', '263382.000000', '263839.000000', '26400.000000', '264317.000000', '26499.000000', '265042.000000', '265156.000000', '265220.000000', '265657.000000', '265709.000000', '266084.000000', '267420.000000', '267502.000000', '267719.000000', '2678.000000', '267894.000000', '267905.000000', '26800.000000', '268321.000000', '268637.000000', '268856.000000', '268965.000000', '268984.000000', '269274.000000', '269276.000000', '269288.000000', '2700.000000', '27000.000000', '270000.000000', '270121.000000', '270243.000000', '270973.000000', '271566.000000', '271791.000000', '271995.000000', '272147.000000', '2725.000000', '272833.000000', '27290.000000', '2731.000000', '274011.000000', '274508.000000', '274822.000000', '27500.000000', '275000.000000', '275294.000000', '275527.000000', '275541.000000', '276729.000000', '276751.000000', '276753.000000', '277134.000000', '277196.000000', '277960.000000', '278070.000000', '278227.000000', '278826.000000', '279019.000000', '2800.000000', '28000.000000', '280000.000000', '280294.000000', '280351.000000', '280967.000000', '281288.000000', '281500.000000', '281866.000000', '281874.000000', '282000.000000', '282900.000000', '283000.000000', '283022.000000', '283067.000000', '2832.000000', '284050.000000', '284393.000000', '284525.000000', '284560.000000', '285154.000000', '286972.000000', '287000.000000', '28713.000000', '287725.000000', '28780.000000', '288000.000000', '288157.000000', '288822.000000', '289206.000000', '289277.000000', '289674.000000', '289680.000000', '289800.000000', '290.000000', '2900.000000', '29000.000000', '29169.000000', '292741.000000', '292973.000000', '293223.000000', '293360.000000', '293422.000000', '294700.000000', '295020.000000', '29561.000000', '29568.000000', '295752.000000', '296000.000000', '296019.000000', '296088.000000', '296265.000000', '296347.000000', '296804.000000', '297276.000000', '29731.000000', '297701.000000', '29800.000000', '298000.000000', '29952.000000', '299974.000000', '3000.000000', '30000.000000', '300000.000000', '3000000.000000', '30000000.000000', '300094.000000', '300378.000000', '30060.000000', '301344.000000', '301565.000000', '30231350.000000', '303212.000000', '304351.000000', '305941.000000', '306000.000000', '308211.000000', '309010.000000', '30989.000000', '3100.000000', '310000.000000', '3102.000000', '310892.000000', '3111.000000', '311633.000000', '311746.000000', '311792.000000', '312956.000000', '313350.000000', '314400.000000', '314546.000000', '314587.000000', '315939.000000', '31600.000000', '316855.000000', '318000.000000', '31880.000000', '319348.000000', '3200.000000', '320000.000000', '320300.000000', '321025.000000', '326220.000000', '32900.000000', '329325.000000', '329479.000000', '3300.000000', '3300000.000000', '33100.000000', '332293.000000', '3323.000000', '332383.000000', '332858.000000', '333249.000000', '33500.000000', '335171.000000', '335867.000000', '3382.000000', '338550.000000', '3400.000000', '34000.000000', '340000.000000', '34126.610000', '34132.000000', '341676.000000', '34200.000000', '342000.000000', '344871.000000', '3450.000000', '34500.000000', '3480.000000', '348868.000000', '3500.000000', '35000.000000', '350000.000000', '3500000.000000', '355000.000000', '355267.000000', '356692.000000', '35800.000000', '358265.000000', '35879.000000', '359168.000000', '3600.000000', '36000.000000', '36000000.000000', '361000.000000', '365000.000000', '365455.000000', '365764.000000', '36625.000000', '369568.000000', '3700.000000', '37000.000000', '371297.000000', '37130.000000', '37229.000000', '3725.000000', '37350.000000', '37460.000000', '37500.000000', '375208.000000', '3777.000000', '378000.000000', '37835.000000', '3793.000000', '3800.000000', '380000.000000', '38090.000000', '381057.000000', '3826000.000000', '38500.000000', '38894.000000', '3900.000000', '39000.000000', '390000.000000', '391760.000000', '3926.510000', '39300.000000', '396000.000000', '39960.000000', '4000.000000', '40000.000000', '400000.000000', '4024.000000', '403040.000000', '4046.000000', '40577.000000', '4065.000000', '409230.000000', '4100.000000', '41000.000000', '4130.000000', '41400.000000', '4150.000000', '41700.000000', '4178.000000', '4180.000000', '41800.000000', '4200.000000', '42000.000000', '421000.000000', '4235.000000', '4250.000000', '42500.000000', '4270.000000', '4275.000000', '4290.000000', '4300.000000', '43000.000000', '4350.000000', '43500.000000', '4352.000000', '43600.000000', '4400.000000', '444928.000000', '4450.000000', '445900.000000', '4490.000000', '4500.000000', '45000.000000', '450000.000000', '45570.000000', '45750.000000', '45800.000000', '458102.000000', '4590.000000', '4600.000000', '46000.000000', '463356.000000', '4641.000000', '465143.000000', '466157.000000', '46650.000000', '466880.000000', '4690.000000', '46900.000000', '4700.000000', '4720.000000', '47436.000000', '47500.000000', '47800.000000', '4781.000000', '4790.000000', '4792.000000', '4800.000000', '4850.000000', '4865.000000', '4878.000000', '4888.000000', '48928.000000', '4893.000000', '4895.000000', '4896.000000', '4900.000000', '4910.000000', '49170.000000', '4925.000000', '4930.000000', '4932.000000', '4950.000000', '4969.000000', '4985.000000', '4990.000000', '4995.000000', '4999.000000', '5000.000000', '50000.000000', '500000.000000', '5000000.000000', '50352.000000', '50410.800000', '50586.000000', '5080.000000', '5090.000000', '5100.000000', '5140.000000', '51900.000000', '5200.000000', '5250.000000', '52760.000000', '5300.000000', '5316.000000', '5372.000000', '5400.000000', '5460.000000', '5500.000000', '550000.000000', '5580.000000', '5646.490000', '5695.000000', '5700.000000', '5750.000000', '575000.000000', '5760.000000', '5800.000000', '582645.000000', '5900.000000', '590000.000000', '593083.000000', '5942.000000', '5952.000000', '5980.000000', '599890.000000', '600.000000', '6000.000000', '60000.000000', '600000.000000', '6023.000000', '6038.000000', '6082.000000', '6100.000000', '61000.000000', '6100000.000000', '6109.000000', '6117.000000', '614347.000000', '6158.000000', '6200.000000', '62000.000000', '6210.000000', '6250.000000', '6300.000000', '6325.000000', '6370.000000', '6380.000000', '6400.000000', '640000.000000', '6500.000000', '65000.000000', '650000.000000', '6550.000000', '6572.000000', '6590.000000', '6600.000000', '663527.000000', '666863.000000', '6725.000000', '6740.000000', '6800.000000', '6820.000000', '6830.000000', '6870.000000', '6890.000000', '6900.000000', '6951.000000', '6990.000000', '700.000000', '7000.000000', '70000.000000', '700000.000000', '70190.000000', '70943.870000', '7098.000000', '7100.000000', '71086.000000', '7114.000000', '7150.000000', '7170.000000', '7200.000000', '72485.000000', '7250.000000', '732312.000000', '7370.000000', '73746.000000', '7400.000000', '7410.000000', '7411.800000', '7428.000000', '7430.000000', '7435.000000', '7476.000000', '7484.000000', '7500.000000', '75000.000000', '7523.910000', '7600.000000', '7670.000000', '7700.000000', '7772.000000', '7800.000000', '7850.000000', '7855.000000', '7870.000000', '7886.000000', '7900.000000', '7910.000000', '7947.000000', '7987.000000', '800.000000', '8000.000000', '80000.000000', '80199.900000', '8050.000000', '80972.000000', '8100.000000', '8120.000000', '8190.000000', '8200.000000', '8205.000000', '8300.000000', '83400.000000', '8455.000000', '8500.000000', '850000.000000', '8600.000000', '86000.000000', '86197.000000', '862000.000000', '8700.000000', '8715.000000', '8794.000000', '8800.000000', '890.000000', '8900.000000', '8960.000000', '900.000000', '9000.000000', '90000.000000', '900000.000000', '9100.000000', '9125.000000', '9200.000000', '9240.000000', '9300.000000', '9306.000000', '9330.000000', '9391.000000', '9400.000000', '9448.000000', '9461.000000', '9500.000000', '95000.000000', '9600.000000', '9700.000000', '9721.000000', '9800.000000', '980000.000000', '9850.000000', '9870.000000', '9878.000000', '9893.000000', '9900.000000', '99000.000000', '9930.000000', '9935.000000', '9950.000000', '9961.000000', '9990.000000']</t>
         </is>
       </c>
     </row>
@@ -3515,7 +3515,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -3539,10 +3539,10 @@
         <v>-1</v>
       </c>
       <c r="L35" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M35" t="n">
-        <v>401</v>
+        <v>504</v>
       </c>
       <c r="N35" t="n">
         <v>0</v>
@@ -3563,7 +3563,7 @@
       </c>
       <c r="S35" t="inlineStr">
         <is>
-          <t>Renovation of kitchen and removal of walls - Sch-1A</t>
+          <t>Construction of a verandah - sch 1a</t>
         </is>
       </c>
       <c r="T35" t="n">
@@ -3575,20 +3575,20 @@
         </is>
       </c>
       <c r="V35" t="n">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="W35" t="n">
         <v>0.167</v>
       </c>
       <c r="X35" t="n">
-        <v>146566</v>
+        <v>164277</v>
       </c>
       <c r="Y35" t="n">
-        <v>1051</v>
+        <v>1164</v>
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t xml:space="preserve">['292/V026/20- Removal of 14 Regulated trees (4 Significant)  and major pruning of 22 Regulated trees( 10 Significant) in conjunction with Gawler Rail electrification', '?Eyre Stage 4A2 ? ENGINEERING', 'A change of use to consulting rooms with an ancillary store, including an internal fit out and addition to an existing building and alterations to an existing car park and the provision of landscaping, the commencement of advertising and demolition of a shed', 'ALMOND GROVE STAGE 9B ? ENGINEERING', 'Addition &amp; Alterations to existing McDonalds Restaurant', 'Addition to existing verandah', 'Additions &amp; Alterations to existing dwelling', 'Additions &amp; alterations to existing dwelling including a new verandah &amp; replacement of a domestic outbuilding &amp; carport', 'Additions and alterations to an existing detached dwelling comprising internal alterations and a partial change of use of an existing outbuilding', 'Additions and alterations to existing dwelling including a two storey addition as well as construction of a domestic outbuilding and retaining walls', 'Additions to an existing carport', 'Aerobic Waste System', 'Aerobic Wasterwater System', 'Aerobic Wastewater System', 'Aerobic Wastewater System - Pressurised Sub-Surface Soakage Bed', 'Aerobic Wastewater System - RiCycle EP20', 'Aerobic Wastewater system', 'Aerobic wastewater system', 'Alteration of a dwelling (install strutting beam) - Sch-1A reference to 292/662/2018', 'Alteration to Irrigation Area', 'Alteration to Septic Soakage Trench', 'Alteration to Underfloor Plumbing', 'Alteration to a road for the construction of a driveway onto an Arterial Road (Womma Road, Edinburgh North) and alterations to existing car parking', 'Alteration to existing Light Industry building in the form of ancillary offices and amenities', 'Alteration to existing Light Industry building in the form of ancillary transportable office building', 'Alteration to existing dwelling - replacement of existing window with a sliding door', 'Alteration to existing soakage', 'Alteration to existing system', 'Alteration to existing wastewater', 'Alteration to existing wastewater plumbing', 'Alteration to existing wastewater system', 'Alteration to irrigation area', 'Alteration to septic soakage trench', 'Alteration to under floor plumbing', 'Alteration to underfloor plumbing', 'Alteration to wastewater system', 'Alterations and additions to an existing dwelling -Withdrawn', 'Alterations and additions to an existing dwelling and retaining wall', 'Alterations and additions to an existing dwelling for the purposes of supported accommodation', 'Alterations and additions to an existing educational establishment and the construction of a car park.', 'Alterations and additions to existing building for the purposes of general industry and the construction of an associated office.\n\nSTAGE 3: Completed Factory Building and Services', 'Alterations and additions to existing dwelling', 'Alterations and additions to existing dwelling and construction of a deck and verandah', 'Alterations and additions to existing fitness centre building and alterations to existing carparking', 'Alterations and additions to existing single storey detached dwelling', 'Alterations to Stage 2 of division:  Amended plan of division to provide 6 additional allotments and amended SMP.\nTorrens title land division 2 into 66 (292/D090/15)', 'Alterations to an existing service station including fa?ade upgrades, internal alterations and signage including pylon sign', 'Alterations to existing dwelling and the construction of a carport and verandah', 'Alterations to existing dwelling and the construction of a verandah and deck', 'Alterations to existing under floor plumbing', 'Amendment to swimming pool safety barriers and increase to boundary fence (maximum hieght 2.5m)', 'Application for a holding tank', 'Application lodged on 292/1788/2020', 'BROOKMONT - ENGINEERING STAGE 5', 'BROOKMONT - ENGINEERING STAGE 6', 'BURGUNDY ESTATE Stage 2B &amp; 3 ? ENGINEERING', 'Boundary Realignment two allotments into two (D017/20)', 'Boundary re-alignment two allotments into two (292/D023/20)', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20.\n\nStage 1: Siteworks and Footings', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20.\n\nStage 2: Structure excluding internal work', 'CHIVELL GROVE STAGE 2 ? ENGINEERING', 'CONSTRUCTION OF A VERANDAH - RESCODE', 'Change of Use from Dwelling to office', 'Change of Use to a Takeaway Shop', 'Change of land use to a restaurant, internal fit out, internal and external alterations to existing shop and associated signage (5076- Zitto)', 'Change of land use to a restaurant, internal fit out, internal and external alterations to existing shop and associated signage (5076- Zitto) \n\nStage 1: Change of class &amp; internal fitout', 'Change of land use to a restaurant, internal fit out, internal and external alterations to existing shop and associated signage (5076- Zitto) \n\nStage 2: External works &amp; associated signage', 'Change of land use to a waste storage facility- FURTHER INFO EMAILED 26/10', 'Change of land use to horticulture and the construction of three glasshouses, a warehouse and packing shed, loading canopy, three dams, staff room and amenities building, four maintenance sheds, six water tanks, staff car park and landscaping', 'Change of land use to horticulture comprising structures (twelve greenhouses) and the construction of an ancillary packing and implement shed, dam and carpark and the placement of rainwater tanks.', 'Change of land use to light industry in the form of sheet metal fabrication, the construction of a canopy and advertising signage and the placement of a shipping container', 'Change of use and conversion of a residential dwelling to a medical clinic and consulting room with associated carparking - WITHDRAWN', 'Change of use and internal and external alterations to an existing building for self storage units', 'Change of use from Storage of Automotive parts to General Industry', 'Change of use from community centre to a multiple dwelling, the construction of a detached transportable unit, installation of three (3) shipping containers and additions and alterations to the existing building', 'Change of use from domestic outbuilding to Place of Worship', 'Change of use from outbuilding to temporary place of worship &amp; proposing marquee installed to be temporarily used for worship and celebrations', 'Change of use to a restaurant', 'Change of use to a training facility and internal alterations', 'Change of use to consulting rooms including alterations and additions of existing building with associated advertising signage, car parking and demolition of existing outbuildings at 24 Siddall Road (Stage 1), alterations to existing car park at 28 &amp; 30 Oldham Road (Stage 2), demolition of dwellings and associated outbuildings and change of use to at grade car park at 28 &amp; 30 Siddall Road (Stage 2)', 'Change of use to disability services with associated car parking', 'Change of use to dog grooming salon', 'Change of use to educational room and associated offices - Australia Workplace Training (Raleigh Chambers)', 'Change of use to include crushing of asphalt waste onsite', 'Change of use to office and assocciated fit-out (HS07C)', 'Change of use to office and supported accommodation', 'Change of use to special events space', 'Change of use to waste processing station in the form of a wrecking yard', 'Community Land Division 1 in to 2  (Existing dwelling to remain ) 292/C025/20 - rescode DPC', 'Con struction of a verandah - Rescode certified', 'Constrtuction of a carport', 'Constructioin of detached dwelling with garage UMR', 'Construction a detached dwelling with attached verandah and a freestanding carport', 'Construction of  a Verandah', 'Construction of  a detached dwelling with garage UMR- withdraw', 'Construction of  verandah - rescode', 'Construction of 2 Retaining Walls with a fence above 2.1 metres in total height.', 'Construction of 2 domestic outbuildings', 'Construction of 2 verandahs', 'Construction of 2 x verandah', 'Construction of 2 x verandahs', 'Construction of 2 x verandahs Sch1a', 'Construction of 3 Verandahs', 'Construction of 3 x dwellings with attached carports', 'Construction of 3x shade sails in association with an existing child care centre', 'Construction of 4 x two storey dwellings', 'Construction of 4x single storey dwelling - rescode certified', 'Construction of 5 green houses and dam with ancillary store, carparking and amenities', 'Construction of 7 x Greenhouses &amp; a Dam', 'Construction of 9 single storey dwellings', 'Construction of Detached Dwelling with a Garage under the main roof', 'Construction of Green House', 'Construction of Greenhouses', 'Construction of Horticulture Structures (Greenhouses) and a Dam', 'Construction of Verandah', 'Construction of Verandah ( Schedule 1A)', 'Construction of Verandah (Schedule 1a)', 'Construction of a 2 storey detached dwelling with attached garage  and verandah', 'Construction of a 2 verandahs', 'Construction of a 66kV Transmission Line - 292/V031/20', 'Construction of a Boundary fence to 2.7m high', 'Construction of a Carport', 'Construction of a Carport &amp; Verandah', 'Construction of a Carport &amp; two x Verandahs', 'Construction of a Carport - Rescode certified', 'Construction of a Carport - SCH1A', 'Construction of a Carport - Sch 1a', 'Construction of a Carport to existing Dwelling &amp; the construction of Storage/Packing Shed with attached verandah', 'Construction of a Carport- Sch1A', 'Construction of a Commerical Storage Shed', 'Construction of a Detached Dwelling', 'Construction of a Detached Dwelling - Res code Certifiied', 'Construction of a Detached Dwelling with Garage Locataed Under Main Roof', 'Construction of a Detached Dwelling with Garage Located Under Main Roof', 'Construction of a Detached Dwelling with Garage Under Main Roof', 'Construction of a Domestic Outbuilding- sch1a', 'Construction of a Domestic outbuilding', 'Construction of a Dwelling - Rescode certified', 'Construction of a Farm building &amp; Greenhouses', 'Construction of a Garage- Sch 1a', 'Construction of a Implement Shed (Farm Building)', 'Construction of a Rumpus Room and Sleep Out', 'Construction of a Shade Sail', 'Construction of a Swimming Pool &amp; Associated Safety Barrier.', 'Construction of a Swimming Pool &amp; Associated Safety Barrier/Fence', 'Construction of a Swimming Pool &amp; safety barrier', 'Construction of a Verandah', 'Construction of a Verandah &amp; Carport', 'Construction of a Verandah &amp; Deck', 'Construction of a Verandah ( Shedule 1A)', 'Construction of a Verandah -  Sch1A', 'Construction of a Verandah - Complying', 'Construction of a Verandah - RESCODE', 'Construction of a Verandah - Rescode certified', 'Construction of a Verandah - SCH1A', 'Construction of a Verandah - Sch1A', 'Construction of a Verandah - rescode certfied', 'Construction of a Verandah - sch1a', 'Construction of a Verandah, Carport &amp; External Dwelling Addition (Rumpus Room)', 'Construction of a Verandah- SCH1A', 'Construction of a Verandah- SCHEDULE 1A', 'Construction of a Verandah- sch1A', 'Construction of a Verandah- sch1a', 'Construction of a Verandah-Sch1A', 'Construction of a boundary fence (western) to a height of 2.6 metres', 'Construction of a canopy', 'Construction of a carport', 'Construction of a carport - SCH1A', 'Construction of a carport - Sch 1A', 'Construction of a carport - Sch 1a', 'Construction of a carport - Sch-1A', 'Construction of a carport - Sch1A', 'Construction of a carport - Schedule 1A', 'Construction of a carport - rescode', 'Construction of a carport - rescode certfied', 'Construction of a carport - sch 1a', 'Construction of a carport and domestic outbuilding - email &amp; letter sent 26/10/2020', 'Construction of a carport and garage', 'Construction of a carport and verandah', 'Construction of a carport attached to existing dependent accommodation', 'Construction of a carport attached to existing outbuilding', 'Construction of a carport, verandah and freestanding domestic outbuilding (shed)', 'Construction of a carport- Sch1A', 'Construction of a carpot - Sch-1A', 'Construction of a childcare centre with associated advertising, car park resulting in tree damaging activity, fencing, retaining walls, masonry entry wall, storage sheds and landscaping', 'Construction of a commercial  shed', 'Construction of a commercial/industrial shed', 'Construction of a dam and associated pump shed with surrounding fence', 'Construction of a deatched dwelling with a garage under the main roof', 'Construction of a deatched two storey dwelling with garage UMR', 'Construction of a deck', 'Construction of a detached Dwelling with Garage Located Under Main Roof', 'Construction of a detached dweling with verandah and garage under main roof', 'Construction of a detached dwelling', 'Construction of a detached dwelling  - rescode certified', 'Construction of a detached dwelling ( Lot 119 Parkvale Drive)', 'Construction of a detached dwelling ( Lot 128 Parkvale Drive)', 'Construction of a detached dwelling ( Res Code  Certified)', 'Construction of a detached dwelling (Lot 102 Parkvale Drive)', 'Construction of a detached dwelling (Lot 105 Damien Street)', 'Construction of a detached dwelling (Lot 110 Damien street)', 'Construction of a detached dwelling (Res Code Certifed)', 'Construction of a detached dwelling (Res Code Certified)', 'Construction of a detached dwelling -  Rescode certified', 'Construction of a detached dwelling - Rescode Certified', 'Construction of a detached dwelling - Rescode certified', 'Construction of a detached dwelling - Rescode certified- WITHDRAWN', 'Construction of a detached dwelling - Schedule 4 1(1)a (Complying)', 'Construction of a detached dwelling - Withdrawn', 'Construction of a detached dwelling - rescode', 'Construction of a detached dwelling - rescode - WITHDRAWN', 'Construction of a detached dwelling - rescode certified', 'Construction of a detached dwelling a with garage under the main roof', 'Construction of a detached dwelling and outbuilding and  placement of a water tank', 'Construction of a detached dwelling and retaining walls (Lot 1081 Highview drive)', 'Construction of a detached dwelling to be used as a display home (Lot 100 Parkvale drive)', 'Construction of a detached dwelling to be used as a display home (Lot 101  Parkvale drive)', 'Construction of a detached dwelling to be used as a display home for a period of up to 5 years', 'Construction of a detached dwelling to be used as a display home for a period of up to 5 years and associated signage', 'Construction of a detached dwelling wiith a garage under the main roof', 'Construction of a detached dwelling with a garage and alfresco under main roof', 'Construction of a detached dwelling with a garage and alfresco under the main roof', 'Construction of a detached dwelling with a garage and terrace under main roof', 'Construction of a detached dwelling with a garage and verandah under main roof', 'Construction of a detached dwelling with a garage under main roof', 'Construction of a detached dwelling with a garage under the main roof', 'Construction of a detached dwelling with a garage under the main roof  and associated retaining walls', 'Construction of a detached dwelling with a garage under the main roof - WITHDRAWN', 'Construction of a detached dwelling with a garage under the main roof and an associated retaining wall', 'Construction of a detached dwelling with a garage under the main roof and retaining walls', 'Construction of a detached dwelling with a garage, alfresco and verandah under main roof and associated retaining wall', 'Construction of a detached dwelling with an attached garage and two verandahs', 'Construction of a detached dwelling with attached carport and verandah', 'Construction of a detached dwelling with attached carport and verandah - Awaiting Civil Plans- WITHDRAWN', 'Construction of a detached dwelling with attached garage', 'Construction of a detached dwelling with attached garage  to be used as a temporary display home with associated office and advertising displays.', 'Construction of a detached dwelling with attached garage - (Lot 3120, Reel Tce)', 'Construction of a detached dwelling with attached garage - Awaiting CT', 'Construction of a detached dwelling with attached garage and freestanding carport', 'Construction of a detached dwelling with attached garage and veradahs', 'Construction of a detached dwelling with attached garage and verandah', 'Construction of a detached dwelling with attached garage and verandah (temporary display home)', 'Construction of a detached dwelling with attached garage and verandah - Awaiting Civil Plan- WITH DRAWN', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary display home with associated office and advertising display.', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary display home with associated office and signage\n\nStage 1: Footings Only', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary display home with associated office and signage\n\nStage 2: Final', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary sales &amp; project office', 'Construction of a detached dwelling with attached garage and verandah under main roof and associated retaining walls', 'Construction of a detached dwelling with attached garage and verandahs', 'Construction of a detached dwelling with attached garage and verandahs - WITHDRAWN', 'Construction of a detached dwelling with attached garage and verandahs to be used as a temporary display home with associated office and signage\n\nStage 1: construction of display building and associated display office (only)', 'Construction of a detached dwelling with attached garage and verandahs- WITHDRAWN', 'Construction of a detached dwelling with attached garage and vernadah - Waiting on civil/stormwater plan- WITHDRAWN', 'Construction of a detached dwelling with attached garage and verndah', 'Construction of a detached dwelling with attached garage to be used as a temporary display home with associated advertising displays.', 'Construction of a detached dwelling with attached garage, verandah and associated retaining wall', 'Construction of a detached dwelling with attached garage, verandah and associated retaining wall -', 'Construction of a detached dwelling with attached garage, verandah and associated retaining wall - (Lot 25 Highview Drive)', 'Construction of a detached dwelling with attached garage.', 'Construction of a detached dwelling with attached verandah', 'Construction of a detached dwelling with attached verandah and a freestanding carport', 'Construction of a detached dwelling with attached verandah and carport', 'Construction of a detached dwelling with carport UMR', 'Construction of a detached dwelling with garage &amp; verandah UMR', 'Construction of a detached dwelling with garage - temporary display home', 'Construction of a detached dwelling with garage UMR', 'Construction of a detached dwelling with garage UMR ( House 1)', 'Construction of a detached dwelling with garage UMR ( House 2)', 'Construction of a detached dwelling with garage UMR ( lot 2031 Lindgren Avenue', 'Construction of a detached dwelling with garage UMR ( lot 2032 Lindgren Avenue', 'Construction of a detached dwelling with garage UMR (Res Code)', 'Construction of a detached dwelling with garage UMR- LODGED IN ERROR', 'Construction of a detached dwelling with garage UMR- WITHDRAWN', 'Construction of a detached dwelling with garage and alfresco under main roof', 'Construction of a detached dwelling with garage and veranda under main roof', 'Construction of a detached dwelling with garage and verandah under main roof', 'Construction of a detached dwelling with garage and verandah under main roof and retaining walls to a maximum height of 3.5m', 'Construction of a detached dwelling with garage and verandahs under main roof', 'Construction of a detached dwelling with garage located under main roof', 'Construction of a detached dwelling with garage located under main roof - Lot 797 Philip Avenue, Angle Vale', 'Construction of a detached dwelling with garage to be used as a temporary display home', 'Construction of a detached dwelling with garage umr', 'Construction of a detached dwelling with garage under main roof', 'Construction of a detached dwelling with garage under main roof ( Lot 87 Parkvale Drive)', 'Construction of a detached dwelling with garage under main roof - WITHDRAWN', 'Construction of a detached dwelling with garage under main roof and a verandah', 'Construction of a detached dwelling with garage under main roof.', 'Construction of a detached dwelling with garage under the main roof', 'Construction of a detached dwelling with garage under the main roof ( Lot 109 Damien Street)', 'Construction of a detached dwelling with garage under the main roof - Lot 111 Damien Street', 'Construction of a detached dwelling with garage under the main roof.', 'Construction of a detached dwelling with garage underthe main roof ( Lot 127 Parkvale Drive)', 'Construction of a detached dwelling with the garage under the main roof', 'Construction of a detached dwelling with the garage under the main roof.', 'Construction of a detached dwelling with verandah and garage (Lot 170 Damien street)', 'Construction of a detached dwelling with verandah and garage under main roof', 'Construction of a detached dwelling with verandah and garage under main roof (Lot 2022 Lindgren Avenue)', 'Construction of a detached dwelling with verandah and garage under main roof (Lot 2023 Lindgren Avenue)', 'Construction of a detached dwelling with verandah and garage under main roof - WITHDRAWN', 'Construction of a detached dwelling with verandah and garage under mian roof', 'Construction of a detached dwelling with verandah, porch and  garage under main roof', 'Construction of a detached dwelling with verandahs and garage under main roof', 'Construction of a detached dwelling with verandahs and garage under main roof (Lot 117 Damien street)', 'Construction of a detached dwelling- Rescode certified', 'Construction of a detached dwelling- WITHDRAWN', 'Construction of a detached dwelling- rescode certified', 'Construction of a detached dwelling- rescode certified WITHDRAWN', 'Construction of a detached dwelling-WITHDRAWN', 'Construction of a detached dwellng with garage UMR', 'Construction of a disability toilet - Fremont Park', 'Construction of a domesetic outbuilding (shed)', 'Construction of a domestic garage', 'Construction of a domestic out building - Sch1a', 'Construction of a domestic out building - sch 1a', 'Construction of a domestic out building - sch1a', 'Construction of a domestic out building and verandah', 'Construction of a domestic outbuilding', 'Construction of a domestic outbuilding  - Sch1A', 'Construction of a domestic outbuilding &amp; a Verandah', 'Construction of a domestic outbuilding (garage)', 'Construction of a domestic outbuilding (garage), 1.8m high masonary fence, pool equipment shed and verandah\n\nStage 1: Domestic outbuilding (garage) and 1.8m high masonary fence', 'Construction of a domestic outbuilding (garage), 1.8m high masonary fence, pool equipment shed and verandah\nStage 1: Domestic outbuilding (garage) and 1.8m high masonary fence\nStage 2: Pool equipment shed and verandah', 'Construction of a domestic outbuilding (partially enclosed verandah)', 'Construction of a domestic outbuilding (shed)', 'Construction of a domestic outbuilding (shed) &amp; verandah', 'Construction of a domestic outbuilding (workshop &amp; garage)', 'Construction of a domestic outbuilding - Rescode certified', 'Construction of a domestic outbuilding - SCH1A', 'Construction of a domestic outbuilding - Sch 1a', 'Construction of a domestic outbuilding - Sch1A', 'Construction of a domestic outbuilding - Sch1a', 'Construction of a domestic outbuilding - Schedule 1A', 'Construction of a domestic outbuilding - Shed', 'Construction of a domestic outbuilding - rescode certified', 'Construction of a domestic outbuilding - sch 1a', 'Construction of a domestic outbuilding - sch1a', 'Construction of a domestic outbuilding -Sch1a', 'Construction of a domestic outbuilding and carport', 'Construction of a domestic outbuilding and two verandahs', 'Construction of a domestic outbuilding and verandahs', 'Construction of a domestic outbuilding- SCH1A', 'Construction of a domestic outbuilding- Sch 1a', 'Construction of a domestic outbuilding- Sch1A', 'Construction of a domestic outbuilding- sch1a', 'Construction of a domestic shed - Sch1A', 'Construction of a double storey detached dwelling - rescode certified', 'Construction of a dwelliing (Res Code Certified )', 'Construction of a dwelling ( Lot 238 Greenhood)', 'Construction of a dwelling ( Lot 240 Greenhood)', 'Construction of a dwelling ( Lot 241 Greenhood)', 'Construction of a dwelling ( Res Code Certified)', 'Construction of a dwelling (Lot 239 Greenhood)', 'Construction of a dwelling (Res Code Certifed)', 'Construction of a dwelling (Res Code Certified)', 'Construction of a dwelling (Res Code)', 'Construction of a dwelling (lot 206)', 'Construction of a dwelling -  rescode certified', 'Construction of a dwelling - -rescode certified', 'Construction of a dwelling - ResCode Certified', 'Construction of a dwelling - Rescode Certfied', 'Construction of a dwelling - Rescode Certified', 'Construction of a dwelling - Rescode certifed', 'Construction of a dwelling - Rescode certified', 'Construction of a dwelling - Rescode certified - (Lot 2)', 'Construction of a dwelling - rescode certifed', 'Construction of a dwelling - rescode certified', 'Construction of a dwelling - rescode certified - WITHDRAWN', 'Construction of a dwelling - rescode certified- WITHDRAWN', 'Construction of a dwelling - resocde certified', 'Construction of a dwelling addition - Rescode certified', 'Construction of a dwelling addition, verandahs and deck', 'Construction of a dwelling and a carport', 'Construction of a dwelling extension (bathroom extension)', 'Construction of a dwelling extension - rescode certified', 'Construction of a dwelling extension, verandah and installation of a pool', 'Construction of a dwelling for the purposes of supported accomodation ( Lot 2)', 'Construction of a dwelling for the purposes of supported accomodation (Lot 1)', 'Construction of a dwelling in the form of dependent accommodation', 'Construction of a dwelling with attached garage - WITHDRAWN', 'Construction of a dwelling with attached garage and verandah', 'Construction of a dwelling with attached garage and verandah- WITHDRAWN', 'Construction of a dwelling with carport - Site 207', 'Construction of a dwelling with carport - Site 213', 'Construction of a dwelling with carport - Site 214', 'Construction of a dwelling with detached carport', 'Construction of a dwelling with garage - Rescode certified', 'Construction of a dwelling with garage under main roof', 'Construction of a dwelling, carport and deck (lot 212 )', 'Construction of a dwelling- Rescode Certified', 'Construction of a dwelling- Rescode certified', 'Construction of a dwelling- Rescode certified - WITHDRAWN', 'Construction of a dwelling- rescode certified', 'Construction of a dwelling. RES CODE certified', 'Construction of a farm building', 'Construction of a farm building and fence', 'Construction of a farm implement shed', 'Construction of a freestanding gable verandah', 'Construction of a freestanding verandah (Site 41)', 'Construction of a gable verandah ( Schedule 1A)', 'Construction of a garage and demolition of existing carport', 'Construction of a glasshouse\n\nStage 2: Final', 'Construction of a greenhouse with associated dam and carparking', 'Construction of a horse shelter', 'Construction of a implement shed', 'Construction of a implement shed for use in association with existing farming operations', 'Construction of a light industrial building (caravan repairs) with associated carparking and landscaping', 'Construction of a masonry fence with  signage', 'Construction of a new dwelling - Rescode certified', 'Construction of a new entry and crossover- refferal from SCAP for Council to provide comment', 'Construction of a new glass balustrade - Level 1 Building 7', 'Construction of a outbuilding', 'Construction of a outbuilding with attached verandah', 'Construction of a packing shed', 'Construction of a pump and storage shed in association with existing horticulture', 'Construction of a replacement fence (2.19m high) on existing retaining wall', 'Construction of a retaining wall', 'Construction of a retaining wall (1m) with a total fence height of 2.8m', 'Construction of a retaining wall (Stage 3 &amp; 4 Evergreen Estate)', 'Construction of a retaining wall (maximum height 750mm) and fence (1.8m)', 'Construction of a retaining wall and fence', 'Construction of a rumpus room', 'Construction of a second dwelling in the form of dependent accomodation', 'Construction of a shade sail', 'Construction of a shade sail ( Fremont park)', 'Construction of a shade sail structure', 'Construction of a shed', 'Construction of a shed - Sch1a', 'Construction of a sign - park reserve (Parkview Walk)\nSchedule 3, Part 2(e) ? buildings in a recreation area- Withdrawn', 'Construction of a sign - park reserve (Perre Reserve)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve (Ramsay Park)', 'Construction of a sign - park reserve (Secombe Street)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve (Virginia Oval-Sign 2)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve (Virginia Oval-sign 1)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve sign (California Reserve)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve sign (Honeysuckle Reserve)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - reserve sign (Smithfield Memorial Garden)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - reserve sign (Smithfield Oval)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - reserve sign (Uley Reserve West)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - reserve sign (Uley Reserve)\nSchedule 3, Part 2(e) ? buildings in a recreation area', 'Construction of a sign - suburb sign (Andrews Farm)', 'Construction of a sign - suburb sign (Davoren Park)', 'Construction of a sign - suburb sign (Elizabeth Downs)', 'Construction of a single storey additions to existing dwelling', 'Construction of a single storey detached dwelling', 'Construction of a single storey detached dwelling\n\nStage 1: Footings Only', 'Construction of a single storey detached dwelling\n\nStage 2: Final', 'Construction of a single storey detached dwelling (transportable)', 'Construction of a single storey detached dwelling - WITHDRAWN', 'Construction of a single storey detached dwelling - rescode', 'Construction of a single storey detached dwelling and associated retaining walls up to a height of 1.0 metre', 'Construction of a single storey detached dwelling and freestanding carport', 'Construction of a single storey detached dwelling with garage under main roof', 'Construction of a single storey detached dwelling- WITHDRAWN', 'Construction of a single storey detached dwelling- rescode certified', 'Construction of a single storey dwelling', 'Construction of a single storey dwelling (Lot 229 Greenhood)', 'Construction of a single storey dwelling (Lot 230 Greenhood)', 'Construction of a single storey dwelling (Lot 231 Greenhood)', 'Construction of a single storey dwelling (Lot 232 Greenhood)', 'Construction of a single storey dwelling - Rescode certified', 'Construction of a single storey dwelling addition', 'Construction of a single storey dwelling with detached carport', 'Construction of a single storey dwelling with garage - Rescode certified', 'Construction of a single storey dwelling with garage - rescode certified', 'Construction of a sleepout- Rescode Certified', 'Construction of a spa and associated safety barrier and decking surrounding the spa', 'Construction of a </t>
+          <t>['292/V026/20- Removal of 14 Regulated trees (4 Significant)  and major pruning of 22 Regulated trees( 10 Significant) in conjunction with Gawler Rail electrification', '?Eyre Stage 4A2 ? ENGINEERING', 'A change of use to consulting rooms with an ancillary store, including an internal fit out and addition to an existing building and alterations to an existing car park and the provision of landscaping, the commencement of advertising and demolition of a shed', 'ALMOND GROVE STAGE 9B ? ENGINEERING', 'Addition &amp; Alterations to existing McDonalds Restaurant', 'Addition to existing verandah', 'Additions &amp; Alterations to existing dwelling', 'Additions &amp; alterations to existing dwelling', 'Additions &amp; alterations to existing dwelling including a new verandah &amp; replacement of a domestic outbuilding &amp; carport', 'Additions and alterations to an existing detached dwelling comprising internal alterations and a partial change of use of an existing outbuilding', 'Additions and alterations to existing dwelling including a two storey addition as well as construction of a domestic outbuilding and retaining walls', 'Additions to an existing carport', 'Aerobic Waste System', 'Aerobic Wasterwater System', 'Aerobic Wastewater System', 'Aerobic Wastewater System - Pressurised Sub-Surface Soakage Bed', 'Aerobic Wastewater System - RiCycle EP20', 'Aerobic Wastewater system', 'Aerobic wastewater system', 'Alteration of a dwelling (install strutting beam) - Sch-1A reference to 292/662/2018', 'Alteration to Irrigation Area', 'Alteration to Septic Soakage Trench', 'Alteration to Underfloor Plumbing', 'Alteration to a road for the construction of a driveway onto an Arterial Road (Womma Road, Edinburgh North) and alterations to existing car parking', 'Alteration to an existing wastewater system', 'Alteration to existing Light Industry building in the form of ancillary offices and amenities', 'Alteration to existing Light Industry building in the form of ancillary transportable office building', 'Alteration to existing dwelling - replacement of existing window with a sliding door', 'Alteration to existing soakage', 'Alteration to existing system', 'Alteration to existing wastewater', 'Alteration to existing wastewater plumbing', 'Alteration to existing wastewater system', 'Alteration to irrigation', 'Alteration to irrigation area', 'Alteration to septic soakage trench', 'Alteration to under floor plumbing', 'Alteration to underfloor plumbing', 'Alteration to wastewater system', 'Alterations and additions to an existing dwelling -Withdrawn', 'Alterations and additions to an existing dwelling and retaining wall', 'Alterations and additions to an existing dwelling for the purposes of supported accommodation', 'Alterations and additions to an existing educational establishment and the construction of a car park.', 'Alterations and additions to existing building for the purposes of general industry and the construction of an associated office.\n\nSTAGE 3: Completed Factory Building and Services', 'Alterations and additions to existing dwelling', 'Alterations and additions to existing dwelling and construction of a deck and verandah', 'Alterations and additions to existing fitness centre building and alterations to existing carparking', 'Alterations and additions to existing single storey detached dwelling', 'Alterations to Stage 2 of division:  Amended plan of division to provide 6 additional allotments and amended SMP.\nTorrens title land division 2 into 66 (292/D090/15)', 'Alterations to an existing retail showroom', 'Alterations to an existing service station including fa?ade upgrades, internal alterations and signage including pylon sign', 'Alterations to existing dwelling and the construction of a carport and verandah', 'Alterations to existing dwelling and the construction of a verandah and deck', 'Alterations to existing under floor plumbing', 'Alterations to existing verandah', 'Amendment to swimming pool safety barriers and increase to boundary fence (maximum hieght 2.5m)', 'Application for a holding tank', 'Application lodged on 292/1788/2020', 'BROOKMONT - ENGINEERING STAGE 5', 'BROOKMONT - ENGINEERING STAGE 6', 'BURGUNDY ESTATE Stage 2B &amp; 3 ? ENGINEERING', 'Boundary Realignment two allotments into two (D017/20)', 'Boundary re-alignment two allotments into two (292/D023/20)', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20.\n\nStage 1: Siteworks and Footings', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20.\n\nStage 2: Structure excluding internal work', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20.\n\nStage 3: Additional 3 bays structure excluding internal work', 'Bulk handling and storage facility associated car parking and landscaping - 292/E013/20.\n\nStage 4: Remainder of work', 'CHIVELL GROVE STAGE 2 ? ENGINEERING', 'CONSTRUCTION OF A VERANDAH - RESCODE', 'Change of Use from Dwelling to office', 'Change of Use to a Takeaway Shop', 'Change of land use to a restaurant, internal fit out, internal and external alterations to existing shop and associated signage (5076- Zitto)', 'Change of land use to a restaurant, internal fit out, internal and external alterations to existing shop and associated signage (5076- Zitto) \n\nStage 1: Change of class &amp; internal fitout', 'Change of land use to a restaurant, internal fit out, internal and external alterations to existing shop and associated signage (5076- Zitto) \n\nStage 2: External works &amp; associated signage', 'Change of land use to a waste storage facility- FURTHER INFO EMAILED 26/10', 'Change of land use to horticulture and the construction of fourteen greenhouses, a packing shed, two rainwater tanks, a stormwater dam and associated car parking', 'Change of land use to horticulture and the construction of three glasshouses, a warehouse and packing shed, loading canopy, three dams, staff room and amenities building, four maintenance sheds, six water tanks, staff car park and landscaping - WITHDRAWN', 'Change of land use to horticulture comprising structures (twelve greenhouses) and the construction of an ancillary packing and implement shed, dam and carpark and the placement of rainwater tanks.', 'Change of land use to light industry in the form of sheet metal fabrication, the construction of a canopy and advertising signage and the placement of a shipping container', 'Change of use and conversion of a residential dwelling to a medical clinic and consulting room with associated carparking - WITHDRAWN', 'Change of use and internal and external alterations to an existing building for self storage units', 'Change of use from Storage of Automotive parts to General Industry', 'Change of use from community centre to a multiple dwelling, the construction of a detached transportable unit, installation of three (3) shipping containers and additions and alterations to the existing building', 'Change of use from domestic outbuilding to Place of Worship', 'Change of use from outbuilding to temporary place of worship &amp; proposing marquee installed to be temporarily used for worship and celebrations', 'Change of use from shop to customer service centre (office) (Tenancy HS07)', 'Change of use to a restaurant', 'Change of use to a showroom with associated fit out &amp; carpark', 'Change of use to a training facility and internal alterations', 'Change of use to consulting rooms including alterations and additions of existing building with associated advertising signage, car parking and demolition of existing outbuildings at 24 Siddall Road (Stage 1), alterations to existing car park at 28 &amp; 30 Oldham Road (Stage 2), demolition of dwellings and associated outbuildings and change of use to at grade car park at 28 &amp; 30 Siddall Road (Stage 2)', 'Change of use to disability services with associated car parking', 'Change of use to dog grooming salon', 'Change of use to educational room and associated offices - Australia Workplace Training (Raleigh Chambers)', 'Change of use to include crushing of asphalt waste onsite', 'Change of use to office &amp; associated fitout - cancelled', 'Change of use to office and assocciated fit-out (HS07C)', 'Change of use to office and supported accommodation', 'Change of use to special events space', 'Change of use to waste processing station in the form of a wrecking yard', 'Community Land Division 1 in to 2  (Existing dwelling to remain ) 292/C025/20 - rescode DPC', 'Con struction of a verandah - Rescode certified', 'Constrtuction of a carport', 'Constructioin of detached dwelling with verandah and garage under main roof', 'Construction a detached dwelling with attached verandah and a freestanding carport', 'Construction a single storey detached dwelling', 'Construction of  a Verandah', 'Construction of  a detached dwelling with garage UMR- withdraw', 'Construction of  verandah - rescode', 'Construction of 2 Retaining Walls with a fence above 2.1 metres in total height.', 'Construction of 2 domestic outbuildings', 'Construction of 2 verandahs', 'Construction of 2 x dependant accommodation', 'Construction of 2 x verandah', 'Construction of 2 x verandahs', 'Construction of 2 x verandahs Sch1a', 'Construction of 2x Verandahs', 'Construction of 3 Verandahs', 'Construction of 3 x dwellings with attached carports', 'Construction of 3x shade sails in association with an existing child care centre', 'Construction of 4 x two storey dwellings', 'Construction of 4x single storey dwelling - rescode certified', 'Construction of 5 green houses and dam with ancillary store, carparking and amenities', 'Construction of 7 x Greenhouses &amp; a Dam', 'Construction of 9 single storey dwellings', 'Construction of Aged living &amp; associated support facilities - staged consent', 'Construction of Detached Dwelling with a Garage under the main roof', 'Construction of Green Houses', 'Construction of Green house', 'Construction of Greenhouses', 'Construction of Horticulture Structures (Greenhouses) and a Dam', 'Construction of Verandah', 'Construction of Verandah ( Schedule 1A)', 'Construction of Verandah (Schedule 1a)', 'Construction of a 2 storey detached dwelling with attached garage  and verandah', 'Construction of a 2 verandahs', 'Construction of a 66kV Transmission Line - 292/V031/20', 'Construction of a Boundary fence to 2.7m high', 'Construction of a Carport', 'Construction of a Carport &amp; Verandah', 'Construction of a Carport &amp; two x Verandahs', 'Construction of a Carport - Rescode certified', 'Construction of a Carport - SCH1A', 'Construction of a Carport - Sch 1a', 'Construction of a Carport to existing Dwelling &amp; the construction of Storage/Packing Shed with attached verandah', 'Construction of a Carport- Sch1A', 'Construction of a Carport- sch1a', 'Construction of a Commerical Storage Shed', 'Construction of a Deck &amp; Verandah', 'Construction of a Dependent Accommodation Building Comprising Bedroom, Rumpas Room and Amenities (Retrospective)', 'Construction of a Detached Dwelling', 'Construction of a Detached Dwelling - Res code Certifiied', 'Construction of a Detached Dwelling with Garage Located Under Main Roof', 'Construction of a Domestic Outbuilding- sch1a', 'Construction of a Domestic outbuilding', 'Construction of a Dwelling - Rescode Certified', 'Construction of a Dwelling - Rescode certified', 'Construction of a Farm building &amp; Greenhouses', 'Construction of a Garage- Sch 1a', 'Construction of a Granny Flat', 'Construction of a Implement Shed (Farm Building)', 'Construction of a Packing Shed', 'Construction of a Shade Sail', 'Construction of a Swimming Pool &amp; Associated Safety Barrier.', 'Construction of a Swimming Pool &amp; Associated Safety Barrier/Fence', 'Construction of a Swimming Pool &amp; safety barrier', 'Construction of a Verandah', 'Construction of a Verandah &amp; Carport', 'Construction of a Verandah &amp; Deck', 'Construction of a Verandah ( Shedule 1A)', 'Construction of a Verandah -  Sch1A', 'Construction of a Verandah - Complying', 'Construction of a Verandah - RESCODE', 'Construction of a Verandah - Rescode certified', 'Construction of a Verandah - SCH1A', 'Construction of a Verandah - Sch1A', 'Construction of a Verandah - rescode certfied', 'Construction of a Verandah - sch1a', 'Construction of a Verandah, Carport &amp; External Dwelling Addition (Rumpus Room)', 'Construction of a Verandah- SCH1A', 'Construction of a Verandah- SCHEDULE 1A', 'Construction of a Verandah- sch1A', 'Construction of a Verandah- sch1a', 'Construction of a Verandah-Sch1A', 'Construction of a an outbuilding', 'Construction of a boundary fence (western) to a height of 2.6 metres', 'Construction of a canopy', 'Construction of a carport', 'Construction of a carport - SCH1A', 'Construction of a carport - Sch 1A', 'Construction of a carport - Sch 1a', 'Construction of a carport - Sch-1A', 'Construction of a carport - Sch1A', 'Construction of a carport - Schedule 1A', 'Construction of a carport - rescode', 'Construction of a carport - rescode certfied', 'Construction of a carport - sch 1a', 'Construction of a carport and domestic outbuilding - email &amp; letter sent 26/10/2020', 'Construction of a carport and garage', 'Construction of a carport and verandah', 'Construction of a carport attached to existing dependent accommodation', 'Construction of a carport attached to existing outbuilding', 'Construction of a carport, verandah and freestanding domestic outbuilding (shed)', 'Construction of a carport- Sch1A', 'Construction of a carpot - Sch-1A', 'Construction of a childcare centre with associated advertising, car park resulting in tree damaging activity, fencing, retaining walls, masonry entry wall, storage sheds and landscaping', 'Construction of a commercial  shed', 'Construction of a commercial/industrial shed', 'Construction of a dam in association with horticulture with a surrounding fence and associated building used as a pump shed and irrigation store', 'Construction of a deatched dwelling with a garage under the main roof', 'Construction of a deatched two storey dwelling', 'Construction of a deck', 'Construction of a detached Dwelling', 'Construction of a detached dweling with verandah and garage under main roof', 'Construction of a detached dwelling', 'Construction of a detached dwelling  - rescode certified', 'Construction of a detached dwelling ( Lot 119 Parkvale Drive)', 'Construction of a detached dwelling ( Lot 128 Parkvale Drive)', 'Construction of a detached dwelling ( Res Code  Certified)', 'Construction of a detached dwelling ( Res Code Certifed)', 'Construction of a detached dwelling (Lot 102 Parkvale Drive)', 'Construction of a detached dwelling (Lot 105 Damien Street)', 'Construction of a detached dwelling (Lot 110 Damien street)', 'Construction of a detached dwelling (Res Code Ceretifed)', 'Construction of a detached dwelling (Res Code Certifed)', 'Construction of a detached dwelling (Res Code Certified)', 'Construction of a detached dwelling (Res Code)', 'Construction of a detached dwelling -  Rescode certified', 'Construction of a detached dwelling - Rescode Certified', 'Construction of a detached dwelling - Rescode certified', 'Construction of a detached dwelling - Rescode certified- WITHDRAWN', 'Construction of a detached dwelling - Schedule 4 1(1)a (Complying)', 'Construction of a detached dwelling - WITHDRAWN', 'Construction of a detached dwelling - Withdrawn', 'Construction of a detached dwelling - rescode', 'Construction of a detached dwelling - rescode - WITHDRAWN', 'Construction of a detached dwelling - rescode certified', 'Construction of a detached dwelling - rescode certified - WITHDRAWN', 'Construction of a detached dwelling a with garage under the main roof', 'Construction of a detached dwelling addition', 'Construction of a detached dwelling and associated retaining wall and fence totalling 3.1m in height', 'Construction of a detached dwelling and detached carport', 'Construction of a detached dwelling and outbuilding and  placement of a water tank', 'Construction of a detached dwelling and retaining walls (Lot 1081 Highview drive) WITHDRAWN', 'Construction of a detached dwelling for temporary use as a display home for a period of 3 years', 'Construction of a detached dwelling to be used as a display home (Lot 100 Parkvale drive)', 'Construction of a detached dwelling to be used as a display home (Lot 101  Parkvale drive)', 'Construction of a detached dwelling to be used as a display home for a period of up to 5 years', 'Construction of a detached dwelling to be used as a display home for a period of up to 5 years and associated signage', 'Construction of a detached dwelling to be used as a temporary display home for a period of up to 4 years', 'Construction of a detached dwelling wiith a garage under the main roof', 'Construction of a detached dwelling with a garage and alfresco under main roof', 'Construction of a detached dwelling with a garage and alfresco under the main roof', 'Construction of a detached dwelling with a garage and terrace under main roof', 'Construction of a detached dwelling with a garage and verandah under main roof', 'Construction of a detached dwelling with a garage under main roof', 'Construction of a detached dwelling with a garage under the main roof', 'Construction of a detached dwelling with a garage under the main roof  and associated retaining walls', 'Construction of a detached dwelling with a garage under the main roof - WITHDRAWN', 'Construction of a detached dwelling with a garage under the main roof and an associated retaining wall', 'Construction of a detached dwelling with a garage under the main roof and retaining walls', 'Construction of a detached dwelling with a garage, alfresco and verandah under main roof and associated retaining wall', 'Construction of a detached dwelling with an attached garage and two verandahs', 'Construction of a detached dwelling with associated retaining walls and colorbond fencing (maximum hieght 3.6m)', 'Construction of a detached dwelling with attached carport and verandah', 'Construction of a detached dwelling with attached carport and verandah - Awaiting Civil Plans- WITHDRAWN', 'Construction of a detached dwelling with attached garage', 'Construction of a detached dwelling with attached garage  to be used as a temporary display home with associated office and advertising displays.', 'Construction of a detached dwelling with attached garage - (Lot 3120, Reel Tce)', 'Construction of a detached dwelling with attached garage and freestanding carport', 'Construction of a detached dwelling with attached garage and veradahs', 'Construction of a detached dwelling with attached garage and verandah', 'Construction of a detached dwelling with attached garage and verandah (temporary display home)', 'Construction of a detached dwelling with attached garage and verandah - Awaiting Civil Plan- WITH DRAWN', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary display home with associated office and advertising display.', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary display home with associated office and signage\n\nStage 1: Footings Only', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary display home with associated office and signage\n\nStage 2: Final', 'Construction of a detached dwelling with attached garage and verandah to be used as a temporary sales &amp; project office', 'Construction of a detached dwelling with attached garage and verandah under main roof', 'Construction of a detached dwelling with attached garage and verandahs', 'Construction of a detached dwelling with attached garage and verandahs - WITHDRAWN', 'Construction of a detached dwelling with attached garage and verandahs to be used as a temporary display home with associated office and signage\n\nStage 1: construction of display building and associated display office (only)', 'Construction of a detached dwelling with attached garage and verandahs- WITHDRAWN', 'Construction of a detached dwelling with attached garage and vernadah - Waiting on civil/stormwater plan- WITHDRAWN', 'Construction of a detached dwelling with attached garage and verndah', 'Construction of a detached dwelling with attached garage to be used as a temporary display home with associated advertising displays.', 'Construction of a detached dwelling with attached garage, verandah and associated retaining wall', 'Construction of a detached dwelling with attached garage, verandah and associated retaining wall -', 'Construction of a detached dwelling with attached garage, verandah and associated retaining wall - (Lot 25 Highview Drive)', 'Construction of a detached dwelling with attached garage.', 'Construction of a detached dwelling with attached verandah', 'Construction of a detached dwelling with attached verandah and a freestanding carport', 'Construction of a detached dwelling with carport UMR', 'Construction of a detached dwelling with carport under main roof', 'Construction of a detached dwelling with garage', 'Construction of a detached dwelling with garage UMR', 'Construction of a detached dwelling with garage UMR ( lot 2031 Lindgren Avenue', 'Construction of a detached dwelling with garage UMR ( lot 2032 Lindgren Avenue', 'Construction of a detached dwelling with garage UMR (Lot 15 Heysen Circuit)', 'Construction of a detached dwelling with garage UMR (Res Code)', 'Construction of a detached dwelling with garage UMR - WITHDRAWN', 'Construction of a detached dwelling with garage UMR- LODGED IN ERROR', 'Construction of a detached dwelling with garage UMR- WITHDRAWN', 'Construction of a detached dwelling with garage UMR- WITHDRAWN- COUNCIL ERROR', 'Construction of a detached dwelling with garage UMR- awaiting civil plan 8/12', 'Construction of a detached dwelling with garage and alfresco under main roof', 'Construction of a detached dwelling with garage and alfresco under main roof and associated retaining walls', 'Construction of a detached dwelling with garage and veranda under main roof', 'Construction of a detached dwelling with garage and verandah under main roof', 'Construction of a detached dwelling with garage and verandah under main roof and retaining walls to a maximum height of 3.5m', 'Construction of a detached dwelling with garage and verandahs under main roof', 'Construction of a detached dwelling with garage located under main roof', 'Construction of a detached dwelling with garage under main roof', 'Construction of a detached dwelling with garage under main roof ( Lot 87 Parkvale Drive)', 'Construction of a detached dwelling with garage under main roof - WITHDRAWN', 'Construction of a detached dwelling with garage under main roof and a verandah', 'Construction of a detached dwelling with garage under main roof.', 'Construction of a detached dwelling with garage under the main roof', 'Construction of a detached dwelling with garage under the main roof ( Lot 109 Damien Street)', 'Construction of a detached dwelling with garage under the main roof - Lot 111 Damien Street', 'Construction of a detached dwelling with garage under the main roof.', 'Construction of a detached dwelling with garage underthe main roof ( Lot 127 Parkvale Drive)', 'Construction of a detached dwelling with the garage under the main roof', 'Construction of a detached dwelling with the garage under the main roof.', 'Construction of a detached dwelling with verandah and garage (Lot 170 Damien street)', 'Construction of a detached dwelling with verandah and garage under main roof', 'Construction of a detached dwelling with verandah and garage under main roof (Lot 2022 Lindgren Avenue)', 'Construction of a detached dwelling with verandah and garage under main roof (Lot 2023 Lindgren Avenue)', 'Construction of a detached dwelling with verandah and garage under main roof - WITHDRAWN', 'Construction of a detached dwelling with verandah and garage under mian roof', 'Construction of a detached dwelling with verandah, porch and  garage under main roof', 'Construction of a detached dwelling with verandahs and garage under main roof', 'Construction of a detached dwelling with verandahs and garage under main roof (Lot 117 Damien street)', 'Construction of a detached dwelling- Rescode certified', 'Construction of a detached dwelling- WITHDRAWN', 'Construction of a detached dwelling- rescode certified', 'Construction of a detached dwelling- rescode certified WITHDRAWN', 'Construction of a detached dwelling-WITHDRAWN', 'Construction of a detached dwelling.', 'Construction of a detached dwellng with garage UMR', 'Construction of a disability toilet - Fremont Park', 'Construction of a domesetic outbuilding (shed)', 'Construction of a domestic garage', 'Construction of a domestic out building - Sch1a', 'Construction of a domestic out building - sch 1a', 'Construction of a domestic out building - sch1a', 'Construction of a domestic out building and verandah', 'Construction of a domestic outbuilding', 'Construction of a domestic outbuilding  - Sch1A', 'Construction of a domestic outbuilding &amp; a Verandah', 'Construction of a domestic outbuilding (garage)', 'Construction of a domestic outbuilding (garage), 1.8m high masonary fence, pool equipment shed and verandah\n\nStage 1: Domestic outbuilding (garage) and 1.8m high masonary fence', 'Construction of a domestic outbuilding (garage), 1.8m high masonary fence, pool equipment shed and verandah\nStage 1: Domestic outbuilding (garage) and 1.8m high masonary fence\nStage 2: Pool equipment shed and verandah', 'Construction of a domestic outbuilding (partially enclosed verandah)', 'Construction of a domestic outbuilding (shed)', 'Construction of a domestic outbuilding (shed) &amp; verandah', 'Construction of a domestic outbuilding (workshop &amp; garage)', 'Construction of a domestic outbuilding - Rescode certified', 'Construction of a domestic outbuilding - SCH1A', 'Construction of a domestic outbuilding - Sch 1a', 'Construction of a domestic outbuilding - Sch1A', 'Construction of a domestic outbuilding - Sch1a', 'Construction of a domestic outbuilding - Schedule 1A', 'Construction of a domestic outbuilding - Shed', 'Construction of a domestic outbuilding - rescode certified', 'Construction of a domestic outbuilding - sch 1a', 'Construction of a domestic outbuilding - sch1a', 'Construction of a domestic outbuilding -Sch1a', 'Construction of a domestic outbuilding and carport', 'Construction of a domestic outbuilding and the temporary placement of three shipping containers for a period of 12 months', 'Construction of a domestic outbuilding and two verandahs', 'Construction of a domestic outbuilding and verandahs', 'Construction of a domestic outbuilding- SCH1A', 'Construction of a domestic outbuilding- Sch 1a', 'Construction of a domestic outbuilding- Sch1A', 'Construction of a domestic outbuilding- sch1a', 'Construction of a domestic shed - Sch1A', 'Construction of a double storey detached dwelling - rescode certified', 'Construction of a dwelliing (Res Code Certified )', 'Construction of a dwelling', 'Construction of a dwelling ( Lot 238 Greenhood)', 'Construction of a dwelling ( Lot 240 Greenhood)', 'Construction of a dwelling ( Lot 241 Greenhood)', 'Construction of a dwelling ( Res Code Certified)', 'Construction of a dwelling (Lot 239 Greenhood)', 'Construction of a dwelling (Res Code Certifed)', 'Construction of a dwelling (Res Code Certified)', 'Construction of a dwelling (Res Code)', 'Construction of a dwelling (lot 206)', 'Construction of a dwelling -  rescode certified', 'Construction of a dwelling - -rescode certified', 'Construction of a dwelling - ResCode Certified', 'Construction of a dwelling - Rescode Certfied', 'Construction of a dwelling - Rescode Certified', 'Construction of a dwelling - Rescode certifed', 'Construction of a dwelling - Rescode certified', 'Construction of a dwelling - Rescode certified - (Lot 2)', 'Construction of a dwelling - rescode certifed', 'Construction of a dwelling - rescode certified', 'Construction of a dwelling - rescode certified - WITHDRAWN', 'Construction of a dwelling - rescode certified- WITHDRAWN', 'Construction of a dwelling - resocde certified', 'Construction of a dwelling -Res Code Certifed', 'Construction of a dwelling -Rescode certified', 'Construction of a dwelling addition - Rescode certified', 'Construction of a dwelling addition, verandahs and deck', 'Construction of a dwelling and a carport', 'Construction of a dwelling extension', 'Construction of a dwelling extension (bathroom extension)', 'Construction of a dwelling extension - rescode certified', 'Construction of a dwelling extension, verandah and installation of a pool', 'Construction of a dwelling for the purposes of supported accomodation ( Lot 2)', 'Construction of a dwelling for the purposes of supported accomodation (Lot 1)', 'Construction of a dwelling in the form of dependent accommodation', 'Construction of a dwelling with attached garage - WITHDRAWN', 'Construction of a dwelling with attached garage and verandah', 'Construction of a dwelling with attached garage and verandah- WITHDRAWN', 'Construction of a dwelling with detached carport', 'Construction of a dwelling with garage - Rescode certified', 'Construction of a dwelling with garage UMR', 'Construction of a dwelling with garage under main roof', 'Construction of a dwelling with retaining walls', 'Construction of a dwelling, carport and deck (lot 212 )', 'Construction of a dwelling- Rescode Certified', 'Construction of a dwelling- Rescode certified', 'Construction of a dwelling- Rescode certified - WITHDRAWN', 'Construction of a dwelling- rescode certified', 'Construction of a dwelling. RES CODE certified', 'Construction of a farm building', 'Construction of a farm building and fence', 'Construction of a farm implement shed', 'Construction of a fence 2.5m - Brookmont Stage 5 perimeter fence', 'Construction of a freestanding gable verandah', 'Construction of a freestanding verandah (Site 41)', 'Construction of a front fence', 'Construction of a gable verandah ( Schedule 1A)', 'Construction of a garage and demolition of existing carport', 'Construction of a glasshouse\n\nStage 2: Final', 'Construction of a greenhouse with associated dam and carparking', 'Construction of a horse shelter', 'Construction of a implement shed', 'Construction of a implement shed and rainwater tank', 'Construction of a implement shed for use in association with existing farming operations', 'Construction of a light industrial building (caravan repairs) with associated carparking and landscaping', 'Construction of a masonry fence with  signage', 'Construction of a new dwelling - Rescode certified', 'Construction of a new entry and crossover- refferal from SCAP for Council to provide comment', 'Construction of a new glass balustrade - Level 1 Building 7', 'Construction of a outbuilding', 'Construction of a outbuilding with attached verandah', 'Construction of a packing shed', 'Construction of a partially enclosed verandah', 'Construction of a pump and storage shed in association with existing horticulture', 'Construction of a replacement fence (2.19m high) on existing retaining wall', 'Construction of a retaining wall', 'Construction of a retaining wall (1m) with a total fence height of 2.8m', 'Construction of a retaining wall (Stage 3 &amp; 4 Evergreen Estate)', 'Construction of a retaining wall (maximum height 750mm) and fence (1.8m)', 'Construction of a retaining wall and fence', 'Construction of a rumpus room', 'Construction of a second dwelling in the form of dependent accomodation', 'Construction of a shade sail', 'Construction of a shade sail ( Fremont park)', 'Construction of a shade sail structure', 'Construction of a shed', 'Construction of a shed - Sch 1a', 'Construction of a shed - Sch1a', 'Construction of a sign - park reserve (Parkview Walk)\nSchedule 3, Part 2(e) ? buildings in a recreation area- Withdrawn', 'Construction of a sign - park reserve (Perre Reserve)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve (Ramsay Park)', 'Construction of a sign - park reserve (Secombe Street)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve (Virginia Oval-Sign 2)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve (Virginia Oval-sign 1)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn', 'Construction of a sign - park reserve sign (California Reserve)\nSchedule 3, Part 2(e) ? buildings in a recreation area - Withdrawn</t>
         </is>
       </c>
     </row>
@@ -3607,22 +3607,22 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E36" t="n">
-        <v>1400</v>
+        <v>1424</v>
       </c>
       <c r="F36" t="n">
-        <v>0.5394990366088632</v>
+        <v>0.490020646937371</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>12.09919011525817</v>
+        <v>11.43461861138663</v>
       </c>
       <c r="I36" t="n">
-        <v>146.390401445161</v>
+        <v>130.7505027878696</v>
       </c>
       <c r="J36" t="n">
         <v>0</v>
@@ -3667,13 +3667,13 @@
         </is>
       </c>
       <c r="V36" t="n">
-        <v>2166</v>
+        <v>2459</v>
       </c>
       <c r="W36" t="n">
         <v>0</v>
       </c>
       <c r="X36" t="n">
-        <v>2600</v>
+        <v>2911</v>
       </c>
       <c r="Y36" t="n">
         <v>11</v>
@@ -3699,7 +3699,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>2595</v>
+        <v>2906</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -3732,7 +3732,7 @@
         <v>0</v>
       </c>
       <c r="O37" t="n">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="P37" t="n">
         <v>0</v>
@@ -3747,7 +3747,7 @@
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>2902805763</t>
+          <t>2917008003</t>
         </is>
       </c>
       <c r="T37" t="n">
@@ -3755,20 +3755,20 @@
       </c>
       <c r="U37" t="inlineStr"/>
       <c r="V37" t="n">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="W37" t="n">
         <v>0</v>
       </c>
       <c r="X37" t="n">
-        <v>24730</v>
+        <v>27710</v>
       </c>
       <c r="Y37" t="n">
-        <v>2119</v>
+        <v>2377</v>
       </c>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>['2900030351', '2900048009', '2900127006', '2900202002', '2900212008', '290023125*', '2900242004', '2900259009', '2900261504', '2900313706', '2900316405', '2900334136', '2900377443', '2900377849', '2900378008', '2900379000', '2900383501', '2900384002', '2900417003', '290042000*', '2900427009', '2900428060', '2900428407', '2900429012', '2900430304', '290043070*', '2900431710', '2900432908', '2900500501', '2900507201', '2900508802', '2900508909', '290050895*', '2900512211', '290051281*', '2900514217', '2900514962', '2900515711', '2900516810', '2900517856', '2900517899', '2900520051', '290052030*', '2900520852', '2900520908', '2900520959', '2900521206', '2900521425', '2900521732', '2900529195', '2900529611', '2900529873', '290053957*', '2900539609', '2900539641', '2900539684', '2900539705', '2900539721', '2900539756', '2900539780', '290053981*', '2900539879', '2900539940', '2900539959', '2900540175', '2900540378', '2900540570', '2900540677', '2900540773', '290054087*', '2900540976', '2900541071', '2900541178', '2900541354', '2900541442', '2900541485', '2900541549', '2900541581', '2900541610', '2900541688', '2900541741', '2900541784', '2900541813', '2900541848', '290054191*', '2900541987', '2900542015', '2900542082', '2900542189', '2900542218', '2900542314', '2900542381', '2900542445', '2900542488', '2900542517', '2900542680', '2900542787', '290054298*', '2900543085', '2900543288', '2900543384', '2900543480', '2900543587', '2900543683', '290054378*', '2900543886', '2900543982', '2900556580', '2900556687', '2900556716', '2900556740', '290055733*', '2900557399', '2900557428', '2900557786', '2900557815', '290055784*', '2900557903', '290055805*', '2900558084', '290055880*', '2900561128', '2900561160', '2900561240', '2900561443', '2900561726', '2900561806', '2900561881', '2900562403', '290056285*', '2900562956', '2900562964', '2900562980', '2900562999', '2900563000', '2900563019', '2900563027', '2900563721', '290056496*', '2900565284', '2900565313', '2900565348', '2900565372', '2900565401', '2900565524', '2900565559', '2900565583', '2900565612', '2900565647', '2900566295', '2900566519', '2900566551', '2900566594', '2900567343', '2900567570', '2900568696', '2900586018', '2900648012', '2900699602', '2900699709', '2900699901', '290079700*', '2900859901', '2901019007', '2901023006', '2901037002', '2901038507', '2901053002', '2901055307', '2901056000', '2901059009', '2901105001', '2901287001', '2901288004', '2901289007', '2901290008', '2901299205', '2901324052', '2901324079', '2901324095', '2901324159', '2901324175', '2901324191', '2901324212', '2901324239', '2901324271', '2901324319', '2901324351', '2901324714', '2901324781', '2901324802', '2901324829', '2901324861', '2901324888', '2901324909', '2901324925', '2901388005', '290159700*', '2901598002', '2901965001', '2901966004', '2901972009', '2901993002', '2902006056', '2902013002', '2902051201', '2902070007', '2902074008', '2902082104', '2902092003', '290209720*', '2902109653', '2902132204', '2902132909', '2902136002', '2902185015', '2902186501', '2902187010', '2902209507', '290222300*', '2902232002', '2902238017', '2902240504', '2902241013', '290224605*', '2902286000', '2902289009', '2902293008', '2902295003', '2902296006', '2902316003', '2902333006', '2902348013', '2902386001', '2902404003', '2902429008', '2902470051', '2902473404', '2902474503', '2902488008', '2902507002', '2902525606', '2902527003', '2902528006', '2902531010', '2902531555', '2902531619', '2902531731', '2902585000', '2902586003', '2902676500', '2902676703', '2902679306', '2902679402', '2902679808', '2902735400', '2902742205', '2902744008', '2902745000', '2902747209', '2902776106', '2902804664', '2902804699', '2902804728', '2902804816', '2902804891', '2902804920', '2902805034', '2902805050', '2902805077', '2902805093', '2902805114', '2902805157', '290280519*', '2902805253', '2902805616', '2902805640', '2902805675', '2902805704', '2902805739', '2902805763', '2902805827', '2902805886', '2902805915', '290280594*', '2902805974', '2902806002', '2902806037', '290280615*', '2902806432', '2902806459', '2902806571', '2902806600', '2902806635', '290280666*', '2902806694', '2902806811', '2902806846', '2902806870', '290280690*', '2902806934', '2902807881', '2902807902', '2902807929', '2902807945', '2902809801', '2902809860', '2902809967', '2902810108', '2902810124', '2902810140', '2902810183', '2902810204', '2902810220', '2902810247', '2902817086', '2902817107', '2902817123', '290281714*', '2902817166', '2902817182', '2902817203', '290281722*', '2902817246', '2902817262', '290281730*', '2902817326', '2902817342', '2902817369', '2902817385', '2902817406', '2902817449', '2902817465', '2902817502', '2902817529', '2902817545', '2902817561', '2902817588', '2902817625', '2902817641', '2902817668', '2902817684', '2902817705', '2902817721', '2902817764', '2902817828', '290281802*', '2902818046', '2902818054', '2902819524', '2902819540', '2902819567', '2902819583', '2902819647', '2902819671', '2902819735', '2902820015', '2902854469', '2902864106', '2902866259', '2902876203', '2902877601', '2902878006', '290287817*', '2902878620', '2902880608', '2902882603', '2902882806', '2902898015', '2902899042', '2902901317', '2902902504', '2902909001', '2903191003', '290320840*', '2903236005', '2903238000', '2903239003', '2903240004', '290324470*', '2903244902', '290324542*', '2903245438', '2903247724', '2903248807', '2903249201', '2903249703', '2903250106', '2903250202', '2903257017', '2903258351', '2903262588', '2903282300', '2903283311', '2903284269', '2903290909', '2903299102', '2903299209', '2903299938', '2903300185', '2903300257', '2903300329', '2903300396', '2903300468', '290330053*', '2903300601', '2903300679', '2903300740', '2903300812', '290330088*', '2903300951', '2903301022', '290330109*', '2903301161', '2903301233', '2903301305', '2903302703', '2903302842', '2903303247', '2903303263', '290330328*', '2903303327', '2903303343', '290330336*', '2903303386', '2903303466', '2903303503', '290330352*', '2903303546', '2903303589', '290330360*', '2903303642', '2903303669', '2903303685', '2903303845', '2903303888', '2903303941', '2903303968', '2903303984', '2903304557', '2903305808', '290330600*', '2903307010', '2903307029', '2903307045', '2903307088', '2903307109', '2903307125', '2903307141', '2903307168', '2903307184', '2903307205', '2903307221', '2903307264', '2903307280', '2903307301', '2903307328', '2903307344', '2903307360', '2903307387', '2903307408', '2903307424', '2903307440', '2903307504', '2903307520', '2903307547', '2903307563', '290330758*', '2903307600', '2903307627', '2903307643', '290330766*', '2903307686', '2903307707', '2903307723', '290330774*', '2903307766', '2903307782', '290330782*', '2903307846', '2903307862', '2903308507', '2903308574', '2903308638', '2903308662', '2903308750', '2903308814', '2903308849', '2903308902', '2903309032', '2903311749', '2903311781', '2903311829', '2903311861', '2903311984', '2903312055', '2903312135', '2903312178', '2903312215', '2903312530', '2903312610', '2903312653', '2903312733', '2903313138', '2903313218', '2903313410', '2903313699', '2903313891', '2903313939', '2903314624', '2903314704', '2903314974', '2903315045', '2903315088', '2903315117', '2903315141', '2903315256', '2903315280', '290331531*', '2903315344', '2903315379', '2903315408', '2903315483', '2903315627', '2903315651', '2903315686', '2903315715', '290331574*', '2903315803', '2903317104', '2903317462', '290331750*', '2903340160', '2903342422', '2903342430', '2903342457', '2903342473', '2903342481', '2903342502', '2903342510', '2903342529', '2903342537', '2903342561', '290334257*', '2903342596', '2903342609', '2903342625', '2903342641', '290334265*', '2903342684', '2903342705', '2903342713', '290334273*', '2903342748', '2903342764', '2903342772', '2903342780', '2903342799', '2903342828', '2903342836', '2903342852', '2903342879', '2903344030', '290334740*', '2903351804', '2903356808', '290335700*', '2903360508', '2903367013', '2903374010', '2903381018', '2903408006', '2903451004', '2903460007', '290346100*', '290359905*', '2903796002', '2903819200', '2903915059', '2903917062', '2903917206', '2903917249', '2903917900', '2903917943', '2903918161', '2903918241', '2903918655', '2903919738', '2903920122', '290392019*', '2903920210', '2903920376', '2903920384', '2903920392', '2903920456', '2903920499', '2903920528', '2903920560', '2903920579', '2903920587', '2903920595', '2903920608', '2903920616', '2903920624', '2903920632', '2903920747', '2903920755', '2903920878', '2903920982', '2903920990', '2903921053', '2903921061', '2903921088', '2903921096', '2903921192', '2903921205', '2903921213', '2903921221', '2903921248', '2903921256', '2903921264', '2903921272', '2903921280', '2903921299', '2903921301', '290392131*', '2903921344', '2903921352', '2903921360', '2903921379', '2903921395', '2903921424', '2903921432', '2903921440', '2903921504', '2903921598', '2903921600', '2903921619', '2903921627', '2903921635', '2903921643', '2903921651', '2903921678', '2903921686', '2903921694', '2903921707', '2903921731', '2903921758', '2903921774', '2903921790', '2903921803', '2903921811', '290392182*', '2903921854', '2903921870', '2903921889', '290392473*', '2903924983', '2903925601', '2903929709', '2903930750', '2903930857', '2903932641', '2903934014', '2903934022', '2903934057', '2903934065', '2903934073', '2903934081', '290393409*', '2903934102', '2903934110', '2903934129', '2903934137', '2903934145', '2903935666', '2903935869', '2903961880', '2903961901', '2903961960', '2903961987', '2903963309', '2903963421', '2903963448', '2903963499', '290396351*', '2903963552', '2903963579', '2903963595', '2903963632', '2903963819', '2903963894', '2903963931', '2903964408', '2903964424', '2903964467', '2903964483', '2903964504', '2903964520', '2903964547', '2903967086', '290396714*', '2903967166', '2903967182', '2903967289', '290396730*', '2903967342', '2903967369', '2903967385', '2903967406', '2903967422', '2903967449', '2903967465', '2903967481', '2903967529', '2903967545', '2903967561', '2903967588', '290396802*', '2903968046', '2903968062', '2903968089', '2903980475', '2903980483', '2903980547', '290398058*', '2903980600', '2903980635', '2903980643', '2903980854', '2903980942', '2903980950', '2903980969', '2903980977', '2903981849', '2903981865', '2903981881', '2903981902', '2903981929', '2904035002', '2904088200', '2904090300', '2904090351', '2904146458', '2904147426', '2904147442', '2904147864', '2904148146', '2904150940', '2904155987', '2904156023', '290415604*', '2904156066', '2904156429', '2904156445', '2904156680', '2904157261', '2904157309', '2904157325', '2904157341', '2904157413', '2904157675', '2904157691', '2904157739', '2904157755', '2904157915', '290415807*', '2904158096', '2904158192', '290415970*', '2904159849', '2904160348', '2904160428', '2904160487', '2904164840', '2904164875', '2904166459', '2904167400', '2904176008', '2904177350', '2904177502', '2904178054', '2904181800', '2904181851', '2904181907', '2904181958', '2904182002', '2904182053', '2904182109', '290418215*', '2904182205', '2904182256', '2904185211', '2904185246', '2904185270', '290418530*', '2904185334', '2904185852', '2904185895', '2904185916', '2904185932', '2904185975', '2904185991', '2904186011', '2904186054', '2904186070', '2904186097', '2904186134', '2904186150', '2904187305', '2904189407', '290419090*', '2904197589', '2904197677', '2904197706', '2904197730', '2904197765', '290419779*', '2904197829', '2904199007', '2904199031', '290419912*', '2904199154', '2904199189', '2904199218', '2904199314', '2904199517', '2904199613', '290419971*', '2904199816', '2904199912', '2904200012', '2904200119', '2904200215', '2904200311', '2904200418', '2904200514', '2904200610', '2904200717', '2904200813', '290420091*', '2904201015', '2904201111', '2904201218', '2904201314', '2904201410', '2904201517', '290420171*', '2904201816', '2904201920', '2904202026', '2904202229', '2904202325', '2904202421', '2904202528', '2904202624', '2904202720', '2904202827', '2904202923', '2904203125', '2904203221', '2904203328', '2904203424', '2904203520', '2904203627', '2904203723', '290420382*', '2904204128', '2904204224', '2904204427', '2904204523', '290420462*', '2904204726', '2904204822', '2904204929', '2904219805', '2904222721', '2904226773', '2904228656', '2904228701', '2904235549', '2904236816', '2904242159', '2904243258', '2904247902', '2904254782', '2904295605', '2904297459', '2904304233', '2904304444', '2904326707', '2904337852', '2904350969', '2904351312', '2904351857', '2904357562', '2904357837', '2904367859', '2904369037', '2904370804', '2904378013', '2904378216', '2904378312', '2904386507', '2904397708', '2904399404', '2904400700', '290440180*', '2904402802', '2904404453', '2904404509', '290440455*', '2904425000', '2904426206', '2904430029', '2904440008', '2904444543', '290444800*', '2904451452', '2904452906', '2904462063', '2904462098', '2904462127', '2904464800', '2904465555', '2904469441', '2904471955', '2904476801', '2904477126', '290447913*', '2904479156', '2904485951', '2904486102', '2904486153', '2904496976', '2904499755', '290450020*', '2904500736', '2904501085', '2904503814', '2904508172', '2904508930', '2904513860', '2904516682', '2904529504', '2904532922', '2904534696', '2904536149', '2904536384', '2904540607', '2904542370', '2904542936', '2904555454', '2904557759', '2904745004', '2904773005', '290493370*', '2904933953', '2904944353', '2905097408', '2905133405', '2905151902', '2905152358', '2905153406', '2905153553', '2905153668', '2905155807', '2905156025', '2905159357', '2905159605', '2905162900', '2905170150', '2905345707', '2905345723', '2905349409', '2905351402', '2905355403', '290612210*', '2906126506', '2906128608', '2906129627', '2906235913', '2906256503', '2906257805', '2906259501', '2906260158', '2906262401', '2906349451', '2906349558', '2906350305', '2906350356', '2906352706', '2906352909', '2906375940', '2906376740', '2906757551', '2906757850', '2906758503', '2906761200', '290676150*', '2906761956', '2906765500', '2906825606', '2906833550', '2906835855', '2906847709', '2906848402', '2906858301', '2906869908', '2906870036', '2906870159', '2906870757', '2906870837', '2906871602', '2906872007', '290687204*', '2906872082', '2906872162', '290687220*', '2906872242', '2906872322', '2906872365', '2906872445', '2906872488', '2906872525', '2906872568', '2906872605', '2906872648', '2906872680', '2906872728', '2906872760', '2906872808', '2906872840', '2906872920', '2906872963', '290687300*', '2906873042', '2906873122', '2906873165', '2906873202', '2906873245', '2906873288', '2906873325', '2906873368', '2906873405', '2906873448', '2906873480', '2906873528', '2906873560', '2906873608', '2906873640', '2906873683', '2906873720', '2906873763', '2906873800', '2906873843', '290693030*', '2906930350', '2906930553', '2906930609', '290693065*', '2906930705', '2906930756', '2906930801', '2906930908', '290694375*', '2906943805', '2906943856', '2906944015', '2906944058', '2906944103', '2906944154', '290694420*', '2906944306', '2906944357', '2906944402', '2906944453', '2906944656', '2906944701', '2906944752', '2906944808', '2906944859', '2906944904', '2906944955', '2906945018', '2906945050', '2906945106', '2906945157', '2906945253', '2906945309', '2906945552', '2906945608', '2906945659', '2906946053', '2906946408', '2906946504', '2906948251', '2906948358', '2906948403', '2906948454', '290694850*', '2906948809', '2906949158', '290694930*', '2906949350', '2906949510', '2906949609', '2906949852', '2906950001', '2906950204', '2906950255', '2906950300', '2906950351', '2906950407', '2906950757', '2906951514', '2907065207', '2907075157', '2907130806', '2907150452', '2907168513', '2907173005', '2907240212', '2907246008', '2907339044', '2907339060', '2907339087', '2907339108', '2907339167', '2907339183', '2907339204', '2907339220', '2907339247', '2907339263', '290733928*', '2907339300', '2907339327', '2907339343', '2907339386', '2907339407', '2907339423', '290733944*', '2907339466', '2907339482', '2907339618', '290734031*', '2907340416', '2907340512', '2907340619', '2907340715', '2907340811', '2907340918', '2907341013', '2907341312', '2907341419', '2907341515', '2907341611', '2907341718', '2907341814', '2907341910', '2907342112', '2907342219', '2907342315', '2907342710', '2907342913', '2907343019', '2907344214', '2907344249', '2907344273', '2907344302', '2907344337', '290734437*', '2907344409', '2907348039', '2907348063', '2907348098', '2907348151', '2907348303', '290734840*', '2907353006', '2907353057', '2907353102', '2907353153', '2907353209', '2907353305', '2907436127', '2907436223', '290743632*', '2907436522', '2907436629', '2907436725', '2907437322', '2907437621', '2907529606', '2907532100', '2907564102', '2907564153', '2907564903', '2907565957', '2907566001', '2907726052', '2907727354', '2907746205', '2907746539', '2907746563', '2907746803', '2907747005', '2907747128', '2907747152', '2907749246', '2907749289', '2907749326', '2907749481', '2907749545', '2907749609', '2907749668', '2907750052', '2907750140', '2907750204', '2907750474', '2907751303', '2907751389', '2907751426', '2907751469', '2907751485', '2907751506', '2907751522', '2907751549', '2907751565', '2907751581', '2907751602', '2907751629', '2907751645', '2907751661', '2907751688', '2907751741', '2907751901', '2907751952', '290779504*', '2908197658', '2908198992', '2908207000', '2908207748', '2908207764', '2908207780', '2908208011', '2908208118', '2908208214', '2908208310', '2908208417', '2908208513', '290820861*', '2908208716', '2908209460', '2908209903', '2908211405', '2908212053', '2908213101', '2908215457', '2908216652', '2908217006', '2908217903', '2908218105', '2908302358', '2908303350', '2908303801', '2908305807', '2908306105', '2908310702', '2908310905', '2908312206', '2908316100', '2908322359', '2908496009', '2908611804', '2908651101', '2908651208', '2908651507', '2908673108', '2908698604', '2908705018', '2908756157', '2908873003', '2908901000', '2908906856', '2908906952', '2908909504', '2908909555', '2908909600', '2908911014', '2908911057', '2908911356', '2908911508', '2908911807', '2909026252', '2909286011', '2909289001', '2909328007', '2909332014', '2909332209', '2909333009', '2909351004', '2909423004', '2909431012', '2909431151', '2909435005', '2909443005', '2909470011', '2909589004', '2909650258', '2909708106', '2909708800', '2909709221', '2909735008', '2909761003', '2909780503', '2909780618', '2909790007', '2909813117', '2909828028', '2909830507', '2909831016', '2909835500', '290983601*', '2909837602', '2909838015', '2909838402', '2909839202', '2909840019', '2909840801', '2909841206', '2909841601', '2909845012', '2909846015', '2909847018', '2909851017', '290985201*', '2909854015', '2909857021', '2909858016', '2909861020', '2909862015', '2909863026', '2909864010', '2909864504', '2909865013', '2909865507', '2909867027', '2909873777', '2909873881', '2909874120', '2909874235', '2909890008', '2909905003', '2909909004', '2909938008', '2910027009', '2910072002', '2910297017', '2910297033', '291029713*', '2910298108', '2910298247', '2910298335', '291029836*', '2910298482', '2910298546', '2910298722', '2910298757', '291029895*', '291034600*', '2910387004', '2910467004', '2910684009', '2910686004', '2910727005', '2910804007', '2910831005', '2910931006', '2910992001', '291110300*', '2911104002', '2911153007', '2911159003', '2911183003', '2911184006', '2911275004', '2911276007', '2911280006', '2911320004', '291133801*', '2911353009', '2911359005', '2911401007', '2911419004', '2911492009', '2911493001', '2911503003', '2911513009', '2911514001', '2911515004', '2911516007', '2911547006', '2911599009', '2911616008', '2911617000', '2911684019', '2911685011', '2911703013', '2911705000', '2911748000', '2911792001', '2911880001', '2911953004', '2911954007', '2911988004', '2912052005', '2912053008', '2912132312', '2912172007', '2912338003', '2912345000', '2912549003', '2912670698', '2912670719', '2912685558', '2912686112', '2912746701', '2912747210', '2912748002', '2912776003', '2912800640', '2912867255', '2912905004', '291293100*', '2912944003', '291296205*', '2912965058', '2912980506', '2912989009', '2913014107', '2913014203', '2913014406', '2913081000', '2913086004', '2913138003', '2913143005', '2913147006', '2913149001', '2913171006', '2913186005', '2913191007', '2913193002', '291320500*', '2913211602', '291352705*', '2913788508', '2913788815', '2913791707', '2913796305', '2913796364', '2913798378', '2913798490', '2913810509', '2913810568', '2913810592', '2913811341', '2913814358', '2913842009', '2913844012', '2913850340', '291386227*', '2913869869', '2913869914', '2913870501', '2913870851', '2913871002', '2913872451', '2914100058', '2914100154', '2914106062', '2914110045', '2914110088', '2914110125', '2914110168', '2914110205', '2914110248', '2914110280', '2914110408', '2914110440', '2914110520', '2914110563', '2914110643', '2914110723', '2914110766', '2914110803', '2914110846', '2914111363', '2914111486', '2914111523', '2914111566', '2914111689', '2914111881', '2914111929', '2914112008', '2914112120', '2914112403', '2914112964', '2914113561', '2914113684', '2914114169', '291411496*', '2914115081', '2914115161', '2914115209', '2914116164', '2914116244', '2914116287', '2914116324', '2914116447', '291411648*', '2914116527', '291411656*', '2914116682', '291411672*', '2914116762', '2914116842', '2914117642', '2914117749', '2914117941', '2914118047', '291411824*', '2914118346', '2914118442', '2914118549', '2914118645', '2914138144', '2914138208', '2914138232', '2914138267', '2914140674', '2914141036', '2914142020', '2914142194', '2914252676', '2914252713', '291425273*', '2914253257', '2914254807', '2914255113', '2914259421', '2914259544', '2914263308', '2914264714', '2914265370', '2914272503', '2914272511', '2914272618', '2914272714', '2914274154', '2914274533', '2914274568', '2914274779', '2914274998', '2914276029', '2914278382', '2914278542', '2914281952', '2914282226', '2914282461', '2914282760', '2914282795', '2914282824', '2914282859', '2914282883', '2914282912', '2914282947', '2914282971', '2914283018', '2914283042', '2914289559', '2914537954', '2914566704', '2914566851', '2914567205', '291456731*', '2914568574', '2914569024', '2914571554', '2914579855', '2914584419', '291458980*', '2914593809', '2914595206', '291460060*', '2914601549', '2914602509', '2914602859', '2914602947', '2914607596', '2914610402', '2914614956', '2914646800', '2914652100', '2914654202', '2914656654', '2914706201', '2914716004', '2914723458', '2914788657', '2914789107', '2914792402', '2914796067', '2914796366', '2915029003', '2915073303', '2915085603', '2915095457', '2915106224', '2915119447', '2915120165', '2915120464', '2915123278', '2915123972', '2915124561', '2915133900', '2915143228', '2915143391', '2915146306', '2915153100', '2915159908', '2915163552', '2915164651', '2915190155', '2915203008', '2915207332', '2915211032', '2915211534', '2915219915', '2915260109', '2915260707', '2915346551', '2915347503', '2915351203', '291535130*', '2915351473', '2915624259', '291562665*', '2915637754', '2915638001', '2915639151', '2915647303', '2915668307', '291566850*', '2915780016', '2915780200', '2915780411', '2915807004', '2915849001', '2915850002', '2915953001', '2915986006', '2916093007', '2916169008', '2916229007', '2916244004', '291628900*', '291632600*', '2916328005', '291634200*', '2916387806', '2916399807', '2916447004', '291644900*', '2916474002', '2916572008', '2916755007', '2916795009', '2916810053', '2916810969', '2916812075', '2916812139', '2916812796', '2916833837', '2917334407', '2917334909', '2917346379', '2917531005', '2917612008', '2917639008', '2917723007', '2917802004', '2917834153', '2917838605', '2917868003', '2917941004', '2918053009', '2918067005', '2918111301', '2918111707', '2918158003', '291816100*', '2918312007', '2918362004', '2918384000', '2918621002', '2918634014', '2918698050', '2918716001', '2918740001', '2918747000', '2918810153', '2918812802', '2918815253', '2918818956', '2918820706', '2918825857', '2918828126', '2918858851', '2918865808', '2918867600', '2918880768', '2918881808', '2918887898', '291888980*', '2918960004', '2919013009', '2919036008', '2919066645', '2919067162', '2919067226', '2919067402', '2919067904', '2919087251', '2919087358', '2919088801', '2919168406', '291919900*', '2919207006', '2919212008', '2919226055', '2919305626', '291940785*', '2919409150', '2919543202', '2919613004', '2919619000', '2919697009', '2919777009', '2919803000', '2919858001', '2919926000', '2919944006', '2919950000', '2919959013', '2919980058', '2919987532', '2920002104', '2920002200', '2920009103', '2920056209', '2920057260', '2920058909', '2920059100', '2920060558', '2920060806', '2920062457', '292006257*', '2920063302', '2920063900', '2920064102', '2920064305', '292006580*', '2920066909', '2920158002', '2920274003', '2920302000', '2920311003', '2920329019', '2920330159', '2920330255', '2920330503', '2920330917', '2920332509', '2920335259', '2920358004', '2920367007', '2920369002', '2920393002', '2920395008', '2920397003', '2920434521', '2920434986', '2920445001', '2920477302', '2920494516', '292049900*', '2920537002', '2921107004', '2921132007', '2921136008', '2921164009', '2921198006', '2921199009', '2921224008', '2921229052', '2921230504', '2921237423', '2921240016', '2921265707', '2921266750', '2921268211', '2921303005', '2921351007', '292138700*', '2921393012', '2921403006', '2921415007', '2921420017', '2921421001', '2921452799', '2921466007', '2921470313', '2921471009', '3229803008', '3229817004', '3229876004', '323003500*', '3230090009', '3230144003', '3230164004', '3230360005', '3230495305', '3230552007', '3230580008', '3230601008', '3230663006', '3230673001', '3230704007', '3230756333', '3230759008', '3230786006', '3230850004', '3230881003', '3230888002', '3230944000', '3230965004', '3230978008', '3231033006', '3231057008', '3231060506', '323106200*', '3231129008', '3231327004', '3231328007', '3231372016', '3231376009', '3231522600', '3231655059', '3231658006', '3231659009', '3231678007', '323167900*', '3231680000', '3231681003', '3231789006', '3231899707', '323191900*', '3231934509', '3231979002', '3232079006', '3232174003', '3232184105', '3232336009', '3232422003', '3232422118', '3232448000', '3232509002', '3232535008', '3232596003', '3232610055', '3232675000', '3232798000', '3232806007', '3232848004', '3233146004', '3233179009', '3233317002', '3233331007', '3233475000', '3233499002', '3233512000', '3233593007', '3233612001', '3233614007', '3233640002', '3233725006', '3233881009', '3233883004', '323388500*', '3234104359', '3234160000', '3234230005', '3234301002', '3234346008', '3234478000', '3234479003', '3234573008', '3234632004', '3234649009', '3234719003', '3234740005', '3234833164', '3234840014', '3234989257', '3235062007', '3235120000', '323512700*', '3235200019', '3235453008', '3235486002', '3235500003', '3235673019', '3235734459', '3235743005', '3235798006', '323580375*', '3235843313', '3235854004', '3235983308', '3236718100', '3236762005', '3236992134', '3237030308', '3237045200', '323710002*', '3237102500', '3237106202', '3237134000', '3237134019', '3237232006', '3237252007', '323725415*', '3237409502', '3237418505', '3237441502', '3237668002', '3237721459', '3237721803', '3237745055', '3237774059', '3237775051', '323788889*', '323788950*', '3237932053', '323793805*', '3237947132', '3237953508', '3237953807', '3237954404', '3238143056', '323815605*', '3238157052', '323820105*', '3238261052', '3238271058', '323827905*', '3238327058', '3238348051', '3238415058', '3238426005', '3238506312', '323851104*', '3238600106', '3238602005', '3238642365', '3238710057', '3238775053', '3238800706', '3238811229', '323885005*', '3238855053', '3238870050', '3238872806', '3238873227', '3238873606', '3238873905', '3238875804', '3238876559', '323887721*', '3238877279', '3238877404', '3238883708', '323888556*', '3238885623', '3238889253', '3238894503', '3238922201', '3238922607', '3238922658', '3241975005', '3241992008', '3241992059', '3242024252', '3242024957', '3242025001', '3242031057', '3242043058', '3242077004', '3242115007', '324212005*', '3242121001', '3242141002', '324482208*', '324488300*', '3244884002', '3244948002', '3245074001', '3245395008', '3245410001', '3245420007', '324544210*', '3245448501', '3245487009', '3245538005', '3245571008', '3245602257', '3245657004', '3245711007', '3245809004', '3246503007', '3246504106', '3246524000', '3246583000', '3246649006', '3246669007', '324668600*', '3246688101', '3246727000', '3246732002', '3246781007', '3246812002', '3246896007', '3246901005', '3246939003', '3246953008', '3247106003', '3247186007', '3247235294', '3247240114', '3247242515', '324724561*', '3247311760', '3247750018', '3247750210', '3247768023', '324776820*', '3247768402', '3247780209', '3247815221', '3247943004', '3247953608', '3247954002', '324795570*', '3248001000', '3248006944', '3248007576', '3248008384', '3248036051', '3248053003', '3248128001', '3248172002', '3248185006', '324823201*', '3248232116', '3248266009', '3248272003', '3248276004', '3248361401', '3248371001', '3248409006', '3248442017', '3248551002', '3248683005', '3248705008', '3248721059', '3248799008', '3248840007', '3248870353', '3248967200', '3248987703', '3249007359', '3249061005', '3249082009', '3249093402', '3249104001', '3249115253', '3249138009', '3249349201', '3249351002', '3249419003', '324952900*', '3249794006', '3249881011', '324996700*', '3250069055', '3250125002', '3250166007', '3250230005', '3250233070', '3250356003', '3250422007', '3250433005', '3250443000', '3250587004', '3250635002', '325171700*', '3251742002', '3251796000']</t>
+          <t>['2900030351', '2900048009', '2900127006', '2900187009', '2900202002', '2900212008', '290023125*', '2900242004', '2900259009', '2900261504', '2900313706', '2900316405', '2900334136', '2900377443', '2900377849', '2900378008', '2900379000', '2900383501', '2900384002', '2900417003', '290042000*', '2900427009', '2900428060', '2900428407', '2900429012', '2900430304', '290043070*', '2900431200', '2900431710', '2900432908', '2900500501', '2900507201', '2900508802', '2900508909', '290050895*', '2900512211', '290051281*', '2900514217', '2900514962', '2900515711', '2900516810', '2900517856', '2900517899', '2900520051', '290052030*', '2900520705', '2900520801', '2900520852', '2900520908', '2900520959', '2900521206', '2900521425', '2900521732', '2900521804', '2900529195', '2900529611', '2900529873', '290053957*', '2900539609', '2900539641', '2900539684', '2900539705', '2900539721', '2900539756', '2900539780', '290053981*', '2900539879', '2900539940', '2900539959', '2900540175', '2900540271', '2900540378', '2900540570', '2900540677', '2900540773', '290054087*', '2900540976', '2900541071', '2900541178', '2900541354', '2900541389', '2900541442', '2900541485', '2900541514', '2900541549', '2900541581', '2900541610', '2900541688', '2900541717', '2900541741', '2900541784', '2900541813', '2900541848', '290054191*', '2900541944', '2900541987', '2900542015', '290054204*', '2900542082', '2900542189', '2900542218', '2900542242', '2900542314', '2900542381', '2900542445', '2900542488', '2900542517', '2900542584', '2900542680', '2900542787', '290054298*', '2900543085', '2900543181', '2900543288', '2900543384', '2900543480', '2900543587', '2900543683', '290054378*', '2900543886', '2900543982', '2900556580', '2900556687', '2900556716', '2900556740', '2900556863', '2900557022', '2900557102', '2900557145', '2900557188', '290055733*', '2900557399', '2900557428', '2900557786', '2900557815', '290055784*', '2900557903', '290055805*', '2900558084', '2900558121', '290055880*', '2900561128', '2900561160', '2900561240', '2900561320', '2900561443', '2900561726', '2900561806', '2900561849', '2900561881', '2900562403', '290056285*', '2900562948', '2900562956', '2900562964', '2900562980', '2900562999', '2900563000', '2900563019', '2900563027', '2900563721', '2900564820', '290056496*', '2900565284', '2900565313', '2900565348', '2900565372', '2900565401', '2900565524', '2900565559', '2900565583', '2900565612', '2900565647', '2900566295', '2900566519', '2900566551', '2900566594', '2900567343', '2900567570', '2900568696', '2900586018', '2900648012', '2900699602', '2900699709', '2900699901', '290079700*', '2900859901', '2901019007', '2901023006', '2901037002', '2901038507', '2901053002', '2901055307', '2901056000', '2901059009', '2901073054', '2901105001', '2901287001', '2901288004', '2901289007', '2901290008', '2901299205', '2901324052', '2901324079', '2901324095', '2901324159', '2901324175', '2901324191', '2901324212', '2901324239', '2901324271', '2901324319', '2901324327', '2901324351', '2901324714', '2901324781', '2901324802', '2901324829', '2901324861', '2901324888', '2901324909', '2901324925', '2901388005', '290159700*', '2901598002', '2901965001', '2901966004', '2901972009', '2901993002', '2902006056', '2902013002', '2902051201', '2902070007', '2902074008', '2902082104', '2902086009', '2902092003', '2902094455', '290209720*', '2902109653', '2902132204', '2902132909', '2902136002', '2902185015', '2902186501', '2902187010', '2902209507', '290222300*', '2902232002', '2902238017', '2902240504', '2902241013', '290224605*', '2902286000', '2902289009', '2902293008', '2902295003', '2902296006', '2902316003', '2902333006', '2902348013', '2902386001', '2902404003', '2902429008', '2902465009', '2902470051', '2902473404', '2902474503', '2902488008', '2902507002', '2902525606', '2902527003', '2902528006', '2902531010', '290253107*', '2902531432', '2902531555', '2902531619', '2902531731', '2902534000', '2902546001', '2902585000', '2902586003', '2902676500', '2902676703', '2902679306', '2902679402', '2902679808', '2902703003', '2902735400', '2902742205', '2902744008', '2902745000', '2902747209', '2902747727', '2902776106', '2902804664', '2902804699', '2902804728', '2902804816', '2902804891', '2902804920', '2902805034', '2902805050', '2902805077', '2902805093', '2902805114', '2902805157', '2902805173', '290280519*', '2902805253', '2902805616', '2902805640', '2902805675', '2902805704', '2902805739', '2902805763', '2902805827', '2902805851', '2902805886', '2902805915', '290280594*', '2902805974', '2902806002', '2902806037', '290280615*', '2902806432', '2902806459', '2902806571', '2902806600', '2902806635', '290280666*', '2902806694', '2902806811', '2902806846', '2902806870', '290280690*', '2902806934', '2902807881', '2902807902', '2902807929', '2902807945', '2902809801', '2902809844', '2902809860', '2902809967', '2902810108', '2902810124', '2902810140', '2902810183', '2902810204', '2902810220', '2902810247', '2902810263', '290281028*', '2902810300', '2902810343', '2902810386', '2902810407', '2902810423', '290281044*', '2902810466', '2902810503', '2902810546', '290281060*', '2902810626', '2902810642', '2902810669', '2902810706', '2902810722', '2902810749', '2902810757', '2902810845', '2902810861', '2902810909', '2902810984', '2902811047', '2902811063', '2902811100', '2902817086', '2902817107', '2902817123', '290281714*', '2902817166', '2902817182', '2902817203', '290281722*', '2902817246', '2902817262', '290281730*', '2902817326', '2902817342', '2902817369', '2902817385', '2902817406', '2902817449', '2902817465', '2902817481', '2902817502', '2902817529', '2902817545', '2902817561', '2902817588', '2902817625', '2902817641', '2902817668', '2902817684', '2902817705', '2902817721', '2902817764', '2902817780', '2902817828', '290281802*', '2902818046', '2902818054', '2902819524', '2902819540', '2902819567', '2902819583', '2902819647', '2902819671', '2902819735', '2902820015', '2902854469', '2902864106', '2902866259', '2902876203', '2902877601', '2902878006', '290287817*', '2902878620', '2902878858', '2902880608', '2902882603', '2902882806', '2902886268', '2902898015', '2902899042', '2902901317', '2902902504', '2902909001', '2903191003', '290320840*', '2903236005', '2903238000', '2903239003', '2903240004', '290324470*', '2903244902', '290324542*', '2903245438', '2903247724', '2903248102', '2903248807', '2903249201', '2903249703', '2903250106', '2903250202', '2903257017', '2903258351', '2903262588', '2903282300', '290328260*', '2903283311', '2903284269', '2903290909', '2903299102', '2903299209', '2903299604', '2903299938', '2903300185', '2903300257', '2903300329', '2903300396', '2903300468', '290330053*', '2903300601', '2903300679', '2903300740', '2903300812', '290330088*', '2903300951', '2903301022', '290330109*', '2903301161', '2903301233', '2903301305', '2903302703', '2903302789', '2903302842', '2903303247', '2903303263', '290330328*', '2903303327', '2903303343', '290330336*', '2903303386', '2903303466', '2903303503', '290330352*', '2903303546', '2903303589', '290330360*', '2903303642', '2903303669', '2903303685', '2903303845', '2903303888', '2903303941', '2903303968', '2903303984', '2903304557', '2903305808', '290330600*', '2903307010', '2903307029', '2903307045', '2903307088', '2903307109', '2903307125', '2903307141', '2903307168', '2903307184', '2903307205', '2903307221', '2903307264', '2903307280', '2903307301', '2903307328', '2903307344', '2903307360', '2903307387', '2903307408', '2903307424', '2903307440', '2903307483', '2903307504', '2903307520', '2903307547', '2903307563', '290330758*', '2903307600', '2903307627', '2903307643', '290330766*', '2903307686', '2903307707', '2903307723', '290330774*', '2903307766', '2903307782', '290330782*', '2903307846', '2903307862', '2903308507', '2903308574', '2903308638', '2903308662', '2903308697', '2903308750', '2903308814', '2903308849', '2903308902', '2903308961', '2903309032', '2903309067', '2903311749', '2903311781', '2903311829', '2903311861', '2903311984', '2903312055', '2903312135', '2903312178', '2903312215', '2903312530', '2903312610', '2903312653', '2903312733', '2903313138', '2903313218', '2903313410', '2903313699', '2903313891', '2903313939', '2903314624', '2903314704', '2903314974', '2903315045', '2903315088', '2903315117', '2903315141', '2903315256', '2903315280', '290331531*', '2903315344', '2903315379', '2903315408', '2903315483', '2903315627', '2903315651', '2903315686', '2903315715', '290331574*', '2903315803', '2903317104', '2903317462', '290331750*', '2903340160', '2903342422', '2903342430', '2903342457', '2903342473', '2903342481', '2903342502', '2903342510', '2903342529', '2903342537', '2903342561', '290334257*', '2903342596', '2903342609', '2903342625', '2903342641', '290334265*', '2903342684', '2903342705', '2903342713', '2903342721', '290334273*', '2903342748', '2903342764', '2903342772', '2903342780', '2903342799', '2903342828', '2903342836', '2903342852', '2903342879', '2903344030', '2903346001', '290334740*', '2903351804', '2903352305', '2903356808', '290335700*', '2903360508', '2903367013', '2903374010', '2903381018', '2903408006', '2903451004', '2903460007', '290346100*', '290354100*', '2903578101', '290359905*', '2903796002', '2903819104', '2903819200', '2903915059', '2903917062', '2903917206', '2903917249', '2903917900', '2903917943', '2903918161', '2903918241', '2903918655', '2903919738', '2903920122', '2903920149', '290392019*', '2903920210', '2903920376', '2903920384', '2903920392', '2903920456', '2903920499', '2903920501', '290392051*', '2903920528', '2903920560', '2903920579', '2903920587', '2903920595', '2903920608', '2903920616', '2903920624', '2903920632', '2903920640', '2903920747', '2903920755', '2903920878', '2903920966', '2903920982', '2903920990', '2903921053', '2903921061', '290392107*', '2903921088', '2903921096', '2903921192', '2903921205', '2903921213', '2903921221', '2903921248', '2903921256', '2903921264', '2903921272', '2903921280', '2903921299', '2903921301', '290392131*', '2903921328', '2903921344', '2903921352', '2903921360', '2903921379', '2903921395', '2903921408', '2903921416', '2903921424', '2903921432', '2903921440', '2903921467', '2903921504', '2903921598', '2903921600', '2903921619', '2903921627', '2903921635', '2903921643', '2903921651', '2903921678', '2903921686', '2903921694', '2903921707', '2903921723', '2903921731', '2903921758', '2903921774', '2903921782', '2903921790', '2903921803', '2903921811', '290392182*', '2903921854', '2903921870', '2903921889', '290392473*', '2903924983', '2903925601', '2903929709', '2903930750', '2903930857', '2903932641', '2903934014', '2903934022', '2903934057', '2903934065', '2903934073', '2903934081', '290393409*', '2903934102', '2903934110', '2903934129', '2903934137', '2903934145', '2903934153', '2903935666', '2903935869', '2903961880', '2903961901', '2903961928', '2903961960', '2903961987', '2903963309', '2903963421', '2903963448', '2903963499', '290396351*', '2903963552', '2903963579', '2903963595', '2903963632', '2903963819', '2903963894', '2903963931', '2903964408', '2903964424', '2903964467', '2903964483', '2903964504', '2903964520', '2903964547', '2903967086', '2903967107', '290396714*', '2903967166', '2903967182', '290396722*', '2903967246', '2903967262', '2903967289', '290396730*', '2903967342', '2903967369', '2903967385', '2903967406', '2903967422', '2903967449', '2903967465', '2903967481', '2903967502', '2903967529', '2903967545', '2903967561', '2903967588', '290396802*', '2903968046', '2903968062', '2903968089', '2903980467', '2903980475', '2903980483', '2903980547', '290398058*', '2903980600', '2903980635', '2903980643', '2903980854', '2903980942', '2903980950', '2903980969', '2903980977', '2903981849', '2903981865', '2903981881', '2903981902', '2903981929', '2904035002', '2904088200', '2904090300', '2904090351', '2904138511', '2904146458', '2904147426', '2904147442', '2904147864', '2904148146', '2904150940', '2904152540', '2904155987', '2904156023', '290415604*', '2904156066', '2904156429', '2904156445', '2904156680', '2904157261', '2904157309', '2904157325', '2904157341', '2904157413', '2904157675', '2904157691', '2904157739', '2904157755', '2904157915', '290415807*', '2904158096', '2904158192', '2904159355', '290415970*', '2904159849', '2904160348', '2904160428', '2904160487', '2904164840', '2904164875', '2904166459', '2904167400', '2904176008', '2904177350', '2904177502', '2904178054', '2904181800', '2904181851', '2904181907', '2904181958', '2904182002', '2904182053', '2904182109', '290418215*', '2904182205', '2904182256', '2904185211', '2904185246', '2904185270', '290418530*', '2904185334', '2904185852', '2904185895', '2904185916', '2904185932', '2904185975', '2904185991', '2904186011', '2904186054', '2904186070', '2904186097', '2904186134', '2904186150', '2904187305', '2904189407', '2904190918', '2904191013', '290419111*', '2904191216', '2904191312', '2904191419', '2904191515', '2904191611', '2904191718', '2904191814', '2904197589', '2904197677', '2904197706', '2904197730', '2904197765', '290419779*', '2904197829', '2904199007', '2904199031', '2904199066', '2904199090', '290419912*', '2904199154', '2904199189', '2904199218', '2904199314', '2904199410', '2904199517', '2904199613', '290419971*', '2904199816', '2904199912', '2904200012', '2904200119', '2904200215', '2904200311', '2904200418', '2904200514', '2904200610', '2904200717', '2904200813', '290420091*', '2904201015', '2904201111', '2904201218', '2904201314', '2904201410', '2904201517', '290420171*', '2904201816', '2904201824', '2904201920', '2904202026', '2904202229', '2904202325', '2904202421', '2904202528', '2904202624', '2904202720', '2904202827', '2904202923', '2904203029', '2904203125', '2904203221', '2904203328', '2904203424', '2904203520', '2904203627', '2904203723', '290420382*', '2904204128', '2904204224', '2904204427', '2904204523', '290420462*', '2904204726', '2904204822', '2904204929', '2904219805', '2904222721', '2904226773', '2904228656', '2904228701', '2904235549', '2904236816', '2904242159', '2904242255', '2904242300', '2904242351', '2904242407', '2904242458', '2904242503', '2904242554', '290424260*', '2904243258', '2904247902', '2904254782', '2904295605', '2904297459', '2904304233', '2904304444', '2904326707', '2904337852', '2904350969', '2904351312', '2904351857', '2904357562', '2904357837', '2904367859', '2904369037', '2904370804', '2904370900', '2904378013', '2904378216', '2904378312', '2904380009', '2904386507', '2904397708', '2904399404', '2904400700', '290440180*', '2904402802', '2904404453', '2904404509', '290440455*', '2904425000', '2904426206', '2904430029', '2904440008', '2904444543', '290444800*', '2904451452', '2904452906', '2904462063', '2904462098', '2904462127', '2904464800', '2904465555', '2904469441', '2904471955', '2904476801', '2904477126', '290447913*', '2904479156', '2904485951', '2904486102', '2904486153', '2904496976', '2904499755', '290450020*', '290450071*', '2904500736', '2904501085', '2904503814', '2904508172', '2904508930', '2904513860', '2904516682', '2904529504', '2904532922', '2904534696', '2904536149', '2904536384', '2904540607', '2904542370', '2904542936', '2904555454', '2904557759', '2904562259', '2904562355', '2904562451', '2904562558', '2904745004', '2904773005', '290493370*', '2904933953', '2904944353', '2905097408', '2905133405', '2905151902', '2905152358', '2905153406', '2905153553', '2905153668', '2905155807', '2905156025', '2905159357', '2905159605', '2905162900', '2905170150', '2905345707', '2905345723', '2905349409', '2905351402', '2905355403', '290612210*', '2906126506', '2906128608', '2906129627', '2906235913', '2906256503', '2906257805', '2906259501', '2906260158', '2906262401', '2906349451', '2906349558', '2906350305', '2906350356', '2906352706', '2906352909', '2906375940', '2906376740', '2906757551', '2906757850', '2906758503', '2906761200', '290676150*', '2906761956', '2906765500', '2906825606', '2906833550', '2906835855', '2906847709', '2906848402', '2906858301', '2906869879', '2906869908', '2906870036', '2906870159', '2906870757', '2906870837', '2906871602', '2906872007', '290687204*', '2906872082', '2906872162', '290687220*', '2906872242', '2906872322', '2906872365', '2906872445', '2906872488', '2906872525', '2906872568', '2906872605', '2906872648', '2906872680', '2906872728', '2906872760', '2906872808', '2906872840', '2906872920', '2906872963', '290687300*', '2906873042', '2906873122', '2906873165', '2906873202', '2906873245', '2906873288', '2906873325', '2906873368', '2906873405', '2906873448', '2906873480', '2906873528', '2906873560', '2906873608', '2906873640', '2906873683', '2906873720', '2906873763', '2906873800', '2906873843', '290693030*', '2906930350', '2906930553', '2906930609', '290693065*', '2906930705', '2906930756', '2906930801', '2906930852', '2906930908', '2906930959', '2906943709', '290694375*', '2906943805', '2906943856', '2906943901', '2906943952', '2906944015', '2906944058', '2906944103', '2906944154', '290694420*', '2906944250', '2906944306', '2906944357', '2906944402', '2906944453', '2906944509', '2906944656', '2906944701', '2906944752', '2906944808', '2906944859', '2906944904', '2906944955', '2906945018', '2906945050', '2906945106', '2906945157', '2906945253', '2906945309', '2906945552', '2906945608', '2906945659', '2906945958', '2906946053', '2906946408', '2906946504', '2906948251', '2906948358', '2906948403', '2906948454', '290694850*', '2906948702', '2906948809', '2906949158', '290694930*', '2906949350', '2906949510', '2906949609', '2906949852', '2906950001', '2906950204', '2906950255', '2906950300', '2906950351', '2906950407', '2906950757', '2906951004', '2906951514', '2907054305', '2907065207', '2907067608', '2907075157', '2907130806', '2907150452', '2907168513', '2907173005', '2907240212', '2907246008', '2907339044', '2907339060', '2907339087', '2907339108', '2907339167', '2907339183', '2907339204', '2907339220', '2907339247', '2907339263', '290733928*', '2907339300', '2907339327', '2907339343', '2907339386', '2907339407', '2907339423', '290733944*', '2907339466', '2907339482', '2907339618', '290734031*', '2907340416', '2907340512', '2907340619', '2907340715', '2907340811', '2907340918', '2907341013', '2907341312', '2907341419', '2907341515', '2907341611', '2907341718', '2907341814', '2907341910', '2907342016', '2907342112', '2907342219', '2907342315', '2907342614', '2907342710', '2907342817', '2907342913', '2907343019', '2907344214', '2907344249', '2907344273', '2907344302', '2907344337', '290734437*', '2907344409', '2907348039', '2907348063', '2907348098', '2907348151', '2907348303', '290734840*', '2907353006', '2907353057', '2907353102', '2907353153', '2907353209', '2907353305', '2907436127', '2907436223', '290743632*', '2907436522', '2907436629', '2907436725', '2907437322', '2907437621', '2907529606', '2907532100', '2907564102', '2907564153', '2907564903', '2907565957', '2907566001', '2907726052', '2907727354', '2907746205', '2907746539', '2907746563', '2907746803', '2907746846', '2907747005', '2907747128', '2907747152', '2907749246', '2907749289', '2907749326', '2907749481', '2907749545', '2907749609', '2907749668', '2907750052', '2907750140', '2907750204', '2907750474', '2907751303', '2907751389', '2907751426', '2907751469', '2907751485', '2907751506', '2907751522', '2907751549', '2907751565', '2907751581', '2907751602', '2907751629', '2907751645', '2907751661', '2907751688', '2907751741', '2907751901', '2907751952', '290779504*', '2908197658', '2908198992', '2908207000', '2908207748', '2908207764', '2908207780', '2908208011', '2908208118', '2908208214', '2908208310', '2908208417', '2908208513', '290820861*', '2908208716', '2908209460', '2908209903', '2908211405', '2908212053', '2908213101', '2908215457', '2908216652', '2908217006', '2908217903', '2908218105', '2908302358', '2908303350', '2908303801', '2908305807', '2908306105', '2908310702', '2908310905', '2908312206', '2908316100', '2908322359', '2908496009', '2908611804', '2908651101', '2908651208', '2908651507', '2908673108', '2908698604', '2908705018', '2908756157', '2908873003', '2908901000', '2908905255', '2908906856', '2908906952', '2908909504', '2908909555', '2908909600', '2908911014', '2908911057', '2908911153', '2908911356', '2908911508', '2908911807', '2909026252', '2909149009', '2909286011', '2909286206', '2909289001', '2909328007', '2909332014', '2909332209', '2909333009', '2909351004', '2909423004', '2909431012', '2909431151', '2909435005', '2909443005', '2909470011', '2909589004', '2909650258', '2909708106', '2909708800', '2909709221', '2909735008', '2909761003', '2909780503', '2909780618', '2909790007', '2909813117', '2909813256', '2909828028', '2909828503', '2909829506', '2909830507', '2909831016', '2909835500', '290983601*', '2909836407', '2909836802', '2909837207', '2909837602', '2909838015', '2909838402', '2909839202', '2909840019', '2909840801', '2909841206', '2909841601', '2909845012', '2909846015', '2909847018', '2909851017', '290985201*', '2909854015', '2909857021', '2909858016', '2909861020', '2909862015', '2909863026', '2909864010', '2909864504', '2909865013', '2909865507', '2909867027', '2909873216', '2909873558', '2909873777', '2909873881', '2909874120', '2909874235', '2909890008', '2909905003', '2909909004', '2909938008', '2909975001', '2910027009', '2910072002', '2910297017', '2910297033', '291029713*', '2910298108', '2910298183', '2910298247', '2910298335', '291029836*', '2910298482', '2910298546', '2910298722', '2910298757', '291029895*', '291034600*', '2910387004', '2910467004', '2910684009', '2910686004', '2910710203', '2910710502', '2910727005', '2910804007', '2910831005', '2910931006', '2910992001', '291099201*', '291110300*', '2911104002', '2911153007', '2911159003', '2911183003', '2911184006', '2911275004', '2911276007', '2911280006', '2911320004', '291133801*', '2911353009', '2911359005', '2911401007', '2911419004', '2911492009', '2911493001', '2911503003', '2911513009', '2911514001', '2911515004', '2911516007', '2911547006', '2911599009', '2911616008', '2911617000', '2911684019', '2911685011', '2911703013', '2911705000', '2911748000', '2911792001', '2911880001', '2911953004', '2911954007', '2911988004', '2912052005', '2912053008', '2912132312', '2912172007', '2912338003', '2912345000', '2912549003', '2912670698', '2912670719', '2912685558', '2912686112', '2912746701', '2912747210', '2912748002', '2912776003', '2912800640', '2912814153', '2912833047', '2912867255', '2912905004', '291293100*', '2912944003', '291296205*', '2912965058', '2912980506', '2912989009', '2913014107', '2913014203', '291301430*', '2913014406', '2913081000', '2913086004', '2913127005', '2913138003', '2913143005', '2913147006', '2913149001', '2913171006', '2913186005', '2913191007', '2913193002', '291320500*', '2913211602', '291352705*', '2913788508', '2913788815', '2913791707', '2913796305', '2913796364', '2913798378', '2913798490', '2913810509', '2913810568', '2913810592', '2913811341', '2913814251', '2913814358', '2913842009', '2913844012', '2913850340', '291386227*', '2913869869', '2913869914', '2913869965', '291387000*', '2913870050', '2913870106', '2913870157', '2913870202', '2913870253', '2913870309', '2913870501', '2913870851', '2913870907', '2913871002', '2913872451', '2914029722', '2914100058', '2914100154', '2914106062', '2914110045', '2914110088', '2914110125', '2914110168', '2914110205', '2914110248', '2914110280', '2914110408', '2914110440', '2914110520', '2914110563', '2914110643', '2914110723', '2914110766', '2914110803', '2914110846', '2914111363', '2914111486', '2914111523', '2914111566', '2914111689', '2914111881', '2914111929', '2914112008', '2914112120', '2914112323', '2914112403', '2914112964', '2914113561', '2914113684', '2914114169', '291411496*', '2914115081', '2914115161', '2914115209', '2914116164', '2914116244', '2914116287', '2914116324', '2914116447', '291411648*', '2914116527', '291411656*', '2914116682', '291411672*', '2914116762', '2914116842', '2914117642', '2914117749', '2914117941', '2914118047', '291411824*', '2914118346', '2914118442', '2914118549', '2914118645', '2914138144', '2914138208', '2914138232', '2914138267', '2914140674', '2914141036', '2914142020', '2914142194', '2914252676', '2914252713', '291425273*', '2914253257', '2914254807', '2914255113', '2914255156', '2914255199', '2914255316', '2914259421', '2914259544', '2914263308', '2914264714', '2914265370', '2914272503', '2914272511', '2914272618', '2914272714', '2914272810', '2914274154', '2914274533', '2914274568', '2914274779', '2914274998', '2914276029', '2914278382', '2914278542', '2914281952', '2914282226', '2914282461', '2914282760', '2914282795', '2914282824', '2914282859', '2914282883', '2914282912', '2914282947', '2914282971', '2914283018', '2914283042', '2914289559', '2914537954', '2914566704', '2914566851', '2914567205', '291456731*', '2914568574', '2914569024', '2914571554', '2914579855', '2914584355', '2914584419', '291458980*', '2914593809', '2914595206', '291460060*', '2914601549', '2914602509', '2914602859', '2914602947', '2914607596', '2914610402', '2914610605', '2914614956', '2914646800', '2914652100', '2914654202', '2914656654', '2914706201', '2914716004', '2914723458', '2914788657', '2914789107', '291479140*', '2914792402', '2914796067', '2914796366', '2915029003', '2915073303', '2915085603', '2915095457', '2915106224', '2915106953', '2915119447', '2915120165', '2915120464', '2915123278', '2915123972', '2915124561', '2915133855', '2915133900', '2915135009', '2915143228', '2915143391', '2915146306', '2915153100', '2915159908', '2915163552', '2915164651', '2915165451', '2915190155', '2915203008', '2915207332', '2915211032', '2915211534', '2915219915', '2915260109', '2915260707', '2915311009', '2915346551', '2915347503', '2915351203', '291535130*', '2915351473', '2915624259', '291562665*', '2915637754', '2915638001', '2915639151', '2915647303', '2915668307', '291566850*', '2915780016', '2915780200', '2915780411', '2915807004', '2915826002', '2915849001', '2915850002', '2915953001', '2915986006', '2916093007', '2916169008', '2916229007', '2916244004', '291628900*', '291632600*', '2916328005', '291634200*', '2916387806', '2916388454', '2916399807', '2916447004', '291644900*', '2916474002', '2916554002', '2916572008', '2916755007', '2916795009', '2916810053', '2916810969', '2916812075', '2916812139', '2916812796', '2916833837', '2917008003', '2917334407', '2917334909', '2917346379', '2917531005', '2917612008', '2917639008', '2917723007', '2917802004', '2917834153', '2917838605', '2917868003', '2917941004', '2918053009', '2918067005', '2918111301', '2918111707', '2918158003', '291816100*', '2918312007', '2918362004', '2918384000', '2918621002', '2918634014', '2918698050', '2918716001', '2918740001', '2918747000', '2918810153', '2918812597', '2918812802', '2918815253', '2918818956', '2918820706', '2918825857', '2918828126', '2918858851', '2918865808', '2918867600', '2918880768', '2918881808', '2918887898', '291888980*', '2918910007', '2918934113', '2918960004', '2919013009', '2919036008', '2919066645', '2919067162', '2919067226', '2919067402', '2919067904', '2919086953', '2919087251', '2919087358', '2919088801', '291916400*', '2919168406', '291919900*', '2919207006', '2919212008', '2919226055', '2919305626', '291940785*', '2919408959', '2919409150', '2919543202', '2919613004', '2919619000', '2919697009', '2919777009', '2919803000', '2919858001', '2919926000', '2919944006', '2919950000', '2919959013', '2919980058', '2919987532', '2920002104', '2920002200', '2920009103', '2920056209', '2920057260', '2920058909', '2920059100', '2920060558', '2920060806', '2920062457', '292006257*', '2920063302', '2920063900', '2920064102', '2920064305', '292006580*', '2920066909', '2920158002', '2920274003', '2920302000', '2920311003', '2920329019', '2920330159', '2920330255', '2920330503', '2920330917', '2920332509', '2920335259', '2920336040', '2920336075', '2920336104', '2920336139', '2920336198', '2920336227', '2920336286', '2920336438', '2920336462', '2920336497', '2920336526', '2920336550', '2920336585', '2920336614', '2920336673', '2920336702', '2920336737', '2920336761', '2920336796', '2920352008', '2920358004', '2920367007', '2920369002', '2920393002', '2920395008', '2920397003', '2920434521', '2920434986', '2920445001', '2920477302', '2920494516', '292049900*', '2920537002', '2921107004', '2921132007', '2921134002', '2921136008', '2921164009', '2921198006', '2921199009', '2921224008', '2921229052', '2921230504', '2921237423', '2921240016', '2921265707', '2921266750', '2921268211', '2921303005', '2921351007', '292138700*', '2921393012', '2921403006', '292140800*', '2921415007', '2921420017', '2921421001', '2921452799', '2921466007', '2921470313', '2921471009', '3229803008', '3229817004', '3229876004', '323003500*', '3230090009', '3230144003', '3230164004', '3230360005', '3230495305', '3230552007', '3230580008', '3230601008', '3230663006', '3230673001', '3230704007', '3230756333', '3230759008', '3230786006', '3230850004', '3230881003', '3230888002', '3230944000', '3230965004', '3230978008', '3231033006', '3231057008', '3231060506', '323106200*', '3231129008', '3231327004', '3231328007', '3231372016', '3231376009', '3231522600', '3231655059', '3231658006', '3231659009', '3231678007', '323167900*', '3231680000', '3231681003', '3231789006', '3231899707', '323191900*', '3231934509', '3231944504', '3231979002', '3232079006', '3232174003', '3232184105', '3232246206', '3232248009', '3232336009', '3232422003', '3232422118', '3232448000', '3232509002', '3232535008', '3232596003', '3232609003', '3232610055', '3232675000', '3232798000', '3232806007', '3232848004', '3233146004', '3233179009', '3233189004', '3233317002', '3233331007', '3233475000', '3233499002', '3233512000', '3233593007', '3233612001', '3233614007', '3233640002', '3233725006', '3233881009', '3233883004', '323388500*', '3234104359', '3234160000', '3234230005', '3234301002', '3234346008', '3234478000', '3234479003', '3234573008', '3234632004', '3234649009', '3234719003', '3234740005', '3234833164', '3234840014', '3234989257', '3235062007', '3235120000', '323512700*', '3235168004', '3235181006', '3235200019', '3235453008', '3235486002', '3235500003', '3235673019', '3235734459', '3235743005', '3235798006', '323580375*', '3235843313', '3235854004', '3235983308', '3236718100', '3236762005', '3236992134', '3237030308', '3237045200', '323710002*', '3237102500', '3237106202', '3237134000', '3237134019', '3237232006', '3237252007', '323725415*', '3237409502', '3237418505', '3237441502', '3237647009', '3237668002', '3237721459', '3237721803', '3237745055', '3237774059', '3237775051', '323788889*', '323788950*', '3237932053', '323793805*', '3237947132', '3237953508', '3237953807', '3237954084', '3237954404', '3238012005', '3238143056', '323815605*', '3238157052', '323820105*', '3238261052', '3238271058', '323827905*', '3238327058', '3238348051', '3238415058', '3238426005', '3238506312', '323851104*', '3238600106', '3238602005', '3238642365', '3238643114', '3238710057', '3238775053', '3238800706', '3238811229', '323885005*', '3238855053', '3238870050', '3238872806', '3238873227', '3238873606', '3238873905', '3238874107', '3238875804', '3238876559', '323887721*', '3238877279', '3238877404', '3238879856', '3238883708', '323888556*', '3238885623', '3238889253', '3238894503', '323891720*', '3238922201', '3238922607', '3238922658', '3241975005', '3241992008', '3241992059', '3242024252', '3242024754', '3242024957', '3242025001', '3242031057', '3242043058', '3242077004', '3242077012', '324207708*', '3242077119', '3242115007', '324212005*', '3242121001', '3242141002', '324482208*', '324488300*', '3244884002', '3244931008', '3244948002', '3245037008', '3245074001', '3245395008', '3245410001', '3245420007', '324544210*', '3245448501', '3245487009', '3245538005', '3245571008', '3245602257', '3245657004', '3245711007', '3245809004', '3246503007', '3246504106', '3246524000', '3246583000', '3246649006', '3246669007', '324668600*', '3246688101', '3246727000', '3246732002', '3246781007', '3246805005', '3246812002', '3246896007', '3246901005', '3246939003', '3246953008', '3247106003', '3247186007', '3247235294', '3247239615', '3247240114', '3247242515', '324724561*', '3247311760', '3247750018', '3247750210', '3247768023', '324776820*', '3247768402', '3247780209', '3247815221', '324785700*', '3247943004', '3247953608', '3247954002', '324795570*', '3248001000', '3248006282', '3248006944', '3248007576', '3248008384', '3248036051', '3248053003', '3248128001', '3248172002', '3248185006', '3248188004', '324823201*', '3248232116', '3248266009', '3248272003', '3248276004', '3248361401', '3248371001', '3248409006', '3248437402', '3248442025', '3248551002', '3248554756', '3248683005', '3248705008', '32487</t>
         </is>
       </c>
     </row>

</xml_diff>